<commit_message>
questionnaire: Added the `end` section
fixes #5

Add the end section widgets to the excel file
Run `yarn generateSurvey`
Rename `customValidations.tsx` to `customValidations.ts` as it does not
contain anything React.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="678" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="924" uniqueCount="537">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -729,6 +729,234 @@
     <t xml:space="preserve">household_save</t>
   </si>
   <si>
+    <t xml:space="preserve">householdOwnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">end</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household.ownership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Est-ce que votre ménage est locataire ou propriétaire de votre logement?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Does your household rent or own your home?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">householdOwnershipChoices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">householdIncome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household.income</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tranche de revenu avant impôts (brut) du ménage, en 2023?
+__Facultatif__</t>
+  </si>
+  <si>
+    <t xml:space="preserve">What was your household's income range before taxes (gross income), in 2023?
+__Not mandatory__</t>
+  </si>
+  <si>
+    <t xml:space="preserve">householdIncomeChoices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wouldLikeToParticipateInOtherSurveysChaireMobilite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Seriez-vous intéressés à **participer à d'autres études** menées par la **Chaire Mobilité de Polytechnique Montréal** ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Would you be interested in **participating in other studies** conducted by the **Chaire Mobilite at Polytechnique Montreal**?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wouldLikeToParticipateInOtherSurveysChaireMobiliteContactEmail</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veuillez fournir l'**adresse e-mail** où vous pouvez être contacté pour participer à d'autres études de la Chaire Mobilité.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please provide the **email address** where you can be reached to participate in other studies by the Chaire Mobilite.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wantToParticipateInOtherSurveysChaireMobiliteConditional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">householdCommentsOnSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commentsOnSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vos **commentaires et suggestions** sur le questionnaire (facultatif)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your **comments and suggestions** about the survey (optional)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optionalValidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optionalIntroText</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L'entrevue est maintenant terminée. Merci pour votre participation et votre patience!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The next questions are optional and are added for research purposes. You can complete the interview without answering them.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buttonCompleteInterviewWithCompleteSectionNoOptional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminer l'entrevue sans les questions optionnelles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete interview without optional questions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">householdHybridCarNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household.hybridCarNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parmi les véhicules possédés par votre ménage, combien sont des **véhicules hybrides rechargeables**?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Among the vehicles owned by your household, how many are **plug-in hybrid vehicles**?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min=0
+max=household.carNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">householdHasCars</t>
+  </si>
+  <si>
+    <t xml:space="preserve">householdHybridCarCountCustomValidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">householdElectricCarNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household.electricCarNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parmi les véhicules possédés par votre ménage, combien sont des **véhicules électriques**?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Among the vehicles owned by your household, how many are **electric vehicles**?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">householdElectricCarCountCustomValidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endDurationOfTheSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">durationOfSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pensez-vous que la **durée de l'enquête était trop courte, correcte ou trop longue**?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you feel that the **length of the survey was too short, about right, or too long**?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sliderTooShortToTooLong</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endTimeSpentAnswering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timeSpentAnswering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combien de **temps** pensez-vous avoir passé **à répondre** à cette enquête (**en minutes**) ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How much **time** do you think you **spent answering** this survey (**in minutes**)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endInterestOfTheSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interestOfTheSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans quelle mesure cette enquête a-t-elle été **intéressante** pour vous ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How **interesting** was this survey to you?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sliderNotAtAllToVeryInteresting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endDifficultyOfTheSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">difficultyOfTheSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans quelle mesure vous a-t-il été **facile** ou **difficile** de répondre aux questions de cette enquête ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How **easy** or **difficult** was it for you to answer the questions in this survey?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sliderVeryEasyToVeryDifficult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endBurdenOfTheSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">burdenOfTheSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans quelle mesure avez-vous trouvé cette enquête **pénible (exigeante)** ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How **burdensome (demanding)** did you find this survey to be?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sliderNotAtAllToVeryBurdensome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endConsideredAbandoningSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">consideredAbandoningSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Avez-vous pensé, à un moment ou un autre, **abandonner l'enquête** ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Have you considered, at any point, to **abandon the survey**?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buttonCompleteInterviewWithCompleteSection</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Terminer l’entrevue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Complete interview</t>
+  </si>
+  <si>
     <t xml:space="preserve">completedText</t>
   </si>
   <si>
@@ -845,6 +1073,9 @@
     <t xml:space="preserve">onTheRoadWithUsualPlace</t>
   </si>
   <si>
+    <t xml:space="preserve">household.carNumber</t>
+  </si>
+  <si>
     <t xml:space="preserve">abbreviation</t>
   </si>
   <si>
@@ -884,6 +1115,15 @@
     <t xml:space="preserve">Household</t>
   </si>
   <si>
+    <t xml:space="preserve">e_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">End</t>
+  </si>
+  <si>
     <t xml:space="preserve">c_</t>
   </si>
   <si>
@@ -1190,6 +1430,147 @@
     <t xml:space="preserve">No, remote studies from home or from elsewhere</t>
   </si>
   <si>
+    <t xml:space="preserve">000000_009999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moins de 10 000 $</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Less than $10,000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">010000_019999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10 000$ à 19 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$10,000 to $19,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">020000_029999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20 000$ à 29 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$20,000 to $29,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">030000_039999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30 000$ à 39 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$30,000 to $39,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">040000_049999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40 000$ à 49 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$40,000 to $49,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">050000_059999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50 000$ à 59 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$50,000 to $59,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">060000_069999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60 000$ à 69 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$60,000 to $69,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">070000_079999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70 000$ à 79 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$70,000 to $79,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">080000_089999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80 000$ à 89 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$80,000 to $89,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">090000_099999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">90 000$ à 99 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$90,000 to $99,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100000_149999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">100 000$ à 149 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$100,000 to $149,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150000_199999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">150 000$ à 199 999$</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$150,000 to $199,999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200000_999999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">200 000 $ et plus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">$200,000 and more</t>
+  </si>
+  <si>
+    <t xml:space="preserve">refusal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I prefer not to respond</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tenant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Locataire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tenant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">owner</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Propriétaire</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Owner</t>
+  </si>
+  <si>
     <t xml:space="preserve">inputRangeName</t>
   </si>
   <si>
@@ -1224,6 +1605,84 @@
   </si>
   <si>
     <t xml:space="preserve">input_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trop court</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juste comme il faut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trop long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too short</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas du tout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neutre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Très intéressante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not at all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neutral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very interesting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red-yellow-green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Très facile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modérément difficile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Très difficile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very easy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderately difficult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very difficult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green-yellow-red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modérément pénible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Très pénible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderately burdensome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very burdensome</t>
   </si>
   <si>
     <t xml:space="preserve">key</t>
@@ -1249,7 +1708,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1342,6 +1801,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1356,12 +1822,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="0"/>
-    </font>
-    <font>
       <b val="true"/>
       <sz val="11"/>
       <color theme="1"/>
@@ -1371,10 +1831,24 @@
     </font>
     <font>
       <b val="true"/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <b val="true"/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1473,7 +1947,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="52">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1590,11 +2064,23 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1606,11 +2092,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1626,11 +2112,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1646,12 +2140,20 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -1663,7 +2165,7 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="12">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1754,6 +2256,34 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Aptos Narrow"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Aptos Narrow"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FFFFFFFF"/>
+        <sz val="11"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="1"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2002,14 +2532,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:X42"/>
+  <dimension ref="A1:X1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="J34" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="M25" activeCellId="0" sqref="M25"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A34" activeCellId="0" sqref="A34"/>
+      <selection pane="bottomRight" activeCell="O48" activeCellId="0" sqref="O48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4047,67 +4577,805 @@
       <c r="W41" s="28"/>
       <c r="X41" s="28"/>
     </row>
-    <row r="42" customFormat="false" ht="116.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="1" t="s">
+    <row r="42" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="29" t="s">
         <v>215</v>
       </c>
-      <c r="B42" s="1" t="s">
+      <c r="B42" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C42" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D42" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E42" s="28"/>
+      <c r="F42" s="28" t="s">
+        <v>217</v>
+      </c>
+      <c r="G42" s="27" t="s">
+        <v>218</v>
+      </c>
+      <c r="H42" s="27" t="s">
+        <v>219</v>
+      </c>
+      <c r="I42" s="27"/>
+      <c r="J42" s="27"/>
+      <c r="K42" s="27"/>
+      <c r="L42" s="28"/>
+      <c r="M42" s="28"/>
+      <c r="N42" s="28"/>
+      <c r="O42" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="P42" s="28"/>
+      <c r="Q42" s="28"/>
+      <c r="R42" s="28"/>
+      <c r="S42" s="28"/>
+      <c r="T42" s="27"/>
+      <c r="U42" s="28"/>
+      <c r="V42" s="28"/>
+      <c r="W42" s="28"/>
+      <c r="X42" s="28"/>
+    </row>
+    <row r="43" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="29" t="s">
+        <v>221</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="C43" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E43" s="28"/>
+      <c r="F43" s="28" t="s">
+        <v>223</v>
+      </c>
+      <c r="G43" s="27" t="s">
+        <v>224</v>
+      </c>
+      <c r="H43" s="27" t="s">
+        <v>225</v>
+      </c>
+      <c r="I43" s="27"/>
+      <c r="J43" s="27"/>
+      <c r="K43" s="27"/>
+      <c r="L43" s="28"/>
+      <c r="M43" s="28"/>
+      <c r="N43" s="28"/>
+      <c r="O43" s="30" t="s">
+        <v>226</v>
+      </c>
+      <c r="P43" s="28"/>
+      <c r="Q43" s="28"/>
+      <c r="R43" s="28"/>
+      <c r="S43" s="28"/>
+      <c r="T43" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U43" s="28"/>
+      <c r="V43" s="28"/>
+      <c r="W43" s="28"/>
+      <c r="X43" s="28"/>
+    </row>
+    <row r="44" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="B44" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C44" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E44" s="28"/>
+      <c r="F44" s="29" t="s">
+        <v>227</v>
+      </c>
+      <c r="G44" s="31" t="s">
+        <v>228</v>
+      </c>
+      <c r="H44" s="31" t="s">
+        <v>229</v>
+      </c>
+      <c r="I44" s="27"/>
+      <c r="J44" s="27"/>
+      <c r="K44" s="27"/>
+      <c r="L44" s="28"/>
+      <c r="M44" s="28"/>
+      <c r="N44" s="0"/>
+      <c r="O44" s="28" t="s">
+        <v>33</v>
+      </c>
+      <c r="P44" s="28"/>
+      <c r="Q44" s="28"/>
+      <c r="R44" s="28"/>
+      <c r="S44" s="28"/>
+      <c r="T44" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U44" s="28"/>
+      <c r="V44" s="28"/>
+      <c r="W44" s="28"/>
+      <c r="X44" s="28"/>
+    </row>
+    <row r="45" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="B45" s="27" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D45" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E45" s="28"/>
+      <c r="F45" s="29" t="s">
+        <v>230</v>
+      </c>
+      <c r="G45" s="31" t="s">
+        <v>231</v>
+      </c>
+      <c r="H45" s="31" t="s">
+        <v>232</v>
+      </c>
+      <c r="I45" s="27"/>
+      <c r="J45" s="27"/>
+      <c r="K45" s="27"/>
+      <c r="L45" s="28"/>
+      <c r="M45" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="N45" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="O45" s="28"/>
+      <c r="P45" s="28"/>
+      <c r="Q45" s="28"/>
+      <c r="R45" s="28"/>
+      <c r="S45" s="28"/>
+      <c r="T45" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U45" s="28"/>
+      <c r="V45" s="28"/>
+      <c r="W45" s="28"/>
+      <c r="X45" s="28"/>
+    </row>
+    <row r="46" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="29" t="s">
+        <v>234</v>
+      </c>
+      <c r="B46" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="C46" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D46" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E46" s="28"/>
+      <c r="F46" s="28" t="s">
+        <v>236</v>
+      </c>
+      <c r="G46" s="30" t="s">
+        <v>237</v>
+      </c>
+      <c r="H46" s="30" t="s">
+        <v>238</v>
+      </c>
+      <c r="I46" s="27"/>
+      <c r="J46" s="27"/>
+      <c r="K46" s="27"/>
+      <c r="L46" s="28"/>
+      <c r="M46" s="28"/>
+      <c r="N46" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="O46" s="28"/>
+      <c r="P46" s="28"/>
+      <c r="Q46" s="28"/>
+      <c r="R46" s="28"/>
+      <c r="S46" s="28"/>
+      <c r="T46" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U46" s="28"/>
+      <c r="V46" s="28"/>
+      <c r="W46" s="28"/>
+      <c r="X46" s="28"/>
+    </row>
+    <row r="47" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="29" t="s">
+        <v>240</v>
+      </c>
+      <c r="B47" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C42" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D42" s="1" t="s">
+      <c r="C47" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D47" s="27" t="s">
         <v>216</v>
       </c>
-      <c r="F42" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="G42" s="1" t="s">
-        <v>217</v>
-      </c>
-      <c r="H42" s="1" t="s">
-        <v>218</v>
-      </c>
-      <c r="L42" s="29"/>
-      <c r="M42" s="30"/>
-      <c r="T42" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
+      <c r="E47" s="28"/>
+      <c r="F47" s="28" t="s">
+        <v>240</v>
+      </c>
+      <c r="G47" s="27" t="s">
+        <v>241</v>
+      </c>
+      <c r="H47" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="I47" s="27"/>
+      <c r="J47" s="27"/>
+      <c r="K47" s="27"/>
+      <c r="L47" s="28"/>
+      <c r="M47" s="28"/>
+      <c r="N47" s="28"/>
+      <c r="O47" s="28"/>
+      <c r="P47" s="28"/>
+      <c r="Q47" s="28"/>
+      <c r="R47" s="28"/>
+      <c r="S47" s="28"/>
+      <c r="T47" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U47" s="28"/>
+      <c r="V47" s="28"/>
+      <c r="W47" s="28"/>
+      <c r="X47" s="28"/>
+    </row>
+    <row r="48" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="B48" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D48" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E48" s="28"/>
+      <c r="F48" s="29" t="s">
+        <v>243</v>
+      </c>
+      <c r="G48" s="29" t="s">
+        <v>244</v>
+      </c>
+      <c r="H48" s="29" t="s">
+        <v>245</v>
+      </c>
+      <c r="I48" s="27"/>
+      <c r="J48" s="27"/>
+      <c r="K48" s="27"/>
+      <c r="L48" s="28"/>
+      <c r="M48" s="28"/>
+      <c r="N48" s="28"/>
+      <c r="O48" s="28"/>
+      <c r="P48" s="28"/>
+      <c r="Q48" s="28"/>
+      <c r="R48" s="28"/>
+      <c r="S48" s="28"/>
+      <c r="T48" s="27"/>
+      <c r="U48" s="28"/>
+      <c r="V48" s="28"/>
+      <c r="W48" s="28"/>
+      <c r="X48" s="28"/>
+    </row>
+    <row r="49" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="29" t="s">
+        <v>246</v>
+      </c>
+      <c r="B49" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C49" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D49" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E49" s="28"/>
+      <c r="F49" s="28" t="s">
+        <v>247</v>
+      </c>
+      <c r="G49" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="H49" s="27" t="s">
+        <v>249</v>
+      </c>
+      <c r="I49" s="27"/>
+      <c r="J49" s="27"/>
+      <c r="K49" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="L49" s="28"/>
+      <c r="M49" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="N49" s="29" t="s">
+        <v>252</v>
+      </c>
+      <c r="O49" s="28"/>
+      <c r="P49" s="28"/>
+      <c r="Q49" s="28"/>
+      <c r="R49" s="28"/>
+      <c r="S49" s="28"/>
+      <c r="T49" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U49" s="28"/>
+      <c r="V49" s="28"/>
+      <c r="W49" s="28"/>
+      <c r="X49" s="28"/>
+    </row>
+    <row r="50" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="29" t="s">
+        <v>253</v>
+      </c>
+      <c r="B50" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="C50" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E50" s="28"/>
+      <c r="F50" s="28" t="s">
+        <v>254</v>
+      </c>
+      <c r="G50" s="27" t="s">
+        <v>255</v>
+      </c>
+      <c r="H50" s="27" t="s">
+        <v>256</v>
+      </c>
+      <c r="I50" s="27"/>
+      <c r="J50" s="27"/>
+      <c r="K50" s="7" t="s">
+        <v>250</v>
+      </c>
+      <c r="L50" s="28"/>
+      <c r="M50" s="28" t="s">
+        <v>251</v>
+      </c>
+      <c r="N50" s="29" t="s">
+        <v>257</v>
+      </c>
+      <c r="O50" s="28"/>
+      <c r="P50" s="28"/>
+      <c r="Q50" s="28"/>
+      <c r="R50" s="28"/>
+      <c r="S50" s="28"/>
+      <c r="T50" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U50" s="28"/>
+      <c r="V50" s="28"/>
+      <c r="W50" s="28"/>
+      <c r="X50" s="28"/>
+    </row>
+    <row r="51" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="29" t="s">
+        <v>258</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C51" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D51" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28" t="s">
+        <v>260</v>
+      </c>
+      <c r="G51" s="30" t="s">
+        <v>261</v>
+      </c>
+      <c r="H51" s="30" t="s">
+        <v>262</v>
+      </c>
+      <c r="I51" s="27"/>
+      <c r="J51" s="27"/>
+      <c r="K51" s="27"/>
+      <c r="L51" s="28"/>
+      <c r="M51" s="28"/>
+      <c r="N51" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="O51" s="28"/>
+      <c r="P51" s="28"/>
+      <c r="Q51" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="R51" s="28"/>
+      <c r="S51" s="28"/>
+      <c r="T51" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U51" s="28"/>
+      <c r="V51" s="28"/>
+      <c r="W51" s="28"/>
+      <c r="X51" s="28"/>
+    </row>
+    <row r="52" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="29" t="s">
+        <v>264</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C52" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E52" s="28"/>
+      <c r="F52" s="28" t="s">
+        <v>265</v>
+      </c>
+      <c r="G52" s="30" t="s">
+        <v>266</v>
+      </c>
+      <c r="H52" s="30" t="s">
+        <v>267</v>
+      </c>
+      <c r="I52" s="27"/>
+      <c r="J52" s="27"/>
+      <c r="K52" s="27"/>
+      <c r="L52" s="28"/>
+      <c r="M52" s="28"/>
+      <c r="N52" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="O52" s="28"/>
+      <c r="P52" s="28"/>
+      <c r="Q52" s="28"/>
+      <c r="R52" s="28"/>
+      <c r="S52" s="28"/>
+      <c r="T52" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U52" s="28"/>
+      <c r="V52" s="28"/>
+      <c r="W52" s="28"/>
+      <c r="X52" s="28"/>
+    </row>
+    <row r="53" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="29" t="s">
+        <v>268</v>
+      </c>
+      <c r="B53" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C53" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E53" s="28"/>
+      <c r="F53" s="28" t="s">
+        <v>269</v>
+      </c>
+      <c r="G53" s="30" t="s">
+        <v>270</v>
+      </c>
+      <c r="H53" s="30" t="s">
+        <v>271</v>
+      </c>
+      <c r="I53" s="27"/>
+      <c r="J53" s="27"/>
+      <c r="K53" s="27"/>
+      <c r="L53" s="28"/>
+      <c r="M53" s="28"/>
+      <c r="N53" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="O53" s="28"/>
+      <c r="P53" s="28"/>
+      <c r="Q53" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="R53" s="28"/>
+      <c r="S53" s="28"/>
+      <c r="T53" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U53" s="28"/>
+      <c r="V53" s="28"/>
+      <c r="W53" s="28"/>
+      <c r="X53" s="28"/>
+    </row>
+    <row r="54" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="29" t="s">
+        <v>273</v>
+      </c>
+      <c r="B54" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C54" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E54" s="28"/>
+      <c r="F54" s="28" t="s">
+        <v>274</v>
+      </c>
+      <c r="G54" s="30" t="s">
+        <v>275</v>
+      </c>
+      <c r="H54" s="30" t="s">
+        <v>276</v>
+      </c>
+      <c r="I54" s="27"/>
+      <c r="J54" s="27"/>
+      <c r="K54" s="27"/>
+      <c r="L54" s="28"/>
+      <c r="M54" s="28"/>
+      <c r="N54" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="O54" s="28"/>
+      <c r="P54" s="28"/>
+      <c r="Q54" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="R54" s="28"/>
+      <c r="S54" s="28"/>
+      <c r="T54" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U54" s="28"/>
+      <c r="V54" s="28"/>
+      <c r="W54" s="28"/>
+      <c r="X54" s="28"/>
+    </row>
+    <row r="55" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="29" t="s">
+        <v>278</v>
+      </c>
+      <c r="B55" s="27" t="s">
+        <v>259</v>
+      </c>
+      <c r="C55" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E55" s="28"/>
+      <c r="F55" s="28" t="s">
+        <v>279</v>
+      </c>
+      <c r="G55" s="30" t="s">
+        <v>280</v>
+      </c>
+      <c r="H55" s="30" t="s">
+        <v>281</v>
+      </c>
+      <c r="I55" s="27"/>
+      <c r="J55" s="27"/>
+      <c r="K55" s="27"/>
+      <c r="L55" s="28"/>
+      <c r="M55" s="28"/>
+      <c r="N55" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="O55" s="28"/>
+      <c r="P55" s="28"/>
+      <c r="Q55" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="R55" s="28"/>
+      <c r="S55" s="28"/>
+      <c r="T55" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U55" s="28"/>
+      <c r="V55" s="28"/>
+      <c r="W55" s="28"/>
+      <c r="X55" s="28"/>
+    </row>
+    <row r="56" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="29" t="s">
+        <v>283</v>
+      </c>
+      <c r="B56" s="27" t="s">
+        <v>30</v>
+      </c>
+      <c r="C56" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D56" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E56" s="28"/>
+      <c r="F56" s="28" t="s">
+        <v>284</v>
+      </c>
+      <c r="G56" s="30" t="s">
+        <v>285</v>
+      </c>
+      <c r="H56" s="30" t="s">
+        <v>286</v>
+      </c>
+      <c r="I56" s="27"/>
+      <c r="J56" s="27"/>
+      <c r="K56" s="27"/>
+      <c r="L56" s="28"/>
+      <c r="M56" s="28"/>
+      <c r="N56" s="28" t="s">
+        <v>239</v>
+      </c>
+      <c r="O56" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="P56" s="28"/>
+      <c r="Q56" s="28"/>
+      <c r="R56" s="28"/>
+      <c r="S56" s="28"/>
+      <c r="T56" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="U56" s="28"/>
+      <c r="V56" s="28"/>
+      <c r="W56" s="28"/>
+      <c r="X56" s="28"/>
+    </row>
+    <row r="57" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="B57" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="C57" s="27" t="b">
+        <v>1</v>
+      </c>
+      <c r="D57" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="E57" s="28"/>
+      <c r="F57" s="29" t="s">
+        <v>287</v>
+      </c>
+      <c r="G57" s="27" t="s">
+        <v>288</v>
+      </c>
+      <c r="H57" s="29" t="s">
+        <v>289</v>
+      </c>
+      <c r="I57" s="27"/>
+      <c r="J57" s="27"/>
+      <c r="K57" s="27"/>
+      <c r="L57" s="28"/>
+      <c r="M57" s="28"/>
+      <c r="N57" s="28"/>
+      <c r="O57" s="28"/>
+      <c r="P57" s="28"/>
+      <c r="Q57" s="28"/>
+      <c r="R57" s="28"/>
+      <c r="S57" s="28"/>
+      <c r="T57" s="27"/>
+      <c r="U57" s="28"/>
+      <c r="V57" s="28"/>
+      <c r="W57" s="28"/>
+      <c r="X57" s="28"/>
+    </row>
+    <row r="58" customFormat="false" ht="116.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="B58" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C58" s="1" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>293</v>
+      </c>
+      <c r="L58" s="32"/>
+      <c r="M58" s="33"/>
+      <c r="T58" s="1" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:X1"/>
-  <conditionalFormatting sqref="N42:Q42">
+  <conditionalFormatting sqref="N58:Q58">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>AND($B1048370="Custom",  $B1048370&lt;&gt;"", ROW(N1048370)&lt;&gt;1)</formula>
+      <formula>AND($B1048386="Custom",  $B1048386&lt;&gt;"", ROW(N1048386)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q42">
+  <conditionalFormatting sqref="Q58">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND($B42&lt;&gt;"Range", $B42&lt;&gt;"", ROW(Q42)&lt;&gt;1)</formula>
+      <formula>AND($B58&lt;&gt;"Range", $B58&lt;&gt;"", ROW(Q58)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C42">
+  <conditionalFormatting sqref="C58">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="5">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",C58)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="6">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C42)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",C58)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O42:P42">
+  <conditionalFormatting sqref="O58:P58">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($B42&lt;&gt;"Select", $B42&lt;&gt;"Checkbox", $B42&lt;&gt;"Radio",  $B42&lt;&gt;"", ROW(O42)&lt;&gt;1)</formula>
+      <formula>AND($B58&lt;&gt;"Select", $B58&lt;&gt;"Checkbox", $B58&lt;&gt;"Radio",  $B58&lt;&gt;"", ROW(O58)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C43:C1048576 C1:C41">
+  <conditionalFormatting sqref="C59:C1048576 C1:C57">
     <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
     <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q51">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+      <formula>AND($B1048380="Custom",  $B1048380&lt;&gt;"", ROW(Q1048380)&lt;&gt;1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q51 Q54:Q55">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND($B51&lt;&gt;"Range", $B51&lt;&gt;"", ROW(Q51)&lt;&gt;1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q54:Q55">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+      <formula>AND(#REF!="Custom",  #REF!&lt;&gt;"", ROW(#REF!)&lt;&gt;1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O43">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+      <formula>AND($B43="Custom",  $B43&lt;&gt;"", ROW(O43)&lt;&gt;1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O43">
+    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+      <formula>AND($B43&lt;&gt;"Select", $B43&lt;&gt;"Checkbox", $B43&lt;&gt;"Radio",  $B43&lt;&gt;"", ROW(O43)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4126,510 +5394,538 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F30"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E39" activeCellId="0" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="27.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="32" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="31" width="12.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="27.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="35" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="12.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="35" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="33" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1" s="33" t="s">
-        <v>220</v>
-      </c>
-      <c r="C1" s="33" t="s">
+    <row r="1" s="38" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="36" t="s">
+        <v>294</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>295</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="34" t="s">
-        <v>221</v>
-      </c>
-      <c r="E1" s="33" t="s">
-        <v>222</v>
-      </c>
-      <c r="F1" s="33" t="s">
-        <v>223</v>
+      <c r="D1" s="37" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1" s="36" t="s">
+        <v>297</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>298</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36" t="s">
-        <v>224</v>
-      </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="D2" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E2" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="F2" s="36"/>
+      <c r="A2" s="39" t="s">
+        <v>299</v>
+      </c>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39" t="s">
+        <v>300</v>
+      </c>
+      <c r="D2" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E2" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="39" t="s">
         <v>95</v>
       </c>
-      <c r="B3" s="36"/>
-      <c r="C3" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="D3" s="37" t="s">
+      <c r="B3" s="39"/>
+      <c r="C3" s="39" t="s">
+        <v>300</v>
+      </c>
+      <c r="D3" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E3" s="39" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="39"/>
+    </row>
+    <row r="4" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39" t="s">
+        <v>303</v>
+      </c>
+      <c r="D4" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E4" s="39" t="s">
+        <v>304</v>
+      </c>
+      <c r="F4" s="39"/>
+    </row>
+    <row r="5" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>305</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>300</v>
+      </c>
+      <c r="D5" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E5" s="39" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" s="39"/>
+    </row>
+    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="B6" s="39"/>
+      <c r="C6" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E6" s="39" t="n">
+        <v>3</v>
+      </c>
+      <c r="F6" s="39"/>
+    </row>
+    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="39" t="s">
+        <v>306</v>
+      </c>
+      <c r="B7" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="C7" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D7" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="E7" s="39" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" s="39"/>
+    </row>
+    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="39" t="s">
+        <v>310</v>
+      </c>
+      <c r="B8" s="39"/>
+      <c r="C8" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D8" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E8" s="39" t="n">
+        <v>4</v>
+      </c>
+      <c r="F8" s="39"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="39" t="s">
+        <v>310</v>
+      </c>
+      <c r="B9" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="C9" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D9" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="E9" s="39" t="n">
+        <v>13</v>
+      </c>
+      <c r="F9" s="39"/>
+    </row>
+    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="39" t="s">
+        <v>311</v>
+      </c>
+      <c r="B10" s="39"/>
+      <c r="C10" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D10" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="E10" s="39" t="n">
+        <v>5</v>
+      </c>
+      <c r="F10" s="39"/>
+    </row>
+    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D11" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E11" s="39" t="n">
+        <v>5</v>
+      </c>
+      <c r="F11" s="39"/>
+    </row>
+    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B12" s="39"/>
+      <c r="C12" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D12" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E12" s="39" t="n">
+        <v>6</v>
+      </c>
+      <c r="F12" s="39"/>
+    </row>
+    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="39" t="s">
+        <v>312</v>
+      </c>
+      <c r="B13" s="39"/>
+      <c r="C13" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D13" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E13" s="39" t="n">
+        <v>11</v>
+      </c>
+      <c r="F13" s="39"/>
+    </row>
+    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="39" t="s">
+        <v>124</v>
+      </c>
+      <c r="B14" s="39"/>
+      <c r="C14" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D14" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E14" s="39" t="n">
+        <v>14</v>
+      </c>
+      <c r="F14" s="39"/>
+    </row>
+    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B15" s="39"/>
+      <c r="C15" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D15" s="40" t="s">
+        <v>309</v>
+      </c>
+      <c r="E15" s="39" t="n">
+        <v>15</v>
+      </c>
+      <c r="F15" s="39"/>
+    </row>
+    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="39" t="s">
+        <v>135</v>
+      </c>
+      <c r="B16" s="39" t="s">
+        <v>308</v>
+      </c>
+      <c r="C16" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D16" s="40" t="s">
+        <v>313</v>
+      </c>
+      <c r="E16" s="39" t="s">
+        <v>314</v>
+      </c>
+      <c r="F16" s="39"/>
+    </row>
+    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="39" t="s">
+        <v>315</v>
+      </c>
+      <c r="B17" s="39"/>
+      <c r="C17" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D17" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E17" s="39" t="n">
+        <v>15</v>
+      </c>
+      <c r="F17" s="39"/>
+    </row>
+    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="39" t="s">
+        <v>130</v>
+      </c>
+      <c r="B18" s="39"/>
+      <c r="C18" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E18" s="39" t="n">
+        <v>16</v>
+      </c>
+      <c r="F18" s="39"/>
+    </row>
+    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="39" t="s">
+        <v>316</v>
+      </c>
+      <c r="B19" s="39"/>
+      <c r="C19" s="39" t="s">
+        <v>307</v>
+      </c>
+      <c r="D19" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E19" s="39" t="n">
+        <v>40</v>
+      </c>
+      <c r="F19" s="39"/>
+    </row>
+    <row r="20" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="39" t="s">
+        <v>152</v>
+      </c>
+      <c r="B20" s="39"/>
+      <c r="C20" s="39" t="s">
+        <v>317</v>
+      </c>
+      <c r="D20" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E20" s="39" t="s">
+        <v>304</v>
+      </c>
+      <c r="F20" s="39"/>
+    </row>
+    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="C21" s="34" t="s">
+        <v>318</v>
+      </c>
+      <c r="D21" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E21" s="35" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="C22" s="34" t="s">
+        <v>318</v>
+      </c>
+      <c r="D22" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E22" s="35" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="34" t="s">
+        <v>169</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="C23" s="34" t="s">
+        <v>318</v>
+      </c>
+      <c r="D23" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E23" s="35" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="C24" s="34" t="s">
+        <v>318</v>
+      </c>
+      <c r="D24" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E24" s="35" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="C25" s="34" t="s">
+        <v>318</v>
+      </c>
+      <c r="D25" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="34" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="C26" s="34" t="s">
+        <v>318</v>
+      </c>
+      <c r="D26" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E26" s="35" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="C27" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D27" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E27" s="34" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="C28" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D28" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E28" s="34" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="34" t="s">
+        <v>180</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>305</v>
+      </c>
+      <c r="C29" s="34" t="s">
+        <v>324</v>
+      </c>
+      <c r="D29" s="40" t="s">
+        <v>301</v>
+      </c>
+      <c r="E29" s="34" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="34" t="s">
+        <v>38</v>
+      </c>
+      <c r="C30" s="41" t="s">
+        <v>29</v>
+      </c>
+      <c r="D30" s="35" t="s">
+        <v>301</v>
+      </c>
+      <c r="E30" s="34" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="28" t="s">
+        <v>233</v>
+      </c>
+      <c r="C31" s="29" t="s">
         <v>227</v>
       </c>
-      <c r="E3" s="36" t="n">
-        <v>2</v>
-      </c>
-      <c r="F3" s="36"/>
-    </row>
-    <row r="4" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="B4" s="36"/>
-      <c r="C4" s="36" t="s">
-        <v>228</v>
-      </c>
-      <c r="D4" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E4" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="F4" s="36"/>
-    </row>
-    <row r="5" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="36" t="s">
-        <v>164</v>
-      </c>
-      <c r="B5" s="36" t="s">
-        <v>230</v>
-      </c>
-      <c r="C5" s="36" t="s">
-        <v>225</v>
-      </c>
-      <c r="D5" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E5" s="36" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="36"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="36" t="s">
-        <v>231</v>
-      </c>
-      <c r="B6" s="36"/>
-      <c r="C6" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D6" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E6" s="36" t="n">
-        <v>3</v>
-      </c>
-      <c r="F6" s="36"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="36" t="s">
-        <v>231</v>
-      </c>
-      <c r="B7" s="36" t="s">
-        <v>233</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D7" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="E7" s="36" t="n">
-        <v>5</v>
-      </c>
-      <c r="F7" s="36"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="36" t="s">
-        <v>235</v>
-      </c>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D8" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E8" s="36" t="n">
-        <v>4</v>
-      </c>
-      <c r="F8" s="36"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="36" t="s">
-        <v>235</v>
-      </c>
-      <c r="B9" s="36" t="s">
-        <v>233</v>
-      </c>
-      <c r="C9" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D9" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="E9" s="36" t="n">
-        <v>13</v>
-      </c>
-      <c r="F9" s="36"/>
-    </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="36" t="s">
-        <v>236</v>
-      </c>
-      <c r="B10" s="36"/>
-      <c r="C10" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D10" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="E10" s="36" t="n">
-        <v>5</v>
-      </c>
-      <c r="F10" s="36"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="36" t="s">
-        <v>119</v>
-      </c>
-      <c r="B11" s="36"/>
-      <c r="C11" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D11" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E11" s="36" t="n">
-        <v>5</v>
-      </c>
-      <c r="F11" s="36"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="36" t="s">
-        <v>158</v>
-      </c>
-      <c r="B12" s="36"/>
-      <c r="C12" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D12" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E12" s="36" t="n">
-        <v>6</v>
-      </c>
-      <c r="F12" s="36"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="36" t="s">
-        <v>237</v>
-      </c>
-      <c r="B13" s="36"/>
-      <c r="C13" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D13" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E13" s="36" t="n">
-        <v>11</v>
-      </c>
-      <c r="F13" s="36"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="36" t="s">
-        <v>124</v>
-      </c>
-      <c r="B14" s="36"/>
-      <c r="C14" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D14" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E14" s="36" t="n">
-        <v>14</v>
-      </c>
-      <c r="F14" s="36"/>
-    </row>
-    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="B15" s="36"/>
-      <c r="C15" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D15" s="37" t="s">
-        <v>234</v>
-      </c>
-      <c r="E15" s="36" t="n">
-        <v>15</v>
-      </c>
-      <c r="F15" s="36"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="36" t="s">
-        <v>135</v>
-      </c>
-      <c r="B16" s="36" t="s">
-        <v>233</v>
-      </c>
-      <c r="C16" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D16" s="37" t="s">
-        <v>238</v>
-      </c>
-      <c r="E16" s="36" t="s">
-        <v>239</v>
-      </c>
-      <c r="F16" s="36"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="36" t="s">
-        <v>240</v>
-      </c>
-      <c r="B17" s="36"/>
-      <c r="C17" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D17" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E17" s="36" t="n">
-        <v>15</v>
-      </c>
-      <c r="F17" s="36"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="36" t="s">
-        <v>130</v>
-      </c>
-      <c r="B18" s="36"/>
-      <c r="C18" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D18" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E18" s="36" t="n">
-        <v>16</v>
-      </c>
-      <c r="F18" s="36"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="36" t="s">
-        <v>241</v>
-      </c>
-      <c r="B19" s="36"/>
-      <c r="C19" s="36" t="s">
-        <v>232</v>
-      </c>
-      <c r="D19" s="37" t="s">
-        <v>227</v>
-      </c>
-      <c r="E19" s="36" t="n">
-        <v>40</v>
-      </c>
-      <c r="F19" s="36"/>
-    </row>
-    <row r="20" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="36" t="s">
-        <v>152</v>
-      </c>
-      <c r="B20" s="36"/>
-      <c r="C20" s="36" t="s">
-        <v>242</v>
-      </c>
-      <c r="D20" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E20" s="36" t="s">
-        <v>229</v>
-      </c>
-      <c r="F20" s="36"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="C21" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D21" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E21" s="32" t="s">
-        <v>244</v>
-      </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="B22" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="C22" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D22" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E22" s="32" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="B23" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="C23" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D23" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E23" s="32" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="C24" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D24" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E24" s="32" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="B25" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="C25" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D25" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="31" t="s">
-        <v>174</v>
-      </c>
-      <c r="B26" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="C26" s="31" t="s">
-        <v>243</v>
-      </c>
-      <c r="D26" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E26" s="32" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="C27" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="D27" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E27" s="31" t="s">
-        <v>250</v>
-      </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="B28" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="C28" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="D28" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E28" s="31" t="s">
+      <c r="D31" s="42" t="s">
+        <v>301</v>
+      </c>
+      <c r="E31" s="43" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="28" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="31" t="s">
-        <v>180</v>
-      </c>
-      <c r="B29" s="31" t="s">
-        <v>230</v>
-      </c>
-      <c r="C29" s="31" t="s">
-        <v>249</v>
-      </c>
-      <c r="D29" s="37" t="s">
-        <v>226</v>
-      </c>
-      <c r="E29" s="31" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="31" t="s">
-        <v>38</v>
-      </c>
-      <c r="C30" s="38" t="s">
-        <v>29</v>
-      </c>
-      <c r="D30" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="E30" s="31" t="s">
-        <v>229</v>
+      <c r="C32" s="34" t="s">
+        <v>328</v>
+      </c>
+      <c r="D32" s="40" t="s">
+        <v>302</v>
+      </c>
+      <c r="E32" s="34" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -4648,124 +5944,147 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H4"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L15" activeCellId="0" sqref="L15"/>
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.70703125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="36" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="36" width="12.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="36" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="36" width="12.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="36" width="10.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="36" width="12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="36" width="15.43"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="36" width="10.7"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="39" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="39" width="12.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="39" width="13.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="39" width="12.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="6" min="5" style="39" width="10.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="39" width="12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="39" width="15.43"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="39" width="10.7"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="44" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>253</v>
-      </c>
-      <c r="C1" s="39" t="s">
-        <v>254</v>
-      </c>
-      <c r="D1" s="39" t="s">
-        <v>255</v>
-      </c>
-      <c r="E1" s="39" t="s">
-        <v>256</v>
-      </c>
-      <c r="F1" s="39" t="s">
-        <v>257</v>
+      <c r="B1" s="45" t="s">
+        <v>329</v>
+      </c>
+      <c r="C1" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="D1" s="44" t="s">
+        <v>331</v>
+      </c>
+      <c r="E1" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="F1" s="44" t="s">
+        <v>333</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>258</v>
-      </c>
-      <c r="H1" s="39" t="s">
-        <v>259</v>
+        <v>334</v>
+      </c>
+      <c r="H1" s="44" t="s">
+        <v>335</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="36" t="s">
+      <c r="A2" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="36" t="s">
-        <v>260</v>
-      </c>
-      <c r="C2" s="36" t="s">
-        <v>261</v>
-      </c>
-      <c r="D2" s="36" t="s">
-        <v>262</v>
-      </c>
-      <c r="E2" s="41" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="41" t="b">
+      <c r="B2" s="39" t="s">
+        <v>336</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>337</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>338</v>
+      </c>
+      <c r="E2" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="41" t="b">
+      <c r="G2" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="39" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="36" t="s">
-        <v>263</v>
-      </c>
-      <c r="C3" s="36" t="s">
-        <v>264</v>
-      </c>
-      <c r="D3" s="36" t="s">
-        <v>265</v>
-      </c>
-      <c r="E3" s="41" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="41" t="b">
+      <c r="B3" s="39" t="s">
+        <v>339</v>
+      </c>
+      <c r="C3" s="39" t="s">
+        <v>340</v>
+      </c>
+      <c r="D3" s="39" t="s">
+        <v>341</v>
+      </c>
+      <c r="E3" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="41" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="36" t="s">
+      <c r="G3" s="46" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="39" t="s">
         <v>216</v>
       </c>
-      <c r="B4" s="36" t="s">
-        <v>266</v>
-      </c>
-      <c r="C4" s="36" t="s">
-        <v>267</v>
-      </c>
-      <c r="D4" s="36" t="s">
-        <v>268</v>
-      </c>
-      <c r="E4" s="41" t="b">
+      <c r="B4" s="39" t="s">
+        <v>342</v>
+      </c>
+      <c r="C4" s="39" t="s">
+        <v>343</v>
+      </c>
+      <c r="D4" s="39" t="s">
+        <v>344</v>
+      </c>
+      <c r="E4" s="46" t="b">
+        <v>1</v>
+      </c>
+      <c r="F4" s="46" t="b">
+        <v>0</v>
+      </c>
+      <c r="G4" s="46" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="39" t="s">
+        <v>291</v>
+      </c>
+      <c r="B5" s="39" t="s">
+        <v>345</v>
+      </c>
+      <c r="C5" s="39" t="s">
+        <v>346</v>
+      </c>
+      <c r="D5" s="39" t="s">
+        <v>347</v>
+      </c>
+      <c r="E5" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F4" s="41" t="b">
+      <c r="F5" s="46" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="41" t="b">
+      <c r="G5" s="46" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -4786,70 +6105,70 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F51"/>
+  <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A22" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="42" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="42" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="42" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="42" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="42" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="42" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="47" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="47" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="47" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="47" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="5" style="47" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="47" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="43" t="s">
-        <v>269</v>
-      </c>
-      <c r="B1" s="43" t="s">
-        <v>222</v>
-      </c>
-      <c r="C1" s="43" t="s">
+      <c r="A1" s="48" t="s">
+        <v>348</v>
+      </c>
+      <c r="B1" s="48" t="s">
+        <v>297</v>
+      </c>
+      <c r="C1" s="48" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="D1" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="43" t="s">
-        <v>270</v>
-      </c>
-      <c r="F1" s="43" t="s">
+      <c r="E1" s="48" t="s">
+        <v>349</v>
+      </c>
+      <c r="F1" s="48" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>271</v>
+        <v>350</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>272</v>
+        <v>351</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>273</v>
+        <v>352</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>273</v>
+        <v>352</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>274</v>
+        <v>353</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>275</v>
+        <v>354</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -4862,58 +6181,58 @@
         <v>137</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>276</v>
+        <v>355</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>277</v>
+        <v>356</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>278</v>
+        <v>357</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>137</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>279</v>
+        <v>358</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>280</v>
+        <v>359</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>281</v>
+        <v>360</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>281</v>
+        <v>360</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>282</v>
+        <v>361</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>283</v>
+        <v>362</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>284</v>
+        <v>363</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>284</v>
+        <v>363</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>285</v>
+        <v>364</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>286</v>
+        <v>365</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -4926,7 +6245,7 @@
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -4938,7 +6257,7 @@
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1" t="s">
-        <v>273</v>
+        <v>352</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -4962,7 +6281,7 @@
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1" t="s">
-        <v>281</v>
+        <v>360</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -4974,7 +6293,7 @@
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1" t="s">
-        <v>229</v>
+        <v>304</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -4986,7 +6305,7 @@
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1" t="s">
-        <v>273</v>
+        <v>352</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -4998,7 +6317,7 @@
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1" t="s">
-        <v>284</v>
+        <v>363</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -5007,13 +6326,13 @@
         <v>116</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>287</v>
+        <v>366</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>288</v>
+        <v>367</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>289</v>
+        <v>368</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -5023,13 +6342,13 @@
         <v>116</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>290</v>
+        <v>369</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>291</v>
+        <v>370</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>292</v>
+        <v>371</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -5042,7 +6361,7 @@
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1" t="s">
-        <v>284</v>
+        <v>363</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -5051,13 +6370,13 @@
         <v>125</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>293</v>
+        <v>372</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>294</v>
+        <v>373</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>295</v>
+        <v>374</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -5067,13 +6386,13 @@
         <v>125</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>296</v>
+        <v>375</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>297</v>
+        <v>376</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>298</v>
+        <v>377</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -5086,7 +6405,7 @@
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1" t="s">
-        <v>273</v>
+        <v>352</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -5095,17 +6414,17 @@
         <v>132</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>299</v>
+        <v>378</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>300</v>
+        <v>379</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>301</v>
+        <v>380</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1" t="s">
-        <v>236</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5113,17 +6432,17 @@
         <v>132</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>302</v>
+        <v>381</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>303</v>
+        <v>382</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>304</v>
+        <v>383</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1" t="s">
-        <v>235</v>
+        <v>310</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5131,17 +6450,17 @@
         <v>132</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>305</v>
+        <v>384</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>306</v>
+        <v>385</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>307</v>
+        <v>386</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1" t="s">
-        <v>237</v>
+        <v>312</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5149,13 +6468,13 @@
         <v>132</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>308</v>
+        <v>387</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>309</v>
+        <v>388</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>310</v>
+        <v>389</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -5165,17 +6484,17 @@
         <v>132</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>311</v>
+        <v>390</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>312</v>
+        <v>391</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>313</v>
+        <v>392</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1" t="s">
-        <v>240</v>
+        <v>315</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5195,13 +6514,13 @@
         <v>138</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>244</v>
+        <v>319</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>314</v>
+        <v>393</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>315</v>
+        <v>394</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
@@ -5211,13 +6530,13 @@
         <v>138</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>245</v>
+        <v>320</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>316</v>
+        <v>395</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>317</v>
+        <v>396</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -5227,13 +6546,13 @@
         <v>138</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>246</v>
+        <v>321</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>318</v>
+        <v>397</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>319</v>
+        <v>398</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -5243,13 +6562,13 @@
         <v>138</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>247</v>
+        <v>322</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>320</v>
+        <v>399</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>321</v>
+        <v>400</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -5259,13 +6578,13 @@
         <v>138</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>248</v>
+        <v>323</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>322</v>
+        <v>401</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>323</v>
+        <v>402</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -5275,17 +6594,17 @@
         <v>138</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>324</v>
+        <v>403</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>325</v>
+        <v>404</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>326</v>
+        <v>405</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1" t="s">
-        <v>241</v>
+        <v>316</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5293,13 +6612,13 @@
         <v>138</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>327</v>
+        <v>406</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>328</v>
+        <v>407</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>329</v>
+        <v>408</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -5309,13 +6628,13 @@
         <v>138</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>330</v>
+        <v>409</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>331</v>
+        <v>410</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>332</v>
+        <v>411</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -5325,13 +6644,13 @@
         <v>138</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>333</v>
+        <v>412</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>334</v>
+        <v>413</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>335</v>
+        <v>414</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -5341,13 +6660,13 @@
         <v>138</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>336</v>
+        <v>415</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>337</v>
+        <v>416</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>338</v>
+        <v>417</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -5357,13 +6676,13 @@
         <v>138</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>339</v>
+        <v>418</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>340</v>
+        <v>419</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>341</v>
+        <v>420</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -5376,10 +6695,10 @@
         <v>137</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>279</v>
+        <v>358</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>280</v>
+        <v>359</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -5389,13 +6708,13 @@
         <v>138</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>342</v>
+        <v>421</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>343</v>
+        <v>422</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>344</v>
+        <v>423</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -5408,7 +6727,7 @@
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1" t="s">
-        <v>273</v>
+        <v>352</v>
       </c>
       <c r="F40" s="1"/>
     </row>
@@ -5417,13 +6736,13 @@
         <v>159</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>345</v>
+        <v>424</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>346</v>
+        <v>425</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>347</v>
+        <v>426</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -5433,13 +6752,13 @@
         <v>159</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>348</v>
+        <v>427</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>349</v>
+        <v>428</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>350</v>
+        <v>429</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -5452,7 +6771,7 @@
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
       <c r="E43" s="1" t="s">
-        <v>281</v>
+        <v>360</v>
       </c>
       <c r="F43" s="1"/>
     </row>
@@ -5461,13 +6780,13 @@
         <v>166</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>250</v>
+        <v>325</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>351</v>
+        <v>430</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>352</v>
+        <v>431</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -5477,13 +6796,13 @@
         <v>166</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>251</v>
+        <v>326</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>353</v>
+        <v>432</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>354</v>
+        <v>433</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -5493,13 +6812,13 @@
         <v>166</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>252</v>
+        <v>327</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>355</v>
+        <v>434</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>356</v>
+        <v>435</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -5509,13 +6828,13 @@
         <v>166</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>357</v>
+        <v>436</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>358</v>
+        <v>437</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>359</v>
+        <v>438</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -5525,59 +6844,327 @@
         <v>166</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>360</v>
+        <v>439</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>361</v>
+        <v>440</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>362</v>
+        <v>441</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
     </row>
     <row r="49" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="42" t="s">
+      <c r="A49" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="B49" s="42" t="s">
-        <v>250</v>
-      </c>
-      <c r="C49" s="42" t="s">
-        <v>363</v>
-      </c>
-      <c r="D49" s="42" t="s">
-        <v>352</v>
+      <c r="B49" s="47" t="s">
+        <v>325</v>
+      </c>
+      <c r="C49" s="47" t="s">
+        <v>442</v>
+      </c>
+      <c r="D49" s="47" t="s">
+        <v>431</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="42" t="s">
+      <c r="A50" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="B50" s="42" t="s">
-        <v>251</v>
-      </c>
-      <c r="C50" s="42" t="s">
+      <c r="B50" s="47" t="s">
+        <v>326</v>
+      </c>
+      <c r="C50" s="47" t="s">
+        <v>443</v>
+      </c>
+      <c r="D50" s="47" t="s">
+        <v>444</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="47" t="s">
+        <v>175</v>
+      </c>
+      <c r="B51" s="47" t="s">
+        <v>439</v>
+      </c>
+      <c r="C51" s="47" t="s">
+        <v>445</v>
+      </c>
+      <c r="D51" s="47" t="s">
+        <v>446</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B52" s="47" t="s">
+        <v>447</v>
+      </c>
+      <c r="C52" s="47" t="s">
+        <v>448</v>
+      </c>
+      <c r="D52" s="47" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B53" s="29" t="s">
+        <v>450</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>451</v>
+      </c>
+      <c r="D53" s="29" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B54" s="29" t="s">
+        <v>453</v>
+      </c>
+      <c r="C54" s="29" t="s">
+        <v>454</v>
+      </c>
+      <c r="D54" s="29" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B55" s="29" t="s">
+        <v>456</v>
+      </c>
+      <c r="C55" s="29" t="s">
+        <v>457</v>
+      </c>
+      <c r="D55" s="29" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B56" s="29" t="s">
+        <v>459</v>
+      </c>
+      <c r="C56" s="29" t="s">
+        <v>460</v>
+      </c>
+      <c r="D56" s="29" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B57" s="29" t="s">
+        <v>462</v>
+      </c>
+      <c r="C57" s="29" t="s">
+        <v>463</v>
+      </c>
+      <c r="D57" s="29" t="s">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B58" s="29" t="s">
+        <v>465</v>
+      </c>
+      <c r="C58" s="29" t="s">
+        <v>466</v>
+      </c>
+      <c r="D58" s="29" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B59" s="29" t="s">
+        <v>468</v>
+      </c>
+      <c r="C59" s="29" t="s">
+        <v>469</v>
+      </c>
+      <c r="D59" s="29" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B60" s="29" t="s">
+        <v>471</v>
+      </c>
+      <c r="C60" s="29" t="s">
+        <v>472</v>
+      </c>
+      <c r="D60" s="29" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B61" s="29" t="s">
+        <v>474</v>
+      </c>
+      <c r="C61" s="29" t="s">
+        <v>475</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B62" s="29" t="s">
+        <v>477</v>
+      </c>
+      <c r="C62" s="29" t="s">
+        <v>478</v>
+      </c>
+      <c r="D62" s="29" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B63" s="29" t="s">
+        <v>480</v>
+      </c>
+      <c r="C63" s="29" t="s">
+        <v>481</v>
+      </c>
+      <c r="D63" s="29" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B64" s="47" t="s">
+        <v>483</v>
+      </c>
+      <c r="C64" s="47" t="s">
+        <v>484</v>
+      </c>
+      <c r="D64" s="47" t="s">
+        <v>485</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B65" s="47" t="s">
+        <v>360</v>
+      </c>
+      <c r="C65" s="47" t="s">
+        <v>361</v>
+      </c>
+      <c r="D65" s="47" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="47" t="s">
+        <v>226</v>
+      </c>
+      <c r="B66" s="47" t="s">
+        <v>486</v>
+      </c>
+      <c r="C66" s="47" t="s">
         <v>364</v>
       </c>
-      <c r="D50" s="42" t="s">
-        <v>365</v>
-      </c>
-    </row>
-    <row r="51" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="42" t="s">
-        <v>175</v>
-      </c>
-      <c r="B51" s="42" t="s">
-        <v>360</v>
-      </c>
-      <c r="C51" s="42" t="s">
-        <v>366</v>
-      </c>
-      <c r="D51" s="42" t="s">
-        <v>367</v>
-      </c>
-    </row>
+      <c r="D66" s="47" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="B67" s="29" t="s">
+        <v>488</v>
+      </c>
+      <c r="C67" s="47" t="s">
+        <v>489</v>
+      </c>
+      <c r="D67" s="47" t="s">
+        <v>490</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="B68" s="47" t="s">
+        <v>491</v>
+      </c>
+      <c r="C68" s="47" t="s">
+        <v>492</v>
+      </c>
+      <c r="D68" s="47" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="B69" s="47" t="s">
+        <v>137</v>
+      </c>
+      <c r="C69" s="47" t="s">
+        <v>358</v>
+      </c>
+      <c r="D69" s="47" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="49" t="s">
+        <v>220</v>
+      </c>
+      <c r="B70" s="47" t="s">
+        <v>421</v>
+      </c>
+      <c r="C70" s="29" t="s">
+        <v>364</v>
+      </c>
+      <c r="D70" s="29" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -5594,62 +7181,214 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L1"/>
+  <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="31" width="18.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="31" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="31" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="31" width="12.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="31" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="31" width="13.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="31" width="14.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="31" width="11.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="31" width="13.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="31" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="34" width="18.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="34" width="17.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="34" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="34" width="12.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="34" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="34" width="13.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="34" width="14.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="34" width="11.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="34" width="13.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="34" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="43" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="44" t="s">
-        <v>368</v>
-      </c>
-      <c r="B1" s="44" t="s">
-        <v>369</v>
-      </c>
-      <c r="C1" s="44" t="s">
-        <v>370</v>
-      </c>
-      <c r="D1" s="44" t="s">
-        <v>371</v>
-      </c>
-      <c r="E1" s="44" t="s">
-        <v>372</v>
-      </c>
-      <c r="F1" s="44" t="s">
-        <v>373</v>
-      </c>
-      <c r="G1" s="44" t="s">
-        <v>374</v>
-      </c>
-      <c r="H1" s="44" t="s">
-        <v>375</v>
-      </c>
-      <c r="I1" s="44" t="s">
-        <v>376</v>
-      </c>
-      <c r="J1" s="44" t="s">
-        <v>377</v>
-      </c>
-      <c r="K1" s="44" t="s">
-        <v>378</v>
-      </c>
-      <c r="L1" s="43" t="s">
-        <v>379</v>
+    <row r="1" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="50" t="s">
+        <v>494</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>495</v>
+      </c>
+      <c r="C1" s="50" t="s">
+        <v>496</v>
+      </c>
+      <c r="D1" s="50" t="s">
+        <v>497</v>
+      </c>
+      <c r="E1" s="50" t="s">
+        <v>498</v>
+      </c>
+      <c r="F1" s="50" t="s">
+        <v>499</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>500</v>
+      </c>
+      <c r="H1" s="50" t="s">
+        <v>501</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>502</v>
+      </c>
+      <c r="J1" s="50" t="s">
+        <v>503</v>
+      </c>
+      <c r="K1" s="50" t="s">
+        <v>504</v>
+      </c>
+      <c r="L1" s="48" t="s">
+        <v>505</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="30" t="s">
+        <v>263</v>
+      </c>
+      <c r="B2" s="30" t="s">
+        <v>506</v>
+      </c>
+      <c r="C2" s="30" t="s">
+        <v>507</v>
+      </c>
+      <c r="D2" s="30" t="s">
+        <v>508</v>
+      </c>
+      <c r="E2" s="30" t="s">
+        <v>509</v>
+      </c>
+      <c r="F2" s="30" t="s">
+        <v>510</v>
+      </c>
+      <c r="G2" s="30" t="s">
+        <v>511</v>
+      </c>
+      <c r="H2" s="30" t="n">
+        <v>-10</v>
+      </c>
+      <c r="I2" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="J2" s="30" t="s">
+        <v>512</v>
+      </c>
+      <c r="K2" s="30" t="s">
+        <v>512</v>
+      </c>
+      <c r="L2" s="30" t="s">
+        <v>513</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="B3" s="30" t="s">
+        <v>514</v>
+      </c>
+      <c r="C3" s="30" t="s">
+        <v>515</v>
+      </c>
+      <c r="D3" s="51" t="s">
+        <v>516</v>
+      </c>
+      <c r="E3" s="51" t="s">
+        <v>517</v>
+      </c>
+      <c r="F3" s="51" t="s">
+        <v>518</v>
+      </c>
+      <c r="G3" s="30" t="s">
+        <v>519</v>
+      </c>
+      <c r="H3" s="30" t="n">
+        <v>-10</v>
+      </c>
+      <c r="I3" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="J3" s="30" t="s">
+        <v>512</v>
+      </c>
+      <c r="K3" s="30" t="s">
+        <v>512</v>
+      </c>
+      <c r="L3" s="30" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="30" t="s">
+        <v>277</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>521</v>
+      </c>
+      <c r="C4" s="30" t="s">
+        <v>522</v>
+      </c>
+      <c r="D4" s="30" t="s">
+        <v>523</v>
+      </c>
+      <c r="E4" s="30" t="s">
+        <v>524</v>
+      </c>
+      <c r="F4" s="30" t="s">
+        <v>525</v>
+      </c>
+      <c r="G4" s="30" t="s">
+        <v>526</v>
+      </c>
+      <c r="H4" s="30" t="n">
+        <v>-10</v>
+      </c>
+      <c r="I4" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="J4" s="30" t="s">
+        <v>512</v>
+      </c>
+      <c r="K4" s="30" t="s">
+        <v>512</v>
+      </c>
+      <c r="L4" s="30" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="30" t="s">
+        <v>282</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>514</v>
+      </c>
+      <c r="C5" s="30" t="s">
+        <v>528</v>
+      </c>
+      <c r="D5" s="30" t="s">
+        <v>529</v>
+      </c>
+      <c r="E5" s="30" t="s">
+        <v>517</v>
+      </c>
+      <c r="F5" s="30" t="s">
+        <v>530</v>
+      </c>
+      <c r="G5" s="30" t="s">
+        <v>531</v>
+      </c>
+      <c r="H5" s="30" t="n">
+        <v>-10</v>
+      </c>
+      <c r="I5" s="30" t="n">
+        <v>100</v>
+      </c>
+      <c r="J5" s="30" t="s">
+        <v>512</v>
+      </c>
+      <c r="K5" s="30" t="s">
+        <v>512</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>527</v>
       </c>
     </row>
   </sheetData>
@@ -5677,20 +7416,20 @@
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="31" t="s">
-        <v>380</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>381</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>382</v>
-      </c>
-      <c r="D1" s="31" t="s">
-        <v>383</v>
-      </c>
-      <c r="E1" s="31" t="s">
-        <v>384</v>
+      <c r="A1" s="34" t="s">
+        <v>532</v>
+      </c>
+      <c r="B1" s="34" t="s">
+        <v>533</v>
+      </c>
+      <c r="C1" s="34" t="s">
+        <v>534</v>
+      </c>
+      <c r="D1" s="34" t="s">
+        <v>535</v>
+      </c>
+      <c r="E1" s="34" t="s">
+        <v>536</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
household: Rename `drivingLicenseOwner` to `drivingLicenseOwnership`
fixes #62

This is the name of the corresponding person attribute in Evolution, so
we should use this one.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -499,10 +499,10 @@
     <t xml:space="preserve">personOccupationCustomConditional</t>
   </si>
   <si>
-    <t xml:space="preserve">personDrivingLicenseOwner</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drivingLicenseOwner</t>
+    <t xml:space="preserve">personDrivingLicenseOwnership</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drivingLicenseOwnership</t>
   </si>
   <si>
     <t xml:space="preserve">**Permis de conduire**
@@ -1928,7 +1928,7 @@
     <t xml:space="preserve">ifAge40OrMoreConditional</t>
   </si>
   <si>
-    <t xml:space="preserve">${currentPerson}.drivingLicenseOwner</t>
+    <t xml:space="preserve">${currentPerson}.drivingLicenseOwnership</t>
   </si>
   <si>
     <t xml:space="preserve">${currentPerson}.occupation</t>
@@ -3807,10 +3807,10 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K102" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="J98" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A102" activeCellId="0" sqref="A102"/>
+      <selection pane="topRight" activeCell="J1" activeCellId="0" sqref="J1"/>
+      <selection pane="bottomLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
       <selection pane="bottomRight" activeCell="T106" activeCellId="0" sqref="T106"/>
     </sheetView>
   </sheetViews>
@@ -9877,8 +9877,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A37" activeCellId="0" sqref="A37"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10257,7 +10257,7 @@
       </c>
       <c r="F22" s="30"/>
     </row>
-    <row r="23" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="30" t="s">
         <v>155</v>
       </c>
@@ -12668,7 +12668,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
household: fix `fullTime` and `partTime` values
fixes #80

These are the values expected by Evolution, excluding the `yes`. Also
update the `personOccupationCustomConditional` to increase type
validation at compile time.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -2123,7 +2123,7 @@
     <t xml:space="preserve">Woman</t>
   </si>
   <si>
-    <t xml:space="preserve">yesFullTime</t>
+    <t xml:space="preserve">fullTime</t>
   </si>
   <si>
     <t xml:space="preserve">Oui, à temps plein</t>
@@ -2132,7 +2132,7 @@
     <t xml:space="preserve">Yes, full time</t>
   </si>
   <si>
-    <t xml:space="preserve">yesPartTime</t>
+    <t xml:space="preserve">partTime</t>
   </si>
   <si>
     <t xml:space="preserve">Oui, à temps partiel</t>
@@ -3785,12 +3785,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="D83" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
-      <selection pane="bottomRight" activeCell="A101" activeCellId="0" sqref="A101:A102"/>
+      <selection pane="bottomRight" activeCell="H104" activeCellId="0" sqref="H104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8796,6 +8796,7 @@
       <c r="R105" s="30"/>
       <c r="S105" s="30"/>
       <c r="T105" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="U105" s="30"/>
@@ -8930,7 +8931,7 @@
       <c r="J108" s="24" t="s">
         <v>483</v>
       </c>
-      <c r="K108" s="0"/>
+      <c r="K108" s="2"/>
       <c r="L108" s="30"/>
       <c r="M108" s="30" t="s">
         <v>484</v>
@@ -8944,6 +8945,7 @@
       <c r="R108" s="30"/>
       <c r="S108" s="30"/>
       <c r="T108" s="13" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="U108" s="30"/>
@@ -9860,7 +9862,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="1" sqref="A101:A102 A30"/>
+      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10478,7 +10480,7 @@
   <dimension ref="A1:H11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="1" sqref="A101:A102 A5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10809,8 +10811,8 @@
   </sheetPr>
   <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B50" activeCellId="1" sqref="A101:A102 B50"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12424,7 +12426,7 @@
   <dimension ref="A1:L5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F4" activeCellId="1" sqref="A101:A102 F4"/>
+      <selection pane="topLeft" activeCell="F4" activeCellId="0" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12650,7 +12652,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C29" activeCellId="1" sqref="A101:A102 C29"/>
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
household: hide the work and study occupations from choices
Prepares #28, who will automatically be fixed in the next Evolution
update.

Also change the `sickOrParentalLeave` to `parentalOrSickLeave`, the
value that Evolution expects.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1641" uniqueCount="920">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1647" uniqueCount="922">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -2057,6 +2057,9 @@
     <t xml:space="preserve">spreadChoicesName</t>
   </si>
   <si>
+    <t xml:space="preserve">hidden</t>
+  </si>
+  <si>
     <t xml:space="preserve">Oui</t>
   </si>
   <si>
@@ -2192,6 +2195,9 @@
     <t xml:space="preserve">Employed full-time (30h and more/week)</t>
   </si>
   <si>
+    <t xml:space="preserve">True</t>
+  </si>
+  <si>
     <t xml:space="preserve">Travail à temps partiel (moins de 30h/semaine)</t>
   </si>
   <si>
@@ -2243,7 +2249,7 @@
     <t xml:space="preserve">Unemployed / searching for a job</t>
   </si>
   <si>
-    <t xml:space="preserve">sickOrParentalLeave</t>
+    <t xml:space="preserve">parentalOrSickLeave</t>
   </si>
   <si>
     <t xml:space="preserve">Congé de maladie ou congé parental</t>
@@ -3170,7 +3176,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="60">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -3389,6 +3395,10 @@
     </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -3786,11 +3796,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D83" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="H17" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
-      <selection pane="bottomRight" activeCell="H104" activeCellId="0" sqref="H104"/>
+      <selection pane="topRight" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="A17" activeCellId="0" sqref="A17"/>
+      <selection pane="bottomRight" activeCell="O26" activeCellId="0" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9861,8 +9871,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10457,6 +10467,8 @@
         <v>599</v>
       </c>
     </row>
+    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -10809,10 +10821,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H1048576"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B20" activeCellId="0" sqref="B20"/>
+      <selection pane="topLeft" activeCell="I32" activeCellId="0" sqref="I32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10825,7 +10837,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="50" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="54" t="s">
         <v>637</v>
       </c>
@@ -10849,6 +10861,9 @@
       </c>
       <c r="H1" s="54" t="s">
         <v>12</v>
+      </c>
+      <c r="I1" s="50" t="s">
+        <v>639</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10859,10 +10874,10 @@
         <v>574</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>639</v>
+        <v>640</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>640</v>
+        <v>641</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -10871,16 +10886,16 @@
     </row>
     <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -10895,10 +10910,10 @@
         <v>140</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>644</v>
+        <v>645</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>645</v>
+        <v>646</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
@@ -10907,16 +10922,16 @@
     </row>
     <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>140</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
@@ -10925,16 +10940,16 @@
     </row>
     <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -10943,16 +10958,16 @@
     </row>
     <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>654</v>
+        <v>655</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -10983,7 +10998,7 @@
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -11011,7 +11026,7 @@
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -11039,7 +11054,7 @@
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -11053,7 +11068,7 @@
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -11062,13 +11077,13 @@
         <v>119</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>655</v>
+        <v>656</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>656</v>
+        <v>657</v>
       </c>
       <c r="D15" s="1" t="s">
-        <v>657</v>
+        <v>658</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
@@ -11080,13 +11095,13 @@
         <v>119</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>658</v>
+        <v>659</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>659</v>
+        <v>660</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>660</v>
+        <v>661</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
@@ -11103,7 +11118,7 @@
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1" t="s">
-        <v>652</v>
+        <v>653</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -11112,13 +11127,13 @@
         <v>128</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>661</v>
+        <v>662</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>662</v>
+        <v>663</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>663</v>
+        <v>664</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -11130,13 +11145,13 @@
         <v>128</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>664</v>
+        <v>665</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>665</v>
+        <v>666</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>666</v>
+        <v>667</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -11153,7 +11168,7 @@
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -11162,13 +11177,13 @@
         <v>135</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>667</v>
+        <v>668</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>668</v>
+        <v>669</v>
       </c>
       <c r="D21" s="1" t="s">
-        <v>669</v>
+        <v>670</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
@@ -11182,13 +11197,13 @@
         <v>135</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>670</v>
+        <v>671</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>671</v>
+        <v>672</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -11202,13 +11217,13 @@
         <v>135</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -11222,13 +11237,13 @@
         <v>135</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
       <c r="D24" s="1" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
       <c r="E24" s="1"/>
       <c r="F24" s="1"/>
@@ -11240,13 +11255,13 @@
         <v>135</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>681</v>
+        <v>682</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -11277,15 +11292,18 @@
         <v>591</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
       <c r="D27" s="1" t="s">
-        <v>683</v>
+        <v>684</v>
       </c>
       <c r="E27" s="1"/>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
+      <c r="I27" s="50" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
@@ -11295,15 +11313,18 @@
         <v>592</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>684</v>
+        <v>686</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
+      <c r="I28" s="50" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
@@ -11313,15 +11334,18 @@
         <v>593</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
+      <c r="I29" s="50" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
@@ -11331,15 +11355,18 @@
         <v>594</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
+      <c r="I30" s="50" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
@@ -11349,28 +11376,31 @@
         <v>595</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>690</v>
+        <v>692</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>691</v>
+        <v>693</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
+      <c r="I31" s="50" t="s">
+        <v>685</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>141</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>692</v>
+        <v>694</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>693</v>
+        <v>695</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>694</v>
+        <v>696</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -11384,13 +11414,13 @@
         <v>141</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>695</v>
+        <v>697</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>696</v>
+        <v>698</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>697</v>
+        <v>699</v>
       </c>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
@@ -11402,13 +11432,13 @@
         <v>141</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>698</v>
+        <v>700</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>699</v>
+        <v>701</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>700</v>
+        <v>702</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
@@ -11419,14 +11449,14 @@
       <c r="A35" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="B35" s="1" t="s">
-        <v>701</v>
+      <c r="B35" s="55" t="s">
+        <v>703</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>702</v>
+        <v>704</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>703</v>
+        <v>705</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
@@ -11438,13 +11468,13 @@
         <v>141</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>704</v>
+        <v>706</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>705</v>
+        <v>707</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>706</v>
+        <v>708</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
@@ -11456,13 +11486,13 @@
         <v>141</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>707</v>
+        <v>709</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>708</v>
+        <v>710</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>709</v>
+        <v>711</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
@@ -11477,10 +11507,10 @@
         <v>140</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
@@ -11492,13 +11522,13 @@
         <v>141</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>711</v>
+        <v>713</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>712</v>
+        <v>714</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -11515,7 +11545,7 @@
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="H40" s="1"/>
     </row>
@@ -11524,13 +11554,13 @@
         <v>162</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>714</v>
+        <v>716</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -11542,13 +11572,13 @@
         <v>162</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -11565,7 +11595,7 @@
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -11577,10 +11607,10 @@
         <v>597</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -11595,10 +11625,10 @@
         <v>598</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>722</v>
+        <v>724</v>
       </c>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
@@ -11613,10 +11643,10 @@
         <v>599</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>723</v>
+        <v>725</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>724</v>
+        <v>726</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -11628,13 +11658,13 @@
         <v>173</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>725</v>
+        <v>727</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>726</v>
+        <v>728</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>727</v>
+        <v>729</v>
       </c>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
@@ -11646,13 +11676,13 @@
         <v>173</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>729</v>
+        <v>731</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>730</v>
+        <v>732</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -11667,10 +11697,10 @@
         <v>597</v>
       </c>
       <c r="C49" s="50" t="s">
-        <v>731</v>
+        <v>733</v>
       </c>
       <c r="D49" s="50" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11681,10 +11711,10 @@
         <v>598</v>
       </c>
       <c r="C50" s="50" t="s">
-        <v>732</v>
+        <v>734</v>
       </c>
       <c r="D50" s="50" t="s">
-        <v>733</v>
+        <v>735</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -11692,13 +11722,13 @@
         <v>179</v>
       </c>
       <c r="B51" s="50" t="s">
-        <v>728</v>
+        <v>730</v>
       </c>
       <c r="C51" s="50" t="s">
-        <v>734</v>
+        <v>736</v>
       </c>
       <c r="D51" s="50" t="s">
-        <v>735</v>
+        <v>737</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11706,13 +11736,13 @@
         <v>497</v>
       </c>
       <c r="B52" s="50" t="s">
-        <v>736</v>
+        <v>738</v>
       </c>
       <c r="C52" s="50" t="s">
-        <v>737</v>
+        <v>739</v>
       </c>
       <c r="D52" s="50" t="s">
-        <v>738</v>
+        <v>740</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11720,13 +11750,13 @@
         <v>497</v>
       </c>
       <c r="B53" s="24" t="s">
-        <v>739</v>
+        <v>741</v>
       </c>
       <c r="C53" s="24" t="s">
-        <v>740</v>
+        <v>742</v>
       </c>
       <c r="D53" s="24" t="s">
-        <v>741</v>
+        <v>743</v>
       </c>
       <c r="E53" s="24"/>
       <c r="F53" s="24"/>
@@ -11736,13 +11766,13 @@
         <v>497</v>
       </c>
       <c r="B54" s="24" t="s">
-        <v>742</v>
+        <v>744</v>
       </c>
       <c r="C54" s="24" t="s">
-        <v>743</v>
+        <v>745</v>
       </c>
       <c r="D54" s="24" t="s">
-        <v>744</v>
+        <v>746</v>
       </c>
       <c r="E54" s="24"/>
       <c r="F54" s="24"/>
@@ -11752,13 +11782,13 @@
         <v>497</v>
       </c>
       <c r="B55" s="24" t="s">
-        <v>745</v>
+        <v>747</v>
       </c>
       <c r="C55" s="24" t="s">
-        <v>746</v>
+        <v>748</v>
       </c>
       <c r="D55" s="24" t="s">
-        <v>747</v>
+        <v>749</v>
       </c>
       <c r="E55" s="24"/>
       <c r="F55" s="24"/>
@@ -11768,13 +11798,13 @@
         <v>497</v>
       </c>
       <c r="B56" s="24" t="s">
-        <v>748</v>
+        <v>750</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>749</v>
+        <v>751</v>
       </c>
       <c r="D56" s="24" t="s">
-        <v>750</v>
+        <v>752</v>
       </c>
       <c r="E56" s="24"/>
       <c r="F56" s="24"/>
@@ -11784,13 +11814,13 @@
         <v>497</v>
       </c>
       <c r="B57" s="24" t="s">
-        <v>751</v>
+        <v>753</v>
       </c>
       <c r="C57" s="24" t="s">
-        <v>752</v>
+        <v>754</v>
       </c>
       <c r="D57" s="24" t="s">
-        <v>753</v>
+        <v>755</v>
       </c>
       <c r="E57" s="24"/>
       <c r="F57" s="24"/>
@@ -11800,13 +11830,13 @@
         <v>497</v>
       </c>
       <c r="B58" s="24" t="s">
-        <v>754</v>
+        <v>756</v>
       </c>
       <c r="C58" s="24" t="s">
-        <v>755</v>
+        <v>757</v>
       </c>
       <c r="D58" s="24" t="s">
-        <v>756</v>
+        <v>758</v>
       </c>
       <c r="E58" s="24"/>
       <c r="F58" s="24"/>
@@ -11816,13 +11846,13 @@
         <v>497</v>
       </c>
       <c r="B59" s="24" t="s">
-        <v>757</v>
+        <v>759</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>758</v>
+        <v>760</v>
       </c>
       <c r="D59" s="24" t="s">
-        <v>759</v>
+        <v>761</v>
       </c>
       <c r="E59" s="24"/>
       <c r="F59" s="24"/>
@@ -11832,13 +11862,13 @@
         <v>497</v>
       </c>
       <c r="B60" s="24" t="s">
-        <v>760</v>
+        <v>762</v>
       </c>
       <c r="C60" s="24" t="s">
-        <v>761</v>
+        <v>763</v>
       </c>
       <c r="D60" s="24" t="s">
-        <v>762</v>
+        <v>764</v>
       </c>
       <c r="E60" s="24"/>
       <c r="F60" s="24"/>
@@ -11848,13 +11878,13 @@
         <v>497</v>
       </c>
       <c r="B61" s="24" t="s">
-        <v>763</v>
+        <v>765</v>
       </c>
       <c r="C61" s="24" t="s">
-        <v>764</v>
+        <v>766</v>
       </c>
       <c r="D61" s="24" t="s">
-        <v>765</v>
+        <v>767</v>
       </c>
       <c r="E61" s="24"/>
       <c r="F61" s="24"/>
@@ -11864,13 +11894,13 @@
         <v>497</v>
       </c>
       <c r="B62" s="24" t="s">
-        <v>766</v>
+        <v>768</v>
       </c>
       <c r="C62" s="24" t="s">
-        <v>767</v>
+        <v>769</v>
       </c>
       <c r="D62" s="24" t="s">
-        <v>768</v>
+        <v>770</v>
       </c>
       <c r="E62" s="24"/>
       <c r="F62" s="24"/>
@@ -11880,13 +11910,13 @@
         <v>497</v>
       </c>
       <c r="B63" s="24" t="s">
-        <v>769</v>
+        <v>771</v>
       </c>
       <c r="C63" s="24" t="s">
-        <v>770</v>
+        <v>772</v>
       </c>
       <c r="D63" s="24" t="s">
-        <v>771</v>
+        <v>773</v>
       </c>
       <c r="E63" s="24"/>
       <c r="F63" s="24"/>
@@ -11896,13 +11926,13 @@
         <v>497</v>
       </c>
       <c r="B64" s="50" t="s">
-        <v>772</v>
+        <v>774</v>
       </c>
       <c r="C64" s="50" t="s">
-        <v>773</v>
+        <v>775</v>
       </c>
       <c r="D64" s="50" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11910,13 +11940,13 @@
         <v>497</v>
       </c>
       <c r="B65" s="50" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
       <c r="C65" s="50" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D65" s="50" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -11924,69 +11954,69 @@
         <v>497</v>
       </c>
       <c r="B66" s="50" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="C66" s="50" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D66" s="50" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="55" t="s">
+      <c r="A67" s="56" t="s">
         <v>492</v>
       </c>
       <c r="B67" s="24" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="C67" s="50" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="D67" s="50" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="55" t="s">
+      <c r="A68" s="56" t="s">
         <v>492</v>
       </c>
       <c r="B68" s="50" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="C68" s="50" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="D68" s="50" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="55" t="s">
+      <c r="A69" s="56" t="s">
         <v>492</v>
       </c>
       <c r="B69" s="50" t="s">
         <v>140</v>
       </c>
       <c r="C69" s="50" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D69" s="50" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="55" t="s">
+      <c r="A70" s="56" t="s">
         <v>492</v>
       </c>
       <c r="B70" s="50" t="s">
-        <v>710</v>
+        <v>712</v>
       </c>
       <c r="C70" s="24" t="s">
-        <v>653</v>
+        <v>654</v>
       </c>
       <c r="D70" s="24" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="E70" s="24"/>
       <c r="F70" s="24"/>
@@ -11996,13 +12026,13 @@
         <v>271</v>
       </c>
       <c r="B71" s="50" t="s">
-        <v>783</v>
-      </c>
-      <c r="C71" s="56" t="s">
-        <v>784</v>
+        <v>785</v>
+      </c>
+      <c r="C71" s="57" t="s">
+        <v>786</v>
       </c>
       <c r="D71" s="50" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="H71" s="24" t="s">
         <v>587</v>
@@ -12013,16 +12043,16 @@
         <v>271</v>
       </c>
       <c r="B72" s="50" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="C72" s="24" t="s">
-        <v>787</v>
-      </c>
-      <c r="D72" s="56" t="s">
-        <v>788</v>
-      </c>
-      <c r="E72" s="56"/>
-      <c r="F72" s="56"/>
+        <v>789</v>
+      </c>
+      <c r="D72" s="57" t="s">
+        <v>790</v>
+      </c>
+      <c r="E72" s="57"/>
+      <c r="F72" s="57"/>
       <c r="H72" s="2" t="s">
         <v>172</v>
       </c>
@@ -12032,13 +12062,13 @@
         <v>271</v>
       </c>
       <c r="B73" s="50" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="C73" s="24" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="D73" s="50" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12046,13 +12076,13 @@
         <v>271</v>
       </c>
       <c r="B74" s="50" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="C74" s="24" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="D74" s="24" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="E74" s="24"/>
       <c r="F74" s="24"/>
@@ -12062,13 +12092,13 @@
         <v>271</v>
       </c>
       <c r="B75" s="50" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="C75" s="24" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="D75" s="24" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="E75" s="24"/>
       <c r="F75" s="24"/>
@@ -12078,13 +12108,13 @@
         <v>271</v>
       </c>
       <c r="B76" s="50" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="C76" s="24" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="D76" s="24" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="E76" s="24"/>
       <c r="F76" s="24"/>
@@ -12097,13 +12127,13 @@
         <v>271</v>
       </c>
       <c r="B77" s="50" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="C77" s="24" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
       <c r="D77" s="24" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="E77" s="24"/>
       <c r="F77" s="24"/>
@@ -12113,13 +12143,13 @@
         <v>271</v>
       </c>
       <c r="B78" s="50" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="C78" s="24" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="D78" s="24" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="E78" s="24"/>
       <c r="F78" s="24"/>
@@ -12135,10 +12165,10 @@
         <v>140</v>
       </c>
       <c r="C79" s="24" t="s">
-        <v>647</v>
+        <v>648</v>
       </c>
       <c r="D79" s="50" t="s">
-        <v>648</v>
+        <v>649</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12160,13 +12190,13 @@
         <v>314</v>
       </c>
       <c r="B81" s="50" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="C81" s="50" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="D81" s="50" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="H81" s="50" t="s">
         <v>601</v>
@@ -12180,10 +12210,10 @@
         <v>140</v>
       </c>
       <c r="C82" s="50" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="D82" s="50" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12191,19 +12221,19 @@
         <v>314</v>
       </c>
       <c r="B83" s="24" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="D83" s="24" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="E83" s="24" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="H83" s="50" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12211,19 +12241,19 @@
         <v>431</v>
       </c>
       <c r="B84" s="50" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="C84" s="24" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="D84" s="24" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="E84" s="24" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="F84" s="24" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12231,19 +12261,19 @@
         <v>431</v>
       </c>
       <c r="B85" s="50" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C85" s="24" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="D85" s="24" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="E85" s="24" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="F85" s="24" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12251,13 +12281,13 @@
         <v>431</v>
       </c>
       <c r="B86" s="50" t="s">
-        <v>641</v>
+        <v>642</v>
       </c>
       <c r="C86" s="50" t="s">
-        <v>642</v>
+        <v>643</v>
       </c>
       <c r="D86" s="50" t="s">
-        <v>643</v>
+        <v>644</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12265,13 +12295,13 @@
         <v>462</v>
       </c>
       <c r="B87" s="24" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="C87" s="24" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="D87" s="24" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12279,13 +12309,13 @@
         <v>462</v>
       </c>
       <c r="B88" s="24" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C88" s="24" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="D88" s="24" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12293,13 +12323,13 @@
         <v>462</v>
       </c>
       <c r="B89" s="24" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C89" s="24" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="D89" s="24" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12307,13 +12337,13 @@
         <v>462</v>
       </c>
       <c r="B90" s="24" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="C90" s="24" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="D90" s="24" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12321,7 +12351,7 @@
         <v>462</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12329,7 +12359,7 @@
         <v>462</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12337,13 +12367,13 @@
         <v>477</v>
       </c>
       <c r="B93" s="24" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="C93" s="24" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="D93" s="24" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12351,13 +12381,13 @@
         <v>477</v>
       </c>
       <c r="B94" s="24" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C94" s="24" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="D94" s="24" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12365,13 +12395,13 @@
         <v>477</v>
       </c>
       <c r="B95" s="24" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C95" s="24" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="D95" s="24" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12379,13 +12409,13 @@
         <v>477</v>
       </c>
       <c r="B96" s="24" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="C96" s="24" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="D96" s="24" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12393,7 +12423,7 @@
         <v>477</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>646</v>
+        <v>647</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -12401,7 +12431,7 @@
         <v>477</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>649</v>
+        <v>650</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -12444,41 +12474,41 @@
   </cols>
   <sheetData>
     <row r="1" s="54" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
-        <v>848</v>
-      </c>
-      <c r="B1" s="57" t="s">
-        <v>849</v>
-      </c>
-      <c r="C1" s="57" t="s">
+      <c r="A1" s="58" t="s">
         <v>850</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="B1" s="58" t="s">
         <v>851</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="C1" s="58" t="s">
         <v>852</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="D1" s="58" t="s">
         <v>853</v>
       </c>
-      <c r="G1" s="57" t="s">
+      <c r="E1" s="58" t="s">
         <v>854</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="F1" s="58" t="s">
         <v>855</v>
       </c>
-      <c r="I1" s="57" t="s">
+      <c r="G1" s="58" t="s">
         <v>856</v>
       </c>
-      <c r="J1" s="57" t="s">
+      <c r="H1" s="58" t="s">
         <v>857</v>
       </c>
-      <c r="K1" s="57" t="s">
+      <c r="I1" s="58" t="s">
         <v>858</v>
       </c>
+      <c r="J1" s="58" t="s">
+        <v>859</v>
+      </c>
+      <c r="K1" s="58" t="s">
+        <v>860</v>
+      </c>
       <c r="L1" s="54" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12486,22 +12516,22 @@
         <v>533</v>
       </c>
       <c r="B2" s="37" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="C2" s="37" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="D2" s="37" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="E2" s="37" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="G2" s="37" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="H2" s="37" t="n">
         <v>-10</v>
@@ -12510,13 +12540,13 @@
         <v>100</v>
       </c>
       <c r="J2" s="37" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="K2" s="37" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="L2" s="37" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12524,22 +12554,22 @@
         <v>542</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>869</v>
-      </c>
-      <c r="D3" s="58" t="s">
-        <v>870</v>
-      </c>
-      <c r="E3" s="58" t="s">
         <v>871</v>
       </c>
-      <c r="F3" s="58" t="s">
+      <c r="D3" s="59" t="s">
         <v>872</v>
       </c>
+      <c r="E3" s="59" t="s">
+        <v>873</v>
+      </c>
+      <c r="F3" s="59" t="s">
+        <v>874</v>
+      </c>
       <c r="G3" s="37" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="H3" s="37" t="n">
         <v>-10</v>
@@ -12548,13 +12578,13 @@
         <v>100</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="K3" s="37" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="L3" s="37" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12562,22 +12592,22 @@
         <v>547</v>
       </c>
       <c r="B4" s="37" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="C4" s="37" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="D4" s="37" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="E4" s="37" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="F4" s="37" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="G4" s="37" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="H4" s="37" t="n">
         <v>-10</v>
@@ -12586,13 +12616,13 @@
         <v>100</v>
       </c>
       <c r="J4" s="37" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="K4" s="37" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="L4" s="37" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12600,22 +12630,22 @@
         <v>552</v>
       </c>
       <c r="B5" s="37" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="C5" s="37" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="D5" s="37" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="E5" s="37" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="G5" s="37" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="H5" s="37" t="n">
         <v>-10</v>
@@ -12624,13 +12654,13 @@
         <v>100</v>
       </c>
       <c r="J5" s="37" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="K5" s="37" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="L5" s="37" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
     </row>
   </sheetData>
@@ -12687,13 +12717,13 @@
         <v>368</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="C2" s="24" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="E2" s="24"/>
     </row>
@@ -12702,13 +12732,13 @@
         <v>368</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12716,13 +12746,13 @@
         <v>368</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="D4" s="24" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12730,13 +12760,13 @@
         <v>368</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
       <c r="C5" s="24" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="D5" s="24" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12744,13 +12774,13 @@
         <v>368</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
       <c r="C6" s="24" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="D6" s="24" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12758,13 +12788,13 @@
         <v>368</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="C7" s="24" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="D7" s="24" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12772,13 +12802,13 @@
         <v>368</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="C8" s="24" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="D8" s="24" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12786,13 +12816,13 @@
         <v>368</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
       <c r="C9" s="24" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="D9" s="24" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12800,13 +12830,13 @@
         <v>368</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="C10" s="24" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="D10" s="24" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12814,13 +12844,13 @@
         <v>368</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="C11" s="24" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="D11" s="24" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12828,13 +12858,13 @@
         <v>368</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="C12" s="24" t="s">
-        <v>650</v>
+        <v>651</v>
       </c>
       <c r="D12" s="24" t="s">
-        <v>651</v>
+        <v>652</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12842,13 +12872,13 @@
         <v>368</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="C13" s="24" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D13" s="24" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
     </row>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
choices: use `customChoices` when labels have placeholders
fixes #65

The widgets whose choices contained {{}} placeholders now use
customChoices.

Update the choices form the nextPlaceCategory to use context and
placeholders and labels from the excel file instead of those from the
`survey` namespace.

The choices are left as is, even though the widgets use the custom ones,
so that when the issue is fixed and nickname and gender are supported,
the custom can just be removed
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1951" uniqueCount="1132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1998" uniqueCount="1153">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -1123,7 +1123,7 @@
     <t xml:space="preserve">currentPlaceWorkOnTheRoadAndNoNextPlaceCustomConditional</t>
   </si>
   <si>
-    <t xml:space="preserve">onTheRoadArrivalTypeChoices</t>
+    <t xml:space="preserve">onTheRoadArrivalTypeCustomChoices</t>
   </si>
   <si>
     <t xml:space="preserve">À transformer en custom si les libellés avec nickname ne viennet pas dans el générateur</t>
@@ -1530,7 +1530,7 @@
     <t xml:space="preserve">isTransitAndNotNationaleCustomConditional</t>
   </si>
   <si>
-    <t xml:space="preserve">onDemandChoices</t>
+    <t xml:space="preserve">onDemandCustomChoices</t>
   </si>
   <si>
     <t xml:space="preserve">tripJunctionQueryString</t>
@@ -2679,6 +2679,9 @@
     <t xml:space="preserve">**School / place of study**: studied or slept there</t>
   </si>
   <si>
+    <t xml:space="preserve">onTheRoadArrivalTypeChoices</t>
+  </si>
+  <si>
     <t xml:space="preserve">usualWorkPlace</t>
   </si>
   <si>
@@ -2700,847 +2703,907 @@
     <t xml:space="preserve">{{nickname}} a complété ses déplacements sur la route après 4:00 du matin le lendemain</t>
   </si>
   <si>
+    <t xml:space="preserve">{{nickname}} completed {{gender :his/her/their}} work on the road trips after 4AM the next day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai complété mes déplacements sur la route après 4:00 du matin le lendemain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I completed my work on the road trips after 4AM the next day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">isLastPlaceCustomConditional</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onDemandChoices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pickupAtOrigin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oui, il est venu chercher {{nickname}} à son lieu de départ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, it picked {{nickname}} up at their departure location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oui, il est venu me chercher à mon lieu de départ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, it picked me up at my departure location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">joinedStop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oui, {{nickname}} a rejoint un arrêt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, {{nickname}} went to a stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Oui, j'ai rejoint un arrêt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yes, I went to a stop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">remoteWorkOrWorkAtHome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Télétravail / travail à la maison</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remote work / work from home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onStrike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">En grève</t>
+  </si>
+  <si>
+    <t xml:space="preserve">On strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">leaveSicknessPersonalReason</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Congé (maladie, personnel, autre)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leave (sick, personal, other)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noWork</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas de travail prévu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No work planned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">distanceLearning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cours à distance</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Distance learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schoolWasClosedStrike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">École fermée (grève)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">School was closed (strike)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noSchool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas de cours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No classes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">inputRangeName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labelFrMin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labelFrMiddle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labelFrMax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labelEnMin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labelEnMiddle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">labelEnMax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">minValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">maxValue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unitFr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">unitEn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">input_color</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trop court</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Juste comme il faut</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Trop long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too short</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Just right</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Too long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">blue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Pas du tout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neutre</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Très intéressante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Not at all</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Neutral</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very interesting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">red-yellow-green</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Très facile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modérément difficile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Très difficile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very easy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderately difficult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very difficult</t>
+  </si>
+  <si>
+    <t xml:space="preserve">green-yellow-red</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modérément pénible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Très pénible</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Moderately burdensome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Very burdensome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">addGroupedObject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ajouter une personne manquante</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add a missing person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deleteThisGroupedObject</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supprimer cette personne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete this person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">segmentsIntroOnTheRoad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veuillez indiquer tous les modes de transport utilisés pour effectuer les déplacements sur la route, dans l'ordre chronologique:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please indicate all modes of transport used to complete work trip on the road, in chronological order:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">segmentsIntroStroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veuillez indiquer tous les modes de transport utilisés pour effectuer la promenade, dans l'ordre chronologique:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please indicate all modes of transport used to complete the stroll, in chronological order:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">junctionGeographyRefreshGeocodingLabel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chercher le lieu de jonction à partir du nom ou de l'adresse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Search the junction location using the place name or address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">driverFamily</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ami ou famille</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Friend or family</t>
+  </si>
+  <si>
+    <t xml:space="preserve">driverColleague</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Un collègue de travail ou d'études</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A work colleague or fellow classmate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">driverTaxi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chauffeur Taxi ou Uber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxi or Uber driver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">driverTransitTaxi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chauffeur Taxi collectif / transport à la demande</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Taxibus / On-demand transport driver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">driverParaTransit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chauffeur Transport adapté</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Para-transit driver</t>
+  </si>
+  <si>
+    <t xml:space="preserve">driverCarpool</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chauffeur Covoiturage (ex: Amigo Express, Kangaride)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Carsharing driver (ex: Amigo Express, Kangaride)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">driverOther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Une autre personne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Another person</t>
+  </si>
+  <si>
+    <t xml:space="preserve">driverDontKnow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">driverFamilyMemberSeq</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Personne {{sequence}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Person {{sequence}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreviousDepartureTime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le lieu précédent ({{previousVisitedPlaceDescription}})?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did {{nickname}} leave the previous location ({{previousVisitedPlaceDescription}})?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure avez-vous quitté le lieu précédent ({{previousVisitedPlaceDescription}})?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did you leave the previous location ({{previousVisitedPlaceDescription}})?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreviousDepartureTime_home_workUsual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile pour aller au travail?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did {{nickname}} leave home before going to work?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure avez-vous quitté le domicile pour aller au travail?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did you leave home before going to work?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreviousDepartureTime_home_schoolUsual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile pour aller au lieu d'études/école?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did {{nickname}} leave home before going to school?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure avez-vous quitté le domicile pour aller au lieu d'études/école?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did you leave home before going to school?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreviousDepartureTime_home_other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile pour aller à cet endroit ({{visitedPlaceDescription}})?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did {{nickname}} leave home before going to this place ({{visitedPlaceDescription}})?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure avez-vous quitté le domicile pour aller à cet endroit ({{visitedPlaceDescription}})?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did you leave home before going to this place ({{visitedPlaceDescription}})?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreviousDepartureTime_home_workOnTheRoad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile avant de débuter ses déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did {{nickname}} leave home before starting {{gender :his/her/their}} on the road trips?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure avez-vous quitté le domicile avant de débuter vos déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did you leave home before starting your on the road trips?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PreviousDepartureTime_usualWorkPlace_workOnTheRoad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">t what time did {{nickname}} leave {{gender :his/her/their}} usual work place before starting {{gender :his/her/their}} on the road trips?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure avez-vous quitté votre lieu de travail habituel avant de débuter vos déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did you leave your usual work place before starting your on the road trips?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spécifier :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specify :</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ActivityCategoryFirstLocation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activité principale au lieu de départ de la journée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main activity carried out at the starting point of the day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ActivityCategoryAfterHome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activité principale au premier lieu visité dans la journée après avoir quitté le domicile</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main activity carried out at the first location visited after leaving home</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ActivityCategory</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Activité principale à ce lieu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Main activity carried out at this location</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VisitedPlaceSequence</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lieu {{count}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Location #{{count}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lieu de départ de la journée</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Departure place for this day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ConfirmDeleteVisitedPlace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Confirmez-vous que vous voulez retirer ce lieu?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Do you confirm that you want to remove this location?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddress</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nom ou adresse du lieu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Name or address of the place</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_workUsual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Édifice du Phare, CPE les petits génies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lighthouse building, Les Petits génies CPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_workUsual_onTheRoadOften</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre de distribution Rivières, Resto St-Hubert Alma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rivière distribution center, Alma St-Hubert BBQ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_workNotUsual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Palais des congrès de Montréal, Le Co-work du lac Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chateau Frontenac, Co-work on the Long lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_schoolUsual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">École Marguerite-Bourgeoys, Collège CDI Québec, UQAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Marguerite-Bourgeoys school, CDI College Québec, UQAR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_schoolNotUsual</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bibliothèque à Livre ouvert, École de musique Dorémi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National library, music school Doremi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_shopping</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centre d’achat Le Carrefour, Provigo St-Félicien, IKEA Boucherville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Le Carrefour shopping mall, Provigo St-Félicien, IKEA Boucherville</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_restaurant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normandin de Lévis, Snack bar chez Raymond, Resto Subway de Rawdon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Normandin in Lévis, Snack bar chez Raymond, Subway restaurant in Rawdon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_dropSomeone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gare d’autocar, Aréna des Collines, École des Pionniers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Central bus station, des Collines arena, des Pionniers high school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_fetchSomeone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_leisureArtsMusicCulture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cinéma des chutes, Théâtre de Verdure, Musée national des petits pots Masson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Des chutes cinema, de Verdure Theatre, Mason Jar National Museum</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_leisureSports</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nautilus St-Georges, Escalade La Grimpe, Parc de la Rose</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nautilus St-Georges, Climbing La Grimpe, de la Rose Park</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_leisureTourism</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camping Ste-Madeleine, Paris France, Hôtel Days Inn St-Flavien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Camping Ste-Madeleine, Paris*France, Hotel Days Inn St-Flavien</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_leisureStroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Parc au bord de l’eau, Petit train du nord, Stroll de la Montagne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waterside park, Petit train du nord, de la Montagne promenade</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_visiting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Addresse de la personne visitée, Coin des Rossignols et de l’Étang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address of the visited person, corner des Rossignols and de l’Étang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_medical</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Clinique Médicale des Marguerites, Hôpital régional de Rimouski, CLSC des Rivières</t>
+  </si>
+  <si>
+    <t xml:space="preserve">des Marguerites medical clinic, Rimouski regional hospital, des Rivières CLSC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_service</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Coiffure Dans le Vent, Caisse Desjardins de Limoilou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">High class Hair saloon, Caisse Desjardins Limoilou</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_worship</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Église Saint-Nicéphore, Mosquée de la Capitale, Synagogue Maison Chabad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Saint-Nicéphore church, de la Capitale mosque, Congregation Beth Israel Ohev Sholem</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_secondaryHome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adresse de la résidence secondaire, nom du chalet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary home address, name of the chalet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LocationNameAddressExample_schoolNotStudent</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Institut Linguistique, École de conduite Tecnic</t>
+  </si>
+  <si>
+    <t xml:space="preserve">language centre, Tecnic driving school</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_previousPreviousDepartureTimeHomeToUsualWorkplace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} a quitté le domicile pour aller à son lieu habituel de travail à?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} left home to go to {{gender :his/her/their}} usual work place?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous avez quitté le domicile pour aller à votre lieu habituel de travail à?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You left home to go to your usual work place at?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_previousArrivalTimeDepartureTypeHome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel}} arriv{{gender :é/ée/é.e}} au domicile avant de débuter ses déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did {{nickname}} arrive home before starting {{gender :his/her/their}} on the road trips?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure êtes-vous arriv{{gender :é/ée/é.e}} au domicile avant de débuter vos déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did you arrive home before starting your on the road trips?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_previousArrivalTimeDepartureTypeUsualWorkPlace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel}} arriv{{gender :é/ée/é.e}} à son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did {{nickname}} arrive at his usual work place before starting {{gender :his/her/their}} on the road trips?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure êtes-vous arriv{{gender :é/ée/é.e}} à votre lieu de travail habituel avant de débuter vos déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did you arrive at your usual work place before starting your on the road trips?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">_previousArrivalTimeDepartureTypeOther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel}} arriv{{gender :é/ée/é.e}} au lieu précédent ({{visitedPlaceDescription}}) avant de débuter ses déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did {{nickname}} arrive at the previous location ({{visitedPlaceDescription}}) before starting {{gender :his/her/their}} on the road trips?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">À quelle heure êtes-vous arriv{{gender :é/ée/é.e}} au le lieu précédent ({{visitedPlaceDescription}}) avant de débuter vos déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did you arrive at the previous location ({{visitedPlaceDescription}}) before starting your on the road trips?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arrivalTimeOnTheRoad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} a commencé ses déplacements sur la route à: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} started their work trip on the road at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous avez commencé vos déplacements sur la route à:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You started your work trip on the road at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">arrivalTimeStroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} a commencé sa promenade à:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} started their stroll at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous avez commencé votre promenade à: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">You started your stroll at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">departureTimeStroll</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} a terminé sa promenade à:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} finished their stroll at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous avez terminé votre promenade à:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You finished your stroll at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">departureTimeOnTheRoad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} a terminé ses déplacements sur la route à:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} finished their work on the road at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous avez terminé vos déplacements sur la route à:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You finished your work on the road at:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errors.selectDontKnowWhenNoOtherChoiceSelected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélectionnez "Je ne sais pas" seulement si aucun autre choix n'est sélectionné.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select "I don't know" only if no other choice is selected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errors.selectNoWhenNoOtherChoiceSelected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélectionnez "Non" seulement si aucun autre choix n'est sélectionné.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select "no" only if no other choice is selected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errors.selectPreferNotToAnswerWhenNoOtherChoiceSelected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélectionnez "Préfère ne pas répondre" seulement si aucun autre choix n'est sélectionné.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select "Prefer not to answer" only if no other choice is selected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errors.selectNoTravelWhenNoOtherChoiceSelected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélectionnez "Pas de déplacement" seulement si aucun autre choix n'est sélectionné.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select "No Travel" only if no other choice is selected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errors.selectOneOrMoreAnswer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélectionnez une ou des réponses.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select one or multiple choices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errors.selectNoRemoteWorkWhenNoOtherChoiceSelected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélectionnez "Pas de télé-travail" seulement si aucun autre choix n'est sélectionné.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select "No remote work" only if no other choice is selected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">errors.selectNoRemoteStudyWhenNoOtherChoiceSelected</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélectionnez "Pas de télé-études" seulement si aucun autre choix n'est sélectionné.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select "No remote studies" only if no other choice is selected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onTheRoadArrivalTypeHome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onTheRoadArrivalTypeUsualWorkPlace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onTheRoadArrivalTypeOther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onTheRoadArrivalTypeStayedThereUntilTheNextDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onDemandChoicesPickupAtOrigin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">onDemandChoicesJoinedStop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nextPlaceRadioChoices.stayedHomeUntilTheNextDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest{{gender :é/ée/é.e}} au domicile jusqu'au lendemain</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Stayed home until the next day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nextPlaceRadioChoices.stayedThereUntilTheNextDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rest{{gender :é/ée/é.e}} à cet endroit jusqu'au lendemain</t>
+  </si>
+  <si>
     <t xml:space="preserve">Stayed at this place until the next day</t>
   </si>
   <si>
-    <t xml:space="preserve">J'ai complété mes déplacements sur la route après 4:00 du matin le lendemain</t>
-  </si>
-  <si>
-    <t xml:space="preserve">isLastPlaceCustomConditional</t>
-  </si>
-  <si>
-    <t xml:space="preserve">pickupAtOrigin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oui, il est venu chercher {{nickname}} à son lieu de départ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, it picked {{nickname}} up at their departure location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oui, il est venu me chercher à mon lieu de départ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, it picked me up at my departure location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">joinedStop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oui, {{nickname}} a rejoint un arrêt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, {{nickname}} went to a stop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Oui, j'ai rejoint un arrêt</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Yes, I went to a stop</t>
-  </si>
-  <si>
-    <t xml:space="preserve">remoteWorkOrWorkAtHome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Télétravail / travail à la maison</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Remote work / work from home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">onStrike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">En grève</t>
-  </si>
-  <si>
-    <t xml:space="preserve">On strike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">leaveSicknessPersonalReason</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Congé (maladie, personnel, autre)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Leave (sick, personal, other)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noWork</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pas de travail prévu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No work planned</t>
-  </si>
-  <si>
-    <t xml:space="preserve">distanceLearning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cours à distance</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Distance learning</t>
-  </si>
-  <si>
-    <t xml:space="preserve">schoolWasClosedStrike</t>
-  </si>
-  <si>
-    <t xml:space="preserve">École fermée (grève)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">School was closed (strike)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noSchool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pas de cours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">No classes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">inputRangeName</t>
-  </si>
-  <si>
-    <t xml:space="preserve">labelFrMin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">labelFrMiddle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">labelFrMax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">labelEnMin</t>
-  </si>
-  <si>
-    <t xml:space="preserve">labelEnMiddle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">labelEnMax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">minValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">maxValue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unitFr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">unitEn</t>
-  </si>
-  <si>
-    <t xml:space="preserve">input_color</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trop court</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Juste comme il faut</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Trop long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Too short</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Just right</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Too long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">%</t>
-  </si>
-  <si>
-    <t xml:space="preserve">blue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pas du tout</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neutre</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Très intéressante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Not at all</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Neutral</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very interesting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">red-yellow-green</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Très facile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modérément difficile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Très difficile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very easy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moderately difficult</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very difficult</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green-yellow-red</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Modérément pénible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Très pénible</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Moderately burdensome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Very burdensome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">addGroupedObject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ajouter une personne manquante</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Add a missing person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deleteThisGroupedObject</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supprimer cette personne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Delete this person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">segmentsIntroOnTheRoad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veuillez indiquer tous les modes de transport utilisés pour effectuer les déplacements sur la route, dans l'ordre chronologique:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please indicate all modes of transport used to complete work trip on the road, in chronological order:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">segmentsIntroStroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veuillez indiquer tous les modes de transport utilisés pour effectuer la promenade, dans l'ordre chronologique:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please indicate all modes of transport used to complete the stroll, in chronological order:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">junctionGeographyRefreshGeocodingLabel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chercher le lieu de jonction à partir du nom ou de l'adresse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Search the junction location using the place name or address</t>
-  </si>
-  <si>
-    <t xml:space="preserve">driverFamily</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Ami ou famille</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Friend or family</t>
-  </si>
-  <si>
-    <t xml:space="preserve">driverColleague</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Un collègue de travail ou d'études</t>
-  </si>
-  <si>
-    <t xml:space="preserve">A work colleague or fellow classmate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">driverTaxi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chauffeur Taxi ou Uber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxi or Uber driver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">driverTransitTaxi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chauffeur Taxi collectif / transport à la demande</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Taxibus / On-demand transport driver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">driverParaTransit</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chauffeur Transport adapté</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Para-transit driver</t>
-  </si>
-  <si>
-    <t xml:space="preserve">driverCarpool</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chauffeur Covoiturage (ex: Amigo Express, Kangaride)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carsharing driver (ex: Amigo Express, Kangaride)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">driverOther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Une autre personne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Another person</t>
-  </si>
-  <si>
-    <t xml:space="preserve">driverDontKnow</t>
-  </si>
-  <si>
-    <t xml:space="preserve">driverFamilyMemberSeq</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Personne {{sequence}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Person {{sequence}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PreviousDepartureTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le lieu précédent ({{previousVisitedPlaceDescription}})?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did {{nickname}} leave the previous location ({{previousVisitedPlaceDescription}})?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure avez-vous quitté le lieu précédent ({{previousVisitedPlaceDescription}})?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did you leave the previous location ({{previousVisitedPlaceDescription}})?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PreviousDepartureTime_home_workUsual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile pour aller au travail?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did {{nickname}} leave home before going to work?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure avez-vous quitté le domicile pour aller au travail?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did you leave home before going to work?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PreviousDepartureTime_home_schoolUsual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile pour aller au lieu d'études/école?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did {{nickname}} leave home before going to school?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure avez-vous quitté le domicile pour aller au lieu d'études/école?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did you leave home before going to school?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PreviousDepartureTime_home_other</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile pour aller à cet endroit ({{visitedPlaceDescription}})?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did {{nickname}} leave home before going to this place ({{visitedPlaceDescription}})?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure avez-vous quitté le domicile pour aller à cet endroit ({{visitedPlaceDescription}})?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did you leave home before going to this place ({{visitedPlaceDescription}})?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PreviousDepartureTime_home_workOnTheRoad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile avant de débuter ses déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did {{nickname}} leave home before starting {{gender :his/her/their}} on the road trips?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure avez-vous quitté le domicile avant de débuter vos déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did you leave home before starting your on the road trips?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PreviousDepartureTime_usualWorkPlace_workOnTheRoad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">t what time did {{nickname}} leave {{gender :his/her/their}} usual work place before starting {{gender :his/her/their}} on the road trips?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure avez-vous quitté votre lieu de travail habituel avant de débuter vos déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did you leave your usual work place before starting your on the road trips?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Spécifier :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Specify :</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ActivityCategoryFirstLocation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activité principale au lieu de départ de la journée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main activity carried out at the starting point of the day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ActivityCategoryAfterHome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activité principale au premier lieu visité dans la journée après avoir quitté le domicile</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main activity carried out at the first location visited after leaving home</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ActivityCategory</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Activité principale à ce lieu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Main activity carried out at this location</t>
-  </si>
-  <si>
-    <t xml:space="preserve">VisitedPlaceSequence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieu {{count}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Location #{{count}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lieu de départ de la journée</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Departure place for this day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ConfirmDeleteVisitedPlace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Confirmez-vous que vous voulez retirer ce lieu?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Do you confirm that you want to remove this location?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddress</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nom ou adresse du lieu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Name or address of the place</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_workUsual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Édifice du Phare, CPE les petits génies</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lighthouse building, Les Petits génies CPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_workUsual_onTheRoadOften</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centre de distribution Rivières, Resto St-Hubert Alma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rivière distribution center, Alma St-Hubert BBQ</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_workNotUsual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Palais des congrès de Montréal, Le Co-work du lac Long</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chateau Frontenac, Co-work on the Long lake</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_schoolUsual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">École Marguerite-Bourgeoys, Collège CDI Québec, UQAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Marguerite-Bourgeoys school, CDI College Québec, UQAR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_schoolNotUsual</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bibliothèque à Livre ouvert, École de musique Dorémi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">National library, music school Doremi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_shopping</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Centre d’achat Le Carrefour, Provigo St-Félicien, IKEA Boucherville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Le Carrefour shopping mall, Provigo St-Félicien, IKEA Boucherville</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_restaurant</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normandin de Lévis, Snack bar chez Raymond, Resto Subway de Rawdon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Normandin in Lévis, Snack bar chez Raymond, Subway restaurant in Rawdon</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_dropSomeone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gare d’autocar, Aréna des Collines, École des Pionniers</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Central bus station, des Collines arena, des Pionniers high school</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_fetchSomeone</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_leisureArtsMusicCulture</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cinéma des chutes, Théâtre de Verdure, Musée national des petits pots Masson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Des chutes cinema, de Verdure Theatre, Mason Jar National Museum</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_leisureSports</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nautilus St-Georges, Escalade La Grimpe, Parc de la Rose</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nautilus St-Georges, Climbing La Grimpe, de la Rose Park</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_leisureTourism</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camping Ste-Madeleine, Paris France, Hôtel Days Inn St-Flavien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Camping Ste-Madeleine, Paris*France, Hotel Days Inn St-Flavien</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_leisureStroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Parc au bord de l’eau, Petit train du nord, Stroll de la Montagne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Waterside park, Petit train du nord, de la Montagne promenade</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_visiting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Addresse de la personne visitée, Coin des Rossignols et de l’Étang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Address of the visited person, corner des Rossignols and de l’Étang</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_medical</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Clinique Médicale des Marguerites, Hôpital régional de Rimouski, CLSC des Rivières</t>
-  </si>
-  <si>
-    <t xml:space="preserve">des Marguerites medical clinic, Rimouski regional hospital, des Rivières CLSC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_service</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Coiffure Dans le Vent, Caisse Desjardins de Limoilou</t>
-  </si>
-  <si>
-    <t xml:space="preserve">High class Hair saloon, Caisse Desjardins Limoilou</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_worship</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Église Saint-Nicéphore, Mosquée de la Capitale, Synagogue Maison Chabad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Saint-Nicéphore church, de la Capitale mosque, Congregation Beth Israel Ohev Sholem</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_secondaryHome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adresse de la résidence secondaire, nom du chalet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary home address, name of the chalet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LocationNameAddressExample_schoolNotStudent</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Institut Linguistique, École de conduite Tecnic</t>
-  </si>
-  <si>
-    <t xml:space="preserve">language centre, Tecnic driving school</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_previousPreviousDepartureTimeHomeToUsualWorkplace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{nickname}} a quitté le domicile pour aller à son lieu habituel de travail à?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{nickname}} left home to go to {{gender :his/her/their}} usual work place?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vous avez quitté le domicile pour aller à votre lieu habituel de travail à?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You left home to go to your usual work place at?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_previousArrivalTimeDepartureTypeHome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel}} arriv{{gender :é/ée/é.e}} au domicile avant de débuter ses déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did {{nickname}} arrive home before starting {{gender :his/her/their}} on the road trips?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure êtes-vous arriv{{gender :é/ée/é.e}} au domicile avant de débuter vos déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did you arrive home before starting your on the road trips?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_previousArrivalTimeDepartureTypeUsualWorkPlace</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel}} arriv{{gender :é/ée/é.e}} à son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did {{nickname}} arrive at his usual work place before starting {{gender :his/her/their}} on the road trips?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure êtes-vous arriv{{gender :é/ée/é.e}} à votre lieu de travail habituel avant de débuter vos déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did you arrive at your usual work place before starting your on the road trips?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">_previousArrivalTimeDepartureTypeOther</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel}} arriv{{gender :é/ée/é.e}} au lieu précédent (${visitedPlaceDescription}) avant de débuter ses déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did {{nickname}} arrive at the previous location ({{visitedPlaceDescription}}) before starting {{gender :his/her/their}} on the road trips?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">À quelle heure êtes-vous arriv{{gender :é/ée/é.e}} au le lieu précédent ({{visitedPlaceDescription}}) avant de débuter vos déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did you arrive at the previous location ({{visitedPlaceDescription}}) before starting your on the road trips?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arrivalTimeOnTheRoad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{nickname}} a commencé ses déplacements sur la route à: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{nickname}} started their work trip on the road at:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vous avez commencé vos déplacements sur la route à:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You started your work trip on the road at:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arrivalTimeStroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{nickname}} a commencé sa promenade à:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{nickname}} started their stroll at:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vous avez commencé votre promenade à: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">You started your stroll at:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">departureTimeStroll</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{nickname}} a terminé sa promenade à:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{nickname}} finished their stroll at:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vous avez terminé votre promenade à:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You finished your stroll at:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">departureTimeOnTheRoad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{nickname}} a terminé ses déplacements sur la route à:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">{{nickname}} finished their work on the road at:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vous avez terminé vos déplacements sur la route à:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You finished your work on the road at:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errors.selectDontKnowWhenNoOtherChoiceSelected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sélectionnez "Je ne sais pas" seulement si aucun autre choix n'est sélectionné.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select "I don't know" only if no other choice is selected.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errors.selectNoWhenNoOtherChoiceSelected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sélectionnez "Non" seulement si aucun autre choix n'est sélectionné.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select "no" only if no other choice is selected.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errors.selectPreferNotToAnswerWhenNoOtherChoiceSelected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sélectionnez "Préfère ne pas répondre" seulement si aucun autre choix n'est sélectionné.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select "Prefer not to answer" only if no other choice is selected.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errors.selectNoTravelWhenNoOtherChoiceSelected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sélectionnez "Pas de déplacement" seulement si aucun autre choix n'est sélectionné.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select "No Travel" only if no other choice is selected.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errors.selectOneOrMoreAnswer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sélectionnez une ou des réponses.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select one or multiple choices.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errors.selectNoRemoteWorkWhenNoOtherChoiceSelected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sélectionnez "Pas de télé-travail" seulement si aucun autre choix n'est sélectionné.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select "No remote work" only if no other choice is selected.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">errors.selectNoRemoteStudyWhenNoOtherChoiceSelected</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sélectionnez "Pas de télé-études" seulement si aucun autre choix n'est sélectionné.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select "No remote studies" only if no other choice is selected.</t>
+    <t xml:space="preserve">nextPlaceRadioChoices.visitedAnotherPlace</t>
+  </si>
+  <si>
+    <t xml:space="preserve">All{{gender :é/ée/é.e}} ou arrét{{gender :é/ée/é.e}} à un autre endroit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Went or stopped elsewhere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nextPlaceRadioChoices.wentBackHome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Retourn{{gender :é/ée/é.e}} au domicile directement ({{address}})</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Returned home directly ({{address}})</t>
   </si>
 </sst>
 </file>
@@ -4457,11 +4520,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="G31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="K85" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
-      <selection pane="bottomLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
-      <selection pane="bottomRight" activeCell="G40" activeCellId="0" sqref="G40"/>
+      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
+      <selection pane="bottomLeft" activeCell="A85" activeCellId="0" sqref="A85"/>
+      <selection pane="bottomRight" activeCell="O96" activeCellId="0" sqref="O96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11705,8 +11768,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A76" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C85" activeCellId="0" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13055,7 +13118,7 @@
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="33" t="s">
-        <v>337</v>
+        <v>844</v>
       </c>
       <c r="B80" s="53" t="s">
         <v>27</v>
@@ -13069,16 +13132,16 @@
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="33" t="s">
-        <v>337</v>
+        <v>844</v>
       </c>
       <c r="B81" s="53" t="s">
-        <v>844</v>
+        <v>845</v>
       </c>
       <c r="C81" s="53" t="s">
-        <v>845</v>
+        <v>846</v>
       </c>
       <c r="D81" s="53" t="s">
-        <v>846</v>
+        <v>847</v>
       </c>
       <c r="H81" s="53" t="s">
         <v>636</v>
@@ -13086,81 +13149,84 @@
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="33" t="s">
-        <v>337</v>
+        <v>844</v>
       </c>
       <c r="B82" s="53" t="s">
         <v>143</v>
       </c>
       <c r="C82" s="53" t="s">
-        <v>847</v>
+        <v>848</v>
       </c>
       <c r="D82" s="53" t="s">
-        <v>848</v>
+        <v>849</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="33" t="s">
-        <v>337</v>
+        <v>844</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>849</v>
+        <v>850</v>
       </c>
       <c r="C83" s="26" t="s">
-        <v>850</v>
+        <v>851</v>
       </c>
       <c r="D83" s="26" t="s">
-        <v>851</v>
+        <v>852</v>
       </c>
       <c r="E83" s="26" t="s">
-        <v>852</v>
+        <v>853</v>
+      </c>
+      <c r="F83" s="26" t="s">
+        <v>854</v>
       </c>
       <c r="H83" s="53" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="33" t="s">
-        <v>466</v>
+        <v>856</v>
       </c>
       <c r="B84" s="53" t="s">
-        <v>854</v>
+        <v>857</v>
       </c>
       <c r="C84" s="26" t="s">
-        <v>855</v>
+        <v>858</v>
       </c>
       <c r="D84" s="26" t="s">
-        <v>856</v>
+        <v>859</v>
       </c>
       <c r="E84" s="26" t="s">
-        <v>857</v>
+        <v>860</v>
       </c>
       <c r="F84" s="26" t="s">
-        <v>858</v>
+        <v>861</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="33" t="s">
-        <v>466</v>
+        <v>856</v>
       </c>
       <c r="B85" s="53" t="s">
-        <v>859</v>
+        <v>862</v>
       </c>
       <c r="C85" s="26" t="s">
-        <v>860</v>
+        <v>863</v>
       </c>
       <c r="D85" s="26" t="s">
-        <v>861</v>
+        <v>864</v>
       </c>
       <c r="E85" s="26" t="s">
-        <v>862</v>
+        <v>865</v>
       </c>
       <c r="F85" s="26" t="s">
-        <v>863</v>
+        <v>866</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="33" t="s">
-        <v>466</v>
+        <v>856</v>
       </c>
       <c r="B86" s="53" t="s">
         <v>680</v>
@@ -13177,13 +13243,13 @@
         <v>497</v>
       </c>
       <c r="B87" s="26" t="s">
-        <v>864</v>
+        <v>867</v>
       </c>
       <c r="C87" s="26" t="s">
-        <v>865</v>
+        <v>868</v>
       </c>
       <c r="D87" s="26" t="s">
-        <v>866</v>
+        <v>869</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13191,13 +13257,13 @@
         <v>497</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>867</v>
+        <v>870</v>
       </c>
       <c r="C88" s="26" t="s">
-        <v>868</v>
+        <v>871</v>
       </c>
       <c r="D88" s="26" t="s">
-        <v>869</v>
+        <v>872</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13205,13 +13271,13 @@
         <v>497</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="C89" s="26" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="D89" s="26" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13219,13 +13285,13 @@
         <v>497</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>873</v>
+        <v>876</v>
       </c>
       <c r="C90" s="26" t="s">
-        <v>874</v>
+        <v>877</v>
       </c>
       <c r="D90" s="26" t="s">
-        <v>875</v>
+        <v>878</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13249,13 +13315,13 @@
         <v>512</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>876</v>
+        <v>879</v>
       </c>
       <c r="C93" s="26" t="s">
-        <v>877</v>
+        <v>880</v>
       </c>
       <c r="D93" s="26" t="s">
-        <v>878</v>
+        <v>881</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13263,13 +13329,13 @@
         <v>512</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>879</v>
+        <v>882</v>
       </c>
       <c r="C94" s="26" t="s">
-        <v>880</v>
+        <v>883</v>
       </c>
       <c r="D94" s="26" t="s">
-        <v>881</v>
+        <v>884</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13277,13 +13343,13 @@
         <v>512</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>870</v>
+        <v>873</v>
       </c>
       <c r="C95" s="26" t="s">
-        <v>871</v>
+        <v>874</v>
       </c>
       <c r="D95" s="26" t="s">
-        <v>872</v>
+        <v>875</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13291,13 +13357,13 @@
         <v>512</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>882</v>
+        <v>885</v>
       </c>
       <c r="C96" s="26" t="s">
-        <v>883</v>
+        <v>886</v>
       </c>
       <c r="D96" s="26" t="s">
-        <v>884</v>
+        <v>887</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13357,40 +13423,40 @@
   <sheetData>
     <row r="1" s="57" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="60" t="s">
-        <v>885</v>
+        <v>888</v>
       </c>
       <c r="B1" s="60" t="s">
-        <v>886</v>
+        <v>889</v>
       </c>
       <c r="C1" s="60" t="s">
-        <v>887</v>
+        <v>890</v>
       </c>
       <c r="D1" s="60" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="E1" s="60" t="s">
-        <v>889</v>
+        <v>892</v>
       </c>
       <c r="F1" s="60" t="s">
-        <v>890</v>
+        <v>893</v>
       </c>
       <c r="G1" s="60" t="s">
-        <v>891</v>
+        <v>894</v>
       </c>
       <c r="H1" s="60" t="s">
-        <v>892</v>
+        <v>895</v>
       </c>
       <c r="I1" s="60" t="s">
-        <v>893</v>
+        <v>896</v>
       </c>
       <c r="J1" s="60" t="s">
-        <v>894</v>
+        <v>897</v>
       </c>
       <c r="K1" s="60" t="s">
-        <v>895</v>
+        <v>898</v>
       </c>
       <c r="L1" s="57" t="s">
-        <v>896</v>
+        <v>899</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13398,22 +13464,22 @@
         <v>568</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>897</v>
+        <v>900</v>
       </c>
       <c r="C2" s="40" t="s">
-        <v>898</v>
+        <v>901</v>
       </c>
       <c r="D2" s="40" t="s">
-        <v>899</v>
+        <v>902</v>
       </c>
       <c r="E2" s="40" t="s">
-        <v>900</v>
+        <v>903</v>
       </c>
       <c r="F2" s="40" t="s">
-        <v>901</v>
+        <v>904</v>
       </c>
       <c r="G2" s="40" t="s">
-        <v>902</v>
+        <v>905</v>
       </c>
       <c r="H2" s="40" t="n">
         <v>-10</v>
@@ -13422,13 +13488,13 @@
         <v>100</v>
       </c>
       <c r="J2" s="40" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="K2" s="40" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="L2" s="40" t="s">
-        <v>904</v>
+        <v>907</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13436,22 +13502,22 @@
         <v>577</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="C3" s="40" t="s">
-        <v>906</v>
+        <v>909</v>
       </c>
       <c r="D3" s="61" t="s">
-        <v>907</v>
+        <v>910</v>
       </c>
       <c r="E3" s="61" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="F3" s="61" t="s">
-        <v>909</v>
+        <v>912</v>
       </c>
       <c r="G3" s="40" t="s">
-        <v>910</v>
+        <v>913</v>
       </c>
       <c r="H3" s="40" t="n">
         <v>-10</v>
@@ -13460,13 +13526,13 @@
         <v>100</v>
       </c>
       <c r="J3" s="40" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="K3" s="40" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="L3" s="40" t="s">
-        <v>911</v>
+        <v>914</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13474,22 +13540,22 @@
         <v>582</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>912</v>
+        <v>915</v>
       </c>
       <c r="C4" s="40" t="s">
-        <v>913</v>
+        <v>916</v>
       </c>
       <c r="D4" s="40" t="s">
-        <v>914</v>
+        <v>917</v>
       </c>
       <c r="E4" s="40" t="s">
-        <v>915</v>
+        <v>918</v>
       </c>
       <c r="F4" s="40" t="s">
-        <v>916</v>
+        <v>919</v>
       </c>
       <c r="G4" s="40" t="s">
-        <v>917</v>
+        <v>920</v>
       </c>
       <c r="H4" s="40" t="n">
         <v>-10</v>
@@ -13498,13 +13564,13 @@
         <v>100</v>
       </c>
       <c r="J4" s="40" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="K4" s="40" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="L4" s="40" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13512,22 +13578,22 @@
         <v>587</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>905</v>
+        <v>908</v>
       </c>
       <c r="C5" s="40" t="s">
-        <v>919</v>
+        <v>922</v>
       </c>
       <c r="D5" s="40" t="s">
-        <v>920</v>
+        <v>923</v>
       </c>
       <c r="E5" s="40" t="s">
-        <v>908</v>
+        <v>911</v>
       </c>
       <c r="F5" s="40" t="s">
-        <v>921</v>
+        <v>924</v>
       </c>
       <c r="G5" s="40" t="s">
-        <v>922</v>
+        <v>925</v>
       </c>
       <c r="H5" s="40" t="n">
         <v>-10</v>
@@ -13536,13 +13602,13 @@
         <v>100</v>
       </c>
       <c r="J5" s="40" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="K5" s="40" t="s">
-        <v>903</v>
+        <v>906</v>
       </c>
       <c r="L5" s="40" t="s">
-        <v>918</v>
+        <v>921</v>
       </c>
     </row>
   </sheetData>
@@ -13563,8 +13629,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A62" activeCellId="0" sqref="A62"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C67" activeCellId="0" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13600,13 +13666,13 @@
         <v>108</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>923</v>
+        <v>926</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>924</v>
+        <v>927</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>925</v>
+        <v>928</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -13616,13 +13682,13 @@
         <v>108</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>926</v>
+        <v>929</v>
       </c>
       <c r="C3" s="26" t="s">
-        <v>927</v>
+        <v>930</v>
       </c>
       <c r="D3" s="26" t="s">
-        <v>928</v>
+        <v>931</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -13632,13 +13698,13 @@
         <v>403</v>
       </c>
       <c r="B4" s="26" t="s">
-        <v>929</v>
+        <v>932</v>
       </c>
       <c r="C4" s="26" t="s">
-        <v>930</v>
+        <v>933</v>
       </c>
       <c r="D4" s="26" t="s">
-        <v>931</v>
+        <v>934</v>
       </c>
       <c r="E4" s="26"/>
     </row>
@@ -13647,13 +13713,13 @@
         <v>403</v>
       </c>
       <c r="B5" s="26" t="s">
-        <v>932</v>
+        <v>935</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>933</v>
+        <v>936</v>
       </c>
       <c r="D5" s="26" t="s">
-        <v>934</v>
+        <v>937</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13661,13 +13727,13 @@
         <v>403</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>935</v>
+        <v>938</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>936</v>
+        <v>939</v>
       </c>
       <c r="D6" s="26" t="s">
-        <v>937</v>
+        <v>940</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13675,13 +13741,13 @@
         <v>403</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>938</v>
+        <v>941</v>
       </c>
       <c r="C7" s="26" t="s">
-        <v>939</v>
+        <v>942</v>
       </c>
       <c r="D7" s="26" t="s">
-        <v>940</v>
+        <v>943</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13689,13 +13755,13 @@
         <v>403</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>941</v>
+        <v>944</v>
       </c>
       <c r="C8" s="26" t="s">
-        <v>942</v>
+        <v>945</v>
       </c>
       <c r="D8" s="26" t="s">
-        <v>943</v>
+        <v>946</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13703,13 +13769,13 @@
         <v>403</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>944</v>
+        <v>947</v>
       </c>
       <c r="C9" s="26" t="s">
-        <v>945</v>
+        <v>948</v>
       </c>
       <c r="D9" s="26" t="s">
-        <v>946</v>
+        <v>949</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13717,13 +13783,13 @@
         <v>403</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>947</v>
+        <v>950</v>
       </c>
       <c r="C10" s="26" t="s">
-        <v>948</v>
+        <v>951</v>
       </c>
       <c r="D10" s="26" t="s">
-        <v>949</v>
+        <v>952</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13731,13 +13797,13 @@
         <v>403</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>950</v>
+        <v>953</v>
       </c>
       <c r="C11" s="26" t="s">
-        <v>951</v>
+        <v>954</v>
       </c>
       <c r="D11" s="26" t="s">
-        <v>952</v>
+        <v>955</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13745,13 +13811,13 @@
         <v>403</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>953</v>
+        <v>956</v>
       </c>
       <c r="C12" s="26" t="s">
-        <v>954</v>
+        <v>957</v>
       </c>
       <c r="D12" s="26" t="s">
-        <v>955</v>
+        <v>958</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13759,13 +13825,13 @@
         <v>403</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>956</v>
+        <v>959</v>
       </c>
       <c r="C13" s="26" t="s">
-        <v>957</v>
+        <v>960</v>
       </c>
       <c r="D13" s="26" t="s">
-        <v>958</v>
+        <v>961</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13773,7 +13839,7 @@
         <v>403</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>959</v>
+        <v>962</v>
       </c>
       <c r="C14" s="26" t="s">
         <v>689</v>
@@ -13787,13 +13853,13 @@
         <v>403</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>960</v>
+        <v>963</v>
       </c>
       <c r="C15" s="26" t="s">
-        <v>961</v>
+        <v>964</v>
       </c>
       <c r="D15" s="26" t="s">
-        <v>962</v>
+        <v>965</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13801,19 +13867,19 @@
         <v>302</v>
       </c>
       <c r="B16" s="26" t="s">
-        <v>963</v>
+        <v>966</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>964</v>
+        <v>967</v>
       </c>
       <c r="D16" s="26" t="s">
-        <v>965</v>
+        <v>968</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>966</v>
+        <v>969</v>
       </c>
       <c r="F16" s="26" t="s">
-        <v>967</v>
+        <v>970</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13821,19 +13887,19 @@
         <v>302</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>968</v>
+        <v>971</v>
       </c>
       <c r="C17" s="26" t="s">
-        <v>969</v>
+        <v>972</v>
       </c>
       <c r="D17" s="26" t="s">
-        <v>970</v>
+        <v>973</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>971</v>
+        <v>974</v>
       </c>
       <c r="F17" s="26" t="s">
-        <v>972</v>
+        <v>975</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13841,19 +13907,19 @@
         <v>302</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>973</v>
+        <v>976</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>974</v>
+        <v>977</v>
       </c>
       <c r="D18" s="26" t="s">
-        <v>975</v>
+        <v>978</v>
       </c>
       <c r="E18" s="26" t="s">
-        <v>976</v>
+        <v>979</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>977</v>
+        <v>980</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13861,19 +13927,19 @@
         <v>302</v>
       </c>
       <c r="B19" s="26" t="s">
-        <v>978</v>
+        <v>981</v>
       </c>
       <c r="C19" s="26" t="s">
-        <v>979</v>
+        <v>982</v>
       </c>
       <c r="D19" s="26" t="s">
-        <v>980</v>
+        <v>983</v>
       </c>
       <c r="E19" s="26" t="s">
-        <v>981</v>
+        <v>984</v>
       </c>
       <c r="F19" s="26" t="s">
-        <v>982</v>
+        <v>985</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13881,19 +13947,19 @@
         <v>302</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>983</v>
+        <v>986</v>
       </c>
       <c r="C20" s="26" t="s">
-        <v>984</v>
+        <v>987</v>
       </c>
       <c r="D20" s="26" t="s">
-        <v>985</v>
+        <v>988</v>
       </c>
       <c r="E20" s="26" t="s">
-        <v>986</v>
+        <v>989</v>
       </c>
       <c r="F20" s="26" t="s">
-        <v>987</v>
+        <v>990</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13901,19 +13967,19 @@
         <v>302</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>988</v>
+        <v>991</v>
       </c>
       <c r="C21" s="26" t="s">
-        <v>989</v>
+        <v>992</v>
       </c>
       <c r="D21" s="26" t="s">
-        <v>990</v>
+        <v>993</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>991</v>
+        <v>994</v>
       </c>
       <c r="F21" s="26" t="s">
-        <v>992</v>
+        <v>995</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13921,13 +13987,13 @@
         <v>302</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>993</v>
+        <v>996</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>994</v>
+        <v>997</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>995</v>
+        <v>998</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13935,13 +14001,13 @@
         <v>302</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>996</v>
+        <v>999</v>
       </c>
       <c r="C23" s="26" t="s">
-        <v>997</v>
+        <v>1000</v>
       </c>
       <c r="D23" s="26" t="s">
-        <v>998</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13949,13 +14015,13 @@
         <v>302</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>999</v>
+        <v>1002</v>
       </c>
       <c r="C24" s="26" t="s">
-        <v>1000</v>
+        <v>1003</v>
       </c>
       <c r="D24" s="26" t="s">
-        <v>1001</v>
+        <v>1004</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13963,13 +14029,13 @@
         <v>302</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>1002</v>
+        <v>1005</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>1003</v>
+        <v>1006</v>
       </c>
       <c r="D25" s="26" t="s">
-        <v>1004</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13977,19 +14043,19 @@
         <v>302</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>1005</v>
+        <v>1008</v>
       </c>
       <c r="C26" s="26" t="s">
-        <v>1006</v>
+        <v>1009</v>
       </c>
       <c r="D26" s="26" t="s">
-        <v>1007</v>
+        <v>1010</v>
       </c>
       <c r="E26" s="26" t="s">
-        <v>1008</v>
+        <v>1011</v>
       </c>
       <c r="F26" s="26" t="s">
-        <v>1009</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13997,13 +14063,13 @@
         <v>302</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>1010</v>
+        <v>1013</v>
       </c>
       <c r="C27" s="26" t="s">
-        <v>1011</v>
+        <v>1014</v>
       </c>
       <c r="D27" s="26" t="s">
-        <v>1012</v>
+        <v>1015</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14011,13 +14077,13 @@
         <v>302</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>1013</v>
+        <v>1016</v>
       </c>
       <c r="C28" s="26" t="s">
-        <v>1014</v>
+        <v>1017</v>
       </c>
       <c r="D28" s="26" t="s">
-        <v>1015</v>
+        <v>1018</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14025,13 +14091,13 @@
         <v>302</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>1016</v>
+        <v>1019</v>
       </c>
       <c r="C29" s="26" t="s">
-        <v>1017</v>
+        <v>1020</v>
       </c>
       <c r="D29" s="26" t="s">
-        <v>1018</v>
+        <v>1021</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14039,13 +14105,13 @@
         <v>302</v>
       </c>
       <c r="B30" s="26" t="s">
-        <v>1019</v>
+        <v>1022</v>
       </c>
       <c r="C30" s="26" t="s">
-        <v>1020</v>
+        <v>1023</v>
       </c>
       <c r="D30" s="26" t="s">
-        <v>1021</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14053,13 +14119,13 @@
         <v>302</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>1022</v>
+        <v>1025</v>
       </c>
       <c r="C31" s="26" t="s">
-        <v>1023</v>
+        <v>1026</v>
       </c>
       <c r="D31" s="26" t="s">
-        <v>1024</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14067,13 +14133,13 @@
         <v>302</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>1025</v>
+        <v>1028</v>
       </c>
       <c r="C32" s="26" t="s">
-        <v>1026</v>
+        <v>1029</v>
       </c>
       <c r="D32" s="26" t="s">
-        <v>1027</v>
+        <v>1030</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14081,13 +14147,13 @@
         <v>302</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>1028</v>
+        <v>1031</v>
       </c>
       <c r="C33" s="26" t="s">
-        <v>1029</v>
+        <v>1032</v>
       </c>
       <c r="D33" s="26" t="s">
-        <v>1030</v>
+        <v>1033</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14095,13 +14161,13 @@
         <v>302</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>1031</v>
+        <v>1034</v>
       </c>
       <c r="C34" s="26" t="s">
-        <v>1032</v>
+        <v>1035</v>
       </c>
       <c r="D34" s="26" t="s">
-        <v>1033</v>
+        <v>1036</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14109,13 +14175,13 @@
         <v>302</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>1034</v>
+        <v>1037</v>
       </c>
       <c r="C35" s="26" t="s">
-        <v>1035</v>
+        <v>1038</v>
       </c>
       <c r="D35" s="26" t="s">
-        <v>1036</v>
+        <v>1039</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14123,13 +14189,13 @@
         <v>302</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>1037</v>
+        <v>1040</v>
       </c>
       <c r="C36" s="26" t="s">
-        <v>1038</v>
+        <v>1041</v>
       </c>
       <c r="D36" s="26" t="s">
-        <v>1039</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14137,13 +14203,13 @@
         <v>302</v>
       </c>
       <c r="B37" s="26" t="s">
-        <v>1040</v>
+        <v>1043</v>
       </c>
       <c r="C37" s="26" t="s">
-        <v>1038</v>
+        <v>1041</v>
       </c>
       <c r="D37" s="26" t="s">
-        <v>1039</v>
+        <v>1042</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14151,13 +14217,13 @@
         <v>302</v>
       </c>
       <c r="B38" s="26" t="s">
-        <v>1041</v>
+        <v>1044</v>
       </c>
       <c r="C38" s="26" t="s">
-        <v>1042</v>
+        <v>1045</v>
       </c>
       <c r="D38" s="26" t="s">
-        <v>1043</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14165,13 +14231,13 @@
         <v>302</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>1044</v>
+        <v>1047</v>
       </c>
       <c r="C39" s="26" t="s">
-        <v>1045</v>
+        <v>1048</v>
       </c>
       <c r="D39" s="26" t="s">
-        <v>1046</v>
+        <v>1049</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14179,13 +14245,13 @@
         <v>302</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>1047</v>
+        <v>1050</v>
       </c>
       <c r="C40" s="26" t="s">
-        <v>1048</v>
+        <v>1051</v>
       </c>
       <c r="D40" s="26" t="s">
-        <v>1049</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14193,13 +14259,13 @@
         <v>302</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>1050</v>
+        <v>1053</v>
       </c>
       <c r="C41" s="26" t="s">
-        <v>1051</v>
+        <v>1054</v>
       </c>
       <c r="D41" s="26" t="s">
-        <v>1052</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14207,13 +14273,13 @@
         <v>302</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>1053</v>
+        <v>1056</v>
       </c>
       <c r="C42" s="26" t="s">
-        <v>1054</v>
+        <v>1057</v>
       </c>
       <c r="D42" s="26" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14221,13 +14287,13 @@
         <v>302</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>1056</v>
+        <v>1059</v>
       </c>
       <c r="C43" s="26" t="s">
-        <v>1057</v>
+        <v>1060</v>
       </c>
       <c r="D43" s="26" t="s">
-        <v>1058</v>
+        <v>1061</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14235,13 +14301,13 @@
         <v>302</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>1059</v>
+        <v>1062</v>
       </c>
       <c r="C44" s="26" t="s">
-        <v>1060</v>
+        <v>1063</v>
       </c>
       <c r="D44" s="26" t="s">
-        <v>1061</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14249,13 +14315,13 @@
         <v>302</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>1062</v>
+        <v>1065</v>
       </c>
       <c r="C45" s="26" t="s">
-        <v>1063</v>
+        <v>1066</v>
       </c>
       <c r="D45" s="26" t="s">
-        <v>1064</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14263,13 +14329,13 @@
         <v>302</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>1065</v>
+        <v>1068</v>
       </c>
       <c r="C46" s="26" t="s">
-        <v>1066</v>
+        <v>1069</v>
       </c>
       <c r="D46" s="26" t="s">
-        <v>1067</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14277,13 +14343,13 @@
         <v>302</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>1068</v>
+        <v>1071</v>
       </c>
       <c r="C47" s="26" t="s">
-        <v>1069</v>
+        <v>1072</v>
       </c>
       <c r="D47" s="26" t="s">
-        <v>1070</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14291,19 +14357,19 @@
         <v>302</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>1071</v>
+        <v>1074</v>
       </c>
       <c r="C48" s="26" t="s">
-        <v>1072</v>
+        <v>1075</v>
       </c>
       <c r="D48" s="26" t="s">
-        <v>1073</v>
+        <v>1076</v>
       </c>
       <c r="E48" s="26" t="s">
-        <v>1074</v>
+        <v>1077</v>
       </c>
       <c r="F48" s="26" t="s">
-        <v>1075</v>
+        <v>1078</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14311,19 +14377,19 @@
         <v>302</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>1076</v>
+        <v>1079</v>
       </c>
       <c r="C49" s="26" t="s">
-        <v>1077</v>
+        <v>1080</v>
       </c>
       <c r="D49" s="26" t="s">
-        <v>1078</v>
+        <v>1081</v>
       </c>
       <c r="E49" s="26" t="s">
-        <v>1079</v>
+        <v>1082</v>
       </c>
       <c r="F49" s="26" t="s">
-        <v>1080</v>
+        <v>1083</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14331,19 +14397,19 @@
         <v>302</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>1081</v>
+        <v>1084</v>
       </c>
       <c r="C50" s="26" t="s">
-        <v>1082</v>
+        <v>1085</v>
       </c>
       <c r="D50" s="26" t="s">
-        <v>1083</v>
+        <v>1086</v>
       </c>
       <c r="E50" s="26" t="s">
-        <v>1084</v>
+        <v>1087</v>
       </c>
       <c r="F50" s="26" t="s">
-        <v>1085</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14351,19 +14417,19 @@
         <v>302</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>1086</v>
+        <v>1089</v>
       </c>
       <c r="C51" s="26" t="s">
-        <v>1087</v>
+        <v>1090</v>
       </c>
       <c r="D51" s="26" t="s">
-        <v>1088</v>
+        <v>1091</v>
       </c>
       <c r="E51" s="26" t="s">
-        <v>1089</v>
+        <v>1092</v>
       </c>
       <c r="F51" s="26" t="s">
-        <v>1090</v>
+        <v>1093</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14371,19 +14437,19 @@
         <v>302</v>
       </c>
       <c r="B52" s="26" t="s">
-        <v>1091</v>
+        <v>1094</v>
       </c>
       <c r="C52" s="26" t="s">
-        <v>1092</v>
+        <v>1095</v>
       </c>
       <c r="D52" s="26" t="s">
-        <v>1093</v>
+        <v>1096</v>
       </c>
       <c r="E52" s="26" t="s">
-        <v>1094</v>
+        <v>1097</v>
       </c>
       <c r="F52" s="26" t="s">
-        <v>1095</v>
+        <v>1098</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14391,19 +14457,19 @@
         <v>302</v>
       </c>
       <c r="B53" s="26" t="s">
-        <v>1096</v>
+        <v>1099</v>
       </c>
       <c r="C53" s="26" t="s">
-        <v>1097</v>
+        <v>1100</v>
       </c>
       <c r="D53" s="26" t="s">
-        <v>1098</v>
+        <v>1101</v>
       </c>
       <c r="E53" s="26" t="s">
-        <v>1099</v>
+        <v>1102</v>
       </c>
       <c r="F53" s="26" t="s">
-        <v>1100</v>
+        <v>1103</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14411,19 +14477,19 @@
         <v>302</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>1101</v>
+        <v>1104</v>
       </c>
       <c r="C54" s="26" t="s">
-        <v>1102</v>
+        <v>1105</v>
       </c>
       <c r="D54" s="26" t="s">
-        <v>1103</v>
+        <v>1106</v>
       </c>
       <c r="E54" s="26" t="s">
-        <v>1104</v>
+        <v>1107</v>
       </c>
       <c r="F54" s="26" t="s">
-        <v>1105</v>
+        <v>1108</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14431,19 +14497,19 @@
         <v>302</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>1106</v>
+        <v>1109</v>
       </c>
       <c r="C55" s="26" t="s">
-        <v>1107</v>
+        <v>1110</v>
       </c>
       <c r="D55" s="26" t="s">
-        <v>1108</v>
+        <v>1111</v>
       </c>
       <c r="E55" s="26" t="s">
-        <v>1109</v>
+        <v>1112</v>
       </c>
       <c r="F55" s="26" t="s">
-        <v>1110</v>
+        <v>1113</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14451,13 +14517,13 @@
         <v>108</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>1111</v>
+        <v>1114</v>
       </c>
       <c r="C56" s="31" t="s">
-        <v>1112</v>
+        <v>1115</v>
       </c>
       <c r="D56" s="31" t="s">
-        <v>1113</v>
+        <v>1116</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14465,13 +14531,13 @@
         <v>108</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>1114</v>
+        <v>1117</v>
       </c>
       <c r="C57" s="31" t="s">
-        <v>1115</v>
+        <v>1118</v>
       </c>
       <c r="D57" s="31" t="s">
-        <v>1116</v>
+        <v>1119</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14479,13 +14545,13 @@
         <v>108</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>1117</v>
+        <v>1120</v>
       </c>
       <c r="C58" s="31" t="s">
-        <v>1118</v>
+        <v>1121</v>
       </c>
       <c r="D58" s="31" t="s">
-        <v>1119</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14493,13 +14559,13 @@
         <v>108</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>1120</v>
+        <v>1123</v>
       </c>
       <c r="C59" s="31" t="s">
-        <v>1121</v>
+        <v>1124</v>
       </c>
       <c r="D59" s="31" t="s">
-        <v>1122</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14507,13 +14573,13 @@
         <v>108</v>
       </c>
       <c r="B60" s="62" t="s">
-        <v>1123</v>
+        <v>1126</v>
       </c>
       <c r="C60" s="31" t="s">
-        <v>1124</v>
+        <v>1127</v>
       </c>
       <c r="D60" s="31" t="s">
-        <v>1125</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14521,13 +14587,13 @@
         <v>108</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>1126</v>
+        <v>1129</v>
       </c>
       <c r="C61" s="31" t="s">
-        <v>1127</v>
+        <v>1130</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>1128</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14535,15 +14601,181 @@
         <v>108</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>1129</v>
+        <v>1132</v>
       </c>
       <c r="C62" s="31" t="s">
-        <v>1130</v>
+        <v>1133</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>1131</v>
-      </c>
-    </row>
+        <v>1134</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="B63" s="53" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C63" s="53" t="s">
+        <v>648</v>
+      </c>
+      <c r="D63" s="53" t="s">
+        <v>649</v>
+      </c>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
+    </row>
+    <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="B64" s="53" t="s">
+        <v>1136</v>
+      </c>
+      <c r="C64" s="53" t="s">
+        <v>846</v>
+      </c>
+      <c r="D64" s="53" t="s">
+        <v>847</v>
+      </c>
+      <c r="E64" s="53"/>
+      <c r="F64" s="53"/>
+    </row>
+    <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="B65" s="53" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C65" s="53" t="s">
+        <v>848</v>
+      </c>
+      <c r="D65" s="53" t="s">
+        <v>849</v>
+      </c>
+      <c r="E65" s="53"/>
+      <c r="F65" s="53"/>
+    </row>
+    <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="33" t="s">
+        <v>302</v>
+      </c>
+      <c r="B66" s="26" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C66" s="26" t="s">
+        <v>851</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>852</v>
+      </c>
+      <c r="E66" s="26" t="s">
+        <v>853</v>
+      </c>
+      <c r="F66" s="26" t="s">
+        <v>854</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="B67" s="53" t="s">
+        <v>1139</v>
+      </c>
+      <c r="C67" s="26" t="s">
+        <v>858</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>859</v>
+      </c>
+      <c r="E67" s="26" t="s">
+        <v>860</v>
+      </c>
+      <c r="F67" s="26" t="s">
+        <v>861</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="33" t="s">
+        <v>403</v>
+      </c>
+      <c r="B68" s="53" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C68" s="26" t="s">
+        <v>863</v>
+      </c>
+      <c r="D68" s="26" t="s">
+        <v>864</v>
+      </c>
+      <c r="E68" s="26" t="s">
+        <v>865</v>
+      </c>
+      <c r="F68" s="26" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B69" s="31" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C69" s="31" t="s">
+        <v>1142</v>
+      </c>
+      <c r="D69" s="31" t="s">
+        <v>1143</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B70" s="31" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C70" s="31" t="s">
+        <v>1145</v>
+      </c>
+      <c r="D70" s="31" t="s">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B71" s="31" t="s">
+        <v>1147</v>
+      </c>
+      <c r="C71" s="31" t="s">
+        <v>1148</v>
+      </c>
+      <c r="D71" s="31" t="s">
+        <v>1149</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="B72" s="31" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C72" s="31" t="s">
+        <v>1151</v>
+      </c>
+      <c r="D72" s="31" t="s">
+        <v>1152</v>
+      </c>
+    </row>
+    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
questionnaire: correctly show the new person popup
fixes #36

This popup is shown in the `tripsIntro` section only, if there are more
than one interviewable person and that person was not manually selected
by the participant in the previous section and the question was not
previously answered for this journey

The value of this popup is set to `true` upon entering the `tripsIntro`
section for the first time for a journey (at journey creation). The widget
will decide whether it should be shown or not in the conditional.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2029" uniqueCount="1181">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2023" uniqueCount="1181">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -880,49 +880,51 @@
     <t xml:space="preserve">Who do you want to continue the interview for?</t>
   </si>
   <si>
+    <t xml:space="preserve">buttonSelectPersonConfirm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sélectionner cette personne et continuer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Select this person and continue</t>
+  </si>
+  <si>
+    <t xml:space="preserve">activePersonTitle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tripsIntro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p class="_center _em" style="margin-bottom: 0;"&gt;Entrevue de **{{nickname}}**&lt;/p&gt;&lt;p class="_center _pale"&gt;•&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;p class="_center _em" style="margin-bottom: 0;"&gt;**{{nickname}}**’s interview&lt;/p&gt;&lt;p class="_center _pale"&gt;•&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Custom because it uses the builtin widget</t>
+  </si>
+  <si>
+    <t xml:space="preserve">buttonSwitchPerson</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changer de personne</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Change person</t>
+  </si>
+  <si>
     <t xml:space="preserve">personNewPerson</t>
   </si>
   <si>
     <t xml:space="preserve">_showNewPersonPopupButton</t>
   </si>
   <si>
-    <t xml:space="preserve">Nous allons débuter avec les déplacements de {{nickname}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We'll start with the trips made by {{nickname}}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buttonSelectPersonConfirm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Sélectionner cette personne et continuer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Select this person and continue</t>
-  </si>
-  <si>
-    <t xml:space="preserve">activePersonTitle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tripsIntro</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p class="_center _em" style="margin-bottom: 0;"&gt;Entrevue de **{{nickname}}**&lt;/p&gt;&lt;p class="_center _pale"&gt;•&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;p class="_center _em" style="margin-bottom: 0;"&gt;**{{nickname}}**’s interview&lt;/p&gt;&lt;p class="_center _pale"&gt;•&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Custom because it uses the builtin widget</t>
-  </si>
-  <si>
-    <t xml:space="preserve">buttonSwitchPerson</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changer de personne</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Change person</t>
+    <t xml:space="preserve">Nous allons vous demander de spécifier les déplacements de **{{nickname}}**.
+L’ordre des personnes interviewées est aléatoire.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We will ask you to specify **{{nickname}}**’s trips.
+The order of the interviewed persons was randomly selected.</t>
   </si>
   <si>
     <t xml:space="preserve">personWhoWillAnswerForThisPerson</t>
@@ -4613,14 +4615,14 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:XFD128"/>
+  <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="M40" activeCellId="0" sqref="M40"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
+      <selection pane="bottomRight" activeCell="H48" activeCellId="0" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6935,7 +6937,7 @@
         <v>257</v>
       </c>
       <c r="B45" s="28" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="C45" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -6944,15 +6946,15 @@
       <c r="D45" s="10" t="s">
         <v>253</v>
       </c>
-      <c r="E45" s="29"/>
+      <c r="E45" s="10"/>
       <c r="F45" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="G45" s="10" t="s">
         <v>258</v>
       </c>
-      <c r="G45" s="10" t="s">
+      <c r="H45" s="10" t="s">
         <v>259</v>
-      </c>
-      <c r="H45" s="10" t="s">
-        <v>260</v>
       </c>
       <c r="I45" s="28"/>
       <c r="J45" s="28"/>
@@ -6971,50 +6973,58 @@
       <c r="W45" s="29"/>
       <c r="X45" s="29"/>
     </row>
-    <row r="46" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
+        <v>260</v>
+      </c>
+      <c r="B46" s="28" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D46" s="28" t="s">
         <v>261</v>
       </c>
-      <c r="B46" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C46" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D46" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="E46" s="10"/>
-      <c r="F46" s="10" t="s">
-        <v>261</v>
+      <c r="E46" s="29"/>
+      <c r="F46" s="29" t="s">
+        <v>260</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>262</v>
       </c>
-      <c r="H46" s="10" t="s">
+      <c r="H46" s="31" t="s">
         <v>263</v>
       </c>
       <c r="I46" s="28"/>
       <c r="J46" s="28"/>
       <c r="K46" s="28"/>
       <c r="L46" s="29"/>
-      <c r="M46" s="29"/>
+      <c r="M46" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="N46" s="29"/>
       <c r="O46" s="29"/>
       <c r="P46" s="29"/>
       <c r="Q46" s="29"/>
       <c r="R46" s="29"/>
       <c r="S46" s="29"/>
-      <c r="T46" s="28"/>
+      <c r="T46" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U46" s="29"/>
       <c r="V46" s="29"/>
       <c r="W46" s="29"/>
       <c r="X46" s="29"/>
-    </row>
-    <row r="47" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y46" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B47" s="28" t="s">
         <v>73</v>
@@ -7024,46 +7034,38 @@
         <v>1</v>
       </c>
       <c r="D47" s="28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E47" s="29"/>
       <c r="F47" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="G47" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="G47" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="H47" s="31" t="s">
+      <c r="H47" s="28" t="s">
         <v>267</v>
       </c>
       <c r="I47" s="28"/>
       <c r="J47" s="28"/>
       <c r="K47" s="28"/>
       <c r="L47" s="29"/>
-      <c r="M47" s="31" t="s">
-        <v>101</v>
-      </c>
+      <c r="M47" s="29"/>
       <c r="N47" s="29"/>
       <c r="O47" s="29"/>
       <c r="P47" s="29"/>
       <c r="Q47" s="29"/>
       <c r="R47" s="29"/>
       <c r="S47" s="29"/>
-      <c r="T47" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T47" s="28"/>
       <c r="U47" s="29"/>
       <c r="V47" s="29"/>
       <c r="W47" s="29"/>
       <c r="X47" s="29"/>
-      <c r="Y47" s="2" t="s">
+    </row>
+    <row r="48" customFormat="false" ht="87.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="10" t="s">
         <v>268</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="10" t="s">
-        <v>269</v>
       </c>
       <c r="B48" s="28" t="s">
         <v>73</v>
@@ -7073,16 +7075,16 @@
         <v>1</v>
       </c>
       <c r="D48" s="28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E48" s="29"/>
-      <c r="F48" s="29" t="s">
+      <c r="F48" s="10" t="s">
         <v>269</v>
       </c>
-      <c r="G48" s="28" t="s">
+      <c r="G48" s="10" t="s">
         <v>270</v>
       </c>
-      <c r="H48" s="28" t="s">
+      <c r="H48" s="10" t="s">
         <v>271</v>
       </c>
       <c r="I48" s="28"/>
@@ -7104,7 +7106,7 @@
     </row>
     <row r="49" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
-        <v>257</v>
+        <v>272</v>
       </c>
       <c r="B49" s="28" t="s">
         <v>73</v>
@@ -7114,17 +7116,17 @@
         <v>1</v>
       </c>
       <c r="D49" s="28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E49" s="29"/>
       <c r="F49" s="10" t="s">
-        <v>258</v>
+        <v>273</v>
       </c>
       <c r="G49" s="10" t="s">
-        <v>259</v>
+        <v>274</v>
       </c>
       <c r="H49" s="10" t="s">
-        <v>260</v>
+        <v>275</v>
       </c>
       <c r="I49" s="28"/>
       <c r="J49" s="28"/>
@@ -7143,9 +7145,9 @@
       <c r="W49" s="29"/>
       <c r="X49" s="29"/>
     </row>
-    <row r="50" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="116.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="B50" s="28" t="s">
         <v>73</v>
@@ -7155,20 +7157,24 @@
         <v>1</v>
       </c>
       <c r="D50" s="28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E50" s="29"/>
       <c r="F50" s="10" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="G50" s="10" t="s">
-        <v>274</v>
+        <v>277</v>
       </c>
       <c r="H50" s="10" t="s">
-        <v>275</v>
-      </c>
-      <c r="I50" s="28"/>
-      <c r="J50" s="28"/>
+        <v>278</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>279</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>280</v>
+      </c>
       <c r="K50" s="28"/>
       <c r="L50" s="29"/>
       <c r="M50" s="29"/>
@@ -7184,9 +7190,9 @@
       <c r="W50" s="29"/>
       <c r="X50" s="29"/>
     </row>
-    <row r="51" customFormat="false" ht="116.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="B51" s="28" t="s">
         <v>73</v>
@@ -7196,23 +7202,23 @@
         <v>1</v>
       </c>
       <c r="D51" s="28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E51" s="29"/>
       <c r="F51" s="10" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="G51" s="10" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="H51" s="10" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="I51" s="10" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="J51" s="10" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="K51" s="28"/>
       <c r="L51" s="29"/>
@@ -7229,9 +7235,9 @@
       <c r="W51" s="29"/>
       <c r="X51" s="29"/>
     </row>
-    <row r="52" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="377.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="B52" s="28" t="s">
         <v>73</v>
@@ -7241,23 +7247,23 @@
         <v>1</v>
       </c>
       <c r="D52" s="28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E52" s="29"/>
-      <c r="F52" s="10" t="s">
-        <v>281</v>
+      <c r="F52" s="29" t="s">
+        <v>287</v>
       </c>
       <c r="G52" s="10" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="H52" s="10" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="I52" s="10" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="J52" s="10" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="K52" s="28"/>
       <c r="L52" s="29"/>
@@ -7274,9 +7280,9 @@
       <c r="W52" s="29"/>
       <c r="X52" s="29"/>
     </row>
-    <row r="53" customFormat="false" ht="377.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="131.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="B53" s="28" t="s">
         <v>73</v>
@@ -7286,23 +7292,23 @@
         <v>1</v>
       </c>
       <c r="D53" s="28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E53" s="29"/>
       <c r="F53" s="29" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="G53" s="10" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="H53" s="10" t="s">
-        <v>289</v>
+        <v>295</v>
       </c>
       <c r="I53" s="10" t="s">
-        <v>290</v>
+        <v>296</v>
       </c>
       <c r="J53" s="10" t="s">
-        <v>291</v>
+        <v>297</v>
       </c>
       <c r="K53" s="28"/>
       <c r="L53" s="29"/>
@@ -7319,126 +7325,122 @@
       <c r="W53" s="29"/>
       <c r="X53" s="29"/>
     </row>
-    <row r="54" customFormat="false" ht="131.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
-        <v>292</v>
+        <v>298</v>
       </c>
       <c r="B54" s="28" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="C54" s="28" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D54" s="28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E54" s="29"/>
-      <c r="F54" s="29" t="s">
-        <v>293</v>
+      <c r="F54" s="10" t="s">
+        <v>299</v>
       </c>
       <c r="G54" s="10" t="s">
-        <v>294</v>
+        <v>300</v>
       </c>
       <c r="H54" s="10" t="s">
-        <v>295</v>
+        <v>301</v>
       </c>
       <c r="I54" s="10" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="J54" s="10" t="s">
-        <v>297</v>
+        <v>303</v>
       </c>
       <c r="K54" s="28"/>
       <c r="L54" s="29"/>
-      <c r="M54" s="29"/>
+      <c r="M54" s="29" t="s">
+        <v>304</v>
+      </c>
       <c r="N54" s="29"/>
-      <c r="O54" s="29"/>
+      <c r="O54" s="29" t="s">
+        <v>305</v>
+      </c>
       <c r="P54" s="29"/>
       <c r="Q54" s="29"/>
       <c r="R54" s="29"/>
       <c r="S54" s="29"/>
-      <c r="T54" s="28"/>
+      <c r="T54" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U54" s="29"/>
       <c r="V54" s="29"/>
       <c r="W54" s="29"/>
       <c r="X54" s="29"/>
     </row>
-    <row r="55" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
-        <v>298</v>
+        <v>306</v>
       </c>
       <c r="B55" s="28" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="C55" s="28" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D55" s="28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E55" s="29"/>
-      <c r="F55" s="10" t="s">
-        <v>299</v>
-      </c>
-      <c r="G55" s="10" t="s">
-        <v>300</v>
-      </c>
-      <c r="H55" s="10" t="s">
-        <v>301</v>
-      </c>
-      <c r="I55" s="10" t="s">
-        <v>302</v>
-      </c>
-      <c r="J55" s="10" t="s">
-        <v>303</v>
-      </c>
+      <c r="F55" s="29" t="s">
+        <v>307</v>
+      </c>
+      <c r="G55" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="H55" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="I55" s="28"/>
+      <c r="J55" s="28"/>
       <c r="K55" s="28"/>
       <c r="L55" s="29"/>
-      <c r="M55" s="29" t="s">
-        <v>304</v>
-      </c>
+      <c r="M55" s="29"/>
       <c r="N55" s="29"/>
-      <c r="O55" s="29" t="s">
-        <v>305</v>
-      </c>
+      <c r="O55" s="29"/>
       <c r="P55" s="29"/>
       <c r="Q55" s="29"/>
       <c r="R55" s="29"/>
       <c r="S55" s="29"/>
-      <c r="T55" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T55" s="28"/>
       <c r="U55" s="29"/>
       <c r="V55" s="29"/>
       <c r="W55" s="29"/>
       <c r="X55" s="29"/>
     </row>
-    <row r="56" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="B56" s="28" t="s">
-        <v>104</v>
+        <v>38</v>
       </c>
       <c r="C56" s="28" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D56" s="28" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="E56" s="29"/>
       <c r="F56" s="29" t="s">
-        <v>307</v>
-      </c>
-      <c r="G56" s="28" t="s">
-        <v>308</v>
-      </c>
-      <c r="H56" s="28" t="s">
-        <v>309</v>
+        <v>310</v>
+      </c>
+      <c r="G56" s="10" t="s">
+        <v>311</v>
+      </c>
+      <c r="H56" s="32" t="s">
+        <v>312</v>
       </c>
       <c r="I56" s="28"/>
       <c r="J56" s="28"/>
@@ -7451,41 +7453,46 @@
       <c r="Q56" s="29"/>
       <c r="R56" s="29"/>
       <c r="S56" s="29"/>
-      <c r="T56" s="28"/>
+      <c r="T56" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U56" s="29"/>
       <c r="V56" s="29"/>
       <c r="W56" s="29"/>
       <c r="X56" s="29"/>
     </row>
-    <row r="57" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="2" customFormat="true" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="10" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="B57" s="28" t="s">
-        <v>38</v>
+        <v>73</v>
       </c>
       <c r="C57" s="28" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D57" s="28" t="s">
-        <v>265</v>
+        <v>313</v>
       </c>
       <c r="E57" s="29"/>
       <c r="F57" s="29" t="s">
-        <v>310</v>
+        <v>260</v>
       </c>
       <c r="G57" s="10" t="s">
-        <v>311</v>
-      </c>
-      <c r="H57" s="32" t="s">
-        <v>312</v>
+        <v>262</v>
+      </c>
+      <c r="H57" s="31" t="s">
+        <v>263</v>
       </c>
       <c r="I57" s="28"/>
       <c r="J57" s="28"/>
       <c r="K57" s="28"/>
       <c r="L57" s="29"/>
-      <c r="M57" s="29"/>
+      <c r="M57" s="31" t="s">
+        <v>101</v>
+      </c>
       <c r="N57" s="29"/>
       <c r="O57" s="29"/>
       <c r="P57" s="29"/>
@@ -7500,10 +7507,13 @@
       <c r="V57" s="29"/>
       <c r="W57" s="29"/>
       <c r="X57" s="29"/>
-    </row>
-    <row r="58" s="2" customFormat="true" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y57" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B58" s="28" t="s">
         <v>73</v>
@@ -7517,47 +7527,42 @@
       </c>
       <c r="E58" s="29"/>
       <c r="F58" s="29" t="s">
-        <v>264</v>
-      </c>
-      <c r="G58" s="10" t="s">
+        <v>265</v>
+      </c>
+      <c r="G58" s="28" t="s">
         <v>266</v>
       </c>
-      <c r="H58" s="31" t="s">
+      <c r="H58" s="28" t="s">
         <v>267</v>
       </c>
       <c r="I58" s="28"/>
       <c r="J58" s="28"/>
       <c r="K58" s="28"/>
       <c r="L58" s="29"/>
-      <c r="M58" s="31" t="s">
-        <v>101</v>
-      </c>
+      <c r="M58" s="29"/>
       <c r="N58" s="29"/>
       <c r="O58" s="29"/>
       <c r="P58" s="29"/>
       <c r="Q58" s="29"/>
       <c r="R58" s="29"/>
       <c r="S58" s="29"/>
-      <c r="T58" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T58" s="28"/>
       <c r="U58" s="29"/>
       <c r="V58" s="29"/>
       <c r="W58" s="29"/>
       <c r="X58" s="29"/>
-      <c r="Y58" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="59" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y58" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="10" t="s">
-        <v>269</v>
+        <v>315</v>
       </c>
       <c r="B59" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C59" s="28" t="b">
+      <c r="C59" s="28" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7565,17 +7570,21 @@
         <v>313</v>
       </c>
       <c r="E59" s="29"/>
-      <c r="F59" s="29" t="s">
-        <v>269</v>
-      </c>
-      <c r="G59" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="H59" s="28" t="s">
-        <v>271</v>
-      </c>
-      <c r="I59" s="28"/>
-      <c r="J59" s="28"/>
+      <c r="F59" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="G59" s="10" t="s">
+        <v>316</v>
+      </c>
+      <c r="H59" s="10" t="s">
+        <v>317</v>
+      </c>
+      <c r="I59" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="J59" s="10" t="s">
+        <v>319</v>
+      </c>
       <c r="K59" s="28"/>
       <c r="L59" s="29"/>
       <c r="M59" s="29"/>
@@ -7585,18 +7594,21 @@
       <c r="Q59" s="29"/>
       <c r="R59" s="29"/>
       <c r="S59" s="29"/>
-      <c r="T59" s="28"/>
+      <c r="T59" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U59" s="29"/>
       <c r="V59" s="29"/>
       <c r="W59" s="29"/>
       <c r="X59" s="29"/>
       <c r="Y59" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="10" t="s">
-        <v>315</v>
+        <v>321</v>
       </c>
       <c r="B60" s="28" t="s">
         <v>73</v>
@@ -7610,19 +7622,17 @@
       </c>
       <c r="E60" s="29"/>
       <c r="F60" s="10" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="G60" s="10" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="H60" s="10" t="s">
-        <v>317</v>
-      </c>
-      <c r="I60" s="10" t="s">
-        <v>318</v>
-      </c>
-      <c r="J60" s="10" t="s">
-        <v>319</v>
+        <v>324</v>
+      </c>
+      <c r="I60" s="10"/>
+      <c r="J60" s="33" t="s">
+        <v>325</v>
       </c>
       <c r="K60" s="28"/>
       <c r="L60" s="29"/>
@@ -7633,26 +7643,23 @@
       <c r="Q60" s="29"/>
       <c r="R60" s="29"/>
       <c r="S60" s="29"/>
-      <c r="T60" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T60" s="28"/>
       <c r="U60" s="29"/>
       <c r="V60" s="29"/>
       <c r="W60" s="29"/>
       <c r="X60" s="29"/>
       <c r="Y60" s="1" t="s">
-        <v>320</v>
-      </c>
-    </row>
-    <row r="61" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="10" t="s">
-        <v>321</v>
+        <v>327</v>
       </c>
       <c r="B61" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C61" s="28" t="n">
+      <c r="C61" s="34" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7661,18 +7668,12 @@
       </c>
       <c r="E61" s="29"/>
       <c r="F61" s="10" t="s">
-        <v>322</v>
-      </c>
-      <c r="G61" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="H61" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="I61" s="10"/>
-      <c r="J61" s="33" t="s">
-        <v>325</v>
-      </c>
+        <v>328</v>
+      </c>
+      <c r="G61" s="10"/>
+      <c r="H61" s="32"/>
+      <c r="I61" s="28"/>
+      <c r="J61" s="28"/>
       <c r="K61" s="28"/>
       <c r="L61" s="29"/>
       <c r="M61" s="29"/>
@@ -7687,13 +7688,10 @@
       <c r="V61" s="29"/>
       <c r="W61" s="29"/>
       <c r="X61" s="29"/>
-      <c r="Y61" s="1" t="s">
-        <v>326</v>
-      </c>
-    </row>
-    <row r="62" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="62" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="10" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="B62" s="28" t="s">
         <v>73</v>
@@ -7705,9 +7703,11 @@
       <c r="D62" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="E62" s="29"/>
-      <c r="F62" s="10" t="s">
-        <v>328</v>
+      <c r="E62" s="29" t="s">
+        <v>327</v>
+      </c>
+      <c r="F62" s="29" t="s">
+        <v>330</v>
       </c>
       <c r="G62" s="10"/>
       <c r="H62" s="32"/>
@@ -7727,10 +7727,13 @@
       <c r="V62" s="29"/>
       <c r="W62" s="29"/>
       <c r="X62" s="29"/>
-    </row>
-    <row r="63" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y62" s="1" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="10" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="B63" s="28" t="s">
         <v>73</v>
@@ -7746,7 +7749,7 @@
         <v>327</v>
       </c>
       <c r="F63" s="29" t="s">
-        <v>330</v>
+        <v>333</v>
       </c>
       <c r="G63" s="10"/>
       <c r="H63" s="32"/>
@@ -7767,12 +7770,12 @@
       <c r="W63" s="29"/>
       <c r="X63" s="29"/>
       <c r="Y63" s="1" t="s">
-        <v>331</v>
-      </c>
-    </row>
-    <row r="64" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="10" t="s">
-        <v>332</v>
+        <v>335</v>
       </c>
       <c r="B64" s="28" t="s">
         <v>73</v>
@@ -7787,13 +7790,21 @@
       <c r="E64" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="F64" s="29" t="s">
-        <v>333</v>
-      </c>
-      <c r="G64" s="10"/>
-      <c r="H64" s="32"/>
-      <c r="I64" s="28"/>
-      <c r="J64" s="28"/>
+      <c r="F64" s="10" t="s">
+        <v>336</v>
+      </c>
+      <c r="G64" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="H64" s="32" t="s">
+        <v>338</v>
+      </c>
+      <c r="I64" s="10" t="s">
+        <v>339</v>
+      </c>
+      <c r="J64" s="10" t="s">
+        <v>340</v>
+      </c>
       <c r="K64" s="28"/>
       <c r="L64" s="29"/>
       <c r="M64" s="29"/>
@@ -7808,16 +7819,13 @@
       <c r="V64" s="29"/>
       <c r="W64" s="29"/>
       <c r="X64" s="29"/>
-      <c r="Y64" s="1" t="s">
-        <v>334</v>
-      </c>
-    </row>
-    <row r="65" customFormat="false" ht="35.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="65" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="10" t="s">
-        <v>335</v>
+        <v>341</v>
       </c>
       <c r="B65" s="28" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="C65" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -7830,25 +7838,29 @@
         <v>327</v>
       </c>
       <c r="F65" s="10" t="s">
-        <v>336</v>
+        <v>342</v>
       </c>
       <c r="G65" s="10" t="s">
-        <v>337</v>
-      </c>
-      <c r="H65" s="32" t="s">
-        <v>338</v>
+        <v>343</v>
+      </c>
+      <c r="H65" s="10" t="s">
+        <v>344</v>
       </c>
       <c r="I65" s="10" t="s">
-        <v>339</v>
+        <v>345</v>
       </c>
       <c r="J65" s="10" t="s">
-        <v>340</v>
+        <v>346</v>
       </c>
       <c r="K65" s="28"/>
       <c r="L65" s="29"/>
-      <c r="M65" s="29"/>
+      <c r="M65" s="29" t="s">
+        <v>347</v>
+      </c>
       <c r="N65" s="29"/>
-      <c r="O65" s="29"/>
+      <c r="O65" s="29" t="s">
+        <v>348</v>
+      </c>
       <c r="P65" s="29"/>
       <c r="Q65" s="29"/>
       <c r="R65" s="29"/>
@@ -7858,10 +7870,13 @@
       <c r="V65" s="29"/>
       <c r="W65" s="29"/>
       <c r="X65" s="29"/>
-    </row>
-    <row r="66" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y65" s="1" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="10" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="B66" s="28" t="s">
         <v>33</v>
@@ -7877,48 +7892,48 @@
         <v>327</v>
       </c>
       <c r="F66" s="10" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
       <c r="G66" s="10" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="H66" s="10" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
       <c r="I66" s="10" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="J66" s="10" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
       <c r="K66" s="28"/>
       <c r="L66" s="29"/>
       <c r="M66" s="29" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="N66" s="29"/>
       <c r="O66" s="29" t="s">
-        <v>348</v>
+        <v>36</v>
       </c>
       <c r="P66" s="29"/>
       <c r="Q66" s="29"/>
       <c r="R66" s="29"/>
       <c r="S66" s="29"/>
-      <c r="T66" s="28"/>
+      <c r="T66" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U66" s="29"/>
       <c r="V66" s="29"/>
       <c r="W66" s="29"/>
       <c r="X66" s="29"/>
-      <c r="Y66" s="1" t="s">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="67" customFormat="false" ht="69.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="67" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="10" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="B67" s="28" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="C67" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -7930,46 +7945,38 @@
       <c r="E67" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="F67" s="10" t="s">
-        <v>351</v>
+      <c r="F67" s="29" t="s">
+        <v>358</v>
       </c>
       <c r="G67" s="10" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="H67" s="10" t="s">
-        <v>353</v>
-      </c>
-      <c r="I67" s="10" t="s">
-        <v>354</v>
-      </c>
-      <c r="J67" s="10" t="s">
-        <v>355</v>
-      </c>
+        <v>360</v>
+      </c>
+      <c r="I67" s="28"/>
+      <c r="J67" s="28"/>
       <c r="K67" s="28"/>
       <c r="L67" s="29"/>
-      <c r="M67" s="29" t="s">
-        <v>356</v>
-      </c>
+      <c r="M67" s="29"/>
       <c r="N67" s="29"/>
-      <c r="O67" s="29" t="s">
-        <v>36</v>
-      </c>
+      <c r="O67" s="29"/>
       <c r="P67" s="29"/>
       <c r="Q67" s="29"/>
       <c r="R67" s="29"/>
       <c r="S67" s="29"/>
-      <c r="T67" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T67" s="28"/>
       <c r="U67" s="29"/>
       <c r="V67" s="29"/>
       <c r="W67" s="29"/>
       <c r="X67" s="29"/>
+      <c r="Y67" s="1" t="s">
+        <v>361</v>
+      </c>
     </row>
     <row r="68" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="10" t="s">
-        <v>357</v>
+        <v>362</v>
       </c>
       <c r="B68" s="28" t="s">
         <v>73</v>
@@ -7985,14 +7992,10 @@
         <v>327</v>
       </c>
       <c r="F68" s="29" t="s">
-        <v>358</v>
-      </c>
-      <c r="G68" s="10" t="s">
-        <v>359</v>
-      </c>
-      <c r="H68" s="10" t="s">
-        <v>360</v>
-      </c>
+        <v>363</v>
+      </c>
+      <c r="G68" s="10"/>
+      <c r="H68" s="32"/>
       <c r="I68" s="28"/>
       <c r="J68" s="28"/>
       <c r="K68" s="28"/>
@@ -8010,12 +8013,12 @@
       <c r="W68" s="29"/>
       <c r="X68" s="29"/>
       <c r="Y68" s="1" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="69" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="10" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B69" s="28" t="s">
         <v>73</v>
@@ -8030,11 +8033,15 @@
       <c r="E69" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="F69" s="29" t="s">
-        <v>363</v>
-      </c>
-      <c r="G69" s="10"/>
-      <c r="H69" s="32"/>
+      <c r="F69" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="G69" s="10" t="s">
+        <v>367</v>
+      </c>
+      <c r="H69" s="10" t="s">
+        <v>368</v>
+      </c>
       <c r="I69" s="28"/>
       <c r="J69" s="28"/>
       <c r="K69" s="28"/>
@@ -8052,12 +8059,12 @@
       <c r="W69" s="29"/>
       <c r="X69" s="29"/>
       <c r="Y69" s="1" t="s">
-        <v>364</v>
-      </c>
-    </row>
-    <row r="70" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="10" t="s">
-        <v>365</v>
+        <v>370</v>
       </c>
       <c r="B70" s="28" t="s">
         <v>73</v>
@@ -8073,16 +8080,20 @@
         <v>327</v>
       </c>
       <c r="F70" s="10" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="G70" s="10" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="H70" s="10" t="s">
-        <v>368</v>
-      </c>
-      <c r="I70" s="28"/>
-      <c r="J70" s="28"/>
+        <v>373</v>
+      </c>
+      <c r="I70" s="10" t="s">
+        <v>374</v>
+      </c>
+      <c r="J70" s="10" t="s">
+        <v>375</v>
+      </c>
       <c r="K70" s="28"/>
       <c r="L70" s="29"/>
       <c r="M70" s="29"/>
@@ -8098,12 +8109,12 @@
       <c r="W70" s="29"/>
       <c r="X70" s="29"/>
       <c r="Y70" s="1" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="10" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="B71" s="28" t="s">
         <v>73</v>
@@ -8119,20 +8130,12 @@
         <v>327</v>
       </c>
       <c r="F71" s="10" t="s">
-        <v>371</v>
-      </c>
-      <c r="G71" s="10" t="s">
-        <v>372</v>
-      </c>
-      <c r="H71" s="10" t="s">
-        <v>373</v>
-      </c>
-      <c r="I71" s="10" t="s">
-        <v>374</v>
-      </c>
-      <c r="J71" s="10" t="s">
-        <v>375</v>
-      </c>
+        <v>378</v>
+      </c>
+      <c r="G71" s="10"/>
+      <c r="H71" s="32"/>
+      <c r="I71" s="28"/>
+      <c r="J71" s="28"/>
       <c r="K71" s="28"/>
       <c r="L71" s="29"/>
       <c r="M71" s="29"/>
@@ -8151,9 +8154,9 @@
         <v>376</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="10" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="B72" s="28" t="s">
         <v>73</v>
@@ -8169,7 +8172,7 @@
         <v>327</v>
       </c>
       <c r="F72" s="10" t="s">
-        <v>378</v>
+        <v>380</v>
       </c>
       <c r="G72" s="10"/>
       <c r="H72" s="32"/>
@@ -8193,9 +8196,9 @@
         <v>376</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="10" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="B73" s="28" t="s">
         <v>73</v>
@@ -8210,13 +8213,21 @@
       <c r="E73" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="F73" s="10" t="s">
-        <v>380</v>
-      </c>
-      <c r="G73" s="10"/>
-      <c r="H73" s="32"/>
-      <c r="I73" s="28"/>
-      <c r="J73" s="28"/>
+      <c r="F73" s="29" t="s">
+        <v>382</v>
+      </c>
+      <c r="G73" s="10" t="s">
+        <v>383</v>
+      </c>
+      <c r="H73" s="10" t="s">
+        <v>384</v>
+      </c>
+      <c r="I73" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="J73" s="10" t="s">
+        <v>386</v>
+      </c>
       <c r="K73" s="28"/>
       <c r="L73" s="29"/>
       <c r="M73" s="29"/>
@@ -8232,12 +8243,12 @@
       <c r="W73" s="29"/>
       <c r="X73" s="29"/>
       <c r="Y73" s="1" t="s">
-        <v>376</v>
-      </c>
-    </row>
-    <row r="74" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="10" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="B74" s="28" t="s">
         <v>73</v>
@@ -8252,20 +8263,20 @@
       <c r="E74" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="F74" s="29" t="s">
-        <v>382</v>
+      <c r="F74" s="10" t="s">
+        <v>389</v>
       </c>
       <c r="G74" s="10" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="H74" s="10" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="I74" s="10" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="J74" s="10" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="K74" s="28"/>
       <c r="L74" s="29"/>
@@ -8282,12 +8293,12 @@
       <c r="W74" s="29"/>
       <c r="X74" s="29"/>
       <c r="Y74" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="75" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>394</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="10" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="B75" s="28" t="s">
         <v>73</v>
@@ -8303,19 +8314,19 @@
         <v>327</v>
       </c>
       <c r="F75" s="10" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="G75" s="10" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="H75" s="10" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="I75" s="10" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="J75" s="10" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="K75" s="28"/>
       <c r="L75" s="29"/>
@@ -8332,12 +8343,12 @@
       <c r="W75" s="29"/>
       <c r="X75" s="29"/>
       <c r="Y75" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-    <row r="76" customFormat="false" ht="44.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="10" t="s">
-        <v>395</v>
+        <v>401</v>
       </c>
       <c r="B76" s="28" t="s">
         <v>73</v>
@@ -8352,21 +8363,17 @@
       <c r="E76" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="F76" s="10" t="s">
-        <v>396</v>
+      <c r="F76" s="29" t="s">
+        <v>402</v>
       </c>
       <c r="G76" s="10" t="s">
-        <v>397</v>
-      </c>
-      <c r="H76" s="10" t="s">
-        <v>398</v>
-      </c>
-      <c r="I76" s="10" t="s">
-        <v>399</v>
-      </c>
-      <c r="J76" s="10" t="s">
-        <v>400</v>
-      </c>
+        <v>403</v>
+      </c>
+      <c r="H76" s="32" t="s">
+        <v>404</v>
+      </c>
+      <c r="I76" s="28"/>
+      <c r="J76" s="28"/>
       <c r="K76" s="28"/>
       <c r="L76" s="29"/>
       <c r="M76" s="29"/>
@@ -8382,12 +8389,12 @@
       <c r="W76" s="29"/>
       <c r="X76" s="29"/>
       <c r="Y76" s="1" t="s">
-        <v>387</v>
-      </c>
-    </row>
-    <row r="77" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>405</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="10" t="s">
-        <v>401</v>
+        <v>406</v>
       </c>
       <c r="B77" s="28" t="s">
         <v>73</v>
@@ -8402,15 +8409,9 @@
       <c r="E77" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="F77" s="29" t="s">
-        <v>402</v>
-      </c>
-      <c r="G77" s="10" t="s">
-        <v>403</v>
-      </c>
-      <c r="H77" s="32" t="s">
-        <v>404</v>
-      </c>
+      <c r="F77" s="29"/>
+      <c r="G77" s="10"/>
+      <c r="H77" s="32"/>
       <c r="I77" s="28"/>
       <c r="J77" s="28"/>
       <c r="K77" s="28"/>
@@ -8431,9 +8432,9 @@
         <v>405</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="41" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="10" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B78" s="28" t="s">
         <v>73</v>
@@ -8471,9 +8472,9 @@
         <v>405</v>
       </c>
     </row>
-    <row r="79" customFormat="false" ht="41.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="10" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="B79" s="28" t="s">
         <v>73</v>
@@ -8485,17 +8486,23 @@
       <c r="D79" s="28" t="s">
         <v>313</v>
       </c>
-      <c r="E79" s="29" t="s">
-        <v>327</v>
-      </c>
-      <c r="F79" s="29"/>
-      <c r="G79" s="10"/>
-      <c r="H79" s="32"/>
+      <c r="E79" s="29"/>
+      <c r="F79" s="29" t="s">
+        <v>409</v>
+      </c>
+      <c r="G79" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="H79" s="10" t="s">
+        <v>411</v>
+      </c>
       <c r="I79" s="28"/>
       <c r="J79" s="28"/>
       <c r="K79" s="28"/>
       <c r="L79" s="29"/>
-      <c r="M79" s="29"/>
+      <c r="M79" s="29" t="s">
+        <v>412</v>
+      </c>
       <c r="N79" s="29"/>
       <c r="O79" s="29"/>
       <c r="P79" s="29"/>
@@ -8508,58 +8515,53 @@
       <c r="W79" s="29"/>
       <c r="X79" s="29"/>
       <c r="Y79" s="1" t="s">
-        <v>405</v>
-      </c>
-    </row>
-    <row r="80" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="80" s="2" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="10" t="s">
-        <v>408</v>
+        <v>260</v>
       </c>
       <c r="B80" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C80" s="34" t="n">
+      <c r="C80" s="28" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D80" s="28" t="s">
-        <v>313</v>
+        <v>414</v>
       </c>
       <c r="E80" s="29"/>
-      <c r="F80" s="29" t="s">
-        <v>409</v>
-      </c>
-      <c r="G80" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="H80" s="10" t="s">
-        <v>411</v>
-      </c>
+      <c r="F80" s="29"/>
+      <c r="G80" s="10"/>
+      <c r="H80" s="31"/>
       <c r="I80" s="28"/>
       <c r="J80" s="28"/>
       <c r="K80" s="28"/>
       <c r="L80" s="29"/>
-      <c r="M80" s="29" t="s">
-        <v>412</v>
-      </c>
+      <c r="M80" s="31"/>
       <c r="N80" s="29"/>
       <c r="O80" s="29"/>
       <c r="P80" s="29"/>
       <c r="Q80" s="29"/>
       <c r="R80" s="29"/>
       <c r="S80" s="29"/>
-      <c r="T80" s="28"/>
+      <c r="T80" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U80" s="29"/>
       <c r="V80" s="29"/>
       <c r="W80" s="29"/>
       <c r="X80" s="29"/>
-      <c r="Y80" s="1" t="s">
-        <v>413</v>
-      </c>
-    </row>
-    <row r="81" s="2" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y80" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B81" s="28" t="s">
         <v>73</v>
@@ -8572,35 +8574,38 @@
         <v>414</v>
       </c>
       <c r="E81" s="29"/>
-      <c r="F81" s="29"/>
-      <c r="G81" s="10"/>
-      <c r="H81" s="31"/>
+      <c r="F81" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="G81" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H81" s="28" t="s">
+        <v>267</v>
+      </c>
       <c r="I81" s="28"/>
       <c r="J81" s="28"/>
       <c r="K81" s="28"/>
       <c r="L81" s="29"/>
-      <c r="M81" s="31"/>
+      <c r="M81" s="29"/>
       <c r="N81" s="29"/>
       <c r="O81" s="29"/>
       <c r="P81" s="29"/>
       <c r="Q81" s="29"/>
       <c r="R81" s="29"/>
       <c r="S81" s="29"/>
-      <c r="T81" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T81" s="28"/>
       <c r="U81" s="29"/>
       <c r="V81" s="29"/>
       <c r="W81" s="29"/>
       <c r="X81" s="29"/>
-      <c r="Y81" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="82" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y81" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="10" t="s">
-        <v>269</v>
+        <v>415</v>
       </c>
       <c r="B82" s="28" t="s">
         <v>73</v>
@@ -8613,17 +8618,21 @@
         <v>414</v>
       </c>
       <c r="E82" s="29"/>
-      <c r="F82" s="29" t="s">
-        <v>269</v>
-      </c>
-      <c r="G82" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="H82" s="28" t="s">
-        <v>271</v>
-      </c>
-      <c r="I82" s="28"/>
-      <c r="J82" s="28"/>
+      <c r="F82" s="10" t="s">
+        <v>416</v>
+      </c>
+      <c r="G82" s="10" t="s">
+        <v>417</v>
+      </c>
+      <c r="H82" s="10" t="s">
+        <v>418</v>
+      </c>
+      <c r="I82" s="10" t="s">
+        <v>419</v>
+      </c>
+      <c r="J82" s="10" t="s">
+        <v>420</v>
+      </c>
       <c r="K82" s="28"/>
       <c r="L82" s="29"/>
       <c r="M82" s="29"/>
@@ -8633,18 +8642,21 @@
       <c r="Q82" s="29"/>
       <c r="R82" s="29"/>
       <c r="S82" s="29"/>
-      <c r="T82" s="28"/>
+      <c r="T82" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U82" s="29"/>
       <c r="V82" s="29"/>
       <c r="W82" s="29"/>
       <c r="X82" s="29"/>
       <c r="Y82" s="1" t="s">
-        <v>314</v>
-      </c>
-    </row>
-    <row r="83" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="10" t="s">
-        <v>415</v>
+        <v>321</v>
       </c>
       <c r="B83" s="28" t="s">
         <v>73</v>
@@ -8658,19 +8670,19 @@
       </c>
       <c r="E83" s="29"/>
       <c r="F83" s="10" t="s">
-        <v>416</v>
+        <v>421</v>
       </c>
       <c r="G83" s="10" t="s">
-        <v>417</v>
+        <v>323</v>
       </c>
       <c r="H83" s="10" t="s">
-        <v>418</v>
+        <v>324</v>
       </c>
       <c r="I83" s="10" t="s">
-        <v>419</v>
-      </c>
-      <c r="J83" s="10" t="s">
-        <v>420</v>
+        <v>422</v>
+      </c>
+      <c r="J83" s="33" t="s">
+        <v>325</v>
       </c>
       <c r="K83" s="28"/>
       <c r="L83" s="29"/>
@@ -8681,26 +8693,23 @@
       <c r="Q83" s="29"/>
       <c r="R83" s="29"/>
       <c r="S83" s="29"/>
-      <c r="T83" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T83" s="28"/>
       <c r="U83" s="29"/>
       <c r="V83" s="29"/>
       <c r="W83" s="29"/>
       <c r="X83" s="29"/>
       <c r="Y83" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="84" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="10" t="s">
-        <v>321</v>
+        <v>423</v>
       </c>
       <c r="B84" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C84" s="28" t="b">
+      <c r="C84" s="34" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8709,20 +8718,12 @@
       </c>
       <c r="E84" s="29"/>
       <c r="F84" s="10" t="s">
-        <v>421</v>
-      </c>
-      <c r="G84" s="10" t="s">
-        <v>323</v>
-      </c>
-      <c r="H84" s="10" t="s">
-        <v>324</v>
-      </c>
-      <c r="I84" s="10" t="s">
-        <v>422</v>
-      </c>
-      <c r="J84" s="33" t="s">
-        <v>325</v>
-      </c>
+        <v>424</v>
+      </c>
+      <c r="G84" s="10"/>
+      <c r="H84" s="32"/>
+      <c r="I84" s="28"/>
+      <c r="J84" s="28"/>
       <c r="K84" s="28"/>
       <c r="L84" s="29"/>
       <c r="M84" s="29"/>
@@ -8738,12 +8739,12 @@
       <c r="W84" s="29"/>
       <c r="X84" s="29"/>
       <c r="Y84" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="85" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="38.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="10" t="s">
-        <v>423</v>
+        <v>425</v>
       </c>
       <c r="B85" s="28" t="s">
         <v>73</v>
@@ -8755,12 +8756,18 @@
       <c r="D85" s="28" t="s">
         <v>414</v>
       </c>
-      <c r="E85" s="29"/>
+      <c r="E85" s="29" t="s">
+        <v>423</v>
+      </c>
       <c r="F85" s="10" t="s">
-        <v>424</v>
-      </c>
-      <c r="G85" s="10"/>
-      <c r="H85" s="32"/>
+        <v>426</v>
+      </c>
+      <c r="G85" s="10" t="s">
+        <v>427</v>
+      </c>
+      <c r="H85" s="10" t="s">
+        <v>427</v>
+      </c>
       <c r="I85" s="28"/>
       <c r="J85" s="28"/>
       <c r="K85" s="28"/>
@@ -8778,12 +8785,12 @@
       <c r="W85" s="29"/>
       <c r="X85" s="29"/>
       <c r="Y85" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="86" customFormat="false" ht="38.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="10" t="s">
-        <v>425</v>
+        <v>414</v>
       </c>
       <c r="B86" s="28" t="s">
         <v>73</v>
@@ -8799,13 +8806,13 @@
         <v>423</v>
       </c>
       <c r="F86" s="10" t="s">
-        <v>426</v>
+        <v>414</v>
       </c>
       <c r="G86" s="10" t="s">
-        <v>427</v>
-      </c>
-      <c r="H86" s="10" t="s">
-        <v>427</v>
+        <v>428</v>
+      </c>
+      <c r="H86" s="32" t="s">
+        <v>429</v>
       </c>
       <c r="I86" s="28"/>
       <c r="J86" s="28"/>
@@ -8824,12 +8831,12 @@
       <c r="W86" s="29"/>
       <c r="X86" s="29"/>
       <c r="Y86" s="1" t="s">
-        <v>268</v>
+        <v>430</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="10" t="s">
-        <v>414</v>
+        <v>431</v>
       </c>
       <c r="B87" s="28" t="s">
         <v>73</v>
@@ -8842,17 +8849,13 @@
         <v>414</v>
       </c>
       <c r="E87" s="29" t="s">
-        <v>423</v>
+        <v>414</v>
       </c>
       <c r="F87" s="10" t="s">
-        <v>414</v>
-      </c>
-      <c r="G87" s="10" t="s">
-        <v>428</v>
-      </c>
-      <c r="H87" s="32" t="s">
-        <v>429</v>
-      </c>
+        <v>432</v>
+      </c>
+      <c r="G87" s="10"/>
+      <c r="H87" s="32"/>
       <c r="I87" s="28"/>
       <c r="J87" s="28"/>
       <c r="K87" s="28"/>
@@ -8870,12 +8873,12 @@
       <c r="W87" s="29"/>
       <c r="X87" s="29"/>
       <c r="Y87" s="1" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="10" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
       <c r="B88" s="28" t="s">
         <v>73</v>
@@ -8891,7 +8894,7 @@
         <v>414</v>
       </c>
       <c r="F88" s="10" t="s">
-        <v>432</v>
+        <v>435</v>
       </c>
       <c r="G88" s="10"/>
       <c r="H88" s="32"/>
@@ -8912,12 +8915,12 @@
       <c r="W88" s="29"/>
       <c r="X88" s="29"/>
       <c r="Y88" s="1" t="s">
-        <v>433</v>
+        <v>436</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="10" t="s">
-        <v>434</v>
+        <v>437</v>
       </c>
       <c r="B89" s="28" t="s">
         <v>73</v>
@@ -8933,7 +8936,7 @@
         <v>414</v>
       </c>
       <c r="F89" s="10" t="s">
-        <v>435</v>
+        <v>438</v>
       </c>
       <c r="G89" s="10"/>
       <c r="H89" s="32"/>
@@ -8957,9 +8960,9 @@
         <v>436</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="71.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="10" t="s">
-        <v>437</v>
+        <v>439</v>
       </c>
       <c r="B90" s="28" t="s">
         <v>73</v>
@@ -8975,13 +8978,21 @@
         <v>414</v>
       </c>
       <c r="F90" s="10" t="s">
-        <v>438</v>
-      </c>
-      <c r="G90" s="10"/>
-      <c r="H90" s="32"/>
-      <c r="I90" s="28"/>
-      <c r="J90" s="28"/>
-      <c r="K90" s="28"/>
+        <v>440</v>
+      </c>
+      <c r="G90" s="10" t="s">
+        <v>441</v>
+      </c>
+      <c r="H90" s="10" t="s">
+        <v>442</v>
+      </c>
+      <c r="I90" s="10" t="s">
+        <v>443</v>
+      </c>
+      <c r="J90" s="15" t="s">
+        <v>444</v>
+      </c>
+      <c r="K90" s="15"/>
       <c r="L90" s="29"/>
       <c r="M90" s="29"/>
       <c r="N90" s="29"/>
@@ -8990,21 +9001,21 @@
       <c r="Q90" s="29"/>
       <c r="R90" s="29"/>
       <c r="S90" s="29"/>
-      <c r="T90" s="28"/>
+      <c r="T90" s="15"/>
       <c r="U90" s="29"/>
       <c r="V90" s="29"/>
       <c r="W90" s="29"/>
       <c r="X90" s="29"/>
       <c r="Y90" s="1" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="91" customFormat="false" ht="71.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>445</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="10" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="B91" s="28" t="s">
-        <v>73</v>
+        <v>33</v>
       </c>
       <c r="C91" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -9017,44 +9028,44 @@
         <v>414</v>
       </c>
       <c r="F91" s="10" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="G91" s="10" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="H91" s="10" t="s">
-        <v>442</v>
-      </c>
-      <c r="I91" s="10" t="s">
-        <v>443</v>
-      </c>
-      <c r="J91" s="15" t="s">
-        <v>444</v>
-      </c>
+        <v>449</v>
+      </c>
+      <c r="I91" s="15"/>
+      <c r="J91" s="15"/>
       <c r="K91" s="15"/>
       <c r="L91" s="29"/>
-      <c r="M91" s="29"/>
+      <c r="M91" s="29" t="s">
+        <v>450</v>
+      </c>
       <c r="N91" s="29"/>
-      <c r="O91" s="29"/>
+      <c r="O91" s="29" t="s">
+        <v>165</v>
+      </c>
       <c r="P91" s="29"/>
       <c r="Q91" s="29"/>
       <c r="R91" s="29"/>
       <c r="S91" s="29"/>
-      <c r="T91" s="15"/>
+      <c r="T91" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U91" s="29"/>
       <c r="V91" s="29"/>
       <c r="W91" s="29"/>
       <c r="X91" s="29"/>
-      <c r="Y91" s="1" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="92" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="92" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="10" t="s">
-        <v>446</v>
+        <v>451</v>
       </c>
       <c r="B92" s="28" t="s">
-        <v>33</v>
+        <v>77</v>
       </c>
       <c r="C92" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -9067,25 +9078,25 @@
         <v>414</v>
       </c>
       <c r="F92" s="10" t="s">
-        <v>447</v>
+        <v>452</v>
       </c>
       <c r="G92" s="10" t="s">
-        <v>448</v>
+        <v>453</v>
       </c>
       <c r="H92" s="10" t="s">
-        <v>449</v>
+        <v>454</v>
       </c>
       <c r="I92" s="15"/>
       <c r="J92" s="15"/>
-      <c r="K92" s="15"/>
+      <c r="K92" s="8" t="s">
+        <v>455</v>
+      </c>
       <c r="L92" s="29"/>
       <c r="M92" s="29" t="s">
-        <v>450</v>
+        <v>456</v>
       </c>
       <c r="N92" s="29"/>
-      <c r="O92" s="29" t="s">
-        <v>165</v>
-      </c>
+      <c r="O92" s="29"/>
       <c r="P92" s="29"/>
       <c r="Q92" s="29"/>
       <c r="R92" s="29"/>
@@ -9099,12 +9110,12 @@
       <c r="W92" s="29"/>
       <c r="X92" s="29"/>
     </row>
-    <row r="93" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="10" t="s">
-        <v>451</v>
+        <v>457</v>
       </c>
       <c r="B93" s="28" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C93" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -9117,23 +9128,19 @@
         <v>414</v>
       </c>
       <c r="F93" s="10" t="s">
-        <v>452</v>
-      </c>
-      <c r="G93" s="10" t="s">
-        <v>453</v>
+        <v>458</v>
+      </c>
+      <c r="G93" s="35" t="s">
+        <v>459</v>
       </c>
       <c r="H93" s="10" t="s">
-        <v>454</v>
+        <v>460</v>
       </c>
       <c r="I93" s="15"/>
       <c r="J93" s="15"/>
-      <c r="K93" s="8" t="s">
-        <v>455</v>
-      </c>
+      <c r="K93" s="15"/>
       <c r="L93" s="29"/>
-      <c r="M93" s="29" t="s">
-        <v>456</v>
-      </c>
+      <c r="M93" s="29"/>
       <c r="N93" s="29"/>
       <c r="O93" s="29"/>
       <c r="P93" s="29"/>
@@ -9148,17 +9155,20 @@
       <c r="V93" s="29"/>
       <c r="W93" s="29"/>
       <c r="X93" s="29"/>
+      <c r="Y93" s="1" t="s">
+        <v>461</v>
+      </c>
     </row>
     <row r="94" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A94" s="10" t="s">
-        <v>457</v>
+        <v>462</v>
       </c>
       <c r="B94" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C94" s="34" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="C94" s="19" t="b">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
       <c r="D94" s="28" t="s">
         <v>414</v>
@@ -9167,13 +9177,13 @@
         <v>414</v>
       </c>
       <c r="F94" s="10" t="s">
-        <v>458</v>
-      </c>
-      <c r="G94" s="35" t="s">
-        <v>459</v>
+        <v>463</v>
+      </c>
+      <c r="G94" s="10" t="s">
+        <v>464</v>
       </c>
       <c r="H94" s="10" t="s">
-        <v>460</v>
+        <v>465</v>
       </c>
       <c r="I94" s="15"/>
       <c r="J94" s="15"/>
@@ -9195,12 +9205,12 @@
       <c r="W94" s="29"/>
       <c r="X94" s="29"/>
       <c r="Y94" s="1" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="95" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="10" t="s">
-        <v>462</v>
+        <v>467</v>
       </c>
       <c r="B95" s="28" t="s">
         <v>73</v>
@@ -9216,13 +9226,13 @@
         <v>414</v>
       </c>
       <c r="F95" s="10" t="s">
-        <v>463</v>
+        <v>468</v>
       </c>
       <c r="G95" s="10" t="s">
-        <v>464</v>
+        <v>469</v>
       </c>
       <c r="H95" s="10" t="s">
-        <v>465</v>
+        <v>470</v>
       </c>
       <c r="I95" s="15"/>
       <c r="J95" s="15"/>
@@ -9244,19 +9254,19 @@
       <c r="W95" s="29"/>
       <c r="X95" s="29"/>
       <c r="Y95" s="1" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="96" customFormat="false" ht="33.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="10" t="s">
-        <v>467</v>
+        <v>472</v>
       </c>
       <c r="B96" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="C96" s="19" t="b">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+        <v>33</v>
+      </c>
+      <c r="C96" s="34" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D96" s="28" t="s">
         <v>414</v>
@@ -9265,26 +9275,30 @@
         <v>414</v>
       </c>
       <c r="F96" s="10" t="s">
-        <v>468</v>
+        <v>473</v>
       </c>
       <c r="G96" s="10" t="s">
-        <v>469</v>
+        <v>474</v>
       </c>
       <c r="H96" s="10" t="s">
-        <v>470</v>
+        <v>475</v>
       </c>
       <c r="I96" s="15"/>
       <c r="J96" s="15"/>
       <c r="K96" s="15"/>
       <c r="L96" s="29"/>
-      <c r="M96" s="29"/>
+      <c r="M96" s="29" t="s">
+        <v>476</v>
+      </c>
       <c r="N96" s="29"/>
-      <c r="O96" s="29"/>
+      <c r="O96" s="29" t="s">
+        <v>477</v>
+      </c>
       <c r="P96" s="29"/>
       <c r="Q96" s="29"/>
       <c r="R96" s="29"/>
       <c r="S96" s="29"/>
-      <c r="T96" s="15" t="b">
+      <c r="T96" s="28" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9292,16 +9306,13 @@
       <c r="V96" s="29"/>
       <c r="W96" s="29"/>
       <c r="X96" s="29"/>
-      <c r="Y96" s="1" t="s">
-        <v>471</v>
-      </c>
-    </row>
-    <row r="97" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="97" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="10" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="B97" s="28" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C97" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -9314,30 +9325,30 @@
         <v>414</v>
       </c>
       <c r="F97" s="10" t="s">
-        <v>473</v>
+        <v>478</v>
       </c>
       <c r="G97" s="10" t="s">
-        <v>474</v>
+        <v>479</v>
       </c>
       <c r="H97" s="10" t="s">
-        <v>475</v>
+        <v>480</v>
       </c>
       <c r="I97" s="15"/>
       <c r="J97" s="15"/>
       <c r="K97" s="15"/>
       <c r="L97" s="29"/>
       <c r="M97" s="29" t="s">
-        <v>476</v>
-      </c>
-      <c r="N97" s="29"/>
-      <c r="O97" s="29" t="s">
-        <v>477</v>
-      </c>
+        <v>481</v>
+      </c>
+      <c r="N97" s="29" t="s">
+        <v>482</v>
+      </c>
+      <c r="O97" s="29"/>
       <c r="P97" s="29"/>
       <c r="Q97" s="29"/>
       <c r="R97" s="29"/>
       <c r="S97" s="29"/>
-      <c r="T97" s="28" t="b">
+      <c r="T97" s="15" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9346,12 +9357,12 @@
       <c r="W97" s="29"/>
       <c r="X97" s="29"/>
     </row>
-    <row r="98" customFormat="false" ht="48.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="10" t="s">
-        <v>478</v>
+        <v>483</v>
       </c>
       <c r="B98" s="28" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="C98" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -9364,41 +9375,37 @@
         <v>414</v>
       </c>
       <c r="F98" s="10" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="G98" s="10" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="H98" s="10" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="I98" s="15"/>
       <c r="J98" s="15"/>
       <c r="K98" s="15"/>
       <c r="L98" s="29"/>
-      <c r="M98" s="29" t="s">
-        <v>481</v>
-      </c>
-      <c r="N98" s="29" t="s">
-        <v>482</v>
-      </c>
+      <c r="M98" s="29"/>
+      <c r="N98" s="29"/>
       <c r="O98" s="29"/>
       <c r="P98" s="29"/>
       <c r="Q98" s="29"/>
       <c r="R98" s="29"/>
       <c r="S98" s="29"/>
-      <c r="T98" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T98" s="15"/>
       <c r="U98" s="29"/>
       <c r="V98" s="29"/>
       <c r="W98" s="29"/>
       <c r="X98" s="29"/>
-    </row>
-    <row r="99" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y98" s="1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="10" t="s">
-        <v>483</v>
+        <v>488</v>
       </c>
       <c r="B99" s="28" t="s">
         <v>73</v>
@@ -9413,15 +9420,9 @@
       <c r="E99" s="29" t="s">
         <v>414</v>
       </c>
-      <c r="F99" s="10" t="s">
-        <v>484</v>
-      </c>
-      <c r="G99" s="10" t="s">
-        <v>485</v>
-      </c>
-      <c r="H99" s="10" t="s">
-        <v>486</v>
-      </c>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="32"/>
       <c r="I99" s="15"/>
       <c r="J99" s="15"/>
       <c r="K99" s="15"/>
@@ -9439,12 +9440,12 @@
       <c r="W99" s="29"/>
       <c r="X99" s="29"/>
       <c r="Y99" s="1" t="s">
-        <v>487</v>
+        <v>264</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="10" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="B100" s="28" t="s">
         <v>73</v>
@@ -9457,11 +9458,17 @@
         <v>414</v>
       </c>
       <c r="E100" s="29" t="s">
-        <v>414</v>
-      </c>
-      <c r="F100" s="10"/>
-      <c r="G100" s="10"/>
-      <c r="H100" s="32"/>
+        <v>423</v>
+      </c>
+      <c r="F100" s="10" t="s">
+        <v>490</v>
+      </c>
+      <c r="G100" s="10" t="s">
+        <v>491</v>
+      </c>
+      <c r="H100" s="10" t="s">
+        <v>492</v>
+      </c>
       <c r="I100" s="15"/>
       <c r="J100" s="15"/>
       <c r="K100" s="15"/>
@@ -9478,13 +9485,10 @@
       <c r="V100" s="29"/>
       <c r="W100" s="29"/>
       <c r="X100" s="29"/>
-      <c r="Y100" s="1" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="101" customFormat="false" ht="18.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="101" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="10" t="s">
-        <v>489</v>
+        <v>493</v>
       </c>
       <c r="B101" s="28" t="s">
         <v>73</v>
@@ -9496,23 +9500,23 @@
       <c r="D101" s="28" t="s">
         <v>414</v>
       </c>
-      <c r="E101" s="29" t="s">
-        <v>423</v>
-      </c>
-      <c r="F101" s="10" t="s">
-        <v>490</v>
+      <c r="E101" s="29"/>
+      <c r="F101" s="29" t="s">
+        <v>494</v>
       </c>
       <c r="G101" s="10" t="s">
-        <v>491</v>
+        <v>410</v>
       </c>
       <c r="H101" s="10" t="s">
-        <v>492</v>
+        <v>411</v>
       </c>
       <c r="I101" s="15"/>
       <c r="J101" s="15"/>
       <c r="K101" s="15"/>
       <c r="L101" s="29"/>
-      <c r="M101" s="29"/>
+      <c r="M101" s="29" t="s">
+        <v>412</v>
+      </c>
       <c r="N101" s="29"/>
       <c r="O101" s="29"/>
       <c r="P101" s="29"/>
@@ -9524,56 +9528,54 @@
       <c r="V101" s="29"/>
       <c r="W101" s="29"/>
       <c r="X101" s="29"/>
-    </row>
-    <row r="102" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="Y101" s="1" t="s">
+        <v>495</v>
+      </c>
+    </row>
+    <row r="102" s="2" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
-        <v>493</v>
+        <v>260</v>
       </c>
       <c r="B102" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C102" s="34" t="n">
+      <c r="C102" s="28" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D102" s="28" t="s">
-        <v>414</v>
+        <v>496</v>
       </c>
       <c r="E102" s="29"/>
-      <c r="F102" s="29" t="s">
-        <v>494</v>
-      </c>
-      <c r="G102" s="10" t="s">
-        <v>410</v>
-      </c>
-      <c r="H102" s="10" t="s">
-        <v>411</v>
-      </c>
-      <c r="I102" s="15"/>
-      <c r="J102" s="15"/>
-      <c r="K102" s="15"/>
+      <c r="F102" s="29"/>
+      <c r="G102" s="10"/>
+      <c r="H102" s="31"/>
+      <c r="I102" s="28"/>
+      <c r="J102" s="28"/>
+      <c r="K102" s="28"/>
       <c r="L102" s="29"/>
-      <c r="M102" s="29" t="s">
-        <v>412</v>
-      </c>
+      <c r="M102" s="31"/>
       <c r="N102" s="29"/>
       <c r="O102" s="29"/>
       <c r="P102" s="29"/>
       <c r="Q102" s="29"/>
       <c r="R102" s="29"/>
       <c r="S102" s="29"/>
-      <c r="T102" s="15"/>
+      <c r="T102" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U102" s="29"/>
       <c r="V102" s="29"/>
       <c r="W102" s="29"/>
       <c r="X102" s="29"/>
-      <c r="Y102" s="1" t="s">
-        <v>495</v>
-      </c>
-    </row>
-    <row r="103" s="2" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y102" s="2" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="103" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B103" s="28" t="s">
         <v>73</v>
@@ -9586,40 +9588,43 @@
         <v>496</v>
       </c>
       <c r="E103" s="29"/>
-      <c r="F103" s="29"/>
-      <c r="G103" s="10"/>
-      <c r="H103" s="31"/>
+      <c r="F103" s="29" t="s">
+        <v>265</v>
+      </c>
+      <c r="G103" s="28" t="s">
+        <v>266</v>
+      </c>
+      <c r="H103" s="28" t="s">
+        <v>267</v>
+      </c>
       <c r="I103" s="28"/>
       <c r="J103" s="28"/>
       <c r="K103" s="28"/>
       <c r="L103" s="29"/>
-      <c r="M103" s="31"/>
+      <c r="M103" s="29"/>
       <c r="N103" s="29"/>
       <c r="O103" s="29"/>
       <c r="P103" s="29"/>
       <c r="Q103" s="29"/>
       <c r="R103" s="29"/>
       <c r="S103" s="29"/>
-      <c r="T103" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T103" s="28"/>
       <c r="U103" s="29"/>
       <c r="V103" s="29"/>
       <c r="W103" s="29"/>
       <c r="X103" s="29"/>
-      <c r="Y103" s="2" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="104" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="Y103" s="1" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="104" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A104" s="10" t="s">
-        <v>269</v>
+        <v>497</v>
       </c>
       <c r="B104" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C104" s="28" t="b">
+      <c r="C104" s="34" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9628,17 +9633,17 @@
       </c>
       <c r="E104" s="29"/>
       <c r="F104" s="29" t="s">
-        <v>269</v>
-      </c>
-      <c r="G104" s="28" t="s">
-        <v>270</v>
-      </c>
-      <c r="H104" s="28" t="s">
-        <v>271</v>
-      </c>
-      <c r="I104" s="28"/>
-      <c r="J104" s="28"/>
-      <c r="K104" s="28"/>
+        <v>497</v>
+      </c>
+      <c r="G104" s="10" t="s">
+        <v>498</v>
+      </c>
+      <c r="H104" s="10" t="s">
+        <v>499</v>
+      </c>
+      <c r="I104" s="15"/>
+      <c r="J104" s="15"/>
+      <c r="K104" s="15"/>
       <c r="L104" s="29"/>
       <c r="M104" s="29"/>
       <c r="N104" s="29"/>
@@ -9647,21 +9652,24 @@
       <c r="Q104" s="29"/>
       <c r="R104" s="29"/>
       <c r="S104" s="29"/>
-      <c r="T104" s="28"/>
+      <c r="T104" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U104" s="29"/>
       <c r="V104" s="29"/>
       <c r="W104" s="29"/>
       <c r="X104" s="29"/>
       <c r="Y104" s="1" t="s">
-        <v>314</v>
+        <v>500</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A105" s="10" t="s">
-        <v>497</v>
+        <v>501</v>
       </c>
       <c r="B105" s="28" t="s">
-        <v>73</v>
+        <v>502</v>
       </c>
       <c r="C105" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -9671,44 +9679,44 @@
         <v>496</v>
       </c>
       <c r="E105" s="29"/>
-      <c r="F105" s="29" t="s">
-        <v>497</v>
+      <c r="F105" s="10" t="s">
+        <v>503</v>
       </c>
       <c r="G105" s="10" t="s">
-        <v>498</v>
+        <v>504</v>
       </c>
       <c r="H105" s="10" t="s">
-        <v>499</v>
+        <v>505</v>
       </c>
       <c r="I105" s="15"/>
       <c r="J105" s="15"/>
       <c r="K105" s="15"/>
       <c r="L105" s="29"/>
-      <c r="M105" s="29"/>
-      <c r="N105" s="29"/>
-      <c r="O105" s="29"/>
+      <c r="M105" s="29" t="s">
+        <v>506</v>
+      </c>
+      <c r="N105" s="29" t="s">
+        <v>507</v>
+      </c>
+      <c r="O105" s="29" t="s">
+        <v>508</v>
+      </c>
       <c r="P105" s="29"/>
       <c r="Q105" s="29"/>
       <c r="R105" s="29"/>
       <c r="S105" s="29"/>
-      <c r="T105" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T105" s="15"/>
       <c r="U105" s="29"/>
       <c r="V105" s="29"/>
       <c r="W105" s="29"/>
       <c r="X105" s="29"/>
-      <c r="Y105" s="1" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="106" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A106" s="10" t="s">
-        <v>501</v>
+        <v>509</v>
       </c>
       <c r="B106" s="28" t="s">
-        <v>502</v>
+        <v>73</v>
       </c>
       <c r="C106" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -9719,40 +9727,48 @@
       </c>
       <c r="E106" s="29"/>
       <c r="F106" s="10" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="G106" s="10" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="H106" s="10" t="s">
-        <v>505</v>
-      </c>
-      <c r="I106" s="15"/>
-      <c r="J106" s="15"/>
+        <v>512</v>
+      </c>
+      <c r="I106" s="10" t="s">
+        <v>513</v>
+      </c>
+      <c r="J106" s="10" t="s">
+        <v>514</v>
+      </c>
       <c r="K106" s="15"/>
       <c r="L106" s="29"/>
       <c r="M106" s="29" t="s">
-        <v>506</v>
+        <v>515</v>
       </c>
       <c r="N106" s="29" t="s">
-        <v>507</v>
-      </c>
-      <c r="O106" s="29" t="s">
-        <v>508</v>
-      </c>
+        <v>482</v>
+      </c>
+      <c r="O106" s="29"/>
       <c r="P106" s="29"/>
       <c r="Q106" s="29"/>
       <c r="R106" s="29"/>
       <c r="S106" s="29"/>
-      <c r="T106" s="15"/>
+      <c r="T106" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U106" s="29"/>
       <c r="V106" s="29"/>
       <c r="W106" s="29"/>
       <c r="X106" s="29"/>
+      <c r="Y106" s="1" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="107" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A107" s="10" t="s">
-        <v>509</v>
+        <v>517</v>
       </c>
       <c r="B107" s="28" t="s">
         <v>73</v>
@@ -9765,29 +9781,21 @@
         <v>496</v>
       </c>
       <c r="E107" s="29"/>
-      <c r="F107" s="10" t="s">
-        <v>510</v>
+      <c r="F107" s="29" t="s">
+        <v>517</v>
       </c>
       <c r="G107" s="10" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="H107" s="10" t="s">
-        <v>512</v>
-      </c>
-      <c r="I107" s="10" t="s">
-        <v>513</v>
-      </c>
-      <c r="J107" s="10" t="s">
-        <v>514</v>
-      </c>
+        <v>519</v>
+      </c>
+      <c r="I107" s="15"/>
+      <c r="J107" s="15"/>
       <c r="K107" s="15"/>
       <c r="L107" s="29"/>
-      <c r="M107" s="29" t="s">
-        <v>515</v>
-      </c>
-      <c r="N107" s="29" t="s">
-        <v>482</v>
-      </c>
+      <c r="M107" s="29"/>
+      <c r="N107" s="29"/>
       <c r="O107" s="29"/>
       <c r="P107" s="29"/>
       <c r="Q107" s="29"/>
@@ -9802,15 +9810,15 @@
       <c r="W107" s="29"/>
       <c r="X107" s="29"/>
       <c r="Y107" s="1" t="s">
-        <v>516</v>
+        <v>500</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A108" s="10" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="B108" s="28" t="s">
-        <v>73</v>
+        <v>502</v>
       </c>
       <c r="C108" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -9820,44 +9828,44 @@
         <v>496</v>
       </c>
       <c r="E108" s="29"/>
-      <c r="F108" s="29" t="s">
-        <v>517</v>
+      <c r="F108" s="10" t="s">
+        <v>521</v>
       </c>
       <c r="G108" s="10" t="s">
-        <v>518</v>
+        <v>504</v>
       </c>
       <c r="H108" s="10" t="s">
-        <v>519</v>
+        <v>505</v>
       </c>
       <c r="I108" s="15"/>
       <c r="J108" s="15"/>
       <c r="K108" s="15"/>
       <c r="L108" s="29"/>
-      <c r="M108" s="29"/>
-      <c r="N108" s="29"/>
-      <c r="O108" s="29"/>
+      <c r="M108" s="29" t="s">
+        <v>522</v>
+      </c>
+      <c r="N108" s="29" t="s">
+        <v>507</v>
+      </c>
+      <c r="O108" s="29" t="s">
+        <v>523</v>
+      </c>
       <c r="P108" s="29"/>
       <c r="Q108" s="29"/>
       <c r="R108" s="29"/>
       <c r="S108" s="29"/>
-      <c r="T108" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T108" s="15"/>
       <c r="U108" s="29"/>
       <c r="V108" s="29"/>
       <c r="W108" s="29"/>
       <c r="X108" s="29"/>
-      <c r="Y108" s="1" t="s">
-        <v>500</v>
-      </c>
     </row>
     <row r="109" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A109" s="10" t="s">
-        <v>520</v>
+        <v>524</v>
       </c>
       <c r="B109" s="28" t="s">
-        <v>502</v>
+        <v>73</v>
       </c>
       <c r="C109" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -9868,43 +9876,51 @@
       </c>
       <c r="E109" s="29"/>
       <c r="F109" s="10" t="s">
-        <v>521</v>
+        <v>525</v>
       </c>
       <c r="G109" s="10" t="s">
-        <v>504</v>
+        <v>526</v>
       </c>
       <c r="H109" s="10" t="s">
-        <v>505</v>
-      </c>
-      <c r="I109" s="15"/>
-      <c r="J109" s="15"/>
-      <c r="K109" s="15"/>
+        <v>527</v>
+      </c>
+      <c r="I109" s="10" t="s">
+        <v>528</v>
+      </c>
+      <c r="J109" s="10" t="s">
+        <v>529</v>
+      </c>
+      <c r="K109" s="2"/>
       <c r="L109" s="29"/>
       <c r="M109" s="29" t="s">
-        <v>522</v>
+        <v>530</v>
       </c>
       <c r="N109" s="29" t="s">
-        <v>507</v>
-      </c>
-      <c r="O109" s="29" t="s">
-        <v>523</v>
-      </c>
+        <v>482</v>
+      </c>
+      <c r="O109" s="29"/>
       <c r="P109" s="29"/>
       <c r="Q109" s="29"/>
       <c r="R109" s="29"/>
       <c r="S109" s="29"/>
-      <c r="T109" s="15"/>
+      <c r="T109" s="15" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U109" s="29"/>
       <c r="V109" s="29"/>
       <c r="W109" s="29"/>
       <c r="X109" s="29"/>
+      <c r="Y109" s="1" t="s">
+        <v>516</v>
+      </c>
     </row>
     <row r="110" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A110" s="10" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="B110" s="28" t="s">
-        <v>73</v>
+        <v>104</v>
       </c>
       <c r="C110" s="34" t="n">
         <f aca="false">TRUE()</f>
@@ -9914,93 +9930,81 @@
         <v>496</v>
       </c>
       <c r="E110" s="29"/>
-      <c r="F110" s="10" t="s">
-        <v>525</v>
-      </c>
-      <c r="G110" s="10" t="s">
-        <v>526</v>
-      </c>
-      <c r="H110" s="10" t="s">
-        <v>527</v>
-      </c>
-      <c r="I110" s="10" t="s">
-        <v>528</v>
-      </c>
-      <c r="J110" s="10" t="s">
-        <v>529</v>
-      </c>
-      <c r="K110" s="2"/>
+      <c r="F110" s="29" t="s">
+        <v>532</v>
+      </c>
+      <c r="G110" s="28" t="s">
+        <v>308</v>
+      </c>
+      <c r="H110" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="I110" s="29"/>
+      <c r="J110" s="29"/>
+      <c r="K110" s="29"/>
       <c r="L110" s="29"/>
-      <c r="M110" s="29" t="s">
-        <v>530</v>
-      </c>
-      <c r="N110" s="29" t="s">
-        <v>482</v>
-      </c>
+      <c r="M110" s="29"/>
+      <c r="N110" s="29"/>
       <c r="O110" s="29"/>
-      <c r="P110" s="29"/>
+      <c r="P110" s="15"/>
       <c r="Q110" s="29"/>
       <c r="R110" s="29"/>
       <c r="S110" s="29"/>
-      <c r="T110" s="15" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="U110" s="29"/>
-      <c r="V110" s="29"/>
-      <c r="W110" s="29"/>
-      <c r="X110" s="29"/>
-      <c r="Y110" s="1" t="s">
-        <v>516</v>
-      </c>
-    </row>
-    <row r="111" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="T110" s="29"/>
+      <c r="XEA110" s="2"/>
+      <c r="XEB110" s="2"/>
+      <c r="XEC110" s="2"/>
+      <c r="XED110" s="2"/>
+    </row>
+    <row r="111" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A111" s="10" t="s">
-        <v>531</v>
+        <v>533</v>
       </c>
       <c r="B111" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C111" s="34" t="n">
+        <v>33</v>
+      </c>
+      <c r="C111" s="28" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="D111" s="28" t="s">
-        <v>496</v>
+        <v>534</v>
       </c>
       <c r="E111" s="29"/>
       <c r="F111" s="29" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="G111" s="28" t="s">
-        <v>308</v>
+        <v>536</v>
       </c>
       <c r="H111" s="28" t="s">
-        <v>309</v>
-      </c>
-      <c r="I111" s="29"/>
-      <c r="J111" s="29"/>
-      <c r="K111" s="29"/>
+        <v>537</v>
+      </c>
+      <c r="I111" s="15"/>
+      <c r="J111" s="15"/>
+      <c r="K111" s="15"/>
       <c r="L111" s="29"/>
       <c r="M111" s="29"/>
       <c r="N111" s="29"/>
-      <c r="O111" s="29"/>
-      <c r="P111" s="15"/>
+      <c r="O111" s="29" t="s">
+        <v>538</v>
+      </c>
+      <c r="P111" s="29"/>
       <c r="Q111" s="29"/>
       <c r="R111" s="29"/>
       <c r="S111" s="29"/>
-      <c r="T111" s="29"/>
-      <c r="XEA111" s="2"/>
-      <c r="XEB111" s="2"/>
-      <c r="XEC111" s="2"/>
-      <c r="XED111" s="2"/>
-    </row>
-    <row r="112" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T111" s="15"/>
+      <c r="U111" s="29"/>
+      <c r="V111" s="29"/>
+      <c r="W111" s="29"/>
+      <c r="X111" s="29"/>
+    </row>
+    <row r="112" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A112" s="10" t="s">
-        <v>533</v>
+        <v>539</v>
       </c>
       <c r="B112" s="28" t="s">
-        <v>33</v>
+        <v>502</v>
       </c>
       <c r="C112" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10011,13 +10015,13 @@
       </c>
       <c r="E112" s="29"/>
       <c r="F112" s="29" t="s">
-        <v>535</v>
+        <v>540</v>
       </c>
       <c r="G112" s="28" t="s">
-        <v>536</v>
+        <v>541</v>
       </c>
       <c r="H112" s="28" t="s">
-        <v>537</v>
+        <v>542</v>
       </c>
       <c r="I112" s="15"/>
       <c r="J112" s="15"/>
@@ -10025,25 +10029,28 @@
       <c r="L112" s="29"/>
       <c r="M112" s="29"/>
       <c r="N112" s="29"/>
-      <c r="O112" s="29" t="s">
-        <v>538</v>
+      <c r="O112" s="36" t="s">
+        <v>543</v>
       </c>
       <c r="P112" s="29"/>
       <c r="Q112" s="29"/>
       <c r="R112" s="29"/>
       <c r="S112" s="29"/>
-      <c r="T112" s="15"/>
+      <c r="T112" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U112" s="29"/>
       <c r="V112" s="29"/>
       <c r="W112" s="29"/>
       <c r="X112" s="29"/>
     </row>
-    <row r="113" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="10" t="s">
-        <v>539</v>
+        <v>544</v>
       </c>
       <c r="B113" s="28" t="s">
-        <v>502</v>
+        <v>33</v>
       </c>
       <c r="C113" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10053,23 +10060,23 @@
         <v>534</v>
       </c>
       <c r="E113" s="29"/>
-      <c r="F113" s="29" t="s">
-        <v>540</v>
-      </c>
-      <c r="G113" s="28" t="s">
-        <v>541</v>
-      </c>
-      <c r="H113" s="28" t="s">
-        <v>542</v>
+      <c r="F113" s="10" t="s">
+        <v>544</v>
+      </c>
+      <c r="G113" s="37" t="s">
+        <v>545</v>
+      </c>
+      <c r="H113" s="37" t="s">
+        <v>546</v>
       </c>
       <c r="I113" s="15"/>
       <c r="J113" s="15"/>
       <c r="K113" s="15"/>
       <c r="L113" s="29"/>
       <c r="M113" s="29"/>
-      <c r="N113" s="29"/>
-      <c r="O113" s="36" t="s">
-        <v>543</v>
+      <c r="N113" s="2"/>
+      <c r="O113" s="29" t="s">
+        <v>36</v>
       </c>
       <c r="P113" s="29"/>
       <c r="Q113" s="29"/>
@@ -10084,12 +10091,12 @@
       <c r="W113" s="29"/>
       <c r="X113" s="29"/>
     </row>
-    <row r="114" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="10" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="B114" s="28" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C114" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10100,23 +10107,25 @@
       </c>
       <c r="E114" s="29"/>
       <c r="F114" s="10" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="G114" s="37" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="H114" s="37" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="I114" s="15"/>
       <c r="J114" s="15"/>
       <c r="K114" s="15"/>
       <c r="L114" s="29"/>
-      <c r="M114" s="29"/>
-      <c r="N114" s="2"/>
-      <c r="O114" s="29" t="s">
-        <v>36</v>
-      </c>
+      <c r="M114" s="29" t="s">
+        <v>550</v>
+      </c>
+      <c r="N114" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="O114" s="29"/>
       <c r="P114" s="29"/>
       <c r="Q114" s="29"/>
       <c r="R114" s="29"/>
@@ -10130,12 +10139,12 @@
       <c r="W114" s="29"/>
       <c r="X114" s="29"/>
     </row>
-    <row r="115" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="10" t="s">
-        <v>547</v>
+        <v>551</v>
       </c>
       <c r="B115" s="28" t="s">
-        <v>26</v>
+        <v>552</v>
       </c>
       <c r="C115" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10145,24 +10154,22 @@
         <v>534</v>
       </c>
       <c r="E115" s="29"/>
-      <c r="F115" s="10" t="s">
-        <v>547</v>
-      </c>
-      <c r="G115" s="37" t="s">
-        <v>548</v>
-      </c>
-      <c r="H115" s="37" t="s">
-        <v>549</v>
+      <c r="F115" s="29" t="s">
+        <v>553</v>
+      </c>
+      <c r="G115" s="36" t="s">
+        <v>554</v>
+      </c>
+      <c r="H115" s="36" t="s">
+        <v>555</v>
       </c>
       <c r="I115" s="15"/>
       <c r="J115" s="15"/>
       <c r="K115" s="15"/>
       <c r="L115" s="29"/>
-      <c r="M115" s="29" t="s">
-        <v>550</v>
-      </c>
-      <c r="N115" s="8" t="s">
-        <v>45</v>
+      <c r="M115" s="29"/>
+      <c r="N115" s="29" t="s">
+        <v>482</v>
       </c>
       <c r="O115" s="29"/>
       <c r="P115" s="29"/>
@@ -10178,12 +10185,12 @@
       <c r="W115" s="29"/>
       <c r="X115" s="29"/>
     </row>
-    <row r="116" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
-        <v>551</v>
-      </c>
-      <c r="B116" s="28" t="s">
-        <v>552</v>
+        <v>556</v>
+      </c>
+      <c r="B116" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="C116" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10194,22 +10201,20 @@
       </c>
       <c r="E116" s="29"/>
       <c r="F116" s="29" t="s">
-        <v>553</v>
-      </c>
-      <c r="G116" s="36" t="s">
-        <v>554</v>
-      </c>
-      <c r="H116" s="36" t="s">
-        <v>555</v>
+        <v>556</v>
+      </c>
+      <c r="G116" s="28" t="s">
+        <v>557</v>
+      </c>
+      <c r="H116" s="28" t="s">
+        <v>558</v>
       </c>
       <c r="I116" s="15"/>
       <c r="J116" s="15"/>
       <c r="K116" s="15"/>
       <c r="L116" s="29"/>
       <c r="M116" s="29"/>
-      <c r="N116" s="29" t="s">
-        <v>482</v>
-      </c>
+      <c r="N116" s="29"/>
       <c r="O116" s="29"/>
       <c r="P116" s="29"/>
       <c r="Q116" s="29"/>
@@ -10224,12 +10229,12 @@
       <c r="W116" s="29"/>
       <c r="X116" s="29"/>
     </row>
-    <row r="117" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
-        <v>556</v>
-      </c>
-      <c r="B117" s="8" t="s">
-        <v>38</v>
+        <v>559</v>
+      </c>
+      <c r="B117" s="28" t="s">
+        <v>104</v>
       </c>
       <c r="C117" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10239,14 +10244,14 @@
         <v>534</v>
       </c>
       <c r="E117" s="29"/>
-      <c r="F117" s="29" t="s">
-        <v>556</v>
-      </c>
-      <c r="G117" s="28" t="s">
-        <v>557</v>
-      </c>
-      <c r="H117" s="28" t="s">
-        <v>558</v>
+      <c r="F117" s="10" t="s">
+        <v>559</v>
+      </c>
+      <c r="G117" s="10" t="s">
+        <v>560</v>
+      </c>
+      <c r="H117" s="10" t="s">
+        <v>561</v>
       </c>
       <c r="I117" s="15"/>
       <c r="J117" s="15"/>
@@ -10259,10 +10264,7 @@
       <c r="Q117" s="29"/>
       <c r="R117" s="29"/>
       <c r="S117" s="29"/>
-      <c r="T117" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T117" s="15"/>
       <c r="U117" s="29"/>
       <c r="V117" s="29"/>
       <c r="W117" s="29"/>
@@ -10270,10 +10272,10 @@
     </row>
     <row r="118" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="B118" s="28" t="s">
-        <v>104</v>
+        <v>77</v>
       </c>
       <c r="C118" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10283,27 +10285,36 @@
         <v>534</v>
       </c>
       <c r="E118" s="29"/>
-      <c r="F118" s="10" t="s">
-        <v>559</v>
-      </c>
-      <c r="G118" s="10" t="s">
-        <v>560</v>
-      </c>
-      <c r="H118" s="10" t="s">
-        <v>561</v>
+      <c r="F118" s="29" t="s">
+        <v>563</v>
+      </c>
+      <c r="G118" s="28" t="s">
+        <v>564</v>
+      </c>
+      <c r="H118" s="28" t="s">
+        <v>565</v>
       </c>
       <c r="I118" s="15"/>
       <c r="J118" s="15"/>
-      <c r="K118" s="15"/>
+      <c r="K118" s="8" t="s">
+        <v>566</v>
+      </c>
       <c r="L118" s="29"/>
-      <c r="M118" s="29"/>
-      <c r="N118" s="29"/>
+      <c r="M118" s="29" t="s">
+        <v>567</v>
+      </c>
+      <c r="N118" s="10" t="s">
+        <v>568</v>
+      </c>
       <c r="O118" s="29"/>
       <c r="P118" s="29"/>
       <c r="Q118" s="29"/>
       <c r="R118" s="29"/>
       <c r="S118" s="29"/>
-      <c r="T118" s="15"/>
+      <c r="T118" s="28" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
       <c r="U118" s="29"/>
       <c r="V118" s="29"/>
       <c r="W118" s="29"/>
@@ -10311,7 +10322,7 @@
     </row>
     <row r="119" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="B119" s="28" t="s">
         <v>77</v>
@@ -10325,13 +10336,13 @@
       </c>
       <c r="E119" s="29"/>
       <c r="F119" s="29" t="s">
-        <v>563</v>
+        <v>570</v>
       </c>
       <c r="G119" s="28" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="H119" s="28" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="I119" s="15"/>
       <c r="J119" s="15"/>
@@ -10343,7 +10354,7 @@
         <v>567</v>
       </c>
       <c r="N119" s="10" t="s">
-        <v>568</v>
+        <v>573</v>
       </c>
       <c r="O119" s="29"/>
       <c r="P119" s="29"/>
@@ -10361,10 +10372,10 @@
     </row>
     <row r="120" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
-        <v>569</v>
+        <v>574</v>
       </c>
       <c r="B120" s="28" t="s">
-        <v>77</v>
+        <v>575</v>
       </c>
       <c r="C120" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10375,29 +10386,27 @@
       </c>
       <c r="E120" s="29"/>
       <c r="F120" s="29" t="s">
-        <v>570</v>
-      </c>
-      <c r="G120" s="28" t="s">
-        <v>571</v>
-      </c>
-      <c r="H120" s="28" t="s">
-        <v>572</v>
+        <v>576</v>
+      </c>
+      <c r="G120" s="36" t="s">
+        <v>577</v>
+      </c>
+      <c r="H120" s="36" t="s">
+        <v>578</v>
       </c>
       <c r="I120" s="15"/>
       <c r="J120" s="15"/>
-      <c r="K120" s="8" t="s">
-        <v>566</v>
-      </c>
+      <c r="K120" s="15"/>
       <c r="L120" s="29"/>
-      <c r="M120" s="29" t="s">
-        <v>567</v>
-      </c>
-      <c r="N120" s="10" t="s">
-        <v>573</v>
+      <c r="M120" s="29"/>
+      <c r="N120" s="29" t="s">
+        <v>482</v>
       </c>
       <c r="O120" s="29"/>
       <c r="P120" s="29"/>
-      <c r="Q120" s="29"/>
+      <c r="Q120" s="36" t="s">
+        <v>579</v>
+      </c>
       <c r="R120" s="29"/>
       <c r="S120" s="29"/>
       <c r="T120" s="28" t="b">
@@ -10411,10 +10420,10 @@
     </row>
     <row r="121" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
-        <v>574</v>
+        <v>580</v>
       </c>
       <c r="B121" s="28" t="s">
-        <v>575</v>
+        <v>114</v>
       </c>
       <c r="C121" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10425,13 +10434,13 @@
       </c>
       <c r="E121" s="29"/>
       <c r="F121" s="29" t="s">
-        <v>576</v>
+        <v>581</v>
       </c>
       <c r="G121" s="36" t="s">
-        <v>577</v>
+        <v>582</v>
       </c>
       <c r="H121" s="36" t="s">
-        <v>578</v>
+        <v>583</v>
       </c>
       <c r="I121" s="15"/>
       <c r="J121" s="15"/>
@@ -10443,9 +10452,7 @@
       </c>
       <c r="O121" s="29"/>
       <c r="P121" s="29"/>
-      <c r="Q121" s="36" t="s">
-        <v>579</v>
-      </c>
+      <c r="Q121" s="29"/>
       <c r="R121" s="29"/>
       <c r="S121" s="29"/>
       <c r="T121" s="28" t="b">
@@ -10459,10 +10466,10 @@
     </row>
     <row r="122" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
-        <v>580</v>
+        <v>584</v>
       </c>
       <c r="B122" s="28" t="s">
-        <v>114</v>
+        <v>575</v>
       </c>
       <c r="C122" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10473,13 +10480,13 @@
       </c>
       <c r="E122" s="29"/>
       <c r="F122" s="29" t="s">
-        <v>581</v>
+        <v>585</v>
       </c>
       <c r="G122" s="36" t="s">
-        <v>582</v>
+        <v>586</v>
       </c>
       <c r="H122" s="36" t="s">
-        <v>583</v>
+        <v>587</v>
       </c>
       <c r="I122" s="15"/>
       <c r="J122" s="15"/>
@@ -10491,7 +10498,9 @@
       </c>
       <c r="O122" s="29"/>
       <c r="P122" s="29"/>
-      <c r="Q122" s="29"/>
+      <c r="Q122" s="36" t="s">
+        <v>588</v>
+      </c>
       <c r="R122" s="29"/>
       <c r="S122" s="29"/>
       <c r="T122" s="28" t="b">
@@ -10503,9 +10512,9 @@
       <c r="W122" s="29"/>
       <c r="X122" s="29"/>
     </row>
-    <row r="123" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
-        <v>584</v>
+        <v>589</v>
       </c>
       <c r="B123" s="28" t="s">
         <v>575</v>
@@ -10519,13 +10528,13 @@
       </c>
       <c r="E123" s="29"/>
       <c r="F123" s="29" t="s">
-        <v>585</v>
+        <v>590</v>
       </c>
       <c r="G123" s="36" t="s">
-        <v>586</v>
+        <v>591</v>
       </c>
       <c r="H123" s="36" t="s">
-        <v>587</v>
+        <v>592</v>
       </c>
       <c r="I123" s="15"/>
       <c r="J123" s="15"/>
@@ -10538,7 +10547,7 @@
       <c r="O123" s="29"/>
       <c r="P123" s="29"/>
       <c r="Q123" s="36" t="s">
-        <v>588</v>
+        <v>593</v>
       </c>
       <c r="R123" s="29"/>
       <c r="S123" s="29"/>
@@ -10551,9 +10560,9 @@
       <c r="W123" s="29"/>
       <c r="X123" s="29"/>
     </row>
-    <row r="124" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
-        <v>589</v>
+        <v>594</v>
       </c>
       <c r="B124" s="28" t="s">
         <v>575</v>
@@ -10567,13 +10576,13 @@
       </c>
       <c r="E124" s="29"/>
       <c r="F124" s="29" t="s">
-        <v>590</v>
+        <v>595</v>
       </c>
       <c r="G124" s="36" t="s">
-        <v>591</v>
+        <v>596</v>
       </c>
       <c r="H124" s="36" t="s">
-        <v>592</v>
+        <v>597</v>
       </c>
       <c r="I124" s="15"/>
       <c r="J124" s="15"/>
@@ -10586,7 +10595,7 @@
       <c r="O124" s="29"/>
       <c r="P124" s="29"/>
       <c r="Q124" s="36" t="s">
-        <v>593</v>
+        <v>598</v>
       </c>
       <c r="R124" s="29"/>
       <c r="S124" s="29"/>
@@ -10599,12 +10608,12 @@
       <c r="W124" s="29"/>
       <c r="X124" s="29"/>
     </row>
-    <row r="125" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
-        <v>594</v>
+        <v>599</v>
       </c>
       <c r="B125" s="28" t="s">
-        <v>575</v>
+        <v>33</v>
       </c>
       <c r="C125" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10615,13 +10624,13 @@
       </c>
       <c r="E125" s="29"/>
       <c r="F125" s="29" t="s">
-        <v>595</v>
+        <v>600</v>
       </c>
       <c r="G125" s="36" t="s">
-        <v>596</v>
+        <v>601</v>
       </c>
       <c r="H125" s="36" t="s">
-        <v>597</v>
+        <v>602</v>
       </c>
       <c r="I125" s="15"/>
       <c r="J125" s="15"/>
@@ -10631,11 +10640,11 @@
       <c r="N125" s="29" t="s">
         <v>482</v>
       </c>
-      <c r="O125" s="29"/>
+      <c r="O125" s="29" t="s">
+        <v>165</v>
+      </c>
       <c r="P125" s="29"/>
-      <c r="Q125" s="36" t="s">
-        <v>598</v>
-      </c>
+      <c r="Q125" s="29"/>
       <c r="R125" s="29"/>
       <c r="S125" s="29"/>
       <c r="T125" s="28" t="b">
@@ -10647,12 +10656,12 @@
       <c r="W125" s="29"/>
       <c r="X125" s="29"/>
     </row>
-    <row r="126" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
-        <v>599</v>
+        <v>603</v>
       </c>
       <c r="B126" s="28" t="s">
-        <v>33</v>
+        <v>104</v>
       </c>
       <c r="C126" s="28" t="b">
         <f aca="false">TRUE()</f>
@@ -10662,136 +10671,89 @@
         <v>534</v>
       </c>
       <c r="E126" s="29"/>
-      <c r="F126" s="29" t="s">
-        <v>600</v>
-      </c>
-      <c r="G126" s="36" t="s">
-        <v>601</v>
-      </c>
-      <c r="H126" s="36" t="s">
-        <v>602</v>
+      <c r="F126" s="10" t="s">
+        <v>603</v>
+      </c>
+      <c r="G126" s="28" t="s">
+        <v>604</v>
+      </c>
+      <c r="H126" s="10" t="s">
+        <v>605</v>
       </c>
       <c r="I126" s="15"/>
       <c r="J126" s="15"/>
       <c r="K126" s="15"/>
       <c r="L126" s="29"/>
       <c r="M126" s="29"/>
-      <c r="N126" s="29" t="s">
-        <v>482</v>
-      </c>
-      <c r="O126" s="29" t="s">
-        <v>165</v>
-      </c>
+      <c r="N126" s="29"/>
+      <c r="O126" s="29"/>
       <c r="P126" s="29"/>
       <c r="Q126" s="29"/>
       <c r="R126" s="29"/>
       <c r="S126" s="29"/>
-      <c r="T126" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
+      <c r="T126" s="15"/>
       <c r="U126" s="29"/>
       <c r="V126" s="29"/>
       <c r="W126" s="29"/>
       <c r="X126" s="29"/>
     </row>
-    <row r="127" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="10" t="s">
-        <v>603</v>
-      </c>
-      <c r="B127" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="C127" s="28" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D127" s="28" t="s">
-        <v>534</v>
-      </c>
-      <c r="E127" s="29"/>
-      <c r="F127" s="10" t="s">
-        <v>603</v>
-      </c>
-      <c r="G127" s="28" t="s">
-        <v>604</v>
-      </c>
-      <c r="H127" s="10" t="s">
-        <v>605</v>
-      </c>
-      <c r="I127" s="15"/>
-      <c r="J127" s="15"/>
-      <c r="K127" s="15"/>
-      <c r="L127" s="29"/>
-      <c r="M127" s="29"/>
-      <c r="N127" s="29"/>
-      <c r="O127" s="29"/>
-      <c r="P127" s="29"/>
-      <c r="Q127" s="29"/>
-      <c r="R127" s="29"/>
-      <c r="S127" s="29"/>
-      <c r="T127" s="15"/>
-      <c r="U127" s="29"/>
-      <c r="V127" s="29"/>
-      <c r="W127" s="29"/>
-      <c r="X127" s="29"/>
-    </row>
-    <row r="128" customFormat="false" ht="116.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="1" t="s">
+    <row r="127" customFormat="false" ht="116.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A127" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="B128" s="1" t="s">
+      <c r="B127" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C128" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="D128" s="1" t="s">
+      <c r="C127" s="1" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="D127" s="1" t="s">
         <v>607</v>
       </c>
-      <c r="F128" s="1" t="s">
+      <c r="F127" s="1" t="s">
         <v>606</v>
       </c>
-      <c r="G128" s="1" t="s">
+      <c r="G127" s="1" t="s">
         <v>608</v>
       </c>
-      <c r="H128" s="1" t="s">
+      <c r="H127" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="L128" s="38"/>
-      <c r="M128" s="39"/>
-      <c r="T128" s="1" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-    </row>
+      <c r="L127" s="38"/>
+      <c r="M127" s="39"/>
+      <c r="T127" s="1" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:X1"/>
-  <conditionalFormatting sqref="N128:Q128">
+  <conditionalFormatting sqref="N127:Q127">
     <cfRule type="expression" priority="2" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>AND($B1048456="Custom",  $B1048456&lt;&gt;"", ROW(N1048456)&lt;&gt;1)</formula>
+      <formula>AND($B1048455="Custom",  $B1048455&lt;&gt;"", ROW(N1048455)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q128">
+  <conditionalFormatting sqref="Q127">
     <cfRule type="expression" priority="3" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
-      <formula>AND($B128&lt;&gt;"Range", $B128&lt;&gt;"", ROW(Q128)&lt;&gt;1)</formula>
+      <formula>AND($B127&lt;&gt;"Range", $B127&lt;&gt;"", ROW(Q127)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C128">
+  <conditionalFormatting sqref="C127">
     <cfRule type="containsText" priority="4" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="5">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C128)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",C127)))</formula>
     </cfRule>
     <cfRule type="containsText" priority="5" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="TRUE" dxfId="6">
-      <formula>NOT(ISERROR(SEARCH("TRUE",C128)))</formula>
+      <formula>NOT(ISERROR(SEARCH("TRUE",C127)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O128:P128">
+  <conditionalFormatting sqref="O127:P127">
     <cfRule type="expression" priority="6" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="7">
-      <formula>AND($B128&lt;&gt;"Select", $B128&lt;&gt;"Checkbox", $B128&lt;&gt;"Radio",  $B128&lt;&gt;"", ROW(O128)&lt;&gt;1)</formula>
+      <formula>AND($B127&lt;&gt;"Select", $B127&lt;&gt;"Checkbox", $B127&lt;&gt;"Radio",  $B127&lt;&gt;"", ROW(O127)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C129:C1048576 C63:C84 C95:C96 C102:C127 C1:C61">
+  <conditionalFormatting sqref="C128:C1048576 C62:C83 C94:C95 C101:C126 C1:C60">
     <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
@@ -10799,42 +10761,42 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q121">
+  <conditionalFormatting sqref="Q120">
     <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>AND($B1048450="Custom",  $B1048450&lt;&gt;"", ROW(Q1048450)&lt;&gt;1)</formula>
+      <formula>AND($B1048449="Custom",  $B1048449&lt;&gt;"", ROW(Q1048449)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q121 Q124:Q125">
+  <conditionalFormatting sqref="Q120 Q123:Q124">
     <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>AND($B121&lt;&gt;"Range", $B121&lt;&gt;"", ROW(Q121)&lt;&gt;1)</formula>
+      <formula>AND($B120&lt;&gt;"Range", $B120&lt;&gt;"", ROW(Q120)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q124:Q125">
+  <conditionalFormatting sqref="Q123:Q124">
     <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(#ref!="Custom",  #ref!&lt;&gt;"", ROW(#ref!)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O113">
+  <conditionalFormatting sqref="O112">
     <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
-      <formula>AND($B113="Custom",  $B113&lt;&gt;"", ROW(O113)&lt;&gt;1)</formula>
+      <formula>AND($B112="Custom",  $B112&lt;&gt;"", ROW(O112)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O113">
+  <conditionalFormatting sqref="O112">
     <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>AND($B113&lt;&gt;"Select", $B113&lt;&gt;"Checkbox", $B113&lt;&gt;"Radio",  $B113&lt;&gt;"", ROW(O113)&lt;&gt;1)</formula>
+      <formula>AND($B112&lt;&gt;"Select", $B112&lt;&gt;"Checkbox", $B112&lt;&gt;"Radio",  $B112&lt;&gt;"", ROW(O112)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C63:C80 C105:C111 C102">
+  <conditionalFormatting sqref="C62:C79 C104:C110 C101">
     <cfRule type="containsText" priority="14" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C63)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",C62)))</formula>
     </cfRule>
     <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C62:C80 C85:C94 C105:C111 C97:C102">
+  <conditionalFormatting sqref="C61:C79 C84:C93 C104:C110 C96:C101">
     <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
-      <formula>NOT(ISERROR(SEARCH("FALSE",C62)))</formula>
+      <formula>NOT(ISERROR(SEARCH("FALSE",C61)))</formula>
     </cfRule>
     <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>1</formula>
@@ -11740,7 +11702,7 @@
     </row>
     <row r="6" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="33" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B6" s="10" t="s">
         <v>670</v>

</xml_diff>

<commit_message>
questionnaire: fix typo in `personDidTripsIntro` english text
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -997,7 +997,7 @@
 &lt;span class="_red"&gt;- **Ne pas inclure les lieux de transfert** en cours de déplacement (arrêts de bus, gares, terminus, lieux de stationnement, etc.) sauf si vous êtes all{{gender:é/ée/é.e}} reconduire ou chercher quelqu'un à cet endroit.&lt;/span&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Please specify the**places you went on {{assignedDate}}** (include all places visited until 4 AM the following morning).
+    <t xml:space="preserve">Please specify the **places you went on {{assignedDate}}** (include all places visited until 4 AM the following morning).
 &lt;span class="_green"&gt;- **Include short stops and errands** (gas station, daycare/school, convenience store or any place where you picked someone up or dropped someone off).
 - **Include all places** regardless of the mode of transport used to get there (walking, cycling, car, public transit, taxi, plane, boat, etc.).&lt;/span&gt;
 &lt;span class="_red"&gt;- **Do not include transfer locations** (bus stops, train stations, terminals, parking lots, etc.) unless you went there to drop someone off or pick someone up.&lt;/span&gt;</t>
@@ -4618,11 +4618,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C41" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G40" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A41" activeCellId="0" sqref="A41"/>
-      <selection pane="bottomRight" activeCell="H48" activeCellId="0" sqref="H48"/>
+      <selection pane="topRight" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="A40" activeCellId="0" sqref="A40"/>
+      <selection pane="bottomRight" activeCell="H49" activeCellId="0" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
segments: activate busLines questions for Saguenay
part of #63

Add the `busRoutesSaguenay.json` file automatically generated as per the
instructions in the README file from a Transition instance.

Add the implementation of the `busLines` and `busLinesWarning` custom
widgets, copied and adapted from 2024.

Activate the widgets and add missing labels in the Excel file and run
`yarn generateSurvey`.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2173" uniqueCount="1259">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2189" uniqueCount="1271">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -3890,6 +3890,42 @@
   </si>
   <si>
     <t xml:space="preserve">onDemandChoicesJoinedStop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">busLinesOther</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Autre(s) ligne(s) de bus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Other bus line(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">busLinesDontKnow</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ligne(s) inconnue(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unknown line(s)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">busLinesAreCorrect</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Les lignes de bus sont correctes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bus lines are correct</t>
+  </si>
+  <si>
+    <t xml:space="preserve">busLinesWarningRequired</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veuillez valider les lignes de bus ou confirmer que ce sont les bonnes lignes.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please validate the bus lines or confirm that lines are correct.</t>
   </si>
   <si>
     <t xml:space="preserve">nextPlaceRadioChoices.stayedHomeUntilTheNextDay</t>
@@ -4942,11 +4978,11 @@
   <dimension ref="A1:XFD134"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C106" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C97" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A106" activeCellId="0" sqref="A106"/>
-      <selection pane="bottomRight" activeCell="H113" activeCellId="0" sqref="H113"/>
+      <selection pane="bottomLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
+      <selection pane="bottomRight" activeCell="H115" activeCellId="0" sqref="H115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9426,9 +9462,9 @@
       <c r="B93" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C93" s="19" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C93" s="29" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D93" s="28" t="s">
         <v>416</v>
@@ -9475,9 +9511,9 @@
       <c r="B94" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="C94" s="19" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="C94" s="29" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
       </c>
       <c r="D94" s="28" t="s">
         <v>416</v>
@@ -11366,7 +11402,7 @@
       <formula>AND($B134&lt;&gt;"Select", $B134&lt;&gt;"Checkbox", $B134&lt;&gt;"Radio",  $B134&lt;&gt;"", ROW(O134)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C135:C1048576 C61:C82 C93:C94 C1:C59 C100:C133">
+  <conditionalFormatting sqref="C135:C1048576 C61:C82 C1:C59 C100:C133">
     <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
@@ -11407,7 +11443,7 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C60:C78 C83:C92 C95:C100 C103:C114">
+  <conditionalFormatting sqref="C60:C78 C83:C100 C103:C114">
     <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
       <formula>NOT(ISERROR(SEARCH("FALSE",C60)))</formula>
     </cfRule>
@@ -12216,7 +12252,7 @@
   <dimension ref="A1:H12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14677,7 +14713,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F73" activeCellId="0" sqref="F73"/>
+      <selection pane="topLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15766,10 +15802,10 @@
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B69" s="10" t="s">
+      <c r="A69" s="30" t="s">
+        <v>416</v>
+      </c>
+      <c r="B69" s="53" t="s">
         <v>1242</v>
       </c>
       <c r="C69" s="10" t="s">
@@ -15778,12 +15814,14 @@
       <c r="D69" s="10" t="s">
         <v>1244</v>
       </c>
+      <c r="E69" s="10"/>
+      <c r="F69" s="10"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B70" s="10" t="s">
+      <c r="A70" s="30" t="s">
+        <v>416</v>
+      </c>
+      <c r="B70" s="53" t="s">
         <v>1245</v>
       </c>
       <c r="C70" s="10" t="s">
@@ -15792,12 +15830,14 @@
       <c r="D70" s="10" t="s">
         <v>1247</v>
       </c>
+      <c r="E70" s="10"/>
+      <c r="F70" s="10"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="2" t="s">
-        <v>315</v>
-      </c>
-      <c r="B71" s="10" t="s">
+      <c r="A71" s="30" t="s">
+        <v>416</v>
+      </c>
+      <c r="B71" s="53" t="s">
         <v>1248</v>
       </c>
       <c r="C71" s="10" t="s">
@@ -15806,10 +15846,12 @@
       <c r="D71" s="10" t="s">
         <v>1250</v>
       </c>
+      <c r="E71" s="10"/>
+      <c r="F71" s="10"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="2" t="s">
-        <v>315</v>
+      <c r="A72" s="30" t="s">
+        <v>416</v>
       </c>
       <c r="B72" s="10" t="s">
         <v>1251</v>
@@ -15820,111 +15862,165 @@
       <c r="D72" s="10" t="s">
         <v>1253</v>
       </c>
+      <c r="E72" s="10"/>
+      <c r="F72" s="10"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B73" s="1" t="s">
+        <v>315</v>
+      </c>
+      <c r="B73" s="10" t="s">
         <v>1254</v>
       </c>
-      <c r="C73" s="1" t="s">
-        <v>962</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>963</v>
-      </c>
-      <c r="E73" s="1" t="s">
-        <v>964</v>
-      </c>
-      <c r="F73" s="1" t="s">
-        <v>965</v>
+      <c r="C73" s="10" t="s">
+        <v>1255</v>
+      </c>
+      <c r="D73" s="10" t="s">
+        <v>1256</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B74" s="1" t="s">
-        <v>1255</v>
-      </c>
-      <c r="C74" s="1" t="s">
-        <v>966</v>
-      </c>
-      <c r="D74" s="1" t="s">
-        <v>967</v>
-      </c>
-      <c r="E74" s="1" t="s">
-        <v>968</v>
-      </c>
-      <c r="F74" s="1" t="s">
-        <v>969</v>
+        <v>315</v>
+      </c>
+      <c r="B74" s="10" t="s">
+        <v>1257</v>
+      </c>
+      <c r="C74" s="10" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D74" s="10" t="s">
+        <v>1259</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B75" s="21" t="s">
-        <v>1256</v>
-      </c>
-      <c r="C75" s="1" t="s">
-        <v>970</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>971</v>
-      </c>
-      <c r="E75" s="1" t="s">
-        <v>972</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>973</v>
+        <v>315</v>
+      </c>
+      <c r="B75" s="10" t="s">
+        <v>1260</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>1261</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>1262</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B76" s="21" t="s">
-        <v>1257</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>974</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>975</v>
-      </c>
-      <c r="E76" s="1" t="s">
-        <v>976</v>
-      </c>
-      <c r="F76" s="1" t="s">
-        <v>977</v>
+        <v>315</v>
+      </c>
+      <c r="B76" s="10" t="s">
+        <v>1263</v>
+      </c>
+      <c r="C76" s="10" t="s">
+        <v>1264</v>
+      </c>
+      <c r="D76" s="10" t="s">
+        <v>1265</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B77" s="21" t="s">
-        <v>1258</v>
+      <c r="B77" s="1" t="s">
+        <v>1266</v>
       </c>
       <c r="C77" s="1" t="s">
+        <v>962</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>963</v>
+      </c>
+      <c r="E77" s="1" t="s">
+        <v>964</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>965</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B78" s="1" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>966</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>967</v>
+      </c>
+      <c r="E78" s="1" t="s">
+        <v>968</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>969</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B79" s="21" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C79" s="1" t="s">
+        <v>970</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>971</v>
+      </c>
+      <c r="E79" s="1" t="s">
+        <v>972</v>
+      </c>
+      <c r="F79" s="1" t="s">
+        <v>973</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B80" s="21" t="s">
+        <v>1269</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>974</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>975</v>
+      </c>
+      <c r="E80" s="1" t="s">
+        <v>976</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>977</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="B81" s="21" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C81" s="1" t="s">
         <v>978</v>
       </c>
-      <c r="D77" s="1" t="s">
+      <c r="D81" s="1" t="s">
         <v>979</v>
       </c>
-      <c r="E77" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>980</v>
       </c>
-      <c r="F77" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>981</v>
       </c>
     </row>
-    <row r="1048569" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048570" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048571" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048572" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
labels: change default from "iel" to "il/elle" in french
fixes #99

If the gender is unknown or some other value from those defined, then
the person should be adressed as "il/elle" and not "iel", which is for
explicitly custom genders.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -1166,7 +1166,7 @@
     <t xml:space="preserve">onTheRoadArrivalType</t>
   </si>
   <si>
-    <t xml:space="preserve">À quel endroit {{nickname}} a-t-{{gender :il/elle/iel}} terminé ses déplacements sur la route?</t>
+    <t xml:space="preserve">À quel endroit {{nickname}} a-t-{{gender :il/elle/iel/"il/elle"}} terminé ses déplacements sur la route?</t>
   </si>
   <si>
     <t xml:space="preserve">Where did {{nickname}} end {{gender:his/her/their}} work trip on the road?</t>
@@ -1259,7 +1259,7 @@
     <t xml:space="preserve">_previousPreviousDepartureTime</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le lieu précédent ({{visitedPlaceDescription}}) avant de se rendre à son lieu habituel de travail?</t>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/"il/elle"}} quitté le lieu précédent ({{visitedPlaceDescription}}) avant de se rendre à son lieu habituel de travail?</t>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} leave the previous location ({{visitedPlaceDescription}}) before going to {{gender:his/her/their}} usual work place?</t>
@@ -1314,7 +1314,7 @@
   </si>
   <si>
     <t xml:space="preserve">Après avoir été {{atPlace}}, {{nickname}} est…
-__Si {{nickname}} a quitté le lieu après 4h du matin le lendemain, merci de considérer pour l'enquête qu'{{gender :il/elle/iel}} y est rest{{gender :é/ée/é.e}} jusqu'au lendemain et de sélectionner la réponse adaptée.__</t>
+__Si {{nickname}} a quitté le lieu après 4h du matin le lendemain, merci de considérer pour l'enquête qu'{{gender :il/elle/iel/"il/elle"}} y est rest{{gender :é/ée/é.e}} jusqu'au lendemain et de sélectionner la réponse adaptée.__</t>
   </si>
   <si>
     <t xml:space="preserve">After being {{atPlace}}, {{nickname}}…
@@ -1322,11 +1322,11 @@
   </si>
   <si>
     <t xml:space="preserve">Après avoir été {{atPlace}}, vous êtes…
-__Si {{nickname}} a quitté le lieu après 4h du matin le lendemain, merci de considérer pour l'enquête qu'{{gender :il/elle/iel}} y est rest{{gender :é/ée/é.e}} jusqu'au lendemain et de sélectionner la réponse adaptée.__</t>
+__Si vous avez quitté le lieu après 4h du matin le lendemain, merci de considérer pour l'enquête que vous y êtes rest{{gender :é/ée/é.e}} jusqu'au lendemain et de sélectionner la réponse adaptée.__</t>
   </si>
   <si>
     <t xml:space="preserve">After being {{atPlace}}, you…
-__If {{nickname}} left this place after 4 AM the following day, please consider for the purposes of the survey that they stayed there until the next day and select the appropriate answer.__</t>
+__If you left this place after 4 AM the following day, please consider for the purposes of the survey that you stayed there until the next day and select the appropriate answer.__</t>
   </si>
   <si>
     <t xml:space="preserve">Custom because of the labels that include the visited place</t>
@@ -3370,7 +3370,7 @@
     <t xml:space="preserve">PreviousDepartureTime</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le lieu précédent ({{previousVisitedPlaceDescription}})?</t>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/"il/elle"}} quitté le lieu précédent ({{previousVisitedPlaceDescription}})?</t>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} leave the previous location ({{previousVisitedPlaceDescription}})?</t>
@@ -3385,7 +3385,7 @@
     <t xml:space="preserve">PreviousDepartureTime_home_workUsual</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile pour aller au travail?</t>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/"il/elle"}} quitté le domicile pour aller au travail?</t>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} leave home before going to work?</t>
@@ -3400,7 +3400,35 @@
     <t xml:space="preserve">PreviousDepartureTime_home_schoolUsual</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile pour aller au lieu d'études/école?</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/"il/elle"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}} quitté le domicile pour aller au lieu d'études/école?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} leave home before going to school?</t>
@@ -3415,7 +3443,35 @@
     <t xml:space="preserve">PreviousDepartureTime_home_other</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile pour aller à cet endroit ({{visitedPlaceDescription}})?</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/"il/elle"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}} quitté le domicile pour aller à cet endroit ({{visitedPlaceDescription}})?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} leave home before going to this place ({{visitedPlaceDescription}})?</t>
@@ -3430,7 +3486,35 @@
     <t xml:space="preserve">PreviousDepartureTime_home_workOnTheRoad</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté le domicile avant de débuter ses déplacements sur la route?</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/"il/elle"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}} quitté le domicile avant de débuter ses déplacements sur la route?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} leave home before starting {{gender :his/her/their}} on the road trips?</t>
@@ -3445,7 +3529,35 @@
     <t xml:space="preserve">PreviousDepartureTime_usualWorkPlace_workOnTheRoad</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel}} quitté son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/"il/elle"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}} quitté son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">t what time did {{nickname}} leave {{gender :his/her/their}} usual work place before starting {{gender :his/her/their}} on the road trips?</t>
@@ -3709,7 +3821,35 @@
     <t xml:space="preserve">_previousArrivalTimeDepartureTypeHome</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel}} arriv{{gender :é/ée/é.e}} au domicile avant de débuter ses déplacements sur la route?</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/"il/elle"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}} arriv{{gender :é/ée/é.e}} au domicile avant de débuter ses déplacements sur la route?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} arrive home before starting {{gender :his/her/their}} on the road trips?</t>
@@ -3724,7 +3864,35 @@
     <t xml:space="preserve">_previousArrivalTimeDepartureTypeUsualWorkPlace</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel}} arriv{{gender :é/ée/é.e}} à son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/"il/elle"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}} arriv{{gender :é/ée/é.e}} à son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} arrive at his usual work place before starting {{gender :his/her/their}} on the road trips?</t>
@@ -3739,7 +3907,35 @@
     <t xml:space="preserve">_previousArrivalTimeDepartureTypeOther</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel}} arriv{{gender :é/ée/é.e}} au lieu précédent ({{visitedPlaceDescription}}) avant de débuter ses déplacements sur la route?</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">/"il/elle"</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">}} arriv{{gender :é/ée/é.e}} au lieu précédent ({{visitedPlaceDescription}}) avant de débuter ses déplacements sur la route?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} arrive at the previous location ({{visitedPlaceDescription}}) before starting {{gender :his/her/their}} on the road trips?</t>
@@ -4045,7 +4241,7 @@
     <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4223,6 +4419,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -4977,12 +5179,12 @@
   </sheetPr>
   <dimension ref="A1:XFD134"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C97" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C77" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A97" activeCellId="0" sqref="A97"/>
-      <selection pane="bottomRight" activeCell="H115" activeCellId="0" sqref="H115"/>
+      <selection pane="bottomLeft" activeCell="A77" activeCellId="0" sqref="A77"/>
+      <selection pane="bottomRight" activeCell="I89" activeCellId="0" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14712,8 +14914,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C64" activeCellId="0" sqref="C64"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
labels: remove spaces before punctuation signs
fixes #138

Canadian french does not have spaces before various punctuations
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -330,7 +330,7 @@
     <t xml:space="preserve">household_electricBicycleNumber</t>
   </si>
   <si>
-    <t xml:space="preserve">Parmi ces vélos, combien sont des **vélos électriques** ou à assistance électrique ?</t>
+    <t xml:space="preserve">Parmi ces vélos, combien sont des **vélos électriques** ou à assistance électrique?</t>
   </si>
   <si>
     <t xml:space="preserve">Among these bicycles, how many are **electric bicycles** (e-bikes)?</t>
@@ -641,13 +641,13 @@
     <t xml:space="preserve">transitFares</t>
   </si>
   <si>
-    <t xml:space="preserve">Est-ce que {{nickname}} détient présentement **un laissez-passer ou un abonnement** de transport en commun valide ?</t>
+    <t xml:space="preserve">Est-ce que {{nickname}} détient présentement **un laissez-passer ou un abonnement** de transport en commun valide?</t>
   </si>
   <si>
     <t xml:space="preserve">Does {{nickname}} currently have a valid transit **fare, pass or ticket**?</t>
   </si>
   <si>
-    <t xml:space="preserve">Détenez-vous présentement **un laissez-passer ou un abonnement** de transport en commun valide ?</t>
+    <t xml:space="preserve">Détenez-vous présentement **un laissez-passer ou un abonnement** de transport en commun valide?</t>
   </si>
   <si>
     <t xml:space="preserve">Do you currently have a valid transit **fare, pass or ticket**?</t>
@@ -668,7 +668,7 @@
     <t xml:space="preserve">hasDisability</t>
   </si>
   <si>
-    <t xml:space="preserve">**Incapacité permanente d'ordre physique, intellectuelle ou autre** qui influence ou limite ses déplacements quotidiens ?</t>
+    <t xml:space="preserve">**Incapacité permanente d'ordre physique, intellectuelle ou autre** qui influence ou limite ses déplacements quotidiens?</t>
   </si>
   <si>
     <t xml:space="preserve">**Permanent physical, intellectual or other disability** which influences or limits their daily mobility?</t>
@@ -683,13 +683,13 @@
     <t xml:space="preserve">workPlaceType</t>
   </si>
   <si>
-    <t xml:space="preserve">Est-ce que {{nickname}} a un **lieu d'emploi** fixe ?</t>
+    <t xml:space="preserve">Est-ce que {{nickname}} a un **lieu d'emploi** fixe?</t>
   </si>
   <si>
     <t xml:space="preserve">Does {{nickname}} have a fixed **work location**?</t>
   </si>
   <si>
-    <t xml:space="preserve">Avez-vous un **lieu d'emploi** fixe ?</t>
+    <t xml:space="preserve">Avez-vous un **lieu d'emploi** fixe?</t>
   </si>
   <si>
     <t xml:space="preserve">Do you have a fixed **work location**?</t>
@@ -707,13 +707,13 @@
     <t xml:space="preserve">workPlaceTypeBeforeLeave</t>
   </si>
   <si>
-    <t xml:space="preserve">**Avant d’être en congé**, est-ce que {{nickname}} avait un **lieu d'emploi** fixe ?</t>
+    <t xml:space="preserve">**Avant d’être en congé**, est-ce que {{nickname}} avait un **lieu d'emploi** fixe?</t>
   </si>
   <si>
     <t xml:space="preserve">**Before being on leave**, did {{nickname}} have a fixed **work location**?</t>
   </si>
   <si>
-    <t xml:space="preserve">**Avant d’être en congé**, aviez-vous un **lieu d'emploi** fixe ?</t>
+    <t xml:space="preserve">**Avant d’être en congé**, aviez-vous un **lieu d'emploi** fixe?</t>
   </si>
   <si>
     <t xml:space="preserve">**Before being on leave**, did you have a fixed **work location**?</t>
@@ -731,13 +731,13 @@
     <t xml:space="preserve">schoolPlaceType</t>
   </si>
   <si>
-    <t xml:space="preserve">Est-ce que {{nickname}} a un **lieu d'études** fixe ?</t>
+    <t xml:space="preserve">Est-ce que {{nickname}} a un **lieu d'études** fixe?</t>
   </si>
   <si>
     <t xml:space="preserve">Does {{nickname}} have a fixed **study location**?</t>
   </si>
   <si>
-    <t xml:space="preserve">Avez-vous a un **lieu d'études** fixe ?</t>
+    <t xml:space="preserve">Avez-vous a un **lieu d'études** fixe?</t>
   </si>
   <si>
     <t xml:space="preserve">Do you have a fixed **study location**?</t>
@@ -849,7 +849,7 @@
     <t xml:space="preserve">travelToWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la dernière **semaine**, quand est-ce que {{nickname}} s'est **déplacé{{gender:/e/·e}}** pour le **travail** ?
+    <t xml:space="preserve">Durant la dernière **semaine**, quand est-ce que {{nickname}} s'est **déplacé{{gender:/e/·e}}** pour le **travail**?
 __Pour se rendre au travail ou toute autre raison concernant le travail.__</t>
   </si>
   <si>
@@ -857,7 +857,7 @@
 __To get to or for any other reason concerning work.__</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la dernière **semaine**, quand vous êtes-vous **déplacé{{gender:/e/·e}}** pour le **travail** ?</t>
+    <t xml:space="preserve">Durant la dernière **semaine**, quand vous êtes-vous **déplacé{{gender:/e/·e}}** pour le **travail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the last **week**, when did you **travel** for **work**?
@@ -876,13 +876,13 @@
     <t xml:space="preserve">remoteWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **dernière semaine**, quand est-ce que {{nickname}} a travaillé en **télé-travail** ?</t>
+    <t xml:space="preserve">Durant la **dernière semaine**, quand est-ce que {{nickname}} a travaillé en **télé-travail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did {{nickname}} **work remotely**?</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **dernière semaine**, quand avez-vous travaillé en **télé-travail** ?</t>
+    <t xml:space="preserve">Durant la **dernière semaine**, quand avez-vous travaillé en **télé-travail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did you **work remotely**?</t>
@@ -1954,7 +1954,7 @@
     <t xml:space="preserve">wouldLikeToParticipateInOtherSurveysChaireMobilite</t>
   </si>
   <si>
-    <t xml:space="preserve">Seriez-vous intéressés à **participer à d'autres études** menées par la **Chaire Mobilité de Polytechnique Montréal** ?</t>
+    <t xml:space="preserve">Seriez-vous intéressés à **participer à d'autres études** menées par la **Chaire Mobilité de Polytechnique Montréal**?</t>
   </si>
   <si>
     <t xml:space="preserve">Would you be interested in **participating in other studies** conducted by the **Chaire Mobilite at Polytechnique Montreal**?</t>
@@ -2063,7 +2063,7 @@
     <t xml:space="preserve">timeSpentAnswering</t>
   </si>
   <si>
-    <t xml:space="preserve">Combien de **temps** pensez-vous avoir passé **à répondre** à cette enquête (**en minutes**) ?</t>
+    <t xml:space="preserve">Combien de **temps** pensez-vous avoir passé **à répondre** à cette enquête (**en minutes**)?</t>
   </si>
   <si>
     <t xml:space="preserve">How much **time** do you think you **spent answering** this survey (**in minutes**)?</t>
@@ -2090,7 +2090,7 @@
     <t xml:space="preserve">difficultyOfTheSurvey</t>
   </si>
   <si>
-    <t xml:space="preserve">Dans quelle mesure vous a-t-il été **facile** ou **difficile** de répondre aux questions de cette enquête ?</t>
+    <t xml:space="preserve">Dans quelle mesure vous a-t-il été **facile** ou **difficile** de répondre aux questions de cette enquête?</t>
   </si>
   <si>
     <t xml:space="preserve">How **easy** or **difficult** was it for you to answer the questions in this survey?</t>
@@ -2120,7 +2120,7 @@
     <t xml:space="preserve">consideredAbandoningSurvey</t>
   </si>
   <si>
-    <t xml:space="preserve">Avez-vous pensé, à un moment ou un autre, **abandonner l'enquête** ?</t>
+    <t xml:space="preserve">Avez-vous pensé, à un moment ou un autre, **abandonner l'enquête**?</t>
   </si>
   <si>
     <t xml:space="preserve">Have you considered, at any point, to **abandon the survey**?</t>
@@ -3436,35 +3436,7 @@
     <t xml:space="preserve">PreviousDepartureTime_home_schoolUsual</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">/"il/elle"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}} quitté le domicile pour aller au lieu d'études/école?</t>
-    </r>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/"il/elle"}} quitté le domicile pour aller au lieu d'études/école?</t>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} leave home before going to school?</t>
@@ -3479,35 +3451,7 @@
     <t xml:space="preserve">PreviousDepartureTime_home_other</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">/"il/elle"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}} quitté le domicile pour aller à cet endroit ({{visitedPlaceDescription}})?</t>
-    </r>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/"il/elle"}} quitté le domicile pour aller à cet endroit ({{visitedPlaceDescription}})?</t>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} leave home before going to this place ({{visitedPlaceDescription}})?</t>
@@ -3522,35 +3466,7 @@
     <t xml:space="preserve">PreviousDepartureTime_home_workOnTheRoad</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">/"il/elle"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}} quitté le domicile avant de débuter ses déplacements sur la route?</t>
-    </r>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/"il/elle"}} quitté le domicile avant de débuter ses déplacements sur la route?</t>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} leave home before starting {{gender :his/her/their}} on the road trips?</t>
@@ -3565,35 +3481,7 @@
     <t xml:space="preserve">PreviousDepartureTime_usualWorkPlace_workOnTheRoad</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">/"il/elle"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}} quitté son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
-    </r>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/"il/elle"}} quitté son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
   </si>
   <si>
     <t xml:space="preserve">t what time did {{nickname}} leave {{gender :his/her/their}} usual work place before starting {{gender :his/her/their}} on the road trips?</t>
@@ -3857,35 +3745,7 @@
     <t xml:space="preserve">_previousArrivalTimeDepartureTypeHome</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">/"il/elle"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}} arriv{{gender :é/ée/é.e}} au domicile avant de débuter ses déplacements sur la route?</t>
-    </r>
+    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel/"il/elle"}} arriv{{gender :é/ée/é.e}} au domicile avant de débuter ses déplacements sur la route?</t>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} arrive home before starting {{gender :his/her/their}} on the road trips?</t>
@@ -3900,35 +3760,7 @@
     <t xml:space="preserve">_previousArrivalTimeDepartureTypeUsualWorkPlace</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">/"il/elle"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}} arriv{{gender :é/ée/é.e}} à son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
-    </r>
+    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel/"il/elle"}} arriv{{gender :é/ée/é.e}} à son lieu de travail habituel avant de débuter ses déplacements sur la route?</t>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} arrive at his usual work place before starting {{gender :his/her/their}} on the road trips?</t>
@@ -3943,35 +3775,7 @@
     <t xml:space="preserve">_previousArrivalTimeDepartureTypeOther</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">/"il/elle"</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">}} arriv{{gender :é/ée/é.e}} au lieu précédent ({{visitedPlaceDescription}}) avant de débuter ses déplacements sur la route?</t>
-    </r>
+    <t xml:space="preserve">À quelle heure {{nickname}} est-{{gender :il/elle/iel/"il/elle"}} arriv{{gender :é/ée/é.e}} au lieu précédent ({{visitedPlaceDescription}}) avant de débuter ses déplacements sur la route?</t>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} arrive at the previous location ({{visitedPlaceDescription}}) before starting {{gender :his/her/their}} on the road trips?</t>
@@ -4277,7 +4081,7 @@
     <numFmt numFmtId="165" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="166" formatCode="@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4455,12 +4259,6 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -5215,12 +5013,12 @@
   </sheetPr>
   <dimension ref="A1:XFD135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="M15" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="E124" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="M1" activeCellId="0" sqref="M1"/>
-      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
-      <selection pane="bottomRight" activeCell="Y24" activeCellId="0" sqref="Y24"/>
+      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A124" activeCellId="0" sqref="A124"/>
+      <selection pane="bottomRight" activeCell="G129" activeCellId="0" sqref="G129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5355,7 +5153,7 @@
       <c r="XFC1" s="2"/>
       <c r="XFD1" s="2"/>
     </row>
-    <row r="2" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="8" t="s">
         <v>25</v>
       </c>
@@ -5403,7 +5201,7 @@
       <c r="W2" s="8"/>
       <c r="X2" s="8"/>
     </row>
-    <row r="3" customFormat="false" ht="51.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="8" t="s">
         <v>32</v>
       </c>
@@ -5448,7 +5246,7 @@
       <c r="W3" s="8"/>
       <c r="X3" s="8"/>
     </row>
-    <row r="4" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="8" t="s">
         <v>37</v>
       </c>
@@ -5494,7 +5292,7 @@
       <c r="W4" s="8"/>
       <c r="X4" s="8"/>
     </row>
-    <row r="5" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="8" t="s">
         <v>42</v>
       </c>
@@ -5542,7 +5340,7 @@
       <c r="W5" s="8"/>
       <c r="X5" s="8"/>
     </row>
-    <row r="6" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="8" t="s">
         <v>46</v>
       </c>
@@ -5684,7 +5482,7 @@
       <c r="W8" s="8"/>
       <c r="X8" s="8"/>
     </row>
-    <row r="9" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="8" t="s">
         <v>58</v>
       </c>
@@ -5733,7 +5531,7 @@
       </c>
       <c r="X9" s="8"/>
     </row>
-    <row r="10" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="8" t="s">
         <v>62</v>
       </c>
@@ -5782,7 +5580,7 @@
       </c>
       <c r="X10" s="8"/>
     </row>
-    <row r="11" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
         <v>67</v>
       </c>
@@ -6027,7 +5825,7 @@
       <c r="W15" s="8"/>
       <c r="X15" s="8"/>
     </row>
-    <row r="16" customFormat="false" ht="39.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="8" t="s">
         <v>93</v>
       </c>
@@ -6336,7 +6134,7 @@
       <c r="W21" s="21"/>
       <c r="X21" s="21"/>
     </row>
-    <row r="22" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="19" t="s">
         <v>122</v>
       </c>
@@ -6386,7 +6184,7 @@
       <c r="W22" s="21"/>
       <c r="X22" s="21"/>
     </row>
-    <row r="23" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="19" t="s">
         <v>128</v>
       </c>
@@ -6428,6 +6226,7 @@
       <c r="R23" s="21"/>
       <c r="S23" s="21"/>
       <c r="T23" s="19" t="b">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="U23" s="21" t="s">
@@ -6442,7 +6241,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="55.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="19" t="s">
         <v>137</v>
       </c>
@@ -6492,7 +6291,7 @@
       <c r="W24" s="21"/>
       <c r="X24" s="21"/>
     </row>
-    <row r="25" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="19" t="s">
         <v>143</v>
       </c>
@@ -6542,7 +6341,7 @@
       <c r="W25" s="21"/>
       <c r="X25" s="21"/>
     </row>
-    <row r="26" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="19" t="s">
         <v>148</v>
       </c>
@@ -6596,7 +6395,7 @@
       <c r="W26" s="21"/>
       <c r="X26" s="21"/>
     </row>
-    <row r="27" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="19" t="s">
         <v>155</v>
       </c>
@@ -6646,7 +6445,7 @@
       <c r="W27" s="21"/>
       <c r="X27" s="21"/>
     </row>
-    <row r="28" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="26.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="19" t="s">
         <v>160</v>
       </c>
@@ -6700,7 +6499,7 @@
       <c r="W28" s="21"/>
       <c r="X28" s="21"/>
     </row>
-    <row r="29" customFormat="false" ht="50" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="45.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="19" t="s">
         <v>167</v>
       </c>
@@ -6850,7 +6649,7 @@
       <c r="W31" s="21"/>
       <c r="X31" s="21"/>
     </row>
-    <row r="32" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="19" t="s">
         <v>182</v>
       </c>
@@ -6906,7 +6705,7 @@
       <c r="W32" s="21"/>
       <c r="X32" s="21"/>
     </row>
-    <row r="33" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="19" t="s">
         <v>192</v>
       </c>
@@ -7010,7 +6809,7 @@
       <c r="W34" s="21"/>
       <c r="X34" s="21"/>
     </row>
-    <row r="35" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="19" t="s">
         <v>205</v>
       </c>
@@ -7170,7 +6969,7 @@
       <c r="W37" s="21"/>
       <c r="X37" s="21"/>
     </row>
-    <row r="38" customFormat="false" ht="87.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="19" t="s">
         <v>228</v>
       </c>
@@ -7274,7 +7073,7 @@
       <c r="W39" s="21"/>
       <c r="X39" s="21"/>
     </row>
-    <row r="40" customFormat="false" ht="87.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="85.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="19" t="s">
         <v>241</v>
       </c>
@@ -7380,7 +7179,7 @@
       <c r="W41" s="21"/>
       <c r="X41" s="21"/>
     </row>
-    <row r="42" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="19" t="s">
         <v>255</v>
       </c>
@@ -7481,7 +7280,7 @@
       <c r="W43" s="30"/>
       <c r="X43" s="30"/>
     </row>
-    <row r="44" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="10" t="s">
         <v>265</v>
       </c>
@@ -7522,7 +7321,7 @@
       <c r="W44" s="30"/>
       <c r="X44" s="30"/>
     </row>
-    <row r="45" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="10" t="s">
         <v>269</v>
       </c>
@@ -7563,7 +7362,7 @@
       <c r="W45" s="30"/>
       <c r="X45" s="30"/>
     </row>
-    <row r="46" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="10" t="s">
         <v>272</v>
       </c>
@@ -7612,7 +7411,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="10" t="s">
         <v>277</v>
       </c>
@@ -7653,7 +7452,7 @@
       <c r="W47" s="30"/>
       <c r="X47" s="30"/>
     </row>
-    <row r="48" customFormat="false" ht="87.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="10" t="s">
         <v>280</v>
       </c>
@@ -7694,7 +7493,7 @@
       <c r="W48" s="30"/>
       <c r="X48" s="30"/>
     </row>
-    <row r="49" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="10" t="s">
         <v>284</v>
       </c>
@@ -7735,7 +7534,7 @@
       <c r="W49" s="30"/>
       <c r="X49" s="30"/>
     </row>
-    <row r="50" customFormat="false" ht="116.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="10" t="s">
         <v>288</v>
       </c>
@@ -7780,7 +7579,7 @@
       <c r="W50" s="30"/>
       <c r="X50" s="30"/>
     </row>
-    <row r="51" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="10" t="s">
         <v>293</v>
       </c>
@@ -7825,7 +7624,7 @@
       <c r="W51" s="30"/>
       <c r="X51" s="30"/>
     </row>
-    <row r="52" customFormat="false" ht="377.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="404.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="10" t="s">
         <v>298</v>
       </c>
@@ -7870,7 +7669,7 @@
       <c r="W52" s="30"/>
       <c r="X52" s="30"/>
     </row>
-    <row r="53" customFormat="false" ht="131.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="10" t="s">
         <v>304</v>
       </c>
@@ -7915,7 +7714,7 @@
       <c r="W53" s="30"/>
       <c r="X53" s="30"/>
     </row>
-    <row r="54" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="105.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="10" t="s">
         <v>310</v>
       </c>
@@ -7967,7 +7766,7 @@
       <c r="W54" s="30"/>
       <c r="X54" s="30"/>
     </row>
-    <row r="55" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="10" t="s">
         <v>318</v>
       </c>
@@ -8008,7 +7807,7 @@
       <c r="W55" s="30"/>
       <c r="X55" s="30"/>
     </row>
-    <row r="56" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="10" t="s">
         <v>322</v>
       </c>
@@ -8052,7 +7851,7 @@
       <c r="W56" s="30"/>
       <c r="X56" s="30"/>
     </row>
-    <row r="57" s="2" customFormat="true" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="2" customFormat="true" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="10" t="s">
         <v>272</v>
       </c>
@@ -8101,7 +7900,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="10" t="s">
         <v>277</v>
       </c>
@@ -9108,7 +8907,7 @@
         <v>425</v>
       </c>
     </row>
-    <row r="80" s="2" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="80" s="2" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="10" t="s">
         <v>272</v>
       </c>
@@ -9149,7 +8948,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A81" s="10" t="s">
         <v>277</v>
       </c>
@@ -10122,7 +9921,7 @@
         <v>507</v>
       </c>
     </row>
-    <row r="102" s="2" customFormat="true" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" s="2" customFormat="true" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="10" t="s">
         <v>272</v>
       </c>
@@ -10163,7 +9962,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="103" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="103" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A103" s="10" t="s">
         <v>277</v>
       </c>
@@ -10631,7 +10430,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="113" s="2" customFormat="true" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="113" s="2" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A113" s="36" t="s">
         <v>554</v>
       </c>
@@ -10675,7 +10474,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" s="2" customFormat="true" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="114" s="2" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="36" t="s">
         <v>563</v>
       </c>
@@ -10719,7 +10518,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" s="2" customFormat="true" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="115" s="2" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A115" s="36" t="s">
         <v>569</v>
       </c>
@@ -10763,7 +10562,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="116" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="10" t="s">
         <v>575</v>
       </c>
@@ -10811,7 +10610,7 @@
       <c r="W116" s="30"/>
       <c r="X116" s="30"/>
     </row>
-    <row r="117" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="117" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A117" s="10" t="s">
         <v>579</v>
       </c>
@@ -10859,7 +10658,7 @@
       <c r="W117" s="30"/>
       <c r="X117" s="30"/>
     </row>
-    <row r="118" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="118" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="10" t="s">
         <v>584</v>
       </c>
@@ -10900,7 +10699,7 @@
       <c r="W118" s="30"/>
       <c r="X118" s="30"/>
     </row>
-    <row r="119" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="119" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A119" s="10" t="s">
         <v>585</v>
       </c>
@@ -10943,7 +10742,7 @@
       <c r="W119" s="30"/>
       <c r="X119" s="30"/>
     </row>
-    <row r="120" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="120" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="10" t="s">
         <v>591</v>
       </c>
@@ -10989,7 +10788,7 @@
       <c r="W120" s="30"/>
       <c r="X120" s="30"/>
     </row>
-    <row r="121" customFormat="false" ht="54.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="121" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A121" s="10" t="s">
         <v>596</v>
       </c>
@@ -11035,7 +10834,7 @@
       <c r="W121" s="30"/>
       <c r="X121" s="30"/>
     </row>
-    <row r="122" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="122" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A122" s="10" t="s">
         <v>599</v>
       </c>
@@ -11083,7 +10882,7 @@
       <c r="W122" s="30"/>
       <c r="X122" s="30"/>
     </row>
-    <row r="123" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="123" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A123" s="10" t="s">
         <v>603</v>
       </c>
@@ -11129,7 +10928,7 @@
       <c r="W123" s="30"/>
       <c r="X123" s="30"/>
     </row>
-    <row r="124" customFormat="false" ht="33.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="124" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A124" s="10" t="s">
         <v>608</v>
       </c>
@@ -11173,7 +10972,7 @@
       <c r="W124" s="30"/>
       <c r="X124" s="30"/>
     </row>
-    <row r="125" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="125" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A125" s="10" t="s">
         <v>611</v>
       </c>
@@ -11214,7 +11013,7 @@
       <c r="W125" s="30"/>
       <c r="X125" s="30"/>
     </row>
-    <row r="126" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="126" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A126" s="10" t="s">
         <v>614</v>
       </c>
@@ -11264,7 +11063,7 @@
       <c r="W126" s="30"/>
       <c r="X126" s="30"/>
     </row>
-    <row r="127" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="127" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A127" s="10" t="s">
         <v>621</v>
       </c>
@@ -11314,7 +11113,7 @@
       <c r="W127" s="30"/>
       <c r="X127" s="30"/>
     </row>
-    <row r="128" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="128" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A128" s="10" t="s">
         <v>626</v>
       </c>
@@ -11362,7 +11161,7 @@
       <c r="W128" s="30"/>
       <c r="X128" s="30"/>
     </row>
-    <row r="129" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="129" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A129" s="10" t="s">
         <v>631</v>
       </c>
@@ -11408,7 +11207,7 @@
       <c r="W129" s="30"/>
       <c r="X129" s="30"/>
     </row>
-    <row r="130" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="130" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A130" s="10" t="s">
         <v>635</v>
       </c>
@@ -11456,7 +11255,7 @@
       <c r="W130" s="30"/>
       <c r="X130" s="30"/>
     </row>
-    <row r="131" customFormat="false" ht="59" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="131" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A131" s="10" t="s">
         <v>640</v>
       </c>
@@ -11504,7 +11303,7 @@
       <c r="W131" s="30"/>
       <c r="X131" s="30"/>
     </row>
-    <row r="132" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="132" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="10" t="s">
         <v>645</v>
       </c>
@@ -11552,7 +11351,7 @@
       <c r="W132" s="30"/>
       <c r="X132" s="30"/>
     </row>
-    <row r="133" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="10" t="s">
         <v>650</v>
       </c>
@@ -11600,7 +11399,7 @@
       <c r="W133" s="30"/>
       <c r="X133" s="30"/>
     </row>
-    <row r="134" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="134" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A134" s="10" t="s">
         <v>654</v>
       </c>
@@ -11641,7 +11440,7 @@
       <c r="W134" s="30"/>
       <c r="X134" s="30"/>
     </row>
-    <row r="135" customFormat="false" ht="116.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="135" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A135" s="1" t="s">
         <v>657</v>
       </c>
@@ -11802,7 +11601,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
         <v>666</v>
       </c>
@@ -11818,7 +11617,7 @@
       </c>
       <c r="F2" s="10"/>
     </row>
-    <row r="3" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>101</v>
       </c>
@@ -11834,7 +11633,7 @@
       </c>
       <c r="F3" s="10"/>
     </row>
-    <row r="4" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>196</v>
       </c>
@@ -11850,7 +11649,7 @@
       </c>
       <c r="F4" s="10"/>
     </row>
-    <row r="5" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>196</v>
       </c>
@@ -11868,7 +11667,7 @@
       </c>
       <c r="F5" s="10"/>
     </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="10" t="s">
         <v>97</v>
       </c>
@@ -11884,7 +11683,7 @@
       </c>
       <c r="F6" s="10"/>
     </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="10" t="s">
         <v>674</v>
       </c>
@@ -11900,7 +11699,7 @@
       </c>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="10" t="s">
         <v>674</v>
       </c>
@@ -11918,7 +11717,7 @@
       </c>
       <c r="F8" s="10"/>
     </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="10" t="s">
         <v>678</v>
       </c>
@@ -11934,7 +11733,7 @@
       </c>
       <c r="F9" s="10"/>
     </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="10" t="s">
         <v>678</v>
       </c>
@@ -11952,7 +11751,7 @@
       </c>
       <c r="F10" s="10"/>
     </row>
-    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
         <v>679</v>
       </c>
@@ -11968,7 +11767,7 @@
       </c>
       <c r="F11" s="10"/>
     </row>
-    <row r="12" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
         <v>126</v>
       </c>
@@ -11984,7 +11783,7 @@
       </c>
       <c r="F12" s="10"/>
     </row>
-    <row r="13" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="10" t="s">
         <v>189</v>
       </c>
@@ -12000,7 +11799,7 @@
       </c>
       <c r="F13" s="10"/>
     </row>
-    <row r="14" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="10" t="s">
         <v>680</v>
       </c>
@@ -12016,7 +11815,7 @@
       </c>
       <c r="F14" s="10"/>
     </row>
-    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="10" t="s">
         <v>141</v>
       </c>
@@ -12032,7 +11831,7 @@
       </c>
       <c r="F15" s="10"/>
     </row>
-    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="10" t="s">
         <v>152</v>
       </c>
@@ -12048,7 +11847,7 @@
       </c>
       <c r="F16" s="10"/>
     </row>
-    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="10" t="s">
         <v>152</v>
       </c>
@@ -12066,7 +11865,7 @@
       </c>
       <c r="F17" s="10"/>
     </row>
-    <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="10" t="s">
         <v>171</v>
       </c>
@@ -12082,7 +11881,7 @@
       </c>
       <c r="F18" s="10"/>
     </row>
-    <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="10" t="s">
         <v>147</v>
       </c>
@@ -12098,7 +11897,7 @@
       </c>
       <c r="F19" s="10"/>
     </row>
-    <row r="20" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="10" t="s">
         <v>683</v>
       </c>
@@ -12114,7 +11913,7 @@
       </c>
       <c r="F20" s="10"/>
     </row>
-    <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="10" t="s">
         <v>683</v>
       </c>
@@ -12132,7 +11931,7 @@
       </c>
       <c r="F21" s="10"/>
     </row>
-    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="10" t="s">
         <v>684</v>
       </c>
@@ -12148,7 +11947,7 @@
       </c>
       <c r="F22" s="10"/>
     </row>
-    <row r="23" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="10" t="s">
         <v>181</v>
       </c>
@@ -12164,7 +11963,7 @@
       </c>
       <c r="F23" s="10"/>
     </row>
-    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="2" t="s">
         <v>203</v>
       </c>
@@ -12178,7 +11977,7 @@
         <v>687</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
         <v>203</v>
       </c>
@@ -12195,7 +11994,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="s">
         <v>203</v>
       </c>
@@ -12212,7 +12011,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
         <v>219</v>
       </c>
@@ -12226,7 +12025,7 @@
         <v>690</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>219</v>
       </c>
@@ -12243,7 +12042,7 @@
         <v>691</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
         <v>219</v>
       </c>
@@ -12260,7 +12059,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
         <v>227</v>
       </c>
@@ -12274,7 +12073,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>227</v>
       </c>
@@ -12291,7 +12090,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>227</v>
       </c>
@@ -12308,7 +12107,7 @@
         <v>695</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>227</v>
       </c>
@@ -12325,7 +12124,7 @@
         <v>693</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
         <v>227</v>
       </c>
@@ -12342,7 +12141,7 @@
         <v>694</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="s">
         <v>227</v>
       </c>
@@ -12587,7 +12386,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="10" t="s">
         <v>27</v>
       </c>
@@ -12613,7 +12412,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="10" t="s">
         <v>108</v>
       </c>
@@ -12639,7 +12438,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="10" t="s">
         <v>717</v>
       </c>
@@ -12665,7 +12464,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="10" t="s">
         <v>265</v>
       </c>
@@ -12694,7 +12493,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="34" t="s">
         <v>273</v>
       </c>
@@ -12723,7 +12522,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="34" t="s">
         <v>325</v>
       </c>
@@ -12749,7 +12548,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="34" t="s">
         <v>426</v>
       </c>
@@ -12775,7 +12574,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="34" t="s">
         <v>508</v>
       </c>
@@ -12804,7 +12603,7 @@
         <v>717</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="34" t="s">
         <v>546</v>
       </c>
@@ -12833,7 +12632,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="10" t="s">
         <v>586</v>
       </c>
@@ -12859,7 +12658,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="10" t="s">
         <v>658</v>
       </c>
@@ -12906,8 +12705,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C30" activeCellId="0" sqref="C30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12920,7 +12719,7 @@
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="53" width="9.14"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="59" t="s">
         <v>742</v>
       </c>
@@ -12949,7 +12748,7 @@
         <v>744</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>671</v>
       </c>
@@ -12967,7 +12766,7 @@
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
     </row>
-    <row r="3" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>747</v>
       </c>
@@ -12985,7 +12784,7 @@
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
     </row>
-    <row r="4" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>154</v>
       </c>
@@ -13003,7 +12802,7 @@
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
     </row>
-    <row r="5" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>752</v>
       </c>
@@ -13021,7 +12820,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
     </row>
-    <row r="6" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
         <v>755</v>
       </c>
@@ -13039,7 +12838,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
     </row>
-    <row r="7" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>758</v>
       </c>
@@ -13057,7 +12856,7 @@
       <c r="G7" s="1"/>
       <c r="H7" s="1"/>
     </row>
-    <row r="8" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>36</v>
       </c>
@@ -13071,7 +12870,7 @@
       </c>
       <c r="H8" s="1"/>
     </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
@@ -13085,7 +12884,7 @@
       </c>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>176</v>
       </c>
@@ -13099,7 +12898,7 @@
       </c>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>176</v>
       </c>
@@ -13113,7 +12912,7 @@
       </c>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>102</v>
       </c>
@@ -13127,7 +12926,7 @@
       </c>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>102</v>
       </c>
@@ -13141,7 +12940,7 @@
       </c>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" s="2" customFormat="true" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" s="2" customFormat="true" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>102</v>
       </c>
@@ -13156,7 +12955,7 @@
       <c r="H14" s="1"/>
       <c r="I14" s="53"/>
     </row>
-    <row r="15" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="21" t="s">
         <v>127</v>
       </c>
@@ -13174,7 +12973,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="21" t="s">
         <v>127</v>
       </c>
@@ -13192,7 +12991,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="21" t="s">
         <v>127</v>
       </c>
@@ -13206,7 +13005,7 @@
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="21" t="s">
         <v>133</v>
       </c>
@@ -13224,7 +13023,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="21" t="s">
         <v>133</v>
       </c>
@@ -13242,7 +13041,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="21" t="s">
         <v>133</v>
       </c>
@@ -13260,7 +13059,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" customFormat="false" ht="22.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="21" t="s">
         <v>133</v>
       </c>
@@ -13274,7 +13073,7 @@
       </c>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>142</v>
       </c>
@@ -13292,7 +13091,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>142</v>
       </c>
@@ -13310,7 +13109,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>142</v>
       </c>
@@ -13324,7 +13123,7 @@
       </c>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>149</v>
       </c>
@@ -13344,7 +13143,7 @@
         <v>679</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>149</v>
       </c>
@@ -13364,7 +13163,7 @@
         <v>678</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>149</v>
       </c>
@@ -13384,7 +13183,7 @@
         <v>680</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>149</v>
       </c>
@@ -13402,7 +13201,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>149</v>
       </c>
@@ -13422,7 +13221,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
         <v>149</v>
       </c>
@@ -13436,7 +13235,7 @@
       </c>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
         <v>155</v>
       </c>
@@ -13457,7 +13256,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
         <v>155</v>
       </c>
@@ -13478,7 +13277,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
         <v>155</v>
       </c>
@@ -13499,7 +13298,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
         <v>155</v>
       </c>
@@ -13520,7 +13319,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
         <v>155</v>
       </c>
@@ -13541,7 +13340,7 @@
         <v>790</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
         <v>155</v>
       </c>
@@ -13561,7 +13360,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
         <v>155</v>
       </c>
@@ -13579,7 +13378,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
         <v>155</v>
       </c>
@@ -13597,7 +13396,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
         <v>155</v>
       </c>
@@ -13615,7 +13414,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
         <v>155</v>
       </c>
@@ -13633,7 +13432,7 @@
       <c r="G40" s="1"/>
       <c r="H40" s="1"/>
     </row>
-    <row r="41" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
         <v>155</v>
       </c>
@@ -13651,7 +13450,7 @@
       <c r="G41" s="1"/>
       <c r="H41" s="1"/>
     </row>
-    <row r="42" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
         <v>155</v>
       </c>
@@ -13669,7 +13468,7 @@
       <c r="G42" s="1"/>
       <c r="H42" s="1"/>
     </row>
-    <row r="43" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
         <v>155</v>
       </c>
@@ -13687,7 +13486,7 @@
       <c r="G43" s="1"/>
       <c r="H43" s="1"/>
     </row>
-    <row r="44" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>191</v>
       </c>
@@ -13701,7 +13500,7 @@
       </c>
       <c r="H44" s="1"/>
     </row>
-    <row r="45" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>191</v>
       </c>
@@ -13719,7 +13518,7 @@
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
     </row>
-    <row r="46" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>191</v>
       </c>
@@ -13737,7 +13536,7 @@
       <c r="G46" s="1"/>
       <c r="H46" s="1"/>
     </row>
-    <row r="47" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
         <v>191</v>
       </c>
@@ -13751,7 +13550,7 @@
       </c>
       <c r="H47" s="1"/>
     </row>
-    <row r="48" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="21" t="s">
         <v>204</v>
       </c>
@@ -13769,7 +13568,7 @@
       <c r="G48" s="1"/>
       <c r="H48" s="1"/>
     </row>
-    <row r="49" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="21" t="s">
         <v>204</v>
       </c>
@@ -13787,7 +13586,7 @@
       <c r="G49" s="1"/>
       <c r="H49" s="1"/>
     </row>
-    <row r="50" customFormat="false" ht="73.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="21" t="s">
         <v>204</v>
       </c>
@@ -13805,7 +13604,7 @@
       <c r="G50" s="1"/>
       <c r="H50" s="1"/>
     </row>
-    <row r="51" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="21" t="s">
         <v>204</v>
       </c>
@@ -13823,7 +13622,7 @@
       <c r="G51" s="1"/>
       <c r="H51" s="1"/>
     </row>
-    <row r="52" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="21" t="s">
         <v>204</v>
       </c>
@@ -13841,7 +13640,7 @@
       <c r="G52" s="1"/>
       <c r="H52" s="1"/>
     </row>
-    <row r="53" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="21" t="s">
         <v>220</v>
       </c>
@@ -13855,7 +13654,7 @@
         <v>825</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="21" t="s">
         <v>220</v>
       </c>
@@ -13869,7 +13668,7 @@
         <v>837</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="44.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="21" t="s">
         <v>220</v>
       </c>
@@ -14445,7 +14244,7 @@
         <v>749</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="30" t="s">
         <v>520</v>
       </c>
@@ -14459,7 +14258,7 @@
         <v>936</v>
       </c>
     </row>
-    <row r="92" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="92" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="30" t="s">
         <v>520</v>
       </c>
@@ -14473,7 +14272,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="93" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="93" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A93" s="30" t="s">
         <v>520</v>
       </c>
@@ -14487,7 +14286,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="94" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="94" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="30" t="s">
         <v>520</v>
       </c>
@@ -14501,7 +14300,7 @@
         <v>945</v>
       </c>
     </row>
-    <row r="95" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="95" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A95" s="30" t="s">
         <v>520</v>
       </c>
@@ -14509,7 +14308,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="96" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="96" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A96" s="30" t="s">
         <v>520</v>
       </c>
@@ -14517,7 +14316,7 @@
         <v>755</v>
       </c>
     </row>
-    <row r="97" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="97" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="30" t="s">
         <v>535</v>
       </c>
@@ -14531,7 +14330,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="98" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="98" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="30" t="s">
         <v>535</v>
       </c>
@@ -14545,7 +14344,7 @@
         <v>951</v>
       </c>
     </row>
-    <row r="99" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="30" t="s">
         <v>535</v>
       </c>
@@ -14559,7 +14358,7 @@
         <v>942</v>
       </c>
     </row>
-    <row r="100" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="100" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="30" t="s">
         <v>535</v>
       </c>
@@ -14573,7 +14372,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="101" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="101" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A101" s="30" t="s">
         <v>535</v>
       </c>
@@ -14581,7 +14380,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="102" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="102" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A102" s="30" t="s">
         <v>535</v>
       </c>
@@ -15082,7 +14881,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="16.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="22.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -15118,7 +14917,7 @@
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
     </row>
-    <row r="3" customFormat="false" ht="30.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
         <v>108</v>
       </c>

</xml_diff>

<commit_message>
tripsIntro: rename field to `personDidTripsConfirm`
fixes #160

This new name explains more the value of the field, as it confirms if
the person did trips, and not the change of value.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2215" uniqueCount="1283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2227" uniqueCount="1293">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -990,10 +990,10 @@
 __Include all trips, whether for personal reasons (shopping, outings, leisure, etc.), for work, or to pick up or drop someone off.__</t>
   </si>
   <si>
-    <t xml:space="preserve">personDidTripsChangeConfirm</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vous avez déjà déclaré des déplacements. Confirmez-vous qu'ils sont erronés et que ${{nickname}} ne s'est pas déplac{{gender:é/ée/é.e}} le {{formattedTripsDate}}?</t>
+    <t xml:space="preserve">personDidTripsConfirm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous avez déjà déclaré des déplacements. Confirmez-vous qu'ils sont erronés et que {{nickname}} ne s'est pas déplac{{gender:é/ée/é.e}} le {{formattedTripsDate}}?</t>
   </si>
   <si>
     <t xml:space="preserve">You already declared trip. Do you confirm they are erroneous and that {{person.nickname}} did not make any trips on {{formattedTripsDate}}?</t>
@@ -4070,6 +4070,36 @@
       </rPr>
       <t xml:space="preserve">emote</t>
     </r>
+  </si>
+  <si>
+    <t xml:space="preserve">personDidTripsConfirmChoiceNo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} n'a effectué aucun déplacement le {{assignedDate}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} did not make any trip on {{assignedDate}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Je n'ai effectué aucun déplacement le {{assignedDate}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I did not make any trip on {{assignedDate}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">personDidTripsConfirmChoiceYes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} a effectué au moins un déplacement le {{assignedDate}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{nickname}} did make at least one trip on {{assignedDate}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J'ai effectué au moins un déplacement le {{assignedDate}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I did make at least one trip on {{assignedDate}}</t>
   </si>
 </sst>
 </file>
@@ -4356,7 +4386,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4619,6 +4649,10 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -5013,12 +5047,12 @@
   </sheetPr>
   <dimension ref="A1:XFD135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="E124" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="I45" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
-      <selection pane="bottomLeft" activeCell="A124" activeCellId="0" sqref="A124"/>
-      <selection pane="bottomRight" activeCell="G129" activeCellId="0" sqref="G129"/>
+      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
+      <selection pane="bottomLeft" activeCell="A45" activeCellId="0" sqref="A45"/>
+      <selection pane="bottomRight" activeCell="J51" activeCellId="0" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12705,7 +12739,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
@@ -14869,8 +14903,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E54" activeCellId="0" sqref="E54"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A46" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C81" activeCellId="0" sqref="C81"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16176,6 +16210,46 @@
       </c>
       <c r="F81" s="1" t="s">
         <v>993</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B82" s="2" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C82" s="66" t="s">
+        <v>1284</v>
+      </c>
+      <c r="D82" s="66" t="s">
+        <v>1285</v>
+      </c>
+      <c r="E82" s="66" t="s">
+        <v>1286</v>
+      </c>
+      <c r="F82" s="66" t="s">
+        <v>1287</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="B83" s="2" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C83" s="66" t="s">
+        <v>1289</v>
+      </c>
+      <c r="D83" s="66" t="s">
+        <v>1290</v>
+      </c>
+      <c r="E83" s="66" t="s">
+        <v>1291</v>
+      </c>
+      <c r="F83" s="66" t="s">
+        <v>1292</v>
       </c>
     </row>
     <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
labels: fix comments from reviews in Excel
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -849,7 +849,7 @@
     <t xml:space="preserve">travelToWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la dernière **semaine**, quand est-ce que {{nickname}} s'est **déplacé{{gender:/e/·e}}** pour le **travail**?
+    <t xml:space="preserve">Durant la dernière **semaine**, quand {{nickname}} s'est-{{gender:il/elle/iel/"il/elle"}} **déplacé{{gender:/e/·e}}** pour le **travail**?
 __Pour se rendre au travail ou toute autre raison concernant le travail.__</t>
   </si>
   <si>
@@ -876,13 +876,13 @@
     <t xml:space="preserve">remoteWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **dernière semaine**, quand est-ce que {{nickname}} a travaillé en **télé-travail**?</t>
+    <t xml:space="preserve">Durant la **dernière semaine**, quand {{nickname}} a-t-{{gender:il/elle/iel/"il/elle"}} fait du **télé-travail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did {{nickname}} **work remotely**?</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **dernière semaine**, quand avez-vous travaillé en **télé-travail**?</t>
+    <t xml:space="preserve">Durant la **dernière semaine**, quand avez-vous fait du **télé-travail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did you **work remotely**?</t>
@@ -996,7 +996,7 @@
     <t xml:space="preserve">Vous avez déjà déclaré des déplacements. Confirmez-vous qu'ils sont erronés et que {{nickname}} ne s'est pas déplac{{gender:é/ée/é.e}} le {{formattedTripsDate}}?</t>
   </si>
   <si>
-    <t xml:space="preserve">You already declared trip. Do you confirm they are erroneous and that {{person.nickname}} did not make any trips on {{formattedTripsDate}}?</t>
+    <t xml:space="preserve">You already declared trip. Do you confirm they are erroneous and that {{nickname}} did not make any trips on {{formattedTripsDate}}?</t>
   </si>
   <si>
     <t xml:space="preserve">Vous avez déjà déclaré des déplacements. Confirmez-vous qu'ils sont erronés et que vous n'avez fait aucun déplacement le {{formattedTripsDate}}?</t>
@@ -1458,7 +1458,7 @@
     <t xml:space="preserve">segmentsIntro</t>
   </si>
   <si>
-    <t xml:space="preserve">Veuillez indiquer tous les modes de transport utilisés pour effectuer ce déplacement (de {{originName}} à {{destinationName}}), dans l'ordre chronologique:</t>
+    <t xml:space="preserve">Veuillez indiquer tous les modes de transport utilisés pour effectuer ce déplacement (de {{originName}} vers {{destinationName}}), dans l'ordre chronologique:</t>
   </si>
   <si>
     <t xml:space="preserve">Please indicate all modes of transport used for this trip (from {{originName}} to {{destinationName}}), in chronological order:</t>
@@ -2473,10 +2473,10 @@
     <t xml:space="preserve">Man</t>
   </si>
   <si>
-    <t xml:space="preserve">Cette personne s’identifie comme:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This person identifies herself as:</t>
+    <t xml:space="preserve">Cette personne s'identifie comme:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This person identifies  as:</t>
   </si>
   <si>
     <t xml:space="preserve">Oui, à temps plein</t>
@@ -4111,10 +4111,10 @@
     <t xml:space="preserve">errors.inputRangeMustBePositiveOrZero</t>
   </si>
   <si>
-    <t xml:space="preserve">Cette réponse doit être d'une valeur minimum de 0.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">This answer must be a minimum value of 0.</t>
+    <t xml:space="preserve">Veuillez placer le bouton à l'intérieur de la plage de réponse.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Make sure your slider button is inside the range.</t>
   </si>
 </sst>
 </file>
@@ -4542,10 +4542,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4668,6 +4664,10 @@
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -5062,12 +5062,12 @@
   </sheetPr>
   <dimension ref="A1:XFD135"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C113" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C51" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A113" activeCellId="0" sqref="A113"/>
-      <selection pane="bottomRight" activeCell="G123" activeCellId="0" sqref="G123"/>
+      <selection pane="bottomLeft" activeCell="A51" activeCellId="0" sqref="A51"/>
+      <selection pane="bottomRight" activeCell="G52" activeCellId="0" sqref="G52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9200,7 +9200,7 @@
       <c r="F85" s="10" t="s">
         <v>438</v>
       </c>
-      <c r="G85" s="35" t="s">
+      <c r="G85" s="10" t="s">
         <v>439</v>
       </c>
       <c r="H85" s="10" t="s">
@@ -9568,7 +9568,7 @@
       <c r="F93" s="10" t="s">
         <v>471</v>
       </c>
-      <c r="G93" s="36" t="s">
+      <c r="G93" s="35" t="s">
         <v>472</v>
       </c>
       <c r="H93" s="10" t="s">
@@ -10445,10 +10445,10 @@
       <c r="XED111" s="2"/>
     </row>
     <row r="112" s="2" customFormat="true" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="37" t="s">
+      <c r="A112" s="36" t="s">
         <v>553</v>
       </c>
-      <c r="B112" s="37" t="s">
+      <c r="B112" s="36" t="s">
         <v>73</v>
       </c>
       <c r="C112" s="29" t="n">
@@ -10458,14 +10458,14 @@
       <c r="D112" s="34" t="s">
         <v>547</v>
       </c>
-      <c r="E112" s="38"/>
-      <c r="F112" s="37" t="str">
+      <c r="E112" s="37"/>
+      <c r="F112" s="36" t="str">
         <f aca="false">A112</f>
         <v>householdLongDistanceIntroMap</v>
       </c>
-      <c r="G112" s="39"/>
-      <c r="H112" s="39"/>
-      <c r="I112" s="39"/>
+      <c r="G112" s="38"/>
+      <c r="H112" s="38"/>
+      <c r="I112" s="38"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
@@ -10480,7 +10480,7 @@
       </c>
     </row>
     <row r="113" s="2" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="37" t="s">
+      <c r="A113" s="36" t="s">
         <v>555</v>
       </c>
       <c r="B113" s="28" t="s">
@@ -10493,20 +10493,20 @@
       <c r="D113" s="34" t="s">
         <v>547</v>
       </c>
-      <c r="E113" s="38"/>
-      <c r="F113" s="37" t="s">
+      <c r="E113" s="37"/>
+      <c r="F113" s="36" t="s">
         <v>557</v>
       </c>
-      <c r="G113" s="39" t="s">
+      <c r="G113" s="38" t="s">
         <v>558</v>
       </c>
-      <c r="H113" s="39" t="s">
+      <c r="H113" s="38" t="s">
         <v>559</v>
       </c>
-      <c r="I113" s="39" t="s">
+      <c r="I113" s="38" t="s">
         <v>560</v>
       </c>
-      <c r="J113" s="39" t="s">
+      <c r="J113" s="38" t="s">
         <v>561</v>
       </c>
       <c r="K113" s="1"/>
@@ -10524,7 +10524,7 @@
       </c>
     </row>
     <row r="114" s="2" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="37" t="s">
+      <c r="A114" s="36" t="s">
         <v>564</v>
       </c>
       <c r="B114" s="28" t="s">
@@ -10537,20 +10537,20 @@
       <c r="D114" s="34" t="s">
         <v>547</v>
       </c>
-      <c r="E114" s="38"/>
-      <c r="F114" s="37" t="s">
+      <c r="E114" s="37"/>
+      <c r="F114" s="36" t="s">
         <v>565</v>
       </c>
-      <c r="G114" s="39" t="s">
+      <c r="G114" s="38" t="s">
         <v>566</v>
       </c>
-      <c r="H114" s="39" t="s">
+      <c r="H114" s="38" t="s">
         <v>567</v>
       </c>
-      <c r="I114" s="39" t="s">
+      <c r="I114" s="38" t="s">
         <v>568</v>
       </c>
-      <c r="J114" s="39" t="s">
+      <c r="J114" s="38" t="s">
         <v>569</v>
       </c>
       <c r="K114" s="1"/>
@@ -10568,7 +10568,7 @@
       </c>
     </row>
     <row r="115" s="2" customFormat="true" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="37" t="s">
+      <c r="A115" s="36" t="s">
         <v>570</v>
       </c>
       <c r="B115" s="28" t="s">
@@ -10581,20 +10581,20 @@
       <c r="D115" s="34" t="s">
         <v>547</v>
       </c>
-      <c r="E115" s="38"/>
-      <c r="F115" s="37" t="s">
+      <c r="E115" s="37"/>
+      <c r="F115" s="36" t="s">
         <v>571</v>
       </c>
-      <c r="G115" s="39" t="s">
+      <c r="G115" s="38" t="s">
         <v>572</v>
       </c>
-      <c r="H115" s="39" t="s">
+      <c r="H115" s="38" t="s">
         <v>573</v>
       </c>
-      <c r="I115" s="39" t="s">
+      <c r="I115" s="38" t="s">
         <v>574</v>
       </c>
-      <c r="J115" s="39" t="s">
+      <c r="J115" s="38" t="s">
         <v>575</v>
       </c>
       <c r="K115" s="1"/>
@@ -10629,10 +10629,10 @@
       <c r="F116" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="G116" s="40" t="s">
+      <c r="G116" s="39" t="s">
         <v>578</v>
       </c>
-      <c r="H116" s="40" t="s">
+      <c r="H116" s="39" t="s">
         <v>579</v>
       </c>
       <c r="I116" s="15"/>
@@ -10677,10 +10677,10 @@
       <c r="F117" s="10" t="s">
         <v>581</v>
       </c>
-      <c r="G117" s="40" t="s">
+      <c r="G117" s="39" t="s">
         <v>582</v>
       </c>
-      <c r="H117" s="40" t="s">
+      <c r="H117" s="39" t="s">
         <v>583</v>
       </c>
       <c r="I117" s="15"/>
@@ -10821,7 +10821,7 @@
       <c r="L120" s="30"/>
       <c r="M120" s="30"/>
       <c r="N120" s="30"/>
-      <c r="O120" s="41" t="s">
+      <c r="O120" s="40" t="s">
         <v>596</v>
       </c>
       <c r="P120" s="30"/>
@@ -10855,10 +10855,10 @@
       <c r="F121" s="10" t="s">
         <v>597</v>
       </c>
-      <c r="G121" s="40" t="s">
+      <c r="G121" s="39" t="s">
         <v>598</v>
       </c>
-      <c r="H121" s="40" t="s">
+      <c r="H121" s="39" t="s">
         <v>599</v>
       </c>
       <c r="I121" s="15"/>
@@ -10901,10 +10901,10 @@
       <c r="F122" s="10" t="s">
         <v>600</v>
       </c>
-      <c r="G122" s="40" t="s">
+      <c r="G122" s="39" t="s">
         <v>601</v>
       </c>
-      <c r="H122" s="40" t="s">
+      <c r="H122" s="39" t="s">
         <v>602</v>
       </c>
       <c r="I122" s="15"/>
@@ -10949,10 +10949,10 @@
       <c r="F123" s="30" t="s">
         <v>606</v>
       </c>
-      <c r="G123" s="41" t="s">
+      <c r="G123" s="40" t="s">
         <v>607</v>
       </c>
-      <c r="H123" s="41" t="s">
+      <c r="H123" s="40" t="s">
         <v>608</v>
       </c>
       <c r="I123" s="15"/>
@@ -11180,10 +11180,10 @@
       <c r="F128" s="30" t="s">
         <v>628</v>
       </c>
-      <c r="G128" s="41" t="s">
+      <c r="G128" s="40" t="s">
         <v>629</v>
       </c>
-      <c r="H128" s="41" t="s">
+      <c r="H128" s="40" t="s">
         <v>630</v>
       </c>
       <c r="I128" s="15"/>
@@ -11196,7 +11196,7 @@
       </c>
       <c r="O128" s="30"/>
       <c r="P128" s="30"/>
-      <c r="Q128" s="41" t="s">
+      <c r="Q128" s="40" t="s">
         <v>632</v>
       </c>
       <c r="R128" s="30"/>
@@ -11228,10 +11228,10 @@
       <c r="F129" s="30" t="s">
         <v>634</v>
       </c>
-      <c r="G129" s="41" t="s">
+      <c r="G129" s="40" t="s">
         <v>635</v>
       </c>
-      <c r="H129" s="41" t="s">
+      <c r="H129" s="40" t="s">
         <v>636</v>
       </c>
       <c r="I129" s="15"/>
@@ -11274,10 +11274,10 @@
       <c r="F130" s="30" t="s">
         <v>638</v>
       </c>
-      <c r="G130" s="41" t="s">
+      <c r="G130" s="40" t="s">
         <v>639</v>
       </c>
-      <c r="H130" s="41" t="s">
+      <c r="H130" s="40" t="s">
         <v>640</v>
       </c>
       <c r="I130" s="15"/>
@@ -11290,7 +11290,7 @@
       </c>
       <c r="O130" s="30"/>
       <c r="P130" s="30"/>
-      <c r="Q130" s="41" t="s">
+      <c r="Q130" s="40" t="s">
         <v>641</v>
       </c>
       <c r="R130" s="30"/>
@@ -11322,10 +11322,10 @@
       <c r="F131" s="30" t="s">
         <v>643</v>
       </c>
-      <c r="G131" s="41" t="s">
+      <c r="G131" s="40" t="s">
         <v>644</v>
       </c>
-      <c r="H131" s="41" t="s">
+      <c r="H131" s="40" t="s">
         <v>645</v>
       </c>
       <c r="I131" s="15"/>
@@ -11338,7 +11338,7 @@
       </c>
       <c r="O131" s="30"/>
       <c r="P131" s="30"/>
-      <c r="Q131" s="41" t="s">
+      <c r="Q131" s="40" t="s">
         <v>646</v>
       </c>
       <c r="R131" s="30"/>
@@ -11370,10 +11370,10 @@
       <c r="F132" s="30" t="s">
         <v>648</v>
       </c>
-      <c r="G132" s="41" t="s">
+      <c r="G132" s="40" t="s">
         <v>649</v>
       </c>
-      <c r="H132" s="41" t="s">
+      <c r="H132" s="40" t="s">
         <v>650</v>
       </c>
       <c r="I132" s="15"/>
@@ -11386,7 +11386,7 @@
       </c>
       <c r="O132" s="30"/>
       <c r="P132" s="30"/>
-      <c r="Q132" s="41" t="s">
+      <c r="Q132" s="40" t="s">
         <v>651</v>
       </c>
       <c r="R132" s="30"/>
@@ -11418,10 +11418,10 @@
       <c r="F133" s="30" t="s">
         <v>653</v>
       </c>
-      <c r="G133" s="41" t="s">
+      <c r="G133" s="40" t="s">
         <v>654</v>
       </c>
-      <c r="H133" s="41" t="s">
+      <c r="H133" s="40" t="s">
         <v>655</v>
       </c>
       <c r="I133" s="15"/>
@@ -11496,7 +11496,7 @@
       <c r="B135" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C135" s="42" t="n">
+      <c r="C135" s="41" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11512,8 +11512,8 @@
       <c r="H135" s="1" t="s">
         <v>662</v>
       </c>
-      <c r="L135" s="43"/>
-      <c r="M135" s="44"/>
+      <c r="L135" s="42"/>
+      <c r="M135" s="43"/>
       <c r="T135" s="1" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
@@ -11625,28 +11625,28 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="27.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="15.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="45" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="44" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="19.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="12.14"/>
   </cols>
   <sheetData>
-    <row r="1" s="48" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="46" t="s">
+    <row r="1" s="47" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="45" t="s">
         <v>663</v>
       </c>
-      <c r="B1" s="46" t="s">
+      <c r="B1" s="45" t="s">
         <v>664</v>
       </c>
-      <c r="C1" s="46" t="s">
+      <c r="C1" s="45" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="47" t="s">
+      <c r="D1" s="46" t="s">
         <v>665</v>
       </c>
-      <c r="E1" s="46" t="s">
+      <c r="E1" s="45" t="s">
         <v>666</v>
       </c>
-      <c r="F1" s="46" t="s">
+      <c r="F1" s="45" t="s">
         <v>667</v>
       </c>
     </row>
@@ -11658,7 +11658,7 @@
       <c r="C2" s="10" t="s">
         <v>669</v>
       </c>
-      <c r="D2" s="49" t="s">
+      <c r="D2" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E2" s="10" t="n">
@@ -11674,7 +11674,7 @@
       <c r="C3" s="10" t="s">
         <v>669</v>
       </c>
-      <c r="D3" s="49" t="s">
+      <c r="D3" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E3" s="10" t="n">
@@ -11690,7 +11690,7 @@
       <c r="C4" s="10" t="s">
         <v>672</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E4" s="10" t="s">
@@ -11708,7 +11708,7 @@
       <c r="C5" s="10" t="s">
         <v>669</v>
       </c>
-      <c r="D5" s="49" t="s">
+      <c r="D5" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E5" s="10" t="n">
@@ -11724,7 +11724,7 @@
       <c r="C6" s="10" t="s">
         <v>675</v>
       </c>
-      <c r="D6" s="49" t="s">
+      <c r="D6" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E6" s="10" t="n">
@@ -11740,7 +11740,7 @@
       <c r="C7" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D7" s="49" t="s">
+      <c r="D7" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E7" s="10" t="n">
@@ -11758,7 +11758,7 @@
       <c r="C8" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D8" s="49" t="s">
+      <c r="D8" s="48" t="s">
         <v>679</v>
       </c>
       <c r="E8" s="10" t="n">
@@ -11774,7 +11774,7 @@
       <c r="C9" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D9" s="49" t="s">
+      <c r="D9" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E9" s="10" t="n">
@@ -11792,7 +11792,7 @@
       <c r="C10" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="48" t="s">
         <v>679</v>
       </c>
       <c r="E10" s="10" t="n">
@@ -11808,7 +11808,7 @@
       <c r="C11" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D11" s="49" t="s">
+      <c r="D11" s="48" t="s">
         <v>679</v>
       </c>
       <c r="E11" s="10" t="n">
@@ -11824,7 +11824,7 @@
       <c r="C12" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D12" s="49" t="s">
+      <c r="D12" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E12" s="10" t="n">
@@ -11840,7 +11840,7 @@
       <c r="C13" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E13" s="10" t="n">
@@ -11856,7 +11856,7 @@
       <c r="C14" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E14" s="10" t="n">
@@ -11872,7 +11872,7 @@
       <c r="C15" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D15" s="49" t="s">
+      <c r="D15" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E15" s="10" t="n">
@@ -11888,7 +11888,7 @@
       <c r="C16" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D16" s="49" t="s">
+      <c r="D16" s="48" t="s">
         <v>679</v>
       </c>
       <c r="E16" s="10" t="n">
@@ -11906,7 +11906,7 @@
       <c r="C17" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="48" t="s">
         <v>683</v>
       </c>
       <c r="E17" s="10" t="s">
@@ -11922,7 +11922,7 @@
       <c r="C18" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D18" s="49" t="s">
+      <c r="D18" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E18" s="10" t="n">
@@ -11938,7 +11938,7 @@
       <c r="C19" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D19" s="49" t="s">
+      <c r="D19" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E19" s="10" t="n">
@@ -11954,7 +11954,7 @@
       <c r="C20" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="48" t="s">
         <v>679</v>
       </c>
       <c r="E20" s="10" t="n">
@@ -11972,7 +11972,7 @@
       <c r="C21" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D21" s="49" t="s">
+      <c r="D21" s="48" t="s">
         <v>683</v>
       </c>
       <c r="E21" s="10" t="s">
@@ -11988,7 +11988,7 @@
       <c r="C22" s="10" t="s">
         <v>677</v>
       </c>
-      <c r="D22" s="49" t="s">
+      <c r="D22" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E22" s="10" t="n">
@@ -12004,7 +12004,7 @@
       <c r="C23" s="10" t="s">
         <v>687</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E23" s="10" t="s">
@@ -12019,10 +12019,10 @@
       <c r="C24" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="D24" s="49" t="s">
+      <c r="D24" s="48" t="s">
         <v>670</v>
       </c>
-      <c r="E24" s="45" t="s">
+      <c r="E24" s="44" t="s">
         <v>689</v>
       </c>
     </row>
@@ -12036,10 +12036,10 @@
       <c r="C25" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="D25" s="49" t="s">
+      <c r="D25" s="48" t="s">
         <v>670</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="44" t="s">
         <v>690</v>
       </c>
     </row>
@@ -12053,10 +12053,10 @@
       <c r="C26" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="D26" s="49" t="s">
+      <c r="D26" s="48" t="s">
         <v>670</v>
       </c>
-      <c r="E26" s="45" t="s">
+      <c r="E26" s="44" t="s">
         <v>691</v>
       </c>
     </row>
@@ -12067,10 +12067,10 @@
       <c r="C27" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="D27" s="49" t="s">
+      <c r="D27" s="48" t="s">
         <v>670</v>
       </c>
-      <c r="E27" s="45" t="s">
+      <c r="E27" s="44" t="s">
         <v>692</v>
       </c>
     </row>
@@ -12084,10 +12084,10 @@
       <c r="C28" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="D28" s="49" t="s">
+      <c r="D28" s="48" t="s">
         <v>670</v>
       </c>
-      <c r="E28" s="45" t="s">
+      <c r="E28" s="44" t="s">
         <v>693</v>
       </c>
     </row>
@@ -12101,10 +12101,10 @@
       <c r="C29" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="D29" s="48" t="s">
         <v>670</v>
       </c>
-      <c r="E29" s="45" t="s">
+      <c r="E29" s="44" t="s">
         <v>691</v>
       </c>
     </row>
@@ -12115,7 +12115,7 @@
       <c r="C30" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="D30" s="49" t="s">
+      <c r="D30" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E30" s="2" t="s">
@@ -12132,7 +12132,7 @@
       <c r="C31" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="D31" s="49" t="s">
+      <c r="D31" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E31" s="2" t="s">
@@ -12149,7 +12149,7 @@
       <c r="C32" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="D32" s="49" t="s">
+      <c r="D32" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E32" s="2" t="s">
@@ -12166,7 +12166,7 @@
       <c r="C33" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="D33" s="49" t="s">
+      <c r="D33" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E33" s="2" t="s">
@@ -12183,7 +12183,7 @@
       <c r="C34" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="D34" s="49" t="s">
+      <c r="D34" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E34" s="2" t="s">
@@ -12200,7 +12200,7 @@
       <c r="C35" s="2" t="s">
         <v>698</v>
       </c>
-      <c r="D35" s="49" t="s">
+      <c r="D35" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E35" s="2" t="s">
@@ -12211,10 +12211,10 @@
       <c r="A36" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C36" s="50" t="s">
+      <c r="C36" s="49" t="s">
         <v>32</v>
       </c>
-      <c r="D36" s="45" t="s">
+      <c r="D36" s="44" t="s">
         <v>670</v>
       </c>
       <c r="E36" s="2" t="s">
@@ -12222,27 +12222,27 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="50" t="s">
         <v>603</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>597</v>
       </c>
-      <c r="D37" s="52" t="s">
+      <c r="D37" s="51" t="s">
         <v>670</v>
       </c>
-      <c r="E37" s="53" t="s">
+      <c r="E37" s="52" t="s">
         <v>673</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="51" t="s">
+      <c r="A38" s="50" t="s">
         <v>620</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>699</v>
       </c>
-      <c r="D38" s="49" t="s">
+      <c r="D38" s="48" t="s">
         <v>671</v>
       </c>
       <c r="E38" s="2" t="n">
@@ -12250,13 +12250,13 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="54" t="s">
+      <c r="A39" s="53" t="s">
         <v>700</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="D39" s="45" t="s">
+      <c r="D39" s="44" t="s">
         <v>670</v>
       </c>
       <c r="E39" s="2" t="s">
@@ -12270,7 +12270,7 @@
       <c r="C40" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="D40" s="49" t="s">
+      <c r="D40" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E40" s="2" t="s">
@@ -12287,7 +12287,7 @@
       <c r="C41" s="2" t="s">
         <v>694</v>
       </c>
-      <c r="D41" s="49" t="s">
+      <c r="D41" s="48" t="s">
         <v>670</v>
       </c>
       <c r="E41" s="2" t="s">
@@ -12295,16 +12295,16 @@
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="55" t="s">
+      <c r="A42" s="54" t="s">
         <v>166</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>688</v>
       </c>
-      <c r="D42" s="45" t="s">
+      <c r="D42" s="44" t="s">
         <v>670</v>
       </c>
-      <c r="E42" s="56" t="s">
+      <c r="E42" s="55" t="s">
         <v>702</v>
       </c>
     </row>
@@ -12315,10 +12315,10 @@
       <c r="C43" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="D43" s="49" t="s">
+      <c r="D43" s="48" t="s">
         <v>670</v>
       </c>
-      <c r="E43" s="45" t="s">
+      <c r="E43" s="44" t="s">
         <v>704</v>
       </c>
     </row>
@@ -12329,10 +12329,10 @@
       <c r="C44" s="2" t="s">
         <v>703</v>
       </c>
-      <c r="D44" s="49" t="s">
+      <c r="D44" s="48" t="s">
         <v>670</v>
       </c>
-      <c r="E44" s="45" t="s">
+      <c r="E44" s="44" t="s">
         <v>705</v>
       </c>
     </row>
@@ -12343,10 +12343,10 @@
       <c r="C45" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="D45" s="52" t="s">
+      <c r="D45" s="51" t="s">
         <v>670</v>
       </c>
-      <c r="E45" s="53" t="s">
+      <c r="E45" s="52" t="s">
         <v>673</v>
       </c>
     </row>
@@ -12357,7 +12357,7 @@
       <c r="C46" s="10" t="s">
         <v>548</v>
       </c>
-      <c r="D46" s="45" t="s">
+      <c r="D46" s="44" t="s">
         <v>670</v>
       </c>
       <c r="E46" s="2" t="s">
@@ -12410,28 +12410,28 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="56" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="57" t="s">
         <v>706</v>
       </c>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="56" t="s">
         <v>707</v>
       </c>
-      <c r="D1" s="57" t="s">
+      <c r="D1" s="56" t="s">
         <v>708</v>
       </c>
-      <c r="E1" s="57" t="s">
+      <c r="E1" s="56" t="s">
         <v>709</v>
       </c>
-      <c r="F1" s="57" t="s">
+      <c r="F1" s="56" t="s">
         <v>710</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>711</v>
       </c>
-      <c r="H1" s="57" t="s">
+      <c r="H1" s="56" t="s">
         <v>712</v>
       </c>
     </row>
@@ -12448,15 +12448,15 @@
       <c r="D2" s="10" t="s">
         <v>715</v>
       </c>
-      <c r="E2" s="59" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="59" t="b">
+      <c r="E2" s="58" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="59" t="b">
+      <c r="G2" s="58" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12474,15 +12474,15 @@
       <c r="D3" s="10" t="s">
         <v>718</v>
       </c>
-      <c r="E3" s="59" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="59" t="b">
+      <c r="E3" s="58" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="59" t="b">
+      <c r="G3" s="58" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12500,15 +12500,15 @@
       <c r="D4" s="10" t="s">
         <v>722</v>
       </c>
-      <c r="E4" s="59" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="59" t="b">
+      <c r="E4" s="58" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="59" t="b">
+      <c r="G4" s="58" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12526,15 +12526,15 @@
       <c r="D5" s="10" t="s">
         <v>725</v>
       </c>
-      <c r="E5" s="59" t="b">
+      <c r="E5" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F5" s="59" t="b">
+      <c r="F5" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="59" t="b">
+      <c r="G5" s="58" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12555,15 +12555,15 @@
       <c r="D6" s="10" t="s">
         <v>722</v>
       </c>
-      <c r="E6" s="59" t="b">
+      <c r="E6" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F6" s="59" t="b">
+      <c r="F6" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G6" s="59" t="b">
+      <c r="G6" s="58" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12584,15 +12584,15 @@
       <c r="D7" s="10" t="s">
         <v>721</v>
       </c>
-      <c r="E7" s="59" t="b">
+      <c r="E7" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F7" s="59" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G7" s="59"/>
+      <c r="F7" s="58" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="58"/>
       <c r="H7" s="10" t="s">
         <v>719</v>
       </c>
@@ -12610,15 +12610,15 @@
       <c r="D8" s="10" t="s">
         <v>731</v>
       </c>
-      <c r="E8" s="59" t="b">
+      <c r="E8" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F8" s="59" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="59"/>
+      <c r="F8" s="58" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="58"/>
       <c r="H8" s="10" t="s">
         <v>719</v>
       </c>
@@ -12636,15 +12636,15 @@
       <c r="D9" s="10" t="s">
         <v>734</v>
       </c>
-      <c r="E9" s="59" t="b">
+      <c r="E9" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F9" s="59" t="b">
+      <c r="F9" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G9" s="59" t="b">
+      <c r="G9" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12665,15 +12665,15 @@
       <c r="D10" s="10" t="s">
         <v>737</v>
       </c>
-      <c r="E10" s="59" t="b">
+      <c r="E10" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F10" s="59" t="b">
+      <c r="F10" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G10" s="59" t="b">
+      <c r="G10" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12694,15 +12694,15 @@
       <c r="D11" s="10" t="s">
         <v>740</v>
       </c>
-      <c r="E11" s="59" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F11" s="59" t="b">
+      <c r="E11" s="58" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G11" s="59" t="b">
+      <c r="G11" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -12720,15 +12720,15 @@
       <c r="D12" s="10" t="s">
         <v>743</v>
       </c>
-      <c r="E12" s="59" t="b">
+      <c r="E12" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F12" s="59" t="b">
+      <c r="F12" s="58" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G12" s="59" t="b">
+      <c r="G12" s="58" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12754,31 +12754,31 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="54" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="54" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="54" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="54" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="54" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="54" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="53" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="53" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="53" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="53" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="53" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="53" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="59" t="s">
         <v>744</v>
       </c>
-      <c r="B1" s="60" t="s">
+      <c r="B1" s="59" t="s">
         <v>666</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="59" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="60" t="s">
+      <c r="D1" s="59" t="s">
         <v>7</v>
       </c>
       <c r="E1" s="5" t="s">
@@ -12787,13 +12787,13 @@
       <c r="F1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="60" t="s">
+      <c r="G1" s="59" t="s">
         <v>745</v>
       </c>
-      <c r="H1" s="60" t="s">
+      <c r="H1" s="59" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="54" t="s">
+      <c r="I1" s="53" t="s">
         <v>746</v>
       </c>
     </row>
@@ -13002,7 +13002,7 @@
         <v>760</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" s="54"/>
+      <c r="I14" s="53"/>
     </row>
     <row r="15" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="21" t="s">
@@ -13301,7 +13301,7 @@
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
-      <c r="I31" s="54" t="s">
+      <c r="I31" s="53" t="s">
         <v>792</v>
       </c>
     </row>
@@ -13322,7 +13322,7 @@
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
-      <c r="I32" s="54" t="s">
+      <c r="I32" s="53" t="s">
         <v>792</v>
       </c>
     </row>
@@ -13343,7 +13343,7 @@
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
-      <c r="I33" s="54" t="s">
+      <c r="I33" s="53" t="s">
         <v>792</v>
       </c>
     </row>
@@ -13364,7 +13364,7 @@
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
-      <c r="I34" s="54" t="s">
+      <c r="I34" s="53" t="s">
         <v>792</v>
       </c>
     </row>
@@ -13385,7 +13385,7 @@
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
-      <c r="I35" s="54" t="s">
+      <c r="I35" s="53" t="s">
         <v>792</v>
       </c>
     </row>
@@ -13693,13 +13693,13 @@
       <c r="A53" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="B53" s="54" t="s">
+      <c r="B53" s="53" t="s">
         <v>695</v>
       </c>
-      <c r="C53" s="54" t="s">
+      <c r="C53" s="53" t="s">
         <v>837</v>
       </c>
-      <c r="D53" s="54" t="s">
+      <c r="D53" s="53" t="s">
         <v>827</v>
       </c>
     </row>
@@ -13707,13 +13707,13 @@
       <c r="A54" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="B54" s="54" t="s">
+      <c r="B54" s="53" t="s">
         <v>696</v>
       </c>
-      <c r="C54" s="54" t="s">
+      <c r="C54" s="53" t="s">
         <v>838</v>
       </c>
-      <c r="D54" s="54" t="s">
+      <c r="D54" s="53" t="s">
         <v>839</v>
       </c>
     </row>
@@ -13721,32 +13721,32 @@
       <c r="A55" s="21" t="s">
         <v>220</v>
       </c>
-      <c r="B55" s="54" t="s">
+      <c r="B55" s="53" t="s">
         <v>701</v>
       </c>
-      <c r="C55" s="54" t="s">
+      <c r="C55" s="53" t="s">
         <v>840</v>
       </c>
-      <c r="D55" s="54" t="s">
+      <c r="D55" s="53" t="s">
         <v>841</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="54" t="s">
+      <c r="A56" s="53" t="s">
         <v>596</v>
       </c>
-      <c r="B56" s="54" t="s">
+      <c r="B56" s="53" t="s">
         <v>842</v>
       </c>
-      <c r="C56" s="54" t="s">
+      <c r="C56" s="53" t="s">
         <v>843</v>
       </c>
-      <c r="D56" s="54" t="s">
+      <c r="D56" s="53" t="s">
         <v>844</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="54" t="s">
+      <c r="A57" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B57" s="10" t="s">
@@ -13762,7 +13762,7 @@
       <c r="F57" s="10"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="54" t="s">
+      <c r="A58" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B58" s="10" t="s">
@@ -13778,7 +13778,7 @@
       <c r="F58" s="10"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="54" t="s">
+      <c r="A59" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B59" s="10" t="s">
@@ -13794,7 +13794,7 @@
       <c r="F59" s="10"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="54" t="s">
+      <c r="A60" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B60" s="10" t="s">
@@ -13810,7 +13810,7 @@
       <c r="F60" s="10"/>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="54" t="s">
+      <c r="A61" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B61" s="10" t="s">
@@ -13826,7 +13826,7 @@
       <c r="F61" s="10"/>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="54" t="s">
+      <c r="A62" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B62" s="10" t="s">
@@ -13842,7 +13842,7 @@
       <c r="F62" s="10"/>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="54" t="s">
+      <c r="A63" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B63" s="10" t="s">
@@ -13858,7 +13858,7 @@
       <c r="F63" s="10"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="54" t="s">
+      <c r="A64" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B64" s="10" t="s">
@@ -13874,7 +13874,7 @@
       <c r="F64" s="10"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="54" t="s">
+      <c r="A65" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B65" s="10" t="s">
@@ -13890,7 +13890,7 @@
       <c r="F65" s="10"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="54" t="s">
+      <c r="A66" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B66" s="10" t="s">
@@ -13906,7 +13906,7 @@
       <c r="F66" s="10"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="54" t="s">
+      <c r="A67" s="53" t="s">
         <v>596</v>
       </c>
       <c r="B67" s="10" t="s">
@@ -13922,94 +13922,94 @@
       <c r="F67" s="10"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="54" t="s">
+      <c r="A68" s="53" t="s">
         <v>596</v>
       </c>
-      <c r="B68" s="54" t="s">
+      <c r="B68" s="53" t="s">
         <v>878</v>
       </c>
-      <c r="C68" s="54" t="s">
+      <c r="C68" s="53" t="s">
         <v>879</v>
       </c>
-      <c r="D68" s="54" t="s">
+      <c r="D68" s="53" t="s">
         <v>880</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="54" t="s">
+      <c r="A69" s="53" t="s">
         <v>596</v>
       </c>
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="53" t="s">
         <v>757</v>
       </c>
-      <c r="C69" s="54" t="s">
+      <c r="C69" s="53" t="s">
         <v>758</v>
       </c>
-      <c r="D69" s="54" t="s">
+      <c r="D69" s="53" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="54" t="s">
+      <c r="A70" s="53" t="s">
         <v>596</v>
       </c>
-      <c r="B70" s="54" t="s">
+      <c r="B70" s="53" t="s">
         <v>881</v>
       </c>
-      <c r="C70" s="54" t="s">
+      <c r="C70" s="53" t="s">
         <v>761</v>
       </c>
-      <c r="D70" s="54" t="s">
+      <c r="D70" s="53" t="s">
         <v>882</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="61" t="s">
+      <c r="A71" s="60" t="s">
         <v>591</v>
       </c>
       <c r="B71" s="10" t="s">
         <v>883</v>
       </c>
-      <c r="C71" s="54" t="s">
+      <c r="C71" s="53" t="s">
         <v>884</v>
       </c>
-      <c r="D71" s="54" t="s">
+      <c r="D71" s="53" t="s">
         <v>885</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="61" t="s">
+      <c r="A72" s="60" t="s">
         <v>591</v>
       </c>
-      <c r="B72" s="54" t="s">
+      <c r="B72" s="53" t="s">
         <v>886</v>
       </c>
-      <c r="C72" s="54" t="s">
+      <c r="C72" s="53" t="s">
         <v>887</v>
       </c>
-      <c r="D72" s="54" t="s">
+      <c r="D72" s="53" t="s">
         <v>888</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="61" t="s">
+      <c r="A73" s="60" t="s">
         <v>591</v>
       </c>
-      <c r="B73" s="54" t="s">
+      <c r="B73" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="C73" s="54" t="s">
+      <c r="C73" s="53" t="s">
         <v>755</v>
       </c>
-      <c r="D73" s="54" t="s">
+      <c r="D73" s="53" t="s">
         <v>756</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="61" t="s">
+      <c r="A74" s="60" t="s">
         <v>591</v>
       </c>
-      <c r="B74" s="54" t="s">
+      <c r="B74" s="53" t="s">
         <v>760</v>
       </c>
       <c r="C74" s="10" t="s">
@@ -14025,13 +14025,13 @@
       <c r="A75" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B75" s="54" t="s">
+      <c r="B75" s="53" t="s">
         <v>889</v>
       </c>
-      <c r="C75" s="62" t="s">
+      <c r="C75" s="61" t="s">
         <v>890</v>
       </c>
-      <c r="D75" s="54" t="s">
+      <c r="D75" s="53" t="s">
         <v>891</v>
       </c>
       <c r="H75" s="10" t="s">
@@ -14042,17 +14042,17 @@
       <c r="A76" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B76" s="54" t="s">
+      <c r="B76" s="53" t="s">
         <v>892</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>893</v>
       </c>
-      <c r="D76" s="62" t="s">
+      <c r="D76" s="61" t="s">
         <v>894</v>
       </c>
-      <c r="E76" s="62"/>
-      <c r="F76" s="62"/>
+      <c r="E76" s="61"/>
+      <c r="F76" s="61"/>
       <c r="H76" s="2" t="s">
         <v>203</v>
       </c>
@@ -14061,13 +14061,13 @@
       <c r="A77" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B77" s="54" t="s">
+      <c r="B77" s="53" t="s">
         <v>895</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>896</v>
       </c>
-      <c r="D77" s="54" t="s">
+      <c r="D77" s="53" t="s">
         <v>897</v>
       </c>
     </row>
@@ -14075,7 +14075,7 @@
       <c r="A78" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B78" s="54" t="s">
+      <c r="B78" s="53" t="s">
         <v>898</v>
       </c>
       <c r="C78" s="10" t="s">
@@ -14091,7 +14091,7 @@
       <c r="A79" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B79" s="54" t="s">
+      <c r="B79" s="53" t="s">
         <v>901</v>
       </c>
       <c r="C79" s="10" t="s">
@@ -14107,7 +14107,7 @@
       <c r="A80" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B80" s="54" t="s">
+      <c r="B80" s="53" t="s">
         <v>904</v>
       </c>
       <c r="C80" s="10" t="s">
@@ -14126,7 +14126,7 @@
       <c r="A81" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B81" s="54" t="s">
+      <c r="B81" s="53" t="s">
         <v>907</v>
       </c>
       <c r="C81" s="10" t="s">
@@ -14142,7 +14142,7 @@
       <c r="A82" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B82" s="54" t="s">
+      <c r="B82" s="53" t="s">
         <v>910</v>
       </c>
       <c r="C82" s="10" t="s">
@@ -14161,13 +14161,13 @@
       <c r="A83" s="30" t="s">
         <v>317</v>
       </c>
-      <c r="B83" s="54" t="s">
+      <c r="B83" s="53" t="s">
         <v>154</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>755</v>
       </c>
-      <c r="D83" s="54" t="s">
+      <c r="D83" s="53" t="s">
         <v>756</v>
       </c>
     </row>
@@ -14175,13 +14175,13 @@
       <c r="A84" s="30" t="s">
         <v>913</v>
       </c>
-      <c r="B84" s="54" t="s">
+      <c r="B84" s="53" t="s">
         <v>27</v>
       </c>
-      <c r="C84" s="54" t="s">
+      <c r="C84" s="53" t="s">
         <v>714</v>
       </c>
-      <c r="D84" s="54" t="s">
+      <c r="D84" s="53" t="s">
         <v>715</v>
       </c>
     </row>
@@ -14189,16 +14189,16 @@
       <c r="A85" s="30" t="s">
         <v>913</v>
       </c>
-      <c r="B85" s="54" t="s">
+      <c r="B85" s="53" t="s">
         <v>914</v>
       </c>
-      <c r="C85" s="54" t="s">
+      <c r="C85" s="53" t="s">
         <v>915</v>
       </c>
-      <c r="D85" s="54" t="s">
+      <c r="D85" s="53" t="s">
         <v>916</v>
       </c>
-      <c r="H85" s="54" t="s">
+      <c r="H85" s="53" t="s">
         <v>700</v>
       </c>
     </row>
@@ -14206,13 +14206,13 @@
       <c r="A86" s="30" t="s">
         <v>913</v>
       </c>
-      <c r="B86" s="54" t="s">
+      <c r="B86" s="53" t="s">
         <v>154</v>
       </c>
-      <c r="C86" s="54" t="s">
+      <c r="C86" s="53" t="s">
         <v>917</v>
       </c>
-      <c r="D86" s="54" t="s">
+      <c r="D86" s="53" t="s">
         <v>918</v>
       </c>
     </row>
@@ -14235,7 +14235,7 @@
       <c r="F87" s="10" t="s">
         <v>923</v>
       </c>
-      <c r="H87" s="54" t="s">
+      <c r="H87" s="53" t="s">
         <v>924</v>
       </c>
     </row>
@@ -14243,7 +14243,7 @@
       <c r="A88" s="30" t="s">
         <v>925</v>
       </c>
-      <c r="B88" s="54" t="s">
+      <c r="B88" s="53" t="s">
         <v>926</v>
       </c>
       <c r="C88" s="10" t="s">
@@ -14263,7 +14263,7 @@
       <c r="A89" s="30" t="s">
         <v>925</v>
       </c>
-      <c r="B89" s="54" t="s">
+      <c r="B89" s="53" t="s">
         <v>931</v>
       </c>
       <c r="C89" s="10" t="s">
@@ -14283,13 +14283,13 @@
       <c r="A90" s="30" t="s">
         <v>925</v>
       </c>
-      <c r="B90" s="54" t="s">
+      <c r="B90" s="53" t="s">
         <v>749</v>
       </c>
-      <c r="C90" s="54" t="s">
+      <c r="C90" s="53" t="s">
         <v>750</v>
       </c>
-      <c r="D90" s="54" t="s">
+      <c r="D90" s="53" t="s">
         <v>751</v>
       </c>
     </row>
@@ -14438,91 +14438,91 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="63" t="s">
+      <c r="A103" s="62" t="s">
         <v>168</v>
       </c>
       <c r="B103" s="10" t="s">
         <v>957</v>
       </c>
-      <c r="C103" s="54" t="s">
+      <c r="C103" s="53" t="s">
         <v>958</v>
       </c>
-      <c r="D103" s="54" t="s">
+      <c r="D103" s="53" t="s">
         <v>959</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="63" t="s">
+      <c r="A104" s="62" t="s">
         <v>168</v>
       </c>
-      <c r="B104" s="54" t="s">
+      <c r="B104" s="53" t="s">
         <v>960</v>
       </c>
-      <c r="C104" s="54" t="s">
+      <c r="C104" s="53" t="s">
         <v>961</v>
       </c>
-      <c r="D104" s="54" t="s">
+      <c r="D104" s="53" t="s">
         <v>962</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="63" t="s">
+      <c r="A105" s="62" t="s">
         <v>168</v>
       </c>
       <c r="B105" s="10" t="s">
         <v>963</v>
       </c>
-      <c r="C105" s="54" t="s">
+      <c r="C105" s="53" t="s">
         <v>964</v>
       </c>
-      <c r="D105" s="54" t="s">
+      <c r="D105" s="53" t="s">
         <v>965</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="63" t="s">
+      <c r="A106" s="62" t="s">
         <v>168</v>
       </c>
       <c r="B106" s="10" t="s">
         <v>966</v>
       </c>
-      <c r="C106" s="54" t="s">
+      <c r="C106" s="53" t="s">
         <v>967</v>
       </c>
-      <c r="D106" s="54" t="s">
+      <c r="D106" s="53" t="s">
         <v>968</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="63" t="s">
+      <c r="A107" s="62" t="s">
         <v>168</v>
       </c>
       <c r="B107" s="10" t="s">
         <v>969</v>
       </c>
-      <c r="C107" s="54" t="s">
+      <c r="C107" s="53" t="s">
         <v>970</v>
       </c>
-      <c r="D107" s="54" t="s">
+      <c r="D107" s="53" t="s">
         <v>971</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="63" t="s">
+      <c r="A108" s="62" t="s">
         <v>168</v>
       </c>
       <c r="B108" s="10" t="s">
         <v>972</v>
       </c>
-      <c r="C108" s="54" t="s">
+      <c r="C108" s="53" t="s">
         <v>973</v>
       </c>
-      <c r="D108" s="54" t="s">
+      <c r="D108" s="53" t="s">
         <v>974</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="63" t="s">
+      <c r="A109" s="62" t="s">
         <v>168</v>
       </c>
       <c r="G109" s="1" t="s">
@@ -14671,193 +14671,193 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="60" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="64" t="s">
+    <row r="1" s="59" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="63" t="s">
         <v>996</v>
       </c>
-      <c r="B1" s="64" t="s">
+      <c r="B1" s="63" t="s">
         <v>997</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="63" t="s">
         <v>998</v>
       </c>
-      <c r="D1" s="64" t="s">
+      <c r="D1" s="63" t="s">
         <v>999</v>
       </c>
-      <c r="E1" s="64" t="s">
+      <c r="E1" s="63" t="s">
         <v>1000</v>
       </c>
-      <c r="F1" s="64" t="s">
+      <c r="F1" s="63" t="s">
         <v>1001</v>
       </c>
-      <c r="G1" s="64" t="s">
+      <c r="G1" s="63" t="s">
         <v>1002</v>
       </c>
-      <c r="H1" s="64" t="s">
+      <c r="H1" s="63" t="s">
         <v>1003</v>
       </c>
-      <c r="I1" s="64" t="s">
+      <c r="I1" s="63" t="s">
         <v>1004</v>
       </c>
-      <c r="J1" s="64" t="s">
+      <c r="J1" s="63" t="s">
         <v>1005</v>
       </c>
-      <c r="K1" s="64" t="s">
+      <c r="K1" s="63" t="s">
         <v>1006</v>
       </c>
-      <c r="L1" s="60" t="s">
+      <c r="L1" s="59" t="s">
         <v>1007</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="41" t="s">
+      <c r="A2" s="40" t="s">
         <v>632</v>
       </c>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="40" t="s">
         <v>1008</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="40" t="s">
         <v>1009</v>
       </c>
-      <c r="D2" s="41" t="s">
+      <c r="D2" s="40" t="s">
         <v>1010</v>
       </c>
-      <c r="E2" s="41" t="s">
+      <c r="E2" s="40" t="s">
         <v>1011</v>
       </c>
-      <c r="F2" s="41" t="s">
+      <c r="F2" s="40" t="s">
         <v>1012</v>
       </c>
-      <c r="G2" s="41" t="s">
+      <c r="G2" s="40" t="s">
         <v>1013</v>
       </c>
-      <c r="H2" s="41" t="n">
+      <c r="H2" s="40" t="n">
         <v>-10</v>
       </c>
-      <c r="I2" s="41" t="n">
+      <c r="I2" s="40" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="41" t="s">
+      <c r="J2" s="40" t="s">
         <v>1014</v>
       </c>
-      <c r="K2" s="41" t="s">
+      <c r="K2" s="40" t="s">
         <v>1014</v>
       </c>
-      <c r="L2" s="41" t="s">
+      <c r="L2" s="40" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="41" t="s">
+      <c r="A3" s="40" t="s">
         <v>641</v>
       </c>
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="40" t="s">
         <v>1016</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="40" t="s">
         <v>1017</v>
       </c>
-      <c r="D3" s="65" t="s">
+      <c r="D3" s="64" t="s">
         <v>1018</v>
       </c>
-      <c r="E3" s="65" t="s">
+      <c r="E3" s="64" t="s">
         <v>1019</v>
       </c>
-      <c r="F3" s="65" t="s">
+      <c r="F3" s="64" t="s">
         <v>1020</v>
       </c>
-      <c r="G3" s="41" t="s">
+      <c r="G3" s="40" t="s">
         <v>1021</v>
       </c>
-      <c r="H3" s="41" t="n">
+      <c r="H3" s="40" t="n">
         <v>-10</v>
       </c>
-      <c r="I3" s="41" t="n">
+      <c r="I3" s="40" t="n">
         <v>100</v>
       </c>
-      <c r="J3" s="41" t="s">
+      <c r="J3" s="40" t="s">
         <v>1014</v>
       </c>
-      <c r="K3" s="41" t="s">
+      <c r="K3" s="40" t="s">
         <v>1014</v>
       </c>
-      <c r="L3" s="41" t="s">
+      <c r="L3" s="40" t="s">
         <v>1022</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="40" t="s">
         <v>646</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="40" t="s">
         <v>1023</v>
       </c>
-      <c r="C4" s="41" t="s">
+      <c r="C4" s="40" t="s">
         <v>1024</v>
       </c>
-      <c r="D4" s="41" t="s">
+      <c r="D4" s="40" t="s">
         <v>1025</v>
       </c>
-      <c r="E4" s="41" t="s">
+      <c r="E4" s="40" t="s">
         <v>1026</v>
       </c>
-      <c r="F4" s="41" t="s">
+      <c r="F4" s="40" t="s">
         <v>1027</v>
       </c>
-      <c r="G4" s="41" t="s">
+      <c r="G4" s="40" t="s">
         <v>1028</v>
       </c>
-      <c r="H4" s="41" t="n">
+      <c r="H4" s="40" t="n">
         <v>-10</v>
       </c>
-      <c r="I4" s="41" t="n">
+      <c r="I4" s="40" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="41" t="s">
+      <c r="J4" s="40" t="s">
         <v>1014</v>
       </c>
-      <c r="K4" s="41" t="s">
+      <c r="K4" s="40" t="s">
         <v>1014</v>
       </c>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="40" t="s">
         <v>1029</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="41" t="s">
+      <c r="A5" s="40" t="s">
         <v>651</v>
       </c>
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="40" t="s">
         <v>1016</v>
       </c>
-      <c r="C5" s="41" t="s">
+      <c r="C5" s="40" t="s">
         <v>1030</v>
       </c>
-      <c r="D5" s="41" t="s">
+      <c r="D5" s="40" t="s">
         <v>1031</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="40" t="s">
         <v>1019</v>
       </c>
-      <c r="F5" s="41" t="s">
+      <c r="F5" s="40" t="s">
         <v>1032</v>
       </c>
-      <c r="G5" s="41" t="s">
+      <c r="G5" s="40" t="s">
         <v>1033</v>
       </c>
-      <c r="H5" s="41" t="n">
+      <c r="H5" s="40" t="n">
         <v>-10</v>
       </c>
-      <c r="I5" s="41" t="n">
+      <c r="I5" s="40" t="n">
         <v>100</v>
       </c>
-      <c r="J5" s="41" t="s">
+      <c r="J5" s="40" t="s">
         <v>1014</v>
       </c>
-      <c r="K5" s="41" t="s">
+      <c r="K5" s="40" t="s">
         <v>1014</v>
       </c>
-      <c r="L5" s="41" t="s">
+      <c r="L5" s="40" t="s">
         <v>1029</v>
       </c>
     </row>
@@ -14919,7 +14919,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C77" activeCellId="0" sqref="C77"/>
+      <selection pane="topLeft" activeCell="C70" activeCellId="0" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" customHeight="true" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15861,7 +15861,7 @@
       <c r="A60" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="66" t="s">
+      <c r="B60" s="65" t="s">
         <v>1241</v>
       </c>
       <c r="C60" s="10" t="s">
@@ -15903,49 +15903,49 @@
       <c r="A63" s="30" t="s">
         <v>325</v>
       </c>
-      <c r="B63" s="54" t="s">
+      <c r="B63" s="53" t="s">
         <v>1250</v>
       </c>
-      <c r="C63" s="54" t="s">
+      <c r="C63" s="53" t="s">
         <v>714</v>
       </c>
-      <c r="D63" s="54" t="s">
+      <c r="D63" s="53" t="s">
         <v>715</v>
       </c>
-      <c r="E63" s="54"/>
-      <c r="F63" s="54"/>
+      <c r="E63" s="53"/>
+      <c r="F63" s="53"/>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="30" t="s">
         <v>325</v>
       </c>
-      <c r="B64" s="54" t="s">
+      <c r="B64" s="53" t="s">
         <v>1251</v>
       </c>
-      <c r="C64" s="54" t="s">
+      <c r="C64" s="53" t="s">
         <v>915</v>
       </c>
-      <c r="D64" s="54" t="s">
+      <c r="D64" s="53" t="s">
         <v>916</v>
       </c>
-      <c r="E64" s="54"/>
-      <c r="F64" s="54"/>
+      <c r="E64" s="53"/>
+      <c r="F64" s="53"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="30" t="s">
         <v>325</v>
       </c>
-      <c r="B65" s="54" t="s">
+      <c r="B65" s="53" t="s">
         <v>1252</v>
       </c>
-      <c r="C65" s="54" t="s">
+      <c r="C65" s="53" t="s">
         <v>917</v>
       </c>
-      <c r="D65" s="54" t="s">
+      <c r="D65" s="53" t="s">
         <v>918</v>
       </c>
-      <c r="E65" s="54"/>
-      <c r="F65" s="54"/>
+      <c r="E65" s="53"/>
+      <c r="F65" s="53"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="30" t="s">
@@ -15971,7 +15971,7 @@
       <c r="A67" s="30" t="s">
         <v>426</v>
       </c>
-      <c r="B67" s="54" t="s">
+      <c r="B67" s="53" t="s">
         <v>1254</v>
       </c>
       <c r="C67" s="10" t="s">
@@ -15991,7 +15991,7 @@
       <c r="A68" s="30" t="s">
         <v>426</v>
       </c>
-      <c r="B68" s="54" t="s">
+      <c r="B68" s="53" t="s">
         <v>1255</v>
       </c>
       <c r="C68" s="10" t="s">
@@ -16011,7 +16011,7 @@
       <c r="A69" s="30" t="s">
         <v>426</v>
       </c>
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="53" t="s">
         <v>1256</v>
       </c>
       <c r="C69" s="10" t="s">
@@ -16027,7 +16027,7 @@
       <c r="A70" s="30" t="s">
         <v>426</v>
       </c>
-      <c r="B70" s="54" t="s">
+      <c r="B70" s="53" t="s">
         <v>1259</v>
       </c>
       <c r="C70" s="10" t="s">
@@ -16043,7 +16043,7 @@
       <c r="A71" s="30" t="s">
         <v>426</v>
       </c>
-      <c r="B71" s="54" t="s">
+      <c r="B71" s="53" t="s">
         <v>1262</v>
       </c>
       <c r="C71" s="10" t="s">
@@ -16234,16 +16234,16 @@
       <c r="B82" s="2" t="s">
         <v>1285</v>
       </c>
-      <c r="C82" s="35" t="s">
+      <c r="C82" s="10" t="s">
         <v>1286</v>
       </c>
-      <c r="D82" s="35" t="s">
+      <c r="D82" s="10" t="s">
         <v>1287</v>
       </c>
-      <c r="E82" s="35" t="s">
+      <c r="E82" s="10" t="s">
         <v>1288</v>
       </c>
-      <c r="F82" s="35" t="s">
+      <c r="F82" s="10" t="s">
         <v>1289</v>
       </c>
     </row>
@@ -16254,16 +16254,16 @@
       <c r="B83" s="2" t="s">
         <v>1290</v>
       </c>
-      <c r="C83" s="35" t="s">
+      <c r="C83" s="10" t="s">
         <v>1291</v>
       </c>
-      <c r="D83" s="35" t="s">
+      <c r="D83" s="10" t="s">
         <v>1292</v>
       </c>
-      <c r="E83" s="35" t="s">
+      <c r="E83" s="10" t="s">
         <v>1293</v>
       </c>
-      <c r="F83" s="35" t="s">
+      <c r="F83" s="10" t="s">
         <v>1294</v>
       </c>
     </row>
@@ -16274,10 +16274,10 @@
       <c r="B84" s="2" t="s">
         <v>1295</v>
       </c>
-      <c r="C84" s="35" t="s">
+      <c r="C84" s="66" t="s">
         <v>1296</v>
       </c>
-      <c r="D84" s="35" t="s">
+      <c r="D84" s="66" t="s">
         <v>1297</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Label: Fix typo with personDeparturePlaceIsHome
Fix: #191
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -1045,7 +1045,7 @@
   </si>
   <si>
     <t xml:space="preserve">Est-ce que {{nickname}} a **commencé sa journée au domicile** ({{address}})?
-__Répondre 'Non' uniquement si {{nickname}} n'a pas dormi au domicile (nuit du {{dayOne}} au {{dayTwo}}), ou y est rentr{{gender:é/ée/é.e}} après 4h du matin (par ex.: travail de nuit).__</t>
+__Répondre 'Non' uniquement si {{nickname}} n'a pas dormi au domicile (nuit du {{dayOne}} au {{dayTwo}}), ou y est rentré{{gender:/e/(-e)}} après 4h du matin (par ex.: travail de nuit).__</t>
   </si>
   <si>
     <t xml:space="preserve">Did {{nickname}} **start their day at home** ({{address}})?
@@ -1053,7 +1053,7 @@
   </si>
   <si>
     <t xml:space="preserve">Avez-vous **commencé votre journée au domicile** ({{address}})?
-__Répondre 'Non' uniquement si vous n'avez pas dormi au domicile (nuit du {{dayOne}} au {{dayTwo}}), ou y êtes rentré{{gender:é/ée/é.e}} après 4h du matin (par ex.: travail de nuit).__</t>
+__Répondre 'Non' uniquement si vous n'avez pas dormi au domicile (nuit du {{dayOne}} au {{dayTwo}}), ou y êtes rentré{{gender:/e/(-e)}} après 4h du matin (par ex.: travail de nuit).__</t>
   </si>
   <si>
     <t xml:space="preserve">Did you **start your day at home** ({{address}})?
@@ -5115,11 +5115,11 @@
   <dimension ref="A1:XFD135"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="F26" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="F53" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="F1" activeCellId="0" sqref="F1"/>
-      <selection pane="bottomLeft" activeCell="A26" activeCellId="0" sqref="A26"/>
-      <selection pane="bottomRight" activeCell="K34" activeCellId="0" sqref="K34"/>
+      <selection pane="bottomLeft" activeCell="A53" activeCellId="0" sqref="A53"/>
+      <selection pane="bottomRight" activeCell="I54" activeCellId="0" sqref="I54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Label: Prepare age validation PR labels
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2242" uniqueCount="1305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2248" uniqueCount="1310">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -4025,6 +4025,21 @@
   </si>
   <si>
     <t xml:space="preserve">Select "No remote studies" only if no other choice is selected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">popup.validateHouseholdAgesHelp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Au moins un membre de votre ménage doit avoir **16 ans** ou plus pour répondre à ce questionnaire. Veuillez vérifier les âges.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At least one member of your household must be **16 years old** or older to respond to this survey. Please verify ages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vous devez avoir au moins **16 ans** pour répondre à ce questionnaire.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You must be at least **16 years old** to respond to this survey.</t>
   </si>
   <si>
     <t xml:space="preserve">onTheRoadArrivalTypeHome</t>
@@ -5229,11 +5244,11 @@
   <dimension ref="A1:XFD135"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="K1" activeCellId="0" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="A21" activeCellId="0" sqref="A21"/>
-      <selection pane="bottomRight" activeCell="O24" activeCellId="0" sqref="O24"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="I11" activeCellId="0" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12922,7 +12937,7 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E25" activeCellId="0" sqref="E25"/>
     </sheetView>
   </sheetViews>
@@ -15133,15 +15148,14 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A52" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C70" activeCellId="0" sqref="C70"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A43" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H60" activeCellId="0" sqref="H60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="16.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="14.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="19.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="2" style="2" width="33.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="16.43"/>
   </cols>
   <sheetData>
@@ -16115,33 +16129,37 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="37" t="s">
-        <v>327</v>
-      </c>
-      <c r="B63" s="62" t="s">
+      <c r="A63" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B63" s="11" t="s">
         <v>1257</v>
       </c>
-      <c r="C63" s="62" t="s">
-        <v>716</v>
-      </c>
-      <c r="D63" s="62" t="s">
-        <v>717</v>
-      </c>
-      <c r="E63" s="62"/>
-      <c r="F63" s="62"/>
+      <c r="C63" s="11" t="s">
+        <v>1258</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>1259</v>
+      </c>
+      <c r="E63" s="0" t="s">
+        <v>1260</v>
+      </c>
+      <c r="F63" s="0" t="s">
+        <v>1261</v>
+      </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="37" t="s">
         <v>327</v>
       </c>
       <c r="B64" s="62" t="s">
-        <v>1258</v>
+        <v>1262</v>
       </c>
       <c r="C64" s="62" t="s">
-        <v>922</v>
+        <v>716</v>
       </c>
       <c r="D64" s="62" t="s">
-        <v>923</v>
+        <v>717</v>
       </c>
       <c r="E64" s="62"/>
       <c r="F64" s="62"/>
@@ -16151,13 +16169,13 @@
         <v>327</v>
       </c>
       <c r="B65" s="62" t="s">
-        <v>1259</v>
+        <v>1263</v>
       </c>
       <c r="C65" s="62" t="s">
-        <v>924</v>
+        <v>922</v>
       </c>
       <c r="D65" s="62" t="s">
-        <v>925</v>
+        <v>923</v>
       </c>
       <c r="E65" s="62"/>
       <c r="F65" s="62"/>
@@ -16166,40 +16184,36 @@
       <c r="A66" s="37" t="s">
         <v>327</v>
       </c>
-      <c r="B66" s="11" t="s">
-        <v>1260</v>
-      </c>
-      <c r="C66" s="11" t="s">
-        <v>927</v>
-      </c>
-      <c r="D66" s="11" t="s">
-        <v>928</v>
-      </c>
-      <c r="E66" s="11" t="s">
-        <v>929</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>930</v>
-      </c>
+      <c r="B66" s="62" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C66" s="62" t="s">
+        <v>924</v>
+      </c>
+      <c r="D66" s="62" t="s">
+        <v>925</v>
+      </c>
+      <c r="E66" s="62"/>
+      <c r="F66" s="62"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="37" t="s">
-        <v>428</v>
-      </c>
-      <c r="B67" s="62" t="s">
-        <v>1261</v>
+        <v>327</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>1265</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>934</v>
+        <v>927</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>935</v>
+        <v>928</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>936</v>
+        <v>929</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>937</v>
+        <v>930</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16207,19 +16221,19 @@
         <v>428</v>
       </c>
       <c r="B68" s="62" t="s">
-        <v>1262</v>
+        <v>1266</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>939</v>
+        <v>934</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>940</v>
+        <v>935</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>941</v>
+        <v>936</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>942</v>
+        <v>937</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16227,29 +16241,33 @@
         <v>428</v>
       </c>
       <c r="B69" s="62" t="s">
-        <v>1263</v>
+        <v>1267</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>1264</v>
+        <v>939</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>1265</v>
-      </c>
-      <c r="E69" s="11"/>
-      <c r="F69" s="11"/>
+        <v>940</v>
+      </c>
+      <c r="E69" s="11" t="s">
+        <v>941</v>
+      </c>
+      <c r="F69" s="11" t="s">
+        <v>942</v>
+      </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="37" t="s">
         <v>428</v>
       </c>
       <c r="B70" s="62" t="s">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>1267</v>
+        <v>1269</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>1268</v>
+        <v>1270</v>
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -16259,13 +16277,13 @@
         <v>428</v>
       </c>
       <c r="B71" s="62" t="s">
-        <v>1269</v>
+        <v>1271</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>1270</v>
+        <v>1272</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>1271</v>
+        <v>1273</v>
       </c>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
@@ -16274,44 +16292,46 @@
       <c r="A72" s="37" t="s">
         <v>428</v>
       </c>
-      <c r="B72" s="11" t="s">
-        <v>1272</v>
+      <c r="B72" s="62" t="s">
+        <v>1274</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>1273</v>
+        <v>1275</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>1274</v>
+        <v>1276</v>
       </c>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="2" t="s">
-        <v>327</v>
+      <c r="A73" s="37" t="s">
+        <v>428</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>1275</v>
+        <v>1277</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>1276</v>
+        <v>1278</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>1277</v>
-      </c>
+        <v>1279</v>
+      </c>
+      <c r="E73" s="11"/>
+      <c r="F73" s="11"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="2" t="s">
         <v>327</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>1278</v>
+        <v>1280</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>1280</v>
+        <v>1282</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16319,13 +16339,13 @@
         <v>327</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16333,33 +16353,27 @@
         <v>327</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>1286</v>
+        <v>1288</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>1287</v>
-      </c>
-      <c r="C77" s="1" t="s">
-        <v>983</v>
-      </c>
-      <c r="D77" s="1" t="s">
-        <v>984</v>
-      </c>
-      <c r="E77" s="1" t="s">
-        <v>985</v>
-      </c>
-      <c r="F77" s="1" t="s">
-        <v>986</v>
+        <v>327</v>
+      </c>
+      <c r="B77" s="11" t="s">
+        <v>1289</v>
+      </c>
+      <c r="C77" s="11" t="s">
+        <v>1290</v>
+      </c>
+      <c r="D77" s="11" t="s">
+        <v>1291</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16367,39 +16381,39 @@
         <v>107</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1288</v>
+        <v>1292</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>987</v>
+        <v>983</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>988</v>
+        <v>984</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>989</v>
+        <v>985</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>990</v>
+        <v>986</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B79" s="27" t="s">
-        <v>1289</v>
+      <c r="B79" s="1" t="s">
+        <v>1293</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>991</v>
+        <v>987</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>992</v>
+        <v>988</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>993</v>
+        <v>989</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>994</v>
+        <v>990</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16407,19 +16421,19 @@
         <v>107</v>
       </c>
       <c r="B80" s="27" t="s">
-        <v>1290</v>
+        <v>1294</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>995</v>
+        <v>991</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>996</v>
+        <v>992</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>997</v>
+        <v>993</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>998</v>
+        <v>994</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16427,39 +16441,39 @@
         <v>107</v>
       </c>
       <c r="B81" s="27" t="s">
-        <v>1291</v>
+        <v>1295</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>999</v>
+        <v>995</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1000</v>
+        <v>996</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>1001</v>
+        <v>997</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1002</v>
+        <v>998</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="B82" s="2" t="s">
-        <v>1292</v>
-      </c>
-      <c r="C82" s="11" t="s">
-        <v>1293</v>
-      </c>
-      <c r="D82" s="11" t="s">
-        <v>1294</v>
-      </c>
-      <c r="E82" s="11" t="s">
-        <v>1295</v>
-      </c>
-      <c r="F82" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B82" s="27" t="s">
         <v>1296</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>999</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>1000</v>
+      </c>
+      <c r="E82" s="1" t="s">
+        <v>1001</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>1002</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16484,7 +16498,7 @@
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>589</v>
+        <v>275</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>1302</v>
@@ -16495,8 +16509,27 @@
       <c r="D84" s="11" t="s">
         <v>1304</v>
       </c>
-    </row>
-    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="E84" s="11" t="s">
+        <v>1305</v>
+      </c>
+      <c r="F84" s="11" t="s">
+        <v>1306</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="2" t="s">
+        <v>589</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>1307</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>1308</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>1309</v>
+      </c>
+    </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Prepare custom widget to personSchoolType
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -5152,12 +5152,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L36" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="P38" activeCellId="0" sqref="P38"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6537,7 +6537,7 @@
         <v>155</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C27" s="25" t="b">
         <f aca="false">TRUE()</f>
@@ -15076,7 +15076,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J53" activeCellId="0" sqref="J53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Label: Use female and male in English for sex assigned
Fix: #136
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="1313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="1315">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -2479,13 +2479,19 @@
     <t xml:space="preserve">Femme</t>
   </si>
   <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
     <t xml:space="preserve">Woman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homme</t>
   </si>
   <si>
     <t xml:space="preserve">Man</t>
@@ -5152,12 +5158,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C64" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="bottomLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
+      <selection pane="bottomRight" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8548,7 +8554,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="11" t="s">
         <v>380</v>
       </c>
@@ -12865,8 +12871,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13176,7 +13182,7 @@
         <v>770</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -13194,7 +13200,7 @@
         <v>773</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -13209,10 +13215,10 @@
         <v>141</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -13241,10 +13247,10 @@
         <v>710</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -13259,10 +13265,10 @@
         <v>711</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -13291,10 +13297,10 @@
         <v>710</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -13309,10 +13315,10 @@
         <v>711</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -13338,13 +13344,13 @@
         <v>156</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -13358,13 +13364,13 @@
         <v>156</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -13378,13 +13384,13 @@
         <v>156</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -13398,13 +13404,13 @@
         <v>156</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -13416,13 +13422,13 @@
         <v>156</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -13453,17 +13459,17 @@
         <v>695</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="63" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13474,17 +13480,17 @@
         <v>696</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="63" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13495,17 +13501,17 @@
         <v>697</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="63" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13516,17 +13522,17 @@
         <v>698</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="63" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13537,17 +13543,17 @@
         <v>699</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="63" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13555,13 +13561,13 @@
         <v>162</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -13575,13 +13581,13 @@
         <v>162</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -13593,13 +13599,13 @@
         <v>162</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -13614,10 +13620,10 @@
         <v>708</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -13629,13 +13635,13 @@
         <v>162</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -13647,13 +13653,13 @@
         <v>162</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -13686,10 +13692,10 @@
         <v>766</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -13715,13 +13721,13 @@
         <v>198</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -13733,13 +13739,13 @@
         <v>198</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -13768,10 +13774,10 @@
         <v>701</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -13786,10 +13792,10 @@
         <v>702</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -13804,10 +13810,10 @@
         <v>703</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -13819,13 +13825,13 @@
         <v>206</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -13840,10 +13846,10 @@
         <v>707</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -13858,10 +13864,10 @@
         <v>701</v>
       </c>
       <c r="C56" s="63" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="D56" s="63" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13872,10 +13878,10 @@
         <v>702</v>
       </c>
       <c r="C57" s="63" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="D57" s="63" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13886,10 +13892,10 @@
         <v>707</v>
       </c>
       <c r="C58" s="63" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="D58" s="63" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13897,13 +13903,13 @@
         <v>600</v>
       </c>
       <c r="B59" s="63" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="C59" s="63" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="D59" s="63" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13911,13 +13917,13 @@
         <v>600</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
@@ -13927,13 +13933,13 @@
         <v>600</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
@@ -13943,13 +13949,13 @@
         <v>600</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
@@ -13959,13 +13965,13 @@
         <v>600</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
@@ -13975,13 +13981,13 @@
         <v>600</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
@@ -13991,13 +13997,13 @@
         <v>600</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
@@ -14007,13 +14013,13 @@
         <v>600</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
@@ -14023,13 +14029,13 @@
         <v>600</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
@@ -14039,13 +14045,13 @@
         <v>600</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
@@ -14055,13 +14061,13 @@
         <v>600</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
@@ -14071,13 +14077,13 @@
         <v>600</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -14087,13 +14093,13 @@
         <v>600</v>
       </c>
       <c r="B71" s="63" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="C71" s="63" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="D71" s="63" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14115,13 +14121,13 @@
         <v>600</v>
       </c>
       <c r="B73" s="63" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="C73" s="63" t="s">
         <v>767</v>
       </c>
       <c r="D73" s="63" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14129,13 +14135,13 @@
         <v>595</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="C74" s="63" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="D74" s="63" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14143,13 +14149,13 @@
         <v>595</v>
       </c>
       <c r="B75" s="63" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="C75" s="63" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="D75" s="63" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14177,7 +14183,7 @@
         <v>767</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
@@ -14187,13 +14193,13 @@
         <v>320</v>
       </c>
       <c r="B78" s="63" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="C78" s="70" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="D78" s="63" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="H78" s="11" t="s">
         <v>691</v>
@@ -14204,13 +14210,13 @@
         <v>320</v>
       </c>
       <c r="B79" s="63" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="D79" s="70" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="E79" s="70"/>
       <c r="F79" s="70"/>
@@ -14223,13 +14229,13 @@
         <v>320</v>
       </c>
       <c r="B80" s="63" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="D80" s="63" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14237,13 +14243,13 @@
         <v>320</v>
       </c>
       <c r="B81" s="63" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
@@ -14253,13 +14259,13 @@
         <v>320</v>
       </c>
       <c r="B82" s="63" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="E82" s="11"/>
       <c r="F82" s="11"/>
@@ -14269,13 +14275,13 @@
         <v>320</v>
       </c>
       <c r="B83" s="63" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
@@ -14288,13 +14294,13 @@
         <v>320</v>
       </c>
       <c r="B84" s="63" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E84" s="11"/>
       <c r="F84" s="11"/>
@@ -14304,13 +14310,13 @@
         <v>320</v>
       </c>
       <c r="B85" s="63" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="E85" s="11"/>
       <c r="F85" s="11"/>
@@ -14334,7 +14340,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="35" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B87" s="63" t="s">
         <v>27</v>
@@ -14348,16 +14354,16 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="35" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B88" s="63" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="C88" s="63" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="D88" s="63" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="H88" s="63" t="s">
         <v>706</v>
@@ -14365,84 +14371,84 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="35" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B89" s="63" t="s">
         <v>161</v>
       </c>
       <c r="C89" s="63" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="D89" s="63" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="35" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="H90" s="63" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="35" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B91" s="63" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="35" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B92" s="63" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="35" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B93" s="63" t="s">
         <v>755</v>
@@ -14459,13 +14465,13 @@
         <v>524</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14473,13 +14479,13 @@
         <v>524</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14487,13 +14493,13 @@
         <v>524</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14501,13 +14507,13 @@
         <v>524</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14531,13 +14537,13 @@
         <v>539</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14545,13 +14551,13 @@
         <v>539</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14559,13 +14565,13 @@
         <v>539</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14573,13 +14579,13 @@
         <v>539</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14603,13 +14609,13 @@
         <v>175</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="C106" s="63" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="D106" s="63" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14617,13 +14623,13 @@
         <v>175</v>
       </c>
       <c r="B107" s="63" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="C107" s="63" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="D107" s="63" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14631,13 +14637,13 @@
         <v>175</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="C108" s="63" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="D108" s="63" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14645,13 +14651,13 @@
         <v>175</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="C109" s="63" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="D109" s="63" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14659,13 +14665,13 @@
         <v>175</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="C110" s="63" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="D110" s="63" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14673,13 +14679,13 @@
         <v>175</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="C111" s="63" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="D111" s="63" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14692,103 +14698,103 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="26" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>701</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="G113" s="26"/>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="26" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>702</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="26" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>703</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="26" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="26" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>707</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -14831,40 +14837,40 @@
   <sheetData>
     <row r="1" s="68" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="72" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="E1" s="72" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="F1" s="72" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="G1" s="72" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="H1" s="72" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="I1" s="72" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="J1" s="72" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="K1" s="72" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="L1" s="68" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14872,22 +14878,22 @@
         <v>636</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="F2" s="46" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="H2" s="46" t="n">
         <v>-10</v>
@@ -14896,13 +14902,13 @@
         <v>100</v>
       </c>
       <c r="J2" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="K2" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="L2" s="46" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14910,22 +14916,22 @@
         <v>645</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="D3" s="73" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="E3" s="73" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="F3" s="73" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="H3" s="46" t="n">
         <v>-10</v>
@@ -14934,13 +14940,13 @@
         <v>100</v>
       </c>
       <c r="J3" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="K3" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="L3" s="46" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14948,22 +14954,22 @@
         <v>650</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="F4" s="46" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="G4" s="46" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="H4" s="46" t="n">
         <v>-10</v>
@@ -14972,13 +14978,13 @@
         <v>100</v>
       </c>
       <c r="J4" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="K4" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14986,22 +14992,22 @@
         <v>655</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="H5" s="46" t="n">
         <v>-10</v>
@@ -15010,13 +15016,13 @@
         <v>100</v>
       </c>
       <c r="J5" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="K5" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="L5" s="46" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15024,22 +15030,22 @@
         <v>566</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>-1</v>
@@ -15048,13 +15054,13 @@
         <v>10</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -15112,13 +15118,13 @@
         <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -15128,13 +15134,13 @@
         <v>107</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -15144,13 +15150,13 @@
         <v>429</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="E4" s="11"/>
     </row>
@@ -15159,13 +15165,13 @@
         <v>429</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15173,13 +15179,13 @@
         <v>429</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15187,13 +15193,13 @@
         <v>429</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15201,13 +15207,13 @@
         <v>429</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15215,13 +15221,13 @@
         <v>429</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15229,13 +15235,13 @@
         <v>429</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15243,13 +15249,13 @@
         <v>429</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15257,13 +15263,13 @@
         <v>429</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15271,13 +15277,13 @@
         <v>429</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15285,7 +15291,7 @@
         <v>429</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>764</v>
@@ -15299,13 +15305,13 @@
         <v>429</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15313,19 +15319,19 @@
         <v>328</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15333,19 +15339,19 @@
         <v>328</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15353,19 +15359,19 @@
         <v>328</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>1105</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15373,19 +15379,19 @@
         <v>328</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15393,19 +15399,19 @@
         <v>328</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15413,19 +15419,19 @@
         <v>328</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15433,13 +15439,13 @@
         <v>328</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15447,13 +15453,13 @@
         <v>328</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15461,13 +15467,13 @@
         <v>328</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15475,13 +15481,13 @@
         <v>328</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15489,19 +15495,19 @@
         <v>328</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15509,13 +15515,13 @@
         <v>328</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15523,13 +15529,13 @@
         <v>328</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15537,13 +15543,13 @@
         <v>328</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>1145</v>
+        <v>1147</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>1146</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15551,13 +15557,13 @@
         <v>328</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>1149</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15565,13 +15571,13 @@
         <v>328</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>1151</v>
+        <v>1153</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15579,13 +15585,13 @@
         <v>328</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>1155</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15593,13 +15599,13 @@
         <v>328</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>1156</v>
+        <v>1158</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>1158</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15607,13 +15613,13 @@
         <v>328</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>1159</v>
+        <v>1161</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>1160</v>
+        <v>1162</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>1161</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15621,13 +15627,13 @@
         <v>328</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>1162</v>
+        <v>1164</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>1163</v>
+        <v>1165</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>1164</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15635,13 +15641,13 @@
         <v>328</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>1165</v>
+        <v>1167</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>1166</v>
+        <v>1168</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>1167</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15649,13 +15655,13 @@
         <v>328</v>
       </c>
       <c r="B37" s="11" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>1168</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>1166</v>
-      </c>
       <c r="D37" s="11" t="s">
-        <v>1167</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15663,13 +15669,13 @@
         <v>328</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>1169</v>
+        <v>1171</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>1170</v>
+        <v>1172</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>1171</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15677,13 +15683,13 @@
         <v>328</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>1172</v>
+        <v>1174</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>1173</v>
+        <v>1175</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>1174</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15691,13 +15697,13 @@
         <v>328</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>1175</v>
+        <v>1177</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>1177</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15705,13 +15711,13 @@
         <v>328</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>1178</v>
+        <v>1180</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>1180</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15719,13 +15725,13 @@
         <v>328</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>1182</v>
+        <v>1184</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>1183</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15733,13 +15739,13 @@
         <v>328</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>1185</v>
+        <v>1187</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>1186</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15747,13 +15753,13 @@
         <v>328</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>1188</v>
+        <v>1190</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>1189</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15761,13 +15767,13 @@
         <v>328</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>1190</v>
+        <v>1192</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>1192</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15775,13 +15781,13 @@
         <v>328</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>1193</v>
+        <v>1195</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>1194</v>
+        <v>1196</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>1195</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15789,13 +15795,13 @@
         <v>328</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>1196</v>
+        <v>1198</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>1198</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15803,19 +15809,19 @@
         <v>328</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>1199</v>
+        <v>1201</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>1200</v>
+        <v>1202</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>1201</v>
+        <v>1203</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15823,19 +15829,19 @@
         <v>328</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>1204</v>
+        <v>1206</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>1205</v>
+        <v>1207</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>1206</v>
+        <v>1208</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>1207</v>
+        <v>1209</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>1208</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15843,19 +15849,19 @@
         <v>328</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>1209</v>
+        <v>1211</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>1210</v>
+        <v>1212</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>1211</v>
+        <v>1213</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>1213</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15863,19 +15869,19 @@
         <v>328</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>1216</v>
+        <v>1218</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>1217</v>
+        <v>1219</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>1218</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15883,19 +15889,19 @@
         <v>328</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>1219</v>
+        <v>1221</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>1222</v>
+        <v>1224</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15903,19 +15909,19 @@
         <v>328</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>1228</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15923,19 +15929,19 @@
         <v>328</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15943,19 +15949,19 @@
         <v>328</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>1237</v>
+        <v>1239</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15963,13 +15969,13 @@
         <v>107</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>1241</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15977,13 +15983,13 @@
         <v>107</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>1242</v>
+        <v>1244</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15991,13 +15997,13 @@
         <v>107</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>1245</v>
+        <v>1247</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>1247</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16005,13 +16011,13 @@
         <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>1249</v>
+        <v>1251</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>1250</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16019,13 +16025,13 @@
         <v>107</v>
       </c>
       <c r="B60" s="74" t="s">
-        <v>1251</v>
+        <v>1253</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>1252</v>
+        <v>1254</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16033,13 +16039,13 @@
         <v>107</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>1254</v>
+        <v>1256</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>1255</v>
+        <v>1257</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>1256</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16047,13 +16053,13 @@
         <v>107</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>1257</v>
+        <v>1259</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>1258</v>
+        <v>1260</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>1259</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16061,19 +16067,19 @@
         <v>107</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>1260</v>
+        <v>1262</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>1261</v>
+        <v>1263</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>1262</v>
+        <v>1264</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>1263</v>
+        <v>1265</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>1264</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16081,7 +16087,7 @@
         <v>328</v>
       </c>
       <c r="B64" s="63" t="s">
-        <v>1265</v>
+        <v>1267</v>
       </c>
       <c r="C64" s="63" t="s">
         <v>720</v>
@@ -16097,13 +16103,13 @@
         <v>328</v>
       </c>
       <c r="B65" s="63" t="s">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c r="C65" s="63" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="D65" s="63" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="E65" s="63"/>
       <c r="F65" s="63"/>
@@ -16113,13 +16119,13 @@
         <v>328</v>
       </c>
       <c r="B66" s="63" t="s">
-        <v>1267</v>
+        <v>1269</v>
       </c>
       <c r="C66" s="63" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="D66" s="63" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="E66" s="63"/>
       <c r="F66" s="63"/>
@@ -16129,19 +16135,19 @@
         <v>328</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>1268</v>
+        <v>1270</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16149,19 +16155,19 @@
         <v>429</v>
       </c>
       <c r="B68" s="63" t="s">
-        <v>1269</v>
+        <v>1271</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16169,19 +16175,19 @@
         <v>429</v>
       </c>
       <c r="B69" s="63" t="s">
-        <v>1270</v>
+        <v>1272</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16189,13 +16195,13 @@
         <v>429</v>
       </c>
       <c r="B70" s="63" t="s">
-        <v>1271</v>
+        <v>1273</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>1272</v>
+        <v>1274</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>1273</v>
+        <v>1275</v>
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -16205,13 +16211,13 @@
         <v>429</v>
       </c>
       <c r="B71" s="63" t="s">
-        <v>1274</v>
+        <v>1276</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>1275</v>
+        <v>1277</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>1276</v>
+        <v>1278</v>
       </c>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
@@ -16221,13 +16227,13 @@
         <v>429</v>
       </c>
       <c r="B72" s="63" t="s">
-        <v>1277</v>
+        <v>1279</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>1278</v>
+        <v>1280</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
@@ -16237,13 +16243,13 @@
         <v>429</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>1280</v>
+        <v>1282</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="E73" s="11"/>
       <c r="F73" s="11"/>
@@ -16253,13 +16259,13 @@
         <v>328</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16267,13 +16273,13 @@
         <v>328</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>1286</v>
+        <v>1288</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>1287</v>
+        <v>1289</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16281,13 +16287,13 @@
         <v>328</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>1290</v>
+        <v>1292</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>1291</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16295,13 +16301,13 @@
         <v>328</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>1292</v>
+        <v>1294</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>1294</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16309,19 +16315,19 @@
         <v>107</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1295</v>
+        <v>1297</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16329,19 +16335,19 @@
         <v>107</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1296</v>
+        <v>1298</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16349,19 +16355,19 @@
         <v>107</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>1297</v>
+        <v>1299</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16369,19 +16375,19 @@
         <v>107</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>1298</v>
+        <v>1300</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16389,19 +16395,19 @@
         <v>107</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>1299</v>
+        <v>1301</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16409,19 +16415,19 @@
         <v>276</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>1301</v>
+        <v>1303</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>1303</v>
+        <v>1305</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>1304</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16429,19 +16435,19 @@
         <v>276</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>1305</v>
+        <v>1307</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>1307</v>
+        <v>1309</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>1308</v>
+        <v>1310</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>1309</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16449,13 +16455,13 @@
         <v>591</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>1310</v>
+        <v>1312</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>1311</v>
+        <v>1313</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>1312</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Excel: Some important Excel fixes. (#264)
* Prepare custom widget to personSchoolType

* Label: Use female and male in English for sex assigned

Fix: #136
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="1313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2253" uniqueCount="1315">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -2479,13 +2479,19 @@
     <t xml:space="preserve">Femme</t>
   </si>
   <si>
+    <t xml:space="preserve">Female</t>
+  </si>
+  <si>
+    <t xml:space="preserve">male</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Homme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Male</t>
+  </si>
+  <si>
     <t xml:space="preserve">Woman</t>
-  </si>
-  <si>
-    <t xml:space="preserve">male</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Homme</t>
   </si>
   <si>
     <t xml:space="preserve">Man</t>
@@ -5153,11 +5159,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="L36" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C64" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="L1" activeCellId="0" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="A36" activeCellId="0" sqref="A36"/>
-      <selection pane="bottomRight" activeCell="P38" activeCellId="0" sqref="P38"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A64" activeCellId="0" sqref="A64"/>
+      <selection pane="bottomRight" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6537,7 +6543,7 @@
         <v>155</v>
       </c>
       <c r="B27" s="23" t="s">
-        <v>33</v>
+        <v>72</v>
       </c>
       <c r="C27" s="25" t="b">
         <f aca="false">TRUE()</f>
@@ -8548,7 +8554,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="69" customFormat="false" ht="39.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="69" customFormat="false" ht="150.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="11" t="s">
         <v>380</v>
       </c>
@@ -12865,8 +12871,8 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13176,7 +13182,7 @@
         <v>770</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>771</v>
+        <v>775</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
@@ -13194,7 +13200,7 @@
         <v>773</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>774</v>
+        <v>776</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
@@ -13209,10 +13215,10 @@
         <v>141</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>775</v>
+        <v>777</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>776</v>
+        <v>778</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
@@ -13241,10 +13247,10 @@
         <v>710</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>777</v>
+        <v>779</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>778</v>
+        <v>780</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
@@ -13259,10 +13265,10 @@
         <v>711</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>779</v>
+        <v>781</v>
       </c>
       <c r="D23" s="1" t="s">
-        <v>780</v>
+        <v>782</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
@@ -13291,10 +13297,10 @@
         <v>710</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>781</v>
+        <v>783</v>
       </c>
       <c r="D25" s="1" t="s">
-        <v>782</v>
+        <v>784</v>
       </c>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
@@ -13309,10 +13315,10 @@
         <v>711</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
@@ -13338,13 +13344,13 @@
         <v>156</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>785</v>
+        <v>787</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>786</v>
+        <v>788</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>787</v>
+        <v>789</v>
       </c>
       <c r="E28" s="1"/>
       <c r="F28" s="1"/>
@@ -13358,13 +13364,13 @@
         <v>156</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>788</v>
+        <v>790</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>789</v>
+        <v>791</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>790</v>
+        <v>792</v>
       </c>
       <c r="E29" s="1"/>
       <c r="F29" s="1"/>
@@ -13378,13 +13384,13 @@
         <v>156</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>791</v>
+        <v>793</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>792</v>
+        <v>794</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>793</v>
+        <v>795</v>
       </c>
       <c r="E30" s="1"/>
       <c r="F30" s="1"/>
@@ -13398,13 +13404,13 @@
         <v>156</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>794</v>
+        <v>796</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>795</v>
+        <v>797</v>
       </c>
       <c r="D31" s="1" t="s">
-        <v>796</v>
+        <v>798</v>
       </c>
       <c r="E31" s="1"/>
       <c r="F31" s="1"/>
@@ -13416,13 +13422,13 @@
         <v>156</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>797</v>
+        <v>799</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>798</v>
+        <v>800</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>799</v>
+        <v>801</v>
       </c>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
@@ -13453,17 +13459,17 @@
         <v>695</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>800</v>
+        <v>802</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>801</v>
+        <v>803</v>
       </c>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="63" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13474,17 +13480,17 @@
         <v>696</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>803</v>
+        <v>805</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>804</v>
+        <v>806</v>
       </c>
       <c r="E35" s="1"/>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="63" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13495,17 +13501,17 @@
         <v>697</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>805</v>
+        <v>807</v>
       </c>
       <c r="D36" s="1" t="s">
-        <v>806</v>
+        <v>808</v>
       </c>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
       <c r="I36" s="63" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13516,17 +13522,17 @@
         <v>698</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>807</v>
+        <v>809</v>
       </c>
       <c r="D37" s="1" t="s">
-        <v>808</v>
+        <v>810</v>
       </c>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
       <c r="I37" s="63" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13537,17 +13543,17 @@
         <v>699</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>809</v>
+        <v>811</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>810</v>
+        <v>812</v>
       </c>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
       <c r="I38" s="63" t="s">
-        <v>802</v>
+        <v>804</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13555,13 +13561,13 @@
         <v>162</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>811</v>
+        <v>813</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>812</v>
+        <v>814</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>813</v>
+        <v>815</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
@@ -13575,13 +13581,13 @@
         <v>162</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>814</v>
+        <v>816</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>816</v>
+        <v>818</v>
       </c>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
@@ -13593,13 +13599,13 @@
         <v>162</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>817</v>
+        <v>819</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>818</v>
+        <v>820</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>819</v>
+        <v>821</v>
       </c>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
@@ -13614,10 +13620,10 @@
         <v>708</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>820</v>
+        <v>822</v>
       </c>
       <c r="D42" s="1" t="s">
-        <v>821</v>
+        <v>823</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
@@ -13629,13 +13635,13 @@
         <v>162</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>822</v>
+        <v>824</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>823</v>
+        <v>825</v>
       </c>
       <c r="D43" s="1" t="s">
-        <v>824</v>
+        <v>826</v>
       </c>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
@@ -13647,13 +13653,13 @@
         <v>162</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>825</v>
+        <v>827</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>826</v>
+        <v>828</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>827</v>
+        <v>829</v>
       </c>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
@@ -13686,10 +13692,10 @@
         <v>766</v>
       </c>
       <c r="C46" s="1" t="s">
-        <v>828</v>
+        <v>830</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>829</v>
+        <v>831</v>
       </c>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
@@ -13715,13 +13721,13 @@
         <v>198</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>830</v>
+        <v>832</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>831</v>
+        <v>833</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>832</v>
+        <v>834</v>
       </c>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
@@ -13733,13 +13739,13 @@
         <v>198</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>833</v>
+        <v>835</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>834</v>
+        <v>836</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>835</v>
+        <v>837</v>
       </c>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
@@ -13768,10 +13774,10 @@
         <v>701</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>836</v>
+        <v>838</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
@@ -13786,10 +13792,10 @@
         <v>702</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>838</v>
+        <v>840</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>839</v>
+        <v>841</v>
       </c>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
@@ -13804,10 +13810,10 @@
         <v>703</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>840</v>
+        <v>842</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>841</v>
+        <v>843</v>
       </c>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -13819,13 +13825,13 @@
         <v>206</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>843</v>
+        <v>845</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>844</v>
+        <v>846</v>
       </c>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
@@ -13840,10 +13846,10 @@
         <v>707</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>845</v>
+        <v>847</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>846</v>
+        <v>848</v>
       </c>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
@@ -13858,10 +13864,10 @@
         <v>701</v>
       </c>
       <c r="C56" s="63" t="s">
-        <v>847</v>
+        <v>849</v>
       </c>
       <c r="D56" s="63" t="s">
-        <v>837</v>
+        <v>839</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13872,10 +13878,10 @@
         <v>702</v>
       </c>
       <c r="C57" s="63" t="s">
-        <v>848</v>
+        <v>850</v>
       </c>
       <c r="D57" s="63" t="s">
-        <v>849</v>
+        <v>851</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13886,10 +13892,10 @@
         <v>707</v>
       </c>
       <c r="C58" s="63" t="s">
-        <v>850</v>
+        <v>852</v>
       </c>
       <c r="D58" s="63" t="s">
-        <v>851</v>
+        <v>853</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13897,13 +13903,13 @@
         <v>600</v>
       </c>
       <c r="B59" s="63" t="s">
-        <v>852</v>
+        <v>854</v>
       </c>
       <c r="C59" s="63" t="s">
-        <v>853</v>
+        <v>855</v>
       </c>
       <c r="D59" s="63" t="s">
-        <v>854</v>
+        <v>856</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13911,13 +13917,13 @@
         <v>600</v>
       </c>
       <c r="B60" s="11" t="s">
-        <v>855</v>
+        <v>857</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>856</v>
+        <v>858</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>857</v>
+        <v>859</v>
       </c>
       <c r="E60" s="11"/>
       <c r="F60" s="11"/>
@@ -13927,13 +13933,13 @@
         <v>600</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>858</v>
+        <v>860</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>859</v>
+        <v>861</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>860</v>
+        <v>862</v>
       </c>
       <c r="E61" s="11"/>
       <c r="F61" s="11"/>
@@ -13943,13 +13949,13 @@
         <v>600</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>861</v>
+        <v>863</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>862</v>
+        <v>864</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>863</v>
+        <v>865</v>
       </c>
       <c r="E62" s="11"/>
       <c r="F62" s="11"/>
@@ -13959,13 +13965,13 @@
         <v>600</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>864</v>
+        <v>866</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>865</v>
+        <v>867</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>866</v>
+        <v>868</v>
       </c>
       <c r="E63" s="11"/>
       <c r="F63" s="11"/>
@@ -13975,13 +13981,13 @@
         <v>600</v>
       </c>
       <c r="B64" s="11" t="s">
-        <v>867</v>
+        <v>869</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>868</v>
+        <v>870</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>869</v>
+        <v>871</v>
       </c>
       <c r="E64" s="11"/>
       <c r="F64" s="11"/>
@@ -13991,13 +13997,13 @@
         <v>600</v>
       </c>
       <c r="B65" s="11" t="s">
-        <v>870</v>
+        <v>872</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>871</v>
+        <v>873</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>872</v>
+        <v>874</v>
       </c>
       <c r="E65" s="11"/>
       <c r="F65" s="11"/>
@@ -14007,13 +14013,13 @@
         <v>600</v>
       </c>
       <c r="B66" s="11" t="s">
-        <v>873</v>
+        <v>875</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>874</v>
+        <v>876</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>875</v>
+        <v>877</v>
       </c>
       <c r="E66" s="11"/>
       <c r="F66" s="11"/>
@@ -14023,13 +14029,13 @@
         <v>600</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>876</v>
+        <v>878</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>877</v>
+        <v>879</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>878</v>
+        <v>880</v>
       </c>
       <c r="E67" s="11"/>
       <c r="F67" s="11"/>
@@ -14039,13 +14045,13 @@
         <v>600</v>
       </c>
       <c r="B68" s="11" t="s">
-        <v>879</v>
+        <v>881</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>880</v>
+        <v>882</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>881</v>
+        <v>883</v>
       </c>
       <c r="E68" s="11"/>
       <c r="F68" s="11"/>
@@ -14055,13 +14061,13 @@
         <v>600</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>882</v>
+        <v>884</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>883</v>
+        <v>885</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>884</v>
+        <v>886</v>
       </c>
       <c r="E69" s="11"/>
       <c r="F69" s="11"/>
@@ -14071,13 +14077,13 @@
         <v>600</v>
       </c>
       <c r="B70" s="11" t="s">
-        <v>885</v>
+        <v>887</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>886</v>
+        <v>888</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>887</v>
+        <v>889</v>
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -14087,13 +14093,13 @@
         <v>600</v>
       </c>
       <c r="B71" s="63" t="s">
-        <v>888</v>
+        <v>890</v>
       </c>
       <c r="C71" s="63" t="s">
-        <v>889</v>
+        <v>891</v>
       </c>
       <c r="D71" s="63" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14115,13 +14121,13 @@
         <v>600</v>
       </c>
       <c r="B73" s="63" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="C73" s="63" t="s">
         <v>767</v>
       </c>
       <c r="D73" s="63" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14129,13 +14135,13 @@
         <v>595</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="C74" s="63" t="s">
-        <v>894</v>
+        <v>896</v>
       </c>
       <c r="D74" s="63" t="s">
-        <v>895</v>
+        <v>897</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14143,13 +14149,13 @@
         <v>595</v>
       </c>
       <c r="B75" s="63" t="s">
-        <v>896</v>
+        <v>898</v>
       </c>
       <c r="C75" s="63" t="s">
-        <v>897</v>
+        <v>899</v>
       </c>
       <c r="D75" s="63" t="s">
-        <v>898</v>
+        <v>900</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14177,7 +14183,7 @@
         <v>767</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="E77" s="11"/>
       <c r="F77" s="11"/>
@@ -14187,13 +14193,13 @@
         <v>320</v>
       </c>
       <c r="B78" s="63" t="s">
-        <v>899</v>
+        <v>901</v>
       </c>
       <c r="C78" s="70" t="s">
-        <v>900</v>
+        <v>902</v>
       </c>
       <c r="D78" s="63" t="s">
-        <v>901</v>
+        <v>903</v>
       </c>
       <c r="H78" s="11" t="s">
         <v>691</v>
@@ -14204,13 +14210,13 @@
         <v>320</v>
       </c>
       <c r="B79" s="63" t="s">
-        <v>902</v>
+        <v>904</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>903</v>
+        <v>905</v>
       </c>
       <c r="D79" s="70" t="s">
-        <v>904</v>
+        <v>906</v>
       </c>
       <c r="E79" s="70"/>
       <c r="F79" s="70"/>
@@ -14223,13 +14229,13 @@
         <v>320</v>
       </c>
       <c r="B80" s="63" t="s">
-        <v>905</v>
+        <v>907</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>906</v>
+        <v>908</v>
       </c>
       <c r="D80" s="63" t="s">
-        <v>907</v>
+        <v>909</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14237,13 +14243,13 @@
         <v>320</v>
       </c>
       <c r="B81" s="63" t="s">
-        <v>908</v>
+        <v>910</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>909</v>
+        <v>911</v>
       </c>
       <c r="D81" s="11" t="s">
-        <v>910</v>
+        <v>912</v>
       </c>
       <c r="E81" s="11"/>
       <c r="F81" s="11"/>
@@ -14253,13 +14259,13 @@
         <v>320</v>
       </c>
       <c r="B82" s="63" t="s">
-        <v>911</v>
+        <v>913</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>912</v>
+        <v>914</v>
       </c>
       <c r="D82" s="11" t="s">
-        <v>913</v>
+        <v>915</v>
       </c>
       <c r="E82" s="11"/>
       <c r="F82" s="11"/>
@@ -14269,13 +14275,13 @@
         <v>320</v>
       </c>
       <c r="B83" s="63" t="s">
-        <v>914</v>
+        <v>916</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>915</v>
+        <v>917</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>916</v>
+        <v>918</v>
       </c>
       <c r="E83" s="11"/>
       <c r="F83" s="11"/>
@@ -14288,13 +14294,13 @@
         <v>320</v>
       </c>
       <c r="B84" s="63" t="s">
-        <v>917</v>
+        <v>919</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>918</v>
+        <v>920</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>919</v>
+        <v>921</v>
       </c>
       <c r="E84" s="11"/>
       <c r="F84" s="11"/>
@@ -14304,13 +14310,13 @@
         <v>320</v>
       </c>
       <c r="B85" s="63" t="s">
-        <v>920</v>
+        <v>922</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>921</v>
+        <v>923</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>922</v>
+        <v>924</v>
       </c>
       <c r="E85" s="11"/>
       <c r="F85" s="11"/>
@@ -14334,7 +14340,7 @@
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="35" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B87" s="63" t="s">
         <v>27</v>
@@ -14348,16 +14354,16 @@
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="35" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B88" s="63" t="s">
-        <v>924</v>
+        <v>926</v>
       </c>
       <c r="C88" s="63" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="D88" s="63" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="H88" s="63" t="s">
         <v>706</v>
@@ -14365,84 +14371,84 @@
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="35" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B89" s="63" t="s">
         <v>161</v>
       </c>
       <c r="C89" s="63" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="D89" s="63" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="35" t="s">
-        <v>923</v>
+        <v>925</v>
       </c>
       <c r="B90" s="11" t="s">
-        <v>929</v>
+        <v>931</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="D90" s="11" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E90" s="11" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="F90" s="11" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
       <c r="H90" s="63" t="s">
-        <v>934</v>
+        <v>936</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="35" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B91" s="63" t="s">
-        <v>936</v>
+        <v>938</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="D91" s="11" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="E91" s="11" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="F91" s="11" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A92" s="35" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B92" s="63" t="s">
-        <v>941</v>
+        <v>943</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="D92" s="11" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="E92" s="11" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="F92" s="11" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A93" s="35" t="s">
-        <v>935</v>
+        <v>937</v>
       </c>
       <c r="B93" s="63" t="s">
         <v>755</v>
@@ -14459,13 +14465,13 @@
         <v>524</v>
       </c>
       <c r="B94" s="11" t="s">
-        <v>946</v>
+        <v>948</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>947</v>
+        <v>949</v>
       </c>
       <c r="D94" s="11" t="s">
-        <v>948</v>
+        <v>950</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14473,13 +14479,13 @@
         <v>524</v>
       </c>
       <c r="B95" s="11" t="s">
-        <v>949</v>
+        <v>951</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>950</v>
+        <v>952</v>
       </c>
       <c r="D95" s="11" t="s">
-        <v>951</v>
+        <v>953</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14487,13 +14493,13 @@
         <v>524</v>
       </c>
       <c r="B96" s="11" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="D96" s="11" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14501,13 +14507,13 @@
         <v>524</v>
       </c>
       <c r="B97" s="11" t="s">
-        <v>955</v>
+        <v>957</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>956</v>
+        <v>958</v>
       </c>
       <c r="D97" s="11" t="s">
-        <v>957</v>
+        <v>959</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14531,13 +14537,13 @@
         <v>539</v>
       </c>
       <c r="B100" s="11" t="s">
-        <v>958</v>
+        <v>960</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>959</v>
+        <v>961</v>
       </c>
       <c r="D100" s="11" t="s">
-        <v>960</v>
+        <v>962</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14545,13 +14551,13 @@
         <v>539</v>
       </c>
       <c r="B101" s="11" t="s">
-        <v>961</v>
+        <v>963</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>962</v>
+        <v>964</v>
       </c>
       <c r="D101" s="11" t="s">
-        <v>963</v>
+        <v>965</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14559,13 +14565,13 @@
         <v>539</v>
       </c>
       <c r="B102" s="11" t="s">
-        <v>952</v>
+        <v>954</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>953</v>
+        <v>955</v>
       </c>
       <c r="D102" s="11" t="s">
-        <v>954</v>
+        <v>956</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14573,13 +14579,13 @@
         <v>539</v>
       </c>
       <c r="B103" s="11" t="s">
-        <v>964</v>
+        <v>966</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>965</v>
+        <v>967</v>
       </c>
       <c r="D103" s="11" t="s">
-        <v>966</v>
+        <v>968</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14603,13 +14609,13 @@
         <v>175</v>
       </c>
       <c r="B106" s="11" t="s">
-        <v>967</v>
+        <v>969</v>
       </c>
       <c r="C106" s="63" t="s">
-        <v>968</v>
+        <v>970</v>
       </c>
       <c r="D106" s="63" t="s">
-        <v>969</v>
+        <v>971</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14617,13 +14623,13 @@
         <v>175</v>
       </c>
       <c r="B107" s="63" t="s">
-        <v>970</v>
+        <v>972</v>
       </c>
       <c r="C107" s="63" t="s">
-        <v>971</v>
+        <v>973</v>
       </c>
       <c r="D107" s="63" t="s">
-        <v>972</v>
+        <v>974</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14631,13 +14637,13 @@
         <v>175</v>
       </c>
       <c r="B108" s="11" t="s">
-        <v>973</v>
+        <v>975</v>
       </c>
       <c r="C108" s="63" t="s">
-        <v>974</v>
+        <v>976</v>
       </c>
       <c r="D108" s="63" t="s">
-        <v>975</v>
+        <v>977</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14645,13 +14651,13 @@
         <v>175</v>
       </c>
       <c r="B109" s="11" t="s">
-        <v>976</v>
+        <v>978</v>
       </c>
       <c r="C109" s="63" t="s">
-        <v>977</v>
+        <v>979</v>
       </c>
       <c r="D109" s="63" t="s">
-        <v>978</v>
+        <v>980</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14659,13 +14665,13 @@
         <v>175</v>
       </c>
       <c r="B110" s="11" t="s">
-        <v>979</v>
+        <v>981</v>
       </c>
       <c r="C110" s="63" t="s">
-        <v>980</v>
+        <v>982</v>
       </c>
       <c r="D110" s="63" t="s">
-        <v>981</v>
+        <v>983</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14673,13 +14679,13 @@
         <v>175</v>
       </c>
       <c r="B111" s="11" t="s">
-        <v>982</v>
+        <v>984</v>
       </c>
       <c r="C111" s="63" t="s">
-        <v>983</v>
+        <v>985</v>
       </c>
       <c r="D111" s="63" t="s">
-        <v>984</v>
+        <v>986</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14692,103 +14698,103 @@
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A113" s="26" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>701</v>
       </c>
       <c r="C113" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="D113" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E113" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="F113" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
       <c r="G113" s="26"/>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A114" s="26" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>702</v>
       </c>
       <c r="C114" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="D114" s="1" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="E114" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="F114" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A115" s="26" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>703</v>
       </c>
       <c r="C115" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="D115" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E115" s="1" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="F115" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A116" s="26" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B116" s="1" t="s">
-        <v>842</v>
+        <v>844</v>
       </c>
       <c r="C116" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="D116" s="1" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="E116" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="F116" s="1" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A117" s="26" t="s">
-        <v>985</v>
+        <v>987</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>707</v>
       </c>
       <c r="C117" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="E117" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="F117" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -14831,40 +14837,40 @@
   <sheetData>
     <row r="1" s="68" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="72" t="s">
-        <v>1006</v>
+        <v>1008</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>1007</v>
+        <v>1009</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>1008</v>
+        <v>1010</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>1009</v>
+        <v>1011</v>
       </c>
       <c r="E1" s="72" t="s">
-        <v>1010</v>
+        <v>1012</v>
       </c>
       <c r="F1" s="72" t="s">
-        <v>1011</v>
+        <v>1013</v>
       </c>
       <c r="G1" s="72" t="s">
-        <v>1012</v>
+        <v>1014</v>
       </c>
       <c r="H1" s="72" t="s">
-        <v>1013</v>
+        <v>1015</v>
       </c>
       <c r="I1" s="72" t="s">
-        <v>1014</v>
+        <v>1016</v>
       </c>
       <c r="J1" s="72" t="s">
-        <v>1015</v>
+        <v>1017</v>
       </c>
       <c r="K1" s="72" t="s">
-        <v>1016</v>
+        <v>1018</v>
       </c>
       <c r="L1" s="68" t="s">
-        <v>1017</v>
+        <v>1019</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14872,22 +14878,22 @@
         <v>636</v>
       </c>
       <c r="B2" s="46" t="s">
-        <v>1018</v>
+        <v>1020</v>
       </c>
       <c r="C2" s="46" t="s">
-        <v>1019</v>
+        <v>1021</v>
       </c>
       <c r="D2" s="46" t="s">
-        <v>1020</v>
+        <v>1022</v>
       </c>
       <c r="E2" s="46" t="s">
-        <v>1021</v>
+        <v>1023</v>
       </c>
       <c r="F2" s="46" t="s">
-        <v>1022</v>
+        <v>1024</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>1023</v>
+        <v>1025</v>
       </c>
       <c r="H2" s="46" t="n">
         <v>-10</v>
@@ -14896,13 +14902,13 @@
         <v>100</v>
       </c>
       <c r="J2" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="K2" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="L2" s="46" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14910,22 +14916,22 @@
         <v>645</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>1027</v>
+        <v>1029</v>
       </c>
       <c r="D3" s="73" t="s">
-        <v>1028</v>
+        <v>1030</v>
       </c>
       <c r="E3" s="73" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="F3" s="73" t="s">
-        <v>1030</v>
+        <v>1032</v>
       </c>
       <c r="G3" s="46" t="s">
-        <v>1031</v>
+        <v>1033</v>
       </c>
       <c r="H3" s="46" t="n">
         <v>-10</v>
@@ -14934,13 +14940,13 @@
         <v>100</v>
       </c>
       <c r="J3" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="K3" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="L3" s="46" t="s">
-        <v>1032</v>
+        <v>1034</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14948,22 +14954,22 @@
         <v>650</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>1033</v>
+        <v>1035</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>1034</v>
+        <v>1036</v>
       </c>
       <c r="D4" s="46" t="s">
-        <v>1035</v>
+        <v>1037</v>
       </c>
       <c r="E4" s="46" t="s">
-        <v>1036</v>
+        <v>1038</v>
       </c>
       <c r="F4" s="46" t="s">
-        <v>1037</v>
+        <v>1039</v>
       </c>
       <c r="G4" s="46" t="s">
-        <v>1038</v>
+        <v>1040</v>
       </c>
       <c r="H4" s="46" t="n">
         <v>-10</v>
@@ -14972,13 +14978,13 @@
         <v>100</v>
       </c>
       <c r="J4" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="K4" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="L4" s="46" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14986,22 +14992,22 @@
         <v>655</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>1026</v>
+        <v>1028</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>1040</v>
+        <v>1042</v>
       </c>
       <c r="D5" s="46" t="s">
-        <v>1041</v>
+        <v>1043</v>
       </c>
       <c r="E5" s="46" t="s">
-        <v>1029</v>
+        <v>1031</v>
       </c>
       <c r="F5" s="46" t="s">
-        <v>1042</v>
+        <v>1044</v>
       </c>
       <c r="G5" s="46" t="s">
-        <v>1043</v>
+        <v>1045</v>
       </c>
       <c r="H5" s="46" t="n">
         <v>-10</v>
@@ -15010,13 +15016,13 @@
         <v>100</v>
       </c>
       <c r="J5" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="K5" s="46" t="s">
-        <v>1024</v>
+        <v>1026</v>
       </c>
       <c r="L5" s="46" t="s">
-        <v>1039</v>
+        <v>1041</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15024,22 +15030,22 @@
         <v>566</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1044</v>
+        <v>1046</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>1045</v>
+        <v>1047</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>1046</v>
+        <v>1048</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>1047</v>
+        <v>1049</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>1048</v>
+        <v>1050</v>
       </c>
       <c r="G6" s="2" t="s">
-        <v>1049</v>
+        <v>1051</v>
       </c>
       <c r="H6" s="2" t="n">
         <v>-1</v>
@@ -15048,13 +15054,13 @@
         <v>10</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>1050</v>
+        <v>1052</v>
       </c>
       <c r="L6" s="2" t="s">
-        <v>1025</v>
+        <v>1027</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -15076,7 +15082,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J53" activeCellId="0" sqref="J53"/>
     </sheetView>
   </sheetViews>
@@ -15112,13 +15118,13 @@
         <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>1051</v>
+        <v>1053</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>1052</v>
+        <v>1054</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>1053</v>
+        <v>1055</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -15128,13 +15134,13 @@
         <v>107</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>1054</v>
+        <v>1056</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>1055</v>
+        <v>1057</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>1056</v>
+        <v>1058</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -15144,13 +15150,13 @@
         <v>429</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>1057</v>
+        <v>1059</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>1058</v>
+        <v>1060</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>1059</v>
+        <v>1061</v>
       </c>
       <c r="E4" s="11"/>
     </row>
@@ -15159,13 +15165,13 @@
         <v>429</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>1060</v>
+        <v>1062</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>1061</v>
+        <v>1063</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>1062</v>
+        <v>1064</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15173,13 +15179,13 @@
         <v>429</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>1063</v>
+        <v>1065</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>1064</v>
+        <v>1066</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>1065</v>
+        <v>1067</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15187,13 +15193,13 @@
         <v>429</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>1066</v>
+        <v>1068</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>1067</v>
+        <v>1069</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>1068</v>
+        <v>1070</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15201,13 +15207,13 @@
         <v>429</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>1069</v>
+        <v>1071</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>1070</v>
+        <v>1072</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>1071</v>
+        <v>1073</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15215,13 +15221,13 @@
         <v>429</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>1072</v>
+        <v>1074</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>1073</v>
+        <v>1075</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>1074</v>
+        <v>1076</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15229,13 +15235,13 @@
         <v>429</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>1075</v>
+        <v>1077</v>
       </c>
       <c r="C10" s="11" t="s">
-        <v>1076</v>
+        <v>1078</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>1077</v>
+        <v>1079</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15243,13 +15249,13 @@
         <v>429</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>1078</v>
+        <v>1080</v>
       </c>
       <c r="C11" s="11" t="s">
-        <v>1079</v>
+        <v>1081</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>1080</v>
+        <v>1082</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15257,13 +15263,13 @@
         <v>429</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>1081</v>
+        <v>1083</v>
       </c>
       <c r="C12" s="11" t="s">
-        <v>1082</v>
+        <v>1084</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>1083</v>
+        <v>1085</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15271,13 +15277,13 @@
         <v>429</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>1084</v>
+        <v>1086</v>
       </c>
       <c r="C13" s="11" t="s">
-        <v>1085</v>
+        <v>1087</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>1086</v>
+        <v>1088</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15285,7 +15291,7 @@
         <v>429</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1087</v>
+        <v>1089</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>764</v>
@@ -15299,13 +15305,13 @@
         <v>429</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>1088</v>
+        <v>1090</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>1089</v>
+        <v>1091</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>1090</v>
+        <v>1092</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15313,19 +15319,19 @@
         <v>328</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>1091</v>
+        <v>1093</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>1092</v>
+        <v>1094</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>1093</v>
+        <v>1095</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>1094</v>
+        <v>1096</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>1095</v>
+        <v>1097</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15333,19 +15339,19 @@
         <v>328</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>1096</v>
+        <v>1098</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>1097</v>
+        <v>1099</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>1098</v>
+        <v>1100</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>1099</v>
+        <v>1101</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>1100</v>
+        <v>1102</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15353,19 +15359,19 @@
         <v>328</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>1101</v>
+        <v>1103</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>1102</v>
+        <v>1104</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>1103</v>
+        <v>1105</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>1104</v>
+        <v>1106</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>1105</v>
+        <v>1107</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15373,19 +15379,19 @@
         <v>328</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>1106</v>
+        <v>1108</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>1107</v>
+        <v>1109</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>1108</v>
+        <v>1110</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>1109</v>
+        <v>1111</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>1110</v>
+        <v>1112</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15393,19 +15399,19 @@
         <v>328</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>1111</v>
+        <v>1113</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>1112</v>
+        <v>1114</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>1113</v>
+        <v>1115</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>1114</v>
+        <v>1116</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>1115</v>
+        <v>1117</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15413,19 +15419,19 @@
         <v>328</v>
       </c>
       <c r="B21" s="11" t="s">
-        <v>1116</v>
+        <v>1118</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>1117</v>
+        <v>1119</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>1118</v>
+        <v>1120</v>
       </c>
       <c r="E21" s="11" t="s">
-        <v>1119</v>
+        <v>1121</v>
       </c>
       <c r="F21" s="11" t="s">
-        <v>1120</v>
+        <v>1122</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15433,13 +15439,13 @@
         <v>328</v>
       </c>
       <c r="B22" s="11" t="s">
-        <v>1121</v>
+        <v>1123</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>1122</v>
+        <v>1124</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>1123</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15447,13 +15453,13 @@
         <v>328</v>
       </c>
       <c r="B23" s="11" t="s">
-        <v>1124</v>
+        <v>1126</v>
       </c>
       <c r="C23" s="11" t="s">
-        <v>1125</v>
+        <v>1127</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>1126</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15461,13 +15467,13 @@
         <v>328</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>1127</v>
+        <v>1129</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>1128</v>
+        <v>1130</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>1129</v>
+        <v>1131</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15475,13 +15481,13 @@
         <v>328</v>
       </c>
       <c r="B25" s="11" t="s">
-        <v>1130</v>
+        <v>1132</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>1131</v>
+        <v>1133</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>1132</v>
+        <v>1134</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15489,19 +15495,19 @@
         <v>328</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>1133</v>
+        <v>1135</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>1134</v>
+        <v>1136</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>1135</v>
+        <v>1137</v>
       </c>
       <c r="E26" s="11" t="s">
-        <v>1136</v>
+        <v>1138</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>1137</v>
+        <v>1139</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15509,13 +15515,13 @@
         <v>328</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>1138</v>
+        <v>1140</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>1139</v>
+        <v>1141</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>1140</v>
+        <v>1142</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15523,13 +15529,13 @@
         <v>328</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>1141</v>
+        <v>1143</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>1142</v>
+        <v>1144</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>1143</v>
+        <v>1145</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15537,13 +15543,13 @@
         <v>328</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>1144</v>
+        <v>1146</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>1145</v>
+        <v>1147</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>1146</v>
+        <v>1148</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15551,13 +15557,13 @@
         <v>328</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>1147</v>
+        <v>1149</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>1148</v>
+        <v>1150</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>1149</v>
+        <v>1151</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15565,13 +15571,13 @@
         <v>328</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>1150</v>
+        <v>1152</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>1151</v>
+        <v>1153</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>1152</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15579,13 +15585,13 @@
         <v>328</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>1153</v>
+        <v>1155</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>1154</v>
+        <v>1156</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>1155</v>
+        <v>1157</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15593,13 +15599,13 @@
         <v>328</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>1156</v>
+        <v>1158</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>1157</v>
+        <v>1159</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>1158</v>
+        <v>1160</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15607,13 +15613,13 @@
         <v>328</v>
       </c>
       <c r="B34" s="11" t="s">
-        <v>1159</v>
+        <v>1161</v>
       </c>
       <c r="C34" s="11" t="s">
-        <v>1160</v>
+        <v>1162</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>1161</v>
+        <v>1163</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15621,13 +15627,13 @@
         <v>328</v>
       </c>
       <c r="B35" s="11" t="s">
-        <v>1162</v>
+        <v>1164</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>1163</v>
+        <v>1165</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>1164</v>
+        <v>1166</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15635,13 +15641,13 @@
         <v>328</v>
       </c>
       <c r="B36" s="11" t="s">
-        <v>1165</v>
+        <v>1167</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>1166</v>
+        <v>1168</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>1167</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15649,13 +15655,13 @@
         <v>328</v>
       </c>
       <c r="B37" s="11" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C37" s="11" t="s">
         <v>1168</v>
       </c>
-      <c r="C37" s="11" t="s">
-        <v>1166</v>
-      </c>
       <c r="D37" s="11" t="s">
-        <v>1167</v>
+        <v>1169</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15663,13 +15669,13 @@
         <v>328</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>1169</v>
+        <v>1171</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>1170</v>
+        <v>1172</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>1171</v>
+        <v>1173</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15677,13 +15683,13 @@
         <v>328</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>1172</v>
+        <v>1174</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>1173</v>
+        <v>1175</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>1174</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15691,13 +15697,13 @@
         <v>328</v>
       </c>
       <c r="B40" s="11" t="s">
-        <v>1175</v>
+        <v>1177</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>1176</v>
+        <v>1178</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>1177</v>
+        <v>1179</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15705,13 +15711,13 @@
         <v>328</v>
       </c>
       <c r="B41" s="11" t="s">
-        <v>1178</v>
+        <v>1180</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>1179</v>
+        <v>1181</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>1180</v>
+        <v>1182</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15719,13 +15725,13 @@
         <v>328</v>
       </c>
       <c r="B42" s="11" t="s">
-        <v>1181</v>
+        <v>1183</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>1182</v>
+        <v>1184</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>1183</v>
+        <v>1185</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15733,13 +15739,13 @@
         <v>328</v>
       </c>
       <c r="B43" s="11" t="s">
-        <v>1184</v>
+        <v>1186</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>1185</v>
+        <v>1187</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>1186</v>
+        <v>1188</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15747,13 +15753,13 @@
         <v>328</v>
       </c>
       <c r="B44" s="11" t="s">
-        <v>1187</v>
+        <v>1189</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>1188</v>
+        <v>1190</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>1189</v>
+        <v>1191</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15761,13 +15767,13 @@
         <v>328</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>1190</v>
+        <v>1192</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>1191</v>
+        <v>1193</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>1192</v>
+        <v>1194</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15775,13 +15781,13 @@
         <v>328</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>1193</v>
+        <v>1195</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>1194</v>
+        <v>1196</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>1195</v>
+        <v>1197</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15789,13 +15795,13 @@
         <v>328</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>1196</v>
+        <v>1198</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>1197</v>
+        <v>1199</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>1198</v>
+        <v>1200</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15803,19 +15809,19 @@
         <v>328</v>
       </c>
       <c r="B48" s="11" t="s">
-        <v>1199</v>
+        <v>1201</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>1200</v>
+        <v>1202</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>1201</v>
+        <v>1203</v>
       </c>
       <c r="E48" s="11" t="s">
-        <v>1202</v>
+        <v>1204</v>
       </c>
       <c r="F48" s="11" t="s">
-        <v>1203</v>
+        <v>1205</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15823,19 +15829,19 @@
         <v>328</v>
       </c>
       <c r="B49" s="11" t="s">
-        <v>1204</v>
+        <v>1206</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>1205</v>
+        <v>1207</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>1206</v>
+        <v>1208</v>
       </c>
       <c r="E49" s="11" t="s">
-        <v>1207</v>
+        <v>1209</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>1208</v>
+        <v>1210</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15843,19 +15849,19 @@
         <v>328</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>1209</v>
+        <v>1211</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>1210</v>
+        <v>1212</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>1211</v>
+        <v>1213</v>
       </c>
       <c r="E50" s="11" t="s">
-        <v>1212</v>
+        <v>1214</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>1213</v>
+        <v>1215</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15863,19 +15869,19 @@
         <v>328</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>1214</v>
+        <v>1216</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>1215</v>
+        <v>1217</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>1216</v>
+        <v>1218</v>
       </c>
       <c r="E51" s="11" t="s">
-        <v>1217</v>
+        <v>1219</v>
       </c>
       <c r="F51" s="11" t="s">
-        <v>1218</v>
+        <v>1220</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15883,19 +15889,19 @@
         <v>328</v>
       </c>
       <c r="B52" s="11" t="s">
-        <v>1219</v>
+        <v>1221</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>1220</v>
+        <v>1222</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>1221</v>
+        <v>1223</v>
       </c>
       <c r="E52" s="11" t="s">
-        <v>1222</v>
+        <v>1224</v>
       </c>
       <c r="F52" s="11" t="s">
-        <v>1223</v>
+        <v>1225</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15903,19 +15909,19 @@
         <v>328</v>
       </c>
       <c r="B53" s="11" t="s">
-        <v>1224</v>
+        <v>1226</v>
       </c>
       <c r="C53" s="11" t="s">
-        <v>1225</v>
+        <v>1227</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>1226</v>
+        <v>1228</v>
       </c>
       <c r="E53" s="11" t="s">
-        <v>1227</v>
+        <v>1229</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>1228</v>
+        <v>1230</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15923,19 +15929,19 @@
         <v>328</v>
       </c>
       <c r="B54" s="11" t="s">
-        <v>1229</v>
+        <v>1231</v>
       </c>
       <c r="C54" s="11" t="s">
-        <v>1230</v>
+        <v>1232</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>1231</v>
+        <v>1233</v>
       </c>
       <c r="E54" s="11" t="s">
-        <v>1232</v>
+        <v>1234</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>1233</v>
+        <v>1235</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15943,19 +15949,19 @@
         <v>328</v>
       </c>
       <c r="B55" s="11" t="s">
-        <v>1234</v>
+        <v>1236</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>1235</v>
+        <v>1237</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>1236</v>
+        <v>1238</v>
       </c>
       <c r="E55" s="11" t="s">
-        <v>1237</v>
+        <v>1239</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>1238</v>
+        <v>1240</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15963,13 +15969,13 @@
         <v>107</v>
       </c>
       <c r="B56" s="2" t="s">
-        <v>1239</v>
+        <v>1241</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>1240</v>
+        <v>1242</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>1241</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15977,13 +15983,13 @@
         <v>107</v>
       </c>
       <c r="B57" s="2" t="s">
-        <v>1242</v>
+        <v>1244</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>1243</v>
+        <v>1245</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>1244</v>
+        <v>1246</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15991,13 +15997,13 @@
         <v>107</v>
       </c>
       <c r="B58" s="2" t="s">
-        <v>1245</v>
+        <v>1247</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>1246</v>
+        <v>1248</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>1247</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16005,13 +16011,13 @@
         <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
-        <v>1248</v>
+        <v>1250</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>1249</v>
+        <v>1251</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>1250</v>
+        <v>1252</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16019,13 +16025,13 @@
         <v>107</v>
       </c>
       <c r="B60" s="74" t="s">
-        <v>1251</v>
+        <v>1253</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>1252</v>
+        <v>1254</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>1253</v>
+        <v>1255</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16033,13 +16039,13 @@
         <v>107</v>
       </c>
       <c r="B61" s="11" t="s">
-        <v>1254</v>
+        <v>1256</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>1255</v>
+        <v>1257</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>1256</v>
+        <v>1258</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16047,13 +16053,13 @@
         <v>107</v>
       </c>
       <c r="B62" s="11" t="s">
-        <v>1257</v>
+        <v>1259</v>
       </c>
       <c r="C62" s="11" t="s">
-        <v>1258</v>
+        <v>1260</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>1259</v>
+        <v>1261</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16061,19 +16067,19 @@
         <v>107</v>
       </c>
       <c r="B63" s="11" t="s">
-        <v>1260</v>
+        <v>1262</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>1261</v>
+        <v>1263</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>1262</v>
+        <v>1264</v>
       </c>
       <c r="E63" s="2" t="s">
-        <v>1263</v>
+        <v>1265</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>1264</v>
+        <v>1266</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16081,7 +16087,7 @@
         <v>328</v>
       </c>
       <c r="B64" s="63" t="s">
-        <v>1265</v>
+        <v>1267</v>
       </c>
       <c r="C64" s="63" t="s">
         <v>720</v>
@@ -16097,13 +16103,13 @@
         <v>328</v>
       </c>
       <c r="B65" s="63" t="s">
-        <v>1266</v>
+        <v>1268</v>
       </c>
       <c r="C65" s="63" t="s">
-        <v>925</v>
+        <v>927</v>
       </c>
       <c r="D65" s="63" t="s">
-        <v>926</v>
+        <v>928</v>
       </c>
       <c r="E65" s="63"/>
       <c r="F65" s="63"/>
@@ -16113,13 +16119,13 @@
         <v>328</v>
       </c>
       <c r="B66" s="63" t="s">
-        <v>1267</v>
+        <v>1269</v>
       </c>
       <c r="C66" s="63" t="s">
-        <v>927</v>
+        <v>929</v>
       </c>
       <c r="D66" s="63" t="s">
-        <v>928</v>
+        <v>930</v>
       </c>
       <c r="E66" s="63"/>
       <c r="F66" s="63"/>
@@ -16129,19 +16135,19 @@
         <v>328</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>1268</v>
+        <v>1270</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>930</v>
+        <v>932</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>931</v>
+        <v>933</v>
       </c>
       <c r="E67" s="11" t="s">
-        <v>932</v>
+        <v>934</v>
       </c>
       <c r="F67" s="11" t="s">
-        <v>933</v>
+        <v>935</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16149,19 +16155,19 @@
         <v>429</v>
       </c>
       <c r="B68" s="63" t="s">
-        <v>1269</v>
+        <v>1271</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>937</v>
+        <v>939</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>938</v>
+        <v>940</v>
       </c>
       <c r="E68" s="11" t="s">
-        <v>939</v>
+        <v>941</v>
       </c>
       <c r="F68" s="11" t="s">
-        <v>940</v>
+        <v>942</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16169,19 +16175,19 @@
         <v>429</v>
       </c>
       <c r="B69" s="63" t="s">
-        <v>1270</v>
+        <v>1272</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>942</v>
+        <v>944</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>943</v>
+        <v>945</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>944</v>
+        <v>946</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>945</v>
+        <v>947</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16189,13 +16195,13 @@
         <v>429</v>
       </c>
       <c r="B70" s="63" t="s">
-        <v>1271</v>
+        <v>1273</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>1272</v>
+        <v>1274</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>1273</v>
+        <v>1275</v>
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -16205,13 +16211,13 @@
         <v>429</v>
       </c>
       <c r="B71" s="63" t="s">
-        <v>1274</v>
+        <v>1276</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>1275</v>
+        <v>1277</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>1276</v>
+        <v>1278</v>
       </c>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
@@ -16221,13 +16227,13 @@
         <v>429</v>
       </c>
       <c r="B72" s="63" t="s">
-        <v>1277</v>
+        <v>1279</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>1278</v>
+        <v>1280</v>
       </c>
       <c r="D72" s="11" t="s">
-        <v>1279</v>
+        <v>1281</v>
       </c>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
@@ -16237,13 +16243,13 @@
         <v>429</v>
       </c>
       <c r="B73" s="11" t="s">
-        <v>1280</v>
+        <v>1282</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>1281</v>
+        <v>1283</v>
       </c>
       <c r="D73" s="11" t="s">
-        <v>1282</v>
+        <v>1284</v>
       </c>
       <c r="E73" s="11"/>
       <c r="F73" s="11"/>
@@ -16253,13 +16259,13 @@
         <v>328</v>
       </c>
       <c r="B74" s="11" t="s">
-        <v>1283</v>
+        <v>1285</v>
       </c>
       <c r="C74" s="11" t="s">
-        <v>1284</v>
+        <v>1286</v>
       </c>
       <c r="D74" s="11" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16267,13 +16273,13 @@
         <v>328</v>
       </c>
       <c r="B75" s="11" t="s">
-        <v>1286</v>
+        <v>1288</v>
       </c>
       <c r="C75" s="11" t="s">
-        <v>1287</v>
+        <v>1289</v>
       </c>
       <c r="D75" s="11" t="s">
-        <v>1288</v>
+        <v>1290</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16281,13 +16287,13 @@
         <v>328</v>
       </c>
       <c r="B76" s="11" t="s">
-        <v>1289</v>
+        <v>1291</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>1290</v>
+        <v>1292</v>
       </c>
       <c r="D76" s="11" t="s">
-        <v>1291</v>
+        <v>1293</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16295,13 +16301,13 @@
         <v>328</v>
       </c>
       <c r="B77" s="11" t="s">
-        <v>1292</v>
+        <v>1294</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>1293</v>
+        <v>1295</v>
       </c>
       <c r="D77" s="11" t="s">
-        <v>1294</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16309,19 +16315,19 @@
         <v>107</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1295</v>
+        <v>1297</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>986</v>
+        <v>988</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>987</v>
+        <v>989</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>988</v>
+        <v>990</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>989</v>
+        <v>991</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16329,19 +16335,19 @@
         <v>107</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1296</v>
+        <v>1298</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>990</v>
+        <v>992</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>991</v>
+        <v>993</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>992</v>
+        <v>994</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>993</v>
+        <v>995</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16349,19 +16355,19 @@
         <v>107</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>1297</v>
+        <v>1299</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>994</v>
+        <v>996</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>995</v>
+        <v>997</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>996</v>
+        <v>998</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>997</v>
+        <v>999</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16369,19 +16375,19 @@
         <v>107</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>1298</v>
+        <v>1300</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>998</v>
+        <v>1000</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>999</v>
+        <v>1001</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>1000</v>
+        <v>1002</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1001</v>
+        <v>1003</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16389,19 +16395,19 @@
         <v>107</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>1299</v>
+        <v>1301</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1002</v>
+        <v>1004</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>1003</v>
+        <v>1005</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>1004</v>
+        <v>1006</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>1005</v>
+        <v>1007</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16409,19 +16415,19 @@
         <v>276</v>
       </c>
       <c r="B83" s="2" t="s">
-        <v>1300</v>
+        <v>1302</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>1301</v>
+        <v>1303</v>
       </c>
       <c r="D83" s="11" t="s">
-        <v>1302</v>
+        <v>1304</v>
       </c>
       <c r="E83" s="11" t="s">
-        <v>1303</v>
+        <v>1305</v>
       </c>
       <c r="F83" s="11" t="s">
-        <v>1304</v>
+        <v>1306</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16429,19 +16435,19 @@
         <v>276</v>
       </c>
       <c r="B84" s="2" t="s">
-        <v>1305</v>
+        <v>1307</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>1306</v>
+        <v>1308</v>
       </c>
       <c r="D84" s="11" t="s">
-        <v>1307</v>
+        <v>1309</v>
       </c>
       <c r="E84" s="11" t="s">
-        <v>1308</v>
+        <v>1310</v>
       </c>
       <c r="F84" s="11" t="s">
-        <v>1309</v>
+        <v>1311</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16449,13 +16455,13 @@
         <v>591</v>
       </c>
       <c r="B85" s="2" t="s">
-        <v>1310</v>
+        <v>1312</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>1311</v>
+        <v>1313</v>
       </c>
       <c r="D85" s="11" t="s">
-        <v>1312</v>
+        <v>1314</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Label: Update the French word for 'teletravail'
Fix: #219
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -882,13 +882,13 @@
     <t xml:space="preserve">remoteWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **dernière semaine**, quand {{nickname}} a-t-{{gender:il/elle/iel/"il/elle"}} fait du **télé-travail**?</t>
+    <t xml:space="preserve">Durant la **dernière semaine**, quand {{nickname}} a-t-{{gender:il/elle/iel/"il/elle"}} fait du **télétravail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did {{nickname}} **work remotely**?</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **dernière semaine**, quand avez-vous fait du **télé-travail**?</t>
+    <t xml:space="preserve">Durant la **dernière semaine**, quand avez-vous fait du **télétravail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did you **work remotely**?</t>
@@ -5502,12 +5502,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C110" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A110" activeCellId="0" sqref="A110"/>
-      <selection pane="bottomRight" activeCell="I115" activeCellId="0" sqref="I115"/>
+      <selection pane="bottomLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+      <selection pane="bottomRight" activeCell="I42" activeCellId="0" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6152,7 +6152,7 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
-      <c r="T12" s="8" t="b">
+      <c r="T12" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6203,7 +6203,7 @@
       <c r="Q13" s="8"/>
       <c r="R13" s="8"/>
       <c r="S13" s="8"/>
-      <c r="T13" s="8" t="b">
+      <c r="T13" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6254,7 +6254,7 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
-      <c r="T14" s="8" t="b">
+      <c r="T14" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6303,7 +6303,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
-      <c r="T15" s="8" t="b">
+      <c r="T15" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6403,7 +6403,7 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
-      <c r="T17" s="8" t="b">
+      <c r="T17" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6612,7 +6612,7 @@
       <c r="Q21" s="26"/>
       <c r="R21" s="26"/>
       <c r="S21" s="26"/>
-      <c r="T21" s="23" t="b">
+      <c r="T21" s="25" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7131,7 +7131,7 @@
       <c r="Q31" s="26"/>
       <c r="R31" s="26"/>
       <c r="S31" s="26"/>
-      <c r="T31" s="23" t="b">
+      <c r="T31" s="25" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7181,7 +7181,7 @@
       <c r="Q32" s="26"/>
       <c r="R32" s="26"/>
       <c r="S32" s="26"/>
-      <c r="T32" s="23" t="b">
+      <c r="T32" s="25" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7661,7 +7661,7 @@
       <c r="Q41" s="26"/>
       <c r="R41" s="26"/>
       <c r="S41" s="26"/>
-      <c r="T41" s="23" t="b">
+      <c r="T41" s="25" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8476,7 +8476,7 @@
       <c r="Q59" s="35"/>
       <c r="R59" s="35"/>
       <c r="S59" s="35"/>
-      <c r="T59" s="33" t="b">
+      <c r="T59" s="36" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8801,7 +8801,7 @@
       <c r="Q66" s="35"/>
       <c r="R66" s="35"/>
       <c r="S66" s="35"/>
-      <c r="T66" s="33" t="b">
+      <c r="T66" s="36" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9524,7 +9524,7 @@
       <c r="Q82" s="35"/>
       <c r="R82" s="35"/>
       <c r="S82" s="35"/>
-      <c r="T82" s="33" t="b">
+      <c r="T82" s="36" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10534,7 +10534,7 @@
       <c r="Q104" s="35"/>
       <c r="R104" s="35"/>
       <c r="S104" s="35"/>
-      <c r="T104" s="17" t="b">
+      <c r="T104" s="19" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10785,7 +10785,7 @@
       <c r="Q109" s="35"/>
       <c r="R109" s="35"/>
       <c r="S109" s="35"/>
-      <c r="T109" s="17" t="b">
+      <c r="T109" s="19" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13247,7 +13247,7 @@
   </sheetPr>
   <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Label: Inverse 'dernière semaine' in French.
Fix: #199, fix: #201
This will make sure that the bold expression are the same in all questions about 'last week'.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -855,19 +855,75 @@
     <t xml:space="preserve">travelToWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la dernière **semaine**, quand {{nickname}} s'est-{{gender:il/elle/iel/"il/elle"}} **déplacé{{gender:/e/·e}}** pour le **travail**?
+    <t xml:space="preserve">Durant la **semaine dernière**, quand {{nickname}} s'est-{{gender:il/elle/iel/"il/elle"}} **déplacé{{gender:/e/·e}}** pour le **travail**?
 __Pour se rendre au travail ou toute autre raison concernant le travail.__</t>
   </si>
   <si>
-    <t xml:space="preserve">During the last **week**, when did {{nickname}} **travel** for **work**?
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">During the **</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">last </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">week**, when did {{nickname}} **travel** for **work**?
 __To get to or for any other reason concerning work.__</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Durant la dernière **semaine**, quand vous êtes-vous **déplacé{{gender:/e/·e}}** pour le **travail**?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">During the last **week**, when did you **travel** for **work**?
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Durant la **semaine dernière**, quand vous êtes-vous **déplacé{{gender:/e/·e}}** pour le **travail**?</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">During the **</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">last </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">week**, when did you **travel** for **work**?
 __To get to or for any other reason concerning work.__</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">travelToPlaceCustomValidation</t>
@@ -882,13 +938,13 @@
     <t xml:space="preserve">remoteWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **dernière semaine**, quand {{nickname}} a-t-{{gender:il/elle/iel/"il/elle"}} fait du **télétravail**?</t>
+    <t xml:space="preserve">Durant la **semaine dernière**, quand {{nickname}} a-t-{{gender:il/elle/iel/"il/elle"}} fait du **télétravail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did {{nickname}} **work remotely**?</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **dernière semaine**, quand avez-vous fait du **télétravail**?</t>
+    <t xml:space="preserve">Durant la **semaine dernière**, quand avez-vous fait du **télétravail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did you **work remotely**?</t>
@@ -4491,7 +4547,7 @@
     <numFmt numFmtId="166" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4587,6 +4643,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
     </font>
     <font>
       <b val="true"/>
@@ -4906,11 +4968,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4918,11 +4980,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4930,7 +4992,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4938,7 +5000,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4950,27 +5012,27 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4982,11 +5044,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5002,11 +5064,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5042,11 +5104,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5058,7 +5120,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5094,15 +5156,15 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5507,7 +5569,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
-      <selection pane="bottomRight" activeCell="I42" activeCellId="0" sqref="I42"/>
+      <selection pane="bottomRight" activeCell="I45" activeCellId="0" sqref="I45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Label: Update the English label of endConsideredAbandoningSurvey
Fix: #196
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -2483,7 +2483,7 @@
     <t xml:space="preserve">Avez-vous pensé, à un moment ou un autre, **abandonner l'enquête**?</t>
   </si>
   <si>
-    <t xml:space="preserve">Have you considered, at any point, to **abandon the survey**?</t>
+    <t xml:space="preserve">Have you considered, at any point, **abandoning the survey**?</t>
   </si>
   <si>
     <t xml:space="preserve">buttonCompleteInterviewWithCompleteSection</t>
@@ -5565,11 +5565,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C39" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C128" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
-      <selection pane="bottomRight" activeCell="I45" activeCellId="0" sqref="I45"/>
+      <selection pane="bottomLeft" activeCell="A128" activeCellId="0" sqref="A128"/>
+      <selection pane="bottomRight" activeCell="I133" activeCellId="0" sqref="I133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11906,7 +11906,7 @@
       <c r="W132" s="35"/>
       <c r="X132" s="35"/>
     </row>
-    <row r="133" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A133" s="11" t="s">
         <v>657</v>
       </c>

</xml_diff>

<commit_message>
Label: Add a word in personDidTrips question label.
Fix: #182
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -1040,7 +1040,7 @@
   </si>
   <si>
     <t xml:space="preserve">Est-ce que {{nickname}} s'est déplac{{gender:é/ée/é.e}} le {{assignedDate}}?
-__Inclure tous les déplacements, qu'ils soient pour motifs personnels (achats, sorties, loisirs, etc.), pour le travail, ou pour aller chercher ou reconduire quelqu'un.__</t>
+__Inclure tous les déplacements, qu'ils soient pour des motifs personnels (achats, sorties, loisirs, etc.), pour le travail, ou pour aller chercher ou reconduire quelqu'un.__</t>
   </si>
   <si>
     <t xml:space="preserve">Did {{nickname}} make any trips on {{assignedDate}}?
@@ -1048,7 +1048,7 @@
   </si>
   <si>
     <t xml:space="preserve">Vous êtes-vous déplac{{gender:é/ée/é.e}} le {{assignedDate}}?
-__Inclure tous les déplacements, qu'ils soient pour motifs personnels (achats, sorties, loisirs, etc.), pour le travail, ou pour aller chercher ou reconduire quelqu'un.__</t>
+__Inclure tous les déplacements, qu'ils soient pour des motifs personnels (achats, sorties, loisirs, etc.), pour le travail, ou pour aller chercher ou reconduire quelqu'un.__</t>
   </si>
   <si>
     <t xml:space="preserve">Did you make any trips on {{assignedDate}}?
@@ -5565,11 +5565,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C128" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A128" activeCellId="0" sqref="A128"/>
-      <selection pane="bottomRight" activeCell="I133" activeCellId="0" sqref="I133"/>
+      <selection pane="bottomLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+      <selection pane="bottomRight" activeCell="H50" activeCellId="0" sqref="H50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Label: Remove some dot and space before question mark
Fix: #203
Note: We remove some dot at the end of the first sentence of a question, that are not in a paragraph.
Note: We don't have space before question mark in French (from Quebec). Same in English.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -154,7 +154,7 @@
     <t xml:space="preserve">Veuillez saisir le courriel **ou** le numéro de téléphone pour vous recontacter.</t>
   </si>
   <si>
-    <t xml:space="preserve">Please enter the email **or** phone number to get in contact.</t>
+    <t xml:space="preserve">Please enter the email **or** phone number to get in contact</t>
   </si>
   <si>
     <t xml:space="preserve">acceptsToBeContactedForHelp</t>
@@ -407,12 +407,12 @@
     <t xml:space="preserve">nickname</t>
   </si>
   <si>
-    <t xml:space="preserve">**Nom ou surnom** pour identifier cette personne pour la suite de l'entrevue.
+    <t xml:space="preserve">**Nom ou surnom** pour identifier cette personne pour la suite de l'entrevue
 __Peut être un surnom, des initiales, ou encore ce que cette personne est pour vous (ex: 'Moi', 'Toto', 'Maman', 'PN').
 Ce nom est seulement utilisé pour faciliter l'enquête et sera ensuite supprimé.__</t>
   </si>
   <si>
-    <t xml:space="preserve">**Name or nickname** that will allow you to identify this person for the remainder of the interview.
+    <t xml:space="preserve">**Name or nickname** that will allow you to identify this person for the remainder of the interview
 __Can be a nickname, initials, or who this person represents to you (ex: 'Me','Kiddo','Mum','JT').
 The name is only used to simplify the response process and will be removed from the final dataset.__</t>
   </si>
@@ -568,16 +568,16 @@
     <t xml:space="preserve">workerTypeBeforeLeave</t>
   </si>
   <si>
-    <t xml:space="preserve">**Avant d’être en congé**, est-ce que {{nickname}} travaillait ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Before being on leave**, did {{nickname}} work ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Avant d’être en congé**, est-ce que vous travailliez ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Before being on leave**, did you work ?</t>
+    <t xml:space="preserve">**Avant d’être en congé**, est-ce que {{nickname}} travaillait?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Before being on leave**, did {{nickname}} work?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Avant d’être en congé**, est-ce que vous travailliez?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Before being on leave**, did you work?</t>
   </si>
   <si>
     <t xml:space="preserve">parentalOrSickLeaveConditional</t>
@@ -782,12 +782,12 @@
     <t xml:space="preserve">usualWorkPlace.geography</t>
   </si>
   <si>
-    <t xml:space="preserve">Veuillez localiser le **lieu de travail habituel** de {{nickname}}.
+    <t xml:space="preserve">Veuillez localiser le **lieu de travail habituel** de {{nickname}}
 __Naviguez, zoomez, et cliquez sur la carte pour localiser le lieu. Une fois localisé, vous pourrez déplacer le point sur la carte pour davantage de précision.
 Vous pouvez également chercher le lieu sur la carte en utilisant le bouton "Chercher le lieu").__</t>
   </si>
   <si>
-    <t xml:space="preserve">Please locate the **usual place of work** for {{nickname}}.
+    <t xml:space="preserve">Please locate the **usual place of work** for {{nickname}}
 __Navigate, zoom, and click on the map to identify the location. Once located, you can move the marker for greater precision.
 You can also search for the place on the map using the "Search location" button.__</t>
   </si>
@@ -1076,7 +1076,7 @@
     <t xml:space="preserve">didTripsIntro</t>
   </si>
   <si>
-    <t xml:space="preserve">Nous allons vous demander d'indiquer les lieux où {{nickname}} est all{{gender:é/ée/é.e}} le {{assignedDate}} (inclure les lieux visités jusqu'à 4:00 le lendemain matin).
+    <t xml:space="preserve">Nous allons vous demander d'indiquer les lieux où {{nickname}} est all{{gender:é/ée/é.e}} le {{assignedDate}} (inclure les lieux visités jusqu'à 4:00 le lendemain matin)
 &lt;span class="_green"&gt;- **Inclure même les petits arrêts** (station-service, garderie/école, dépanneur ou tout lieu où {{nickname}} est all{{gender:é/ée/é.e}} chercher ou reconduire quelqu'un).
 - **Inclure tous les lieux** peu importe les modes de transport utilisés pour s'y rendre (marche, vélo, voiture, transport collectif, taxi, avion, bateau, etc.).&lt;/span&gt;
 &lt;span class="_red"&gt;- **Ne pas inclure les lieux de transfert** en cours de déplacement (arrêts de bus, gares, terminus, lieux de stationnement, etc.) sauf si {{nickname}} est all{{gender:é/ée/é.e}} reconduire ou chercher quelqu'un à cet endroit.&lt;/span&gt;</t>
@@ -1088,13 +1088,13 @@
 &lt;span class="_red"&gt;- **Do not include transfer locations** (bus stops, train stations, terminals, parking lots, etc.) unless {{nickname}} went there to drop someone off or pick someone up.&lt;/span&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Nous allons vous demander d'indiquer les **lieux où vous êtes all{{gender:é/ée/é.e}} le {{assignedDate}}** (inclure les lieux visités jusqu'à 4:00 le lendemain matin).
+    <t xml:space="preserve">Nous allons vous demander d'indiquer les **lieux où vous êtes all{{gender:é/ée/é.e}} le {{assignedDate}}** (inclure les lieux visités jusqu'à 4:00 le lendemain matin)
 &lt;span class="_green"&gt;- **Inclure même les petits arrêts** (station-service, garderie/école, dépanneur ou tout lieu où vous êtes all{{gender:é/ée/é.e}} chercher ou reconduire quelqu'un).
 - **Inclure tous les lieux** peu importe les modes de transport utilisés pour s'y rendre (marche, vélo, voiture, transport collectif, taxi, avion, bateau, etc.).&lt;/span&gt;
 &lt;span class="_red"&gt;- **Ne pas inclure les lieux de transfert** en cours de déplacement (arrêts de bus, gares, terminus, lieux de stationnement, etc.) sauf si vous êtes all{{gender:é/ée/é.e}} reconduire ou chercher quelqu'un à cet endroit.&lt;/span&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Please specify the **places you went on {{assignedDate}}** (include all places visited until 4 AM the following morning).
+    <t xml:space="preserve">Please specify the **places you went on {{assignedDate}}** (include all places visited until 4 AM the following morning)
 &lt;span class="_green"&gt;- **Include short stops and errands** (gas station, daycare/school, convenience store or any place where you picked someone up or dropped someone off).
 - **Include all places** regardless of the mode of transport used to get there (walking, cycling, car, public transit, taxi, plane, boat, etc.).&lt;/span&gt;
 &lt;span class="_red"&gt;- **Do not include transfer locations** (bus stops, train stations, terminals, parking lots, etc.) unless you went there to drop someone off or pick someone up.&lt;/span&gt;</t>
@@ -1161,10 +1161,10 @@
     <t xml:space="preserve">tripsIntroOutro</t>
   </si>
   <si>
-    <t xml:space="preserve">__Vos réponses serviront à évaluer l'usage et l'achalandage des réseaux routiers et de transport collectif et demeureront entièrement confidentielles.__</t>
-  </si>
-  <si>
-    <t xml:space="preserve">__Your answers will be used to assess the use and traffic of the road and public transit networks and will remain entirely confidential.__</t>
+    <t xml:space="preserve">__Vos réponses serviront à évaluer l'usage et l'achalandage des réseaux routiers et de transport collectif et demeureront entièrement confidentielles__</t>
+  </si>
+  <si>
+    <t xml:space="preserve">__Your answers will be used to assess the use and traffic of the road and public transit networks and will remain entirely confidential__</t>
   </si>
   <si>
     <t xml:space="preserve">visitedPlaces</t>
@@ -1692,10 +1692,10 @@
     <t xml:space="preserve">tripJunctionQueryString</t>
   </si>
   <si>
-    <t xml:space="preserve">Indiquez l'adresse ou le nom du lieu où s'est effectué le changement de mode de transport (terminus, arrêt, stationnement etc.) ou cliquez directement sur la carte.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Please specify the address or the name of the location where the change in mode of transport occurred (terminal, transit stop, parking lot, etc.) or click directly on map.</t>
+    <t xml:space="preserve">Indiquez l'adresse ou le nom du lieu où s'est effectué le changement de mode de transport (terminus, arrêt, stationnement etc.) ou cliquez directement sur la carte</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Please specify the address or the name of the location where the change in mode of transport occurred (terminal, transit stop, parking lot, etc.) or click directly on map</t>
   </si>
   <si>
     <t xml:space="preserve">shouldAskTripJunctionCustomConditional</t>
@@ -1753,10 +1753,10 @@
     <t xml:space="preserve">personNoWorkTripIntro</t>
   </si>
   <si>
-    <t xml:space="preserve">**Vous n'avez déclaré aucun déplacement pour le travail** pour {{nickname}} le {{assignedDate}}.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**You didn't report any work trips** by {{nickname}} on {{assignedDate}}.</t>
+    <t xml:space="preserve">**Vous n'avez déclaré aucun déplacement pour le travail** pour {{nickname}} le {{assignedDate}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**You didn't report any work trips** by {{nickname}} on {{assignedDate}}</t>
   </si>
   <si>
     <t xml:space="preserve">Custom because of the label</t>
@@ -1771,10 +1771,10 @@
     <t xml:space="preserve">household.persons.{_activePersonId}.journeys.{_activeJourneyId}.noWorkTripReason</t>
   </si>
   <si>
-    <t xml:space="preserve">Pour quelle raison ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Why ?</t>
+    <t xml:space="preserve">Pour quelle raison?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Why?</t>
   </si>
   <si>
     <t xml:space="preserve">shouldAskForNoWorkTripReasonCustomConditional</t>
@@ -1792,18 +1792,18 @@
     <t xml:space="preserve">household.persons.{_activePersonId}.journeys.{_activeJourneyId}.noWorkTripReasonSpecify</t>
   </si>
   <si>
-    <t xml:space="preserve">Veuillez préciser la raison pour laquelle {{nickname}} n'a effectué aucun déplacement pour le travail le {{assignedDate}} ?
+    <t xml:space="preserve">Veuillez préciser la raison pour laquelle {{nickname}} n'a effectué aucun déplacement pour le travail le {{assignedDate}}?
 __(Facultatif)__</t>
   </si>
   <si>
-    <t xml:space="preserve">Please specify the reason why {{nickname}} made no trip for work on {{assignedDate}} ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veuillez préciser la raison pour laquelle vous n'avez effectué aucun déplacement pour le travail le {{assignedDate}} ?
+    <t xml:space="preserve">Please specify the reason why {{nickname}} made no trip for work on {{assignedDate}}?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veuillez préciser la raison pour laquelle vous n'avez effectué aucun déplacement pour le travail le {{assignedDate}}?
 __(Facultatif)__</t>
   </si>
   <si>
-    <t xml:space="preserve">Please specify the reason why you made no trip for work on {{assignedDate}} ?
+    <t xml:space="preserve">Please specify the reason why you made no trip for work on {{assignedDate}}?
 __(Optional)__</t>
   </si>
   <si>
@@ -1840,18 +1840,18 @@
     <t xml:space="preserve">household.persons.{_activePersonId}.journeys.{_activeJourneyId}.noSchoolTripReasonSpecify</t>
   </si>
   <si>
-    <t xml:space="preserve">Veuillez préciser la raison pour laquelle {{nickname}} n'a effectué aucun déplacement pour les études le {{assignedDate}} ?
+    <t xml:space="preserve">Veuillez préciser la raison pour laquelle {{nickname}} n'a effectué aucun déplacement pour les études le {{assignedDate}}?
 __(Facultatif)__</t>
   </si>
   <si>
-    <t xml:space="preserve">Please specify the reason why {{nickname}} made no trip for school on {{assignedDate}} ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Veuillez préciser la raison pour laquelle vous n'avez effectué aucun déplacement pour les études le {{assignedDate}} ?
+    <t xml:space="preserve">Please specify the reason why {{nickname}} made no trip for school on {{assignedDate}}?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Veuillez préciser la raison pour laquelle vous n'avez effectué aucun déplacement pour les études le {{assignedDate}}?
 __(Facultatif)__</t>
   </si>
   <si>
-    <t xml:space="preserve">Please specify the reason why you made no trip for school on {{assignedDate}} ?
+    <t xml:space="preserve">Please specify the reason why you made no trip for school on {{assignedDate}}?
 __(Optional)__</t>
   </si>
   <si>
@@ -2435,7 +2435,7 @@
     <t xml:space="preserve">interestOfTheSurvey</t>
   </si>
   <si>
-    <t xml:space="preserve">Dans quelle mesure cette enquête a-t-elle été **intéressante** pour vous ?</t>
+    <t xml:space="preserve">Dans quelle mesure cette enquête a-t-elle été **intéressante** pour vous?</t>
   </si>
   <si>
     <t xml:space="preserve">How **interesting** was this survey to you?</t>
@@ -2465,7 +2465,7 @@
     <t xml:space="preserve">burdenOfTheSurvey</t>
   </si>
   <si>
-    <t xml:space="preserve">Dans quelle mesure avez-vous trouvé cette enquête **pénible (exigeante)** ?</t>
+    <t xml:space="preserve">Dans quelle mesure avez-vous trouvé cette enquête **pénible (exigeante)**?</t>
   </si>
   <si>
     <t xml:space="preserve">How **burdensome (demanding)** did you find this survey to be?</t>
@@ -5565,11 +5565,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C46" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C129" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
-      <selection pane="bottomRight" activeCell="H50" activeCellId="0" sqref="H50"/>
+      <selection pane="bottomLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
+      <selection pane="bottomRight" activeCell="H110" activeCellId="0" sqref="H110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Range input: Change the color of a range input to green and red.
Fix: #227
Fix some error with the UI testing.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2280" uniqueCount="1325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2280" uniqueCount="1324">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -3637,7 +3637,7 @@
     <t xml:space="preserve">%</t>
   </si>
   <si>
-    <t xml:space="preserve">blue</t>
+    <t xml:space="preserve">green-yellow-red</t>
   </si>
   <si>
     <t xml:space="preserve">Pas du tout</t>
@@ -3677,9 +3677,6 @@
   </si>
   <si>
     <t xml:space="preserve">Very difficult</t>
-  </si>
-  <si>
-    <t xml:space="preserve">green-yellow-red</t>
   </si>
   <si>
     <t xml:space="preserve">Modérément pénible</t>
@@ -4547,7 +4544,7 @@
     <numFmt numFmtId="166" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4734,6 +4731,12 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="0"/>
@@ -4835,7 +4838,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5165,6 +5168,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5564,12 +5571,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="1" topLeftCell="C129" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A129" activeCellId="0" sqref="A129"/>
-      <selection pane="bottomRight" activeCell="H110" activeCellId="0" sqref="H110"/>
+      <selection pane="bottomRight" activeCell="F135" activeCellId="0" sqref="F135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15380,8 +15387,8 @@
   </sheetPr>
   <dimension ref="A1:L1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M10" activeCellId="0" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15470,7 +15477,7 @@
       <c r="K2" s="50" t="s">
         <v>1043</v>
       </c>
-      <c r="L2" s="50" t="s">
+      <c r="L2" s="82" t="s">
         <v>1044</v>
       </c>
     </row>
@@ -15484,13 +15491,13 @@
       <c r="C3" s="50" t="s">
         <v>1046</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="83" t="s">
         <v>1047</v>
       </c>
-      <c r="E3" s="82" t="s">
+      <c r="E3" s="83" t="s">
         <v>1048</v>
       </c>
-      <c r="F3" s="82" t="s">
+      <c r="F3" s="83" t="s">
         <v>1049</v>
       </c>
       <c r="G3" s="50" t="s">
@@ -15547,7 +15554,7 @@
         <v>1043</v>
       </c>
       <c r="L4" s="50" t="s">
-        <v>1058</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15558,19 +15565,19 @@
         <v>1045</v>
       </c>
       <c r="C5" s="50" t="s">
+        <v>1058</v>
+      </c>
+      <c r="D5" s="50" t="s">
         <v>1059</v>
-      </c>
-      <c r="D5" s="50" t="s">
-        <v>1060</v>
       </c>
       <c r="E5" s="50" t="s">
         <v>1048</v>
       </c>
       <c r="F5" s="50" t="s">
+        <v>1060</v>
+      </c>
+      <c r="G5" s="50" t="s">
         <v>1061</v>
-      </c>
-      <c r="G5" s="50" t="s">
-        <v>1062</v>
       </c>
       <c r="H5" s="50" t="n">
         <v>-10</v>
@@ -15585,7 +15592,7 @@
         <v>1043</v>
       </c>
       <c r="L5" s="50" t="s">
-        <v>1058</v>
+        <v>1044</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -15644,13 +15651,13 @@
         <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1062</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1063</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>1064</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>1065</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -15660,13 +15667,13 @@
         <v>107</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>1065</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>1066</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>1067</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>1068</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -15676,13 +15683,13 @@
         <v>429</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>1068</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>1069</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>1070</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>1071</v>
       </c>
       <c r="E4" s="11"/>
     </row>
@@ -15691,13 +15698,13 @@
         <v>429</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>1071</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>1072</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>1073</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>1074</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15705,13 +15712,13 @@
         <v>429</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>1074</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>1075</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>1076</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>1077</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15719,13 +15726,13 @@
         <v>429</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>1077</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>1078</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>1079</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>1080</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15733,13 +15740,13 @@
         <v>429</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>1080</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>1081</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>1082</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>1083</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15747,13 +15754,13 @@
         <v>429</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>1083</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>1084</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>1085</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>1086</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15761,13 +15768,13 @@
         <v>429</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>1086</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>1087</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>1088</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>1089</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15775,13 +15782,13 @@
         <v>429</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>1089</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>1090</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>1091</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>1092</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15789,13 +15796,13 @@
         <v>429</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>1092</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>1093</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>1094</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>1095</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15803,13 +15810,13 @@
         <v>429</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>1095</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>1096</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>1097</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>1098</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15817,7 +15824,7 @@
         <v>429</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>766</v>
@@ -15831,13 +15838,13 @@
         <v>429</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>1099</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>1100</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>1101</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>1102</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15845,19 +15852,19 @@
         <v>328</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>1102</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>1103</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>1104</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>1105</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>1106</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>1107</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15865,19 +15872,19 @@
         <v>328</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>1107</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>1108</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>1109</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>1110</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>1111</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>1112</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15885,19 +15892,19 @@
         <v>328</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>1112</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>1113</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>1114</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>1115</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>1116</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>1117</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15905,19 +15912,19 @@
         <v>328</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>1117</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>1118</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>1119</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>1120</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>1121</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>1122</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15925,19 +15932,19 @@
         <v>328</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>1122</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>1123</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>1124</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>1125</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>1126</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>1127</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15945,19 +15952,19 @@
         <v>328</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>1127</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>1128</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>1129</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>1130</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>1131</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>1132</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15965,13 +15972,13 @@
         <v>328</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>1132</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>1133</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>1134</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>1135</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15979,13 +15986,13 @@
         <v>328</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>1135</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>1136</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>1137</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>1138</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15993,13 +16000,13 @@
         <v>328</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>1138</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>1139</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>1140</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>1141</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16007,13 +16014,13 @@
         <v>328</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>1141</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>1142</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>1143</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>1144</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16021,19 +16028,19 @@
         <v>328</v>
       </c>
       <c r="B26" s="11" t="s">
+        <v>1144</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>1145</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>1146</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>1147</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>1148</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>1149</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16041,13 +16048,13 @@
         <v>328</v>
       </c>
       <c r="B27" s="11" t="s">
+        <v>1149</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>1150</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="D27" s="11" t="s">
         <v>1151</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>1152</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16055,13 +16062,13 @@
         <v>328</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>1152</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>1153</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="D28" s="11" t="s">
         <v>1154</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>1155</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16069,13 +16076,13 @@
         <v>328</v>
       </c>
       <c r="B29" s="11" t="s">
+        <v>1155</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>1156</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="D29" s="11" t="s">
         <v>1157</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>1158</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16083,13 +16090,13 @@
         <v>328</v>
       </c>
       <c r="B30" s="11" t="s">
+        <v>1158</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>1159</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>1160</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>1161</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16097,13 +16104,13 @@
         <v>328</v>
       </c>
       <c r="B31" s="11" t="s">
+        <v>1161</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>1162</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="D31" s="11" t="s">
         <v>1163</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>1164</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16111,13 +16118,13 @@
         <v>328</v>
       </c>
       <c r="B32" s="11" t="s">
+        <v>1164</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>1165</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="D32" s="11" t="s">
         <v>1166</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>1167</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16125,13 +16132,13 @@
         <v>328</v>
       </c>
       <c r="B33" s="11" t="s">
+        <v>1167</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>1168</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="D33" s="11" t="s">
         <v>1169</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>1170</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16139,13 +16146,13 @@
         <v>328</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>1170</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>1171</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="D34" s="11" t="s">
         <v>1172</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>1173</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16153,13 +16160,13 @@
         <v>328</v>
       </c>
       <c r="B35" s="11" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>1174</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="D35" s="11" t="s">
         <v>1175</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>1176</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16167,13 +16174,13 @@
         <v>328</v>
       </c>
       <c r="B36" s="11" t="s">
+        <v>1176</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>1177</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>1178</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>1179</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16181,13 +16188,13 @@
         <v>328</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>1180</v>
+        <v>1179</v>
       </c>
       <c r="C37" s="11" t="s">
+        <v>1177</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>1178</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>1179</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16195,13 +16202,13 @@
         <v>328</v>
       </c>
       <c r="B38" s="11" t="s">
+        <v>1180</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>1181</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="D38" s="11" t="s">
         <v>1182</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>1183</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16209,13 +16216,13 @@
         <v>328</v>
       </c>
       <c r="B39" s="11" t="s">
+        <v>1183</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>1184</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>1185</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>1186</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16223,13 +16230,13 @@
         <v>328</v>
       </c>
       <c r="B40" s="11" t="s">
+        <v>1186</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>1187</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="D40" s="11" t="s">
         <v>1188</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>1189</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16237,13 +16244,13 @@
         <v>328</v>
       </c>
       <c r="B41" s="11" t="s">
+        <v>1189</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>1190</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="11" t="s">
         <v>1191</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>1192</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16251,13 +16258,13 @@
         <v>328</v>
       </c>
       <c r="B42" s="11" t="s">
+        <v>1192</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>1193</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>1194</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>1195</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16265,13 +16272,13 @@
         <v>328</v>
       </c>
       <c r="B43" s="11" t="s">
+        <v>1195</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>1196</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>1197</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>1198</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16279,13 +16286,13 @@
         <v>328</v>
       </c>
       <c r="B44" s="11" t="s">
+        <v>1198</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>1199</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="D44" s="11" t="s">
         <v>1200</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>1201</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16293,13 +16300,13 @@
         <v>328</v>
       </c>
       <c r="B45" s="11" t="s">
+        <v>1201</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>1202</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="11" t="s">
         <v>1203</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>1204</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16307,13 +16314,13 @@
         <v>328</v>
       </c>
       <c r="B46" s="11" t="s">
+        <v>1204</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>1205</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="D46" s="11" t="s">
         <v>1206</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>1207</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16321,13 +16328,13 @@
         <v>328</v>
       </c>
       <c r="B47" s="11" t="s">
+        <v>1207</v>
+      </c>
+      <c r="C47" s="11" t="s">
         <v>1208</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="D47" s="11" t="s">
         <v>1209</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>1210</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16335,19 +16342,19 @@
         <v>328</v>
       </c>
       <c r="B48" s="11" t="s">
+        <v>1210</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>1211</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="11" t="s">
         <v>1212</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>1213</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="F48" s="11" t="s">
         <v>1214</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>1215</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16355,19 +16362,19 @@
         <v>328</v>
       </c>
       <c r="B49" s="11" t="s">
+        <v>1215</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>1216</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="D49" s="11" t="s">
         <v>1217</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="E49" s="11" t="s">
         <v>1218</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="F49" s="11" t="s">
         <v>1219</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>1220</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16375,19 +16382,19 @@
         <v>328</v>
       </c>
       <c r="B50" s="11" t="s">
+        <v>1220</v>
+      </c>
+      <c r="C50" s="11" t="s">
         <v>1221</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>1222</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>1223</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="F50" s="11" t="s">
         <v>1224</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>1225</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16395,19 +16402,19 @@
         <v>328</v>
       </c>
       <c r="B51" s="11" t="s">
+        <v>1225</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>1226</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="D51" s="11" t="s">
         <v>1227</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="E51" s="11" t="s">
         <v>1228</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="F51" s="11" t="s">
         <v>1229</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>1230</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16415,19 +16422,19 @@
         <v>328</v>
       </c>
       <c r="B52" s="11" t="s">
+        <v>1230</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>1231</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>1232</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="E52" s="11" t="s">
         <v>1233</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="F52" s="11" t="s">
         <v>1234</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>1235</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16435,19 +16442,19 @@
         <v>328</v>
       </c>
       <c r="B53" s="11" t="s">
+        <v>1235</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>1236</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>1237</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="E53" s="11" t="s">
         <v>1238</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="F53" s="11" t="s">
         <v>1239</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>1240</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16455,19 +16462,19 @@
         <v>328</v>
       </c>
       <c r="B54" s="11" t="s">
+        <v>1240</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>1241</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="D54" s="11" t="s">
         <v>1242</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="E54" s="11" t="s">
         <v>1243</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="F54" s="11" t="s">
         <v>1244</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>1245</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16475,19 +16482,19 @@
         <v>328</v>
       </c>
       <c r="B55" s="11" t="s">
+        <v>1245</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>1246</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="D55" s="11" t="s">
         <v>1247</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="E55" s="11" t="s">
         <v>1248</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>1249</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>1250</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16495,13 +16502,13 @@
         <v>107</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>1250</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>1251</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="D56" s="11" t="s">
         <v>1252</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>1253</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16509,13 +16516,13 @@
         <v>107</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>1253</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>1254</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="D57" s="11" t="s">
         <v>1255</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>1256</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16523,13 +16530,13 @@
         <v>107</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>1256</v>
+      </c>
+      <c r="C58" s="11" t="s">
         <v>1257</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="D58" s="11" t="s">
         <v>1258</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>1259</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16537,27 +16544,27 @@
         <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>1259</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>1260</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="D59" s="11" t="s">
         <v>1261</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>1262</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B60" s="83" t="s">
+      <c r="B60" s="84" t="s">
+        <v>1262</v>
+      </c>
+      <c r="C60" s="11" t="s">
         <v>1263</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="D60" s="11" t="s">
         <v>1264</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>1265</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16565,13 +16572,13 @@
         <v>107</v>
       </c>
       <c r="B61" s="11" t="s">
+        <v>1265</v>
+      </c>
+      <c r="C61" s="11" t="s">
         <v>1266</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="D61" s="11" t="s">
         <v>1267</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>1268</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16579,13 +16586,13 @@
         <v>107</v>
       </c>
       <c r="B62" s="11" t="s">
+        <v>1268</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>1269</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="D62" s="11" t="s">
         <v>1270</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>1271</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16593,19 +16600,19 @@
         <v>107</v>
       </c>
       <c r="B63" s="11" t="s">
+        <v>1271</v>
+      </c>
+      <c r="C63" s="11" t="s">
         <v>1272</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="D63" s="2" t="s">
         <v>1273</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>1274</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>1275</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>1276</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16613,7 +16620,7 @@
         <v>328</v>
       </c>
       <c r="B64" s="66" t="s">
-        <v>1277</v>
+        <v>1276</v>
       </c>
       <c r="C64" s="66" t="s">
         <v>722</v>
@@ -16629,7 +16636,7 @@
         <v>328</v>
       </c>
       <c r="B65" s="66" t="s">
-        <v>1278</v>
+        <v>1277</v>
       </c>
       <c r="C65" s="66" t="s">
         <v>944</v>
@@ -16645,7 +16652,7 @@
         <v>328</v>
       </c>
       <c r="B66" s="66" t="s">
-        <v>1279</v>
+        <v>1278</v>
       </c>
       <c r="C66" s="66" t="s">
         <v>946</v>
@@ -16661,7 +16668,7 @@
         <v>328</v>
       </c>
       <c r="B67" s="11" t="s">
-        <v>1280</v>
+        <v>1279</v>
       </c>
       <c r="C67" s="11" t="s">
         <v>949</v>
@@ -16681,7 +16688,7 @@
         <v>429</v>
       </c>
       <c r="B68" s="66" t="s">
-        <v>1281</v>
+        <v>1280</v>
       </c>
       <c r="C68" s="11" t="s">
         <v>956</v>
@@ -16701,7 +16708,7 @@
         <v>429</v>
       </c>
       <c r="B69" s="66" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="C69" s="11" t="s">
         <v>961</v>
@@ -16721,13 +16728,13 @@
         <v>429</v>
       </c>
       <c r="B70" s="66" t="s">
+        <v>1282</v>
+      </c>
+      <c r="C70" s="11" t="s">
         <v>1283</v>
       </c>
-      <c r="C70" s="11" t="s">
+      <c r="D70" s="11" t="s">
         <v>1284</v>
-      </c>
-      <c r="D70" s="11" t="s">
-        <v>1285</v>
       </c>
       <c r="E70" s="11"/>
       <c r="F70" s="11"/>
@@ -16737,13 +16744,13 @@
         <v>429</v>
       </c>
       <c r="B71" s="66" t="s">
+        <v>1285</v>
+      </c>
+      <c r="C71" s="11" t="s">
         <v>1286</v>
       </c>
-      <c r="C71" s="11" t="s">
+      <c r="D71" s="11" t="s">
         <v>1287</v>
-      </c>
-      <c r="D71" s="11" t="s">
-        <v>1288</v>
       </c>
       <c r="E71" s="11"/>
       <c r="F71" s="11"/>
@@ -16753,13 +16760,13 @@
         <v>429</v>
       </c>
       <c r="B72" s="66" t="s">
+        <v>1288</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>1289</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="D72" s="11" t="s">
         <v>1290</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>1291</v>
       </c>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
@@ -16769,13 +16776,13 @@
         <v>429</v>
       </c>
       <c r="B73" s="11" t="s">
+        <v>1291</v>
+      </c>
+      <c r="C73" s="11" t="s">
         <v>1292</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="D73" s="11" t="s">
         <v>1293</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>1294</v>
       </c>
       <c r="E73" s="11"/>
       <c r="F73" s="11"/>
@@ -16785,13 +16792,13 @@
         <v>328</v>
       </c>
       <c r="B74" s="11" t="s">
+        <v>1294</v>
+      </c>
+      <c r="C74" s="11" t="s">
         <v>1295</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="D74" s="11" t="s">
         <v>1296</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>1297</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16799,13 +16806,13 @@
         <v>328</v>
       </c>
       <c r="B75" s="11" t="s">
+        <v>1297</v>
+      </c>
+      <c r="C75" s="11" t="s">
         <v>1298</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="D75" s="11" t="s">
         <v>1299</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>1300</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16813,13 +16820,13 @@
         <v>328</v>
       </c>
       <c r="B76" s="11" t="s">
+        <v>1300</v>
+      </c>
+      <c r="C76" s="11" t="s">
         <v>1301</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="D76" s="11" t="s">
         <v>1302</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>1303</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16827,13 +16834,13 @@
         <v>328</v>
       </c>
       <c r="B77" s="11" t="s">
+        <v>1303</v>
+      </c>
+      <c r="C77" s="11" t="s">
         <v>1304</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="D77" s="11" t="s">
         <v>1305</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>1306</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16841,7 +16848,7 @@
         <v>107</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>1307</v>
+        <v>1306</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>1005</v>
@@ -16861,7 +16868,7 @@
         <v>107</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>1308</v>
+        <v>1307</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>1009</v>
@@ -16881,7 +16888,7 @@
         <v>107</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>1309</v>
+        <v>1308</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>1013</v>
@@ -16901,7 +16908,7 @@
         <v>107</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>1310</v>
+        <v>1309</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>1017</v>
@@ -16921,7 +16928,7 @@
         <v>107</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>1311</v>
+        <v>1310</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>1021</v>
@@ -16941,19 +16948,19 @@
         <v>276</v>
       </c>
       <c r="B83" s="2" t="s">
+        <v>1311</v>
+      </c>
+      <c r="C83" s="11" t="s">
         <v>1312</v>
       </c>
-      <c r="C83" s="11" t="s">
+      <c r="D83" s="11" t="s">
         <v>1313</v>
       </c>
-      <c r="D83" s="11" t="s">
+      <c r="E83" s="11" t="s">
         <v>1314</v>
       </c>
-      <c r="E83" s="11" t="s">
+      <c r="F83" s="11" t="s">
         <v>1315</v>
-      </c>
-      <c r="F83" s="11" t="s">
-        <v>1316</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16961,19 +16968,19 @@
         <v>276</v>
       </c>
       <c r="B84" s="2" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C84" s="11" t="s">
         <v>1317</v>
       </c>
-      <c r="C84" s="11" t="s">
+      <c r="D84" s="11" t="s">
         <v>1318</v>
       </c>
-      <c r="D84" s="11" t="s">
+      <c r="E84" s="11" t="s">
         <v>1319</v>
       </c>
-      <c r="E84" s="11" t="s">
+      <c r="F84" s="11" t="s">
         <v>1320</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>1321</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16981,13 +16988,13 @@
         <v>591</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C85" s="11" t="s">
         <v>1322</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="D85" s="11" t="s">
         <v>1323</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>1324</v>
       </c>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Label: Fix some errors.
Fix the type for householdMember in the UI tests.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -784,7 +784,7 @@
   <si>
     <t xml:space="preserve">Veuillez localiser le **lieu de travail habituel** de {{nickname}}
 __Naviguez, zoomez, et cliquez sur la carte pour localiser le lieu. Une fois localisé, vous pourrez déplacer le point sur la carte pour davantage de précision.
-Vous pouvez également chercher le lieu sur la carte en utilisant le bouton "Chercher le lieu").__</t>
+Vous pouvez également chercher le lieu sur la carte en utilisant le bouton "Chercher le lieu".__</t>
   </si>
   <si>
     <t xml:space="preserve">Please locate the **usual place of work** for {{nickname}}
@@ -794,7 +794,7 @@
   <si>
     <t xml:space="preserve">Veuillez localiser votre **lieu de travail habituel**.
 __Naviguez, zoomez, et cliquez sur la carte pour localiser le lieu. Une fois localisé, vous pourrez déplacer le point sur la carte pour davantage de précision.
-Vous pouvez également chercher le lieu sur la carte en utilisant le bouton "Chercher le lieu").__</t>
+Vous pouvez également chercher le lieu sur la carte en utilisant le bouton "Chercher le lieu".__</t>
   </si>
   <si>
     <t xml:space="preserve">Please locate your **usual place of work**.
@@ -5592,11 +5592,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C23" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C32" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A23" activeCellId="0" sqref="A23"/>
-      <selection pane="bottomRight" activeCell="A33" activeCellId="0" sqref="A33"/>
+      <selection pane="bottomLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
+      <selection pane="bottomRight" activeCell="I37" activeCellId="0" sqref="I37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Questions: Change the order of some questions in the end section
Fix: #227.
Now all the green-yellow-red range questions are together, and the red-yellow-green question is alone to help the user response.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -2340,12 +2340,42 @@
     <t xml:space="preserve">householdElectricCarCountCustomValidation</t>
   </si>
   <si>
+    <t xml:space="preserve">endInterestOfTheSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">interestOfTheSurvey</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dans quelle mesure cette enquête a-t-elle été **intéressante** pour vous?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How **interesting** was this survey to you?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rangeOptionalOrValidCustomValidation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sliderNotAtAllToVeryInteresting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">endTimeSpentAnswering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">timeSpentAnswering</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Combien de **temps** pensez-vous avoir passé **à répondre** à cette enquête (**en minutes**)?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">How much **time** do you think you **spent answering** this survey (**in minutes**)?</t>
+  </si>
+  <si>
     <t xml:space="preserve">endDurationOfTheSurvey</t>
   </si>
   <si>
-    <t xml:space="preserve">Range</t>
-  </si>
-  <si>
     <t xml:space="preserve">durationOfSurvey</t>
   </si>
   <si>
@@ -2355,37 +2385,7 @@
     <t xml:space="preserve">Do you feel that the **length of the survey was too short, about right, or too long**?</t>
   </si>
   <si>
-    <t xml:space="preserve">rangeOptionalOrValidCustomValidation</t>
-  </si>
-  <si>
     <t xml:space="preserve">sliderTooShortToTooLong</t>
-  </si>
-  <si>
-    <t xml:space="preserve">endTimeSpentAnswering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">timeSpentAnswering</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Combien de **temps** pensez-vous avoir passé **à répondre** à cette enquête (**en minutes**)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How much **time** do you think you **spent answering** this survey (**in minutes**)?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">endInterestOfTheSurvey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">interestOfTheSurvey</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dans quelle mesure cette enquête a-t-elle été **intéressante** pour vous?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">How **interesting** was this survey to you?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">sliderNotAtAllToVeryInteresting</t>
   </si>
   <si>
     <t xml:space="preserve">endDifficultyOfTheSurvey</t>
@@ -4943,7 +4943,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5508,11 +5508,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="I87" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C123" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="I1" activeCellId="0" sqref="I1"/>
-      <selection pane="bottomLeft" activeCell="A87" activeCellId="0" sqref="A87"/>
-      <selection pane="bottomRight" activeCell="L95" activeCellId="0" sqref="L95"/>
+      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="bottomLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
+      <selection pane="bottomRight" activeCell="I129" activeCellId="0" sqref="I129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11602,7 +11602,7 @@
       <c r="Q127" s="36"/>
       <c r="R127" s="36"/>
       <c r="S127" s="36"/>
-      <c r="T127" s="34" t="n">
+      <c r="T127" s="34" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11650,7 +11650,7 @@
       </c>
       <c r="R128" s="36"/>
       <c r="S128" s="36"/>
-      <c r="T128" s="34" t="n">
+      <c r="T128" s="37" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11696,7 +11696,7 @@
       <c r="Q129" s="36"/>
       <c r="R129" s="36"/>
       <c r="S129" s="36"/>
-      <c r="T129" s="34" t="n">
+      <c r="T129" s="34" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11744,7 +11744,7 @@
       </c>
       <c r="R130" s="36"/>
       <c r="S130" s="36"/>
-      <c r="T130" s="34" t="n">
+      <c r="T130" s="37" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11888,7 +11888,7 @@
       <c r="Q133" s="36"/>
       <c r="R133" s="36"/>
       <c r="S133" s="36"/>
-      <c r="T133" s="34" t="n">
+      <c r="T133" s="34" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11968,7 +11968,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <autoFilter ref="A1:X1"/>
   <conditionalFormatting sqref="N135:Q135">
@@ -11994,7 +11994,7 @@
       <formula>AND($B135&lt;&gt;"Select", $B135&lt;&gt;"Checkbox", $B135&lt;&gt;"Radio",  $B135&lt;&gt;"", ROW(O135)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C136:C1048576 C62:C83 C101:C134 C1:C60">
+  <conditionalFormatting sqref="C136:C1048576 C62:C83 C1:C60 C101:C134">
     <cfRule type="containsText" priority="7" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
       <formula>NOT(ISERROR(SEARCH("FALSE",C1)))</formula>
     </cfRule>
@@ -12002,50 +12002,50 @@
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Q128">
-    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
-      <formula>AND($B1048457="Custom",  $B1048457&lt;&gt;"", ROW(Q1048457)&lt;&gt;1)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q128 Q131:Q132">
-    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
-      <formula>AND($B128&lt;&gt;"Range", $B128&lt;&gt;"", ROW(Q128)&lt;&gt;1)</formula>
+  <conditionalFormatting sqref="Q130:Q132">
+    <cfRule type="expression" priority="9" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="3">
+      <formula>AND($B130&lt;&gt;"Range", $B130&lt;&gt;"", ROW(Q130)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q131:Q132">
-    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
+    <cfRule type="expression" priority="10" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="4">
       <formula>AND(#ref!="Custom",  #ref!&lt;&gt;"", ROW(#ref!)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O120">
-    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+    <cfRule type="expression" priority="11" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
       <formula>AND($B120="Custom",  $B120&lt;&gt;"", ROW(O120)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O120">
-    <cfRule type="expression" priority="13" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="10">
+    <cfRule type="expression" priority="12" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
       <formula>AND($B120&lt;&gt;"Select", $B120&lt;&gt;"Checkbox", $B120&lt;&gt;"Radio",  $B120&lt;&gt;"", ROW(O120)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C62:C79 C101 C104:C115">
-    <cfRule type="containsText" priority="14" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
+    <cfRule type="containsText" priority="13" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
       <formula>NOT(ISERROR(SEARCH("FALSE",C62)))</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C61:C79 C84:C101 C104:C115">
-    <cfRule type="containsText" priority="16" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
+    <cfRule type="containsText" priority="15" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="FALSE" dxfId="8">
       <formula>NOT(ISERROR(SEARCH("FALSE",C61)))</formula>
     </cfRule>
-    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
+    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="9">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I112">
-    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
+    <cfRule type="expression" priority="17" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="12">
       <formula>AND($B112="Custom",  $B112&lt;&gt;"", ROW(I112)&lt;&gt;1)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Q130">
+    <cfRule type="expression" priority="18" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="11">
+      <formula>AND($B1048460="Custom",  $B1048460&lt;&gt;"", ROW(Q1048460)&lt;&gt;1)</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -15381,7 +15381,7 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="52" t="s">
-        <v>637</v>
+        <v>646</v>
       </c>
       <c r="B2" s="52" t="s">
         <v>1037</v>
@@ -15419,7 +15419,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="52" t="s">
-        <v>646</v>
+        <v>637</v>
       </c>
       <c r="B3" s="52" t="s">
         <v>1045</v>

</xml_diff>

<commit_message>
Label: Fix small typo in drivingLicenseOwnership
Fix: #204
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -630,7 +630,7 @@
   </si>
   <si>
     <t xml:space="preserve">**Driver's licence**
-__Include learner's and probationary permits, but do not include moped (motorized scooter and moped) permits.__</t>
+__Include learner's and probationary permits, but do not include moped (motorized scooter) permits.__</t>
   </si>
   <si>
     <t xml:space="preserve">yesNoDontKnow</t>
@@ -5508,11 +5508,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C123" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A123" activeCellId="0" sqref="A123"/>
-      <selection pane="bottomRight" activeCell="I129" activeCellId="0" sqref="I129"/>
+      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
+      <selection pane="bottomRight" activeCell="H31" activeCellId="0" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11602,7 +11602,7 @@
       <c r="Q127" s="36"/>
       <c r="R127" s="36"/>
       <c r="S127" s="36"/>
-      <c r="T127" s="34" t="b">
+      <c r="T127" s="37" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11696,7 +11696,7 @@
       <c r="Q129" s="36"/>
       <c r="R129" s="36"/>
       <c r="S129" s="36"/>
-      <c r="T129" s="34" t="b">
+      <c r="T129" s="37" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11888,7 +11888,7 @@
       <c r="Q133" s="36"/>
       <c r="R133" s="36"/>
       <c r="S133" s="36"/>
-      <c r="T133" s="34" t="b">
+      <c r="T133" s="37" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Label: Use of inclusive writing
Fix: #167
We did use the recommendation from the inclusive writing of 'Office québécois de la langue française'
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -494,8 +494,55 @@
     <t xml:space="preserve">workerType</t>
   </si>
   <si>
-    <t xml:space="preserve">**Travaill{{gender:eur/euse/eur·euse}}**
-__Incluant travaill{{gender:eur/euse/eur·euse}} autonome, artiste, travaill{{gender:eur/euse/eur·euse}} en congé de maladie ou parental.__</t>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">**Travaill{{gender:eur/euse/eur(euse)/eur(euse)}}**
+__Incluant travaill</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:eur/euse/eur(euse)/eur(euse)}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> autonome, artiste, travaill</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:eur/euse/eur(euse)/eur(euse)}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> en congé de maladie ou parental.__</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">**Worker**
@@ -514,7 +561,7 @@
     <t xml:space="preserve">studentType</t>
   </si>
   <si>
-    <t xml:space="preserve">**Étudiant{{gender:/e/·e}}**</t>
+    <t xml:space="preserve">**Étudiant{{gender:/e/(e)/(e)}}**</t>
   </si>
   <si>
     <t xml:space="preserve">**Student**</t>
@@ -626,7 +673,7 @@
   </si>
   <si>
     <t xml:space="preserve">**Permis de conduire**
-__Inclure les permis d’apprenti{{gender:e}} conduct{{gender:eur/rice/eur·rice}} et probatoires, mais ne pas inclure les permis de cyclomoteur/scooter.__</t>
+__Inclure les permis d’apprenti{{gender:e}} conduct{{gender:eur/rice/eur(rice)/eur(rice)}} et probatoires, mais ne pas inclure les permis de cyclomoteur/scooter.__</t>
   </si>
   <si>
     <t xml:space="preserve">**Driver's licence**
@@ -855,7 +902,7 @@
     <t xml:space="preserve">travelToWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **semaine dernière**, quand {{nickname}} s'est-{{gender:il/elle/iel/"il/elle"}} **déplacé{{gender:/e/·e}}** pour le **travail**?
+    <t xml:space="preserve">Durant la **semaine dernière**, quand {{nickname}} s'est-{{gender:il/elle/iel/il(elle)}} **déplacé{{gender:/e/(e)/(e)}}** pour le **travail**?
 __Pour se rendre au travail ou toute autre raison concernant le travail.__</t>
   </si>
   <si>
@@ -863,7 +910,7 @@
 __To get to or for any other reason concerning work.__</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **semaine dernière**, quand vous êtes-vous **déplacé{{gender:/e/·e}}** pour le **travail**?</t>
+    <t xml:space="preserve">Durant la **semaine dernière**, quand vous êtes-vous **déplacé{{gender:/e/(e)/(e)}}** pour le **travail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did you **travel** for **work**?
@@ -882,7 +929,7 @@
     <t xml:space="preserve">remoteWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **semaine dernière**, quand {{nickname}} a-t-{{gender:il/elle/iel/"il/elle"}} fait du **télétravail**?</t>
+    <t xml:space="preserve">Durant la **semaine dernière**, quand {{nickname}} a-t-{{gender:il/elle/iel/il(elle)}} fait du **télétravail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did {{nickname}} **work remotely**?</t>
@@ -983,7 +1030,7 @@
     <t xml:space="preserve">personDidTrips</t>
   </si>
   <si>
-    <t xml:space="preserve">Est-ce que {{nickname}} s'est déplac{{gender:é/ée/é.e}} le {{assignedDate}}?
+    <t xml:space="preserve">Est-ce que {{nickname}} s'est déplac{{gender:é/ée/é(e)/é(e)}} le {{assignedDate}}?
 __Inclure tous les déplacements, qu'ils soient pour des motifs personnels (achats, sorties, loisirs, etc.), pour le travail, ou pour aller chercher ou reconduire quelqu'un.__</t>
   </si>
   <si>
@@ -991,8 +1038,36 @@
 __Include all trips, whether for personal reasons (shopping, outings, leisure, etc.), for work, or to pick up or drop someone off.__</t>
   </si>
   <si>
-    <t xml:space="preserve">Vous êtes-vous déplac{{gender:é/ée/é.e}} le {{assignedDate}}?
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Vous êtes-vous déplac</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:é/ée/é(e)/é(e)}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> le {{assignedDate}}?
 __Inclure tous les déplacements, qu'ils soient pour des motifs personnels (achats, sorties, loisirs, etc.), pour le travail, ou pour aller chercher ou reconduire quelqu'un.__</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Did you make any trips on {{assignedDate}}?
@@ -1002,7 +1077,35 @@
     <t xml:space="preserve">personDidTripsConfirm</t>
   </si>
   <si>
-    <t xml:space="preserve">Vous avez déjà déclaré des déplacements. Confirmez-vous qu'ils sont erronés et que {{nickname}} ne s'est pas déplac{{gender:é/ée/é.e}} le {{formattedTripsDate}}?</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Vous avez déjà déclaré des déplacements. Confirmez-vous qu'ils sont erronés et que {{nickname}} ne s'est pas déplac</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:é/ée/é(e)/é(e)}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> le {{formattedTripsDate}}?</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">You already declared trip. Do you confirm they are erroneous and that {{nickname}} did not make any trips on {{formattedTripsDate}}?</t>
@@ -1020,10 +1123,57 @@
     <t xml:space="preserve">didTripsIntro</t>
   </si>
   <si>
-    <t xml:space="preserve">Nous allons vous demander d'indiquer les lieux où {{nickname}} est all{{gender:é/ée/é.e}} le {{assignedDate}} (inclure les lieux visités jusqu'à 4:00 le lendemain matin)
-&lt;span class="_green"&gt;- **Inclure même les petits arrêts** (station-service, garderie/école, dépanneur ou tout lieu où {{nickname}} est all{{gender:é/ée/é.e}} chercher ou reconduire quelqu'un).
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nous allons vous demander d'indiquer les lieux où {{nickname}} est all{{gender:é/ée/é(e)/é(e)}} le {{assignedDate}} (inclure les lieux visités jusqu'à 4:00 le lendemain matin)
+&lt;span class="_green"&gt;- **Inclure même les petits arrêts** (station-service, garderie/école, dépanneur ou tout lieu où {{nickname}} est all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:é/ée/é(e)/é(e)}} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">chercher ou reconduire quelqu'un).
 - **Inclure tous les lieux** peu importe les modes de transport utilisés pour s'y rendre (marche, vélo, voiture, transport collectif, taxi, avion, bateau, etc.).&lt;/span&gt;
-&lt;span class="_red"&gt;- **Ne pas inclure les lieux de transfert** en cours de déplacement (arrêts de bus, gares, terminus, lieux de stationnement, etc.) sauf si {{nickname}} est all{{gender:é/ée/é.e}} reconduire ou chercher quelqu'un à cet endroit.&lt;/span&gt;</t>
+&lt;span class="_red"&gt;- **Ne pas inclure les lieux de transfert** en cours de déplacement (arrêts de bus, gares, terminus, lieux de stationnement, etc.) sauf si {{nickname}} est all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:é/ée/é(e)/é(e)}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> reconduire ou chercher quelqu'un à cet endroit.&lt;/span&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Please specify the **places {{nickname}} went on {{assignedDate}}** (include all places visited until 4 AM the following morning)
@@ -1032,10 +1182,57 @@
 &lt;span class="_red"&gt;- **Do not include transfer locations** (bus stops, train stations, terminals, parking lots, etc.) unless {{nickname}} went there to drop someone off or pick someone up.&lt;/span&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">Nous allons vous demander d'indiquer les **lieux où vous êtes all{{gender:é/ée/é.e}} le {{assignedDate}}** (inclure les lieux visités jusqu'à 4:00 le lendemain matin)
-&lt;span class="_green"&gt;- **Inclure même les petits arrêts** (station-service, garderie/école, dépanneur ou tout lieu où vous êtes all{{gender:é/ée/é.e}} chercher ou reconduire quelqu'un).
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nous allons vous demander d'indiquer les **lieux où vous êtes all{{gender:é/ée/é(e)/é(e)}} le {{assignedDate}}** (inclure les lieux visités jusqu'à 4:00 le lendemain matin)
+&lt;span class="_green"&gt;- **Inclure même les petits arrêts** (station-service, garderie/école, dépanneur ou tout lieu où vous êtes all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:é/ée/é(e)/é(e)}} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">chercher ou reconduire quelqu'un).
 - **Inclure tous les lieux** peu importe les modes de transport utilisés pour s'y rendre (marche, vélo, voiture, transport collectif, taxi, avion, bateau, etc.).&lt;/span&gt;
-&lt;span class="_red"&gt;- **Ne pas inclure les lieux de transfert** en cours de déplacement (arrêts de bus, gares, terminus, lieux de stationnement, etc.) sauf si vous êtes all{{gender:é/ée/é.e}} reconduire ou chercher quelqu'un à cet endroit.&lt;/span&gt;</t>
+&lt;span class="_red"&gt;- **Ne pas inclure les lieux de transfert** en cours de déplacement (arrêts de bus, gares, terminus, lieux de stationnement, etc.) sauf si vous êtes all</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:é/ée/é(e)/é(e)}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> reconduire ou chercher quelqu'un à cet endroit.&lt;/span&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Please specify the **places you went on {{assignedDate}}** (include all places visited until 4 AM the following morning)
@@ -1051,15 +1248,43 @@
   </si>
   <si>
     <t xml:space="preserve">Est-ce que {{nickname}} a **commencé sa journée au domicile** ({{address}})?
-__Répondre 'Non' uniquement si {{nickname}} n'a pas dormi au domicile (nuit du {{dayOne}} au {{dayTwo}}), ou y est rentré{{gender:/e/(-e)}} après 4h du matin (par ex.: travail de nuit).__</t>
+__Répondre 'Non' uniquement si {{nickname}} n'a pas dormi au domicile (nuit du {{dayOne}} au {{dayTwo}}), ou y est rentré{{gender:/e/(e)/(e)}} après 4h du matin (par ex.: travail de nuit).__</t>
   </si>
   <si>
     <t xml:space="preserve">Did {{nickname}} **start their day at home** ({{address}})?
 __Answer 'No' only if {{nickname}} did not sleep at home (nuit du {{dayOne}} au {{dayTwo}}) or came home after 4 AM (ex: overnight work shift).__</t>
   </si>
   <si>
-    <t xml:space="preserve">Avez-vous **commencé votre journée au domicile** ({{address}})?
-__Répondre 'Non' uniquement si vous n'avez pas dormi au domicile (nuit du {{dayOne}} au {{dayTwo}}), ou y êtes rentré{{gender:/e/(-e)}} après 4h du matin (par ex.: travail de nuit).__</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Avez-vous **commencé votre journée au domicile** ({{address}})?
+__Répondre 'Non' uniquement si vous n'avez pas dormi au domicile (nuit du {{dayOne}} au {{dayTwo}}), ou y êtes rentré</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:/e/(e)/(e)}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> après 4h du matin (par ex.: travail de nuit).__</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Did you **start your day at home** ({{address}})?
@@ -1120,16 +1345,72 @@
     <t xml:space="preserve">personVisitedPlacesTitle</t>
   </si>
   <si>
-    <t xml:space="preserve">Lieux où {{nickname}} est all{{gender:é/ée/é.e}} le {{assignedDate}}:
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lieux où {{nickname}} est allé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:/e/(e)/(e)}}</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> le {{assignedDate}}:
 L'ordre chronologique doit être respecté.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Places {{nickname}} went on {{assignedDate}}:
 Chronological order must be respected (i.e. sequence matters).</t>
   </si>
   <si>
-    <t xml:space="preserve">Lieux où vous êtes all{{gender:é/ée/é.e}} le {{assignedDate}}:
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Lieux où vous êtes allé</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">{{gender:/e/(e)/(e)}} </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">le {{assignedDate}}:
 L'ordre chronologique doit être respecté.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Places you went on {{assignedDate}}:
@@ -1205,10 +1486,10 @@
     <t xml:space="preserve">onTheRoadArrivalType</t>
   </si>
   <si>
-    <t xml:space="preserve">À quel endroit {{nickname}} a-t-{{gender :il/elle/iel/"il/elle"}} terminé ses déplacements sur la route?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Where did {{nickname}} end {{gender:his/her/their}} work trip on the road?</t>
+    <t xml:space="preserve">À quel endroit {{nickname}} a-t-{{gender :il/elle/iel/il(elle)}} terminé ses déplacements sur la route?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Where did {{nickname}} end {{gender:his/her/their/his (her)}} work trip on the road?</t>
   </si>
   <si>
     <t xml:space="preserve">À quel endroit avez-vous terminé vos déplacements sur la route?</t>
@@ -1298,10 +1579,10 @@
     <t xml:space="preserve">_previousPreviousDepartureTime</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/"il/elle"}} quitté le lieu précédent ({{visitedPlaceDescription}}) avant de se rendre à son lieu habituel de travail?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At what time did {{nickname}} leave the previous location ({{visitedPlaceDescription}}) before going to {{gender:his/her/their}} usual work place?</t>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/il(elle)}} quitté le lieu précédent ({{visitedPlaceDescription}}) avant de se rendre à son lieu habituel de travail?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At what time did {{nickname}} leave the previous location ({{visitedPlaceDescription}}) before going to {{gender:his/her/their/his (her)}} usual work place?</t>
   </si>
   <si>
     <t xml:space="preserve">À quelle heure avez-vous quitté le lieu précédent ({{visitedPlaceDescription}}) avant de vous rendre à votre lieu habituel de travail?</t>
@@ -4488,7 +4769,7 @@
     <numFmt numFmtId="166" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4573,6 +4854,12 @@
     </font>
     <font>
       <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="9"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -4607,6 +4894,12 @@
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
@@ -4887,11 +5180,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4907,11 +5200,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4919,11 +5212,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4931,7 +5224,7 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4939,7 +5232,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4947,27 +5240,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4976,6 +5253,22 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false" readingOrder="1"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -4987,11 +5280,11 @@
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="21" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5007,11 +5300,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5047,11 +5340,11 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5063,7 +5356,7 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5095,19 +5388,19 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5508,11 +5801,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C55" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A25" activeCellId="0" sqref="A25"/>
-      <selection pane="bottomRight" activeCell="H31" activeCellId="0" sqref="H31"/>
+      <selection pane="bottomLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
+      <selection pane="bottomRight" activeCell="I59" activeCellId="0" sqref="I59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6787,7 +7080,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
         <v>143</v>
       </c>
@@ -8442,7 +8735,7 @@
         <v>329</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="29.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" customFormat="false" ht="76.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="11" t="s">
         <v>330</v>
       </c>
@@ -8707,7 +9000,7 @@
       <c r="W64" s="36"/>
       <c r="X64" s="36"/>
     </row>
-    <row r="65" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" customFormat="false" ht="61.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="11" t="s">
         <v>356</v>
       </c>
@@ -8949,7 +9242,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="40.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A70" s="11" t="s">
         <v>385</v>
       </c>
@@ -15551,7 +15844,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J53" activeCellId="0" sqref="J53"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Label: Change schoolType label depending of the person age
Fix: #225
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2280" uniqueCount="1324">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="1330">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -579,10 +579,10 @@
     <t xml:space="preserve">schoolType</t>
   </si>
   <si>
-    <t xml:space="preserve">**Établissement d'enseignement / type d'école**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**School type**</t>
+    <t xml:space="preserve">**Établissement d'enseignement**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Educational institution**</t>
   </si>
   <si>
     <t xml:space="preserve">ifAge15OrLessConditional</t>
@@ -4558,6 +4558,24 @@
     <t xml:space="preserve">You must be at least 16 years old to respond to this survey.</t>
   </si>
   <si>
+    <t xml:space="preserve">schoolTypeLessThan4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Type de garde**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Childcare type**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">schoolTypeBetween4And15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Type d'école**</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**School type**</t>
+  </si>
+  <si>
     <t xml:space="preserve">onTheRoadArrivalTypeHome</t>
   </si>
   <si>
@@ -4769,7 +4787,7 @@
     <numFmt numFmtId="166" formatCode="&quot;VRAI&quot;;&quot;VRAI&quot;;&quot;FAUX&quot;"/>
     <numFmt numFmtId="167" formatCode="@"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -4967,6 +4985,12 @@
       <family val="0"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -5063,7 +5087,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="88">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5405,6 +5429,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5801,11 +5833,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C55" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A55" activeCellId="0" sqref="A55"/>
-      <selection pane="bottomRight" activeCell="I59" activeCellId="0" sqref="I59"/>
+      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="I26" activeCellId="0" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15844,8 +15876,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A58" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J53" activeCellId="0" sqref="J53"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G65" activeCellId="0" sqref="G65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16845,49 +16877,49 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="36" t="s">
-        <v>328</v>
-      </c>
-      <c r="B64" s="68" t="s">
+      <c r="A64" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B64" s="86" t="s">
         <v>1276</v>
       </c>
-      <c r="C64" s="68" t="s">
-        <v>722</v>
-      </c>
-      <c r="D64" s="68" t="s">
-        <v>723</v>
-      </c>
-      <c r="E64" s="68"/>
-      <c r="F64" s="68"/>
+      <c r="C64" s="86" t="s">
+        <v>1277</v>
+      </c>
+      <c r="D64" s="87" t="s">
+        <v>1278</v>
+      </c>
+      <c r="E64" s="2"/>
+      <c r="F64" s="2"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="36" t="s">
-        <v>328</v>
-      </c>
-      <c r="B65" s="68" t="s">
-        <v>1277</v>
-      </c>
-      <c r="C65" s="68" t="s">
-        <v>944</v>
-      </c>
-      <c r="D65" s="68" t="s">
-        <v>945</v>
-      </c>
-      <c r="E65" s="68"/>
-      <c r="F65" s="68"/>
+      <c r="A65" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B65" s="86" t="s">
+        <v>1279</v>
+      </c>
+      <c r="C65" s="86" t="s">
+        <v>1280</v>
+      </c>
+      <c r="D65" s="87" t="s">
+        <v>1281</v>
+      </c>
+      <c r="E65" s="2"/>
+      <c r="F65" s="2"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="36" t="s">
         <v>328</v>
       </c>
       <c r="B66" s="68" t="s">
-        <v>1278</v>
+        <v>1282</v>
       </c>
       <c r="C66" s="68" t="s">
-        <v>946</v>
+        <v>722</v>
       </c>
       <c r="D66" s="68" t="s">
-        <v>947</v>
+        <v>723</v>
       </c>
       <c r="E66" s="68"/>
       <c r="F66" s="68"/>
@@ -16896,60 +16928,52 @@
       <c r="A67" s="36" t="s">
         <v>328</v>
       </c>
-      <c r="B67" s="11" t="s">
-        <v>1279</v>
-      </c>
-      <c r="C67" s="11" t="s">
-        <v>949</v>
-      </c>
-      <c r="D67" s="11" t="s">
-        <v>950</v>
-      </c>
-      <c r="E67" s="11" t="s">
-        <v>951</v>
-      </c>
-      <c r="F67" s="11" t="s">
-        <v>952</v>
-      </c>
+      <c r="B67" s="68" t="s">
+        <v>1283</v>
+      </c>
+      <c r="C67" s="68" t="s">
+        <v>944</v>
+      </c>
+      <c r="D67" s="68" t="s">
+        <v>945</v>
+      </c>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="36" t="s">
-        <v>429</v>
+        <v>328</v>
       </c>
       <c r="B68" s="68" t="s">
-        <v>1280</v>
-      </c>
-      <c r="C68" s="11" t="s">
-        <v>956</v>
-      </c>
-      <c r="D68" s="11" t="s">
-        <v>957</v>
-      </c>
-      <c r="E68" s="11" t="s">
-        <v>958</v>
-      </c>
-      <c r="F68" s="11" t="s">
-        <v>959</v>
-      </c>
+        <v>1284</v>
+      </c>
+      <c r="C68" s="68" t="s">
+        <v>946</v>
+      </c>
+      <c r="D68" s="68" t="s">
+        <v>947</v>
+      </c>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="36" t="s">
-        <v>429</v>
-      </c>
-      <c r="B69" s="68" t="s">
-        <v>1281</v>
+        <v>328</v>
+      </c>
+      <c r="B69" s="11" t="s">
+        <v>1285</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>961</v>
+        <v>949</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>962</v>
+        <v>950</v>
       </c>
       <c r="E69" s="11" t="s">
-        <v>963</v>
+        <v>951</v>
       </c>
       <c r="F69" s="11" t="s">
-        <v>964</v>
+        <v>952</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16957,32 +16981,40 @@
         <v>429</v>
       </c>
       <c r="B70" s="68" t="s">
-        <v>1282</v>
+        <v>1286</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>1283</v>
+        <v>956</v>
       </c>
       <c r="D70" s="11" t="s">
-        <v>1284</v>
-      </c>
-      <c r="E70" s="11"/>
-      <c r="F70" s="11"/>
+        <v>957</v>
+      </c>
+      <c r="E70" s="11" t="s">
+        <v>958</v>
+      </c>
+      <c r="F70" s="11" t="s">
+        <v>959</v>
+      </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="36" t="s">
         <v>429</v>
       </c>
       <c r="B71" s="68" t="s">
-        <v>1285</v>
+        <v>1287</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>1286</v>
+        <v>961</v>
       </c>
       <c r="D71" s="11" t="s">
-        <v>1287</v>
-      </c>
-      <c r="E71" s="11"/>
-      <c r="F71" s="11"/>
+        <v>962</v>
+      </c>
+      <c r="E71" s="11" t="s">
+        <v>963</v>
+      </c>
+      <c r="F71" s="11" t="s">
+        <v>964</v>
+      </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="36" t="s">
@@ -17004,7 +17036,7 @@
       <c r="A73" s="36" t="s">
         <v>429</v>
       </c>
-      <c r="B73" s="11" t="s">
+      <c r="B73" s="68" t="s">
         <v>1291</v>
       </c>
       <c r="C73" s="11" t="s">
@@ -17017,10 +17049,10 @@
       <c r="F73" s="11"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="2" t="s">
-        <v>328</v>
-      </c>
-      <c r="B74" s="11" t="s">
+      <c r="A74" s="36" t="s">
+        <v>429</v>
+      </c>
+      <c r="B74" s="68" t="s">
         <v>1294</v>
       </c>
       <c r="C74" s="11" t="s">
@@ -17029,10 +17061,12 @@
       <c r="D74" s="11" t="s">
         <v>1296</v>
       </c>
+      <c r="E74" s="11"/>
+      <c r="F74" s="11"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="2" t="s">
-        <v>328</v>
+      <c r="A75" s="36" t="s">
+        <v>429</v>
       </c>
       <c r="B75" s="11" t="s">
         <v>1297</v>
@@ -17043,6 +17077,8 @@
       <c r="D75" s="11" t="s">
         <v>1299</v>
       </c>
+      <c r="E75" s="11"/>
+      <c r="F75" s="11"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="2" t="s">
@@ -17074,82 +17110,70 @@
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B78" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="B78" s="11" t="s">
         <v>1306</v>
       </c>
-      <c r="C78" s="1" t="s">
-        <v>1005</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>1006</v>
-      </c>
-      <c r="E78" s="1" t="s">
-        <v>1007</v>
-      </c>
-      <c r="F78" s="1" t="s">
-        <v>1008</v>
+      <c r="C78" s="11" t="s">
+        <v>1307</v>
+      </c>
+      <c r="D78" s="11" t="s">
+        <v>1308</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B79" s="1" t="s">
-        <v>1307</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>1009</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>1010</v>
-      </c>
-      <c r="E79" s="1" t="s">
-        <v>1011</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>1012</v>
+        <v>328</v>
+      </c>
+      <c r="B79" s="11" t="s">
+        <v>1309</v>
+      </c>
+      <c r="C79" s="11" t="s">
+        <v>1310</v>
+      </c>
+      <c r="D79" s="11" t="s">
+        <v>1311</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B80" s="26" t="s">
-        <v>1308</v>
+      <c r="B80" s="1" t="s">
+        <v>1312</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1013</v>
+        <v>1005</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>1014</v>
+        <v>1006</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>1015</v>
+        <v>1007</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>1016</v>
+        <v>1008</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B81" s="26" t="s">
-        <v>1309</v>
+      <c r="B81" s="1" t="s">
+        <v>1313</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1017</v>
+        <v>1009</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>1018</v>
+        <v>1010</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>1019</v>
+        <v>1011</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>1020</v>
+        <v>1012</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17157,77 +17181,115 @@
         <v>107</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>1310</v>
+        <v>1314</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1021</v>
+        <v>1013</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>1022</v>
+        <v>1014</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>1023</v>
+        <v>1015</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>1024</v>
+        <v>1016</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>1311</v>
-      </c>
-      <c r="C83" s="11" t="s">
-        <v>1312</v>
-      </c>
-      <c r="D83" s="11" t="s">
-        <v>1313</v>
-      </c>
-      <c r="E83" s="11" t="s">
-        <v>1314</v>
-      </c>
-      <c r="F83" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B83" s="26" t="s">
         <v>1315</v>
+      </c>
+      <c r="C83" s="1" t="s">
+        <v>1017</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>1018</v>
+      </c>
+      <c r="E83" s="1" t="s">
+        <v>1019</v>
+      </c>
+      <c r="F83" s="1" t="s">
+        <v>1020</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="2" t="s">
-        <v>276</v>
-      </c>
-      <c r="B84" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B84" s="26" t="s">
         <v>1316</v>
       </c>
-      <c r="C84" s="11" t="s">
-        <v>1317</v>
-      </c>
-      <c r="D84" s="11" t="s">
-        <v>1318</v>
-      </c>
-      <c r="E84" s="11" t="s">
-        <v>1319</v>
-      </c>
-      <c r="F84" s="11" t="s">
-        <v>1320</v>
+      <c r="C84" s="1" t="s">
+        <v>1021</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>1022</v>
+      </c>
+      <c r="E84" s="1" t="s">
+        <v>1023</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>1024</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B85" s="2" t="s">
+        <v>1317</v>
+      </c>
+      <c r="C85" s="11" t="s">
+        <v>1318</v>
+      </c>
+      <c r="D85" s="11" t="s">
+        <v>1319</v>
+      </c>
+      <c r="E85" s="11" t="s">
+        <v>1320</v>
+      </c>
+      <c r="F85" s="11" t="s">
+        <v>1321</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="2" t="s">
+        <v>276</v>
+      </c>
+      <c r="B86" s="2" t="s">
+        <v>1322</v>
+      </c>
+      <c r="C86" s="11" t="s">
+        <v>1323</v>
+      </c>
+      <c r="D86" s="11" t="s">
+        <v>1324</v>
+      </c>
+      <c r="E86" s="11" t="s">
+        <v>1325</v>
+      </c>
+      <c r="F86" s="11" t="s">
+        <v>1326</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="2" t="s">
         <v>591</v>
       </c>
-      <c r="B85" s="2" t="s">
-        <v>1321</v>
-      </c>
-      <c r="C85" s="11" t="s">
-        <v>1322</v>
-      </c>
-      <c r="D85" s="11" t="s">
-        <v>1323</v>
-      </c>
-    </row>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+      <c r="B87" s="2" t="s">
+        <v>1327</v>
+      </c>
+      <c r="C87" s="11" t="s">
+        <v>1328</v>
+      </c>
+      <c r="D87" s="11" t="s">
+        <v>1329</v>
+      </c>
+    </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
Label: Fix more gender label
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -502,7 +502,7 @@
         <family val="0"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">**Travaill{{gender:eur/euse/eur(euse)/eur(euse)}}**
+      <t xml:space="preserve">**Travaill{{gender:eur/euse/eur(-se)/eur(-se)}}**
 __Incluant travaill</t>
     </r>
     <r>
@@ -512,7 +512,7 @@
         <rFont val="Calibri"/>
         <family val="0"/>
       </rPr>
-      <t xml:space="preserve">{{gender:eur/euse/eur(euse)/eur(euse)}}</t>
+      <t xml:space="preserve">{{gender:eur/euse/eur(-se)/eur(-se)}}</t>
     </r>
     <r>
       <rPr>
@@ -531,7 +531,7 @@
         <rFont val="Calibri"/>
         <family val="0"/>
       </rPr>
-      <t xml:space="preserve">{{gender:eur/euse/eur(euse)/eur(euse)}}</t>
+      <t xml:space="preserve">{{gender:eur/euse/eur(-se)/eur(-se)}}</t>
     </r>
     <r>
       <rPr>
@@ -673,7 +673,7 @@
   </si>
   <si>
     <t xml:space="preserve">**Permis de conduire**
-__Inclure les permis d’apprenti{{gender:e}} conduct{{gender:eur/rice/eur(rice)/eur(rice)}} et probatoires, mais ne pas inclure les permis de cyclomoteur/scooter.__</t>
+__Inclure les permis d’apprenti{{gender:e}} conduct{{gender:eur/rice/eur(-rice)/eur(-rice)}} et probatoires, mais ne pas inclure les permis de cyclomoteur/scooter.__</t>
   </si>
   <si>
     <t xml:space="preserve">**Driver's licence**
@@ -902,7 +902,7 @@
     <t xml:space="preserve">travelToWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **semaine dernière**, quand {{nickname}} s'est-{{gender:il/elle/iel/il(elle)}} **déplacé{{gender:/e/(e)/(e)}}** pour le **travail**?
+    <t xml:space="preserve">Durant la **semaine dernière**, quand {{nickname}} s'est-{{gender:il/elle/iel/il(-elle)}} **déplacé{{gender:/e/(e)/(e)}}** pour le **travail**?
 __Pour se rendre au travail ou toute autre raison concernant le travail.__</t>
   </si>
   <si>
@@ -929,7 +929,7 @@
     <t xml:space="preserve">remoteWorkDays</t>
   </si>
   <si>
-    <t xml:space="preserve">Durant la **semaine dernière**, quand {{nickname}} a-t-{{gender:il/elle/iel/il(elle)}} fait du **télétravail**?</t>
+    <t xml:space="preserve">Durant la **semaine dernière**, quand {{nickname}} a-t-{{gender:il/elle/iel/il(-elle)}} fait du **télétravail**?</t>
   </si>
   <si>
     <t xml:space="preserve">During the **last week**, when did {{nickname}} **work remotely**?</t>
@@ -1486,7 +1486,7 @@
     <t xml:space="preserve">onTheRoadArrivalType</t>
   </si>
   <si>
-    <t xml:space="preserve">À quel endroit {{nickname}} a-t-{{gender :il/elle/iel/il(elle)}} terminé ses déplacements sur la route?</t>
+    <t xml:space="preserve">À quel endroit {{nickname}} a-t-{{gender:il/elle/iel/il(-elle)}} terminé ses déplacements sur la route?</t>
   </si>
   <si>
     <t xml:space="preserve">Where did {{nickname}} end {{gender:his/her/their/his (her)}} work trip on the road?</t>
@@ -1579,7 +1579,7 @@
     <t xml:space="preserve">_previousPreviousDepartureTime</t>
   </si>
   <si>
-    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/il(elle)}} quitté le lieu précédent ({{visitedPlaceDescription}}) avant de se rendre à son lieu habituel de travail?</t>
+    <t xml:space="preserve">À quelle heure {{nickname}} a-t-{{gender :il/elle/iel/il(-elle)}} quitté le lieu précédent ({{visitedPlaceDescription}}) avant de se rendre à son lieu habituel de travail?</t>
   </si>
   <si>
     <t xml:space="preserve">At what time did {{nickname}} leave the previous location ({{visitedPlaceDescription}}) before going to {{gender:his/her/their/his (her)}} usual work place?</t>
@@ -1612,13 +1612,13 @@
     <t xml:space="preserve">arrivalTime</t>
   </si>
   <si>
-    <t xml:space="preserve">{{nickname}} est arriv{{gender :é/ée/é.e}} {{atPlace}} à:</t>
+    <t xml:space="preserve">{{nickname}} est arriv{{gender :é/ée/é(e)/é(e)}} {{atPlace}} à:</t>
   </si>
   <si>
     <t xml:space="preserve">{{nickname}} arrived {{atPlace}} at:</t>
   </si>
   <si>
-    <t xml:space="preserve">Vous êtes arriv{{gender :é/ée/é.e}} {{atPlace}} à:</t>
+    <t xml:space="preserve">Vous êtes arriv{{gender :é/ée/é(e)/é(e)}} {{atPlace}} à:</t>
   </si>
   <si>
     <t xml:space="preserve">You arrived {{atPlace}} at:</t>
@@ -1634,7 +1634,7 @@
   </si>
   <si>
     <t xml:space="preserve">Après avoir été {{atPlace}}, {{nickname}} est…
-__Si {{nickname}} a quitté le lieu après 4h du matin le lendemain, merci de considérer pour l'enquête qu'{{gender :il/elle/iel/"il/elle"}} y est rest{{gender :é/ée/é.e}} jusqu'au lendemain et de sélectionner la réponse adaptée.__</t>
+__Si {{nickname}} a quitté le lieu après 4h du matin le lendemain, merci de considérer pour l'enquête qu'{{gender :il/elle/iel/il(-elle)}} y est rest{{gender :é/ée/é(e)/é(e)}} jusqu'au lendemain et de sélectionner la réponse adaptée.__</t>
   </si>
   <si>
     <t xml:space="preserve">After being {{atPlace}}, {{nickname}}…
@@ -1642,7 +1642,7 @@
   </si>
   <si>
     <t xml:space="preserve">Après avoir été {{atPlace}}, vous êtes…
-__Si vous avez quitté le lieu après 4h du matin le lendemain, merci de considérer pour l'enquête que vous y êtes rest{{gender :é/ée/é.e}} jusqu'au lendemain et de sélectionner la réponse adaptée.__</t>
+__Si vous avez quitté le lieu après 4h du matin le lendemain, merci de considérer pour l'enquête que vous y êtes rest{{gender :é/ée/é(e)/é(e)}} jusqu'au lendemain et de sélectionner la réponse adaptée.__</t>
   </si>
   <si>
     <t xml:space="preserve">After being {{atPlace}}, you…
@@ -1793,7 +1793,7 @@
     <t xml:space="preserve">howToBus</t>
   </si>
   <si>
-    <t xml:space="preserve">Comment est-ce que {{nickname}} s'est rend{{gender :u/ue/u.e}} à l'arrêt/station de transport collectif?
+    <t xml:space="preserve">Comment est-ce que {{nickname}} s'est rend{{gender :u/ue/u(e)/u(e)}} à l'arrêt/station de transport collectif?
 __Si le mode de déplacement n'est pas présent, créer un premier mode de transport avant le transport collectif.__</t>
   </si>
   <si>
@@ -1801,7 +1801,7 @@
 __If the mode used is not present, create a first mode before the transit mode.__</t>
   </si>
   <si>
-    <t xml:space="preserve">Comment vous êtes-vous rend{{gender :u/ue/u.e}} à l'arrêt/station de transport collectif?
+    <t xml:space="preserve">Comment vous êtes-vous rend{{gender :u/ue/u(e)/u(e)}} à l'arrêt/station de transport collectif?
 __Si le mode de déplacement n'est pas présent, créer un premier mode de transport avant le transport collectif.__</t>
   </si>
   <si>
@@ -5837,7 +5837,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="I26" activeCellId="0" sqref="I26"/>
+      <selection pane="bottomRight" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7112,7 +7112,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
         <v>143</v>
       </c>
@@ -9458,7 +9458,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="74" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="74" customFormat="false" ht="135.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A74" s="11" t="s">
         <v>403</v>
       </c>
@@ -10172,7 +10172,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="71.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="120.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="11" t="s">
         <v>455</v>
       </c>

</xml_diff>

<commit_message>
Conditional: Fix typo on conditional of hasPreferNotToAnswerToSexAssignedConditional
Fix: #309
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="1330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="1329">
   <si>
     <t xml:space="preserve">questionName</t>
   </si>
@@ -2495,7 +2495,7 @@
     <t xml:space="preserve">${currentPerson}.sexAssignedAtBirth</t>
   </si>
   <si>
-    <t xml:space="preserve">preferNoToAnswer</t>
+    <t xml:space="preserve">preferNotToAnswer</t>
   </si>
   <si>
     <t xml:space="preserve">ifAge3to5Conditional</t>
@@ -2751,9 +2751,6 @@
   </si>
   <si>
     <t xml:space="preserve">I don't know</t>
-  </si>
-  <si>
-    <t xml:space="preserve">preferNotToAnswer</t>
   </si>
   <si>
     <t xml:space="preserve">Je préfère ne pas répondre</t>
@@ -5521,12 +5518,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
-      <selection pane="bottomRight" activeCell="H25" activeCellId="0" sqref="H25"/>
+      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="bottomRight" activeCell="O17" activeCellId="0" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12080,8 +12077,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H15" activeCellId="0" sqref="H15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13266,8 +13263,8 @@
   </sheetPr>
   <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G35" activeCellId="0" sqref="G35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13401,16 +13398,16 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="74" t="s">
+        <v>682</v>
+      </c>
+      <c r="B7" s="74" t="s">
+        <v>682</v>
+      </c>
+      <c r="C7" s="74" t="s">
         <v>768</v>
       </c>
-      <c r="B7" s="74" t="s">
-        <v>768</v>
-      </c>
-      <c r="C7" s="74" t="s">
+      <c r="D7" s="74" t="s">
         <v>769</v>
-      </c>
-      <c r="D7" s="74" t="s">
-        <v>770</v>
       </c>
       <c r="E7" s="74"/>
       <c r="F7" s="74"/>
@@ -13512,7 +13509,7 @@
       <c r="E14" s="74"/>
       <c r="F14" s="74"/>
       <c r="G14" s="74" t="s">
-        <v>768</v>
+        <v>682</v>
       </c>
       <c r="H14" s="74"/>
       <c r="I14" s="71"/>
@@ -13537,13 +13534,13 @@
         <v>556</v>
       </c>
       <c r="B16" s="74" t="s">
+        <v>770</v>
+      </c>
+      <c r="C16" s="74" t="s">
         <v>771</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="D16" s="74" t="s">
         <v>772</v>
-      </c>
-      <c r="D16" s="74" t="s">
-        <v>773</v>
       </c>
       <c r="E16" s="74"/>
       <c r="F16" s="74"/>
@@ -13570,13 +13567,13 @@
         <v>133</v>
       </c>
       <c r="B18" s="74" t="s">
+        <v>773</v>
+      </c>
+      <c r="C18" s="74" t="s">
         <v>774</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="D18" s="74" t="s">
         <v>775</v>
-      </c>
-      <c r="D18" s="74" t="s">
-        <v>776</v>
       </c>
       <c r="E18" s="74"/>
       <c r="F18" s="74"/>
@@ -13588,13 +13585,13 @@
         <v>133</v>
       </c>
       <c r="B19" s="74" t="s">
+        <v>776</v>
+      </c>
+      <c r="C19" s="74" t="s">
         <v>777</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="D19" s="74" t="s">
         <v>778</v>
-      </c>
-      <c r="D19" s="74" t="s">
-        <v>779</v>
       </c>
       <c r="E19" s="74"/>
       <c r="F19" s="74"/>
@@ -13611,7 +13608,7 @@
       <c r="E20" s="74"/>
       <c r="F20" s="74"/>
       <c r="G20" s="74" t="s">
-        <v>768</v>
+        <v>682</v>
       </c>
       <c r="H20" s="74"/>
     </row>
@@ -13620,13 +13617,13 @@
         <v>139</v>
       </c>
       <c r="B21" s="74" t="s">
+        <v>773</v>
+      </c>
+      <c r="C21" s="74" t="s">
         <v>774</v>
       </c>
-      <c r="C21" s="74" t="s">
-        <v>775</v>
-      </c>
       <c r="D21" s="74" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="E21" s="74"/>
       <c r="F21" s="74"/>
@@ -13638,13 +13635,13 @@
         <v>139</v>
       </c>
       <c r="B22" s="74" t="s">
+        <v>776</v>
+      </c>
+      <c r="C22" s="74" t="s">
         <v>777</v>
       </c>
-      <c r="C22" s="74" t="s">
-        <v>778</v>
-      </c>
       <c r="D22" s="74" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="E22" s="74"/>
       <c r="F22" s="74"/>
@@ -13659,10 +13656,10 @@
         <v>141</v>
       </c>
       <c r="C23" s="74" t="s">
+        <v>781</v>
+      </c>
+      <c r="D23" s="74" t="s">
         <v>782</v>
-      </c>
-      <c r="D23" s="74" t="s">
-        <v>783</v>
       </c>
       <c r="E23" s="74"/>
       <c r="F23" s="74"/>
@@ -13679,7 +13676,7 @@
       <c r="E24" s="74"/>
       <c r="F24" s="74"/>
       <c r="G24" s="74" t="s">
-        <v>768</v>
+        <v>682</v>
       </c>
       <c r="H24" s="74"/>
     </row>
@@ -13691,10 +13688,10 @@
         <v>712</v>
       </c>
       <c r="C25" s="74" t="s">
+        <v>783</v>
+      </c>
+      <c r="D25" s="74" t="s">
         <v>784</v>
-      </c>
-      <c r="D25" s="74" t="s">
-        <v>785</v>
       </c>
       <c r="E25" s="74"/>
       <c r="F25" s="74"/>
@@ -13709,10 +13706,10 @@
         <v>713</v>
       </c>
       <c r="C26" s="74" t="s">
+        <v>785</v>
+      </c>
+      <c r="D26" s="74" t="s">
         <v>786</v>
-      </c>
-      <c r="D26" s="74" t="s">
-        <v>787</v>
       </c>
       <c r="E26" s="74"/>
       <c r="F26" s="74"/>
@@ -13741,10 +13738,10 @@
         <v>712</v>
       </c>
       <c r="C28" s="74" t="s">
+        <v>787</v>
+      </c>
+      <c r="D28" s="74" t="s">
         <v>788</v>
-      </c>
-      <c r="D28" s="74" t="s">
-        <v>789</v>
       </c>
       <c r="E28" s="74"/>
       <c r="F28" s="74"/>
@@ -13759,10 +13756,10 @@
         <v>713</v>
       </c>
       <c r="C29" s="74" t="s">
+        <v>789</v>
+      </c>
+      <c r="D29" s="74" t="s">
         <v>790</v>
-      </c>
-      <c r="D29" s="74" t="s">
-        <v>791</v>
       </c>
       <c r="E29" s="74"/>
       <c r="F29" s="74"/>
@@ -13788,13 +13785,13 @@
         <v>156</v>
       </c>
       <c r="B31" s="74" t="s">
+        <v>791</v>
+      </c>
+      <c r="C31" s="74" t="s">
         <v>792</v>
       </c>
-      <c r="C31" s="74" t="s">
+      <c r="D31" s="74" t="s">
         <v>793</v>
-      </c>
-      <c r="D31" s="74" t="s">
-        <v>794</v>
       </c>
       <c r="E31" s="74"/>
       <c r="F31" s="74"/>
@@ -13808,13 +13805,13 @@
         <v>156</v>
       </c>
       <c r="B32" s="74" t="s">
+        <v>794</v>
+      </c>
+      <c r="C32" s="74" t="s">
         <v>795</v>
       </c>
-      <c r="C32" s="74" t="s">
+      <c r="D32" s="74" t="s">
         <v>796</v>
-      </c>
-      <c r="D32" s="74" t="s">
-        <v>797</v>
       </c>
       <c r="E32" s="74"/>
       <c r="F32" s="74"/>
@@ -13828,13 +13825,13 @@
         <v>156</v>
       </c>
       <c r="B33" s="74" t="s">
+        <v>797</v>
+      </c>
+      <c r="C33" s="74" t="s">
         <v>798</v>
       </c>
-      <c r="C33" s="74" t="s">
+      <c r="D33" s="74" t="s">
         <v>799</v>
-      </c>
-      <c r="D33" s="74" t="s">
-        <v>800</v>
       </c>
       <c r="E33" s="74"/>
       <c r="F33" s="74"/>
@@ -13848,13 +13845,13 @@
         <v>156</v>
       </c>
       <c r="B34" s="74" t="s">
+        <v>800</v>
+      </c>
+      <c r="C34" s="74" t="s">
         <v>801</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="D34" s="74" t="s">
         <v>802</v>
-      </c>
-      <c r="D34" s="74" t="s">
-        <v>803</v>
       </c>
       <c r="E34" s="74"/>
       <c r="F34" s="74"/>
@@ -13868,13 +13865,13 @@
         <v>156</v>
       </c>
       <c r="B35" s="74" t="s">
+        <v>803</v>
+      </c>
+      <c r="C35" s="74" t="s">
         <v>804</v>
       </c>
-      <c r="C35" s="74" t="s">
+      <c r="D35" s="74" t="s">
         <v>805</v>
-      </c>
-      <c r="D35" s="74" t="s">
-        <v>806</v>
       </c>
       <c r="E35" s="74"/>
       <c r="F35" s="74"/>
@@ -13888,13 +13885,13 @@
         <v>156</v>
       </c>
       <c r="B36" s="74" t="s">
+        <v>806</v>
+      </c>
+      <c r="C36" s="74" t="s">
         <v>807</v>
       </c>
-      <c r="C36" s="74" t="s">
+      <c r="D36" s="74" t="s">
         <v>808</v>
-      </c>
-      <c r="D36" s="74" t="s">
-        <v>809</v>
       </c>
       <c r="E36" s="74"/>
       <c r="F36" s="74"/>
@@ -13925,17 +13922,17 @@
         <v>697</v>
       </c>
       <c r="C38" s="74" t="s">
+        <v>809</v>
+      </c>
+      <c r="D38" s="74" t="s">
         <v>810</v>
-      </c>
-      <c r="D38" s="74" t="s">
-        <v>811</v>
       </c>
       <c r="E38" s="74"/>
       <c r="F38" s="74"/>
       <c r="G38" s="74"/>
       <c r="H38" s="74"/>
       <c r="I38" s="71" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13946,17 +13943,17 @@
         <v>698</v>
       </c>
       <c r="C39" s="74" t="s">
+        <v>812</v>
+      </c>
+      <c r="D39" s="74" t="s">
         <v>813</v>
-      </c>
-      <c r="D39" s="74" t="s">
-        <v>814</v>
       </c>
       <c r="E39" s="74"/>
       <c r="F39" s="74"/>
       <c r="G39" s="74"/>
       <c r="H39" s="74"/>
       <c r="I39" s="71" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13967,17 +13964,17 @@
         <v>699</v>
       </c>
       <c r="C40" s="74" t="s">
+        <v>814</v>
+      </c>
+      <c r="D40" s="74" t="s">
         <v>815</v>
-      </c>
-      <c r="D40" s="74" t="s">
-        <v>816</v>
       </c>
       <c r="E40" s="74"/>
       <c r="F40" s="74"/>
       <c r="G40" s="74"/>
       <c r="H40" s="74"/>
       <c r="I40" s="71" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -13988,17 +13985,17 @@
         <v>700</v>
       </c>
       <c r="C41" s="74" t="s">
+        <v>816</v>
+      </c>
+      <c r="D41" s="74" t="s">
         <v>817</v>
-      </c>
-      <c r="D41" s="74" t="s">
-        <v>818</v>
       </c>
       <c r="E41" s="74"/>
       <c r="F41" s="74"/>
       <c r="G41" s="74"/>
       <c r="H41" s="74"/>
       <c r="I41" s="71" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14009,17 +14006,17 @@
         <v>701</v>
       </c>
       <c r="C42" s="74" t="s">
+        <v>818</v>
+      </c>
+      <c r="D42" s="74" t="s">
         <v>819</v>
-      </c>
-      <c r="D42" s="74" t="s">
-        <v>820</v>
       </c>
       <c r="E42" s="74"/>
       <c r="F42" s="74"/>
       <c r="G42" s="74"/>
       <c r="H42" s="74"/>
       <c r="I42" s="71" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14027,13 +14024,13 @@
         <v>162</v>
       </c>
       <c r="B43" s="74" t="s">
+        <v>820</v>
+      </c>
+      <c r="C43" s="74" t="s">
         <v>821</v>
       </c>
-      <c r="C43" s="74" t="s">
+      <c r="D43" s="74" t="s">
         <v>822</v>
-      </c>
-      <c r="D43" s="74" t="s">
-        <v>823</v>
       </c>
       <c r="E43" s="74"/>
       <c r="F43" s="74"/>
@@ -14047,13 +14044,13 @@
         <v>162</v>
       </c>
       <c r="B44" s="74" t="s">
+        <v>803</v>
+      </c>
+      <c r="C44" s="74" t="s">
         <v>804</v>
       </c>
-      <c r="C44" s="74" t="s">
+      <c r="D44" s="74" t="s">
         <v>805</v>
-      </c>
-      <c r="D44" s="74" t="s">
-        <v>806</v>
       </c>
       <c r="E44" s="74"/>
       <c r="F44" s="74"/>
@@ -14065,13 +14062,13 @@
         <v>162</v>
       </c>
       <c r="B45" s="74" t="s">
+        <v>823</v>
+      </c>
+      <c r="C45" s="74" t="s">
         <v>824</v>
       </c>
-      <c r="C45" s="74" t="s">
+      <c r="D45" s="74" t="s">
         <v>825</v>
-      </c>
-      <c r="D45" s="74" t="s">
-        <v>826</v>
       </c>
       <c r="E45" s="74"/>
       <c r="F45" s="74"/>
@@ -14086,10 +14083,10 @@
         <v>710</v>
       </c>
       <c r="C46" s="74" t="s">
+        <v>826</v>
+      </c>
+      <c r="D46" s="74" t="s">
         <v>827</v>
-      </c>
-      <c r="D46" s="74" t="s">
-        <v>828</v>
       </c>
       <c r="E46" s="74"/>
       <c r="F46" s="74"/>
@@ -14101,13 +14098,13 @@
         <v>162</v>
       </c>
       <c r="B47" s="74" t="s">
+        <v>828</v>
+      </c>
+      <c r="C47" s="74" t="s">
         <v>829</v>
       </c>
-      <c r="C47" s="74" t="s">
+      <c r="D47" s="74" t="s">
         <v>830</v>
-      </c>
-      <c r="D47" s="74" t="s">
-        <v>831</v>
       </c>
       <c r="E47" s="74"/>
       <c r="F47" s="74"/>
@@ -14119,13 +14116,13 @@
         <v>162</v>
       </c>
       <c r="B48" s="74" t="s">
+        <v>831</v>
+      </c>
+      <c r="C48" s="74" t="s">
         <v>832</v>
       </c>
-      <c r="C48" s="74" t="s">
+      <c r="D48" s="74" t="s">
         <v>833</v>
-      </c>
-      <c r="D48" s="74" t="s">
-        <v>834</v>
       </c>
       <c r="E48" s="74"/>
       <c r="F48" s="74"/>
@@ -14155,13 +14152,13 @@
         <v>162</v>
       </c>
       <c r="B50" s="74" t="s">
-        <v>768</v>
+        <v>682</v>
       </c>
       <c r="C50" s="74" t="s">
+        <v>834</v>
+      </c>
+      <c r="D50" s="74" t="s">
         <v>835</v>
-      </c>
-      <c r="D50" s="74" t="s">
-        <v>836</v>
       </c>
       <c r="E50" s="74"/>
       <c r="F50" s="74"/>
@@ -14187,13 +14184,13 @@
         <v>198</v>
       </c>
       <c r="B52" s="74" t="s">
+        <v>836</v>
+      </c>
+      <c r="C52" s="74" t="s">
         <v>837</v>
       </c>
-      <c r="C52" s="74" t="s">
+      <c r="D52" s="74" t="s">
         <v>838</v>
-      </c>
-      <c r="D52" s="74" t="s">
-        <v>839</v>
       </c>
       <c r="E52" s="74"/>
       <c r="F52" s="74"/>
@@ -14205,13 +14202,13 @@
         <v>198</v>
       </c>
       <c r="B53" s="74" t="s">
+        <v>839</v>
+      </c>
+      <c r="C53" s="74" t="s">
         <v>840</v>
       </c>
-      <c r="C53" s="74" t="s">
+      <c r="D53" s="74" t="s">
         <v>841</v>
-      </c>
-      <c r="D53" s="74" t="s">
-        <v>842</v>
       </c>
       <c r="E53" s="74"/>
       <c r="F53" s="74"/>
@@ -14240,10 +14237,10 @@
         <v>703</v>
       </c>
       <c r="C55" s="74" t="s">
+        <v>842</v>
+      </c>
+      <c r="D55" s="74" t="s">
         <v>843</v>
-      </c>
-      <c r="D55" s="74" t="s">
-        <v>844</v>
       </c>
       <c r="E55" s="74"/>
       <c r="F55" s="74"/>
@@ -14258,10 +14255,10 @@
         <v>704</v>
       </c>
       <c r="C56" s="74" t="s">
+        <v>844</v>
+      </c>
+      <c r="D56" s="74" t="s">
         <v>845</v>
-      </c>
-      <c r="D56" s="74" t="s">
-        <v>846</v>
       </c>
       <c r="E56" s="74"/>
       <c r="F56" s="74"/>
@@ -14276,10 +14273,10 @@
         <v>705</v>
       </c>
       <c r="C57" s="74" t="s">
+        <v>846</v>
+      </c>
+      <c r="D57" s="74" t="s">
         <v>847</v>
-      </c>
-      <c r="D57" s="74" t="s">
-        <v>848</v>
       </c>
       <c r="E57" s="74"/>
       <c r="F57" s="74"/>
@@ -14291,13 +14288,13 @@
         <v>206</v>
       </c>
       <c r="B58" s="74" t="s">
+        <v>848</v>
+      </c>
+      <c r="C58" s="74" t="s">
         <v>849</v>
       </c>
-      <c r="C58" s="74" t="s">
+      <c r="D58" s="74" t="s">
         <v>850</v>
-      </c>
-      <c r="D58" s="74" t="s">
-        <v>851</v>
       </c>
       <c r="E58" s="74"/>
       <c r="F58" s="74"/>
@@ -14312,10 +14309,10 @@
         <v>709</v>
       </c>
       <c r="C59" s="74" t="s">
+        <v>851</v>
+      </c>
+      <c r="D59" s="74" t="s">
         <v>852</v>
-      </c>
-      <c r="D59" s="74" t="s">
-        <v>853</v>
       </c>
       <c r="E59" s="74"/>
       <c r="F59" s="74"/>
@@ -14330,10 +14327,10 @@
         <v>703</v>
       </c>
       <c r="C60" s="71" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="D60" s="71" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14344,10 +14341,10 @@
         <v>704</v>
       </c>
       <c r="C61" s="71" t="s">
+        <v>854</v>
+      </c>
+      <c r="D61" s="71" t="s">
         <v>855</v>
-      </c>
-      <c r="D61" s="71" t="s">
-        <v>856</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14358,10 +14355,10 @@
         <v>709</v>
       </c>
       <c r="C62" s="71" t="s">
+        <v>856</v>
+      </c>
+      <c r="D62" s="71" t="s">
         <v>857</v>
-      </c>
-      <c r="D62" s="71" t="s">
-        <v>858</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14369,13 +14366,13 @@
         <v>566</v>
       </c>
       <c r="B63" s="71" t="s">
+        <v>858</v>
+      </c>
+      <c r="C63" s="71" t="s">
         <v>859</v>
       </c>
-      <c r="C63" s="71" t="s">
+      <c r="D63" s="71" t="s">
         <v>860</v>
-      </c>
-      <c r="D63" s="71" t="s">
-        <v>861</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14383,13 +14380,13 @@
         <v>566</v>
       </c>
       <c r="B64" s="71" t="s">
+        <v>861</v>
+      </c>
+      <c r="C64" s="71" t="s">
         <v>862</v>
       </c>
-      <c r="C64" s="71" t="s">
+      <c r="D64" s="71" t="s">
         <v>863</v>
-      </c>
-      <c r="D64" s="71" t="s">
-        <v>864</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14397,13 +14394,13 @@
         <v>566</v>
       </c>
       <c r="B65" s="71" t="s">
+        <v>864</v>
+      </c>
+      <c r="C65" s="71" t="s">
         <v>865</v>
       </c>
-      <c r="C65" s="71" t="s">
+      <c r="D65" s="71" t="s">
         <v>866</v>
-      </c>
-      <c r="D65" s="71" t="s">
-        <v>867</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14411,13 +14408,13 @@
         <v>566</v>
       </c>
       <c r="B66" s="71" t="s">
+        <v>867</v>
+      </c>
+      <c r="C66" s="71" t="s">
         <v>868</v>
       </c>
-      <c r="C66" s="71" t="s">
+      <c r="D66" s="71" t="s">
         <v>869</v>
-      </c>
-      <c r="D66" s="71" t="s">
-        <v>870</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14425,13 +14422,13 @@
         <v>600</v>
       </c>
       <c r="B67" s="71" t="s">
+        <v>870</v>
+      </c>
+      <c r="C67" s="71" t="s">
         <v>871</v>
       </c>
-      <c r="C67" s="71" t="s">
+      <c r="D67" s="71" t="s">
         <v>872</v>
-      </c>
-      <c r="D67" s="71" t="s">
-        <v>873</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14439,13 +14436,13 @@
         <v>600</v>
       </c>
       <c r="B68" s="76" t="s">
+        <v>873</v>
+      </c>
+      <c r="C68" s="76" t="s">
         <v>874</v>
       </c>
-      <c r="C68" s="76" t="s">
+      <c r="D68" s="76" t="s">
         <v>875</v>
-      </c>
-      <c r="D68" s="76" t="s">
-        <v>876</v>
       </c>
       <c r="E68" s="76"/>
       <c r="F68" s="76"/>
@@ -14455,13 +14452,13 @@
         <v>600</v>
       </c>
       <c r="B69" s="76" t="s">
+        <v>876</v>
+      </c>
+      <c r="C69" s="76" t="s">
         <v>877</v>
       </c>
-      <c r="C69" s="76" t="s">
+      <c r="D69" s="76" t="s">
         <v>878</v>
-      </c>
-      <c r="D69" s="76" t="s">
-        <v>879</v>
       </c>
       <c r="E69" s="76"/>
       <c r="F69" s="76"/>
@@ -14471,13 +14468,13 @@
         <v>600</v>
       </c>
       <c r="B70" s="76" t="s">
+        <v>879</v>
+      </c>
+      <c r="C70" s="76" t="s">
         <v>880</v>
       </c>
-      <c r="C70" s="76" t="s">
+      <c r="D70" s="76" t="s">
         <v>881</v>
-      </c>
-      <c r="D70" s="76" t="s">
-        <v>882</v>
       </c>
       <c r="E70" s="76"/>
       <c r="F70" s="76"/>
@@ -14487,13 +14484,13 @@
         <v>600</v>
       </c>
       <c r="B71" s="76" t="s">
+        <v>882</v>
+      </c>
+      <c r="C71" s="76" t="s">
         <v>883</v>
       </c>
-      <c r="C71" s="76" t="s">
+      <c r="D71" s="76" t="s">
         <v>884</v>
-      </c>
-      <c r="D71" s="76" t="s">
-        <v>885</v>
       </c>
       <c r="E71" s="76"/>
       <c r="F71" s="76"/>
@@ -14503,13 +14500,13 @@
         <v>600</v>
       </c>
       <c r="B72" s="76" t="s">
+        <v>885</v>
+      </c>
+      <c r="C72" s="76" t="s">
         <v>886</v>
       </c>
-      <c r="C72" s="76" t="s">
+      <c r="D72" s="76" t="s">
         <v>887</v>
-      </c>
-      <c r="D72" s="76" t="s">
-        <v>888</v>
       </c>
       <c r="E72" s="76"/>
       <c r="F72" s="76"/>
@@ -14519,13 +14516,13 @@
         <v>600</v>
       </c>
       <c r="B73" s="76" t="s">
+        <v>888</v>
+      </c>
+      <c r="C73" s="76" t="s">
         <v>889</v>
       </c>
-      <c r="C73" s="76" t="s">
+      <c r="D73" s="76" t="s">
         <v>890</v>
-      </c>
-      <c r="D73" s="76" t="s">
-        <v>891</v>
       </c>
       <c r="E73" s="76"/>
       <c r="F73" s="76"/>
@@ -14535,13 +14532,13 @@
         <v>600</v>
       </c>
       <c r="B74" s="76" t="s">
+        <v>891</v>
+      </c>
+      <c r="C74" s="76" t="s">
         <v>892</v>
       </c>
-      <c r="C74" s="76" t="s">
+      <c r="D74" s="76" t="s">
         <v>893</v>
-      </c>
-      <c r="D74" s="76" t="s">
-        <v>894</v>
       </c>
       <c r="E74" s="76"/>
       <c r="F74" s="76"/>
@@ -14551,13 +14548,13 @@
         <v>600</v>
       </c>
       <c r="B75" s="76" t="s">
+        <v>894</v>
+      </c>
+      <c r="C75" s="76" t="s">
         <v>895</v>
       </c>
-      <c r="C75" s="76" t="s">
+      <c r="D75" s="76" t="s">
         <v>896</v>
-      </c>
-      <c r="D75" s="76" t="s">
-        <v>897</v>
       </c>
       <c r="E75" s="76"/>
       <c r="F75" s="76"/>
@@ -14567,13 +14564,13 @@
         <v>600</v>
       </c>
       <c r="B76" s="76" t="s">
+        <v>897</v>
+      </c>
+      <c r="C76" s="76" t="s">
         <v>898</v>
       </c>
-      <c r="C76" s="76" t="s">
+      <c r="D76" s="76" t="s">
         <v>899</v>
-      </c>
-      <c r="D76" s="76" t="s">
-        <v>900</v>
       </c>
       <c r="E76" s="76"/>
       <c r="F76" s="76"/>
@@ -14583,13 +14580,13 @@
         <v>600</v>
       </c>
       <c r="B77" s="76" t="s">
+        <v>900</v>
+      </c>
+      <c r="C77" s="76" t="s">
         <v>901</v>
       </c>
-      <c r="C77" s="76" t="s">
+      <c r="D77" s="76" t="s">
         <v>902</v>
-      </c>
-      <c r="D77" s="76" t="s">
-        <v>903</v>
       </c>
       <c r="E77" s="76"/>
       <c r="F77" s="76"/>
@@ -14599,13 +14596,13 @@
         <v>600</v>
       </c>
       <c r="B78" s="76" t="s">
+        <v>903</v>
+      </c>
+      <c r="C78" s="76" t="s">
         <v>904</v>
       </c>
-      <c r="C78" s="76" t="s">
+      <c r="D78" s="76" t="s">
         <v>905</v>
-      </c>
-      <c r="D78" s="76" t="s">
-        <v>906</v>
       </c>
       <c r="E78" s="76"/>
       <c r="F78" s="76"/>
@@ -14615,13 +14612,13 @@
         <v>600</v>
       </c>
       <c r="B79" s="71" t="s">
+        <v>906</v>
+      </c>
+      <c r="C79" s="71" t="s">
         <v>907</v>
       </c>
-      <c r="C79" s="71" t="s">
+      <c r="D79" s="71" t="s">
         <v>908</v>
-      </c>
-      <c r="D79" s="71" t="s">
-        <v>909</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14643,13 +14640,13 @@
         <v>600</v>
       </c>
       <c r="B81" s="71" t="s">
+        <v>909</v>
+      </c>
+      <c r="C81" s="71" t="s">
+        <v>768</v>
+      </c>
+      <c r="D81" s="71" t="s">
         <v>910</v>
-      </c>
-      <c r="C81" s="71" t="s">
-        <v>769</v>
-      </c>
-      <c r="D81" s="71" t="s">
-        <v>911</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14657,13 +14654,13 @@
         <v>595</v>
       </c>
       <c r="B82" s="76" t="s">
+        <v>911</v>
+      </c>
+      <c r="C82" s="71" t="s">
         <v>912</v>
       </c>
-      <c r="C82" s="71" t="s">
+      <c r="D82" s="71" t="s">
         <v>913</v>
-      </c>
-      <c r="D82" s="71" t="s">
-        <v>914</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14671,13 +14668,13 @@
         <v>595</v>
       </c>
       <c r="B83" s="71" t="s">
+        <v>914</v>
+      </c>
+      <c r="C83" s="71" t="s">
         <v>915</v>
       </c>
-      <c r="C83" s="71" t="s">
+      <c r="D83" s="71" t="s">
         <v>916</v>
-      </c>
-      <c r="D83" s="71" t="s">
-        <v>917</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14699,13 +14696,13 @@
         <v>595</v>
       </c>
       <c r="B85" s="71" t="s">
+        <v>682</v>
+      </c>
+      <c r="C85" s="76" t="s">
         <v>768</v>
       </c>
-      <c r="C85" s="76" t="s">
-        <v>769</v>
-      </c>
       <c r="D85" s="76" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="E85" s="76"/>
       <c r="F85" s="76"/>
@@ -14715,13 +14712,13 @@
         <v>320</v>
       </c>
       <c r="B86" s="71" t="s">
+        <v>917</v>
+      </c>
+      <c r="C86" s="79" t="s">
         <v>918</v>
       </c>
-      <c r="C86" s="79" t="s">
+      <c r="D86" s="71" t="s">
         <v>919</v>
-      </c>
-      <c r="D86" s="71" t="s">
-        <v>920</v>
       </c>
       <c r="H86" s="76" t="s">
         <v>693</v>
@@ -14732,13 +14729,13 @@
         <v>320</v>
       </c>
       <c r="B87" s="71" t="s">
+        <v>920</v>
+      </c>
+      <c r="C87" s="76" t="s">
         <v>921</v>
       </c>
-      <c r="C87" s="76" t="s">
+      <c r="D87" s="79" t="s">
         <v>922</v>
-      </c>
-      <c r="D87" s="79" t="s">
-        <v>923</v>
       </c>
       <c r="E87" s="79"/>
       <c r="F87" s="79"/>
@@ -14751,13 +14748,13 @@
         <v>320</v>
       </c>
       <c r="B88" s="71" t="s">
+        <v>923</v>
+      </c>
+      <c r="C88" s="76" t="s">
         <v>924</v>
       </c>
-      <c r="C88" s="76" t="s">
+      <c r="D88" s="71" t="s">
         <v>925</v>
-      </c>
-      <c r="D88" s="71" t="s">
-        <v>926</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -14765,13 +14762,13 @@
         <v>320</v>
       </c>
       <c r="B89" s="71" t="s">
+        <v>926</v>
+      </c>
+      <c r="C89" s="76" t="s">
         <v>927</v>
       </c>
-      <c r="C89" s="76" t="s">
+      <c r="D89" s="76" t="s">
         <v>928</v>
-      </c>
-      <c r="D89" s="76" t="s">
-        <v>929</v>
       </c>
       <c r="E89" s="76"/>
       <c r="F89" s="76"/>
@@ -14781,13 +14778,13 @@
         <v>320</v>
       </c>
       <c r="B90" s="71" t="s">
+        <v>929</v>
+      </c>
+      <c r="C90" s="76" t="s">
         <v>930</v>
       </c>
-      <c r="C90" s="76" t="s">
+      <c r="D90" s="76" t="s">
         <v>931</v>
-      </c>
-      <c r="D90" s="76" t="s">
-        <v>932</v>
       </c>
       <c r="E90" s="76"/>
       <c r="F90" s="76"/>
@@ -14797,13 +14794,13 @@
         <v>320</v>
       </c>
       <c r="B91" s="71" t="s">
+        <v>932</v>
+      </c>
+      <c r="C91" s="76" t="s">
         <v>933</v>
       </c>
-      <c r="C91" s="76" t="s">
+      <c r="D91" s="76" t="s">
         <v>934</v>
-      </c>
-      <c r="D91" s="76" t="s">
-        <v>935</v>
       </c>
       <c r="E91" s="76"/>
       <c r="F91" s="76"/>
@@ -14816,13 +14813,13 @@
         <v>320</v>
       </c>
       <c r="B92" s="71" t="s">
+        <v>935</v>
+      </c>
+      <c r="C92" s="76" t="s">
         <v>936</v>
       </c>
-      <c r="C92" s="76" t="s">
+      <c r="D92" s="76" t="s">
         <v>937</v>
-      </c>
-      <c r="D92" s="76" t="s">
-        <v>938</v>
       </c>
       <c r="E92" s="76"/>
       <c r="F92" s="76"/>
@@ -14832,13 +14829,13 @@
         <v>320</v>
       </c>
       <c r="B93" s="71" t="s">
+        <v>938</v>
+      </c>
+      <c r="C93" s="76" t="s">
         <v>939</v>
       </c>
-      <c r="C93" s="76" t="s">
+      <c r="D93" s="76" t="s">
         <v>940</v>
-      </c>
-      <c r="D93" s="76" t="s">
-        <v>941</v>
       </c>
       <c r="E93" s="76"/>
       <c r="F93" s="76"/>
@@ -14862,7 +14859,7 @@
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A95" s="78" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B95" s="71" t="s">
         <v>27</v>
@@ -14876,16 +14873,16 @@
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A96" s="78" t="s">
+        <v>941</v>
+      </c>
+      <c r="B96" s="71" t="s">
         <v>942</v>
       </c>
-      <c r="B96" s="71" t="s">
+      <c r="C96" s="71" t="s">
         <v>943</v>
       </c>
-      <c r="C96" s="71" t="s">
+      <c r="D96" s="71" t="s">
         <v>944</v>
-      </c>
-      <c r="D96" s="71" t="s">
-        <v>945</v>
       </c>
       <c r="H96" s="71" t="s">
         <v>708</v>
@@ -14893,84 +14890,84 @@
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A97" s="78" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B97" s="71" t="s">
         <v>161</v>
       </c>
       <c r="C97" s="71" t="s">
+        <v>945</v>
+      </c>
+      <c r="D97" s="71" t="s">
         <v>946</v>
-      </c>
-      <c r="D97" s="71" t="s">
-        <v>947</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A98" s="78" t="s">
-        <v>942</v>
+        <v>941</v>
       </c>
       <c r="B98" s="76" t="s">
+        <v>947</v>
+      </c>
+      <c r="C98" s="76" t="s">
         <v>948</v>
       </c>
-      <c r="C98" s="76" t="s">
+      <c r="D98" s="76" t="s">
         <v>949</v>
       </c>
-      <c r="D98" s="76" t="s">
+      <c r="E98" s="76" t="s">
         <v>950</v>
       </c>
-      <c r="E98" s="76" t="s">
+      <c r="F98" s="76" t="s">
         <v>951</v>
       </c>
-      <c r="F98" s="76" t="s">
+      <c r="H98" s="71" t="s">
         <v>952</v>
-      </c>
-      <c r="H98" s="71" t="s">
-        <v>953</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A99" s="78" t="s">
+        <v>953</v>
+      </c>
+      <c r="B99" s="71" t="s">
         <v>954</v>
       </c>
-      <c r="B99" s="71" t="s">
+      <c r="C99" s="76" t="s">
         <v>955</v>
       </c>
-      <c r="C99" s="76" t="s">
+      <c r="D99" s="76" t="s">
         <v>956</v>
       </c>
-      <c r="D99" s="76" t="s">
+      <c r="E99" s="76" t="s">
         <v>957</v>
       </c>
-      <c r="E99" s="76" t="s">
+      <c r="F99" s="76" t="s">
         <v>958</v>
-      </c>
-      <c r="F99" s="76" t="s">
-        <v>959</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A100" s="78" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B100" s="71" t="s">
+        <v>959</v>
+      </c>
+      <c r="C100" s="76" t="s">
         <v>960</v>
       </c>
-      <c r="C100" s="76" t="s">
+      <c r="D100" s="76" t="s">
         <v>961</v>
       </c>
-      <c r="D100" s="76" t="s">
+      <c r="E100" s="76" t="s">
         <v>962</v>
       </c>
-      <c r="E100" s="76" t="s">
+      <c r="F100" s="76" t="s">
         <v>963</v>
-      </c>
-      <c r="F100" s="76" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A101" s="78" t="s">
-        <v>954</v>
+        <v>953</v>
       </c>
       <c r="B101" s="71" t="s">
         <v>757</v>
@@ -14987,13 +14984,13 @@
         <v>524</v>
       </c>
       <c r="B102" s="76" t="s">
+        <v>964</v>
+      </c>
+      <c r="C102" s="76" t="s">
         <v>965</v>
       </c>
-      <c r="C102" s="76" t="s">
+      <c r="D102" s="76" t="s">
         <v>966</v>
-      </c>
-      <c r="D102" s="76" t="s">
-        <v>967</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15001,13 +14998,13 @@
         <v>524</v>
       </c>
       <c r="B103" s="76" t="s">
+        <v>967</v>
+      </c>
+      <c r="C103" s="76" t="s">
         <v>968</v>
       </c>
-      <c r="C103" s="76" t="s">
+      <c r="D103" s="76" t="s">
         <v>969</v>
-      </c>
-      <c r="D103" s="76" t="s">
-        <v>970</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15015,13 +15012,13 @@
         <v>524</v>
       </c>
       <c r="B104" s="76" t="s">
+        <v>970</v>
+      </c>
+      <c r="C104" s="76" t="s">
         <v>971</v>
       </c>
-      <c r="C104" s="76" t="s">
+      <c r="D104" s="76" t="s">
         <v>972</v>
-      </c>
-      <c r="D104" s="76" t="s">
-        <v>973</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15029,13 +15026,13 @@
         <v>524</v>
       </c>
       <c r="B105" s="76" t="s">
+        <v>973</v>
+      </c>
+      <c r="C105" s="76" t="s">
         <v>974</v>
       </c>
-      <c r="C105" s="76" t="s">
+      <c r="D105" s="76" t="s">
         <v>975</v>
-      </c>
-      <c r="D105" s="76" t="s">
-        <v>976</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15059,13 +15056,13 @@
         <v>539</v>
       </c>
       <c r="B108" s="76" t="s">
+        <v>976</v>
+      </c>
+      <c r="C108" s="76" t="s">
         <v>977</v>
       </c>
-      <c r="C108" s="76" t="s">
+      <c r="D108" s="76" t="s">
         <v>978</v>
-      </c>
-      <c r="D108" s="76" t="s">
-        <v>979</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15073,13 +15070,13 @@
         <v>539</v>
       </c>
       <c r="B109" s="76" t="s">
+        <v>979</v>
+      </c>
+      <c r="C109" s="76" t="s">
         <v>980</v>
       </c>
-      <c r="C109" s="76" t="s">
+      <c r="D109" s="76" t="s">
         <v>981</v>
-      </c>
-      <c r="D109" s="76" t="s">
-        <v>982</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15087,13 +15084,13 @@
         <v>539</v>
       </c>
       <c r="B110" s="76" t="s">
+        <v>970</v>
+      </c>
+      <c r="C110" s="76" t="s">
         <v>971</v>
       </c>
-      <c r="C110" s="76" t="s">
+      <c r="D110" s="76" t="s">
         <v>972</v>
-      </c>
-      <c r="D110" s="76" t="s">
-        <v>973</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15101,13 +15098,13 @@
         <v>539</v>
       </c>
       <c r="B111" s="76" t="s">
+        <v>982</v>
+      </c>
+      <c r="C111" s="76" t="s">
         <v>983</v>
       </c>
-      <c r="C111" s="76" t="s">
+      <c r="D111" s="76" t="s">
         <v>984</v>
-      </c>
-      <c r="D111" s="76" t="s">
-        <v>985</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15131,13 +15128,13 @@
         <v>175</v>
       </c>
       <c r="B114" s="76" t="s">
+        <v>985</v>
+      </c>
+      <c r="C114" s="71" t="s">
         <v>986</v>
       </c>
-      <c r="C114" s="71" t="s">
+      <c r="D114" s="71" t="s">
         <v>987</v>
-      </c>
-      <c r="D114" s="71" t="s">
-        <v>988</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15145,13 +15142,13 @@
         <v>175</v>
       </c>
       <c r="B115" s="71" t="s">
+        <v>988</v>
+      </c>
+      <c r="C115" s="71" t="s">
         <v>989</v>
       </c>
-      <c r="C115" s="71" t="s">
+      <c r="D115" s="71" t="s">
         <v>990</v>
-      </c>
-      <c r="D115" s="71" t="s">
-        <v>991</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15159,13 +15156,13 @@
         <v>175</v>
       </c>
       <c r="B116" s="76" t="s">
+        <v>991</v>
+      </c>
+      <c r="C116" s="71" t="s">
         <v>992</v>
       </c>
-      <c r="C116" s="71" t="s">
+      <c r="D116" s="71" t="s">
         <v>993</v>
-      </c>
-      <c r="D116" s="71" t="s">
-        <v>994</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15173,13 +15170,13 @@
         <v>175</v>
       </c>
       <c r="B117" s="76" t="s">
+        <v>994</v>
+      </c>
+      <c r="C117" s="71" t="s">
         <v>995</v>
       </c>
-      <c r="C117" s="71" t="s">
+      <c r="D117" s="71" t="s">
         <v>996</v>
-      </c>
-      <c r="D117" s="71" t="s">
-        <v>997</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15187,13 +15184,13 @@
         <v>175</v>
       </c>
       <c r="B118" s="76" t="s">
+        <v>997</v>
+      </c>
+      <c r="C118" s="71" t="s">
         <v>998</v>
       </c>
-      <c r="C118" s="71" t="s">
+      <c r="D118" s="71" t="s">
         <v>999</v>
-      </c>
-      <c r="D118" s="71" t="s">
-        <v>1000</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15201,13 +15198,13 @@
         <v>175</v>
       </c>
       <c r="B119" s="76" t="s">
+        <v>1000</v>
+      </c>
+      <c r="C119" s="71" t="s">
         <v>1001</v>
       </c>
-      <c r="C119" s="71" t="s">
+      <c r="D119" s="71" t="s">
         <v>1002</v>
-      </c>
-      <c r="D119" s="71" t="s">
-        <v>1003</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15215,108 +15212,108 @@
         <v>175</v>
       </c>
       <c r="G120" s="74" t="s">
-        <v>768</v>
+        <v>682</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A121" s="75" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B121" s="74" t="s">
         <v>703</v>
       </c>
       <c r="C121" s="74" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D121" s="74" t="s">
         <v>1005</v>
       </c>
-      <c r="D121" s="74" t="s">
+      <c r="E121" s="74" t="s">
         <v>1006</v>
       </c>
-      <c r="E121" s="74" t="s">
+      <c r="F121" s="74" t="s">
         <v>1007</v>
-      </c>
-      <c r="F121" s="74" t="s">
-        <v>1008</v>
       </c>
       <c r="G121" s="75"/>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A122" s="75" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B122" s="74" t="s">
         <v>704</v>
       </c>
       <c r="C122" s="74" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D122" s="74" t="s">
         <v>1009</v>
       </c>
-      <c r="D122" s="74" t="s">
+      <c r="E122" s="74" t="s">
         <v>1010</v>
       </c>
-      <c r="E122" s="74" t="s">
+      <c r="F122" s="74" t="s">
         <v>1011</v>
-      </c>
-      <c r="F122" s="74" t="s">
-        <v>1012</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A123" s="75" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B123" s="74" t="s">
         <v>705</v>
       </c>
       <c r="C123" s="74" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D123" s="74" t="s">
         <v>1013</v>
       </c>
-      <c r="D123" s="74" t="s">
+      <c r="E123" s="74" t="s">
         <v>1014</v>
       </c>
-      <c r="E123" s="74" t="s">
+      <c r="F123" s="74" t="s">
         <v>1015</v>
-      </c>
-      <c r="F123" s="74" t="s">
-        <v>1016</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A124" s="75" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B124" s="74" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C124" s="74" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D124" s="74" t="s">
         <v>1017</v>
       </c>
-      <c r="D124" s="74" t="s">
+      <c r="E124" s="74" t="s">
         <v>1018</v>
       </c>
-      <c r="E124" s="74" t="s">
+      <c r="F124" s="74" t="s">
         <v>1019</v>
-      </c>
-      <c r="F124" s="74" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A125" s="75" t="s">
-        <v>1004</v>
+        <v>1003</v>
       </c>
       <c r="B125" s="74" t="s">
         <v>709</v>
       </c>
       <c r="C125" s="74" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D125" s="74" t="s">
         <v>1021</v>
       </c>
-      <c r="D125" s="74" t="s">
+      <c r="E125" s="74" t="s">
         <v>1022</v>
       </c>
-      <c r="E125" s="74" t="s">
+      <c r="F125" s="74" t="s">
         <v>1023</v>
-      </c>
-      <c r="F125" s="74" t="s">
-        <v>1024</v>
       </c>
     </row>
   </sheetData>
@@ -15357,40 +15354,40 @@
   <sheetData>
     <row r="1" s="82" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="81" t="s">
+        <v>1024</v>
+      </c>
+      <c r="B1" s="81" t="s">
         <v>1025</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="C1" s="81" t="s">
         <v>1026</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="D1" s="81" t="s">
         <v>1027</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="E1" s="81" t="s">
         <v>1028</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="F1" s="81" t="s">
         <v>1029</v>
       </c>
-      <c r="F1" s="81" t="s">
+      <c r="G1" s="81" t="s">
         <v>1030</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="H1" s="81" t="s">
         <v>1031</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="I1" s="81" t="s">
         <v>1032</v>
       </c>
-      <c r="I1" s="81" t="s">
+      <c r="J1" s="81" t="s">
         <v>1033</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="K1" s="81" t="s">
         <v>1034</v>
       </c>
-      <c r="K1" s="81" t="s">
+      <c r="L1" s="82" t="s">
         <v>1035</v>
-      </c>
-      <c r="L1" s="82" t="s">
-        <v>1036</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15398,22 +15395,22 @@
         <v>646</v>
       </c>
       <c r="B2" s="51" t="s">
+        <v>1036</v>
+      </c>
+      <c r="C2" s="51" t="s">
         <v>1037</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="D2" s="51" t="s">
         <v>1038</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="E2" s="51" t="s">
         <v>1039</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="F2" s="51" t="s">
         <v>1040</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="G2" s="51" t="s">
         <v>1041</v>
-      </c>
-      <c r="G2" s="51" t="s">
-        <v>1042</v>
       </c>
       <c r="H2" s="51" t="n">
         <v>-10</v>
@@ -15422,13 +15419,13 @@
         <v>100</v>
       </c>
       <c r="J2" s="51" t="s">
+        <v>1042</v>
+      </c>
+      <c r="K2" s="51" t="s">
+        <v>1042</v>
+      </c>
+      <c r="L2" s="51" t="s">
         <v>1043</v>
-      </c>
-      <c r="K2" s="51" t="s">
-        <v>1043</v>
-      </c>
-      <c r="L2" s="51" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15436,22 +15433,22 @@
         <v>637</v>
       </c>
       <c r="B3" s="51" t="s">
+        <v>1044</v>
+      </c>
+      <c r="C3" s="51" t="s">
         <v>1045</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="D3" s="83" t="s">
         <v>1046</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="E3" s="83" t="s">
         <v>1047</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="F3" s="83" t="s">
         <v>1048</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="G3" s="51" t="s">
         <v>1049</v>
-      </c>
-      <c r="G3" s="51" t="s">
-        <v>1050</v>
       </c>
       <c r="H3" s="51" t="n">
         <v>-10</v>
@@ -15460,13 +15457,13 @@
         <v>100</v>
       </c>
       <c r="J3" s="51" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="K3" s="51" t="s">
-        <v>1043</v>
+        <v>1042</v>
       </c>
       <c r="L3" s="51" t="s">
-        <v>1051</v>
+        <v>1050</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15474,22 +15471,22 @@
         <v>651</v>
       </c>
       <c r="B4" s="51" t="s">
+        <v>1051</v>
+      </c>
+      <c r="C4" s="51" t="s">
         <v>1052</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="D4" s="51" t="s">
         <v>1053</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="E4" s="51" t="s">
         <v>1054</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="F4" s="51" t="s">
         <v>1055</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="G4" s="51" t="s">
         <v>1056</v>
-      </c>
-      <c r="G4" s="51" t="s">
-        <v>1057</v>
       </c>
       <c r="H4" s="51" t="n">
         <v>-10</v>
@@ -15498,13 +15495,13 @@
         <v>100</v>
       </c>
       <c r="J4" s="51" t="s">
+        <v>1042</v>
+      </c>
+      <c r="K4" s="51" t="s">
+        <v>1042</v>
+      </c>
+      <c r="L4" s="51" t="s">
         <v>1043</v>
-      </c>
-      <c r="K4" s="51" t="s">
-        <v>1043</v>
-      </c>
-      <c r="L4" s="51" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15512,22 +15509,22 @@
         <v>656</v>
       </c>
       <c r="B5" s="51" t="s">
-        <v>1045</v>
+        <v>1044</v>
       </c>
       <c r="C5" s="51" t="s">
+        <v>1057</v>
+      </c>
+      <c r="D5" s="51" t="s">
         <v>1058</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="E5" s="51" t="s">
+        <v>1047</v>
+      </c>
+      <c r="F5" s="51" t="s">
         <v>1059</v>
       </c>
-      <c r="E5" s="51" t="s">
-        <v>1048</v>
-      </c>
-      <c r="F5" s="51" t="s">
+      <c r="G5" s="51" t="s">
         <v>1060</v>
-      </c>
-      <c r="G5" s="51" t="s">
-        <v>1061</v>
       </c>
       <c r="H5" s="51" t="n">
         <v>-10</v>
@@ -15536,13 +15533,13 @@
         <v>100</v>
       </c>
       <c r="J5" s="51" t="s">
+        <v>1042</v>
+      </c>
+      <c r="K5" s="51" t="s">
+        <v>1042</v>
+      </c>
+      <c r="L5" s="51" t="s">
         <v>1043</v>
-      </c>
-      <c r="K5" s="51" t="s">
-        <v>1043</v>
-      </c>
-      <c r="L5" s="51" t="s">
-        <v>1044</v>
       </c>
     </row>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
@@ -15601,13 +15598,13 @@
         <v>107</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>1061</v>
+      </c>
+      <c r="C2" s="4" t="s">
         <v>1062</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="D2" s="4" t="s">
         <v>1063</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>1064</v>
       </c>
       <c r="E2" s="5"/>
       <c r="F2" s="5"/>
@@ -15617,13 +15614,13 @@
         <v>107</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>1064</v>
+      </c>
+      <c r="C3" s="11" t="s">
         <v>1065</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>1066</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>1067</v>
       </c>
       <c r="E3" s="5"/>
       <c r="F3" s="5"/>
@@ -15633,13 +15630,13 @@
         <v>429</v>
       </c>
       <c r="B4" s="11" t="s">
+        <v>1067</v>
+      </c>
+      <c r="C4" s="11" t="s">
         <v>1068</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="D4" s="11" t="s">
         <v>1069</v>
-      </c>
-      <c r="D4" s="11" t="s">
-        <v>1070</v>
       </c>
       <c r="E4" s="11"/>
     </row>
@@ -15648,13 +15645,13 @@
         <v>429</v>
       </c>
       <c r="B5" s="11" t="s">
+        <v>1070</v>
+      </c>
+      <c r="C5" s="11" t="s">
         <v>1071</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="D5" s="11" t="s">
         <v>1072</v>
-      </c>
-      <c r="D5" s="11" t="s">
-        <v>1073</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15662,13 +15659,13 @@
         <v>429</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>1073</v>
+      </c>
+      <c r="C6" s="11" t="s">
         <v>1074</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="D6" s="11" t="s">
         <v>1075</v>
-      </c>
-      <c r="D6" s="11" t="s">
-        <v>1076</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15676,13 +15673,13 @@
         <v>429</v>
       </c>
       <c r="B7" s="2" t="s">
+        <v>1076</v>
+      </c>
+      <c r="C7" s="11" t="s">
         <v>1077</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="D7" s="11" t="s">
         <v>1078</v>
-      </c>
-      <c r="D7" s="11" t="s">
-        <v>1079</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15690,13 +15687,13 @@
         <v>429</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>1079</v>
+      </c>
+      <c r="C8" s="11" t="s">
         <v>1080</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="D8" s="11" t="s">
         <v>1081</v>
-      </c>
-      <c r="D8" s="11" t="s">
-        <v>1082</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15704,13 +15701,13 @@
         <v>429</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>1082</v>
+      </c>
+      <c r="C9" s="11" t="s">
         <v>1083</v>
       </c>
-      <c r="C9" s="11" t="s">
+      <c r="D9" s="11" t="s">
         <v>1084</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>1085</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15718,13 +15715,13 @@
         <v>429</v>
       </c>
       <c r="B10" s="2" t="s">
+        <v>1085</v>
+      </c>
+      <c r="C10" s="11" t="s">
         <v>1086</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="11" t="s">
         <v>1087</v>
-      </c>
-      <c r="D10" s="11" t="s">
-        <v>1088</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15732,13 +15729,13 @@
         <v>429</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>1088</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>1089</v>
       </c>
-      <c r="C11" s="11" t="s">
+      <c r="D11" s="11" t="s">
         <v>1090</v>
-      </c>
-      <c r="D11" s="11" t="s">
-        <v>1091</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15746,13 +15743,13 @@
         <v>429</v>
       </c>
       <c r="B12" s="2" t="s">
+        <v>1091</v>
+      </c>
+      <c r="C12" s="11" t="s">
         <v>1092</v>
       </c>
-      <c r="C12" s="11" t="s">
+      <c r="D12" s="11" t="s">
         <v>1093</v>
-      </c>
-      <c r="D12" s="11" t="s">
-        <v>1094</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15760,13 +15757,13 @@
         <v>429</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>1094</v>
+      </c>
+      <c r="C13" s="11" t="s">
         <v>1095</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="D13" s="11" t="s">
         <v>1096</v>
-      </c>
-      <c r="D13" s="11" t="s">
-        <v>1097</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15774,7 +15771,7 @@
         <v>429</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="C14" s="11" t="s">
         <v>766</v>
@@ -15788,13 +15785,13 @@
         <v>429</v>
       </c>
       <c r="B15" s="2" t="s">
+        <v>1098</v>
+      </c>
+      <c r="C15" s="11" t="s">
         <v>1099</v>
       </c>
-      <c r="C15" s="11" t="s">
+      <c r="D15" s="11" t="s">
         <v>1100</v>
-      </c>
-      <c r="D15" s="11" t="s">
-        <v>1101</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15802,19 +15799,19 @@
         <v>328</v>
       </c>
       <c r="B16" s="11" t="s">
+        <v>1101</v>
+      </c>
+      <c r="C16" s="11" t="s">
         <v>1102</v>
       </c>
-      <c r="C16" s="11" t="s">
+      <c r="D16" s="11" t="s">
         <v>1103</v>
       </c>
-      <c r="D16" s="11" t="s">
+      <c r="E16" s="11" t="s">
         <v>1104</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="F16" s="11" t="s">
         <v>1105</v>
-      </c>
-      <c r="F16" s="11" t="s">
-        <v>1106</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15822,19 +15819,19 @@
         <v>328</v>
       </c>
       <c r="B17" s="11" t="s">
+        <v>1106</v>
+      </c>
+      <c r="C17" s="11" t="s">
         <v>1107</v>
       </c>
-      <c r="C17" s="11" t="s">
+      <c r="D17" s="11" t="s">
         <v>1108</v>
       </c>
-      <c r="D17" s="11" t="s">
+      <c r="E17" s="11" t="s">
         <v>1109</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="F17" s="11" t="s">
         <v>1110</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>1111</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15842,19 +15839,19 @@
         <v>328</v>
       </c>
       <c r="B18" s="11" t="s">
+        <v>1111</v>
+      </c>
+      <c r="C18" s="11" t="s">
         <v>1112</v>
       </c>
-      <c r="C18" s="11" t="s">
+      <c r="D18" s="11" t="s">
         <v>1113</v>
       </c>
-      <c r="D18" s="11" t="s">
+      <c r="E18" s="11" t="s">
         <v>1114</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="F18" s="11" t="s">
         <v>1115</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>1116</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15862,19 +15859,19 @@
         <v>328</v>
       </c>
       <c r="B19" s="11" t="s">
+        <v>1116</v>
+      </c>
+      <c r="C19" s="11" t="s">
         <v>1117</v>
       </c>
-      <c r="C19" s="11" t="s">
+      <c r="D19" s="11" t="s">
         <v>1118</v>
       </c>
-      <c r="D19" s="11" t="s">
+      <c r="E19" s="11" t="s">
         <v>1119</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="F19" s="11" t="s">
         <v>1120</v>
-      </c>
-      <c r="F19" s="11" t="s">
-        <v>1121</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15882,19 +15879,19 @@
         <v>328</v>
       </c>
       <c r="B20" s="11" t="s">
+        <v>1121</v>
+      </c>
+      <c r="C20" s="11" t="s">
         <v>1122</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="D20" s="11" t="s">
         <v>1123</v>
       </c>
-      <c r="D20" s="11" t="s">
+      <c r="E20" s="11" t="s">
         <v>1124</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="F20" s="11" t="s">
         <v>1125</v>
-      </c>
-      <c r="F20" s="11" t="s">
-        <v>1126</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15902,19 +15899,19 @@
         <v>328</v>
       </c>
       <c r="B21" s="11" t="s">
+        <v>1126</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>1127</v>
       </c>
-      <c r="C21" s="11" t="s">
+      <c r="D21" s="11" t="s">
         <v>1128</v>
       </c>
-      <c r="D21" s="11" t="s">
+      <c r="E21" s="11" t="s">
         <v>1129</v>
       </c>
-      <c r="E21" s="11" t="s">
+      <c r="F21" s="11" t="s">
         <v>1130</v>
-      </c>
-      <c r="F21" s="11" t="s">
-        <v>1131</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15922,13 +15919,13 @@
         <v>328</v>
       </c>
       <c r="B22" s="11" t="s">
+        <v>1131</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>1132</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="D22" s="2" t="s">
         <v>1133</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>1134</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15936,13 +15933,13 @@
         <v>328</v>
       </c>
       <c r="B23" s="11" t="s">
+        <v>1134</v>
+      </c>
+      <c r="C23" s="11" t="s">
         <v>1135</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="D23" s="11" t="s">
         <v>1136</v>
-      </c>
-      <c r="D23" s="11" t="s">
-        <v>1137</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15950,13 +15947,13 @@
         <v>328</v>
       </c>
       <c r="B24" s="11" t="s">
+        <v>1137</v>
+      </c>
+      <c r="C24" s="11" t="s">
         <v>1138</v>
       </c>
-      <c r="C24" s="11" t="s">
+      <c r="D24" s="11" t="s">
         <v>1139</v>
-      </c>
-      <c r="D24" s="11" t="s">
-        <v>1140</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15964,13 +15961,13 @@
         <v>328</v>
       </c>
       <c r="B25" s="11" t="s">
+        <v>1140</v>
+      </c>
+      <c r="C25" s="11" t="s">
         <v>1141</v>
       </c>
-      <c r="C25" s="11" t="s">
+      <c r="D25" s="11" t="s">
         <v>1142</v>
-      </c>
-      <c r="D25" s="11" t="s">
-        <v>1143</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15978,19 +15975,19 @@
         <v>328</v>
       </c>
       <c r="B26" s="11" t="s">
+        <v>1143</v>
+      </c>
+      <c r="C26" s="11" t="s">
         <v>1144</v>
       </c>
-      <c r="C26" s="11" t="s">
+      <c r="D26" s="11" t="s">
         <v>1145</v>
       </c>
-      <c r="D26" s="11" t="s">
+      <c r="E26" s="11" t="s">
         <v>1146</v>
       </c>
-      <c r="E26" s="11" t="s">
+      <c r="F26" s="11" t="s">
         <v>1147</v>
-      </c>
-      <c r="F26" s="11" t="s">
-        <v>1148</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -15998,13 +15995,13 @@
         <v>328</v>
       </c>
       <c r="B27" s="11" t="s">
+        <v>1148</v>
+      </c>
+      <c r="C27" s="11" t="s">
         <v>1149</v>
       </c>
-      <c r="C27" s="11" t="s">
+      <c r="D27" s="11" t="s">
         <v>1150</v>
-      </c>
-      <c r="D27" s="11" t="s">
-        <v>1151</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16012,13 +16009,13 @@
         <v>328</v>
       </c>
       <c r="B28" s="11" t="s">
+        <v>1151</v>
+      </c>
+      <c r="C28" s="11" t="s">
         <v>1152</v>
       </c>
-      <c r="C28" s="11" t="s">
+      <c r="D28" s="11" t="s">
         <v>1153</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>1154</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16026,13 +16023,13 @@
         <v>328</v>
       </c>
       <c r="B29" s="11" t="s">
+        <v>1154</v>
+      </c>
+      <c r="C29" s="11" t="s">
         <v>1155</v>
       </c>
-      <c r="C29" s="11" t="s">
+      <c r="D29" s="11" t="s">
         <v>1156</v>
-      </c>
-      <c r="D29" s="11" t="s">
-        <v>1157</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16040,13 +16037,13 @@
         <v>328</v>
       </c>
       <c r="B30" s="11" t="s">
+        <v>1157</v>
+      </c>
+      <c r="C30" s="11" t="s">
         <v>1158</v>
       </c>
-      <c r="C30" s="11" t="s">
+      <c r="D30" s="11" t="s">
         <v>1159</v>
-      </c>
-      <c r="D30" s="11" t="s">
-        <v>1160</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16054,13 +16051,13 @@
         <v>328</v>
       </c>
       <c r="B31" s="11" t="s">
+        <v>1160</v>
+      </c>
+      <c r="C31" s="11" t="s">
         <v>1161</v>
       </c>
-      <c r="C31" s="11" t="s">
+      <c r="D31" s="11" t="s">
         <v>1162</v>
-      </c>
-      <c r="D31" s="11" t="s">
-        <v>1163</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16068,13 +16065,13 @@
         <v>328</v>
       </c>
       <c r="B32" s="11" t="s">
+        <v>1163</v>
+      </c>
+      <c r="C32" s="11" t="s">
         <v>1164</v>
       </c>
-      <c r="C32" s="11" t="s">
+      <c r="D32" s="11" t="s">
         <v>1165</v>
-      </c>
-      <c r="D32" s="11" t="s">
-        <v>1166</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16082,13 +16079,13 @@
         <v>328</v>
       </c>
       <c r="B33" s="11" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C33" s="11" t="s">
         <v>1167</v>
       </c>
-      <c r="C33" s="11" t="s">
+      <c r="D33" s="11" t="s">
         <v>1168</v>
-      </c>
-      <c r="D33" s="11" t="s">
-        <v>1169</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16096,13 +16093,13 @@
         <v>328</v>
       </c>
       <c r="B34" s="11" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C34" s="11" t="s">
         <v>1170</v>
       </c>
-      <c r="C34" s="11" t="s">
+      <c r="D34" s="11" t="s">
         <v>1171</v>
-      </c>
-      <c r="D34" s="11" t="s">
-        <v>1172</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16110,13 +16107,13 @@
         <v>328</v>
       </c>
       <c r="B35" s="11" t="s">
+        <v>1172</v>
+      </c>
+      <c r="C35" s="11" t="s">
         <v>1173</v>
       </c>
-      <c r="C35" s="11" t="s">
+      <c r="D35" s="11" t="s">
         <v>1174</v>
-      </c>
-      <c r="D35" s="11" t="s">
-        <v>1175</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16124,13 +16121,13 @@
         <v>328</v>
       </c>
       <c r="B36" s="11" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C36" s="11" t="s">
         <v>1176</v>
       </c>
-      <c r="C36" s="11" t="s">
+      <c r="D36" s="11" t="s">
         <v>1177</v>
-      </c>
-      <c r="D36" s="11" t="s">
-        <v>1178</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16138,13 +16135,13 @@
         <v>328</v>
       </c>
       <c r="B37" s="11" t="s">
-        <v>1179</v>
+        <v>1178</v>
       </c>
       <c r="C37" s="11" t="s">
+        <v>1176</v>
+      </c>
+      <c r="D37" s="11" t="s">
         <v>1177</v>
-      </c>
-      <c r="D37" s="11" t="s">
-        <v>1178</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16152,13 +16149,13 @@
         <v>328</v>
       </c>
       <c r="B38" s="11" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C38" s="11" t="s">
         <v>1180</v>
       </c>
-      <c r="C38" s="11" t="s">
+      <c r="D38" s="11" t="s">
         <v>1181</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>1182</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16166,13 +16163,13 @@
         <v>328</v>
       </c>
       <c r="B39" s="11" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C39" s="11" t="s">
         <v>1183</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="D39" s="11" t="s">
         <v>1184</v>
-      </c>
-      <c r="D39" s="11" t="s">
-        <v>1185</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16180,13 +16177,13 @@
         <v>328</v>
       </c>
       <c r="B40" s="11" t="s">
+        <v>1185</v>
+      </c>
+      <c r="C40" s="11" t="s">
         <v>1186</v>
       </c>
-      <c r="C40" s="11" t="s">
+      <c r="D40" s="11" t="s">
         <v>1187</v>
-      </c>
-      <c r="D40" s="11" t="s">
-        <v>1188</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16194,13 +16191,13 @@
         <v>328</v>
       </c>
       <c r="B41" s="11" t="s">
+        <v>1188</v>
+      </c>
+      <c r="C41" s="11" t="s">
         <v>1189</v>
       </c>
-      <c r="C41" s="11" t="s">
+      <c r="D41" s="11" t="s">
         <v>1190</v>
-      </c>
-      <c r="D41" s="11" t="s">
-        <v>1191</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16208,13 +16205,13 @@
         <v>328</v>
       </c>
       <c r="B42" s="11" t="s">
+        <v>1191</v>
+      </c>
+      <c r="C42" s="11" t="s">
         <v>1192</v>
       </c>
-      <c r="C42" s="11" t="s">
+      <c r="D42" s="11" t="s">
         <v>1193</v>
-      </c>
-      <c r="D42" s="11" t="s">
-        <v>1194</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16222,13 +16219,13 @@
         <v>328</v>
       </c>
       <c r="B43" s="11" t="s">
+        <v>1194</v>
+      </c>
+      <c r="C43" s="11" t="s">
         <v>1195</v>
       </c>
-      <c r="C43" s="11" t="s">
+      <c r="D43" s="11" t="s">
         <v>1196</v>
-      </c>
-      <c r="D43" s="11" t="s">
-        <v>1197</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16236,13 +16233,13 @@
         <v>328</v>
       </c>
       <c r="B44" s="11" t="s">
+        <v>1197</v>
+      </c>
+      <c r="C44" s="11" t="s">
         <v>1198</v>
       </c>
-      <c r="C44" s="11" t="s">
+      <c r="D44" s="11" t="s">
         <v>1199</v>
-      </c>
-      <c r="D44" s="11" t="s">
-        <v>1200</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16250,13 +16247,13 @@
         <v>328</v>
       </c>
       <c r="B45" s="11" t="s">
+        <v>1200</v>
+      </c>
+      <c r="C45" s="11" t="s">
         <v>1201</v>
       </c>
-      <c r="C45" s="11" t="s">
+      <c r="D45" s="11" t="s">
         <v>1202</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>1203</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16264,13 +16261,13 @@
         <v>328</v>
       </c>
       <c r="B46" s="11" t="s">
+        <v>1203</v>
+      </c>
+      <c r="C46" s="11" t="s">
         <v>1204</v>
       </c>
-      <c r="C46" s="11" t="s">
+      <c r="D46" s="11" t="s">
         <v>1205</v>
-      </c>
-      <c r="D46" s="11" t="s">
-        <v>1206</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16278,13 +16275,13 @@
         <v>328</v>
       </c>
       <c r="B47" s="11" t="s">
+        <v>1206</v>
+      </c>
+      <c r="C47" s="11" t="s">
         <v>1207</v>
       </c>
-      <c r="C47" s="11" t="s">
+      <c r="D47" s="11" t="s">
         <v>1208</v>
-      </c>
-      <c r="D47" s="11" t="s">
-        <v>1209</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16292,19 +16289,19 @@
         <v>328</v>
       </c>
       <c r="B48" s="11" t="s">
+        <v>1209</v>
+      </c>
+      <c r="C48" s="11" t="s">
         <v>1210</v>
       </c>
-      <c r="C48" s="11" t="s">
+      <c r="D48" s="11" t="s">
         <v>1211</v>
       </c>
-      <c r="D48" s="11" t="s">
+      <c r="E48" s="11" t="s">
         <v>1212</v>
       </c>
-      <c r="E48" s="11" t="s">
+      <c r="F48" s="11" t="s">
         <v>1213</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>1214</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16312,19 +16309,19 @@
         <v>328</v>
       </c>
       <c r="B49" s="11" t="s">
+        <v>1214</v>
+      </c>
+      <c r="C49" s="11" t="s">
         <v>1215</v>
       </c>
-      <c r="C49" s="11" t="s">
+      <c r="D49" s="11" t="s">
         <v>1216</v>
       </c>
-      <c r="D49" s="11" t="s">
+      <c r="E49" s="11" t="s">
         <v>1217</v>
       </c>
-      <c r="E49" s="11" t="s">
+      <c r="F49" s="11" t="s">
         <v>1218</v>
-      </c>
-      <c r="F49" s="11" t="s">
-        <v>1219</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16332,19 +16329,19 @@
         <v>328</v>
       </c>
       <c r="B50" s="11" t="s">
+        <v>1219</v>
+      </c>
+      <c r="C50" s="11" t="s">
         <v>1220</v>
       </c>
-      <c r="C50" s="11" t="s">
+      <c r="D50" s="11" t="s">
         <v>1221</v>
       </c>
-      <c r="D50" s="11" t="s">
+      <c r="E50" s="11" t="s">
         <v>1222</v>
       </c>
-      <c r="E50" s="11" t="s">
+      <c r="F50" s="11" t="s">
         <v>1223</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>1224</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16352,19 +16349,19 @@
         <v>328</v>
       </c>
       <c r="B51" s="11" t="s">
+        <v>1224</v>
+      </c>
+      <c r="C51" s="11" t="s">
         <v>1225</v>
       </c>
-      <c r="C51" s="11" t="s">
+      <c r="D51" s="11" t="s">
         <v>1226</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="E51" s="11" t="s">
         <v>1227</v>
       </c>
-      <c r="E51" s="11" t="s">
+      <c r="F51" s="11" t="s">
         <v>1228</v>
-      </c>
-      <c r="F51" s="11" t="s">
-        <v>1229</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16372,19 +16369,19 @@
         <v>328</v>
       </c>
       <c r="B52" s="11" t="s">
+        <v>1229</v>
+      </c>
+      <c r="C52" s="11" t="s">
         <v>1230</v>
       </c>
-      <c r="C52" s="11" t="s">
+      <c r="D52" s="11" t="s">
         <v>1231</v>
       </c>
-      <c r="D52" s="11" t="s">
+      <c r="E52" s="11" t="s">
         <v>1232</v>
       </c>
-      <c r="E52" s="11" t="s">
+      <c r="F52" s="11" t="s">
         <v>1233</v>
-      </c>
-      <c r="F52" s="11" t="s">
-        <v>1234</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16392,19 +16389,19 @@
         <v>328</v>
       </c>
       <c r="B53" s="11" t="s">
+        <v>1234</v>
+      </c>
+      <c r="C53" s="11" t="s">
         <v>1235</v>
       </c>
-      <c r="C53" s="11" t="s">
+      <c r="D53" s="11" t="s">
         <v>1236</v>
       </c>
-      <c r="D53" s="11" t="s">
+      <c r="E53" s="11" t="s">
         <v>1237</v>
       </c>
-      <c r="E53" s="11" t="s">
+      <c r="F53" s="11" t="s">
         <v>1238</v>
-      </c>
-      <c r="F53" s="11" t="s">
-        <v>1239</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16412,19 +16409,19 @@
         <v>328</v>
       </c>
       <c r="B54" s="11" t="s">
+        <v>1239</v>
+      </c>
+      <c r="C54" s="11" t="s">
         <v>1240</v>
       </c>
-      <c r="C54" s="11" t="s">
+      <c r="D54" s="11" t="s">
         <v>1241</v>
       </c>
-      <c r="D54" s="11" t="s">
+      <c r="E54" s="11" t="s">
         <v>1242</v>
       </c>
-      <c r="E54" s="11" t="s">
+      <c r="F54" s="11" t="s">
         <v>1243</v>
-      </c>
-      <c r="F54" s="11" t="s">
-        <v>1244</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16432,19 +16429,19 @@
         <v>328</v>
       </c>
       <c r="B55" s="11" t="s">
+        <v>1244</v>
+      </c>
+      <c r="C55" s="11" t="s">
         <v>1245</v>
       </c>
-      <c r="C55" s="11" t="s">
+      <c r="D55" s="11" t="s">
         <v>1246</v>
       </c>
-      <c r="D55" s="11" t="s">
+      <c r="E55" s="11" t="s">
         <v>1247</v>
       </c>
-      <c r="E55" s="11" t="s">
+      <c r="F55" s="11" t="s">
         <v>1248</v>
-      </c>
-      <c r="F55" s="11" t="s">
-        <v>1249</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16452,13 +16449,13 @@
         <v>107</v>
       </c>
       <c r="B56" s="2" t="s">
+        <v>1249</v>
+      </c>
+      <c r="C56" s="11" t="s">
         <v>1250</v>
       </c>
-      <c r="C56" s="11" t="s">
+      <c r="D56" s="11" t="s">
         <v>1251</v>
-      </c>
-      <c r="D56" s="11" t="s">
-        <v>1252</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16466,13 +16463,13 @@
         <v>107</v>
       </c>
       <c r="B57" s="2" t="s">
+        <v>1252</v>
+      </c>
+      <c r="C57" s="11" t="s">
         <v>1253</v>
       </c>
-      <c r="C57" s="11" t="s">
+      <c r="D57" s="11" t="s">
         <v>1254</v>
-      </c>
-      <c r="D57" s="11" t="s">
-        <v>1255</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16480,13 +16477,13 @@
         <v>107</v>
       </c>
       <c r="B58" s="2" t="s">
+        <v>1255</v>
+      </c>
+      <c r="C58" s="11" t="s">
         <v>1256</v>
       </c>
-      <c r="C58" s="11" t="s">
+      <c r="D58" s="11" t="s">
         <v>1257</v>
-      </c>
-      <c r="D58" s="11" t="s">
-        <v>1258</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16494,13 +16491,13 @@
         <v>107</v>
       </c>
       <c r="B59" s="2" t="s">
+        <v>1258</v>
+      </c>
+      <c r="C59" s="11" t="s">
         <v>1259</v>
       </c>
-      <c r="C59" s="11" t="s">
+      <c r="D59" s="11" t="s">
         <v>1260</v>
-      </c>
-      <c r="D59" s="11" t="s">
-        <v>1261</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16508,13 +16505,13 @@
         <v>107</v>
       </c>
       <c r="B60" s="84" t="s">
+        <v>1261</v>
+      </c>
+      <c r="C60" s="11" t="s">
         <v>1262</v>
       </c>
-      <c r="C60" s="11" t="s">
+      <c r="D60" s="11" t="s">
         <v>1263</v>
-      </c>
-      <c r="D60" s="11" t="s">
-        <v>1264</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16522,13 +16519,13 @@
         <v>107</v>
       </c>
       <c r="B61" s="11" t="s">
+        <v>1264</v>
+      </c>
+      <c r="C61" s="11" t="s">
         <v>1265</v>
       </c>
-      <c r="C61" s="11" t="s">
+      <c r="D61" s="11" t="s">
         <v>1266</v>
-      </c>
-      <c r="D61" s="11" t="s">
-        <v>1267</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16536,13 +16533,13 @@
         <v>107</v>
       </c>
       <c r="B62" s="11" t="s">
+        <v>1267</v>
+      </c>
+      <c r="C62" s="11" t="s">
         <v>1268</v>
       </c>
-      <c r="C62" s="11" t="s">
+      <c r="D62" s="11" t="s">
         <v>1269</v>
-      </c>
-      <c r="D62" s="11" t="s">
-        <v>1270</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16550,19 +16547,19 @@
         <v>107</v>
       </c>
       <c r="B63" s="11" t="s">
+        <v>1270</v>
+      </c>
+      <c r="C63" s="11" t="s">
         <v>1271</v>
       </c>
-      <c r="C63" s="11" t="s">
+      <c r="D63" s="2" t="s">
         <v>1272</v>
       </c>
-      <c r="D63" s="2" t="s">
+      <c r="E63" s="2" t="s">
         <v>1273</v>
       </c>
-      <c r="E63" s="2" t="s">
+      <c r="F63" s="2" t="s">
         <v>1274</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>1275</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16570,13 +16567,13 @@
         <v>107</v>
       </c>
       <c r="B64" s="41" t="s">
+        <v>1275</v>
+      </c>
+      <c r="C64" s="41" t="s">
         <v>1276</v>
       </c>
-      <c r="C64" s="41" t="s">
+      <c r="D64" s="84" t="s">
         <v>1277</v>
-      </c>
-      <c r="D64" s="84" t="s">
-        <v>1278</v>
       </c>
       <c r="E64" s="2"/>
       <c r="F64" s="2"/>
@@ -16586,13 +16583,13 @@
         <v>107</v>
       </c>
       <c r="B65" s="41" t="s">
+        <v>1278</v>
+      </c>
+      <c r="C65" s="41" t="s">
         <v>1279</v>
       </c>
-      <c r="C65" s="41" t="s">
+      <c r="D65" s="84" t="s">
         <v>1280</v>
-      </c>
-      <c r="D65" s="84" t="s">
-        <v>1281</v>
       </c>
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
@@ -16602,7 +16599,7 @@
         <v>328</v>
       </c>
       <c r="B66" s="67" t="s">
-        <v>1282</v>
+        <v>1281</v>
       </c>
       <c r="C66" s="67" t="s">
         <v>722</v>
@@ -16618,13 +16615,13 @@
         <v>328</v>
       </c>
       <c r="B67" s="67" t="s">
-        <v>1283</v>
+        <v>1282</v>
       </c>
       <c r="C67" s="67" t="s">
+        <v>943</v>
+      </c>
+      <c r="D67" s="67" t="s">
         <v>944</v>
-      </c>
-      <c r="D67" s="67" t="s">
-        <v>945</v>
       </c>
       <c r="E67" s="67"/>
       <c r="F67" s="67"/>
@@ -16634,13 +16631,13 @@
         <v>328</v>
       </c>
       <c r="B68" s="67" t="s">
-        <v>1284</v>
+        <v>1283</v>
       </c>
       <c r="C68" s="67" t="s">
+        <v>945</v>
+      </c>
+      <c r="D68" s="67" t="s">
         <v>946</v>
-      </c>
-      <c r="D68" s="67" t="s">
-        <v>947</v>
       </c>
       <c r="E68" s="67"/>
       <c r="F68" s="67"/>
@@ -16650,19 +16647,19 @@
         <v>328</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>1285</v>
+        <v>1284</v>
       </c>
       <c r="C69" s="11" t="s">
+        <v>948</v>
+      </c>
+      <c r="D69" s="11" t="s">
         <v>949</v>
       </c>
-      <c r="D69" s="11" t="s">
+      <c r="E69" s="11" t="s">
         <v>950</v>
       </c>
-      <c r="E69" s="11" t="s">
+      <c r="F69" s="11" t="s">
         <v>951</v>
-      </c>
-      <c r="F69" s="11" t="s">
-        <v>952</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16670,19 +16667,19 @@
         <v>429</v>
       </c>
       <c r="B70" s="67" t="s">
-        <v>1286</v>
+        <v>1285</v>
       </c>
       <c r="C70" s="11" t="s">
+        <v>955</v>
+      </c>
+      <c r="D70" s="11" t="s">
         <v>956</v>
       </c>
-      <c r="D70" s="11" t="s">
+      <c r="E70" s="11" t="s">
         <v>957</v>
       </c>
-      <c r="E70" s="11" t="s">
+      <c r="F70" s="11" t="s">
         <v>958</v>
-      </c>
-      <c r="F70" s="11" t="s">
-        <v>959</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16690,19 +16687,19 @@
         <v>429</v>
       </c>
       <c r="B71" s="67" t="s">
-        <v>1287</v>
+        <v>1286</v>
       </c>
       <c r="C71" s="11" t="s">
+        <v>960</v>
+      </c>
+      <c r="D71" s="11" t="s">
         <v>961</v>
       </c>
-      <c r="D71" s="11" t="s">
+      <c r="E71" s="11" t="s">
         <v>962</v>
       </c>
-      <c r="E71" s="11" t="s">
+      <c r="F71" s="11" t="s">
         <v>963</v>
-      </c>
-      <c r="F71" s="11" t="s">
-        <v>964</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16710,13 +16707,13 @@
         <v>429</v>
       </c>
       <c r="B72" s="67" t="s">
+        <v>1287</v>
+      </c>
+      <c r="C72" s="11" t="s">
         <v>1288</v>
       </c>
-      <c r="C72" s="11" t="s">
+      <c r="D72" s="11" t="s">
         <v>1289</v>
-      </c>
-      <c r="D72" s="11" t="s">
-        <v>1290</v>
       </c>
       <c r="E72" s="11"/>
       <c r="F72" s="11"/>
@@ -16726,13 +16723,13 @@
         <v>429</v>
       </c>
       <c r="B73" s="67" t="s">
+        <v>1290</v>
+      </c>
+      <c r="C73" s="11" t="s">
         <v>1291</v>
       </c>
-      <c r="C73" s="11" t="s">
+      <c r="D73" s="11" t="s">
         <v>1292</v>
-      </c>
-      <c r="D73" s="11" t="s">
-        <v>1293</v>
       </c>
       <c r="E73" s="11"/>
       <c r="F73" s="11"/>
@@ -16742,13 +16739,13 @@
         <v>429</v>
       </c>
       <c r="B74" s="67" t="s">
+        <v>1293</v>
+      </c>
+      <c r="C74" s="11" t="s">
         <v>1294</v>
       </c>
-      <c r="C74" s="11" t="s">
+      <c r="D74" s="11" t="s">
         <v>1295</v>
-      </c>
-      <c r="D74" s="11" t="s">
-        <v>1296</v>
       </c>
       <c r="E74" s="11"/>
       <c r="F74" s="11"/>
@@ -16758,13 +16755,13 @@
         <v>429</v>
       </c>
       <c r="B75" s="11" t="s">
+        <v>1296</v>
+      </c>
+      <c r="C75" s="11" t="s">
         <v>1297</v>
       </c>
-      <c r="C75" s="11" t="s">
+      <c r="D75" s="11" t="s">
         <v>1298</v>
-      </c>
-      <c r="D75" s="11" t="s">
-        <v>1299</v>
       </c>
       <c r="E75" s="11"/>
       <c r="F75" s="11"/>
@@ -16774,13 +16771,13 @@
         <v>328</v>
       </c>
       <c r="B76" s="11" t="s">
+        <v>1299</v>
+      </c>
+      <c r="C76" s="11" t="s">
         <v>1300</v>
       </c>
-      <c r="C76" s="11" t="s">
+      <c r="D76" s="11" t="s">
         <v>1301</v>
-      </c>
-      <c r="D76" s="11" t="s">
-        <v>1302</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16788,13 +16785,13 @@
         <v>328</v>
       </c>
       <c r="B77" s="11" t="s">
+        <v>1302</v>
+      </c>
+      <c r="C77" s="11" t="s">
         <v>1303</v>
       </c>
-      <c r="C77" s="11" t="s">
+      <c r="D77" s="11" t="s">
         <v>1304</v>
-      </c>
-      <c r="D77" s="11" t="s">
-        <v>1305</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16802,13 +16799,13 @@
         <v>328</v>
       </c>
       <c r="B78" s="11" t="s">
+        <v>1305</v>
+      </c>
+      <c r="C78" s="11" t="s">
         <v>1306</v>
       </c>
-      <c r="C78" s="11" t="s">
+      <c r="D78" s="11" t="s">
         <v>1307</v>
-      </c>
-      <c r="D78" s="11" t="s">
-        <v>1308</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16816,13 +16813,13 @@
         <v>328</v>
       </c>
       <c r="B79" s="11" t="s">
+        <v>1308</v>
+      </c>
+      <c r="C79" s="11" t="s">
         <v>1309</v>
       </c>
-      <c r="C79" s="11" t="s">
+      <c r="D79" s="11" t="s">
         <v>1310</v>
-      </c>
-      <c r="D79" s="11" t="s">
-        <v>1311</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16830,19 +16827,19 @@
         <v>107</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>1312</v>
+        <v>1311</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>1004</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>1005</v>
       </c>
-      <c r="D80" s="1" t="s">
+      <c r="E80" s="1" t="s">
         <v>1006</v>
       </c>
-      <c r="E80" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>1007</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>1008</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16850,19 +16847,19 @@
         <v>107</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>1313</v>
+        <v>1312</v>
       </c>
       <c r="C81" s="1" t="s">
+        <v>1008</v>
+      </c>
+      <c r="D81" s="1" t="s">
         <v>1009</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="E81" s="1" t="s">
         <v>1010</v>
       </c>
-      <c r="E81" s="1" t="s">
+      <c r="F81" s="1" t="s">
         <v>1011</v>
-      </c>
-      <c r="F81" s="1" t="s">
-        <v>1012</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16870,19 +16867,19 @@
         <v>107</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>1314</v>
+        <v>1313</v>
       </c>
       <c r="C82" s="1" t="s">
+        <v>1012</v>
+      </c>
+      <c r="D82" s="1" t="s">
         <v>1013</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="E82" s="1" t="s">
         <v>1014</v>
       </c>
-      <c r="E82" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>1015</v>
-      </c>
-      <c r="F82" s="1" t="s">
-        <v>1016</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16890,19 +16887,19 @@
         <v>107</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>1315</v>
+        <v>1314</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>1016</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>1017</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="E83" s="1" t="s">
         <v>1018</v>
       </c>
-      <c r="E83" s="1" t="s">
+      <c r="F83" s="1" t="s">
         <v>1019</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>1020</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16910,19 +16907,19 @@
         <v>107</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>1316</v>
+        <v>1315</v>
       </c>
       <c r="C84" s="1" t="s">
+        <v>1020</v>
+      </c>
+      <c r="D84" s="1" t="s">
         <v>1021</v>
       </c>
-      <c r="D84" s="1" t="s">
+      <c r="E84" s="1" t="s">
         <v>1022</v>
       </c>
-      <c r="E84" s="1" t="s">
+      <c r="F84" s="1" t="s">
         <v>1023</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>1024</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16930,19 +16927,19 @@
         <v>276</v>
       </c>
       <c r="B85" s="2" t="s">
+        <v>1316</v>
+      </c>
+      <c r="C85" s="11" t="s">
         <v>1317</v>
       </c>
-      <c r="C85" s="11" t="s">
+      <c r="D85" s="11" t="s">
         <v>1318</v>
       </c>
-      <c r="D85" s="11" t="s">
+      <c r="E85" s="11" t="s">
         <v>1319</v>
       </c>
-      <c r="E85" s="11" t="s">
+      <c r="F85" s="11" t="s">
         <v>1320</v>
-      </c>
-      <c r="F85" s="11" t="s">
-        <v>1321</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16950,19 +16947,19 @@
         <v>276</v>
       </c>
       <c r="B86" s="2" t="s">
+        <v>1321</v>
+      </c>
+      <c r="C86" s="11" t="s">
         <v>1322</v>
       </c>
-      <c r="C86" s="11" t="s">
+      <c r="D86" s="11" t="s">
         <v>1323</v>
       </c>
-      <c r="D86" s="11" t="s">
+      <c r="E86" s="11" t="s">
         <v>1324</v>
       </c>
-      <c r="E86" s="11" t="s">
+      <c r="F86" s="11" t="s">
         <v>1325</v>
-      </c>
-      <c r="F86" s="11" t="s">
-        <v>1326</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -16970,13 +16967,13 @@
         <v>591</v>
       </c>
       <c r="B87" s="2" t="s">
+        <v>1326</v>
+      </c>
+      <c r="C87" s="11" t="s">
         <v>1327</v>
       </c>
-      <c r="C87" s="11" t="s">
+      <c r="D87" s="11" t="s">
         <v>1328</v>
-      </c>
-      <c r="D87" s="11" t="s">
-        <v>1329</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Label: Remove sick leave or parental leave on the label.
Fix: #192
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -495,11 +495,11 @@
   </si>
   <si>
     <t xml:space="preserve">**Travaill{{gender:eur/euse/eur(-euse)/eur(-euse)}}**
-__Incluant travaill{{gender:eur/euse/eur(-euse)/eur(-euse)}} autonome, artiste, travaill{{gender:eur/euse/eur(-euse)/eur(-euse)}} en congé de maladie ou parental.__</t>
+__Incluant travaill{{gender:eur/euse/eur(-euse)/eur(-euse)}} autonome et artiste.__</t>
   </si>
   <si>
     <t xml:space="preserve">**Worker**
-__Including self-employed, artist, on sick leave or parental leave.__</t>
+__Including self-employed and artist.__</t>
   </si>
   <si>
     <t xml:space="preserve">ifAge14orMoreConditional</t>
@@ -5518,12 +5518,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C22" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="O17" activeCellId="0" sqref="O17"/>
+      <selection pane="bottomLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+      <selection pane="bottomRight" activeCell="H25" activeCellId="0" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6798,7 +6798,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="74.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="53.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="23" t="s">
         <v>143</v>
       </c>
@@ -12077,7 +12077,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Label: Update label for household_size
Fix: #289
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -266,12 +266,12 @@
     <t xml:space="preserve">household_size</t>
   </si>
   <si>
-    <t xml:space="preserve">**Personnes habitant votre domicile** ou logement.
-__Y compris vous-même et les enfants en garde partagée s'ils étaient présents le {{assignedDate}}.__</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Persons living in your home**
-__Including yourself and children in shared custody if they were present on {{assignedDate}}.__</t>
+    <t xml:space="preserve">**Personnes habitant votre domicile** ou logement en date du {{assignedDate}}
+__Y compris vous-même et les enfants en garde partagée.__</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Persons living in your home** or accommodation as of {{assignedDate}}
+__Including yourself and children in shared custody.__</t>
   </si>
   <si>
     <t xml:space="preserve">min=1
@@ -5518,11 +5518,11 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
       <selection pane="bottomRight" activeCell="I13" activeCellId="0" sqref="I13"/>
     </sheetView>
   </sheetViews>
@@ -6177,7 +6177,7 @@
       <c r="W12" s="8"/>
       <c r="X12" s="8"/>
     </row>
-    <row r="13" customFormat="false" ht="57.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
         <v>75</v>
       </c>
@@ -6270,7 +6270,7 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
-      <c r="T14" s="8" t="b">
+      <c r="T14" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6319,7 +6319,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
-      <c r="T15" s="8" t="b">
+      <c r="T15" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6419,7 +6419,7 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
-      <c r="T17" s="8" t="b">
+      <c r="T17" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6628,7 +6628,7 @@
       <c r="Q21" s="26"/>
       <c r="R21" s="26"/>
       <c r="S21" s="26"/>
-      <c r="T21" s="23" t="b">
+      <c r="T21" s="25" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7147,7 +7147,7 @@
       <c r="Q31" s="26"/>
       <c r="R31" s="26"/>
       <c r="S31" s="26"/>
-      <c r="T31" s="23" t="b">
+      <c r="T31" s="25" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7197,7 +7197,7 @@
       <c r="Q32" s="26"/>
       <c r="R32" s="26"/>
       <c r="S32" s="26"/>
-      <c r="T32" s="23" t="b">
+      <c r="T32" s="25" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7677,7 +7677,7 @@
       <c r="Q41" s="26"/>
       <c r="R41" s="26"/>
       <c r="S41" s="26"/>
-      <c r="T41" s="23" t="b">
+      <c r="T41" s="25" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8817,7 +8817,7 @@
       <c r="Q66" s="36"/>
       <c r="R66" s="36"/>
       <c r="S66" s="36"/>
-      <c r="T66" s="34" t="b">
+      <c r="T66" s="37" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9540,7 +9540,7 @@
       <c r="Q82" s="36"/>
       <c r="R82" s="36"/>
       <c r="S82" s="36"/>
-      <c r="T82" s="34" t="b">
+      <c r="T82" s="37" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10550,7 +10550,7 @@
       <c r="Q104" s="36"/>
       <c r="R104" s="36"/>
       <c r="S104" s="36"/>
-      <c r="T104" s="17" t="b">
+      <c r="T104" s="19" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10801,7 +10801,7 @@
       <c r="Q109" s="36"/>
       <c r="R109" s="36"/>
       <c r="S109" s="36"/>
-      <c r="T109" s="17" t="b">
+      <c r="T109" s="19" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13263,7 +13263,7 @@
   </sheetPr>
   <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A86" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A86" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E109" activeCellId="0" sqref="E109"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Label: Use last year for household income year.
Fix: #330
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -2238,11 +2238,11 @@
     <t xml:space="preserve">household.income</t>
   </si>
   <si>
-    <t xml:space="preserve">Tranche de revenu avant impôts (brut) du ménage, en 2023?
+    <t xml:space="preserve">Tranche de revenu avant impôts (brut) du ménage, en {{lastYear}}?
 __Facultatif__</t>
   </si>
   <si>
-    <t xml:space="preserve">What was your household's income range before taxes (gross income), in 2023?
+    <t xml:space="preserve">What was your household's income range before taxes (gross income), in {{lastYear}}?
 __Not mandatory__</t>
   </si>
   <si>
@@ -4785,7 +4785,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="86">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -4987,6 +4987,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5519,11 +5523,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C115" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I13" activeCellId="0" sqref="I13"/>
+      <selection pane="bottomLeft" activeCell="A115" activeCellId="0" sqref="A115"/>
+      <selection pane="bottomRight" activeCell="I119" activeCellId="0" sqref="I119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -11256,7 +11260,7 @@
         <v>596</v>
       </c>
       <c r="B120" s="34" t="s">
-        <v>518</v>
+        <v>72</v>
       </c>
       <c r="C120" s="35" t="n">
         <f aca="false">TRUE()</f>
@@ -11269,10 +11273,10 @@
       <c r="F120" s="36" t="s">
         <v>597</v>
       </c>
-      <c r="G120" s="34" t="s">
+      <c r="G120" s="51" t="s">
         <v>598</v>
       </c>
-      <c r="H120" s="34" t="s">
+      <c r="H120" s="51" t="s">
         <v>599</v>
       </c>
       <c r="I120" s="17"/>
@@ -11281,7 +11285,7 @@
       <c r="L120" s="36"/>
       <c r="M120" s="36"/>
       <c r="N120" s="36"/>
-      <c r="O120" s="51" t="s">
+      <c r="O120" s="52" t="s">
         <v>600</v>
       </c>
       <c r="P120" s="36"/>
@@ -11409,10 +11413,10 @@
       <c r="F123" s="36" t="s">
         <v>610</v>
       </c>
-      <c r="G123" s="51" t="s">
+      <c r="G123" s="52" t="s">
         <v>611</v>
       </c>
-      <c r="H123" s="51" t="s">
+      <c r="H123" s="52" t="s">
         <v>612</v>
       </c>
       <c r="I123" s="17"/>
@@ -11640,10 +11644,10 @@
       <c r="F128" s="36" t="s">
         <v>633</v>
       </c>
-      <c r="G128" s="51" t="s">
+      <c r="G128" s="52" t="s">
         <v>634</v>
       </c>
-      <c r="H128" s="51" t="s">
+      <c r="H128" s="52" t="s">
         <v>635</v>
       </c>
       <c r="I128" s="17"/>
@@ -11656,7 +11660,7 @@
       </c>
       <c r="O128" s="36"/>
       <c r="P128" s="36"/>
-      <c r="Q128" s="51" t="s">
+      <c r="Q128" s="52" t="s">
         <v>637</v>
       </c>
       <c r="R128" s="36"/>
@@ -11688,10 +11692,10 @@
       <c r="F129" s="36" t="s">
         <v>639</v>
       </c>
-      <c r="G129" s="51" t="s">
+      <c r="G129" s="52" t="s">
         <v>640</v>
       </c>
-      <c r="H129" s="51" t="s">
+      <c r="H129" s="52" t="s">
         <v>641</v>
       </c>
       <c r="I129" s="17"/>
@@ -11734,10 +11738,10 @@
       <c r="F130" s="36" t="s">
         <v>643</v>
       </c>
-      <c r="G130" s="51" t="s">
+      <c r="G130" s="52" t="s">
         <v>644</v>
       </c>
-      <c r="H130" s="51" t="s">
+      <c r="H130" s="52" t="s">
         <v>645</v>
       </c>
       <c r="I130" s="17"/>
@@ -11750,7 +11754,7 @@
       </c>
       <c r="O130" s="36"/>
       <c r="P130" s="36"/>
-      <c r="Q130" s="51" t="s">
+      <c r="Q130" s="52" t="s">
         <v>646</v>
       </c>
       <c r="R130" s="36"/>
@@ -11782,10 +11786,10 @@
       <c r="F131" s="36" t="s">
         <v>648</v>
       </c>
-      <c r="G131" s="51" t="s">
+      <c r="G131" s="52" t="s">
         <v>649</v>
       </c>
-      <c r="H131" s="51" t="s">
+      <c r="H131" s="52" t="s">
         <v>650</v>
       </c>
       <c r="I131" s="17"/>
@@ -11798,7 +11802,7 @@
       </c>
       <c r="O131" s="36"/>
       <c r="P131" s="36"/>
-      <c r="Q131" s="51" t="s">
+      <c r="Q131" s="52" t="s">
         <v>651</v>
       </c>
       <c r="R131" s="36"/>
@@ -11830,10 +11834,10 @@
       <c r="F132" s="36" t="s">
         <v>653</v>
       </c>
-      <c r="G132" s="51" t="s">
+      <c r="G132" s="52" t="s">
         <v>654</v>
       </c>
-      <c r="H132" s="51" t="s">
+      <c r="H132" s="52" t="s">
         <v>655</v>
       </c>
       <c r="I132" s="17"/>
@@ -11846,7 +11850,7 @@
       </c>
       <c r="O132" s="36"/>
       <c r="P132" s="36"/>
-      <c r="Q132" s="51" t="s">
+      <c r="Q132" s="52" t="s">
         <v>656</v>
       </c>
       <c r="R132" s="36"/>
@@ -11878,10 +11882,10 @@
       <c r="F133" s="36" t="s">
         <v>658</v>
       </c>
-      <c r="G133" s="51" t="s">
+      <c r="G133" s="52" t="s">
         <v>659</v>
       </c>
-      <c r="H133" s="51" t="s">
+      <c r="H133" s="52" t="s">
         <v>660</v>
       </c>
       <c r="I133" s="17"/>
@@ -11956,7 +11960,7 @@
       <c r="B135" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="C135" s="52" t="n">
+      <c r="C135" s="53" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11972,9 +11976,9 @@
       <c r="H135" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="L135" s="53"/>
-      <c r="M135" s="54"/>
-      <c r="T135" s="55" t="b">
+      <c r="L135" s="54"/>
+      <c r="M135" s="55"/>
+      <c r="T135" s="56" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12083,32 +12087,32 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="56" width="27.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="56" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="56" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="57" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="56" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="56" width="12.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="56" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="57" width="27.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="57" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="57" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="58" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="57" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="57" width="12.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="57" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" s="60" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="58" t="s">
+    <row r="1" s="61" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="59" t="s">
         <v>668</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="59" t="s">
         <v>669</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="59" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="60" t="s">
         <v>670</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="59" t="s">
         <v>671</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="59" t="s">
         <v>672</v>
       </c>
     </row>
@@ -12120,7 +12124,7 @@
       <c r="C2" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="62" t="s">
         <v>675</v>
       </c>
       <c r="E2" s="11" t="n">
@@ -12136,7 +12140,7 @@
       <c r="C3" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E3" s="11" t="n">
@@ -12152,7 +12156,7 @@
       <c r="C4" s="11" t="s">
         <v>677</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="62" t="s">
         <v>675</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -12170,7 +12174,7 @@
       <c r="C5" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="62" t="s">
         <v>675</v>
       </c>
       <c r="E5" s="11" t="n">
@@ -12186,7 +12190,7 @@
       <c r="C6" s="11" t="s">
         <v>680</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E6" s="11" t="n">
@@ -12195,14 +12199,14 @@
       <c r="F6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="63" t="s">
         <v>138</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
         <v>681</v>
       </c>
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="62" t="s">
         <v>675</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -12218,7 +12222,7 @@
       <c r="C8" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E8" s="11" t="n">
@@ -12236,7 +12240,7 @@
       <c r="C9" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="62" t="s">
         <v>686</v>
       </c>
       <c r="E9" s="11" t="n">
@@ -12252,7 +12256,7 @@
       <c r="C10" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E10" s="11" t="n">
@@ -12270,7 +12274,7 @@
       <c r="C11" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="62" t="s">
         <v>686</v>
       </c>
       <c r="E11" s="11" t="n">
@@ -12286,7 +12290,7 @@
       <c r="C12" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E12" s="11" t="n">
@@ -12304,7 +12308,7 @@
       <c r="C13" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D13" s="61" t="s">
+      <c r="D13" s="62" t="s">
         <v>686</v>
       </c>
       <c r="E13" s="11" t="n">
@@ -12320,7 +12324,7 @@
       <c r="C14" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="62" t="s">
         <v>686</v>
       </c>
       <c r="E14" s="11" t="n">
@@ -12336,7 +12340,7 @@
       <c r="C15" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E15" s="11" t="n">
@@ -12352,7 +12356,7 @@
       <c r="C16" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E16" s="11" t="n">
@@ -12368,7 +12372,7 @@
       <c r="C17" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E17" s="11" t="n">
@@ -12384,7 +12388,7 @@
       <c r="C18" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E18" s="11" t="n">
@@ -12400,7 +12404,7 @@
       <c r="C19" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D19" s="61" t="s">
+      <c r="D19" s="62" t="s">
         <v>686</v>
       </c>
       <c r="E19" s="11" t="n">
@@ -12418,7 +12422,7 @@
       <c r="C20" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="62" t="s">
         <v>691</v>
       </c>
       <c r="E20" s="11" t="s">
@@ -12434,7 +12438,7 @@
       <c r="C21" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D21" s="61" t="s">
+      <c r="D21" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E21" s="11" t="n">
@@ -12450,7 +12454,7 @@
       <c r="C22" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E22" s="11" t="n">
@@ -12466,7 +12470,7 @@
       <c r="C23" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D23" s="61" t="s">
+      <c r="D23" s="62" t="s">
         <v>686</v>
       </c>
       <c r="E23" s="11" t="n">
@@ -12484,7 +12488,7 @@
       <c r="C24" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D24" s="61" t="s">
+      <c r="D24" s="62" t="s">
         <v>691</v>
       </c>
       <c r="E24" s="11" t="s">
@@ -12500,7 +12504,7 @@
       <c r="C25" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D25" s="61" t="s">
+      <c r="D25" s="62" t="s">
         <v>676</v>
       </c>
       <c r="E25" s="11" t="n">
@@ -12516,7 +12520,7 @@
       <c r="C26" s="11" t="s">
         <v>695</v>
       </c>
-      <c r="D26" s="61" t="s">
+      <c r="D26" s="62" t="s">
         <v>675</v>
       </c>
       <c r="E26" s="11" t="s">
@@ -12525,253 +12529,253 @@
       <c r="F26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="57" t="s">
         <v>205</v>
       </c>
-      <c r="C27" s="56" t="s">
+      <c r="C27" s="57" t="s">
         <v>696</v>
       </c>
-      <c r="D27" s="61" t="s">
+      <c r="D27" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E27" s="57" t="s">
+      <c r="E27" s="58" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="57" t="s">
         <v>205</v>
       </c>
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="57" t="s">
         <v>696</v>
       </c>
-      <c r="D28" s="61" t="s">
+      <c r="D28" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E28" s="57" t="s">
+      <c r="E28" s="58" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="57" t="s">
         <v>205</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="57" t="s">
         <v>696</v>
       </c>
-      <c r="D29" s="61" t="s">
+      <c r="D29" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E29" s="57" t="s">
+      <c r="E29" s="58" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="57" t="s">
         <v>221</v>
       </c>
-      <c r="C30" s="56" t="s">
+      <c r="C30" s="57" t="s">
         <v>696</v>
       </c>
-      <c r="D30" s="61" t="s">
+      <c r="D30" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E30" s="57" t="s">
+      <c r="E30" s="58" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="57" t="s">
         <v>221</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="57" t="s">
         <v>696</v>
       </c>
-      <c r="D31" s="61" t="s">
+      <c r="D31" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E31" s="57" t="s">
+      <c r="E31" s="58" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="57" t="s">
         <v>221</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="57" t="s">
         <v>696</v>
       </c>
-      <c r="D32" s="61" t="s">
+      <c r="D32" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="58" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="57" t="s">
         <v>229</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="57" t="s">
         <v>702</v>
       </c>
-      <c r="D33" s="61" t="s">
+      <c r="D33" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E33" s="56" t="s">
+      <c r="E33" s="57" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="57" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C34" s="57" t="s">
         <v>702</v>
       </c>
-      <c r="D34" s="61" t="s">
+      <c r="D34" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E34" s="56" t="s">
+      <c r="E34" s="57" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="57" t="s">
         <v>229</v>
       </c>
-      <c r="B35" s="56" t="s">
+      <c r="B35" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="57" t="s">
         <v>702</v>
       </c>
-      <c r="D35" s="61" t="s">
+      <c r="D35" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E35" s="56" t="s">
+      <c r="E35" s="57" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="57" t="s">
         <v>229</v>
       </c>
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="57" t="s">
         <v>706</v>
       </c>
-      <c r="D36" s="61" t="s">
+      <c r="D36" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E36" s="56" t="s">
+      <c r="E36" s="57" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="56" t="s">
+      <c r="A37" s="57" t="s">
         <v>229</v>
       </c>
-      <c r="B37" s="56" t="s">
+      <c r="B37" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="C37" s="56" t="s">
+      <c r="C37" s="57" t="s">
         <v>706</v>
       </c>
-      <c r="D37" s="61" t="s">
+      <c r="D37" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E37" s="56" t="s">
+      <c r="E37" s="57" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="56" t="s">
+      <c r="A38" s="57" t="s">
         <v>229</v>
       </c>
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C38" s="57" t="s">
         <v>706</v>
       </c>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E38" s="56" t="s">
+      <c r="E38" s="57" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="57" t="s">
         <v>41</v>
       </c>
-      <c r="C39" s="63" t="s">
+      <c r="C39" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="D39" s="57" t="s">
+      <c r="D39" s="58" t="s">
         <v>675</v>
       </c>
-      <c r="E39" s="56" t="s">
+      <c r="E39" s="57" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="64" t="s">
+      <c r="A40" s="65" t="s">
         <v>607</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>601</v>
       </c>
-      <c r="D40" s="65" t="s">
+      <c r="D40" s="66" t="s">
         <v>675</v>
       </c>
-      <c r="E40" s="66" t="s">
+      <c r="E40" s="67" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="64" t="s">
+      <c r="A41" s="65" t="s">
         <v>624</v>
       </c>
-      <c r="C41" s="56" t="s">
+      <c r="C41" s="57" t="s">
         <v>707</v>
       </c>
-      <c r="D41" s="61" t="s">
+      <c r="D41" s="62" t="s">
         <v>676</v>
       </c>
-      <c r="E41" s="56" t="n">
+      <c r="E41" s="57" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="67" t="s">
+      <c r="A42" s="68" t="s">
         <v>708</v>
       </c>
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="57" t="s">
         <v>702</v>
       </c>
-      <c r="D42" s="57" t="s">
+      <c r="D42" s="58" t="s">
         <v>675</v>
       </c>
-      <c r="E42" s="56" t="s">
+      <c r="E42" s="57" t="s">
         <v>705</v>
       </c>
     </row>
@@ -12779,13 +12783,13 @@
       <c r="A43" s="26" t="s">
         <v>263</v>
       </c>
-      <c r="C43" s="56" t="s">
+      <c r="C43" s="57" t="s">
         <v>702</v>
       </c>
-      <c r="D43" s="61" t="s">
+      <c r="D43" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E43" s="56" t="s">
+      <c r="E43" s="57" t="s">
         <v>709</v>
       </c>
     </row>
@@ -12793,27 +12797,27 @@
       <c r="A44" s="26" t="s">
         <v>263</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="57" t="s">
         <v>679</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C44" s="57" t="s">
         <v>702</v>
       </c>
-      <c r="D44" s="61" t="s">
+      <c r="D44" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E44" s="56" t="s">
+      <c r="E44" s="57" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="62" t="s">
+      <c r="A45" s="63" t="s">
         <v>173</v>
       </c>
-      <c r="C45" s="56" t="s">
+      <c r="C45" s="57" t="s">
         <v>696</v>
       </c>
-      <c r="D45" s="57" t="s">
+      <c r="D45" s="58" t="s">
         <v>675</v>
       </c>
       <c r="E45" s="11" t="s">
@@ -12824,13 +12828,13 @@
       <c r="A46" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="C46" s="56" t="s">
+      <c r="C46" s="57" t="s">
         <v>711</v>
       </c>
-      <c r="D46" s="61" t="s">
+      <c r="D46" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E46" s="57" t="s">
+      <c r="E46" s="58" t="s">
         <v>712</v>
       </c>
     </row>
@@ -12838,13 +12842,13 @@
       <c r="A47" s="26" t="s">
         <v>213</v>
       </c>
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="57" t="s">
         <v>711</v>
       </c>
-      <c r="D47" s="61" t="s">
+      <c r="D47" s="62" t="s">
         <v>675</v>
       </c>
-      <c r="E47" s="57" t="s">
+      <c r="E47" s="58" t="s">
         <v>713</v>
       </c>
     </row>
@@ -12855,10 +12859,10 @@
       <c r="C48" s="11" t="s">
         <v>580</v>
       </c>
-      <c r="D48" s="65" t="s">
+      <c r="D48" s="66" t="s">
         <v>675</v>
       </c>
-      <c r="E48" s="66" t="s">
+      <c r="E48" s="67" t="s">
         <v>678</v>
       </c>
     </row>
@@ -12869,10 +12873,10 @@
       <c r="C49" s="11" t="s">
         <v>551</v>
       </c>
-      <c r="D49" s="57" t="s">
+      <c r="D49" s="58" t="s">
         <v>675</v>
       </c>
-      <c r="E49" s="56" t="s">
+      <c r="E49" s="57" t="s">
         <v>678</v>
       </c>
     </row>
@@ -12919,28 +12923,28 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="69" t="s">
+      <c r="B1" s="70" t="s">
         <v>714</v>
       </c>
-      <c r="C1" s="68" t="s">
+      <c r="C1" s="69" t="s">
         <v>715</v>
       </c>
-      <c r="D1" s="68" t="s">
+      <c r="D1" s="69" t="s">
         <v>716</v>
       </c>
-      <c r="E1" s="68" t="s">
+      <c r="E1" s="69" t="s">
         <v>717</v>
       </c>
-      <c r="F1" s="68" t="s">
+      <c r="F1" s="69" t="s">
         <v>718</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>719</v>
       </c>
-      <c r="H1" s="68" t="s">
+      <c r="H1" s="69" t="s">
         <v>720</v>
       </c>
     </row>
@@ -12957,15 +12961,15 @@
       <c r="D2" s="11" t="s">
         <v>723</v>
       </c>
-      <c r="E2" s="70" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="70" t="b">
+      <c r="E2" s="71" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="70" t="b">
+      <c r="G2" s="71" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12983,15 +12987,15 @@
       <c r="D3" s="11" t="s">
         <v>726</v>
       </c>
-      <c r="E3" s="70" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="70" t="b">
+      <c r="E3" s="71" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="70" t="b">
+      <c r="G3" s="71" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13009,15 +13013,15 @@
       <c r="D4" s="11" t="s">
         <v>730</v>
       </c>
-      <c r="E4" s="70" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="70" t="b">
+      <c r="E4" s="71" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="70" t="b">
+      <c r="G4" s="71" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13035,15 +13039,15 @@
       <c r="D5" s="11" t="s">
         <v>733</v>
       </c>
-      <c r="E5" s="70" t="b">
+      <c r="E5" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F5" s="70" t="b">
+      <c r="F5" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="70" t="b">
+      <c r="G5" s="71" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13064,15 +13068,15 @@
       <c r="D6" s="11" t="s">
         <v>730</v>
       </c>
-      <c r="E6" s="70" t="b">
+      <c r="E6" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F6" s="70" t="b">
+      <c r="F6" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G6" s="70" t="b">
+      <c r="G6" s="71" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13093,15 +13097,15 @@
       <c r="D7" s="11" t="s">
         <v>729</v>
       </c>
-      <c r="E7" s="70" t="b">
+      <c r="E7" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F7" s="70" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G7" s="56"/>
+      <c r="F7" s="71" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="57"/>
       <c r="H7" s="11" t="s">
         <v>727</v>
       </c>
@@ -13119,15 +13123,15 @@
       <c r="D8" s="11" t="s">
         <v>739</v>
       </c>
-      <c r="E8" s="70" t="b">
+      <c r="E8" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F8" s="70" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="56"/>
+      <c r="F8" s="71" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="57"/>
       <c r="H8" s="11" t="s">
         <v>727</v>
       </c>
@@ -13145,15 +13149,15 @@
       <c r="D9" s="11" t="s">
         <v>742</v>
       </c>
-      <c r="E9" s="70" t="b">
+      <c r="E9" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F9" s="70" t="b">
+      <c r="F9" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G9" s="70" t="b">
+      <c r="G9" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -13174,15 +13178,15 @@
       <c r="D10" s="11" t="s">
         <v>745</v>
       </c>
-      <c r="E10" s="70" t="b">
+      <c r="E10" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F10" s="70" t="b">
+      <c r="F10" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G10" s="70" t="b">
+      <c r="G10" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -13203,15 +13207,15 @@
       <c r="D11" s="11" t="s">
         <v>748</v>
       </c>
-      <c r="E11" s="70" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F11" s="70" t="b">
+      <c r="E11" s="71" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G11" s="70" t="b">
+      <c r="G11" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -13229,15 +13233,15 @@
       <c r="D12" s="11" t="s">
         <v>751</v>
       </c>
-      <c r="E12" s="70" t="b">
+      <c r="E12" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F12" s="70" t="b">
+      <c r="F12" s="71" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G12" s="70" t="b">
+      <c r="G12" s="71" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13269,2050 +13273,2050 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="71" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="71" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="71" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="71" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="71" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="71" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="72" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="72" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="72" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="72" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="72" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="72" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="72" t="s">
+      <c r="A1" s="73" t="s">
         <v>752</v>
       </c>
-      <c r="B1" s="72" t="s">
+      <c r="B1" s="73" t="s">
         <v>671</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="72" t="s">
+      <c r="D1" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="73" t="s">
+      <c r="E1" s="74" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="73" t="s">
+      <c r="F1" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="73" t="s">
         <v>753</v>
       </c>
-      <c r="H1" s="72" t="s">
+      <c r="H1" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="71" t="s">
+      <c r="I1" s="72" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="74" t="s">
+      <c r="A2" s="75" t="s">
         <v>678</v>
       </c>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="75" t="s">
         <v>678</v>
       </c>
-      <c r="C2" s="74" t="s">
+      <c r="C2" s="75" t="s">
         <v>755</v>
       </c>
-      <c r="D2" s="74" t="s">
+      <c r="D2" s="75" t="s">
         <v>756</v>
       </c>
-      <c r="E2" s="74"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="74"/>
-      <c r="H2" s="74"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="74" t="s">
+      <c r="A3" s="75" t="s">
         <v>757</v>
       </c>
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="75" t="s">
         <v>757</v>
       </c>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="75" t="s">
         <v>758</v>
       </c>
-      <c r="D3" s="74" t="s">
+      <c r="D3" s="75" t="s">
         <v>759</v>
       </c>
-      <c r="E3" s="74"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-      <c r="H3" s="74"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="75"/>
+      <c r="H3" s="75"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="B4" s="74" t="s">
+      <c r="B4" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="C4" s="74" t="s">
+      <c r="C4" s="75" t="s">
         <v>760</v>
       </c>
-      <c r="D4" s="74" t="s">
+      <c r="D4" s="75" t="s">
         <v>761</v>
       </c>
-      <c r="E4" s="74"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-      <c r="H4" s="74"/>
+      <c r="E4" s="75"/>
+      <c r="F4" s="75"/>
+      <c r="G4" s="75"/>
+      <c r="H4" s="75"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="74" t="s">
+      <c r="A5" s="75" t="s">
         <v>762</v>
       </c>
-      <c r="B5" s="74" t="s">
+      <c r="B5" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="C5" s="74" t="s">
+      <c r="C5" s="75" t="s">
         <v>763</v>
       </c>
-      <c r="D5" s="74" t="s">
+      <c r="D5" s="75" t="s">
         <v>764</v>
       </c>
-      <c r="E5" s="74"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-      <c r="H5" s="74"/>
+      <c r="E5" s="75"/>
+      <c r="F5" s="75"/>
+      <c r="G5" s="75"/>
+      <c r="H5" s="75"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="74" t="s">
+      <c r="A6" s="75" t="s">
         <v>765</v>
       </c>
-      <c r="B6" s="74" t="s">
+      <c r="B6" s="75" t="s">
         <v>765</v>
       </c>
-      <c r="C6" s="74" t="s">
+      <c r="C6" s="75" t="s">
         <v>766</v>
       </c>
-      <c r="D6" s="74" t="s">
+      <c r="D6" s="75" t="s">
         <v>767</v>
       </c>
-      <c r="E6" s="74"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="74"/>
-      <c r="H6" s="74"/>
+      <c r="E6" s="75"/>
+      <c r="F6" s="75"/>
+      <c r="G6" s="75"/>
+      <c r="H6" s="75"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="74" t="s">
+      <c r="A7" s="75" t="s">
         <v>682</v>
       </c>
-      <c r="B7" s="74" t="s">
+      <c r="B7" s="75" t="s">
         <v>682</v>
       </c>
-      <c r="C7" s="74" t="s">
+      <c r="C7" s="75" t="s">
         <v>768</v>
       </c>
-      <c r="D7" s="74" t="s">
+      <c r="D7" s="75" t="s">
         <v>769</v>
       </c>
-      <c r="E7" s="74"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="74"/>
-      <c r="H7" s="74"/>
+      <c r="E7" s="75"/>
+      <c r="F7" s="75"/>
+      <c r="G7" s="75"/>
+      <c r="H7" s="75"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B8" s="74"/>
-      <c r="C8" s="74"/>
-      <c r="D8" s="74"/>
-      <c r="E8" s="74"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="74" t="s">
+      <c r="B8" s="75"/>
+      <c r="C8" s="75"/>
+      <c r="D8" s="75"/>
+      <c r="E8" s="75"/>
+      <c r="F8" s="75"/>
+      <c r="G8" s="75" t="s">
         <v>678</v>
       </c>
-      <c r="H8" s="74"/>
+      <c r="H8" s="75"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="74" t="s">
+      <c r="A9" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="B9" s="74"/>
-      <c r="C9" s="74"/>
-      <c r="D9" s="74"/>
-      <c r="E9" s="74"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="74" t="s">
+      <c r="B9" s="75"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75" t="s">
         <v>757</v>
       </c>
-      <c r="H9" s="74"/>
+      <c r="H9" s="75"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="75" t="s">
         <v>183</v>
       </c>
-      <c r="B10" s="74"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74" t="s">
+      <c r="B10" s="75"/>
+      <c r="C10" s="75"/>
+      <c r="D10" s="75"/>
+      <c r="E10" s="75"/>
+      <c r="F10" s="75"/>
+      <c r="G10" s="75" t="s">
         <v>36</v>
       </c>
-      <c r="H10" s="74"/>
+      <c r="H10" s="75"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="74" t="s">
+      <c r="A11" s="75" t="s">
         <v>183</v>
       </c>
-      <c r="B11" s="74"/>
-      <c r="C11" s="74"/>
-      <c r="D11" s="74"/>
-      <c r="E11" s="74"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="74" t="s">
+      <c r="B11" s="75"/>
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75" t="s">
         <v>765</v>
       </c>
-      <c r="H11" s="74"/>
+      <c r="H11" s="75"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="74" t="s">
+      <c r="A12" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="B12" s="74"/>
-      <c r="C12" s="74"/>
-      <c r="D12" s="74"/>
-      <c r="E12" s="74"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="74" t="s">
+      <c r="B12" s="75"/>
+      <c r="C12" s="75"/>
+      <c r="D12" s="75"/>
+      <c r="E12" s="75"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="75" t="s">
         <v>678</v>
       </c>
-      <c r="H12" s="74"/>
+      <c r="H12" s="75"/>
     </row>
     <row r="13" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="74" t="s">
+      <c r="A13" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="B13" s="74"/>
-      <c r="C13" s="74"/>
-      <c r="D13" s="74"/>
-      <c r="E13" s="74"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="74" t="s">
+      <c r="B13" s="75"/>
+      <c r="C13" s="75"/>
+      <c r="D13" s="75"/>
+      <c r="E13" s="75"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="75" t="s">
         <v>757</v>
       </c>
-      <c r="H13" s="74"/>
-      <c r="I13" s="71"/>
+      <c r="H13" s="75"/>
+      <c r="I13" s="72"/>
     </row>
     <row r="14" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="74" t="s">
+      <c r="A14" s="75" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="74"/>
-      <c r="C14" s="74"/>
-      <c r="D14" s="74"/>
-      <c r="E14" s="74"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="74" t="s">
+      <c r="B14" s="75"/>
+      <c r="C14" s="75"/>
+      <c r="D14" s="75"/>
+      <c r="E14" s="75"/>
+      <c r="F14" s="75"/>
+      <c r="G14" s="75" t="s">
         <v>682</v>
       </c>
-      <c r="H14" s="74"/>
-      <c r="I14" s="71"/>
+      <c r="H14" s="75"/>
+      <c r="I14" s="72"/>
     </row>
     <row r="15" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="74" t="s">
+      <c r="A15" s="75" t="s">
         <v>556</v>
       </c>
-      <c r="B15" s="74"/>
-      <c r="C15" s="74"/>
-      <c r="D15" s="74"/>
-      <c r="E15" s="74"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="74" t="s">
+      <c r="B15" s="75"/>
+      <c r="C15" s="75"/>
+      <c r="D15" s="75"/>
+      <c r="E15" s="75"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="75" t="s">
         <v>678</v>
       </c>
-      <c r="H15" s="74"/>
-      <c r="I15" s="71"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="72"/>
     </row>
     <row r="16" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="74" t="s">
+      <c r="A16" s="75" t="s">
         <v>556</v>
       </c>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="75" t="s">
         <v>770</v>
       </c>
-      <c r="C16" s="74" t="s">
+      <c r="C16" s="75" t="s">
         <v>771</v>
       </c>
-      <c r="D16" s="74" t="s">
+      <c r="D16" s="75" t="s">
         <v>772</v>
       </c>
-      <c r="E16" s="74"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="74"/>
-      <c r="H16" s="74"/>
-      <c r="I16" s="71"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="75"/>
+      <c r="G16" s="75"/>
+      <c r="H16" s="75"/>
+      <c r="I16" s="72"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="74" t="s">
+      <c r="A17" s="75" t="s">
         <v>556</v>
       </c>
-      <c r="B17" s="74"/>
-      <c r="C17" s="74"/>
-      <c r="D17" s="74"/>
-      <c r="E17" s="74"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="74" t="s">
+      <c r="B17" s="75"/>
+      <c r="C17" s="75"/>
+      <c r="D17" s="75"/>
+      <c r="E17" s="75"/>
+      <c r="F17" s="75"/>
+      <c r="G17" s="75" t="s">
         <v>765</v>
       </c>
-      <c r="H17" s="74"/>
+      <c r="H17" s="75"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="75" t="s">
+      <c r="A18" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="B18" s="74" t="s">
+      <c r="B18" s="75" t="s">
         <v>773</v>
       </c>
-      <c r="C18" s="74" t="s">
+      <c r="C18" s="75" t="s">
         <v>774</v>
       </c>
-      <c r="D18" s="74" t="s">
+      <c r="D18" s="75" t="s">
         <v>775</v>
       </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="74"/>
-      <c r="H18" s="74"/>
+      <c r="E18" s="75"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="75"/>
+      <c r="H18" s="75"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="75" t="s">
+      <c r="A19" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="B19" s="74" t="s">
+      <c r="B19" s="75" t="s">
         <v>776</v>
       </c>
-      <c r="C19" s="74" t="s">
+      <c r="C19" s="75" t="s">
         <v>777</v>
       </c>
-      <c r="D19" s="74" t="s">
+      <c r="D19" s="75" t="s">
         <v>778</v>
       </c>
-      <c r="E19" s="74"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="74"/>
-      <c r="H19" s="74"/>
+      <c r="E19" s="75"/>
+      <c r="F19" s="75"/>
+      <c r="G19" s="75"/>
+      <c r="H19" s="75"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="75" t="s">
+      <c r="A20" s="76" t="s">
         <v>133</v>
       </c>
-      <c r="B20" s="74"/>
-      <c r="C20" s="74"/>
-      <c r="D20" s="74"/>
-      <c r="E20" s="74"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="74" t="s">
+      <c r="B20" s="75"/>
+      <c r="C20" s="75"/>
+      <c r="D20" s="75"/>
+      <c r="E20" s="75"/>
+      <c r="F20" s="75"/>
+      <c r="G20" s="75" t="s">
         <v>682</v>
       </c>
-      <c r="H20" s="74"/>
+      <c r="H20" s="75"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="75" t="s">
+      <c r="A21" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="B21" s="74" t="s">
+      <c r="B21" s="75" t="s">
         <v>773</v>
       </c>
-      <c r="C21" s="74" t="s">
+      <c r="C21" s="75" t="s">
         <v>774</v>
       </c>
-      <c r="D21" s="74" t="s">
+      <c r="D21" s="75" t="s">
         <v>779</v>
       </c>
-      <c r="E21" s="74"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="74"/>
-      <c r="H21" s="74"/>
+      <c r="E21" s="75"/>
+      <c r="F21" s="75"/>
+      <c r="G21" s="75"/>
+      <c r="H21" s="75"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="B22" s="74" t="s">
+      <c r="B22" s="75" t="s">
         <v>776</v>
       </c>
-      <c r="C22" s="74" t="s">
+      <c r="C22" s="75" t="s">
         <v>777</v>
       </c>
-      <c r="D22" s="74" t="s">
+      <c r="D22" s="75" t="s">
         <v>780</v>
       </c>
-      <c r="E22" s="74"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="74"/>
-      <c r="H22" s="74"/>
+      <c r="E22" s="75"/>
+      <c r="F22" s="75"/>
+      <c r="G22" s="75"/>
+      <c r="H22" s="75"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="B23" s="74" t="s">
+      <c r="B23" s="75" t="s">
         <v>141</v>
       </c>
-      <c r="C23" s="74" t="s">
+      <c r="C23" s="75" t="s">
         <v>781</v>
       </c>
-      <c r="D23" s="74" t="s">
+      <c r="D23" s="75" t="s">
         <v>782</v>
       </c>
-      <c r="E23" s="74"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="74"/>
-      <c r="H23" s="74"/>
+      <c r="E23" s="75"/>
+      <c r="F23" s="75"/>
+      <c r="G23" s="75"/>
+      <c r="H23" s="75"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="76" t="s">
         <v>139</v>
       </c>
-      <c r="B24" s="74"/>
-      <c r="C24" s="74"/>
-      <c r="D24" s="74"/>
-      <c r="E24" s="74"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="74" t="s">
+      <c r="B24" s="75"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="75"/>
+      <c r="E24" s="75"/>
+      <c r="F24" s="75"/>
+      <c r="G24" s="75" t="s">
         <v>682</v>
       </c>
-      <c r="H24" s="74"/>
+      <c r="H24" s="75"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="74" t="s">
+      <c r="A25" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="B25" s="74" t="s">
+      <c r="B25" s="75" t="s">
         <v>712</v>
       </c>
-      <c r="C25" s="74" t="s">
+      <c r="C25" s="75" t="s">
         <v>783</v>
       </c>
-      <c r="D25" s="74" t="s">
+      <c r="D25" s="75" t="s">
         <v>784</v>
       </c>
-      <c r="E25" s="74"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="74"/>
-      <c r="H25" s="74"/>
+      <c r="E25" s="75"/>
+      <c r="F25" s="75"/>
+      <c r="G25" s="75"/>
+      <c r="H25" s="75"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="74" t="s">
+      <c r="A26" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="B26" s="74" t="s">
+      <c r="B26" s="75" t="s">
         <v>713</v>
       </c>
-      <c r="C26" s="74" t="s">
+      <c r="C26" s="75" t="s">
         <v>785</v>
       </c>
-      <c r="D26" s="74" t="s">
+      <c r="D26" s="75" t="s">
         <v>786</v>
       </c>
-      <c r="E26" s="74"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="74"/>
-      <c r="H26" s="74"/>
+      <c r="E26" s="75"/>
+      <c r="F26" s="75"/>
+      <c r="G26" s="75"/>
+      <c r="H26" s="75"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="74" t="s">
+      <c r="A27" s="75" t="s">
         <v>148</v>
       </c>
-      <c r="B27" s="74"/>
-      <c r="C27" s="74"/>
-      <c r="D27" s="74"/>
-      <c r="E27" s="74"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="74" t="s">
+      <c r="B27" s="75"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="75"/>
+      <c r="F27" s="75"/>
+      <c r="G27" s="75" t="s">
         <v>757</v>
       </c>
-      <c r="H27" s="74"/>
+      <c r="H27" s="75"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="74" t="s">
+      <c r="A28" s="75" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="74" t="s">
+      <c r="B28" s="75" t="s">
         <v>712</v>
       </c>
-      <c r="C28" s="74" t="s">
+      <c r="C28" s="75" t="s">
         <v>787</v>
       </c>
-      <c r="D28" s="74" t="s">
+      <c r="D28" s="75" t="s">
         <v>788</v>
       </c>
-      <c r="E28" s="74"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="74"/>
-      <c r="H28" s="74"/>
+      <c r="E28" s="75"/>
+      <c r="F28" s="75"/>
+      <c r="G28" s="75"/>
+      <c r="H28" s="75"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="74" t="s">
+      <c r="A29" s="75" t="s">
         <v>154</v>
       </c>
-      <c r="B29" s="74" t="s">
+      <c r="B29" s="75" t="s">
         <v>713</v>
       </c>
-      <c r="C29" s="74" t="s">
+      <c r="C29" s="75" t="s">
         <v>789</v>
       </c>
-      <c r="D29" s="74" t="s">
+      <c r="D29" s="75" t="s">
         <v>790</v>
       </c>
-      <c r="E29" s="74"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="74"/>
-      <c r="H29" s="74"/>
+      <c r="E29" s="75"/>
+      <c r="F29" s="75"/>
+      <c r="G29" s="75"/>
+      <c r="H29" s="75"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="74" t="s">
+      <c r="A30" s="75" t="s">
         <v>154</v>
       </c>
-      <c r="B30" s="74"/>
-      <c r="C30" s="74"/>
-      <c r="D30" s="74"/>
-      <c r="E30" s="74"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="74" t="s">
+      <c r="B30" s="75"/>
+      <c r="C30" s="75"/>
+      <c r="D30" s="75"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="75"/>
+      <c r="G30" s="75" t="s">
         <v>757</v>
       </c>
-      <c r="H30" s="74"/>
+      <c r="H30" s="75"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="74" t="s">
+      <c r="A31" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="B31" s="74" t="s">
+      <c r="B31" s="75" t="s">
         <v>791</v>
       </c>
-      <c r="C31" s="74" t="s">
+      <c r="C31" s="75" t="s">
         <v>792</v>
       </c>
-      <c r="D31" s="74" t="s">
+      <c r="D31" s="75" t="s">
         <v>793</v>
       </c>
-      <c r="E31" s="74"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="74"/>
-      <c r="H31" s="74" t="s">
+      <c r="E31" s="75"/>
+      <c r="F31" s="75"/>
+      <c r="G31" s="75"/>
+      <c r="H31" s="75" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="74" t="s">
+      <c r="A32" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="B32" s="74" t="s">
+      <c r="B32" s="75" t="s">
         <v>794</v>
       </c>
-      <c r="C32" s="74" t="s">
+      <c r="C32" s="75" t="s">
         <v>795</v>
       </c>
-      <c r="D32" s="74" t="s">
+      <c r="D32" s="75" t="s">
         <v>796</v>
       </c>
-      <c r="E32" s="74"/>
-      <c r="F32" s="74"/>
-      <c r="G32" s="74"/>
-      <c r="H32" s="74" t="s">
+      <c r="E32" s="75"/>
+      <c r="F32" s="75"/>
+      <c r="G32" s="75"/>
+      <c r="H32" s="75" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="74" t="s">
+      <c r="A33" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="B33" s="74" t="s">
+      <c r="B33" s="75" t="s">
         <v>797</v>
       </c>
-      <c r="C33" s="74" t="s">
+      <c r="C33" s="75" t="s">
         <v>798</v>
       </c>
-      <c r="D33" s="74" t="s">
+      <c r="D33" s="75" t="s">
         <v>799</v>
       </c>
-      <c r="E33" s="74"/>
-      <c r="F33" s="74"/>
-      <c r="G33" s="74"/>
-      <c r="H33" s="74" t="s">
+      <c r="E33" s="75"/>
+      <c r="F33" s="75"/>
+      <c r="G33" s="75"/>
+      <c r="H33" s="75" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="74" t="s">
+      <c r="A34" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="B34" s="74" t="s">
+      <c r="B34" s="75" t="s">
         <v>800</v>
       </c>
-      <c r="C34" s="74" t="s">
+      <c r="C34" s="75" t="s">
         <v>801</v>
       </c>
-      <c r="D34" s="74" t="s">
+      <c r="D34" s="75" t="s">
         <v>802</v>
       </c>
-      <c r="E34" s="74"/>
-      <c r="F34" s="74"/>
-      <c r="G34" s="74"/>
-      <c r="H34" s="74" t="s">
+      <c r="E34" s="75"/>
+      <c r="F34" s="75"/>
+      <c r="G34" s="75"/>
+      <c r="H34" s="75" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="74" t="s">
+      <c r="A35" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="B35" s="74" t="s">
+      <c r="B35" s="75" t="s">
         <v>803</v>
       </c>
-      <c r="C35" s="74" t="s">
+      <c r="C35" s="75" t="s">
         <v>804</v>
       </c>
-      <c r="D35" s="74" t="s">
+      <c r="D35" s="75" t="s">
         <v>805</v>
       </c>
-      <c r="E35" s="74"/>
-      <c r="F35" s="74"/>
-      <c r="G35" s="74"/>
-      <c r="H35" s="74" t="s">
+      <c r="E35" s="75"/>
+      <c r="F35" s="75"/>
+      <c r="G35" s="75"/>
+      <c r="H35" s="75" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="74" t="s">
+      <c r="A36" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="B36" s="74" t="s">
+      <c r="B36" s="75" t="s">
         <v>806</v>
       </c>
-      <c r="C36" s="74" t="s">
+      <c r="C36" s="75" t="s">
         <v>807</v>
       </c>
-      <c r="D36" s="74" t="s">
+      <c r="D36" s="75" t="s">
         <v>808</v>
       </c>
-      <c r="E36" s="74"/>
-      <c r="F36" s="74"/>
-      <c r="G36" s="74"/>
-      <c r="H36" s="74" t="s">
+      <c r="E36" s="75"/>
+      <c r="F36" s="75"/>
+      <c r="G36" s="75"/>
+      <c r="H36" s="75" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="74" t="s">
+      <c r="A37" s="75" t="s">
         <v>156</v>
       </c>
-      <c r="B37" s="74"/>
-      <c r="C37" s="74"/>
-      <c r="D37" s="74"/>
-      <c r="E37" s="74"/>
-      <c r="F37" s="74"/>
-      <c r="G37" s="74" t="s">
+      <c r="B37" s="75"/>
+      <c r="C37" s="75"/>
+      <c r="D37" s="75"/>
+      <c r="E37" s="75"/>
+      <c r="F37" s="75"/>
+      <c r="G37" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="H37" s="74"/>
+      <c r="H37" s="75"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="74" t="s">
+      <c r="A38" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B38" s="74" t="s">
+      <c r="B38" s="75" t="s">
         <v>697</v>
       </c>
-      <c r="C38" s="74" t="s">
+      <c r="C38" s="75" t="s">
         <v>809</v>
       </c>
-      <c r="D38" s="74" t="s">
+      <c r="D38" s="75" t="s">
         <v>810</v>
       </c>
-      <c r="E38" s="74"/>
-      <c r="F38" s="74"/>
-      <c r="G38" s="74"/>
-      <c r="H38" s="74"/>
-      <c r="I38" s="71" t="s">
+      <c r="E38" s="75"/>
+      <c r="F38" s="75"/>
+      <c r="G38" s="75"/>
+      <c r="H38" s="75"/>
+      <c r="I38" s="72" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="74" t="s">
+      <c r="A39" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B39" s="74" t="s">
+      <c r="B39" s="75" t="s">
         <v>698</v>
       </c>
-      <c r="C39" s="74" t="s">
+      <c r="C39" s="75" t="s">
         <v>812</v>
       </c>
-      <c r="D39" s="74" t="s">
+      <c r="D39" s="75" t="s">
         <v>813</v>
       </c>
-      <c r="E39" s="74"/>
-      <c r="F39" s="74"/>
-      <c r="G39" s="74"/>
-      <c r="H39" s="74"/>
-      <c r="I39" s="71" t="s">
+      <c r="E39" s="75"/>
+      <c r="F39" s="75"/>
+      <c r="G39" s="75"/>
+      <c r="H39" s="75"/>
+      <c r="I39" s="72" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="74" t="s">
+      <c r="A40" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B40" s="74" t="s">
+      <c r="B40" s="75" t="s">
         <v>699</v>
       </c>
-      <c r="C40" s="74" t="s">
+      <c r="C40" s="75" t="s">
         <v>814</v>
       </c>
-      <c r="D40" s="74" t="s">
+      <c r="D40" s="75" t="s">
         <v>815</v>
       </c>
-      <c r="E40" s="74"/>
-      <c r="F40" s="74"/>
-      <c r="G40" s="74"/>
-      <c r="H40" s="74"/>
-      <c r="I40" s="71" t="s">
+      <c r="E40" s="75"/>
+      <c r="F40" s="75"/>
+      <c r="G40" s="75"/>
+      <c r="H40" s="75"/>
+      <c r="I40" s="72" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="74" t="s">
+      <c r="A41" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B41" s="74" t="s">
+      <c r="B41" s="75" t="s">
         <v>700</v>
       </c>
-      <c r="C41" s="74" t="s">
+      <c r="C41" s="75" t="s">
         <v>816</v>
       </c>
-      <c r="D41" s="74" t="s">
+      <c r="D41" s="75" t="s">
         <v>817</v>
       </c>
-      <c r="E41" s="74"/>
-      <c r="F41" s="74"/>
-      <c r="G41" s="74"/>
-      <c r="H41" s="74"/>
-      <c r="I41" s="71" t="s">
+      <c r="E41" s="75"/>
+      <c r="F41" s="75"/>
+      <c r="G41" s="75"/>
+      <c r="H41" s="75"/>
+      <c r="I41" s="72" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="74" t="s">
+      <c r="A42" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B42" s="74" t="s">
+      <c r="B42" s="75" t="s">
         <v>701</v>
       </c>
-      <c r="C42" s="74" t="s">
+      <c r="C42" s="75" t="s">
         <v>818</v>
       </c>
-      <c r="D42" s="74" t="s">
+      <c r="D42" s="75" t="s">
         <v>819</v>
       </c>
-      <c r="E42" s="74"/>
-      <c r="F42" s="74"/>
-      <c r="G42" s="74"/>
-      <c r="H42" s="74"/>
-      <c r="I42" s="71" t="s">
+      <c r="E42" s="75"/>
+      <c r="F42" s="75"/>
+      <c r="G42" s="75"/>
+      <c r="H42" s="75"/>
+      <c r="I42" s="72" t="s">
         <v>811</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="74" t="s">
+      <c r="A43" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B43" s="74" t="s">
+      <c r="B43" s="75" t="s">
         <v>820</v>
       </c>
-      <c r="C43" s="74" t="s">
+      <c r="C43" s="75" t="s">
         <v>821</v>
       </c>
-      <c r="D43" s="74" t="s">
+      <c r="D43" s="75" t="s">
         <v>822</v>
       </c>
-      <c r="E43" s="74"/>
-      <c r="F43" s="74"/>
-      <c r="G43" s="74"/>
-      <c r="H43" s="74" t="s">
+      <c r="E43" s="75"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="75"/>
+      <c r="H43" s="75" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="74" t="s">
+      <c r="A44" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B44" s="74" t="s">
+      <c r="B44" s="75" t="s">
         <v>803</v>
       </c>
-      <c r="C44" s="74" t="s">
+      <c r="C44" s="75" t="s">
         <v>804</v>
       </c>
-      <c r="D44" s="74" t="s">
+      <c r="D44" s="75" t="s">
         <v>805</v>
       </c>
-      <c r="E44" s="74"/>
-      <c r="F44" s="74"/>
-      <c r="G44" s="74"/>
-      <c r="H44" s="74"/>
+      <c r="E44" s="75"/>
+      <c r="F44" s="75"/>
+      <c r="G44" s="75"/>
+      <c r="H44" s="75"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="74" t="s">
+      <c r="A45" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B45" s="74" t="s">
+      <c r="B45" s="75" t="s">
         <v>823</v>
       </c>
-      <c r="C45" s="74" t="s">
+      <c r="C45" s="75" t="s">
         <v>824</v>
       </c>
-      <c r="D45" s="74" t="s">
+      <c r="D45" s="75" t="s">
         <v>825</v>
       </c>
-      <c r="E45" s="74"/>
-      <c r="F45" s="74"/>
-      <c r="G45" s="74"/>
-      <c r="H45" s="74"/>
+      <c r="E45" s="75"/>
+      <c r="F45" s="75"/>
+      <c r="G45" s="75"/>
+      <c r="H45" s="75"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="74" t="s">
+      <c r="A46" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B46" s="76" t="s">
+      <c r="B46" s="77" t="s">
         <v>710</v>
       </c>
-      <c r="C46" s="74" t="s">
+      <c r="C46" s="75" t="s">
         <v>826</v>
       </c>
-      <c r="D46" s="74" t="s">
+      <c r="D46" s="75" t="s">
         <v>827</v>
       </c>
-      <c r="E46" s="74"/>
-      <c r="F46" s="74"/>
-      <c r="G46" s="74"/>
-      <c r="H46" s="74"/>
+      <c r="E46" s="75"/>
+      <c r="F46" s="75"/>
+      <c r="G46" s="75"/>
+      <c r="H46" s="75"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="74" t="s">
+      <c r="A47" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B47" s="74" t="s">
+      <c r="B47" s="75" t="s">
         <v>828</v>
       </c>
-      <c r="C47" s="74" t="s">
+      <c r="C47" s="75" t="s">
         <v>829</v>
       </c>
-      <c r="D47" s="74" t="s">
+      <c r="D47" s="75" t="s">
         <v>830</v>
       </c>
-      <c r="E47" s="74"/>
-      <c r="F47" s="74"/>
-      <c r="G47" s="74"/>
-      <c r="H47" s="74"/>
+      <c r="E47" s="75"/>
+      <c r="F47" s="75"/>
+      <c r="G47" s="75"/>
+      <c r="H47" s="75"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="74" t="s">
+      <c r="A48" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B48" s="74" t="s">
+      <c r="B48" s="75" t="s">
         <v>831</v>
       </c>
-      <c r="C48" s="74" t="s">
+      <c r="C48" s="75" t="s">
         <v>832</v>
       </c>
-      <c r="D48" s="74" t="s">
+      <c r="D48" s="75" t="s">
         <v>833</v>
       </c>
-      <c r="E48" s="74"/>
-      <c r="F48" s="74"/>
-      <c r="G48" s="74"/>
-      <c r="H48" s="74"/>
+      <c r="E48" s="75"/>
+      <c r="F48" s="75"/>
+      <c r="G48" s="75"/>
+      <c r="H48" s="75"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="74" t="s">
+      <c r="A49" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B49" s="74" t="s">
+      <c r="B49" s="75" t="s">
         <v>161</v>
       </c>
-      <c r="C49" s="74" t="s">
+      <c r="C49" s="75" t="s">
         <v>763</v>
       </c>
-      <c r="D49" s="74" t="s">
+      <c r="D49" s="75" t="s">
         <v>764</v>
       </c>
-      <c r="E49" s="74"/>
-      <c r="F49" s="74"/>
-      <c r="G49" s="74"/>
-      <c r="H49" s="74"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="75"/>
+      <c r="H49" s="75"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="74" t="s">
+      <c r="A50" s="75" t="s">
         <v>162</v>
       </c>
-      <c r="B50" s="74" t="s">
+      <c r="B50" s="75" t="s">
         <v>682</v>
       </c>
-      <c r="C50" s="74" t="s">
+      <c r="C50" s="75" t="s">
         <v>834</v>
       </c>
-      <c r="D50" s="74" t="s">
+      <c r="D50" s="75" t="s">
         <v>835</v>
       </c>
-      <c r="E50" s="74"/>
-      <c r="F50" s="74"/>
-      <c r="G50" s="74"/>
-      <c r="H50" s="74"/>
+      <c r="E50" s="75"/>
+      <c r="F50" s="75"/>
+      <c r="G50" s="75"/>
+      <c r="H50" s="75"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="74" t="s">
+      <c r="A51" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="B51" s="74"/>
-      <c r="C51" s="74"/>
-      <c r="D51" s="74"/>
-      <c r="E51" s="74"/>
-      <c r="F51" s="74"/>
-      <c r="G51" s="74" t="s">
+      <c r="B51" s="75"/>
+      <c r="C51" s="75"/>
+      <c r="D51" s="75"/>
+      <c r="E51" s="75"/>
+      <c r="F51" s="75"/>
+      <c r="G51" s="75" t="s">
         <v>757</v>
       </c>
-      <c r="H51" s="74"/>
+      <c r="H51" s="75"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="74" t="s">
+      <c r="A52" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="B52" s="74" t="s">
+      <c r="B52" s="75" t="s">
         <v>836</v>
       </c>
-      <c r="C52" s="74" t="s">
+      <c r="C52" s="75" t="s">
         <v>837</v>
       </c>
-      <c r="D52" s="74" t="s">
+      <c r="D52" s="75" t="s">
         <v>838</v>
       </c>
-      <c r="E52" s="74"/>
-      <c r="F52" s="74"/>
-      <c r="G52" s="74"/>
-      <c r="H52" s="74"/>
+      <c r="E52" s="75"/>
+      <c r="F52" s="75"/>
+      <c r="G52" s="75"/>
+      <c r="H52" s="75"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="74" t="s">
+      <c r="A53" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="B53" s="74" t="s">
+      <c r="B53" s="75" t="s">
         <v>839</v>
       </c>
-      <c r="C53" s="74" t="s">
+      <c r="C53" s="75" t="s">
         <v>840</v>
       </c>
-      <c r="D53" s="74" t="s">
+      <c r="D53" s="75" t="s">
         <v>841</v>
       </c>
-      <c r="E53" s="74"/>
-      <c r="F53" s="74"/>
-      <c r="G53" s="74"/>
-      <c r="H53" s="74"/>
+      <c r="E53" s="75"/>
+      <c r="F53" s="75"/>
+      <c r="G53" s="75"/>
+      <c r="H53" s="75"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="74" t="s">
+      <c r="A54" s="75" t="s">
         <v>198</v>
       </c>
-      <c r="B54" s="74"/>
-      <c r="C54" s="74"/>
-      <c r="D54" s="74"/>
-      <c r="E54" s="74"/>
-      <c r="F54" s="74"/>
-      <c r="G54" s="74" t="s">
+      <c r="B54" s="75"/>
+      <c r="C54" s="75"/>
+      <c r="D54" s="75"/>
+      <c r="E54" s="75"/>
+      <c r="F54" s="75"/>
+      <c r="G54" s="75" t="s">
         <v>765</v>
       </c>
-      <c r="H54" s="74"/>
+      <c r="H54" s="75"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="75" t="s">
+      <c r="A55" s="76" t="s">
         <v>206</v>
       </c>
-      <c r="B55" s="74" t="s">
+      <c r="B55" s="75" t="s">
         <v>703</v>
       </c>
-      <c r="C55" s="74" t="s">
+      <c r="C55" s="75" t="s">
         <v>842</v>
       </c>
-      <c r="D55" s="74" t="s">
+      <c r="D55" s="75" t="s">
         <v>843</v>
       </c>
-      <c r="E55" s="74"/>
-      <c r="F55" s="74"/>
-      <c r="G55" s="74"/>
-      <c r="H55" s="74"/>
+      <c r="E55" s="75"/>
+      <c r="F55" s="75"/>
+      <c r="G55" s="75"/>
+      <c r="H55" s="75"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="75" t="s">
+      <c r="A56" s="76" t="s">
         <v>206</v>
       </c>
-      <c r="B56" s="74" t="s">
+      <c r="B56" s="75" t="s">
         <v>704</v>
       </c>
-      <c r="C56" s="74" t="s">
+      <c r="C56" s="75" t="s">
         <v>844</v>
       </c>
-      <c r="D56" s="74" t="s">
+      <c r="D56" s="75" t="s">
         <v>845</v>
       </c>
-      <c r="E56" s="74"/>
-      <c r="F56" s="74"/>
-      <c r="G56" s="74"/>
-      <c r="H56" s="74"/>
+      <c r="E56" s="75"/>
+      <c r="F56" s="75"/>
+      <c r="G56" s="75"/>
+      <c r="H56" s="75"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="75" t="s">
+      <c r="A57" s="76" t="s">
         <v>206</v>
       </c>
-      <c r="B57" s="74" t="s">
+      <c r="B57" s="75" t="s">
         <v>705</v>
       </c>
-      <c r="C57" s="74" t="s">
+      <c r="C57" s="75" t="s">
         <v>846</v>
       </c>
-      <c r="D57" s="74" t="s">
+      <c r="D57" s="75" t="s">
         <v>847</v>
       </c>
-      <c r="E57" s="74"/>
-      <c r="F57" s="74"/>
-      <c r="G57" s="74"/>
-      <c r="H57" s="74"/>
+      <c r="E57" s="75"/>
+      <c r="F57" s="75"/>
+      <c r="G57" s="75"/>
+      <c r="H57" s="75"/>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="75" t="s">
+      <c r="A58" s="76" t="s">
         <v>206</v>
       </c>
-      <c r="B58" s="74" t="s">
+      <c r="B58" s="75" t="s">
         <v>848</v>
       </c>
-      <c r="C58" s="74" t="s">
+      <c r="C58" s="75" t="s">
         <v>849</v>
       </c>
-      <c r="D58" s="74" t="s">
+      <c r="D58" s="75" t="s">
         <v>850</v>
       </c>
-      <c r="E58" s="74"/>
-      <c r="F58" s="74"/>
-      <c r="G58" s="74"/>
-      <c r="H58" s="74"/>
+      <c r="E58" s="75"/>
+      <c r="F58" s="75"/>
+      <c r="G58" s="75"/>
+      <c r="H58" s="75"/>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="75" t="s">
+      <c r="A59" s="76" t="s">
         <v>206</v>
       </c>
-      <c r="B59" s="74" t="s">
+      <c r="B59" s="75" t="s">
         <v>709</v>
       </c>
-      <c r="C59" s="74" t="s">
+      <c r="C59" s="75" t="s">
         <v>851</v>
       </c>
-      <c r="D59" s="74" t="s">
+      <c r="D59" s="75" t="s">
         <v>852</v>
       </c>
-      <c r="E59" s="74"/>
-      <c r="F59" s="74"/>
-      <c r="G59" s="74"/>
-      <c r="H59" s="74"/>
+      <c r="E59" s="75"/>
+      <c r="F59" s="75"/>
+      <c r="G59" s="75"/>
+      <c r="H59" s="75"/>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="75" t="s">
+      <c r="A60" s="76" t="s">
         <v>222</v>
       </c>
-      <c r="B60" s="71" t="s">
+      <c r="B60" s="72" t="s">
         <v>703</v>
       </c>
-      <c r="C60" s="71" t="s">
+      <c r="C60" s="72" t="s">
         <v>853</v>
       </c>
-      <c r="D60" s="71" t="s">
+      <c r="D60" s="72" t="s">
         <v>843</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="75" t="s">
+      <c r="A61" s="76" t="s">
         <v>222</v>
       </c>
-      <c r="B61" s="71" t="s">
+      <c r="B61" s="72" t="s">
         <v>704</v>
       </c>
-      <c r="C61" s="71" t="s">
+      <c r="C61" s="72" t="s">
         <v>854</v>
       </c>
-      <c r="D61" s="71" t="s">
+      <c r="D61" s="72" t="s">
         <v>855</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="75" t="s">
+      <c r="A62" s="76" t="s">
         <v>222</v>
       </c>
-      <c r="B62" s="71" t="s">
+      <c r="B62" s="72" t="s">
         <v>709</v>
       </c>
-      <c r="C62" s="71" t="s">
+      <c r="C62" s="72" t="s">
         <v>856</v>
       </c>
-      <c r="D62" s="71" t="s">
+      <c r="D62" s="72" t="s">
         <v>857</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="75" t="s">
+      <c r="A63" s="76" t="s">
         <v>566</v>
       </c>
-      <c r="B63" s="71" t="s">
+      <c r="B63" s="72" t="s">
         <v>858</v>
       </c>
-      <c r="C63" s="71" t="s">
+      <c r="C63" s="72" t="s">
         <v>859</v>
       </c>
-      <c r="D63" s="71" t="s">
+      <c r="D63" s="72" t="s">
         <v>860</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="75" t="s">
+      <c r="A64" s="76" t="s">
         <v>566</v>
       </c>
-      <c r="B64" s="71" t="s">
+      <c r="B64" s="72" t="s">
         <v>861</v>
       </c>
-      <c r="C64" s="71" t="s">
+      <c r="C64" s="72" t="s">
         <v>862</v>
       </c>
-      <c r="D64" s="71" t="s">
+      <c r="D64" s="72" t="s">
         <v>863</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="75" t="s">
+      <c r="A65" s="76" t="s">
         <v>566</v>
       </c>
-      <c r="B65" s="71" t="s">
+      <c r="B65" s="72" t="s">
         <v>864</v>
       </c>
-      <c r="C65" s="71" t="s">
+      <c r="C65" s="72" t="s">
         <v>865</v>
       </c>
-      <c r="D65" s="71" t="s">
+      <c r="D65" s="72" t="s">
         <v>866</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A66" s="75" t="s">
+      <c r="A66" s="76" t="s">
         <v>566</v>
       </c>
-      <c r="B66" s="71" t="s">
+      <c r="B66" s="72" t="s">
         <v>867</v>
       </c>
-      <c r="C66" s="71" t="s">
+      <c r="C66" s="72" t="s">
         <v>868</v>
       </c>
-      <c r="D66" s="71" t="s">
+      <c r="D66" s="72" t="s">
         <v>869</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="71" t="s">
+      <c r="A67" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B67" s="71" t="s">
+      <c r="B67" s="72" t="s">
         <v>870</v>
       </c>
-      <c r="C67" s="71" t="s">
+      <c r="C67" s="72" t="s">
         <v>871</v>
       </c>
-      <c r="D67" s="71" t="s">
+      <c r="D67" s="72" t="s">
         <v>872</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="71" t="s">
+      <c r="A68" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B68" s="76" t="s">
+      <c r="B68" s="77" t="s">
         <v>873</v>
       </c>
-      <c r="C68" s="76" t="s">
+      <c r="C68" s="77" t="s">
         <v>874</v>
       </c>
-      <c r="D68" s="76" t="s">
+      <c r="D68" s="77" t="s">
         <v>875</v>
       </c>
-      <c r="E68" s="76"/>
-      <c r="F68" s="76"/>
+      <c r="E68" s="77"/>
+      <c r="F68" s="77"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="71" t="s">
+      <c r="A69" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B69" s="76" t="s">
+      <c r="B69" s="77" t="s">
         <v>876</v>
       </c>
-      <c r="C69" s="76" t="s">
+      <c r="C69" s="77" t="s">
         <v>877</v>
       </c>
-      <c r="D69" s="76" t="s">
+      <c r="D69" s="77" t="s">
         <v>878</v>
       </c>
-      <c r="E69" s="76"/>
-      <c r="F69" s="76"/>
+      <c r="E69" s="77"/>
+      <c r="F69" s="77"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="71" t="s">
+      <c r="A70" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B70" s="76" t="s">
+      <c r="B70" s="77" t="s">
         <v>879</v>
       </c>
-      <c r="C70" s="76" t="s">
+      <c r="C70" s="77" t="s">
         <v>880</v>
       </c>
-      <c r="D70" s="76" t="s">
+      <c r="D70" s="77" t="s">
         <v>881</v>
       </c>
-      <c r="E70" s="76"/>
-      <c r="F70" s="76"/>
+      <c r="E70" s="77"/>
+      <c r="F70" s="77"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="71" t="s">
+      <c r="A71" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B71" s="76" t="s">
+      <c r="B71" s="77" t="s">
         <v>882</v>
       </c>
-      <c r="C71" s="76" t="s">
+      <c r="C71" s="77" t="s">
         <v>883</v>
       </c>
-      <c r="D71" s="76" t="s">
+      <c r="D71" s="77" t="s">
         <v>884</v>
       </c>
-      <c r="E71" s="76"/>
-      <c r="F71" s="76"/>
+      <c r="E71" s="77"/>
+      <c r="F71" s="77"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="71" t="s">
+      <c r="A72" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B72" s="76" t="s">
+      <c r="B72" s="77" t="s">
         <v>885</v>
       </c>
-      <c r="C72" s="76" t="s">
+      <c r="C72" s="77" t="s">
         <v>886</v>
       </c>
-      <c r="D72" s="76" t="s">
+      <c r="D72" s="77" t="s">
         <v>887</v>
       </c>
-      <c r="E72" s="76"/>
-      <c r="F72" s="76"/>
+      <c r="E72" s="77"/>
+      <c r="F72" s="77"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="71" t="s">
+      <c r="A73" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B73" s="76" t="s">
+      <c r="B73" s="77" t="s">
         <v>888</v>
       </c>
-      <c r="C73" s="76" t="s">
+      <c r="C73" s="77" t="s">
         <v>889</v>
       </c>
-      <c r="D73" s="76" t="s">
+      <c r="D73" s="77" t="s">
         <v>890</v>
       </c>
-      <c r="E73" s="76"/>
-      <c r="F73" s="76"/>
+      <c r="E73" s="77"/>
+      <c r="F73" s="77"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="71" t="s">
+      <c r="A74" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B74" s="76" t="s">
+      <c r="B74" s="77" t="s">
         <v>891</v>
       </c>
-      <c r="C74" s="76" t="s">
+      <c r="C74" s="77" t="s">
         <v>892</v>
       </c>
-      <c r="D74" s="76" t="s">
+      <c r="D74" s="77" t="s">
         <v>893</v>
       </c>
-      <c r="E74" s="76"/>
-      <c r="F74" s="76"/>
+      <c r="E74" s="77"/>
+      <c r="F74" s="77"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="71" t="s">
+      <c r="A75" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B75" s="76" t="s">
+      <c r="B75" s="77" t="s">
         <v>894</v>
       </c>
-      <c r="C75" s="76" t="s">
+      <c r="C75" s="77" t="s">
         <v>895</v>
       </c>
-      <c r="D75" s="76" t="s">
+      <c r="D75" s="77" t="s">
         <v>896</v>
       </c>
-      <c r="E75" s="76"/>
-      <c r="F75" s="76"/>
+      <c r="E75" s="77"/>
+      <c r="F75" s="77"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="71" t="s">
+      <c r="A76" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B76" s="76" t="s">
+      <c r="B76" s="77" t="s">
         <v>897</v>
       </c>
-      <c r="C76" s="76" t="s">
+      <c r="C76" s="77" t="s">
         <v>898</v>
       </c>
-      <c r="D76" s="76" t="s">
+      <c r="D76" s="77" t="s">
         <v>899</v>
       </c>
-      <c r="E76" s="76"/>
-      <c r="F76" s="76"/>
+      <c r="E76" s="77"/>
+      <c r="F76" s="77"/>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="71" t="s">
+      <c r="A77" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B77" s="76" t="s">
+      <c r="B77" s="77" t="s">
         <v>900</v>
       </c>
-      <c r="C77" s="76" t="s">
+      <c r="C77" s="77" t="s">
         <v>901</v>
       </c>
-      <c r="D77" s="76" t="s">
+      <c r="D77" s="77" t="s">
         <v>902</v>
       </c>
-      <c r="E77" s="76"/>
-      <c r="F77" s="76"/>
+      <c r="E77" s="77"/>
+      <c r="F77" s="77"/>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="71" t="s">
+      <c r="A78" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B78" s="76" t="s">
+      <c r="B78" s="77" t="s">
         <v>903</v>
       </c>
-      <c r="C78" s="76" t="s">
+      <c r="C78" s="77" t="s">
         <v>904</v>
       </c>
-      <c r="D78" s="76" t="s">
+      <c r="D78" s="77" t="s">
         <v>905</v>
       </c>
-      <c r="E78" s="76"/>
-      <c r="F78" s="76"/>
+      <c r="E78" s="77"/>
+      <c r="F78" s="77"/>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="71" t="s">
+      <c r="A79" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B79" s="71" t="s">
+      <c r="B79" s="72" t="s">
         <v>906</v>
       </c>
-      <c r="C79" s="71" t="s">
+      <c r="C79" s="72" t="s">
         <v>907</v>
       </c>
-      <c r="D79" s="71" t="s">
+      <c r="D79" s="72" t="s">
         <v>908</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="71" t="s">
+      <c r="A80" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B80" s="71" t="s">
+      <c r="B80" s="72" t="s">
         <v>765</v>
       </c>
-      <c r="C80" s="71" t="s">
+      <c r="C80" s="72" t="s">
         <v>766</v>
       </c>
-      <c r="D80" s="71" t="s">
+      <c r="D80" s="72" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="71" t="s">
+      <c r="A81" s="72" t="s">
         <v>600</v>
       </c>
-      <c r="B81" s="71" t="s">
+      <c r="B81" s="72" t="s">
         <v>909</v>
       </c>
-      <c r="C81" s="71" t="s">
+      <c r="C81" s="72" t="s">
         <v>768</v>
       </c>
-      <c r="D81" s="71" t="s">
+      <c r="D81" s="72" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="77" t="s">
+      <c r="A82" s="78" t="s">
         <v>595</v>
       </c>
-      <c r="B82" s="76" t="s">
+      <c r="B82" s="77" t="s">
         <v>911</v>
       </c>
-      <c r="C82" s="71" t="s">
+      <c r="C82" s="72" t="s">
         <v>912</v>
       </c>
-      <c r="D82" s="71" t="s">
+      <c r="D82" s="72" t="s">
         <v>913</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="77" t="s">
+      <c r="A83" s="78" t="s">
         <v>595</v>
       </c>
-      <c r="B83" s="71" t="s">
+      <c r="B83" s="72" t="s">
         <v>914</v>
       </c>
-      <c r="C83" s="71" t="s">
+      <c r="C83" s="72" t="s">
         <v>915</v>
       </c>
-      <c r="D83" s="71" t="s">
+      <c r="D83" s="72" t="s">
         <v>916</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="77" t="s">
+      <c r="A84" s="78" t="s">
         <v>595</v>
       </c>
-      <c r="B84" s="71" t="s">
+      <c r="B84" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="C84" s="71" t="s">
+      <c r="C84" s="72" t="s">
         <v>763</v>
       </c>
-      <c r="D84" s="71" t="s">
+      <c r="D84" s="72" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="77" t="s">
+      <c r="A85" s="78" t="s">
         <v>595</v>
       </c>
-      <c r="B85" s="71" t="s">
+      <c r="B85" s="72" t="s">
         <v>682</v>
       </c>
-      <c r="C85" s="76" t="s">
+      <c r="C85" s="77" t="s">
         <v>768</v>
       </c>
-      <c r="D85" s="76" t="s">
+      <c r="D85" s="77" t="s">
         <v>910</v>
       </c>
-      <c r="E85" s="76"/>
-      <c r="F85" s="76"/>
+      <c r="E85" s="77"/>
+      <c r="F85" s="77"/>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="78" t="s">
+      <c r="A86" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="B86" s="71" t="s">
+      <c r="B86" s="72" t="s">
         <v>917</v>
       </c>
-      <c r="C86" s="79" t="s">
+      <c r="C86" s="80" t="s">
         <v>918</v>
       </c>
-      <c r="D86" s="71" t="s">
+      <c r="D86" s="72" t="s">
         <v>919</v>
       </c>
-      <c r="H86" s="76" t="s">
+      <c r="H86" s="77" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="78" t="s">
+      <c r="A87" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="B87" s="71" t="s">
+      <c r="B87" s="72" t="s">
         <v>920</v>
       </c>
-      <c r="C87" s="76" t="s">
+      <c r="C87" s="77" t="s">
         <v>921</v>
       </c>
-      <c r="D87" s="79" t="s">
+      <c r="D87" s="80" t="s">
         <v>922</v>
       </c>
-      <c r="E87" s="79"/>
-      <c r="F87" s="79"/>
+      <c r="E87" s="80"/>
+      <c r="F87" s="80"/>
       <c r="H87" s="2" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="78" t="s">
+      <c r="A88" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="B88" s="71" t="s">
+      <c r="B88" s="72" t="s">
         <v>923</v>
       </c>
-      <c r="C88" s="76" t="s">
+      <c r="C88" s="77" t="s">
         <v>924</v>
       </c>
-      <c r="D88" s="71" t="s">
+      <c r="D88" s="72" t="s">
         <v>925</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="78" t="s">
+      <c r="A89" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="B89" s="71" t="s">
+      <c r="B89" s="72" t="s">
         <v>926</v>
       </c>
-      <c r="C89" s="76" t="s">
+      <c r="C89" s="77" t="s">
         <v>927</v>
       </c>
-      <c r="D89" s="76" t="s">
+      <c r="D89" s="77" t="s">
         <v>928</v>
       </c>
-      <c r="E89" s="76"/>
-      <c r="F89" s="76"/>
+      <c r="E89" s="77"/>
+      <c r="F89" s="77"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="78" t="s">
+      <c r="A90" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="B90" s="71" t="s">
+      <c r="B90" s="72" t="s">
         <v>929</v>
       </c>
-      <c r="C90" s="76" t="s">
+      <c r="C90" s="77" t="s">
         <v>930</v>
       </c>
-      <c r="D90" s="76" t="s">
+      <c r="D90" s="77" t="s">
         <v>931</v>
       </c>
-      <c r="E90" s="76"/>
-      <c r="F90" s="76"/>
+      <c r="E90" s="77"/>
+      <c r="F90" s="77"/>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="78" t="s">
+      <c r="A91" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="B91" s="71" t="s">
+      <c r="B91" s="72" t="s">
         <v>932</v>
       </c>
-      <c r="C91" s="76" t="s">
+      <c r="C91" s="77" t="s">
         <v>933</v>
       </c>
-      <c r="D91" s="76" t="s">
+      <c r="D91" s="77" t="s">
         <v>934</v>
       </c>
-      <c r="E91" s="76"/>
-      <c r="F91" s="76"/>
+      <c r="E91" s="77"/>
+      <c r="F91" s="77"/>
       <c r="H91" s="2" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="78" t="s">
+      <c r="A92" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="B92" s="71" t="s">
+      <c r="B92" s="72" t="s">
         <v>935</v>
       </c>
-      <c r="C92" s="76" t="s">
+      <c r="C92" s="77" t="s">
         <v>936</v>
       </c>
-      <c r="D92" s="76" t="s">
+      <c r="D92" s="77" t="s">
         <v>937</v>
       </c>
-      <c r="E92" s="76"/>
-      <c r="F92" s="76"/>
+      <c r="E92" s="77"/>
+      <c r="F92" s="77"/>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="78" t="s">
+      <c r="A93" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="B93" s="71" t="s">
+      <c r="B93" s="72" t="s">
         <v>938</v>
       </c>
-      <c r="C93" s="76" t="s">
+      <c r="C93" s="77" t="s">
         <v>939</v>
       </c>
-      <c r="D93" s="76" t="s">
+      <c r="D93" s="77" t="s">
         <v>940</v>
       </c>
-      <c r="E93" s="76"/>
-      <c r="F93" s="76"/>
+      <c r="E93" s="77"/>
+      <c r="F93" s="77"/>
       <c r="H93" s="2" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="78" t="s">
+      <c r="A94" s="79" t="s">
         <v>320</v>
       </c>
-      <c r="B94" s="71" t="s">
+      <c r="B94" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="C94" s="76" t="s">
+      <c r="C94" s="77" t="s">
         <v>763</v>
       </c>
-      <c r="D94" s="71" t="s">
+      <c r="D94" s="72" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="78" t="s">
+      <c r="A95" s="79" t="s">
         <v>941</v>
       </c>
-      <c r="B95" s="71" t="s">
+      <c r="B95" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="C95" s="71" t="s">
+      <c r="C95" s="72" t="s">
         <v>722</v>
       </c>
-      <c r="D95" s="71" t="s">
+      <c r="D95" s="72" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="78" t="s">
+      <c r="A96" s="79" t="s">
         <v>941</v>
       </c>
-      <c r="B96" s="71" t="s">
+      <c r="B96" s="72" t="s">
         <v>942</v>
       </c>
-      <c r="C96" s="71" t="s">
+      <c r="C96" s="72" t="s">
         <v>943</v>
       </c>
-      <c r="D96" s="71" t="s">
+      <c r="D96" s="72" t="s">
         <v>944</v>
       </c>
-      <c r="H96" s="71" t="s">
+      <c r="H96" s="72" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="78" t="s">
+      <c r="A97" s="79" t="s">
         <v>941</v>
       </c>
-      <c r="B97" s="71" t="s">
+      <c r="B97" s="72" t="s">
         <v>161</v>
       </c>
-      <c r="C97" s="71" t="s">
+      <c r="C97" s="72" t="s">
         <v>945</v>
       </c>
-      <c r="D97" s="71" t="s">
+      <c r="D97" s="72" t="s">
         <v>946</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="78" t="s">
+      <c r="A98" s="79" t="s">
         <v>941</v>
       </c>
-      <c r="B98" s="76" t="s">
+      <c r="B98" s="77" t="s">
         <v>947</v>
       </c>
-      <c r="C98" s="76" t="s">
+      <c r="C98" s="77" t="s">
         <v>948</v>
       </c>
-      <c r="D98" s="76" t="s">
+      <c r="D98" s="77" t="s">
         <v>949</v>
       </c>
-      <c r="E98" s="76" t="s">
+      <c r="E98" s="77" t="s">
         <v>950</v>
       </c>
-      <c r="F98" s="76" t="s">
+      <c r="F98" s="77" t="s">
         <v>951</v>
       </c>
-      <c r="H98" s="71" t="s">
+      <c r="H98" s="72" t="s">
         <v>952</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="78" t="s">
+      <c r="A99" s="79" t="s">
         <v>953</v>
       </c>
-      <c r="B99" s="71" t="s">
+      <c r="B99" s="72" t="s">
         <v>954</v>
       </c>
-      <c r="C99" s="76" t="s">
+      <c r="C99" s="77" t="s">
         <v>955</v>
       </c>
-      <c r="D99" s="76" t="s">
+      <c r="D99" s="77" t="s">
         <v>956</v>
       </c>
-      <c r="E99" s="76" t="s">
+      <c r="E99" s="77" t="s">
         <v>957</v>
       </c>
-      <c r="F99" s="76" t="s">
+      <c r="F99" s="77" t="s">
         <v>958</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="78" t="s">
+      <c r="A100" s="79" t="s">
         <v>953</v>
       </c>
-      <c r="B100" s="71" t="s">
+      <c r="B100" s="72" t="s">
         <v>959</v>
       </c>
-      <c r="C100" s="76" t="s">
+      <c r="C100" s="77" t="s">
         <v>960</v>
       </c>
-      <c r="D100" s="76" t="s">
+      <c r="D100" s="77" t="s">
         <v>961</v>
       </c>
-      <c r="E100" s="76" t="s">
+      <c r="E100" s="77" t="s">
         <v>962</v>
       </c>
-      <c r="F100" s="76" t="s">
+      <c r="F100" s="77" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="78" t="s">
+      <c r="A101" s="79" t="s">
         <v>953</v>
       </c>
-      <c r="B101" s="71" t="s">
+      <c r="B101" s="72" t="s">
         <v>757</v>
       </c>
-      <c r="C101" s="71" t="s">
+      <c r="C101" s="72" t="s">
         <v>758</v>
       </c>
-      <c r="D101" s="71" t="s">
+      <c r="D101" s="72" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="78" t="s">
+      <c r="A102" s="79" t="s">
         <v>524</v>
       </c>
-      <c r="B102" s="76" t="s">
+      <c r="B102" s="77" t="s">
         <v>964</v>
       </c>
-      <c r="C102" s="76" t="s">
+      <c r="C102" s="77" t="s">
         <v>965</v>
       </c>
-      <c r="D102" s="76" t="s">
+      <c r="D102" s="77" t="s">
         <v>966</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="78" t="s">
+      <c r="A103" s="79" t="s">
         <v>524</v>
       </c>
-      <c r="B103" s="76" t="s">
+      <c r="B103" s="77" t="s">
         <v>967</v>
       </c>
-      <c r="C103" s="76" t="s">
+      <c r="C103" s="77" t="s">
         <v>968</v>
       </c>
-      <c r="D103" s="76" t="s">
+      <c r="D103" s="77" t="s">
         <v>969</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="78" t="s">
+      <c r="A104" s="79" t="s">
         <v>524</v>
       </c>
-      <c r="B104" s="76" t="s">
+      <c r="B104" s="77" t="s">
         <v>970</v>
       </c>
-      <c r="C104" s="76" t="s">
+      <c r="C104" s="77" t="s">
         <v>971</v>
       </c>
-      <c r="D104" s="76" t="s">
+      <c r="D104" s="77" t="s">
         <v>972</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="78" t="s">
+      <c r="A105" s="79" t="s">
         <v>524</v>
       </c>
-      <c r="B105" s="76" t="s">
+      <c r="B105" s="77" t="s">
         <v>973</v>
       </c>
-      <c r="C105" s="76" t="s">
+      <c r="C105" s="77" t="s">
         <v>974</v>
       </c>
-      <c r="D105" s="76" t="s">
+      <c r="D105" s="77" t="s">
         <v>975</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="78" t="s">
+      <c r="A106" s="79" t="s">
         <v>524</v>
       </c>
-      <c r="G106" s="74" t="s">
+      <c r="G106" s="75" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="78" t="s">
+      <c r="A107" s="79" t="s">
         <v>524</v>
       </c>
-      <c r="G107" s="74" t="s">
+      <c r="G107" s="75" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="78" t="s">
+      <c r="A108" s="79" t="s">
         <v>539</v>
       </c>
-      <c r="B108" s="76" t="s">
+      <c r="B108" s="77" t="s">
         <v>976</v>
       </c>
-      <c r="C108" s="76" t="s">
+      <c r="C108" s="77" t="s">
         <v>977</v>
       </c>
-      <c r="D108" s="76" t="s">
+      <c r="D108" s="77" t="s">
         <v>978</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="78" t="s">
+      <c r="A109" s="79" t="s">
         <v>539</v>
       </c>
-      <c r="B109" s="76" t="s">
+      <c r="B109" s="77" t="s">
         <v>979</v>
       </c>
-      <c r="C109" s="76" t="s">
+      <c r="C109" s="77" t="s">
         <v>980</v>
       </c>
-      <c r="D109" s="76" t="s">
+      <c r="D109" s="77" t="s">
         <v>981</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="78" t="s">
+      <c r="A110" s="79" t="s">
         <v>539</v>
       </c>
-      <c r="B110" s="76" t="s">
+      <c r="B110" s="77" t="s">
         <v>970</v>
       </c>
-      <c r="C110" s="76" t="s">
+      <c r="C110" s="77" t="s">
         <v>971</v>
       </c>
-      <c r="D110" s="76" t="s">
+      <c r="D110" s="77" t="s">
         <v>972</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A111" s="78" t="s">
+      <c r="A111" s="79" t="s">
         <v>539</v>
       </c>
-      <c r="B111" s="76" t="s">
+      <c r="B111" s="77" t="s">
         <v>982</v>
       </c>
-      <c r="C111" s="76" t="s">
+      <c r="C111" s="77" t="s">
         <v>983</v>
       </c>
-      <c r="D111" s="76" t="s">
+      <c r="D111" s="77" t="s">
         <v>984</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="78" t="s">
+      <c r="A112" s="79" t="s">
         <v>539</v>
       </c>
-      <c r="G112" s="74" t="s">
+      <c r="G112" s="75" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="78" t="s">
+      <c r="A113" s="79" t="s">
         <v>539</v>
       </c>
-      <c r="G113" s="74" t="s">
+      <c r="G113" s="75" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="80" t="s">
+      <c r="A114" s="81" t="s">
         <v>175</v>
       </c>
-      <c r="B114" s="76" t="s">
+      <c r="B114" s="77" t="s">
         <v>985</v>
       </c>
-      <c r="C114" s="71" t="s">
+      <c r="C114" s="72" t="s">
         <v>986</v>
       </c>
-      <c r="D114" s="71" t="s">
+      <c r="D114" s="72" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="80" t="s">
+      <c r="A115" s="81" t="s">
         <v>175</v>
       </c>
-      <c r="B115" s="71" t="s">
+      <c r="B115" s="72" t="s">
         <v>988</v>
       </c>
-      <c r="C115" s="71" t="s">
+      <c r="C115" s="72" t="s">
         <v>989</v>
       </c>
-      <c r="D115" s="71" t="s">
+      <c r="D115" s="72" t="s">
         <v>990</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="80" t="s">
+      <c r="A116" s="81" t="s">
         <v>175</v>
       </c>
-      <c r="B116" s="76" t="s">
+      <c r="B116" s="77" t="s">
         <v>991</v>
       </c>
-      <c r="C116" s="71" t="s">
+      <c r="C116" s="72" t="s">
         <v>992</v>
       </c>
-      <c r="D116" s="71" t="s">
+      <c r="D116" s="72" t="s">
         <v>993</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="80" t="s">
+      <c r="A117" s="81" t="s">
         <v>175</v>
       </c>
-      <c r="B117" s="76" t="s">
+      <c r="B117" s="77" t="s">
         <v>994</v>
       </c>
-      <c r="C117" s="71" t="s">
+      <c r="C117" s="72" t="s">
         <v>995</v>
       </c>
-      <c r="D117" s="71" t="s">
+      <c r="D117" s="72" t="s">
         <v>996</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="80" t="s">
+      <c r="A118" s="81" t="s">
         <v>175</v>
       </c>
-      <c r="B118" s="76" t="s">
+      <c r="B118" s="77" t="s">
         <v>997</v>
       </c>
-      <c r="C118" s="71" t="s">
+      <c r="C118" s="72" t="s">
         <v>998</v>
       </c>
-      <c r="D118" s="71" t="s">
+      <c r="D118" s="72" t="s">
         <v>999</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="80" t="s">
+      <c r="A119" s="81" t="s">
         <v>175</v>
       </c>
-      <c r="B119" s="76" t="s">
+      <c r="B119" s="77" t="s">
         <v>1000</v>
       </c>
-      <c r="C119" s="71" t="s">
+      <c r="C119" s="72" t="s">
         <v>1001</v>
       </c>
-      <c r="D119" s="71" t="s">
+      <c r="D119" s="72" t="s">
         <v>1002</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="80" t="s">
+      <c r="A120" s="81" t="s">
         <v>175</v>
       </c>
-      <c r="G120" s="74" t="s">
+      <c r="G120" s="75" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="75" t="s">
+      <c r="A121" s="76" t="s">
         <v>1003</v>
       </c>
-      <c r="B121" s="74" t="s">
+      <c r="B121" s="75" t="s">
         <v>703</v>
       </c>
-      <c r="C121" s="74" t="s">
+      <c r="C121" s="75" t="s">
         <v>1004</v>
       </c>
-      <c r="D121" s="74" t="s">
+      <c r="D121" s="75" t="s">
         <v>1005</v>
       </c>
-      <c r="E121" s="74" t="s">
+      <c r="E121" s="75" t="s">
         <v>1006</v>
       </c>
-      <c r="F121" s="74" t="s">
+      <c r="F121" s="75" t="s">
         <v>1007</v>
       </c>
-      <c r="G121" s="75"/>
+      <c r="G121" s="76"/>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="75" t="s">
+      <c r="A122" s="76" t="s">
         <v>1003</v>
       </c>
-      <c r="B122" s="74" t="s">
+      <c r="B122" s="75" t="s">
         <v>704</v>
       </c>
-      <c r="C122" s="74" t="s">
+      <c r="C122" s="75" t="s">
         <v>1008</v>
       </c>
-      <c r="D122" s="74" t="s">
+      <c r="D122" s="75" t="s">
         <v>1009</v>
       </c>
-      <c r="E122" s="74" t="s">
+      <c r="E122" s="75" t="s">
         <v>1010</v>
       </c>
-      <c r="F122" s="74" t="s">
+      <c r="F122" s="75" t="s">
         <v>1011</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="75" t="s">
+      <c r="A123" s="76" t="s">
         <v>1003</v>
       </c>
-      <c r="B123" s="74" t="s">
+      <c r="B123" s="75" t="s">
         <v>705</v>
       </c>
-      <c r="C123" s="74" t="s">
+      <c r="C123" s="75" t="s">
         <v>1012</v>
       </c>
-      <c r="D123" s="74" t="s">
+      <c r="D123" s="75" t="s">
         <v>1013</v>
       </c>
-      <c r="E123" s="74" t="s">
+      <c r="E123" s="75" t="s">
         <v>1014</v>
       </c>
-      <c r="F123" s="74" t="s">
+      <c r="F123" s="75" t="s">
         <v>1015</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="75" t="s">
+      <c r="A124" s="76" t="s">
         <v>1003</v>
       </c>
-      <c r="B124" s="74" t="s">
+      <c r="B124" s="75" t="s">
         <v>848</v>
       </c>
-      <c r="C124" s="74" t="s">
+      <c r="C124" s="75" t="s">
         <v>1016</v>
       </c>
-      <c r="D124" s="74" t="s">
+      <c r="D124" s="75" t="s">
         <v>1017</v>
       </c>
-      <c r="E124" s="74" t="s">
+      <c r="E124" s="75" t="s">
         <v>1018</v>
       </c>
-      <c r="F124" s="74" t="s">
+      <c r="F124" s="75" t="s">
         <v>1019</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="75" t="s">
+      <c r="A125" s="76" t="s">
         <v>1003</v>
       </c>
-      <c r="B125" s="74" t="s">
+      <c r="B125" s="75" t="s">
         <v>709</v>
       </c>
-      <c r="C125" s="74" t="s">
+      <c r="C125" s="75" t="s">
         <v>1020</v>
       </c>
-      <c r="D125" s="74" t="s">
+      <c r="D125" s="75" t="s">
         <v>1021</v>
       </c>
-      <c r="E125" s="74" t="s">
+      <c r="E125" s="75" t="s">
         <v>1022</v>
       </c>
-      <c r="F125" s="74" t="s">
+      <c r="F125" s="75" t="s">
         <v>1023</v>
       </c>
     </row>
@@ -15352,193 +15356,193 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="82" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="81" t="s">
+    <row r="1" s="83" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="82" t="s">
         <v>1024</v>
       </c>
-      <c r="B1" s="81" t="s">
+      <c r="B1" s="82" t="s">
         <v>1025</v>
       </c>
-      <c r="C1" s="81" t="s">
+      <c r="C1" s="82" t="s">
         <v>1026</v>
       </c>
-      <c r="D1" s="81" t="s">
+      <c r="D1" s="82" t="s">
         <v>1027</v>
       </c>
-      <c r="E1" s="81" t="s">
+      <c r="E1" s="82" t="s">
         <v>1028</v>
       </c>
-      <c r="F1" s="81" t="s">
+      <c r="F1" s="82" t="s">
         <v>1029</v>
       </c>
-      <c r="G1" s="81" t="s">
+      <c r="G1" s="82" t="s">
         <v>1030</v>
       </c>
-      <c r="H1" s="81" t="s">
+      <c r="H1" s="82" t="s">
         <v>1031</v>
       </c>
-      <c r="I1" s="81" t="s">
+      <c r="I1" s="82" t="s">
         <v>1032</v>
       </c>
-      <c r="J1" s="81" t="s">
+      <c r="J1" s="82" t="s">
         <v>1033</v>
       </c>
-      <c r="K1" s="81" t="s">
+      <c r="K1" s="82" t="s">
         <v>1034</v>
       </c>
-      <c r="L1" s="82" t="s">
+      <c r="L1" s="83" t="s">
         <v>1035</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="52" t="s">
         <v>646</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="52" t="s">
         <v>1036</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="52" t="s">
         <v>1037</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="52" t="s">
         <v>1038</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="52" t="s">
         <v>1039</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="52" t="s">
         <v>1040</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="52" t="s">
         <v>1041</v>
       </c>
-      <c r="H2" s="51" t="n">
+      <c r="H2" s="52" t="n">
         <v>-10</v>
       </c>
-      <c r="I2" s="51" t="n">
+      <c r="I2" s="52" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="L2" s="51" t="s">
+      <c r="L2" s="52" t="s">
         <v>1043</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="52" t="s">
         <v>637</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="52" t="s">
         <v>1044</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="52" t="s">
         <v>1045</v>
       </c>
-      <c r="D3" s="83" t="s">
+      <c r="D3" s="84" t="s">
         <v>1046</v>
       </c>
-      <c r="E3" s="83" t="s">
+      <c r="E3" s="84" t="s">
         <v>1047</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="84" t="s">
         <v>1048</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="52" t="s">
         <v>1049</v>
       </c>
-      <c r="H3" s="51" t="n">
+      <c r="H3" s="52" t="n">
         <v>-10</v>
       </c>
-      <c r="I3" s="51" t="n">
+      <c r="I3" s="52" t="n">
         <v>100</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="L3" s="51" t="s">
+      <c r="L3" s="52" t="s">
         <v>1050</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="52" t="s">
         <v>651</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="52" t="s">
         <v>1051</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="52" t="s">
         <v>1052</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="52" t="s">
         <v>1053</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="52" t="s">
         <v>1054</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="52" t="s">
         <v>1055</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="52" t="s">
         <v>1056</v>
       </c>
-      <c r="H4" s="51" t="n">
+      <c r="H4" s="52" t="n">
         <v>-10</v>
       </c>
-      <c r="I4" s="51" t="n">
+      <c r="I4" s="52" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="K4" s="51" t="s">
+      <c r="K4" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="L4" s="51" t="s">
+      <c r="L4" s="52" t="s">
         <v>1043</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="52" t="s">
         <v>656</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="52" t="s">
         <v>1044</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="52" t="s">
         <v>1057</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="52" t="s">
         <v>1058</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="52" t="s">
         <v>1047</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="52" t="s">
         <v>1059</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="52" t="s">
         <v>1060</v>
       </c>
-      <c r="H5" s="51" t="n">
+      <c r="H5" s="52" t="n">
         <v>-10</v>
       </c>
-      <c r="I5" s="51" t="n">
+      <c r="I5" s="52" t="n">
         <v>100</v>
       </c>
-      <c r="J5" s="51" t="s">
+      <c r="J5" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="K5" s="51" t="s">
+      <c r="K5" s="52" t="s">
         <v>1042</v>
       </c>
-      <c r="L5" s="51" t="s">
+      <c r="L5" s="52" t="s">
         <v>1043</v>
       </c>
     </row>
@@ -16504,7 +16508,7 @@
       <c r="A60" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="B60" s="84" t="s">
+      <c r="B60" s="85" t="s">
         <v>1261</v>
       </c>
       <c r="C60" s="11" t="s">
@@ -16572,7 +16576,7 @@
       <c r="C64" s="41" t="s">
         <v>1276</v>
       </c>
-      <c r="D64" s="84" t="s">
+      <c r="D64" s="85" t="s">
         <v>1277</v>
       </c>
       <c r="E64" s="2"/>
@@ -16588,7 +16592,7 @@
       <c r="C65" s="41" t="s">
         <v>1279</v>
       </c>
-      <c r="D65" s="84" t="s">
+      <c r="D65" s="85" t="s">
         <v>1280</v>
       </c>
       <c r="E65" s="2"/>
@@ -16598,49 +16602,49 @@
       <c r="A66" s="36" t="s">
         <v>328</v>
       </c>
-      <c r="B66" s="67" t="s">
+      <c r="B66" s="68" t="s">
         <v>1281</v>
       </c>
-      <c r="C66" s="67" t="s">
+      <c r="C66" s="68" t="s">
         <v>722</v>
       </c>
-      <c r="D66" s="67" t="s">
+      <c r="D66" s="68" t="s">
         <v>723</v>
       </c>
-      <c r="E66" s="67"/>
-      <c r="F66" s="67"/>
+      <c r="E66" s="68"/>
+      <c r="F66" s="68"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="36" t="s">
         <v>328</v>
       </c>
-      <c r="B67" s="67" t="s">
+      <c r="B67" s="68" t="s">
         <v>1282</v>
       </c>
-      <c r="C67" s="67" t="s">
+      <c r="C67" s="68" t="s">
         <v>943</v>
       </c>
-      <c r="D67" s="67" t="s">
+      <c r="D67" s="68" t="s">
         <v>944</v>
       </c>
-      <c r="E67" s="67"/>
-      <c r="F67" s="67"/>
+      <c r="E67" s="68"/>
+      <c r="F67" s="68"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="36" t="s">
         <v>328</v>
       </c>
-      <c r="B68" s="67" t="s">
+      <c r="B68" s="68" t="s">
         <v>1283</v>
       </c>
-      <c r="C68" s="67" t="s">
+      <c r="C68" s="68" t="s">
         <v>945</v>
       </c>
-      <c r="D68" s="67" t="s">
+      <c r="D68" s="68" t="s">
         <v>946</v>
       </c>
-      <c r="E68" s="67"/>
-      <c r="F68" s="67"/>
+      <c r="E68" s="68"/>
+      <c r="F68" s="68"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="36" t="s">
@@ -16666,7 +16670,7 @@
       <c r="A70" s="36" t="s">
         <v>429</v>
       </c>
-      <c r="B70" s="67" t="s">
+      <c r="B70" s="68" t="s">
         <v>1285</v>
       </c>
       <c r="C70" s="11" t="s">
@@ -16686,7 +16690,7 @@
       <c r="A71" s="36" t="s">
         <v>429</v>
       </c>
-      <c r="B71" s="67" t="s">
+      <c r="B71" s="68" t="s">
         <v>1286</v>
       </c>
       <c r="C71" s="11" t="s">
@@ -16706,7 +16710,7 @@
       <c r="A72" s="36" t="s">
         <v>429</v>
       </c>
-      <c r="B72" s="67" t="s">
+      <c r="B72" s="68" t="s">
         <v>1287</v>
       </c>
       <c r="C72" s="11" t="s">
@@ -16722,7 +16726,7 @@
       <c r="A73" s="36" t="s">
         <v>429</v>
       </c>
-      <c r="B73" s="67" t="s">
+      <c r="B73" s="68" t="s">
         <v>1290</v>
       </c>
       <c r="C73" s="11" t="s">
@@ -16738,7 +16742,7 @@
       <c r="A74" s="36" t="s">
         <v>429</v>
       </c>
-      <c r="B74" s="67" t="s">
+      <c r="B74" s="68" t="s">
         <v>1293</v>
       </c>
       <c r="C74" s="11" t="s">

</xml_diff>

<commit_message>
Label: Add cottage for secondary residency
Fix: #362
Did 'yarn generateSurvey'
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -4303,10 +4303,10 @@
     <t xml:space="preserve">LocationNameAddressExample_secondaryHome</t>
   </si>
   <si>
-    <t xml:space="preserve">Adresse de la résidence secondaire, nom du chalet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Secondary home address, name of the chalet</t>
+    <t xml:space="preserve">Adresse de la résidence secondaire ou du chalet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Secondary home or cottage address</t>
   </si>
   <si>
     <t xml:space="preserve">LocationNameAddressExample_schoolNotStudent</t>
@@ -5035,7 +5035,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="85">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5366,10 +5366,6 @@
     </xf>
     <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
@@ -5768,12 +5764,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C67" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A67" activeCellId="0" sqref="A67"/>
-      <selection pane="bottomRight" activeCell="D69" activeCellId="0" sqref="D69"/>
+      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="bottomRight" activeCell="A70" activeCellId="0" sqref="A70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6420,7 +6416,7 @@
       <c r="Q12" s="8"/>
       <c r="R12" s="8"/>
       <c r="S12" s="8"/>
-      <c r="T12" s="8" t="b">
+      <c r="T12" s="9" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13477,8 +13473,8 @@
   </sheetPr>
   <dimension ref="A1:I125"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A95" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D98" activeCellId="0" sqref="D98"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C88" activeCellId="0" sqref="C88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15776,8 +15772,8 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J46" activeCellId="0" sqref="J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16528,7 +16524,7 @@
       <c r="C49" s="11" t="s">
         <v>1216</v>
       </c>
-      <c r="D49" s="83" t="s">
+      <c r="D49" s="11" t="s">
         <v>1217</v>
       </c>
       <c r="E49" s="11" t="s">
@@ -16548,7 +16544,7 @@
       <c r="C50" s="11" t="s">
         <v>1221</v>
       </c>
-      <c r="D50" s="83" t="s">
+      <c r="D50" s="11" t="s">
         <v>1222</v>
       </c>
       <c r="E50" s="11" t="s">
@@ -16568,7 +16564,7 @@
       <c r="C51" s="11" t="s">
         <v>1226</v>
       </c>
-      <c r="D51" s="83" t="s">
+      <c r="D51" s="11" t="s">
         <v>1227</v>
       </c>
       <c r="E51" s="11" t="s">
@@ -16718,7 +16714,7 @@
       <c r="A60" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="84" t="s">
+      <c r="B60" s="83" t="s">
         <v>1262</v>
       </c>
       <c r="C60" s="11" t="s">
@@ -16786,7 +16782,7 @@
       <c r="C64" s="40" t="s">
         <v>1277</v>
       </c>
-      <c r="D64" s="84" t="s">
+      <c r="D64" s="83" t="s">
         <v>1278</v>
       </c>
       <c r="E64" s="2"/>
@@ -16802,7 +16798,7 @@
       <c r="C65" s="40" t="s">
         <v>1280</v>
       </c>
-      <c r="D65" s="84" t="s">
+      <c r="D65" s="83" t="s">
         <v>1281</v>
       </c>
       <c r="E65" s="2"/>

</xml_diff>

<commit_message>
Label: Change the value of one of the choice from hybridCarNumber to pluginHybridCarNumber
Fix: #382
Did 'yarn generateSurvey'
Note: One of the variable had a wrong name in householdElectricCarCountCustomValidation, but the logic was good.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -2369,10 +2369,10 @@
     <t xml:space="preserve">The **next questions are optional** and are added for research purposes. You can complete the interview without answering them.</t>
   </si>
   <si>
-    <t xml:space="preserve">householdHybridCarNumber</t>
-  </si>
-  <si>
-    <t xml:space="preserve">household.hybridCarNumber</t>
+    <t xml:space="preserve">householdPluginHybridCarNumber</t>
+  </si>
+  <si>
+    <t xml:space="preserve">household.pluginHybridCarNumber</t>
   </si>
   <si>
     <t xml:space="preserve">Parmi les véhicules possédés par votre ménage, combien sont des **véhicules hybrides rechargeables**?
@@ -5764,12 +5764,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C121" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
-      <selection pane="bottomRight" activeCell="A70" activeCellId="0" sqref="A70"/>
+      <selection pane="bottomLeft" activeCell="A121" activeCellId="0" sqref="A121"/>
+      <selection pane="bottomRight" activeCell="F125" activeCellId="0" sqref="F125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -15772,7 +15772,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J46" activeCellId="0" sqref="J46"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Label: Improve the personNewPerson helpPopup
Fix: #286
Simplify a bit the UI tests for this widget.
Align the text to the left, so it's easier to read.
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Widgets" sheetId="1" state="visible" r:id="rId3"/>
@@ -963,12 +963,52 @@
     <t xml:space="preserve">_showNewPersonPopupButton</t>
   </si>
   <si>
-    <t xml:space="preserve">Nous allons vous demander de spécifier les déplacements de **{{nickname}}**.
-L’ordre des personnes interviewées est aléatoire.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">We will ask you to specify **{{nickname}}**’s trips.
-The order of the interviewed persons was randomly selected.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Nous allons vous demander de spécifier les déplacements de **{{nickname}}**.
+L’ordre des personnes interviewées est aléatoire.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;details&gt;&lt;summary&gt;Pourquoi l'ordre des personnes peut avoir été changé?&lt;/summary&gt; L'ordre des personnes pour lesquelles on demande de spécifier les déplacements est aléatoire (tiré au sort). Cela permet d'éviter tout biais lié à la séquence de déclaration et d'assurer des données de qualité homogène.&lt;/details&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">We will ask you to specify **{{nickname}}**’s trips.
+The order of the interviewed persons was randomly selected.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">&lt;details&gt;&lt;summary&gt;Why might the order of persons have been changed?&lt;/summary&gt;The order of persons for whom we ask you to specify trips is randomized. This helps avoid any bias related to the reporting sequence and ensures consistent data quality.&lt;/details&gt;</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">personWhoWillAnswerForThisPerson</t>
@@ -5023,7 +5063,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="84">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5192,10 +5232,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -5273,10 +5309,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -5760,12 +5792,12 @@
   </sheetPr>
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C98" activePane="bottomRight" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="A98" activeCellId="0" sqref="A98"/>
-      <selection pane="bottomRight" activeCell="F111" activeCellId="0" sqref="F111"/>
+      <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
+      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
+      <selection pane="bottomRight" activeCell="I48" activeCellId="0" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6514,7 +6546,7 @@
       <c r="Q14" s="8"/>
       <c r="R14" s="8"/>
       <c r="S14" s="8"/>
-      <c r="T14" s="9" t="b">
+      <c r="T14" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6563,7 +6595,7 @@
       <c r="Q15" s="8"/>
       <c r="R15" s="8"/>
       <c r="S15" s="8"/>
-      <c r="T15" s="9" t="b">
+      <c r="T15" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6663,7 +6695,7 @@
       <c r="Q17" s="8"/>
       <c r="R17" s="8"/>
       <c r="S17" s="8"/>
-      <c r="T17" s="9" t="b">
+      <c r="T17" s="8" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -6872,7 +6904,7 @@
       <c r="Q21" s="25"/>
       <c r="R21" s="25"/>
       <c r="S21" s="25"/>
-      <c r="T21" s="24" t="b">
+      <c r="T21" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7391,7 +7423,7 @@
       <c r="Q31" s="25"/>
       <c r="R31" s="25"/>
       <c r="S31" s="25"/>
-      <c r="T31" s="24" t="b">
+      <c r="T31" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7441,7 +7473,7 @@
       <c r="Q32" s="25"/>
       <c r="R32" s="25"/>
       <c r="S32" s="25"/>
-      <c r="T32" s="24" t="b">
+      <c r="T32" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -7921,7 +7953,7 @@
       <c r="Q41" s="25"/>
       <c r="R41" s="25"/>
       <c r="S41" s="25"/>
-      <c r="T41" s="24" t="b">
+      <c r="T41" s="22" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -8205,7 +8237,7 @@
       <c r="W47" s="35"/>
       <c r="X47" s="35"/>
     </row>
-    <row r="48" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="226.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="11" t="s">
         <v>284</v>
       </c>
@@ -9061,7 +9093,7 @@
       <c r="Q66" s="35"/>
       <c r="R66" s="35"/>
       <c r="S66" s="35"/>
-      <c r="T66" s="36" t="b">
+      <c r="T66" s="33" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -9784,7 +9816,7 @@
       <c r="Q82" s="35"/>
       <c r="R82" s="35"/>
       <c r="S82" s="35"/>
-      <c r="T82" s="36" t="b">
+      <c r="T82" s="33" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -10794,7 +10826,7 @@
       <c r="Q104" s="35"/>
       <c r="R104" s="35"/>
       <c r="S104" s="35"/>
-      <c r="T104" s="18" t="b">
+      <c r="T104" s="16" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11045,7 +11077,7 @@
       <c r="Q109" s="35"/>
       <c r="R109" s="35"/>
       <c r="S109" s="35"/>
-      <c r="T109" s="18" t="b">
+      <c r="T109" s="16" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -11113,19 +11145,19 @@
         <v>551</v>
       </c>
       <c r="E111" s="35"/>
-      <c r="F111" s="42" t="s">
+      <c r="F111" s="11" t="s">
         <v>552</v>
       </c>
-      <c r="G111" s="43" t="s">
+      <c r="G111" s="42" t="s">
         <v>553</v>
       </c>
-      <c r="H111" s="43" t="s">
+      <c r="H111" s="42" t="s">
         <v>554</v>
       </c>
-      <c r="I111" s="44" t="s">
+      <c r="I111" s="43" t="s">
         <v>555</v>
       </c>
-      <c r="J111" s="43" t="s">
+      <c r="J111" s="42" t="s">
         <v>556</v>
       </c>
       <c r="K111" s="35"/>
@@ -11149,10 +11181,10 @@
       <c r="XED111" s="2"/>
     </row>
     <row r="112" s="2" customFormat="true" ht="27.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="45" t="s">
+      <c r="A112" s="44" t="s">
         <v>557</v>
       </c>
-      <c r="B112" s="45" t="s">
+      <c r="B112" s="44" t="s">
         <v>73</v>
       </c>
       <c r="C112" s="34" t="n">
@@ -11162,14 +11194,14 @@
       <c r="D112" s="40" t="s">
         <v>551</v>
       </c>
-      <c r="E112" s="46"/>
-      <c r="F112" s="45" t="str">
+      <c r="E112" s="45"/>
+      <c r="F112" s="44" t="str">
         <f aca="false">A112</f>
         <v>householdLongDistanceIntroMap</v>
       </c>
-      <c r="G112" s="47"/>
-      <c r="H112" s="47"/>
-      <c r="I112" s="48"/>
+      <c r="G112" s="46"/>
+      <c r="H112" s="46"/>
+      <c r="I112" s="47"/>
       <c r="J112" s="1"/>
       <c r="K112" s="1"/>
       <c r="L112" s="1"/>
@@ -11184,7 +11216,7 @@
       </c>
     </row>
     <row r="113" s="2" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A113" s="45" t="s">
+      <c r="A113" s="44" t="s">
         <v>559</v>
       </c>
       <c r="B113" s="33" t="s">
@@ -11197,20 +11229,20 @@
       <c r="D113" s="40" t="s">
         <v>551</v>
       </c>
-      <c r="E113" s="46"/>
-      <c r="F113" s="45" t="s">
+      <c r="E113" s="45"/>
+      <c r="F113" s="44" t="s">
         <v>560</v>
       </c>
-      <c r="G113" s="47" t="s">
+      <c r="G113" s="46" t="s">
         <v>561</v>
       </c>
-      <c r="H113" s="49" t="s">
+      <c r="H113" s="48" t="s">
         <v>562</v>
       </c>
-      <c r="I113" s="47" t="s">
+      <c r="I113" s="46" t="s">
         <v>563</v>
       </c>
-      <c r="J113" s="49" t="s">
+      <c r="J113" s="48" t="s">
         <v>564</v>
       </c>
       <c r="K113" s="1"/>
@@ -11228,7 +11260,7 @@
       </c>
     </row>
     <row r="114" s="2" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A114" s="45" t="s">
+      <c r="A114" s="44" t="s">
         <v>567</v>
       </c>
       <c r="B114" s="33" t="s">
@@ -11241,20 +11273,20 @@
       <c r="D114" s="40" t="s">
         <v>551</v>
       </c>
-      <c r="E114" s="46"/>
-      <c r="F114" s="45" t="s">
+      <c r="E114" s="45"/>
+      <c r="F114" s="44" t="s">
         <v>568</v>
       </c>
-      <c r="G114" s="47" t="s">
+      <c r="G114" s="46" t="s">
         <v>569</v>
       </c>
-      <c r="H114" s="49" t="s">
+      <c r="H114" s="48" t="s">
         <v>570</v>
       </c>
-      <c r="I114" s="47" t="s">
+      <c r="I114" s="46" t="s">
         <v>571</v>
       </c>
-      <c r="J114" s="49" t="s">
+      <c r="J114" s="48" t="s">
         <v>572</v>
       </c>
       <c r="K114" s="1"/>
@@ -11272,7 +11304,7 @@
       </c>
     </row>
     <row r="115" s="2" customFormat="true" ht="68.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A115" s="45" t="s">
+      <c r="A115" s="44" t="s">
         <v>573</v>
       </c>
       <c r="B115" s="33" t="s">
@@ -11285,20 +11317,20 @@
       <c r="D115" s="40" t="s">
         <v>551</v>
       </c>
-      <c r="E115" s="46"/>
-      <c r="F115" s="45" t="s">
+      <c r="E115" s="45"/>
+      <c r="F115" s="44" t="s">
         <v>574</v>
       </c>
-      <c r="G115" s="47" t="s">
+      <c r="G115" s="46" t="s">
         <v>575</v>
       </c>
-      <c r="H115" s="49" t="s">
+      <c r="H115" s="48" t="s">
         <v>576</v>
       </c>
-      <c r="I115" s="47" t="s">
+      <c r="I115" s="46" t="s">
         <v>577</v>
       </c>
-      <c r="J115" s="49" t="s">
+      <c r="J115" s="48" t="s">
         <v>578</v>
       </c>
       <c r="K115" s="1"/>
@@ -11333,10 +11365,10 @@
       <c r="F116" s="11" t="s">
         <v>580</v>
       </c>
-      <c r="G116" s="50" t="s">
+      <c r="G116" s="49" t="s">
         <v>581</v>
       </c>
-      <c r="H116" s="50" t="s">
+      <c r="H116" s="49" t="s">
         <v>582</v>
       </c>
       <c r="I116" s="16"/>
@@ -11381,10 +11413,10 @@
       <c r="F117" s="11" t="s">
         <v>584</v>
       </c>
-      <c r="G117" s="50" t="s">
+      <c r="G117" s="49" t="s">
         <v>585</v>
       </c>
-      <c r="H117" s="50" t="s">
+      <c r="H117" s="49" t="s">
         <v>586</v>
       </c>
       <c r="I117" s="16"/>
@@ -11525,7 +11557,7 @@
       <c r="L120" s="35"/>
       <c r="M120" s="35"/>
       <c r="N120" s="35"/>
-      <c r="O120" s="51" t="s">
+      <c r="O120" s="50" t="s">
         <v>600</v>
       </c>
       <c r="P120" s="35"/>
@@ -11559,10 +11591,10 @@
       <c r="F121" s="11" t="s">
         <v>602</v>
       </c>
-      <c r="G121" s="50" t="s">
+      <c r="G121" s="49" t="s">
         <v>603</v>
       </c>
-      <c r="H121" s="50" t="s">
+      <c r="H121" s="49" t="s">
         <v>604</v>
       </c>
       <c r="I121" s="16"/>
@@ -11605,10 +11637,10 @@
       <c r="F122" s="11" t="s">
         <v>606</v>
       </c>
-      <c r="G122" s="50" t="s">
+      <c r="G122" s="49" t="s">
         <v>607</v>
       </c>
-      <c r="H122" s="50" t="s">
+      <c r="H122" s="49" t="s">
         <v>608</v>
       </c>
       <c r="I122" s="16"/>
@@ -11653,10 +11685,10 @@
       <c r="F123" s="35" t="s">
         <v>612</v>
       </c>
-      <c r="G123" s="51" t="s">
+      <c r="G123" s="50" t="s">
         <v>613</v>
       </c>
-      <c r="H123" s="51" t="s">
+      <c r="H123" s="50" t="s">
         <v>614</v>
       </c>
       <c r="I123" s="16"/>
@@ -11699,7 +11731,7 @@
       <c r="F124" s="35" t="s">
         <v>616</v>
       </c>
-      <c r="G124" s="51" t="s">
+      <c r="G124" s="50" t="s">
         <v>617</v>
       </c>
       <c r="H124" s="10" t="s">
@@ -11842,10 +11874,10 @@
       <c r="F127" s="35" t="s">
         <v>633</v>
       </c>
-      <c r="G127" s="51" t="s">
+      <c r="G127" s="50" t="s">
         <v>634</v>
       </c>
-      <c r="H127" s="51" t="s">
+      <c r="H127" s="50" t="s">
         <v>635</v>
       </c>
       <c r="I127" s="16"/>
@@ -11858,7 +11890,7 @@
       </c>
       <c r="O127" s="35"/>
       <c r="P127" s="35"/>
-      <c r="Q127" s="51" t="s">
+      <c r="Q127" s="50" t="s">
         <v>637</v>
       </c>
       <c r="R127" s="35"/>
@@ -11890,10 +11922,10 @@
       <c r="F128" s="35" t="s">
         <v>639</v>
       </c>
-      <c r="G128" s="51" t="s">
+      <c r="G128" s="50" t="s">
         <v>640</v>
       </c>
-      <c r="H128" s="51" t="s">
+      <c r="H128" s="50" t="s">
         <v>641</v>
       </c>
       <c r="I128" s="16"/>
@@ -11936,10 +11968,10 @@
       <c r="F129" s="35" t="s">
         <v>643</v>
       </c>
-      <c r="G129" s="51" t="s">
+      <c r="G129" s="50" t="s">
         <v>644</v>
       </c>
-      <c r="H129" s="51" t="s">
+      <c r="H129" s="50" t="s">
         <v>645</v>
       </c>
       <c r="I129" s="16"/>
@@ -11952,7 +11984,7 @@
       </c>
       <c r="O129" s="35"/>
       <c r="P129" s="35"/>
-      <c r="Q129" s="51" t="s">
+      <c r="Q129" s="50" t="s">
         <v>646</v>
       </c>
       <c r="R129" s="35"/>
@@ -11984,10 +12016,10 @@
       <c r="F130" s="35" t="s">
         <v>648</v>
       </c>
-      <c r="G130" s="51" t="s">
+      <c r="G130" s="50" t="s">
         <v>649</v>
       </c>
-      <c r="H130" s="51" t="s">
+      <c r="H130" s="50" t="s">
         <v>650</v>
       </c>
       <c r="I130" s="16"/>
@@ -12000,7 +12032,7 @@
       </c>
       <c r="O130" s="35"/>
       <c r="P130" s="35"/>
-      <c r="Q130" s="51" t="s">
+      <c r="Q130" s="50" t="s">
         <v>651</v>
       </c>
       <c r="R130" s="35"/>
@@ -12032,10 +12064,10 @@
       <c r="F131" s="35" t="s">
         <v>653</v>
       </c>
-      <c r="G131" s="51" t="s">
+      <c r="G131" s="50" t="s">
         <v>654</v>
       </c>
-      <c r="H131" s="51" t="s">
+      <c r="H131" s="50" t="s">
         <v>655</v>
       </c>
       <c r="I131" s="16"/>
@@ -12048,7 +12080,7 @@
       </c>
       <c r="O131" s="35"/>
       <c r="P131" s="35"/>
-      <c r="Q131" s="51" t="s">
+      <c r="Q131" s="50" t="s">
         <v>656</v>
       </c>
       <c r="R131" s="35"/>
@@ -12080,10 +12112,10 @@
       <c r="F132" s="35" t="s">
         <v>658</v>
       </c>
-      <c r="G132" s="51" t="s">
+      <c r="G132" s="50" t="s">
         <v>659</v>
       </c>
-      <c r="H132" s="51" t="s">
+      <c r="H132" s="50" t="s">
         <v>660</v>
       </c>
       <c r="I132" s="16"/>
@@ -12158,7 +12190,7 @@
       <c r="B134" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C134" s="52" t="n">
+      <c r="C134" s="51" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12174,9 +12206,9 @@
       <c r="H134" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="L134" s="53"/>
-      <c r="M134" s="54"/>
-      <c r="T134" s="55" t="b">
+      <c r="L134" s="52"/>
+      <c r="M134" s="53"/>
+      <c r="T134" s="54" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -12280,38 +12312,38 @@
   </sheetPr>
   <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F16" activeCellId="0" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.58984375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="56" width="27.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="56" width="15.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="56" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="57" width="20.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="56" width="19.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="56" width="12.14"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="56" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="55" width="27.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="55" width="15.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="55" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="56" width="20.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="55" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="55" width="12.14"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="7" style="55" width="8.59"/>
   </cols>
   <sheetData>
-    <row r="1" s="60" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="58" t="s">
+    <row r="1" s="59" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="57" t="s">
         <v>668</v>
       </c>
-      <c r="B1" s="58" t="s">
+      <c r="B1" s="57" t="s">
         <v>669</v>
       </c>
-      <c r="C1" s="58" t="s">
+      <c r="C1" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="59" t="s">
+      <c r="D1" s="58" t="s">
         <v>670</v>
       </c>
-      <c r="E1" s="58" t="s">
+      <c r="E1" s="57" t="s">
         <v>671</v>
       </c>
-      <c r="F1" s="58" t="s">
+      <c r="F1" s="57" t="s">
         <v>672</v>
       </c>
     </row>
@@ -12323,7 +12355,7 @@
       <c r="C2" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="D2" s="61" t="s">
+      <c r="D2" s="60" t="s">
         <v>675</v>
       </c>
       <c r="E2" s="11" t="n">
@@ -12339,7 +12371,7 @@
       <c r="C3" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="D3" s="61" t="s">
+      <c r="D3" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E3" s="11" t="n">
@@ -12355,7 +12387,7 @@
       <c r="C4" s="11" t="s">
         <v>677</v>
       </c>
-      <c r="D4" s="61" t="s">
+      <c r="D4" s="60" t="s">
         <v>675</v>
       </c>
       <c r="E4" s="11" t="s">
@@ -12373,7 +12405,7 @@
       <c r="C5" s="11" t="s">
         <v>674</v>
       </c>
-      <c r="D5" s="61" t="s">
+      <c r="D5" s="60" t="s">
         <v>675</v>
       </c>
       <c r="E5" s="11" t="n">
@@ -12389,7 +12421,7 @@
       <c r="C6" s="11" t="s">
         <v>680</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E6" s="11" t="n">
@@ -12398,14 +12430,14 @@
       <c r="F6" s="11"/>
     </row>
     <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="61" t="s">
         <v>139</v>
       </c>
       <c r="B7" s="11"/>
       <c r="C7" s="11" t="s">
         <v>681</v>
       </c>
-      <c r="D7" s="61" t="s">
+      <c r="D7" s="60" t="s">
         <v>675</v>
       </c>
       <c r="E7" s="11" t="s">
@@ -12421,7 +12453,7 @@
       <c r="C8" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D8" s="61" t="s">
+      <c r="D8" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E8" s="11" t="n">
@@ -12439,7 +12471,7 @@
       <c r="C9" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D9" s="61" t="s">
+      <c r="D9" s="60" t="s">
         <v>686</v>
       </c>
       <c r="E9" s="11" t="n">
@@ -12455,7 +12487,7 @@
       <c r="C10" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E10" s="11" t="n">
@@ -12473,7 +12505,7 @@
       <c r="C11" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D11" s="61" t="s">
+      <c r="D11" s="60" t="s">
         <v>686</v>
       </c>
       <c r="E11" s="11" t="n">
@@ -12489,7 +12521,7 @@
       <c r="C12" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E12" s="11" t="n">
@@ -12507,7 +12539,7 @@
       <c r="C13" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D13" s="61" t="s">
+      <c r="D13" s="60" t="s">
         <v>686</v>
       </c>
       <c r="E13" s="11" t="n">
@@ -12523,7 +12555,7 @@
       <c r="C14" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D14" s="61" t="s">
+      <c r="D14" s="60" t="s">
         <v>686</v>
       </c>
       <c r="E14" s="11" t="n">
@@ -12539,7 +12571,7 @@
       <c r="C15" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D15" s="61" t="s">
+      <c r="D15" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E15" s="11" t="n">
@@ -12547,7 +12579,7 @@
       </c>
       <c r="F15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="91" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="11" t="s">
         <v>197</v>
       </c>
@@ -12555,14 +12587,14 @@
       <c r="C16" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D16" s="61" t="s">
+      <c r="D16" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E16" s="11" t="n">
         <v>6</v>
       </c>
       <c r="F16" s="11"/>
-      <c r="I16" s="63"/>
+      <c r="I16" s="11"/>
     </row>
     <row r="17" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="11" t="s">
@@ -12572,7 +12604,7 @@
       <c r="C17" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D17" s="61" t="s">
+      <c r="D17" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E17" s="11" t="n">
@@ -12588,7 +12620,7 @@
       <c r="C18" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D18" s="61" t="s">
+      <c r="D18" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E18" s="11" t="n">
@@ -12604,7 +12636,7 @@
       <c r="C19" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D19" s="61" t="s">
+      <c r="D19" s="60" t="s">
         <v>686</v>
       </c>
       <c r="E19" s="11" t="n">
@@ -12622,7 +12654,7 @@
       <c r="C20" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D20" s="61" t="s">
+      <c r="D20" s="60" t="s">
         <v>691</v>
       </c>
       <c r="E20" s="11" t="s">
@@ -12638,7 +12670,7 @@
       <c r="C21" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D21" s="61" t="s">
+      <c r="D21" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E21" s="11" t="n">
@@ -12654,7 +12686,7 @@
       <c r="C22" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D22" s="61" t="s">
+      <c r="D22" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E22" s="11" t="n">
@@ -12670,7 +12702,7 @@
       <c r="C23" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D23" s="61" t="s">
+      <c r="D23" s="60" t="s">
         <v>686</v>
       </c>
       <c r="E23" s="11" t="n">
@@ -12688,7 +12720,7 @@
       <c r="C24" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D24" s="61" t="s">
+      <c r="D24" s="60" t="s">
         <v>691</v>
       </c>
       <c r="E24" s="11" t="s">
@@ -12704,7 +12736,7 @@
       <c r="C25" s="11" t="s">
         <v>684</v>
       </c>
-      <c r="D25" s="61" t="s">
+      <c r="D25" s="60" t="s">
         <v>676</v>
       </c>
       <c r="E25" s="11" t="n">
@@ -12720,7 +12752,7 @@
       <c r="C26" s="11" t="s">
         <v>695</v>
       </c>
-      <c r="D26" s="61" t="s">
+      <c r="D26" s="60" t="s">
         <v>675</v>
       </c>
       <c r="E26" s="11" t="s">
@@ -12729,253 +12761,253 @@
       <c r="F26" s="11"/>
     </row>
     <row r="27" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="56" t="s">
+      <c r="A27" s="55" t="s">
         <v>206</v>
       </c>
-      <c r="C27" s="56" t="s">
+      <c r="C27" s="55" t="s">
         <v>696</v>
       </c>
-      <c r="D27" s="61" t="s">
+      <c r="D27" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E27" s="57" t="s">
+      <c r="E27" s="56" t="s">
         <v>697</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="56" t="s">
+      <c r="A28" s="55" t="s">
         <v>206</v>
       </c>
-      <c r="B28" s="56" t="s">
+      <c r="B28" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C28" s="56" t="s">
+      <c r="C28" s="55" t="s">
         <v>696</v>
       </c>
-      <c r="D28" s="61" t="s">
+      <c r="D28" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E28" s="57" t="s">
+      <c r="E28" s="56" t="s">
         <v>698</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="56" t="s">
+      <c r="A29" s="55" t="s">
         <v>206</v>
       </c>
-      <c r="B29" s="56" t="s">
+      <c r="B29" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C29" s="56" t="s">
+      <c r="C29" s="55" t="s">
         <v>696</v>
       </c>
-      <c r="D29" s="61" t="s">
+      <c r="D29" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E29" s="57" t="s">
+      <c r="E29" s="56" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="55" t="s">
         <v>222</v>
       </c>
-      <c r="C30" s="56" t="s">
+      <c r="C30" s="55" t="s">
         <v>696</v>
       </c>
-      <c r="D30" s="61" t="s">
+      <c r="D30" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E30" s="57" t="s">
+      <c r="E30" s="56" t="s">
         <v>700</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="55" t="s">
         <v>222</v>
       </c>
-      <c r="B31" s="56" t="s">
+      <c r="B31" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C31" s="56" t="s">
+      <c r="C31" s="55" t="s">
         <v>696</v>
       </c>
-      <c r="D31" s="61" t="s">
+      <c r="D31" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E31" s="57" t="s">
+      <c r="E31" s="56" t="s">
         <v>701</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="56" t="s">
+      <c r="A32" s="55" t="s">
         <v>222</v>
       </c>
-      <c r="B32" s="56" t="s">
+      <c r="B32" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C32" s="56" t="s">
+      <c r="C32" s="55" t="s">
         <v>696</v>
       </c>
-      <c r="D32" s="61" t="s">
+      <c r="D32" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="56" t="s">
         <v>699</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="56" t="s">
+      <c r="A33" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="C33" s="56" t="s">
+      <c r="C33" s="55" t="s">
         <v>702</v>
       </c>
-      <c r="D33" s="61" t="s">
+      <c r="D33" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E33" s="56" t="s">
+      <c r="E33" s="55" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="56" t="s">
+      <c r="A34" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="B34" s="56" t="s">
+      <c r="B34" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C34" s="56" t="s">
+      <c r="C34" s="55" t="s">
         <v>702</v>
       </c>
-      <c r="D34" s="61" t="s">
+      <c r="D34" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E34" s="56" t="s">
+      <c r="E34" s="55" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="56" t="s">
+      <c r="A35" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="B35" s="56" t="s">
+      <c r="B35" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C35" s="56" t="s">
+      <c r="C35" s="55" t="s">
         <v>702</v>
       </c>
-      <c r="D35" s="61" t="s">
+      <c r="D35" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E35" s="56" t="s">
+      <c r="E35" s="55" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="56" t="s">
+      <c r="A36" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="B36" s="56" t="s">
+      <c r="B36" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C36" s="56" t="s">
+      <c r="C36" s="55" t="s">
         <v>706</v>
       </c>
-      <c r="D36" s="61" t="s">
+      <c r="D36" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E36" s="56" t="s">
+      <c r="E36" s="55" t="s">
         <v>703</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="56" t="s">
+      <c r="A37" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="B37" s="56" t="s">
+      <c r="B37" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C37" s="56" t="s">
+      <c r="C37" s="55" t="s">
         <v>706</v>
       </c>
-      <c r="D37" s="61" t="s">
+      <c r="D37" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E37" s="56" t="s">
+      <c r="E37" s="55" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="56" t="s">
+      <c r="A38" s="55" t="s">
         <v>230</v>
       </c>
-      <c r="B38" s="56" t="s">
+      <c r="B38" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C38" s="56" t="s">
+      <c r="C38" s="55" t="s">
         <v>706</v>
       </c>
-      <c r="D38" s="61" t="s">
+      <c r="D38" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E38" s="56" t="s">
+      <c r="E38" s="55" t="s">
         <v>705</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="56" t="s">
+      <c r="A39" s="55" t="s">
         <v>42</v>
       </c>
-      <c r="C39" s="64" t="s">
+      <c r="C39" s="62" t="s">
         <v>33</v>
       </c>
-      <c r="D39" s="57" t="s">
+      <c r="D39" s="56" t="s">
         <v>675</v>
       </c>
-      <c r="E39" s="56" t="s">
+      <c r="E39" s="55" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="31.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="65" t="s">
+      <c r="A40" s="63" t="s">
         <v>609</v>
       </c>
       <c r="C40" s="11" t="s">
         <v>602</v>
       </c>
-      <c r="D40" s="66" t="s">
+      <c r="D40" s="64" t="s">
         <v>675</v>
       </c>
-      <c r="E40" s="67" t="s">
+      <c r="E40" s="65" t="s">
         <v>678</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="65" t="s">
+      <c r="A41" s="63" t="s">
         <v>624</v>
       </c>
-      <c r="C41" s="56" t="s">
+      <c r="C41" s="55" t="s">
         <v>707</v>
       </c>
-      <c r="D41" s="61" t="s">
+      <c r="D41" s="60" t="s">
         <v>676</v>
       </c>
-      <c r="E41" s="56" t="n">
+      <c r="E41" s="55" t="n">
         <v>1</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="68" t="s">
+      <c r="A42" s="66" t="s">
         <v>708</v>
       </c>
-      <c r="C42" s="56" t="s">
+      <c r="C42" s="55" t="s">
         <v>702</v>
       </c>
-      <c r="D42" s="57" t="s">
+      <c r="D42" s="56" t="s">
         <v>675</v>
       </c>
-      <c r="E42" s="56" t="s">
+      <c r="E42" s="55" t="s">
         <v>705</v>
       </c>
     </row>
@@ -12983,13 +13015,13 @@
       <c r="A43" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="C43" s="56" t="s">
+      <c r="C43" s="55" t="s">
         <v>702</v>
       </c>
-      <c r="D43" s="61" t="s">
+      <c r="D43" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E43" s="56" t="s">
+      <c r="E43" s="55" t="s">
         <v>709</v>
       </c>
     </row>
@@ -12997,27 +13029,27 @@
       <c r="A44" s="25" t="s">
         <v>264</v>
       </c>
-      <c r="B44" s="56" t="s">
+      <c r="B44" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C44" s="56" t="s">
+      <c r="C44" s="55" t="s">
         <v>702</v>
       </c>
-      <c r="D44" s="61" t="s">
+      <c r="D44" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E44" s="56" t="s">
+      <c r="E44" s="55" t="s">
         <v>704</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="62" t="s">
+      <c r="A45" s="61" t="s">
         <v>174</v>
       </c>
-      <c r="C45" s="56" t="s">
+      <c r="C45" s="55" t="s">
         <v>696</v>
       </c>
-      <c r="D45" s="57" t="s">
+      <c r="D45" s="56" t="s">
         <v>675</v>
       </c>
       <c r="E45" s="11" t="s">
@@ -13028,13 +13060,13 @@
       <c r="A46" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="C46" s="56" t="s">
+      <c r="C46" s="55" t="s">
         <v>711</v>
       </c>
-      <c r="D46" s="61" t="s">
+      <c r="D46" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E46" s="57" t="s">
+      <c r="E46" s="56" t="s">
         <v>712</v>
       </c>
     </row>
@@ -13042,16 +13074,16 @@
       <c r="A47" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="55" t="s">
         <v>679</v>
       </c>
-      <c r="C47" s="56" t="s">
+      <c r="C47" s="55" t="s">
         <v>711</v>
       </c>
-      <c r="D47" s="61" t="s">
+      <c r="D47" s="60" t="s">
         <v>675</v>
       </c>
-      <c r="E47" s="57" t="s">
+      <c r="E47" s="56" t="s">
         <v>713</v>
       </c>
     </row>
@@ -13062,10 +13094,10 @@
       <c r="C48" s="11" t="s">
         <v>580</v>
       </c>
-      <c r="D48" s="66" t="s">
+      <c r="D48" s="64" t="s">
         <v>675</v>
       </c>
-      <c r="E48" s="67" t="s">
+      <c r="E48" s="65" t="s">
         <v>678</v>
       </c>
     </row>
@@ -13076,10 +13108,10 @@
       <c r="C49" s="11" t="s">
         <v>552</v>
       </c>
-      <c r="D49" s="57" t="s">
+      <c r="D49" s="56" t="s">
         <v>675</v>
       </c>
-      <c r="E49" s="56" t="s">
+      <c r="E49" s="55" t="s">
         <v>678</v>
       </c>
     </row>
@@ -13126,28 +13158,28 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="19.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="70" t="s">
+      <c r="B1" s="68" t="s">
         <v>714</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="67" t="s">
         <v>715</v>
       </c>
-      <c r="D1" s="69" t="s">
+      <c r="D1" s="67" t="s">
         <v>716</v>
       </c>
-      <c r="E1" s="69" t="s">
+      <c r="E1" s="67" t="s">
         <v>717</v>
       </c>
-      <c r="F1" s="69" t="s">
+      <c r="F1" s="67" t="s">
         <v>718</v>
       </c>
       <c r="G1" s="7" t="s">
         <v>719</v>
       </c>
-      <c r="H1" s="69" t="s">
+      <c r="H1" s="67" t="s">
         <v>720</v>
       </c>
     </row>
@@ -13164,15 +13196,15 @@
       <c r="D2" s="11" t="s">
         <v>723</v>
       </c>
-      <c r="E2" s="71" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F2" s="71" t="b">
+      <c r="E2" s="69" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F2" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G2" s="71" t="b">
+      <c r="G2" s="69" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13190,15 +13222,15 @@
       <c r="D3" s="11" t="s">
         <v>726</v>
       </c>
-      <c r="E3" s="71" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F3" s="71" t="b">
+      <c r="E3" s="69" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G3" s="71" t="b">
+      <c r="G3" s="69" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13216,15 +13248,15 @@
       <c r="D4" s="11" t="s">
         <v>730</v>
       </c>
-      <c r="E4" s="71" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F4" s="71" t="b">
+      <c r="E4" s="69" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F4" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G4" s="71" t="b">
+      <c r="G4" s="69" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13242,15 +13274,15 @@
       <c r="D5" s="11" t="s">
         <v>733</v>
       </c>
-      <c r="E5" s="71" t="b">
+      <c r="E5" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F5" s="71" t="b">
+      <c r="F5" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G5" s="71" t="b">
+      <c r="G5" s="69" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13271,15 +13303,15 @@
       <c r="D6" s="11" t="s">
         <v>730</v>
       </c>
-      <c r="E6" s="71" t="b">
+      <c r="E6" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F6" s="71" t="b">
+      <c r="F6" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G6" s="71" t="b">
+      <c r="G6" s="69" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13300,15 +13332,15 @@
       <c r="D7" s="11" t="s">
         <v>729</v>
       </c>
-      <c r="E7" s="71" t="b">
+      <c r="E7" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F7" s="71" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G7" s="56"/>
+      <c r="F7" s="69" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G7" s="55"/>
       <c r="H7" s="11" t="s">
         <v>727</v>
       </c>
@@ -13326,15 +13358,15 @@
       <c r="D8" s="11" t="s">
         <v>739</v>
       </c>
-      <c r="E8" s="71" t="b">
+      <c r="E8" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F8" s="71" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="G8" s="56"/>
+      <c r="F8" s="69" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="G8" s="55"/>
       <c r="H8" s="11" t="s">
         <v>727</v>
       </c>
@@ -13352,15 +13384,15 @@
       <c r="D9" s="11" t="s">
         <v>742</v>
       </c>
-      <c r="E9" s="71" t="b">
+      <c r="E9" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F9" s="71" t="b">
+      <c r="F9" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G9" s="71" t="b">
+      <c r="G9" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -13381,15 +13413,15 @@
       <c r="D10" s="11" t="s">
         <v>745</v>
       </c>
-      <c r="E10" s="71" t="b">
+      <c r="E10" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F10" s="71" t="b">
+      <c r="F10" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G10" s="71" t="b">
+      <c r="G10" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -13410,15 +13442,15 @@
       <c r="D11" s="11" t="s">
         <v>748</v>
       </c>
-      <c r="E11" s="71" t="b">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
-      </c>
-      <c r="F11" s="71" t="b">
+      <c r="E11" s="69" t="b">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F11" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G11" s="71" t="b">
+      <c r="G11" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
@@ -13436,15 +13468,15 @@
       <c r="D12" s="11" t="s">
         <v>751</v>
       </c>
-      <c r="E12" s="71" t="b">
+      <c r="E12" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="F12" s="71" t="b">
+      <c r="F12" s="69" t="b">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="G12" s="71" t="b">
+      <c r="G12" s="69" t="b">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -13476,2002 +13508,2002 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="72" width="21.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="72" width="15.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="72" width="23.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="72" width="19.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="72" width="24.29"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="72" width="9.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="70" width="21.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="70" width="15.72"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="70" width="23.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="70" width="19.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="5" style="70" width="24.29"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="9" style="70" width="9.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="73" t="s">
+      <c r="A1" s="71" t="s">
         <v>752</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="71" t="s">
         <v>671</v>
       </c>
-      <c r="C1" s="73" t="s">
+      <c r="C1" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="73" t="s">
+      <c r="D1" s="71" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="74" t="s">
+      <c r="E1" s="72" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="74" t="s">
+      <c r="F1" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="73" t="s">
+      <c r="G1" s="71" t="s">
         <v>753</v>
       </c>
-      <c r="H1" s="73" t="s">
+      <c r="H1" s="71" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="72" t="s">
+      <c r="I1" s="70" t="s">
         <v>754</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="73" t="s">
         <v>678</v>
       </c>
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="73" t="s">
         <v>678</v>
       </c>
-      <c r="C2" s="75" t="s">
+      <c r="C2" s="73" t="s">
         <v>755</v>
       </c>
-      <c r="D2" s="75" t="s">
+      <c r="D2" s="73" t="s">
         <v>756</v>
       </c>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="73" t="s">
         <v>757</v>
       </c>
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="73" t="s">
         <v>757</v>
       </c>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="73" t="s">
         <v>758</v>
       </c>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="73" t="s">
         <v>759</v>
       </c>
-      <c r="E3" s="75"/>
-      <c r="F3" s="75"/>
-      <c r="G3" s="75"/>
-      <c r="H3" s="75"/>
+      <c r="E3" s="73"/>
+      <c r="F3" s="73"/>
+      <c r="G3" s="73"/>
+      <c r="H3" s="73"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="B4" s="75" t="s">
+      <c r="B4" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="C4" s="75" t="s">
+      <c r="C4" s="73" t="s">
         <v>760</v>
       </c>
-      <c r="D4" s="75" t="s">
+      <c r="D4" s="73" t="s">
         <v>761</v>
       </c>
-      <c r="E4" s="75"/>
-      <c r="F4" s="75"/>
-      <c r="G4" s="75"/>
-      <c r="H4" s="75"/>
+      <c r="E4" s="73"/>
+      <c r="F4" s="73"/>
+      <c r="G4" s="73"/>
+      <c r="H4" s="73"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="73" t="s">
         <v>762</v>
       </c>
-      <c r="B5" s="75" t="s">
+      <c r="B5" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="C5" s="75" t="s">
+      <c r="C5" s="73" t="s">
         <v>763</v>
       </c>
-      <c r="D5" s="75" t="s">
+      <c r="D5" s="73" t="s">
         <v>764</v>
       </c>
-      <c r="E5" s="75"/>
-      <c r="F5" s="75"/>
-      <c r="G5" s="75"/>
-      <c r="H5" s="75"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="73"/>
+      <c r="H5" s="73"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="75" t="s">
+      <c r="A6" s="73" t="s">
         <v>765</v>
       </c>
-      <c r="B6" s="75" t="s">
+      <c r="B6" s="73" t="s">
         <v>765</v>
       </c>
-      <c r="C6" s="75" t="s">
+      <c r="C6" s="73" t="s">
         <v>766</v>
       </c>
-      <c r="D6" s="75" t="s">
+      <c r="D6" s="73" t="s">
         <v>767</v>
       </c>
-      <c r="E6" s="75"/>
-      <c r="F6" s="75"/>
-      <c r="G6" s="75"/>
-      <c r="H6" s="75"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="73"/>
+      <c r="H6" s="73"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="75" t="s">
+      <c r="A7" s="73" t="s">
         <v>682</v>
       </c>
-      <c r="B7" s="75" t="s">
+      <c r="B7" s="73" t="s">
         <v>682</v>
       </c>
-      <c r="C7" s="75" t="s">
+      <c r="C7" s="73" t="s">
         <v>768</v>
       </c>
-      <c r="D7" s="75" t="s">
+      <c r="D7" s="73" t="s">
         <v>769</v>
       </c>
-      <c r="E7" s="75"/>
-      <c r="F7" s="75"/>
-      <c r="G7" s="75"/>
-      <c r="H7" s="75"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="73"/>
+      <c r="H7" s="73"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="75"/>
-      <c r="D8" s="75"/>
-      <c r="E8" s="75"/>
-      <c r="F8" s="75"/>
-      <c r="G8" s="75" t="s">
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73" t="s">
         <v>678</v>
       </c>
-      <c r="H8" s="75"/>
+      <c r="H8" s="73"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="75" t="s">
+      <c r="A9" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="B9" s="75"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75" t="s">
+      <c r="B9" s="73"/>
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="73" t="s">
         <v>757</v>
       </c>
-      <c r="H9" s="75"/>
+      <c r="H9" s="73"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="75" t="s">
+      <c r="A10" s="73" t="s">
         <v>184</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="75"/>
-      <c r="D10" s="75"/>
-      <c r="E10" s="75"/>
-      <c r="F10" s="75"/>
-      <c r="G10" s="75" t="s">
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="73" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="75"/>
+      <c r="H10" s="73"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="75" t="s">
+      <c r="A11" s="73" t="s">
         <v>184</v>
       </c>
-      <c r="B11" s="75"/>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75" t="s">
+      <c r="B11" s="73"/>
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="73"/>
+      <c r="G11" s="73" t="s">
         <v>765</v>
       </c>
-      <c r="H11" s="75"/>
+      <c r="H11" s="73"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="75" t="s">
+      <c r="A12" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="B12" s="75"/>
-      <c r="C12" s="75"/>
-      <c r="D12" s="75"/>
-      <c r="E12" s="75"/>
-      <c r="F12" s="75"/>
-      <c r="G12" s="75" t="s">
+      <c r="B12" s="73"/>
+      <c r="C12" s="73"/>
+      <c r="D12" s="73"/>
+      <c r="E12" s="73"/>
+      <c r="F12" s="73"/>
+      <c r="G12" s="73" t="s">
         <v>678</v>
       </c>
-      <c r="H12" s="75"/>
+      <c r="H12" s="73"/>
     </row>
     <row r="13" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="75" t="s">
+      <c r="A13" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="B13" s="75"/>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="75"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="75" t="s">
+      <c r="B13" s="73"/>
+      <c r="C13" s="73"/>
+      <c r="D13" s="73"/>
+      <c r="E13" s="73"/>
+      <c r="F13" s="73"/>
+      <c r="G13" s="73" t="s">
         <v>757</v>
       </c>
-      <c r="H13" s="75"/>
-      <c r="I13" s="72"/>
+      <c r="H13" s="73"/>
+      <c r="I13" s="70"/>
     </row>
     <row r="14" s="2" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="75" t="s">
+      <c r="A14" s="73" t="s">
         <v>102</v>
       </c>
-      <c r="B14" s="75"/>
-      <c r="C14" s="75"/>
-      <c r="D14" s="75"/>
-      <c r="E14" s="75"/>
-      <c r="F14" s="75"/>
-      <c r="G14" s="75" t="s">
+      <c r="B14" s="73"/>
+      <c r="C14" s="73"/>
+      <c r="D14" s="73"/>
+      <c r="E14" s="73"/>
+      <c r="F14" s="73"/>
+      <c r="G14" s="73" t="s">
         <v>682</v>
       </c>
-      <c r="H14" s="75"/>
-      <c r="I14" s="72"/>
+      <c r="H14" s="73"/>
+      <c r="I14" s="70"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="76" t="s">
+      <c r="A15" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="B15" s="75" t="s">
+      <c r="B15" s="73" t="s">
         <v>770</v>
       </c>
-      <c r="C15" s="75" t="s">
+      <c r="C15" s="73" t="s">
         <v>771</v>
       </c>
-      <c r="D15" s="75" t="s">
+      <c r="D15" s="73" t="s">
         <v>772</v>
       </c>
-      <c r="E15" s="75"/>
-      <c r="F15" s="75"/>
-      <c r="G15" s="75"/>
-      <c r="H15" s="75"/>
+      <c r="E15" s="73"/>
+      <c r="F15" s="73"/>
+      <c r="G15" s="73"/>
+      <c r="H15" s="73"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="76" t="s">
+      <c r="A16" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="B16" s="75" t="s">
+      <c r="B16" s="73" t="s">
         <v>773</v>
       </c>
-      <c r="C16" s="75" t="s">
+      <c r="C16" s="73" t="s">
         <v>774</v>
       </c>
-      <c r="D16" s="75" t="s">
+      <c r="D16" s="73" t="s">
         <v>775</v>
       </c>
-      <c r="E16" s="75"/>
-      <c r="F16" s="75"/>
-      <c r="G16" s="75"/>
-      <c r="H16" s="75"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="73"/>
+      <c r="G16" s="73"/>
+      <c r="H16" s="73"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="74" t="s">
         <v>134</v>
       </c>
-      <c r="B17" s="75"/>
-      <c r="C17" s="75"/>
-      <c r="D17" s="75"/>
-      <c r="E17" s="75"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="75" t="s">
+      <c r="B17" s="73"/>
+      <c r="C17" s="73"/>
+      <c r="D17" s="73"/>
+      <c r="E17" s="73"/>
+      <c r="F17" s="73"/>
+      <c r="G17" s="73" t="s">
         <v>682</v>
       </c>
-      <c r="H17" s="75"/>
+      <c r="H17" s="73"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="76" t="s">
+      <c r="A18" s="74" t="s">
         <v>140</v>
       </c>
-      <c r="B18" s="75" t="s">
+      <c r="B18" s="73" t="s">
         <v>770</v>
       </c>
-      <c r="C18" s="75" t="s">
+      <c r="C18" s="73" t="s">
         <v>771</v>
       </c>
-      <c r="D18" s="75" t="s">
+      <c r="D18" s="73" t="s">
         <v>776</v>
       </c>
-      <c r="E18" s="75"/>
-      <c r="F18" s="75"/>
-      <c r="G18" s="75"/>
-      <c r="H18" s="75"/>
+      <c r="E18" s="73"/>
+      <c r="F18" s="73"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="73"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="76" t="s">
+      <c r="A19" s="74" t="s">
         <v>140</v>
       </c>
-      <c r="B19" s="75" t="s">
+      <c r="B19" s="73" t="s">
         <v>773</v>
       </c>
-      <c r="C19" s="75" t="s">
+      <c r="C19" s="73" t="s">
         <v>774</v>
       </c>
-      <c r="D19" s="75" t="s">
+      <c r="D19" s="73" t="s">
         <v>777</v>
       </c>
-      <c r="E19" s="75"/>
-      <c r="F19" s="75"/>
-      <c r="G19" s="75"/>
-      <c r="H19" s="75"/>
+      <c r="E19" s="73"/>
+      <c r="F19" s="73"/>
+      <c r="G19" s="73"/>
+      <c r="H19" s="73"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="76" t="s">
+      <c r="A20" s="74" t="s">
         <v>140</v>
       </c>
-      <c r="B20" s="75" t="s">
+      <c r="B20" s="73" t="s">
         <v>142</v>
       </c>
-      <c r="C20" s="75" t="s">
+      <c r="C20" s="73" t="s">
         <v>778</v>
       </c>
-      <c r="D20" s="75" t="s">
+      <c r="D20" s="73" t="s">
         <v>779</v>
       </c>
-      <c r="E20" s="75"/>
-      <c r="F20" s="75"/>
-      <c r="G20" s="75"/>
-      <c r="H20" s="75"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="73"/>
+      <c r="G20" s="73"/>
+      <c r="H20" s="73"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="76" t="s">
+      <c r="A21" s="74" t="s">
         <v>140</v>
       </c>
-      <c r="B21" s="75"/>
-      <c r="C21" s="75"/>
-      <c r="D21" s="75"/>
-      <c r="E21" s="75"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="75" t="s">
+      <c r="B21" s="73"/>
+      <c r="C21" s="73"/>
+      <c r="D21" s="73"/>
+      <c r="E21" s="73"/>
+      <c r="F21" s="73"/>
+      <c r="G21" s="73" t="s">
         <v>682</v>
       </c>
-      <c r="H21" s="75"/>
+      <c r="H21" s="73"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="75" t="s">
+      <c r="A22" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="B22" s="75" t="s">
+      <c r="B22" s="73" t="s">
         <v>712</v>
       </c>
-      <c r="C22" s="75" t="s">
+      <c r="C22" s="73" t="s">
         <v>780</v>
       </c>
-      <c r="D22" s="75" t="s">
+      <c r="D22" s="73" t="s">
         <v>781</v>
       </c>
-      <c r="E22" s="75"/>
-      <c r="F22" s="75"/>
-      <c r="G22" s="75"/>
-      <c r="H22" s="75"/>
+      <c r="E22" s="73"/>
+      <c r="F22" s="73"/>
+      <c r="G22" s="73"/>
+      <c r="H22" s="73"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="75" t="s">
+      <c r="A23" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="B23" s="75" t="s">
+      <c r="B23" s="73" t="s">
         <v>713</v>
       </c>
-      <c r="C23" s="75" t="s">
+      <c r="C23" s="73" t="s">
         <v>782</v>
       </c>
-      <c r="D23" s="75" t="s">
+      <c r="D23" s="73" t="s">
         <v>783</v>
       </c>
-      <c r="E23" s="75"/>
-      <c r="F23" s="75"/>
-      <c r="G23" s="75"/>
-      <c r="H23" s="75"/>
+      <c r="E23" s="73"/>
+      <c r="F23" s="73"/>
+      <c r="G23" s="73"/>
+      <c r="H23" s="73"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="75" t="s">
+      <c r="A24" s="73" t="s">
         <v>149</v>
       </c>
-      <c r="B24" s="75"/>
-      <c r="C24" s="75"/>
-      <c r="D24" s="75"/>
-      <c r="E24" s="75"/>
-      <c r="F24" s="75"/>
-      <c r="G24" s="75" t="s">
+      <c r="B24" s="73"/>
+      <c r="C24" s="73"/>
+      <c r="D24" s="73"/>
+      <c r="E24" s="73"/>
+      <c r="F24" s="73"/>
+      <c r="G24" s="73" t="s">
         <v>757</v>
       </c>
-      <c r="H24" s="75"/>
+      <c r="H24" s="73"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="75" t="s">
+      <c r="A25" s="73" t="s">
         <v>155</v>
       </c>
-      <c r="B25" s="75" t="s">
+      <c r="B25" s="73" t="s">
         <v>712</v>
       </c>
-      <c r="C25" s="75" t="s">
+      <c r="C25" s="73" t="s">
         <v>784</v>
       </c>
-      <c r="D25" s="75" t="s">
+      <c r="D25" s="73" t="s">
         <v>785</v>
       </c>
-      <c r="E25" s="75"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="75"/>
-      <c r="H25" s="75"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="73"/>
+      <c r="G25" s="73"/>
+      <c r="H25" s="73"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="75" t="s">
+      <c r="A26" s="73" t="s">
         <v>155</v>
       </c>
-      <c r="B26" s="75" t="s">
+      <c r="B26" s="73" t="s">
         <v>713</v>
       </c>
-      <c r="C26" s="75" t="s">
+      <c r="C26" s="73" t="s">
         <v>786</v>
       </c>
-      <c r="D26" s="75" t="s">
+      <c r="D26" s="73" t="s">
         <v>787</v>
       </c>
-      <c r="E26" s="75"/>
-      <c r="F26" s="75"/>
-      <c r="G26" s="75"/>
-      <c r="H26" s="75"/>
+      <c r="E26" s="73"/>
+      <c r="F26" s="73"/>
+      <c r="G26" s="73"/>
+      <c r="H26" s="73"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="75" t="s">
+      <c r="A27" s="73" t="s">
         <v>155</v>
       </c>
-      <c r="B27" s="75"/>
-      <c r="C27" s="75"/>
-      <c r="D27" s="75"/>
-      <c r="E27" s="75"/>
-      <c r="F27" s="75"/>
-      <c r="G27" s="75" t="s">
+      <c r="B27" s="73"/>
+      <c r="C27" s="73"/>
+      <c r="D27" s="73"/>
+      <c r="E27" s="73"/>
+      <c r="F27" s="73"/>
+      <c r="G27" s="73" t="s">
         <v>757</v>
       </c>
-      <c r="H27" s="75"/>
+      <c r="H27" s="73"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="75" t="s">
+      <c r="A28" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="B28" s="75" t="s">
+      <c r="B28" s="73" t="s">
         <v>788</v>
       </c>
-      <c r="C28" s="75" t="s">
+      <c r="C28" s="73" t="s">
         <v>789</v>
       </c>
-      <c r="D28" s="75" t="s">
+      <c r="D28" s="73" t="s">
         <v>790</v>
       </c>
-      <c r="E28" s="75"/>
-      <c r="F28" s="75"/>
-      <c r="G28" s="75"/>
-      <c r="H28" s="75" t="s">
+      <c r="E28" s="73"/>
+      <c r="F28" s="73"/>
+      <c r="G28" s="73"/>
+      <c r="H28" s="73" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="75" t="s">
+      <c r="A29" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="B29" s="75" t="s">
+      <c r="B29" s="73" t="s">
         <v>791</v>
       </c>
-      <c r="C29" s="75" t="s">
+      <c r="C29" s="73" t="s">
         <v>792</v>
       </c>
-      <c r="D29" s="75" t="s">
+      <c r="D29" s="73" t="s">
         <v>793</v>
       </c>
-      <c r="E29" s="75"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="75"/>
-      <c r="H29" s="75" t="s">
+      <c r="E29" s="73"/>
+      <c r="F29" s="73"/>
+      <c r="G29" s="73"/>
+      <c r="H29" s="73" t="s">
         <v>687</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="75" t="s">
+      <c r="A30" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="B30" s="75" t="s">
+      <c r="B30" s="73" t="s">
         <v>794</v>
       </c>
-      <c r="C30" s="75" t="s">
+      <c r="C30" s="73" t="s">
         <v>795</v>
       </c>
-      <c r="D30" s="75" t="s">
+      <c r="D30" s="73" t="s">
         <v>796</v>
       </c>
-      <c r="E30" s="75"/>
-      <c r="F30" s="75"/>
-      <c r="G30" s="75"/>
-      <c r="H30" s="75" t="s">
+      <c r="E30" s="73"/>
+      <c r="F30" s="73"/>
+      <c r="G30" s="73"/>
+      <c r="H30" s="73" t="s">
         <v>690</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="B31" s="75" t="s">
+      <c r="B31" s="73" t="s">
         <v>797</v>
       </c>
-      <c r="C31" s="75" t="s">
+      <c r="C31" s="73" t="s">
         <v>798</v>
       </c>
-      <c r="D31" s="75" t="s">
+      <c r="D31" s="73" t="s">
         <v>799</v>
       </c>
-      <c r="E31" s="75"/>
-      <c r="F31" s="75"/>
-      <c r="G31" s="75"/>
-      <c r="H31" s="75" t="s">
+      <c r="E31" s="73"/>
+      <c r="F31" s="73"/>
+      <c r="G31" s="73"/>
+      <c r="H31" s="73" t="s">
         <v>688</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="75" t="s">
+      <c r="A32" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="B32" s="75" t="s">
+      <c r="B32" s="73" t="s">
         <v>800</v>
       </c>
-      <c r="C32" s="75" t="s">
+      <c r="C32" s="73" t="s">
         <v>801</v>
       </c>
-      <c r="D32" s="75" t="s">
+      <c r="D32" s="73" t="s">
         <v>802</v>
       </c>
-      <c r="E32" s="75"/>
-      <c r="F32" s="75"/>
-      <c r="G32" s="75"/>
-      <c r="H32" s="75" t="s">
+      <c r="E32" s="73"/>
+      <c r="F32" s="73"/>
+      <c r="G32" s="73"/>
+      <c r="H32" s="73" t="s">
         <v>689</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="75" t="s">
+      <c r="A33" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="B33" s="75" t="s">
+      <c r="B33" s="73" t="s">
         <v>803</v>
       </c>
-      <c r="C33" s="75" t="s">
+      <c r="C33" s="73" t="s">
         <v>804</v>
       </c>
-      <c r="D33" s="75" t="s">
+      <c r="D33" s="73" t="s">
         <v>805</v>
       </c>
-      <c r="E33" s="75"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="75"/>
-      <c r="H33" s="75" t="s">
+      <c r="E33" s="73"/>
+      <c r="F33" s="73"/>
+      <c r="G33" s="73"/>
+      <c r="H33" s="73" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="75" t="s">
+      <c r="A34" s="73" t="s">
         <v>157</v>
       </c>
-      <c r="B34" s="75"/>
-      <c r="C34" s="75"/>
-      <c r="D34" s="75"/>
-      <c r="E34" s="75"/>
-      <c r="F34" s="75"/>
-      <c r="G34" s="75" t="s">
+      <c r="B34" s="73"/>
+      <c r="C34" s="73"/>
+      <c r="D34" s="73"/>
+      <c r="E34" s="73"/>
+      <c r="F34" s="73"/>
+      <c r="G34" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="H34" s="75"/>
+      <c r="H34" s="73"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="75" t="s">
+      <c r="A35" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B35" s="75" t="s">
+      <c r="B35" s="73" t="s">
         <v>697</v>
       </c>
-      <c r="C35" s="75" t="s">
+      <c r="C35" s="73" t="s">
         <v>806</v>
       </c>
-      <c r="D35" s="75" t="s">
+      <c r="D35" s="73" t="s">
         <v>807</v>
       </c>
-      <c r="E35" s="75"/>
-      <c r="F35" s="75"/>
-      <c r="G35" s="75"/>
-      <c r="H35" s="75"/>
-      <c r="I35" s="72" t="s">
+      <c r="E35" s="73"/>
+      <c r="F35" s="73"/>
+      <c r="G35" s="73"/>
+      <c r="H35" s="73"/>
+      <c r="I35" s="70" t="s">
         <v>808</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="75" t="s">
+      <c r="A36" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B36" s="75" t="s">
+      <c r="B36" s="73" t="s">
         <v>698</v>
       </c>
-      <c r="C36" s="75" t="s">
+      <c r="C36" s="73" t="s">
         <v>809</v>
       </c>
-      <c r="D36" s="75" t="s">
+      <c r="D36" s="73" t="s">
         <v>810</v>
       </c>
-      <c r="E36" s="75"/>
-      <c r="F36" s="75"/>
-      <c r="G36" s="75"/>
-      <c r="H36" s="75"/>
-      <c r="I36" s="72" t="s">
+      <c r="E36" s="73"/>
+      <c r="F36" s="73"/>
+      <c r="G36" s="73"/>
+      <c r="H36" s="73"/>
+      <c r="I36" s="70" t="s">
         <v>808</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="75" t="s">
+      <c r="A37" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B37" s="75" t="s">
+      <c r="B37" s="73" t="s">
         <v>699</v>
       </c>
-      <c r="C37" s="75" t="s">
+      <c r="C37" s="73" t="s">
         <v>811</v>
       </c>
-      <c r="D37" s="75" t="s">
+      <c r="D37" s="73" t="s">
         <v>812</v>
       </c>
-      <c r="E37" s="75"/>
-      <c r="F37" s="75"/>
-      <c r="G37" s="75"/>
-      <c r="H37" s="75"/>
-      <c r="I37" s="72" t="s">
+      <c r="E37" s="73"/>
+      <c r="F37" s="73"/>
+      <c r="G37" s="73"/>
+      <c r="H37" s="73"/>
+      <c r="I37" s="70" t="s">
         <v>808</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="75" t="s">
+      <c r="A38" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B38" s="75" t="s">
+      <c r="B38" s="73" t="s">
         <v>700</v>
       </c>
-      <c r="C38" s="75" t="s">
+      <c r="C38" s="73" t="s">
         <v>813</v>
       </c>
-      <c r="D38" s="75" t="s">
+      <c r="D38" s="73" t="s">
         <v>814</v>
       </c>
-      <c r="E38" s="75"/>
-      <c r="F38" s="75"/>
-      <c r="G38" s="75"/>
-      <c r="H38" s="75"/>
-      <c r="I38" s="72" t="s">
+      <c r="E38" s="73"/>
+      <c r="F38" s="73"/>
+      <c r="G38" s="73"/>
+      <c r="H38" s="73"/>
+      <c r="I38" s="70" t="s">
         <v>808</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="75" t="s">
+      <c r="A39" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B39" s="75" t="s">
+      <c r="B39" s="73" t="s">
         <v>701</v>
       </c>
-      <c r="C39" s="75" t="s">
+      <c r="C39" s="73" t="s">
         <v>815</v>
       </c>
-      <c r="D39" s="75" t="s">
+      <c r="D39" s="73" t="s">
         <v>816</v>
       </c>
-      <c r="E39" s="75"/>
-      <c r="F39" s="75"/>
-      <c r="G39" s="75"/>
-      <c r="H39" s="75"/>
-      <c r="I39" s="72" t="s">
+      <c r="E39" s="73"/>
+      <c r="F39" s="73"/>
+      <c r="G39" s="73"/>
+      <c r="H39" s="73"/>
+      <c r="I39" s="70" t="s">
         <v>808</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="75" t="s">
+      <c r="A40" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B40" s="75" t="s">
+      <c r="B40" s="73" t="s">
         <v>817</v>
       </c>
-      <c r="C40" s="75" t="s">
+      <c r="C40" s="73" t="s">
         <v>818</v>
       </c>
-      <c r="D40" s="75" t="s">
+      <c r="D40" s="73" t="s">
         <v>819</v>
       </c>
-      <c r="E40" s="75"/>
-      <c r="F40" s="75"/>
-      <c r="G40" s="75"/>
-      <c r="H40" s="75" t="s">
+      <c r="E40" s="73"/>
+      <c r="F40" s="73"/>
+      <c r="G40" s="73"/>
+      <c r="H40" s="73" t="s">
         <v>694</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="75" t="s">
+      <c r="A41" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B41" s="75" t="s">
+      <c r="B41" s="73" t="s">
         <v>800</v>
       </c>
-      <c r="C41" s="75" t="s">
+      <c r="C41" s="73" t="s">
         <v>801</v>
       </c>
-      <c r="D41" s="75" t="s">
+      <c r="D41" s="73" t="s">
         <v>802</v>
       </c>
-      <c r="E41" s="75"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="75"/>
-      <c r="H41" s="75"/>
+      <c r="E41" s="73"/>
+      <c r="F41" s="73"/>
+      <c r="G41" s="73"/>
+      <c r="H41" s="73"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="75" t="s">
+      <c r="A42" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B42" s="75" t="s">
+      <c r="B42" s="73" t="s">
         <v>820</v>
       </c>
-      <c r="C42" s="75" t="s">
+      <c r="C42" s="73" t="s">
         <v>821</v>
       </c>
-      <c r="D42" s="75" t="s">
+      <c r="D42" s="73" t="s">
         <v>822</v>
       </c>
-      <c r="E42" s="75"/>
-      <c r="F42" s="75"/>
-      <c r="G42" s="75"/>
-      <c r="H42" s="75"/>
+      <c r="E42" s="73"/>
+      <c r="F42" s="73"/>
+      <c r="G42" s="73"/>
+      <c r="H42" s="73"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="75" t="s">
+      <c r="A43" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B43" s="77" t="s">
+      <c r="B43" s="75" t="s">
         <v>710</v>
       </c>
-      <c r="C43" s="75" t="s">
+      <c r="C43" s="73" t="s">
         <v>823</v>
       </c>
-      <c r="D43" s="75" t="s">
+      <c r="D43" s="73" t="s">
         <v>824</v>
       </c>
-      <c r="E43" s="75"/>
-      <c r="F43" s="75"/>
-      <c r="G43" s="75"/>
-      <c r="H43" s="75"/>
+      <c r="E43" s="73"/>
+      <c r="F43" s="73"/>
+      <c r="G43" s="73"/>
+      <c r="H43" s="73"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="75" t="s">
+      <c r="A44" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B44" s="75" t="s">
+      <c r="B44" s="73" t="s">
         <v>825</v>
       </c>
-      <c r="C44" s="75" t="s">
+      <c r="C44" s="73" t="s">
         <v>826</v>
       </c>
-      <c r="D44" s="75" t="s">
+      <c r="D44" s="73" t="s">
         <v>827</v>
       </c>
-      <c r="E44" s="75"/>
-      <c r="F44" s="75"/>
-      <c r="G44" s="75"/>
-      <c r="H44" s="75"/>
+      <c r="E44" s="73"/>
+      <c r="F44" s="73"/>
+      <c r="G44" s="73"/>
+      <c r="H44" s="73"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="75" t="s">
+      <c r="A45" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B45" s="75" t="s">
+      <c r="B45" s="73" t="s">
         <v>828</v>
       </c>
-      <c r="C45" s="75" t="s">
+      <c r="C45" s="73" t="s">
         <v>829</v>
       </c>
-      <c r="D45" s="75" t="s">
+      <c r="D45" s="73" t="s">
         <v>830</v>
       </c>
-      <c r="E45" s="75"/>
-      <c r="F45" s="75"/>
-      <c r="G45" s="75"/>
-      <c r="H45" s="75"/>
+      <c r="E45" s="73"/>
+      <c r="F45" s="73"/>
+      <c r="G45" s="73"/>
+      <c r="H45" s="73"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="75" t="s">
+      <c r="A46" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B46" s="75" t="s">
+      <c r="B46" s="73" t="s">
         <v>162</v>
       </c>
-      <c r="C46" s="75" t="s">
+      <c r="C46" s="73" t="s">
         <v>763</v>
       </c>
-      <c r="D46" s="75" t="s">
+      <c r="D46" s="73" t="s">
         <v>764</v>
       </c>
-      <c r="E46" s="75"/>
-      <c r="F46" s="75"/>
-      <c r="G46" s="75"/>
-      <c r="H46" s="75"/>
+      <c r="E46" s="73"/>
+      <c r="F46" s="73"/>
+      <c r="G46" s="73"/>
+      <c r="H46" s="73"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="75" t="s">
+      <c r="A47" s="73" t="s">
         <v>163</v>
       </c>
-      <c r="B47" s="75" t="s">
+      <c r="B47" s="73" t="s">
         <v>682</v>
       </c>
-      <c r="C47" s="75" t="s">
+      <c r="C47" s="73" t="s">
         <v>831</v>
       </c>
-      <c r="D47" s="75" t="s">
+      <c r="D47" s="73" t="s">
         <v>832</v>
       </c>
-      <c r="E47" s="75"/>
-      <c r="F47" s="75"/>
-      <c r="G47" s="75"/>
-      <c r="H47" s="75"/>
+      <c r="E47" s="73"/>
+      <c r="F47" s="73"/>
+      <c r="G47" s="73"/>
+      <c r="H47" s="73"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="75" t="s">
+      <c r="A48" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="B48" s="75"/>
-      <c r="C48" s="75"/>
-      <c r="D48" s="75"/>
-      <c r="E48" s="75"/>
-      <c r="F48" s="75"/>
-      <c r="G48" s="75" t="s">
+      <c r="B48" s="73"/>
+      <c r="C48" s="73"/>
+      <c r="D48" s="73"/>
+      <c r="E48" s="73"/>
+      <c r="F48" s="73"/>
+      <c r="G48" s="73" t="s">
         <v>757</v>
       </c>
-      <c r="H48" s="75"/>
+      <c r="H48" s="73"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="75" t="s">
+      <c r="A49" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="B49" s="75" t="s">
+      <c r="B49" s="73" t="s">
         <v>833</v>
       </c>
-      <c r="C49" s="75" t="s">
+      <c r="C49" s="73" t="s">
         <v>834</v>
       </c>
-      <c r="D49" s="75" t="s">
+      <c r="D49" s="73" t="s">
         <v>835</v>
       </c>
-      <c r="E49" s="75"/>
-      <c r="F49" s="75"/>
-      <c r="G49" s="75"/>
-      <c r="H49" s="75"/>
+      <c r="E49" s="73"/>
+      <c r="F49" s="73"/>
+      <c r="G49" s="73"/>
+      <c r="H49" s="73"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="75" t="s">
+      <c r="A50" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="B50" s="75" t="s">
+      <c r="B50" s="73" t="s">
         <v>836</v>
       </c>
-      <c r="C50" s="75" t="s">
+      <c r="C50" s="73" t="s">
         <v>837</v>
       </c>
-      <c r="D50" s="75" t="s">
+      <c r="D50" s="73" t="s">
         <v>838</v>
       </c>
-      <c r="E50" s="75"/>
-      <c r="F50" s="75"/>
-      <c r="G50" s="75"/>
-      <c r="H50" s="75"/>
+      <c r="E50" s="73"/>
+      <c r="F50" s="73"/>
+      <c r="G50" s="73"/>
+      <c r="H50" s="73"/>
     </row>
     <row r="51" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="75" t="s">
+      <c r="A51" s="73" t="s">
         <v>199</v>
       </c>
-      <c r="B51" s="75"/>
-      <c r="C51" s="75"/>
-      <c r="D51" s="75"/>
-      <c r="E51" s="75"/>
-      <c r="F51" s="75"/>
-      <c r="G51" s="75" t="s">
+      <c r="B51" s="73"/>
+      <c r="C51" s="73"/>
+      <c r="D51" s="73"/>
+      <c r="E51" s="73"/>
+      <c r="F51" s="73"/>
+      <c r="G51" s="73" t="s">
         <v>765</v>
       </c>
-      <c r="H51" s="75"/>
+      <c r="H51" s="73"/>
     </row>
     <row r="52" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="76" t="s">
+      <c r="A52" s="74" t="s">
         <v>207</v>
       </c>
-      <c r="B52" s="75" t="s">
+      <c r="B52" s="73" t="s">
         <v>703</v>
       </c>
-      <c r="C52" s="75" t="s">
+      <c r="C52" s="73" t="s">
         <v>839</v>
       </c>
-      <c r="D52" s="75" t="s">
+      <c r="D52" s="73" t="s">
         <v>840</v>
       </c>
-      <c r="E52" s="75"/>
-      <c r="F52" s="75"/>
-      <c r="G52" s="75"/>
-      <c r="H52" s="75"/>
+      <c r="E52" s="73"/>
+      <c r="F52" s="73"/>
+      <c r="G52" s="73"/>
+      <c r="H52" s="73"/>
     </row>
     <row r="53" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="76" t="s">
+      <c r="A53" s="74" t="s">
         <v>207</v>
       </c>
-      <c r="B53" s="75" t="s">
+      <c r="B53" s="73" t="s">
         <v>704</v>
       </c>
-      <c r="C53" s="75" t="s">
+      <c r="C53" s="73" t="s">
         <v>841</v>
       </c>
-      <c r="D53" s="75" t="s">
+      <c r="D53" s="73" t="s">
         <v>842</v>
       </c>
-      <c r="E53" s="75"/>
-      <c r="F53" s="75"/>
-      <c r="G53" s="75"/>
-      <c r="H53" s="75"/>
+      <c r="E53" s="73"/>
+      <c r="F53" s="73"/>
+      <c r="G53" s="73"/>
+      <c r="H53" s="73"/>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="76" t="s">
+      <c r="A54" s="74" t="s">
         <v>207</v>
       </c>
-      <c r="B54" s="75" t="s">
+      <c r="B54" s="73" t="s">
         <v>705</v>
       </c>
-      <c r="C54" s="75" t="s">
+      <c r="C54" s="73" t="s">
         <v>843</v>
       </c>
-      <c r="D54" s="75" t="s">
+      <c r="D54" s="73" t="s">
         <v>844</v>
       </c>
-      <c r="E54" s="75"/>
-      <c r="F54" s="75"/>
-      <c r="G54" s="75"/>
-      <c r="H54" s="75"/>
+      <c r="E54" s="73"/>
+      <c r="F54" s="73"/>
+      <c r="G54" s="73"/>
+      <c r="H54" s="73"/>
     </row>
     <row r="55" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="76" t="s">
+      <c r="A55" s="74" t="s">
         <v>207</v>
       </c>
-      <c r="B55" s="75" t="s">
+      <c r="B55" s="73" t="s">
         <v>845</v>
       </c>
-      <c r="C55" s="75" t="s">
+      <c r="C55" s="73" t="s">
         <v>846</v>
       </c>
-      <c r="D55" s="75" t="s">
+      <c r="D55" s="73" t="s">
         <v>847</v>
       </c>
-      <c r="E55" s="75"/>
-      <c r="F55" s="75"/>
-      <c r="G55" s="75"/>
-      <c r="H55" s="75"/>
+      <c r="E55" s="73"/>
+      <c r="F55" s="73"/>
+      <c r="G55" s="73"/>
+      <c r="H55" s="73"/>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="76" t="s">
+      <c r="A56" s="74" t="s">
         <v>207</v>
       </c>
-      <c r="B56" s="75" t="s">
+      <c r="B56" s="73" t="s">
         <v>709</v>
       </c>
-      <c r="C56" s="75" t="s">
+      <c r="C56" s="73" t="s">
         <v>848</v>
       </c>
-      <c r="D56" s="75" t="s">
+      <c r="D56" s="73" t="s">
         <v>849</v>
       </c>
-      <c r="E56" s="75"/>
-      <c r="F56" s="75"/>
-      <c r="G56" s="75"/>
-      <c r="H56" s="75"/>
+      <c r="E56" s="73"/>
+      <c r="F56" s="73"/>
+      <c r="G56" s="73"/>
+      <c r="H56" s="73"/>
     </row>
     <row r="57" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="76" t="s">
+      <c r="A57" s="74" t="s">
         <v>223</v>
       </c>
-      <c r="B57" s="72" t="s">
+      <c r="B57" s="70" t="s">
         <v>703</v>
       </c>
-      <c r="C57" s="72" t="s">
+      <c r="C57" s="70" t="s">
         <v>850</v>
       </c>
-      <c r="D57" s="72" t="s">
+      <c r="D57" s="70" t="s">
         <v>840</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="76" t="s">
+      <c r="A58" s="74" t="s">
         <v>223</v>
       </c>
-      <c r="B58" s="72" t="s">
+      <c r="B58" s="70" t="s">
         <v>704</v>
       </c>
-      <c r="C58" s="72" t="s">
+      <c r="C58" s="70" t="s">
         <v>851</v>
       </c>
-      <c r="D58" s="72" t="s">
+      <c r="D58" s="70" t="s">
         <v>852</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A59" s="76" t="s">
+      <c r="A59" s="74" t="s">
         <v>223</v>
       </c>
-      <c r="B59" s="72" t="s">
+      <c r="B59" s="70" t="s">
         <v>709</v>
       </c>
-      <c r="C59" s="72" t="s">
+      <c r="C59" s="70" t="s">
         <v>853</v>
       </c>
-      <c r="D59" s="72" t="s">
+      <c r="D59" s="70" t="s">
         <v>854</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="76" t="s">
+      <c r="A60" s="74" t="s">
         <v>566</v>
       </c>
-      <c r="B60" s="72" t="s">
+      <c r="B60" s="70" t="s">
         <v>855</v>
       </c>
-      <c r="C60" s="72" t="s">
+      <c r="C60" s="70" t="s">
         <v>856</v>
       </c>
-      <c r="D60" s="72" t="s">
+      <c r="D60" s="70" t="s">
         <v>857</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="76" t="s">
+      <c r="A61" s="74" t="s">
         <v>566</v>
       </c>
-      <c r="B61" s="72" t="s">
+      <c r="B61" s="70" t="s">
         <v>858</v>
       </c>
-      <c r="C61" s="72" t="s">
+      <c r="C61" s="70" t="s">
         <v>859</v>
       </c>
-      <c r="D61" s="72" t="s">
+      <c r="D61" s="70" t="s">
         <v>860</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="76" t="s">
+      <c r="A62" s="74" t="s">
         <v>566</v>
       </c>
-      <c r="B62" s="72" t="s">
+      <c r="B62" s="70" t="s">
         <v>861</v>
       </c>
-      <c r="C62" s="72" t="s">
+      <c r="C62" s="70" t="s">
         <v>862</v>
       </c>
-      <c r="D62" s="72" t="s">
+      <c r="D62" s="70" t="s">
         <v>863</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="76" t="s">
+      <c r="A63" s="74" t="s">
         <v>566</v>
       </c>
-      <c r="B63" s="72" t="s">
+      <c r="B63" s="70" t="s">
         <v>864</v>
       </c>
-      <c r="C63" s="72" t="s">
+      <c r="C63" s="70" t="s">
         <v>865</v>
       </c>
-      <c r="D63" s="72" t="s">
+      <c r="D63" s="70" t="s">
         <v>866</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="72" t="s">
+      <c r="A64" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B64" s="72" t="s">
+      <c r="B64" s="70" t="s">
         <v>867</v>
       </c>
-      <c r="C64" s="72" t="s">
+      <c r="C64" s="70" t="s">
         <v>868</v>
       </c>
-      <c r="D64" s="72" t="s">
+      <c r="D64" s="70" t="s">
         <v>869</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="72" t="s">
+      <c r="A65" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B65" s="77" t="s">
+      <c r="B65" s="75" t="s">
         <v>870</v>
       </c>
-      <c r="C65" s="77" t="s">
+      <c r="C65" s="75" t="s">
         <v>871</v>
       </c>
-      <c r="D65" s="77" t="s">
+      <c r="D65" s="75" t="s">
         <v>872</v>
       </c>
-      <c r="E65" s="77"/>
-      <c r="F65" s="77"/>
+      <c r="E65" s="75"/>
+      <c r="F65" s="75"/>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="72" t="s">
+      <c r="A66" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B66" s="77" t="s">
+      <c r="B66" s="75" t="s">
         <v>873</v>
       </c>
-      <c r="C66" s="77" t="s">
+      <c r="C66" s="75" t="s">
         <v>874</v>
       </c>
-      <c r="D66" s="77" t="s">
+      <c r="D66" s="75" t="s">
         <v>875</v>
       </c>
-      <c r="E66" s="77"/>
-      <c r="F66" s="77"/>
+      <c r="E66" s="75"/>
+      <c r="F66" s="75"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="72" t="s">
+      <c r="A67" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B67" s="77" t="s">
+      <c r="B67" s="75" t="s">
         <v>876</v>
       </c>
-      <c r="C67" s="77" t="s">
+      <c r="C67" s="75" t="s">
         <v>877</v>
       </c>
-      <c r="D67" s="77" t="s">
+      <c r="D67" s="75" t="s">
         <v>878</v>
       </c>
-      <c r="E67" s="77"/>
-      <c r="F67" s="77"/>
+      <c r="E67" s="75"/>
+      <c r="F67" s="75"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="72" t="s">
+      <c r="A68" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B68" s="77" t="s">
+      <c r="B68" s="75" t="s">
         <v>879</v>
       </c>
-      <c r="C68" s="77" t="s">
+      <c r="C68" s="75" t="s">
         <v>880</v>
       </c>
-      <c r="D68" s="77" t="s">
+      <c r="D68" s="75" t="s">
         <v>881</v>
       </c>
-      <c r="E68" s="77"/>
-      <c r="F68" s="77"/>
+      <c r="E68" s="75"/>
+      <c r="F68" s="75"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="72" t="s">
+      <c r="A69" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B69" s="77" t="s">
+      <c r="B69" s="75" t="s">
         <v>882</v>
       </c>
-      <c r="C69" s="77" t="s">
+      <c r="C69" s="75" t="s">
         <v>883</v>
       </c>
-      <c r="D69" s="77" t="s">
+      <c r="D69" s="75" t="s">
         <v>884</v>
       </c>
-      <c r="E69" s="77"/>
-      <c r="F69" s="77"/>
+      <c r="E69" s="75"/>
+      <c r="F69" s="75"/>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="72" t="s">
+      <c r="A70" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B70" s="77" t="s">
+      <c r="B70" s="75" t="s">
         <v>885</v>
       </c>
-      <c r="C70" s="77" t="s">
+      <c r="C70" s="75" t="s">
         <v>886</v>
       </c>
-      <c r="D70" s="77" t="s">
+      <c r="D70" s="75" t="s">
         <v>887</v>
       </c>
-      <c r="E70" s="77"/>
-      <c r="F70" s="77"/>
+      <c r="E70" s="75"/>
+      <c r="F70" s="75"/>
     </row>
     <row r="71" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="72" t="s">
+      <c r="A71" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B71" s="77" t="s">
+      <c r="B71" s="75" t="s">
         <v>888</v>
       </c>
-      <c r="C71" s="77" t="s">
+      <c r="C71" s="75" t="s">
         <v>889</v>
       </c>
-      <c r="D71" s="77" t="s">
+      <c r="D71" s="75" t="s">
         <v>890</v>
       </c>
-      <c r="E71" s="77"/>
-      <c r="F71" s="77"/>
+      <c r="E71" s="75"/>
+      <c r="F71" s="75"/>
     </row>
     <row r="72" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="72" t="s">
+      <c r="A72" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B72" s="77" t="s">
+      <c r="B72" s="75" t="s">
         <v>891</v>
       </c>
-      <c r="C72" s="77" t="s">
+      <c r="C72" s="75" t="s">
         <v>892</v>
       </c>
-      <c r="D72" s="77" t="s">
+      <c r="D72" s="75" t="s">
         <v>893</v>
       </c>
-      <c r="E72" s="77"/>
-      <c r="F72" s="77"/>
+      <c r="E72" s="75"/>
+      <c r="F72" s="75"/>
     </row>
     <row r="73" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="72" t="s">
+      <c r="A73" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B73" s="77" t="s">
+      <c r="B73" s="75" t="s">
         <v>894</v>
       </c>
-      <c r="C73" s="77" t="s">
+      <c r="C73" s="75" t="s">
         <v>895</v>
       </c>
-      <c r="D73" s="77" t="s">
+      <c r="D73" s="75" t="s">
         <v>896</v>
       </c>
-      <c r="E73" s="77"/>
-      <c r="F73" s="77"/>
+      <c r="E73" s="75"/>
+      <c r="F73" s="75"/>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="72" t="s">
+      <c r="A74" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B74" s="77" t="s">
+      <c r="B74" s="75" t="s">
         <v>897</v>
       </c>
-      <c r="C74" s="77" t="s">
+      <c r="C74" s="75" t="s">
         <v>898</v>
       </c>
-      <c r="D74" s="77" t="s">
+      <c r="D74" s="75" t="s">
         <v>899</v>
       </c>
-      <c r="E74" s="77"/>
-      <c r="F74" s="77"/>
+      <c r="E74" s="75"/>
+      <c r="F74" s="75"/>
     </row>
     <row r="75" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="72" t="s">
+      <c r="A75" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B75" s="77" t="s">
+      <c r="B75" s="75" t="s">
         <v>900</v>
       </c>
-      <c r="C75" s="77" t="s">
+      <c r="C75" s="75" t="s">
         <v>901</v>
       </c>
-      <c r="D75" s="77" t="s">
+      <c r="D75" s="75" t="s">
         <v>902</v>
       </c>
-      <c r="E75" s="77"/>
-      <c r="F75" s="77"/>
+      <c r="E75" s="75"/>
+      <c r="F75" s="75"/>
     </row>
     <row r="76" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="72" t="s">
+      <c r="A76" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B76" s="72" t="s">
+      <c r="B76" s="70" t="s">
         <v>903</v>
       </c>
-      <c r="C76" s="72" t="s">
+      <c r="C76" s="70" t="s">
         <v>904</v>
       </c>
-      <c r="D76" s="72" t="s">
+      <c r="D76" s="70" t="s">
         <v>905</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="72" t="s">
+      <c r="A77" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B77" s="72" t="s">
+      <c r="B77" s="70" t="s">
         <v>765</v>
       </c>
-      <c r="C77" s="72" t="s">
+      <c r="C77" s="70" t="s">
         <v>766</v>
       </c>
-      <c r="D77" s="72" t="s">
+      <c r="D77" s="70" t="s">
         <v>767</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="72" t="s">
+      <c r="A78" s="70" t="s">
         <v>600</v>
       </c>
-      <c r="B78" s="72" t="s">
+      <c r="B78" s="70" t="s">
         <v>906</v>
       </c>
-      <c r="C78" s="72" t="s">
+      <c r="C78" s="70" t="s">
         <v>768</v>
       </c>
-      <c r="D78" s="72" t="s">
+      <c r="D78" s="70" t="s">
         <v>907</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="78" t="s">
+      <c r="A79" s="76" t="s">
         <v>595</v>
       </c>
-      <c r="B79" s="77" t="s">
+      <c r="B79" s="75" t="s">
         <v>908</v>
       </c>
-      <c r="C79" s="72" t="s">
+      <c r="C79" s="70" t="s">
         <v>909</v>
       </c>
-      <c r="D79" s="72" t="s">
+      <c r="D79" s="70" t="s">
         <v>910</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="78" t="s">
+      <c r="A80" s="76" t="s">
         <v>595</v>
       </c>
-      <c r="B80" s="72" t="s">
+      <c r="B80" s="70" t="s">
         <v>911</v>
       </c>
-      <c r="C80" s="72" t="s">
+      <c r="C80" s="70" t="s">
         <v>912</v>
       </c>
-      <c r="D80" s="72" t="s">
+      <c r="D80" s="70" t="s">
         <v>913</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="78" t="s">
+      <c r="A81" s="76" t="s">
         <v>595</v>
       </c>
-      <c r="B81" s="72" t="s">
+      <c r="B81" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="C81" s="72" t="s">
+      <c r="C81" s="70" t="s">
         <v>763</v>
       </c>
-      <c r="D81" s="72" t="s">
+      <c r="D81" s="70" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="78" t="s">
+      <c r="A82" s="76" t="s">
         <v>595</v>
       </c>
-      <c r="B82" s="72" t="s">
+      <c r="B82" s="70" t="s">
         <v>682</v>
       </c>
-      <c r="C82" s="77" t="s">
+      <c r="C82" s="75" t="s">
         <v>768</v>
       </c>
-      <c r="D82" s="77" t="s">
+      <c r="D82" s="75" t="s">
         <v>907</v>
       </c>
-      <c r="E82" s="77"/>
-      <c r="F82" s="77"/>
+      <c r="E82" s="75"/>
+      <c r="F82" s="75"/>
     </row>
     <row r="83" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="79" t="s">
+      <c r="A83" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="B83" s="72" t="s">
+      <c r="B83" s="70" t="s">
         <v>914</v>
       </c>
-      <c r="C83" s="80" t="s">
+      <c r="C83" s="78" t="s">
         <v>915</v>
       </c>
-      <c r="D83" s="72" t="s">
+      <c r="D83" s="70" t="s">
         <v>916</v>
       </c>
-      <c r="H83" s="77" t="s">
+      <c r="H83" s="75" t="s">
         <v>693</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="79" t="s">
+      <c r="A84" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="B84" s="72" t="s">
+      <c r="B84" s="70" t="s">
         <v>917</v>
       </c>
-      <c r="C84" s="77" t="s">
+      <c r="C84" s="75" t="s">
         <v>918</v>
       </c>
-      <c r="D84" s="80" t="s">
+      <c r="D84" s="78" t="s">
         <v>919</v>
       </c>
-      <c r="E84" s="80"/>
-      <c r="F84" s="80"/>
+      <c r="E84" s="78"/>
+      <c r="F84" s="78"/>
       <c r="H84" s="2" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="79" t="s">
+      <c r="A85" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="B85" s="72" t="s">
+      <c r="B85" s="70" t="s">
         <v>920</v>
       </c>
-      <c r="C85" s="77" t="s">
+      <c r="C85" s="75" t="s">
         <v>921</v>
       </c>
-      <c r="D85" s="72" t="s">
+      <c r="D85" s="70" t="s">
         <v>922</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="79" t="s">
+      <c r="A86" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="B86" s="72" t="s">
+      <c r="B86" s="70" t="s">
         <v>923</v>
       </c>
-      <c r="C86" s="77" t="s">
+      <c r="C86" s="75" t="s">
         <v>924</v>
       </c>
-      <c r="D86" s="77" t="s">
+      <c r="D86" s="75" t="s">
         <v>925</v>
       </c>
-      <c r="E86" s="77"/>
-      <c r="F86" s="77"/>
+      <c r="E86" s="75"/>
+      <c r="F86" s="75"/>
     </row>
     <row r="87" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="79" t="s">
+      <c r="A87" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="B87" s="72" t="s">
+      <c r="B87" s="70" t="s">
         <v>926</v>
       </c>
-      <c r="C87" s="77" t="s">
+      <c r="C87" s="75" t="s">
         <v>927</v>
       </c>
-      <c r="D87" s="77" t="s">
+      <c r="D87" s="75" t="s">
         <v>928</v>
       </c>
-      <c r="E87" s="77"/>
-      <c r="F87" s="77"/>
+      <c r="E87" s="75"/>
+      <c r="F87" s="75"/>
     </row>
     <row r="88" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="79" t="s">
+      <c r="A88" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="B88" s="72" t="s">
+      <c r="B88" s="70" t="s">
         <v>929</v>
       </c>
-      <c r="C88" s="77" t="s">
+      <c r="C88" s="75" t="s">
         <v>930</v>
       </c>
-      <c r="D88" s="77" t="s">
+      <c r="D88" s="75" t="s">
         <v>931</v>
       </c>
-      <c r="E88" s="77"/>
-      <c r="F88" s="77"/>
+      <c r="E88" s="75"/>
+      <c r="F88" s="75"/>
       <c r="H88" s="2" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="79" t="s">
+      <c r="A89" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="B89" s="72" t="s">
+      <c r="B89" s="70" t="s">
         <v>932</v>
       </c>
-      <c r="C89" s="77" t="s">
+      <c r="C89" s="75" t="s">
         <v>933</v>
       </c>
-      <c r="D89" s="77" t="s">
+      <c r="D89" s="75" t="s">
         <v>934</v>
       </c>
-      <c r="E89" s="77"/>
-      <c r="F89" s="77"/>
+      <c r="E89" s="75"/>
+      <c r="F89" s="75"/>
     </row>
     <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="79" t="s">
+      <c r="A90" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="B90" s="72" t="s">
+      <c r="B90" s="70" t="s">
         <v>935</v>
       </c>
-      <c r="C90" s="77" t="s">
+      <c r="C90" s="75" t="s">
         <v>936</v>
       </c>
-      <c r="D90" s="77" t="s">
+      <c r="D90" s="75" t="s">
         <v>937</v>
       </c>
-      <c r="E90" s="77"/>
-      <c r="F90" s="77"/>
+      <c r="E90" s="75"/>
+      <c r="F90" s="75"/>
       <c r="H90" s="2" t="s">
         <v>222</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="79" t="s">
+      <c r="A91" s="77" t="s">
         <v>321</v>
       </c>
-      <c r="B91" s="72" t="s">
+      <c r="B91" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="C91" s="77" t="s">
+      <c r="C91" s="75" t="s">
         <v>763</v>
       </c>
-      <c r="D91" s="72" t="s">
+      <c r="D91" s="70" t="s">
         <v>764</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="79" t="s">
+      <c r="A92" s="77" t="s">
         <v>938</v>
       </c>
-      <c r="B92" s="72" t="s">
+      <c r="B92" s="70" t="s">
         <v>27</v>
       </c>
-      <c r="C92" s="72" t="s">
+      <c r="C92" s="70" t="s">
         <v>722</v>
       </c>
-      <c r="D92" s="72" t="s">
+      <c r="D92" s="70" t="s">
         <v>723</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="79" t="s">
+      <c r="A93" s="77" t="s">
         <v>938</v>
       </c>
-      <c r="B93" s="72" t="s">
+      <c r="B93" s="70" t="s">
         <v>939</v>
       </c>
-      <c r="C93" s="72" t="s">
+      <c r="C93" s="70" t="s">
         <v>940</v>
       </c>
-      <c r="D93" s="72" t="s">
+      <c r="D93" s="70" t="s">
         <v>941</v>
       </c>
-      <c r="H93" s="72" t="s">
+      <c r="H93" s="70" t="s">
         <v>708</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="79" t="s">
+      <c r="A94" s="77" t="s">
         <v>938</v>
       </c>
-      <c r="B94" s="72" t="s">
+      <c r="B94" s="70" t="s">
         <v>162</v>
       </c>
-      <c r="C94" s="72" t="s">
+      <c r="C94" s="70" t="s">
         <v>942</v>
       </c>
-      <c r="D94" s="72" t="s">
+      <c r="D94" s="70" t="s">
         <v>943</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="79" t="s">
+      <c r="A95" s="77" t="s">
         <v>938</v>
       </c>
-      <c r="B95" s="77" t="s">
+      <c r="B95" s="75" t="s">
         <v>944</v>
       </c>
-      <c r="C95" s="77" t="s">
+      <c r="C95" s="75" t="s">
         <v>945</v>
       </c>
-      <c r="D95" s="77" t="s">
+      <c r="D95" s="75" t="s">
         <v>946</v>
       </c>
-      <c r="E95" s="77" t="s">
+      <c r="E95" s="75" t="s">
         <v>947</v>
       </c>
-      <c r="F95" s="77" t="s">
+      <c r="F95" s="75" t="s">
         <v>948</v>
       </c>
-      <c r="H95" s="72" t="s">
+      <c r="H95" s="70" t="s">
         <v>949</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="79" t="s">
+      <c r="A96" s="77" t="s">
         <v>950</v>
       </c>
-      <c r="B96" s="72" t="s">
+      <c r="B96" s="70" t="s">
         <v>951</v>
       </c>
-      <c r="C96" s="77" t="s">
+      <c r="C96" s="75" t="s">
         <v>952</v>
       </c>
-      <c r="D96" s="77" t="s">
+      <c r="D96" s="75" t="s">
         <v>953</v>
       </c>
-      <c r="E96" s="77" t="s">
+      <c r="E96" s="75" t="s">
         <v>954</v>
       </c>
-      <c r="F96" s="77" t="s">
+      <c r="F96" s="75" t="s">
         <v>955</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="79" t="s">
+      <c r="A97" s="77" t="s">
         <v>950</v>
       </c>
-      <c r="B97" s="72" t="s">
+      <c r="B97" s="70" t="s">
         <v>956</v>
       </c>
-      <c r="C97" s="77" t="s">
+      <c r="C97" s="75" t="s">
         <v>957</v>
       </c>
-      <c r="D97" s="77" t="s">
+      <c r="D97" s="75" t="s">
         <v>958</v>
       </c>
-      <c r="E97" s="77" t="s">
+      <c r="E97" s="75" t="s">
         <v>959</v>
       </c>
-      <c r="F97" s="77" t="s">
+      <c r="F97" s="75" t="s">
         <v>960</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="79" t="s">
+      <c r="A98" s="77" t="s">
         <v>950</v>
       </c>
-      <c r="B98" s="72" t="s">
+      <c r="B98" s="70" t="s">
         <v>757</v>
       </c>
-      <c r="C98" s="72" t="s">
+      <c r="C98" s="70" t="s">
         <v>758</v>
       </c>
-      <c r="D98" s="72" t="s">
+      <c r="D98" s="70" t="s">
         <v>759</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A99" s="79" t="s">
+      <c r="A99" s="77" t="s">
         <v>525</v>
       </c>
-      <c r="B99" s="77" t="s">
+      <c r="B99" s="75" t="s">
         <v>961</v>
       </c>
-      <c r="C99" s="77" t="s">
+      <c r="C99" s="75" t="s">
         <v>962</v>
       </c>
-      <c r="D99" s="77" t="s">
+      <c r="D99" s="75" t="s">
         <v>963</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A100" s="79" t="s">
+      <c r="A100" s="77" t="s">
         <v>525</v>
       </c>
-      <c r="B100" s="77" t="s">
+      <c r="B100" s="75" t="s">
         <v>964</v>
       </c>
-      <c r="C100" s="77" t="s">
+      <c r="C100" s="75" t="s">
         <v>965</v>
       </c>
-      <c r="D100" s="77" t="s">
+      <c r="D100" s="75" t="s">
         <v>966</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A101" s="79" t="s">
+      <c r="A101" s="77" t="s">
         <v>525</v>
       </c>
-      <c r="B101" s="77" t="s">
+      <c r="B101" s="75" t="s">
         <v>967</v>
       </c>
-      <c r="C101" s="77" t="s">
+      <c r="C101" s="75" t="s">
         <v>968</v>
       </c>
-      <c r="D101" s="77" t="s">
+      <c r="D101" s="75" t="s">
         <v>969</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A102" s="79" t="s">
+      <c r="A102" s="77" t="s">
         <v>525</v>
       </c>
-      <c r="B102" s="77" t="s">
+      <c r="B102" s="75" t="s">
         <v>970</v>
       </c>
-      <c r="C102" s="77" t="s">
+      <c r="C102" s="75" t="s">
         <v>971</v>
       </c>
-      <c r="D102" s="77" t="s">
+      <c r="D102" s="75" t="s">
         <v>972</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A103" s="79" t="s">
+      <c r="A103" s="77" t="s">
         <v>525</v>
       </c>
-      <c r="G103" s="75" t="s">
+      <c r="G103" s="73" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A104" s="79" t="s">
+      <c r="A104" s="77" t="s">
         <v>525</v>
       </c>
-      <c r="G104" s="75" t="s">
+      <c r="G104" s="73" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A105" s="79" t="s">
+      <c r="A105" s="77" t="s">
         <v>540</v>
       </c>
-      <c r="B105" s="77" t="s">
+      <c r="B105" s="75" t="s">
         <v>973</v>
       </c>
-      <c r="C105" s="77" t="s">
+      <c r="C105" s="75" t="s">
         <v>974</v>
       </c>
-      <c r="D105" s="77" t="s">
+      <c r="D105" s="75" t="s">
         <v>975</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="79" t="s">
+      <c r="A106" s="77" t="s">
         <v>540</v>
       </c>
-      <c r="B106" s="77" t="s">
+      <c r="B106" s="75" t="s">
         <v>976</v>
       </c>
-      <c r="C106" s="77" t="s">
+      <c r="C106" s="75" t="s">
         <v>977</v>
       </c>
-      <c r="D106" s="77" t="s">
+      <c r="D106" s="75" t="s">
         <v>978</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A107" s="79" t="s">
+      <c r="A107" s="77" t="s">
         <v>540</v>
       </c>
-      <c r="B107" s="77" t="s">
+      <c r="B107" s="75" t="s">
         <v>967</v>
       </c>
-      <c r="C107" s="77" t="s">
+      <c r="C107" s="75" t="s">
         <v>968</v>
       </c>
-      <c r="D107" s="77" t="s">
+      <c r="D107" s="75" t="s">
         <v>969</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A108" s="79" t="s">
+      <c r="A108" s="77" t="s">
         <v>540</v>
       </c>
-      <c r="B108" s="77" t="s">
+      <c r="B108" s="75" t="s">
         <v>979</v>
       </c>
-      <c r="C108" s="77" t="s">
+      <c r="C108" s="75" t="s">
         <v>980</v>
       </c>
-      <c r="D108" s="77" t="s">
+      <c r="D108" s="75" t="s">
         <v>981</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A109" s="79" t="s">
+      <c r="A109" s="77" t="s">
         <v>540</v>
       </c>
-      <c r="G109" s="75" t="s">
+      <c r="G109" s="73" t="s">
         <v>762</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A110" s="79" t="s">
+      <c r="A110" s="77" t="s">
         <v>540</v>
       </c>
-      <c r="G110" s="75" t="s">
+      <c r="G110" s="73" t="s">
         <v>765</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="81" t="s">
+      <c r="A111" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="B111" s="77" t="s">
+      <c r="B111" s="75" t="s">
         <v>982</v>
       </c>
-      <c r="C111" s="72" t="s">
+      <c r="C111" s="70" t="s">
         <v>983</v>
       </c>
-      <c r="D111" s="72" t="s">
+      <c r="D111" s="70" t="s">
         <v>984</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="81" t="s">
+      <c r="A112" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="B112" s="72" t="s">
+      <c r="B112" s="70" t="s">
         <v>985</v>
       </c>
-      <c r="C112" s="72" t="s">
+      <c r="C112" s="70" t="s">
         <v>986</v>
       </c>
-      <c r="D112" s="72" t="s">
+      <c r="D112" s="70" t="s">
         <v>987</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="81" t="s">
+      <c r="A113" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="B113" s="77" t="s">
+      <c r="B113" s="75" t="s">
         <v>988</v>
       </c>
-      <c r="C113" s="72" t="s">
+      <c r="C113" s="70" t="s">
         <v>989</v>
       </c>
-      <c r="D113" s="72" t="s">
+      <c r="D113" s="70" t="s">
         <v>990</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="81" t="s">
+      <c r="A114" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="B114" s="77" t="s">
+      <c r="B114" s="75" t="s">
         <v>991</v>
       </c>
-      <c r="C114" s="72" t="s">
+      <c r="C114" s="70" t="s">
         <v>992</v>
       </c>
-      <c r="D114" s="72" t="s">
+      <c r="D114" s="70" t="s">
         <v>993</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="81" t="s">
+      <c r="A115" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="B115" s="77" t="s">
+      <c r="B115" s="75" t="s">
         <v>994</v>
       </c>
-      <c r="C115" s="72" t="s">
+      <c r="C115" s="70" t="s">
         <v>995</v>
       </c>
-      <c r="D115" s="72" t="s">
+      <c r="D115" s="70" t="s">
         <v>996</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="81" t="s">
+      <c r="A116" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="B116" s="77" t="s">
+      <c r="B116" s="75" t="s">
         <v>997</v>
       </c>
-      <c r="C116" s="72" t="s">
+      <c r="C116" s="70" t="s">
         <v>998</v>
       </c>
-      <c r="D116" s="72" t="s">
+      <c r="D116" s="70" t="s">
         <v>999</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="81" t="s">
+      <c r="A117" s="79" t="s">
         <v>176</v>
       </c>
-      <c r="G117" s="75" t="s">
+      <c r="G117" s="73" t="s">
         <v>682</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="76" t="s">
+      <c r="A118" s="74" t="s">
         <v>1000</v>
       </c>
-      <c r="B118" s="75" t="s">
+      <c r="B118" s="73" t="s">
         <v>703</v>
       </c>
-      <c r="C118" s="75" t="s">
+      <c r="C118" s="73" t="s">
         <v>1001</v>
       </c>
-      <c r="D118" s="75" t="s">
+      <c r="D118" s="73" t="s">
         <v>1002</v>
       </c>
-      <c r="E118" s="75" t="s">
+      <c r="E118" s="73" t="s">
         <v>1003</v>
       </c>
-      <c r="F118" s="75" t="s">
+      <c r="F118" s="73" t="s">
         <v>1004</v>
       </c>
-      <c r="G118" s="76"/>
+      <c r="G118" s="74"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="76" t="s">
+      <c r="A119" s="74" t="s">
         <v>1000</v>
       </c>
-      <c r="B119" s="75" t="s">
+      <c r="B119" s="73" t="s">
         <v>704</v>
       </c>
-      <c r="C119" s="75" t="s">
+      <c r="C119" s="73" t="s">
         <v>1005</v>
       </c>
-      <c r="D119" s="75" t="s">
+      <c r="D119" s="73" t="s">
         <v>1006</v>
       </c>
-      <c r="E119" s="75" t="s">
+      <c r="E119" s="73" t="s">
         <v>1007</v>
       </c>
-      <c r="F119" s="75" t="s">
+      <c r="F119" s="73" t="s">
         <v>1008</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="76" t="s">
+      <c r="A120" s="74" t="s">
         <v>1000</v>
       </c>
-      <c r="B120" s="75" t="s">
+      <c r="B120" s="73" t="s">
         <v>705</v>
       </c>
-      <c r="C120" s="75" t="s">
+      <c r="C120" s="73" t="s">
         <v>1009</v>
       </c>
-      <c r="D120" s="75" t="s">
+      <c r="D120" s="73" t="s">
         <v>1010</v>
       </c>
-      <c r="E120" s="75" t="s">
+      <c r="E120" s="73" t="s">
         <v>1011</v>
       </c>
-      <c r="F120" s="75" t="s">
+      <c r="F120" s="73" t="s">
         <v>1012</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="76" t="s">
+      <c r="A121" s="74" t="s">
         <v>1000</v>
       </c>
-      <c r="B121" s="75" t="s">
+      <c r="B121" s="73" t="s">
         <v>845</v>
       </c>
-      <c r="C121" s="75" t="s">
+      <c r="C121" s="73" t="s">
         <v>1013</v>
       </c>
-      <c r="D121" s="75" t="s">
+      <c r="D121" s="73" t="s">
         <v>1014</v>
       </c>
-      <c r="E121" s="75" t="s">
+      <c r="E121" s="73" t="s">
         <v>1015</v>
       </c>
-      <c r="F121" s="75" t="s">
+      <c r="F121" s="73" t="s">
         <v>1016</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="76" t="s">
+      <c r="A122" s="74" t="s">
         <v>1000</v>
       </c>
-      <c r="B122" s="75" t="s">
+      <c r="B122" s="73" t="s">
         <v>709</v>
       </c>
-      <c r="C122" s="75" t="s">
+      <c r="C122" s="73" t="s">
         <v>1017</v>
       </c>
-      <c r="D122" s="75" t="s">
+      <c r="D122" s="73" t="s">
         <v>1018</v>
       </c>
-      <c r="E122" s="75" t="s">
+      <c r="E122" s="73" t="s">
         <v>1019</v>
       </c>
-      <c r="F122" s="75" t="s">
+      <c r="F122" s="73" t="s">
         <v>1020</v>
       </c>
     </row>
@@ -15514,193 +15546,193 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" s="83" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="82" t="s">
+    <row r="1" s="81" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="80" t="s">
         <v>1021</v>
       </c>
-      <c r="B1" s="82" t="s">
+      <c r="B1" s="80" t="s">
         <v>1022</v>
       </c>
-      <c r="C1" s="82" t="s">
+      <c r="C1" s="80" t="s">
         <v>1023</v>
       </c>
-      <c r="D1" s="82" t="s">
+      <c r="D1" s="80" t="s">
         <v>1024</v>
       </c>
-      <c r="E1" s="82" t="s">
+      <c r="E1" s="80" t="s">
         <v>1025</v>
       </c>
-      <c r="F1" s="82" t="s">
+      <c r="F1" s="80" t="s">
         <v>1026</v>
       </c>
-      <c r="G1" s="82" t="s">
+      <c r="G1" s="80" t="s">
         <v>1027</v>
       </c>
-      <c r="H1" s="82" t="s">
+      <c r="H1" s="80" t="s">
         <v>1028</v>
       </c>
-      <c r="I1" s="82" t="s">
+      <c r="I1" s="80" t="s">
         <v>1029</v>
       </c>
-      <c r="J1" s="82" t="s">
+      <c r="J1" s="80" t="s">
         <v>1030</v>
       </c>
-      <c r="K1" s="82" t="s">
+      <c r="K1" s="80" t="s">
         <v>1031</v>
       </c>
-      <c r="L1" s="83" t="s">
+      <c r="L1" s="81" t="s">
         <v>1032</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="51" t="s">
+      <c r="A2" s="50" t="s">
         <v>646</v>
       </c>
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="50" t="s">
         <v>1033</v>
       </c>
-      <c r="C2" s="51" t="s">
+      <c r="C2" s="50" t="s">
         <v>1034</v>
       </c>
-      <c r="D2" s="51" t="s">
+      <c r="D2" s="50" t="s">
         <v>1035</v>
       </c>
-      <c r="E2" s="51" t="s">
+      <c r="E2" s="50" t="s">
         <v>1036</v>
       </c>
-      <c r="F2" s="51" t="s">
+      <c r="F2" s="50" t="s">
         <v>1037</v>
       </c>
-      <c r="G2" s="51" t="s">
+      <c r="G2" s="50" t="s">
         <v>1038</v>
       </c>
-      <c r="H2" s="51" t="n">
+      <c r="H2" s="50" t="n">
         <v>-10</v>
       </c>
-      <c r="I2" s="51" t="n">
+      <c r="I2" s="50" t="n">
         <v>100</v>
       </c>
-      <c r="J2" s="51" t="s">
+      <c r="J2" s="50" t="s">
         <v>1039</v>
       </c>
-      <c r="K2" s="51" t="s">
+      <c r="K2" s="50" t="s">
         <v>1039</v>
       </c>
-      <c r="L2" s="51" t="s">
+      <c r="L2" s="50" t="s">
         <v>1040</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="51" t="s">
+      <c r="A3" s="50" t="s">
         <v>637</v>
       </c>
-      <c r="B3" s="51" t="s">
+      <c r="B3" s="50" t="s">
         <v>1041</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="50" t="s">
         <v>1042</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="82" t="s">
         <v>1043</v>
       </c>
-      <c r="E3" s="84" t="s">
+      <c r="E3" s="82" t="s">
         <v>1044</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="82" t="s">
         <v>1045</v>
       </c>
-      <c r="G3" s="51" t="s">
+      <c r="G3" s="50" t="s">
         <v>1046</v>
       </c>
-      <c r="H3" s="51" t="n">
+      <c r="H3" s="50" t="n">
         <v>-10</v>
       </c>
-      <c r="I3" s="51" t="n">
+      <c r="I3" s="50" t="n">
         <v>100</v>
       </c>
-      <c r="J3" s="51" t="s">
+      <c r="J3" s="50" t="s">
         <v>1039</v>
       </c>
-      <c r="K3" s="51" t="s">
+      <c r="K3" s="50" t="s">
         <v>1039</v>
       </c>
-      <c r="L3" s="51" t="s">
+      <c r="L3" s="50" t="s">
         <v>1047</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="50" t="s">
         <v>651</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="50" t="s">
         <v>1048</v>
       </c>
-      <c r="C4" s="51" t="s">
+      <c r="C4" s="50" t="s">
         <v>1049</v>
       </c>
-      <c r="D4" s="51" t="s">
+      <c r="D4" s="50" t="s">
         <v>1050</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="50" t="s">
         <v>1051</v>
       </c>
-      <c r="F4" s="51" t="s">
+      <c r="F4" s="50" t="s">
         <v>1052</v>
       </c>
-      <c r="G4" s="51" t="s">
+      <c r="G4" s="50" t="s">
         <v>1053</v>
       </c>
-      <c r="H4" s="51" t="n">
+      <c r="H4" s="50" t="n">
         <v>-10</v>
       </c>
-      <c r="I4" s="51" t="n">
+      <c r="I4" s="50" t="n">
         <v>100</v>
       </c>
-      <c r="J4" s="51" t="s">
+      <c r="J4" s="50" t="s">
         <v>1039</v>
       </c>
-      <c r="K4" s="51" t="s">
+      <c r="K4" s="50" t="s">
         <v>1039</v>
       </c>
-      <c r="L4" s="51" t="s">
+      <c r="L4" s="50" t="s">
         <v>1040</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="51" t="s">
+      <c r="A5" s="50" t="s">
         <v>656</v>
       </c>
-      <c r="B5" s="51" t="s">
+      <c r="B5" s="50" t="s">
         <v>1041</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="C5" s="50" t="s">
         <v>1054</v>
       </c>
-      <c r="D5" s="51" t="s">
+      <c r="D5" s="50" t="s">
         <v>1055</v>
       </c>
-      <c r="E5" s="51" t="s">
+      <c r="E5" s="50" t="s">
         <v>1044</v>
       </c>
-      <c r="F5" s="51" t="s">
+      <c r="F5" s="50" t="s">
         <v>1056</v>
       </c>
-      <c r="G5" s="51" t="s">
+      <c r="G5" s="50" t="s">
         <v>1057</v>
       </c>
-      <c r="H5" s="51" t="n">
+      <c r="H5" s="50" t="n">
         <v>-10</v>
       </c>
-      <c r="I5" s="51" t="n">
+      <c r="I5" s="50" t="n">
         <v>100</v>
       </c>
-      <c r="J5" s="51" t="s">
+      <c r="J5" s="50" t="s">
         <v>1039</v>
       </c>
-      <c r="K5" s="51" t="s">
+      <c r="K5" s="50" t="s">
         <v>1039</v>
       </c>
-      <c r="L5" s="51" t="s">
+      <c r="L5" s="50" t="s">
         <v>1040</v>
       </c>
     </row>
@@ -15724,7 +15756,7 @@
   </sheetPr>
   <dimension ref="A1:F1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J46" activeCellId="0" sqref="J46"/>
     </sheetView>
   </sheetViews>
@@ -16666,7 +16698,7 @@
       <c r="A60" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="B60" s="85" t="s">
+      <c r="B60" s="83" t="s">
         <v>1258</v>
       </c>
       <c r="C60" s="11" t="s">
@@ -16734,7 +16766,7 @@
       <c r="C64" s="40" t="s">
         <v>1273</v>
       </c>
-      <c r="D64" s="85" t="s">
+      <c r="D64" s="83" t="s">
         <v>1274</v>
       </c>
       <c r="E64" s="2"/>
@@ -16750,7 +16782,7 @@
       <c r="C65" s="40" t="s">
         <v>1276</v>
       </c>
-      <c r="D65" s="85" t="s">
+      <c r="D65" s="83" t="s">
         <v>1277</v>
       </c>
       <c r="E65" s="2"/>
@@ -16760,49 +16792,49 @@
       <c r="A66" s="35" t="s">
         <v>329</v>
       </c>
-      <c r="B66" s="68" t="s">
+      <c r="B66" s="66" t="s">
         <v>1278</v>
       </c>
-      <c r="C66" s="68" t="s">
+      <c r="C66" s="66" t="s">
         <v>722</v>
       </c>
-      <c r="D66" s="68" t="s">
+      <c r="D66" s="66" t="s">
         <v>723</v>
       </c>
-      <c r="E66" s="68"/>
-      <c r="F66" s="68"/>
+      <c r="E66" s="66"/>
+      <c r="F66" s="66"/>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="35" t="s">
         <v>329</v>
       </c>
-      <c r="B67" s="68" t="s">
+      <c r="B67" s="66" t="s">
         <v>1279</v>
       </c>
-      <c r="C67" s="68" t="s">
+      <c r="C67" s="66" t="s">
         <v>940</v>
       </c>
-      <c r="D67" s="68" t="s">
+      <c r="D67" s="66" t="s">
         <v>941</v>
       </c>
-      <c r="E67" s="68"/>
-      <c r="F67" s="68"/>
+      <c r="E67" s="66"/>
+      <c r="F67" s="66"/>
     </row>
     <row r="68" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="35" t="s">
         <v>329</v>
       </c>
-      <c r="B68" s="68" t="s">
+      <c r="B68" s="66" t="s">
         <v>1280</v>
       </c>
-      <c r="C68" s="68" t="s">
+      <c r="C68" s="66" t="s">
         <v>942</v>
       </c>
-      <c r="D68" s="68" t="s">
+      <c r="D68" s="66" t="s">
         <v>943</v>
       </c>
-      <c r="E68" s="68"/>
-      <c r="F68" s="68"/>
+      <c r="E68" s="66"/>
+      <c r="F68" s="66"/>
     </row>
     <row r="69" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="35" t="s">
@@ -16828,7 +16860,7 @@
       <c r="A70" s="35" t="s">
         <v>430</v>
       </c>
-      <c r="B70" s="68" t="s">
+      <c r="B70" s="66" t="s">
         <v>1282</v>
       </c>
       <c r="C70" s="11" t="s">
@@ -16848,7 +16880,7 @@
       <c r="A71" s="35" t="s">
         <v>430</v>
       </c>
-      <c r="B71" s="68" t="s">
+      <c r="B71" s="66" t="s">
         <v>1283</v>
       </c>
       <c r="C71" s="11" t="s">
@@ -16868,7 +16900,7 @@
       <c r="A72" s="35" t="s">
         <v>430</v>
       </c>
-      <c r="B72" s="68" t="s">
+      <c r="B72" s="66" t="s">
         <v>1284</v>
       </c>
       <c r="C72" s="11" t="s">
@@ -16884,7 +16916,7 @@
       <c r="A73" s="35" t="s">
         <v>430</v>
       </c>
-      <c r="B73" s="68" t="s">
+      <c r="B73" s="66" t="s">
         <v>1287</v>
       </c>
       <c r="C73" s="11" t="s">
@@ -16900,7 +16932,7 @@
       <c r="A74" s="35" t="s">
         <v>430</v>
       </c>
-      <c r="B74" s="68" t="s">
+      <c r="B74" s="66" t="s">
         <v>1290</v>
       </c>
       <c r="C74" s="11" t="s">

</xml_diff>

<commit_message>
Label:  update age label localization files for clarity
Fix: #419
</commit_message>
<xml_diff>
--- a/survey/references/OD_nationale_quebec_2025.xlsx
+++ b/survey/references/OD_nationale_quebec_2025.xlsx
@@ -387,18 +387,16 @@
     <t xml:space="preserve">age</t>
   </si>
   <si>
-    <t xml:space="preserve">**Âge**
-__Pour les bébés de moins de 1 an, inscrivez "0"__</t>
-  </si>
-  <si>
-    <t xml:space="preserve">**Age**
-__For babies under the age of 1, write "0"__</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Votre **âge**</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Your **age**</t>
+    <t xml:space="preserve">**Âge** (en années)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">**Age** (in years)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Votre **âge** (en années)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your **age** (in years)</t>
   </si>
   <si>
     <t xml:space="preserve">ageValidation</t>
@@ -5793,11 +5791,11 @@
   <dimension ref="A1:XFD1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="D42" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="D15" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A42" activeCellId="0" sqref="A42"/>
-      <selection pane="bottomRight" activeCell="I48" activeCellId="0" sqref="I48"/>
+      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
+      <selection pane="bottomRight" activeCell="I21" activeCellId="0" sqref="I21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14453125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>